<commit_message>
Tried removing PMU measurements
I tried to remove the PMU measurements from the IEEE 14 bus case, but
that really messed up the state estimation. Maybe the system becomes
unobservable?
Also did an actual power flow for the IEEE 14 bus case and ran those
measurements through the SE. The residuals are on the order of 1e-6 if I
remove P5-4 (something probably wrong with how Pto-from is calculated).
The decentralized solution still doesn't converge (try formulating in
rectangular form).
</commit_message>
<xml_diff>
--- a/DMASE - Test Results.xlsx
+++ b/DMASE - Test Results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="180">
   <si>
     <t>Abur 3-Bus Case Measurements (run through SE, rerun new estimate again)</t>
   </si>
@@ -543,20 +543,26 @@
     <t>-6.57189649021577i</t>
   </si>
   <si>
-    <t>Line Records</t>
-  </si>
-  <si>
-    <t>LineMW</t>
-  </si>
-  <si>
-    <t>?</t>
+    <t>something wrong with the way that Pto-from is calculated</t>
+  </si>
+  <si>
+    <t>Why 0?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>PowerWorld IEEE 14-Bus Case (construct DC case, use DCPF results); no PMU measurements</t>
+  </si>
+  <si>
+    <t>Created large res</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -575,6 +581,23 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -636,11 +659,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -679,6 +703,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -998,31 +1034,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="I1" s="5" t="s">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="I1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="6" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1040,7 +1076,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="10" t="s">
         <v>12</v>
       </c>
       <c r="J2" s="1">
@@ -1052,32 +1088,32 @@
       <c r="L2" s="1">
         <v>0.89269444819999999</v>
       </c>
-      <c r="M2" s="2">
+      <c r="M2" s="3">
         <v>-4.6099999999999999E-6</v>
       </c>
-      <c r="N2" s="2">
+      <c r="N2" s="3">
         <v>9.9900000000000006E-16</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5" t="s">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="10" t="s">
         <v>16</v>
       </c>
       <c r="J3" s="1">
@@ -1089,10 +1125,10 @@
       <c r="L3" s="1">
         <v>1.170863486</v>
       </c>
-      <c r="M3" s="2">
+      <c r="M3" s="3">
         <v>-7.9300000000000003E-5</v>
       </c>
-      <c r="N3" s="2">
+      <c r="N3" s="3">
         <v>-4.4400000000000002E-16</v>
       </c>
     </row>
@@ -1118,7 +1154,7 @@
       <c r="G4" s="1">
         <v>0</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="I4" s="10" t="s">
         <v>18</v>
       </c>
       <c r="J4" s="1">
@@ -1130,10 +1166,10 @@
       <c r="L4" s="1">
         <v>-0.4956651876</v>
       </c>
-      <c r="M4" s="2">
+      <c r="M4" s="3">
         <v>-4.2400000000000001E-5</v>
       </c>
-      <c r="N4" s="2">
+      <c r="N4" s="3">
         <v>1.6099999999999999E-15</v>
       </c>
     </row>
@@ -1159,7 +1195,7 @@
       <c r="G5" s="1">
         <v>-1.2903313789999999E-7</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="I5" s="10" t="s">
         <v>20</v>
       </c>
       <c r="J5" s="1">
@@ -1171,7 +1207,7 @@
       <c r="L5" s="1">
         <v>0</v>
       </c>
-      <c r="M5" s="2">
+      <c r="M5" s="3">
         <v>-5.04E-6</v>
       </c>
       <c r="N5" s="1">
@@ -1200,7 +1236,7 @@
       <c r="G6" s="1">
         <v>5.8433450400000004E-6</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="I6" s="10" t="s">
         <v>22</v>
       </c>
       <c r="J6" s="1">
@@ -1212,7 +1248,7 @@
       <c r="L6" s="1">
         <v>0</v>
       </c>
-      <c r="M6" s="2">
+      <c r="M6" s="3">
         <v>-4.1100000000000003E-5</v>
       </c>
       <c r="N6" s="1">
@@ -1241,7 +1277,7 @@
       <c r="G7" s="1">
         <v>-2.10700941E-7</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="I7" s="10" t="s">
         <v>24</v>
       </c>
       <c r="J7" s="1">
@@ -1253,7 +1289,7 @@
       <c r="L7" s="1">
         <v>0</v>
       </c>
-      <c r="M7" s="2">
+      <c r="M7" s="3">
         <v>-1.88E-5</v>
       </c>
       <c r="N7" s="1">
@@ -1282,7 +1318,7 @@
       <c r="G8" s="1">
         <v>-8.7038090069999994E-9</v>
       </c>
-      <c r="I8" s="9" t="s">
+      <c r="I8" s="10" t="s">
         <v>26</v>
       </c>
       <c r="J8" s="1">
@@ -1294,7 +1330,7 @@
       <c r="L8" s="1">
         <v>1</v>
       </c>
-      <c r="M8" s="2">
+      <c r="M8" s="3">
         <v>-1.02E-7</v>
       </c>
       <c r="N8" s="1">
@@ -1323,7 +1359,7 @@
       <c r="G9" s="1">
         <v>3.2929260540000001E-6</v>
       </c>
-      <c r="I9" s="9" t="s">
+      <c r="I9" s="10" t="s">
         <v>28</v>
       </c>
       <c r="J9" s="1">
@@ -1335,7 +1371,7 @@
       <c r="L9" s="1">
         <v>1</v>
       </c>
-      <c r="M9" s="2">
+      <c r="M9" s="3">
         <v>9.0600000000000004E-8</v>
       </c>
       <c r="N9" s="1">
@@ -1359,48 +1395,48 @@
       <c r="N11" s="1"/>
     </row>
     <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
       <c r="I12" s="1"/>
-      <c r="J12" s="5" t="s">
+      <c r="J12" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="K12" s="5" t="s">
+      <c r="K12" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="L12" s="5" t="s">
+      <c r="L12" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="M12" s="5" t="s">
+      <c r="M12" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="N12" s="5" t="s">
+      <c r="N12" s="6" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
       <c r="I13" s="1"/>
-      <c r="J13" s="9" t="s">
+      <c r="J13" s="10" t="s">
         <v>12</v>
       </c>
       <c r="K13" s="1">
@@ -1409,33 +1445,33 @@
       <c r="L13" s="1">
         <v>0.48125000969999998</v>
       </c>
-      <c r="M13" s="2">
+      <c r="M13" s="3">
         <v>2.5799999999999999E-6</v>
       </c>
-      <c r="N13" s="2">
+      <c r="N13" s="3">
         <v>5.62E-9</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5" t="s">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="G14" s="6" t="s">
         <v>11</v>
       </c>
       <c r="I14" s="1"/>
-      <c r="J14" s="9" t="s">
+      <c r="J14" s="10" t="s">
         <v>16</v>
       </c>
       <c r="K14" s="1">
@@ -1444,10 +1480,10 @@
       <c r="L14" s="1">
         <v>0.41874999619999997</v>
       </c>
-      <c r="M14" s="2">
+      <c r="M14" s="3">
         <v>-4.0200000000000003E-7</v>
       </c>
-      <c r="N14" s="2">
+      <c r="N14" s="3">
         <v>-2.5500000000000001E-9</v>
       </c>
     </row>
@@ -1474,7 +1510,7 @@
         <v>0</v>
       </c>
       <c r="I15" s="1"/>
-      <c r="J15" s="9" t="s">
+      <c r="J15" s="10" t="s">
         <v>18</v>
       </c>
       <c r="K15" s="1">
@@ -1483,10 +1519,10 @@
       <c r="L15" s="1">
         <v>-0.4</v>
       </c>
-      <c r="M15" s="2">
+      <c r="M15" s="3">
         <v>-7.8999999999999995E-7</v>
       </c>
-      <c r="N15" s="2">
+      <c r="N15" s="3">
         <v>6.3899999999999996E-9</v>
       </c>
     </row>
@@ -1506,14 +1542,14 @@
       <c r="E16" s="1">
         <v>-4.3600324780000002E-5</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="3">
         <v>9.2199999999999998E-6</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G16" s="3">
         <v>-3.4400000000000003E-5</v>
       </c>
       <c r="I16" s="1"/>
-      <c r="J16" s="9" t="s">
+      <c r="J16" s="10" t="s">
         <v>20</v>
       </c>
       <c r="K16" s="1">
@@ -1522,7 +1558,7 @@
       <c r="L16" s="1">
         <v>0</v>
       </c>
-      <c r="M16" s="2">
+      <c r="M16" s="3">
         <v>-8.8800000000000004E-5</v>
       </c>
       <c r="N16" s="1">
@@ -1545,14 +1581,14 @@
       <c r="E17" s="1">
         <v>2.7874991740000001E-2</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="3">
         <v>1.13E-5</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G17" s="3">
         <v>2.7900000000000001E-2</v>
       </c>
       <c r="I17" s="1"/>
-      <c r="J17" s="9" t="s">
+      <c r="J17" s="10" t="s">
         <v>22</v>
       </c>
       <c r="K17" s="1">
@@ -1561,7 +1597,7 @@
       <c r="L17" s="1">
         <v>0</v>
       </c>
-      <c r="M17" s="2">
+      <c r="M17" s="3">
         <v>4.07E-5</v>
       </c>
       <c r="N17" s="1">
@@ -1584,14 +1620,14 @@
       <c r="E18" s="1">
         <v>-1.422356891E-3</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="3">
         <v>2.8400000000000002E-4</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G18" s="3">
         <v>-1.14E-3</v>
       </c>
       <c r="I18" s="1"/>
-      <c r="J18" s="9" t="s">
+      <c r="J18" s="10" t="s">
         <v>24</v>
       </c>
       <c r="K18" s="1">
@@ -1623,14 +1659,14 @@
       <c r="E19" s="1">
         <v>-1.4323660430000001E-3</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19" s="3">
         <v>2.8200000000000002E-4</v>
       </c>
-      <c r="G19" s="2">
+      <c r="G19" s="3">
         <v>-1.15E-3</v>
       </c>
       <c r="I19" s="1"/>
-      <c r="J19" s="9" t="s">
+      <c r="J19" s="10" t="s">
         <v>26</v>
       </c>
       <c r="K19" s="1">
@@ -1639,7 +1675,7 @@
       <c r="L19" s="1">
         <v>1</v>
       </c>
-      <c r="M19" s="2">
+      <c r="M19" s="3">
         <v>-1.42E-6</v>
       </c>
       <c r="N19" s="1">
@@ -1662,14 +1698,14 @@
       <c r="E20" s="1">
         <v>3.6848139049999999</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20" s="3">
         <v>2.9100000000000003E-4</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G20" s="3">
         <v>3.69</v>
       </c>
       <c r="I20" s="1"/>
-      <c r="J20" s="9" t="s">
+      <c r="J20" s="10" t="s">
         <v>28</v>
       </c>
       <c r="K20" s="1">
@@ -1678,7 +1714,7 @@
       <c r="L20" s="1">
         <v>1</v>
       </c>
-      <c r="M20" s="2">
+      <c r="M20" s="3">
         <v>1.2300000000000001E-6</v>
       </c>
       <c r="N20" s="1">
@@ -1686,36 +1722,36 @@
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
     </row>
     <row r="23" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5" t="s">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="E23" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="F23" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G23" s="5" t="s">
+      <c r="G23" s="6" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1749,13 +1785,13 @@
       <c r="D25" s="1">
         <v>-1.443749678E-2</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E25" s="3">
         <v>-3.5100000000000001E-9</v>
       </c>
-      <c r="F25" s="2">
+      <c r="F25" s="3">
         <v>1.6900000000000001E-10</v>
       </c>
-      <c r="G25" s="2">
+      <c r="G25" s="3">
         <v>-3.34E-9</v>
       </c>
     </row>
@@ -1772,13 +1808,13 @@
       <c r="D26" s="1">
         <v>-2.0937470489999999E-2</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E26" s="3">
         <v>-3.0899999999999999E-8</v>
       </c>
-      <c r="F26" s="2">
+      <c r="F26" s="3">
         <v>1.4100000000000001E-9</v>
       </c>
-      <c r="G26" s="2">
+      <c r="G26" s="3">
         <v>-2.9499999999999999E-8</v>
       </c>
     </row>
@@ -1859,10 +1895,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O32"/>
+  <dimension ref="A1:Q66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="P42" sqref="P42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1875,52 +1911,55 @@
     <col min="15" max="15" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="L1" s="14" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="L1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="M1" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="N1" s="14" t="s">
+      <c r="N1" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="O1" s="14" t="s">
+      <c r="O1" s="15" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="Q1" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11" t="s">
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="L2" s="9" t="s">
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="L2" s="10" t="s">
         <v>42</v>
       </c>
       <c r="M2" s="1">
@@ -1929,50 +1968,61 @@
       <c r="N2" s="1">
         <v>0</v>
       </c>
-      <c r="O2" s="1"/>
-    </row>
-    <row r="3" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13" t="s">
+      <c r="O2" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H3" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="13" t="s">
+      <c r="I3" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="J3" s="13" t="s">
+      <c r="J3" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="L3" s="9" t="s">
+      <c r="L3" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="1">
         <v>147.88057038816899</v>
       </c>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-    </row>
-    <row r="4" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="N3" s="1">
+        <f>M3/100</f>
+        <v>1.47880570388169</v>
+      </c>
+      <c r="O3" s="3">
+        <v>1.1932121375402001E-6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -1980,453 +2030,1401 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-      <c r="L4" s="9" t="s">
+      <c r="L4" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="1">
         <v>71.119424158005401</v>
       </c>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N4" s="1">
+        <f t="shared" ref="N4:N7" si="0">M4/100</f>
+        <v>0.71119424158005407</v>
+      </c>
+      <c r="O4" s="3">
+        <v>1.3336969236776901E-6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="B5" s="1">
+        <v>-8.7500862770198903E-2</v>
+      </c>
+      <c r="C5">
+        <v>-8.7501679306362601E-2</v>
+      </c>
+      <c r="D5" s="1">
+        <v>-7.1552944282417097E-2</v>
+      </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
+      <c r="G5" s="1">
+        <f>B5-C5</f>
+        <v>8.1653616369747883E-7</v>
+      </c>
+      <c r="H5" s="1">
+        <f>B5-D5</f>
+        <v>-1.5947918487781806E-2</v>
+      </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
-      <c r="L5" s="9" t="s">
+      <c r="L5" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="1">
         <v>40.903974663241002</v>
       </c>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N5" s="1">
+        <f t="shared" si="0"/>
+        <v>0.40903974663241</v>
+      </c>
+      <c r="O5" s="3">
+        <v>1.3103505847045199E-6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="B6" s="1">
+        <v>-0.226178988779838</v>
+      </c>
+      <c r="D6" s="1">
+        <v>-0.209607457171119</v>
+      </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
+      <c r="H6" s="1">
+        <f>B6-D6</f>
+        <v>-1.6571531608718992E-2</v>
+      </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
-      <c r="L6" s="9" t="s">
+      <c r="L6" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M6" s="1">
+        <v>219</v>
+      </c>
+      <c r="N6" s="1">
+        <f t="shared" si="0"/>
+        <v>2.19</v>
+      </c>
+      <c r="O6" s="3">
+        <v>-1.1280097340638E-6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="B7" s="1">
+        <v>-0.18487578840753599</v>
+      </c>
+      <c r="C7">
+        <v>-0.18484998302695499</v>
+      </c>
+      <c r="D7" s="1">
+        <v>-0.16763503909714</v>
+      </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
+      <c r="G7" s="1">
+        <f>B7-C7</f>
+        <v>-2.5805380581001014E-5</v>
+      </c>
+      <c r="H7" s="1">
+        <f>B7-D7</f>
+        <v>-1.7240749310395986E-2</v>
+      </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
-      <c r="L7" s="9" t="s">
+      <c r="K7" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="L7" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="18">
         <v>62.339801271691996</v>
       </c>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N7" s="18">
+        <f t="shared" si="0"/>
+        <v>0.62339801271691997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>5</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="B8" s="1">
+        <v>-0.15862446742014399</v>
+      </c>
+      <c r="C8">
+        <v>-0.15861267245650701</v>
+      </c>
+      <c r="D8" s="1">
+        <v>-0.141384141319391</v>
+      </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
+      <c r="G8" s="1">
+        <f>B8-C8</f>
+        <v>-1.1794963636985178E-5</v>
+      </c>
+      <c r="H8" s="1">
+        <f>B8-D8</f>
+        <v>-1.724032610075299E-2</v>
+      </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
-      <c r="L8" s="9" t="s">
+      <c r="L8" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="1">
         <v>-0.22617938916486699</v>
       </c>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N8" s="1">
+        <f>M8</f>
+        <v>-0.22617938916486699</v>
+      </c>
+      <c r="O8" s="3">
+        <v>-4.0090743502752002E-7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>6</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="B9" s="1">
+        <v>-0.26468385792833099</v>
+      </c>
+      <c r="C9">
+        <v>-0.264719131577967</v>
+      </c>
+      <c r="E9" s="1">
+        <v>-0.26185691410801698</v>
+      </c>
       <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+      <c r="G9" s="1">
+        <f>B9-C9</f>
+        <v>3.5273649636013982E-5</v>
+      </c>
       <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
+      <c r="I9" s="1">
+        <f>B9-E9</f>
+        <v>-2.8269438203140096E-3</v>
+      </c>
       <c r="J9" s="1"/>
-      <c r="L9" s="9" t="s">
+      <c r="L9" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="M9">
+      <c r="M9" s="1">
         <v>-24.149760653480001</v>
       </c>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N9" s="1">
+        <f>M9/100</f>
+        <v>-0.24149760653480001</v>
+      </c>
+      <c r="O9" s="3">
+        <v>-7.9000820596419896E-7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>7</v>
       </c>
-      <c r="B10" s="1"/>
+      <c r="B10" s="1">
+        <v>-0.245489496582636</v>
+      </c>
       <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="D10" s="1">
+        <v>-0.22735161688810701</v>
+      </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
+      <c r="H10" s="1">
+        <f>B10-D10</f>
+        <v>-1.8137879694528986E-2</v>
+      </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
-      <c r="L10" s="9" t="s">
+      <c r="L10" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="M10">
+      <c r="M10" s="1">
         <v>28.985080382272201</v>
       </c>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N10" s="1">
+        <f t="shared" ref="N10:N11" si="1">M10/100</f>
+        <v>0.28985080382272199</v>
+      </c>
+      <c r="O10" s="3">
+        <v>-5.20655416835769E-7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>8</v>
       </c>
-      <c r="B11" s="1"/>
+      <c r="B11" s="1">
+        <v>-0.245489496582636</v>
+      </c>
       <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+      <c r="D11" s="1">
+        <v>-0.22698927965487201</v>
+      </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
+      <c r="H11" s="1">
+        <f>B11-D11</f>
+        <v>-1.8500216927763991E-2</v>
+      </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" t="s">
-        <v>177</v>
-      </c>
-      <c r="L11" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="L11" s="10" t="s">
         <v>55</v>
       </c>
       <c r="M11" s="1">
         <v>0</v>
       </c>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N11" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O11" s="3">
+        <v>-1.57567843404081E-16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>9</v>
       </c>
-      <c r="B12" s="1"/>
+      <c r="B12" s="1">
+        <v>-0.27737601339101797</v>
+      </c>
       <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+      <c r="D12" s="1">
+        <v>-0.25927308272722099</v>
+      </c>
+      <c r="F12" s="1">
+        <v>-0.26939109597458399</v>
+      </c>
       <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
+      <c r="H12" s="1">
+        <f>B12-D12</f>
+        <v>-1.8102930663796979E-2</v>
+      </c>
       <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="L12" s="9" t="s">
+      <c r="J12" s="1">
+        <f>B12-F12</f>
+        <v>-7.9849174164339787E-3</v>
+      </c>
+      <c r="L12" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="M12">
+      <c r="M12" s="1">
         <v>-0.26468384711479698</v>
       </c>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N12" s="1">
+        <f>M12</f>
+        <v>-0.26468384711479698</v>
+      </c>
+      <c r="O12" s="3">
+        <v>1.28220175033E-8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>10</v>
       </c>
-      <c r="B13" s="1"/>
+      <c r="B13" s="1">
+        <v>-0.28261100297480202</v>
+      </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
+      <c r="F13" s="1">
+        <v>-0.27452348221491601</v>
+      </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="L13" s="9" t="s">
+      <c r="J13" s="1">
+        <f>B13-F13</f>
+        <v>-8.0875207598860022E-3</v>
+      </c>
+      <c r="L13" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="M13">
+      <c r="M13" s="1">
         <v>6.3047604774040904</v>
       </c>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N13" s="1">
+        <f>M13/100</f>
+        <v>6.3047604774040908E-2</v>
+      </c>
+      <c r="O13" s="3">
+        <v>3.3468593840790801E-7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>11</v>
       </c>
-      <c r="B14" s="1"/>
+      <c r="B14" s="1">
+        <v>-0.27722396080129502</v>
+      </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
+      <c r="E14" s="1">
+        <v>-0.274421565294028</v>
+      </c>
+      <c r="F14" s="1">
+        <v>-0.269113560161097</v>
+      </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="L14" s="9" t="s">
+      <c r="I14" s="1">
+        <f>B14-E14</f>
+        <v>-2.8023955072670192E-3</v>
+      </c>
+      <c r="J14" s="1">
+        <f>B14-F14</f>
+        <v>-8.1104006401980233E-3</v>
+      </c>
+      <c r="L14" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="M14">
+      <c r="M14" s="1">
         <v>7.5451451109037899</v>
       </c>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N14" s="1">
+        <f t="shared" ref="N14:N17" si="2">M14/100</f>
+        <v>7.5451451109037893E-2</v>
+      </c>
+      <c r="O14" s="3">
+        <v>3.7929140388193199E-7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>12</v>
       </c>
-      <c r="B15" s="1"/>
+      <c r="B15" s="1">
+        <v>-0.28398499667581101</v>
+      </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
+      <c r="E15" s="1">
+        <v>-0.28108079818493498</v>
+      </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
+      <c r="I15" s="1">
+        <f>B15-E15</f>
+        <v>-2.904198490876031E-3</v>
+      </c>
       <c r="J15" s="1"/>
-      <c r="L15" s="9" t="s">
+      <c r="L15" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="M15">
+      <c r="M15" s="1">
         <v>17.033691859918299</v>
       </c>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N15" s="1">
+        <f t="shared" si="2"/>
+        <v>0.17033691859918298</v>
+      </c>
+      <c r="O15" s="3">
+        <v>5.6078568202999602E-7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>13</v>
       </c>
-      <c r="B16" s="1"/>
+      <c r="B16" s="1">
+        <v>-0.286873575508024</v>
+      </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
+      <c r="E16" s="1">
+        <v>-0.284035212391686</v>
+      </c>
+      <c r="F16" s="1">
+        <v>-0.27843212378369597</v>
+      </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="L16" s="9" t="s">
+      <c r="I16" s="1">
+        <f>B16-E16</f>
+        <v>-2.8383631163380052E-3</v>
+      </c>
+      <c r="J16" s="1">
+        <f>B16-F16</f>
+        <v>-8.4414517243280307E-3</v>
+      </c>
+      <c r="L16" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="M16">
+      <c r="M16" s="1">
         <v>1.44514504235841</v>
       </c>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
+      <c r="N16" s="1">
+        <f t="shared" si="2"/>
+        <v>1.4451450423584099E-2</v>
+      </c>
+      <c r="O16" s="3">
+        <v>-1.14592771794167E-7</v>
+      </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>14</v>
       </c>
-      <c r="B17" s="1"/>
+      <c r="B17" s="1">
+        <v>-0.30420089313857501</v>
+      </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
+      <c r="E17" s="1">
+        <v>-0.30137834758413701</v>
+      </c>
+      <c r="F17" s="1">
+        <v>-0.29607073439730403</v>
+      </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="L17" s="9" t="s">
+      <c r="I17" s="1">
+        <f>B17-F17</f>
+        <v>-8.1301587412709875E-3</v>
+      </c>
+      <c r="J17" s="1">
+        <f>B17-F17</f>
+        <v>-8.1301587412709875E-3</v>
+      </c>
+      <c r="L17" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="1"/>
+      <c r="M17" s="1">
+        <v>-6.1</v>
+      </c>
+      <c r="N17" s="1">
+        <f t="shared" si="2"/>
+        <v>-6.0999999999999999E-2</v>
+      </c>
+      <c r="O17" s="3">
+        <v>4.5183513249641401E-7</v>
+      </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="L18" s="9" t="s">
+      <c r="L18" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="M18">
+      <c r="M18" s="1">
         <v>-0.27737614157951601</v>
       </c>
-      <c r="N18" s="1"/>
-      <c r="O18" s="1"/>
+      <c r="N18" s="1">
+        <f>M18</f>
+        <v>-0.27737614157951601</v>
+      </c>
+      <c r="O18" s="3">
+        <v>-1.2842617186370499E-7</v>
+      </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I19" t="s">
-        <v>175</v>
-      </c>
-      <c r="L19" s="9" t="s">
+      <c r="L19" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="M19">
+      <c r="M19" s="1">
         <v>6.1952398951249403</v>
       </c>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
+      <c r="N19" s="1">
+        <f>M19/100</f>
+        <v>6.1952398951249404E-2</v>
+      </c>
+      <c r="O19" s="3">
+        <v>-1.42186835874747E-7</v>
+      </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I20" t="s">
-        <v>176</v>
-      </c>
-      <c r="L20" s="9" t="s">
+      <c r="L20" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="M20">
+      <c r="M20" s="1">
         <v>9.9211640275555908</v>
       </c>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
+      <c r="N20" s="1">
+        <f t="shared" ref="N20:N25" si="3">M20/100</f>
+        <v>9.9211640275555901E-2</v>
+      </c>
+      <c r="O20" s="3">
+        <v>-1.3748886061593101E-7</v>
+      </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I21">
+      <c r="L21" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="M21" s="1">
+        <v>-7.6</v>
+      </c>
+      <c r="N21" s="1">
+        <f t="shared" si="3"/>
+        <v>-7.5999999999999998E-2</v>
+      </c>
+      <c r="O21" s="3">
+        <v>6.4740440693100698E-7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L22" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="M22" s="1">
+        <v>-62.339801271691996</v>
+      </c>
+      <c r="N22" s="1">
+        <f t="shared" si="3"/>
+        <v>-0.62339801271691997</v>
+      </c>
+      <c r="O22" s="3">
+        <v>7.3348635232228798E-7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L23" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="M23" s="1">
+        <v>16.6313222291061</v>
+      </c>
+      <c r="N23" s="1">
+        <f t="shared" si="3"/>
+        <v>0.16631322229106099</v>
+      </c>
+      <c r="O23" s="3">
+        <v>-2.4862348460552601E-7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L24" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="M24" s="1">
+        <v>28.985080382272098</v>
+      </c>
+      <c r="N24" s="1">
+        <f t="shared" si="3"/>
+        <v>0.28985080382272099</v>
+      </c>
+      <c r="O24" s="3">
+        <v>-2.7389681767076002E-7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L25" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="M25" s="1">
+        <v>-94.2</v>
+      </c>
+      <c r="N25" s="1">
+        <f t="shared" si="3"/>
+        <v>-0.94200000000000006</v>
+      </c>
+      <c r="O25" s="3">
+        <v>4.97415676092849E-7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L26" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="M26" s="1">
+        <v>-0.22617938916486699</v>
+      </c>
+      <c r="N26" s="1">
+        <f>M26</f>
+        <v>-0.22617938916486699</v>
+      </c>
+      <c r="O26" s="3">
+        <v>-4.0090743502752002E-7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L27" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="M27" s="1">
+        <v>4.9788363658350603</v>
+      </c>
+      <c r="N27" s="1">
+        <f>M27/100</f>
+        <v>4.9788363658350605E-2</v>
+      </c>
+      <c r="O27" s="3">
+        <v>8.5266968763431095E-8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L28" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="M28" s="1">
+        <v>-13.5</v>
+      </c>
+      <c r="N28" s="1">
+        <f>M28/100</f>
+        <v>-0.13500000000000001</v>
+      </c>
+      <c r="O28" s="3">
+        <v>3.93929590863928E-7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L29" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="M29" s="1">
+        <v>-0.26468384711479698</v>
+      </c>
+      <c r="N29" s="1">
+        <f>M29</f>
+        <v>-0.26468384711479698</v>
+      </c>
+      <c r="O29" s="3">
+        <v>1.28220175033E-8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L30" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="M30" s="1">
         <v>-2.8047604625028999</v>
       </c>
-      <c r="L21" s="9" t="s">
+      <c r="N30" s="1">
+        <f>M30/100</f>
+        <v>-2.8047604625028998E-2</v>
+      </c>
+      <c r="O30" s="3">
+        <v>-3.2319320363363702E-7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L31" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="M31" s="1">
+        <v>-14.9</v>
+      </c>
+      <c r="N31" s="1">
+        <f>M31/100</f>
+        <v>-0.14899999999999999</v>
+      </c>
+      <c r="O31" s="3">
+        <v>1.32141526387741E-7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L32" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="M32" s="1">
+        <v>-0.27737614157951601</v>
+      </c>
+      <c r="N32" s="1">
+        <f>M32</f>
+        <v>-0.27737614157951601</v>
+      </c>
+      <c r="O32" s="3">
+        <v>-1.2842617186370499E-7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O33" s="1"/>
+    </row>
+    <row r="35" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="B35" s="13"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="13"/>
+      <c r="L35" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="M35" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="N35" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="O35" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="H36" s="11"/>
+      <c r="I36" s="11"/>
+      <c r="J36" s="11"/>
+      <c r="L36" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="M36" s="1">
+        <v>147.88057038816899</v>
+      </c>
+      <c r="N36" s="1">
+        <f>M36/100</f>
+        <v>1.47880570388169</v>
+      </c>
+      <c r="O36" s="20">
+        <v>1.1932028856076501E-6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="14"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D37" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E37" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F37" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="G37" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H37" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="I37" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="J37" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="L37" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="M37" s="1">
+        <v>71.119424158005401</v>
+      </c>
+      <c r="N37" s="1">
+        <f t="shared" ref="N37:N39" si="4">M37/100</f>
+        <v>0.71119424158005407</v>
+      </c>
+      <c r="O37" s="3">
+        <v>1.37286101276057E-6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>1</v>
+      </c>
+      <c r="B38" s="1">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="L38" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="M38" s="1">
+        <v>40.903974663241002</v>
+      </c>
+      <c r="N38" s="1">
+        <f t="shared" si="4"/>
+        <v>0.40903974663241</v>
+      </c>
+      <c r="O38" s="3">
+        <v>1.3605904390368001E-6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>2</v>
+      </c>
+      <c r="B39" s="1">
+        <v>-8.7500862781776406E-2</v>
+      </c>
+      <c r="C39" s="1">
+        <v>-8.7508936150494002E-2</v>
+      </c>
+      <c r="D39" s="1">
+        <v>6.1810561579258398E-2</v>
+      </c>
+      <c r="G39" s="1">
+        <f>B39-C39</f>
+        <v>8.0733687175954527E-6</v>
+      </c>
+      <c r="H39" s="1">
+        <f>B39-D39</f>
+        <v>-0.14931142436103481</v>
+      </c>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+      <c r="L39" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="M39" s="1">
+        <v>219</v>
+      </c>
+      <c r="N39" s="1">
+        <f t="shared" si="4"/>
+        <v>2.19</v>
+      </c>
+      <c r="O39" s="3">
+        <v>-1.08885490313071E-6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>3</v>
+      </c>
+      <c r="B40" s="1">
+        <v>-0.22617897691258701</v>
+      </c>
+      <c r="D40" s="1">
+        <v>-7.6495960726050902E-2</v>
+      </c>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+      <c r="L40" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="M40" s="1">
+        <v>-24.149760653480001</v>
+      </c>
+      <c r="N40" s="1">
+        <f>M40/100</f>
+        <v>-0.24149760653480001</v>
+      </c>
+      <c r="O40" s="3">
+        <v>-7.99245762184153E-7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>4</v>
+      </c>
+      <c r="B41" s="1">
+        <v>-0.18487577807552</v>
+      </c>
+      <c r="C41" s="1">
+        <v>-0.22584681376426499</v>
+      </c>
+      <c r="D41" s="1">
+        <v>-3.4959843053773497E-2</v>
+      </c>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="L41" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="M41" s="1">
+        <v>28.985080382272201</v>
+      </c>
+      <c r="N41" s="1">
+        <f t="shared" ref="N41:N42" si="5">M41/100</f>
+        <v>0.28985080382272199</v>
+      </c>
+      <c r="O41" s="3">
+        <v>-4.7651516216218299E-7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>5</v>
+      </c>
+      <c r="B42" s="1">
+        <v>-0.158624458532023</v>
+      </c>
+      <c r="C42" s="1">
+        <v>-0.15845173951557601</v>
+      </c>
+      <c r="D42" s="1">
+        <v>-8.7151391052258404E-3</v>
+      </c>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="L42" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="M42" s="1">
+        <v>0</v>
+      </c>
+      <c r="N42" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O42" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>6</v>
+      </c>
+      <c r="B43" s="1">
+        <v>-0.26468383586175498</v>
+      </c>
+      <c r="C43" s="1">
+        <v>-1.7763990657028699E-2</v>
+      </c>
+      <c r="E43" s="1">
+        <v>1.3950959767079701E-2</v>
+      </c>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+      <c r="L43" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="M43" s="1">
+        <v>6.3047604774040904</v>
+      </c>
+      <c r="N43" s="1">
+        <f>M43/100</f>
+        <v>6.3047604774040908E-2</v>
+      </c>
+      <c r="O43" s="3">
+        <v>3.3575807029118099E-7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>7</v>
+      </c>
+      <c r="B44" s="1">
+        <v>-0.24548947685952399</v>
+      </c>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1">
+        <v>-9.5109598575578394E-2</v>
+      </c>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
+      <c r="L44" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="M44" s="1">
+        <v>7.5451451109037899</v>
+      </c>
+      <c r="N44" s="1">
+        <f t="shared" ref="N44:N47" si="6">M44/100</f>
+        <v>7.5451451109037893E-2</v>
+      </c>
+      <c r="O44" s="3">
+        <v>3.7938750536980999E-7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>8</v>
+      </c>
+      <c r="B45" s="1">
+        <v>-0.24548947685952399</v>
+      </c>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1">
+        <v>-9.4963573066871101E-2</v>
+      </c>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
+      <c r="L45" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="M45" s="1">
+        <v>17.033691859918299</v>
+      </c>
+      <c r="N45" s="1">
+        <f t="shared" si="6"/>
+        <v>0.17033691859918298</v>
+      </c>
+      <c r="O45" s="3">
+        <v>5.6117956662160605E-7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>9</v>
+      </c>
+      <c r="B46" s="1">
+        <v>-0.27737599107252198</v>
+      </c>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1">
+        <v>-0.126981901136799</v>
+      </c>
+      <c r="F46" s="1">
+        <v>-2.07652454529514E-2</v>
+      </c>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1"/>
+      <c r="L46" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="M46" s="1">
+        <v>1.44514504235841</v>
+      </c>
+      <c r="N46" s="1">
+        <f t="shared" si="6"/>
+        <v>1.4451450423584099E-2</v>
+      </c>
+      <c r="O46" s="3">
+        <v>-1.1445905346262099E-7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>10</v>
+      </c>
+      <c r="B47" s="1">
+        <v>-0.28261098067782497</v>
+      </c>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="F47" s="1">
+        <v>-2.59880093040946E-2</v>
+      </c>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+      <c r="L47" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="M47" s="1">
+        <v>-6.1</v>
+      </c>
+      <c r="N47" s="1">
+        <f t="shared" si="6"/>
+        <v>-6.0999999999999999E-2</v>
+      </c>
+      <c r="O47" s="3">
+        <v>4.51872748087612E-7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>11</v>
+      </c>
+      <c r="B48" s="1">
+        <v>-0.27722393861549399</v>
+      </c>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1">
+        <v>1.3876920270285201E-3</v>
+      </c>
+      <c r="F48" s="1">
+        <v>-2.05793495576241E-2</v>
+      </c>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1"/>
+      <c r="L48" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="M48" s="1">
+        <v>6.1952398951249403</v>
+      </c>
+      <c r="N48" s="1">
+        <f>M48/100</f>
+        <v>6.1952398951249404E-2</v>
+      </c>
+      <c r="O48" s="3">
+        <v>-1.4264231767979799E-7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>12</v>
+      </c>
+      <c r="B49" s="1">
+        <v>-0.28398497459549199</v>
+      </c>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1">
+        <v>-5.2806221153084204E-3</v>
+      </c>
+      <c r="F49" s="1">
+        <v>-3.0095200429465899E-2</v>
+      </c>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1"/>
+      <c r="L49" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="M49" s="1">
+        <v>9.9211640275555908</v>
+      </c>
+      <c r="N49" s="1">
+        <f t="shared" ref="N49:N54" si="7">M49/100</f>
+        <v>9.9211640275555901E-2</v>
+      </c>
+      <c r="O49" s="3">
+        <v>-1.38124769413772E-7</v>
+      </c>
+      <c r="P49" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>13</v>
+      </c>
+      <c r="B50" s="1">
+        <v>-0.28687355341276</v>
+      </c>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1">
+        <v>-8.1835881362442801E-3</v>
+      </c>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+      <c r="J50" s="1"/>
+      <c r="L50" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="L22" s="9" t="s">
+      <c r="M50" s="1">
+        <v>-7.6</v>
+      </c>
+      <c r="N50" s="1">
+        <f t="shared" si="7"/>
+        <v>-7.5999999999999998E-2</v>
+      </c>
+      <c r="O50" s="3">
+        <v>6.4287659591599798E-7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>14</v>
+      </c>
+      <c r="B51" s="1">
+        <v>-0.30420087091620301</v>
+      </c>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1">
+        <v>-2.5676651572644999E-2</v>
+      </c>
+      <c r="F51" s="1">
+        <v>-4.7499811323096497E-2</v>
+      </c>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+      <c r="J51" s="1"/>
+      <c r="L51" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="M22">
+      <c r="M51" s="1">
         <v>-62.339801271691996</v>
       </c>
-      <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="L23" s="9" t="s">
+      <c r="N51" s="1">
+        <f t="shared" si="7"/>
+        <v>-0.62339801271691997</v>
+      </c>
+      <c r="O51" s="3">
+        <v>6.9929696500103902E-7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L52" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="M23">
+      <c r="M52" s="1">
         <v>16.6313222291061</v>
       </c>
-      <c r="N23" s="1"/>
-      <c r="O23" s="1"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="L24" s="9" t="s">
+      <c r="N52" s="1">
+        <f t="shared" si="7"/>
+        <v>0.16631322229106099</v>
+      </c>
+      <c r="O52" s="3">
+        <v>-2.27434127780812E-7</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L53" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="M24">
+      <c r="M53" s="1">
         <v>28.985080382272098</v>
       </c>
-      <c r="N24" s="1"/>
-      <c r="O24" s="1"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="L25" s="9" t="s">
+      <c r="N53" s="1">
+        <f t="shared" si="7"/>
+        <v>0.28985080382272099</v>
+      </c>
+      <c r="O53" s="3">
+        <v>-2.5067632475339602E-7</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L54" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
-      <c r="O25" s="1"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="L26" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="M26">
-        <v>-0.22617938916486699</v>
-      </c>
-      <c r="N26" s="1"/>
-      <c r="O26" s="1"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="L27" s="9" t="s">
+      <c r="M54" s="1">
+        <v>-94.2</v>
+      </c>
+      <c r="N54" s="1">
+        <f t="shared" si="7"/>
+        <v>-0.94200000000000006</v>
+      </c>
+      <c r="O54" s="3">
+        <v>4.2879851425148301E-7</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L55" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="M27">
+      <c r="M55" s="1">
         <v>4.9788363658350603</v>
       </c>
-      <c r="N27" s="1"/>
-      <c r="O27" s="1"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="L28" s="9" t="s">
+      <c r="N55" s="1">
+        <f>M55/100</f>
+        <v>4.9788363658350605E-2</v>
+      </c>
+      <c r="O55" s="3">
+        <v>8.5920207504308595E-8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L56" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="M28" s="1"/>
-      <c r="N28" s="1"/>
-      <c r="O28" s="1"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="L29" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="M29">
-        <v>-0.26468384711479698</v>
-      </c>
-      <c r="N29" s="1"/>
-      <c r="O29" s="1"/>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="L30" s="9" t="s">
+      <c r="M56" s="1">
+        <v>-13.5</v>
+      </c>
+      <c r="N56" s="1">
+        <f>M56/100</f>
+        <v>-0.13500000000000001</v>
+      </c>
+      <c r="O56" s="3">
+        <v>3.9405522533897402E-7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L57" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="M30">
+      <c r="M57" s="1">
         <v>-2.8047604625028999</v>
       </c>
-      <c r="N30" s="1"/>
-      <c r="O30" s="1"/>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="L31" s="9" t="s">
+      <c r="N57" s="1">
+        <f>M57/100</f>
+        <v>-2.8047604625028998E-2</v>
+      </c>
+      <c r="O57" s="3">
+        <v>-3.2422852027508302E-7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L58" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="M31" s="1"/>
-      <c r="N31" s="1"/>
-      <c r="O31" s="1"/>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="L32" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="M32">
-        <v>-0.27737614157951601</v>
-      </c>
-      <c r="N32" s="1"/>
-      <c r="O32" s="1"/>
+      <c r="M58" s="1">
+        <v>-14.9</v>
+      </c>
+      <c r="N58" s="1">
+        <f>M58/100</f>
+        <v>-0.14899999999999999</v>
+      </c>
+      <c r="O58" s="3">
+        <v>1.3212419627817199E-7</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O59" s="3"/>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O60" s="3"/>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O61" s="3"/>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O62" s="3"/>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O63" s="3"/>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O64" s="3"/>
+    </row>
+    <row r="65" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O65" s="3"/>
+    </row>
+    <row r="66" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O66" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
+    <mergeCell ref="A35:J35"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="G2:J2"/>
@@ -2441,7 +3439,7 @@
   <dimension ref="A1:P32"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2513,7 +3511,7 @@
       <c r="B3" t="s">
         <v>93</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="16" t="s">
         <v>94</v>
       </c>
       <c r="D3" t="s">
@@ -2947,7 +3945,7 @@
       <c r="I26" t="s">
         <v>157</v>
       </c>
-      <c r="J26" s="15" t="s">
+      <c r="J26" s="16" t="s">
         <v>163</v>
       </c>
     </row>
@@ -2964,7 +3962,7 @@
       <c r="I27" t="s">
         <v>159</v>
       </c>
-      <c r="K27" s="15" t="s">
+      <c r="K27" s="16" t="s">
         <v>164</v>
       </c>
       <c r="L27" t="s">
@@ -2984,7 +3982,7 @@
       <c r="K28" t="s">
         <v>165</v>
       </c>
-      <c r="L28" s="15" t="s">
+      <c r="L28" s="16" t="s">
         <v>167</v>
       </c>
       <c r="M28" t="s">
@@ -3004,7 +4002,7 @@
       <c r="L29" t="s">
         <v>168</v>
       </c>
-      <c r="M29" s="15" t="s">
+      <c r="M29" s="16" t="s">
         <v>169</v>
       </c>
     </row>
@@ -3018,7 +4016,7 @@
       <c r="H30" t="s">
         <v>161</v>
       </c>
-      <c r="N30" s="15" t="s">
+      <c r="N30" s="16" t="s">
         <v>170</v>
       </c>
       <c r="O30" t="s">
@@ -3038,7 +4036,7 @@
       <c r="N31" t="s">
         <v>171</v>
       </c>
-      <c r="O31" s="15" t="s">
+      <c r="O31" s="16" t="s">
         <v>172</v>
       </c>
       <c r="P31" t="s">
@@ -3058,7 +4056,7 @@
       <c r="O32" t="s">
         <v>173</v>
       </c>
-      <c r="P32" s="15" t="s">
+      <c r="P32" s="16" t="s">
         <v>174</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Tried adding line 2-3 measurements for 3 bus case
Tried to add in P2-3 and Q2-3 measurements to see if ADMM state vector
error for V3 would go away (it didn't, seemed to get worse/become
oscillatory). Also moved some old files to "old files" folder.
</commit_message>
<xml_diff>
--- a/DMASE - Test Results.xlsx
+++ b/DMASE - Test Results.xlsx
@@ -4,19 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="18195" windowHeight="7740" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="18195" windowHeight="7740"/>
   </bookViews>
   <sheets>
     <sheet name="3 Bus" sheetId="1" r:id="rId1"/>
     <sheet name="14 Bus DC" sheetId="2" r:id="rId2"/>
-    <sheet name="14 Ybus noRnoC" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="83">
   <si>
     <t>Abur 3-Bus Case Measurements (run through SE, rerun new estimate again)</t>
   </si>
@@ -246,303 +245,6 @@
     <t>Central - Decentral</t>
   </si>
   <si>
-    <t>YBus Records</t>
-  </si>
-  <si>
-    <t>Number</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Bus     1</t>
-  </si>
-  <si>
-    <t>Bus     2</t>
-  </si>
-  <si>
-    <t>Bus     3</t>
-  </si>
-  <si>
-    <t>Bus     4</t>
-  </si>
-  <si>
-    <t>Bus     5</t>
-  </si>
-  <si>
-    <t>Bus     6</t>
-  </si>
-  <si>
-    <t>Bus     7</t>
-  </si>
-  <si>
-    <t>Bus     8</t>
-  </si>
-  <si>
-    <t>Bus     9</t>
-  </si>
-  <si>
-    <t>Bus    10</t>
-  </si>
-  <si>
-    <t>Bus    11</t>
-  </si>
-  <si>
-    <t>Bus    12</t>
-  </si>
-  <si>
-    <t>Bus    13</t>
-  </si>
-  <si>
-    <t>Bus    14</t>
-  </si>
-  <si>
-    <t>Bus 1</t>
-  </si>
-  <si>
-    <t>0.00 - j21.38</t>
-  </si>
-  <si>
-    <t>Bus 2</t>
-  </si>
-  <si>
-    <t>0.00 - j33.37</t>
-  </si>
-  <si>
-    <t>Bus 3</t>
-  </si>
-  <si>
-    <t>0.00 - j10.90</t>
-  </si>
-  <si>
-    <t>Bus 4</t>
-  </si>
-  <si>
-    <t>0.00 - j41.85</t>
-  </si>
-  <si>
-    <t>Bus 5</t>
-  </si>
-  <si>
-    <t>0.00 - j37.95</t>
-  </si>
-  <si>
-    <t>Bus 6</t>
-  </si>
-  <si>
-    <t>0.00 - j20.58</t>
-  </si>
-  <si>
-    <t>Bus 7</t>
-  </si>
-  <si>
-    <t>0.00 - j19.55</t>
-  </si>
-  <si>
-    <t>Bus 8</t>
-  </si>
-  <si>
-    <t>0.00 - j5.68</t>
-  </si>
-  <si>
-    <t>Bus 9</t>
-  </si>
-  <si>
-    <t>0.00 - j26.23</t>
-  </si>
-  <si>
-    <t>Bus 10</t>
-  </si>
-  <si>
-    <t>0.00 - j17.04</t>
-  </si>
-  <si>
-    <t>Bus 11</t>
-  </si>
-  <si>
-    <t>0.00 - j10.23</t>
-  </si>
-  <si>
-    <t>Bus 12</t>
-  </si>
-  <si>
-    <t>0.00 - j8.91</t>
-  </si>
-  <si>
-    <t>Bus 13</t>
-  </si>
-  <si>
-    <t>0.00 - j15.55</t>
-  </si>
-  <si>
-    <t>Bus 14</t>
-  </si>
-  <si>
-    <t>0.00 - j6.57</t>
-  </si>
-  <si>
-    <t>0 + j16.90</t>
-  </si>
-  <si>
-    <t>0 + j5.05</t>
-  </si>
-  <si>
-    <t>0 + j5.67</t>
-  </si>
-  <si>
-    <t>0 + j5.75</t>
-  </si>
-  <si>
-    <t>0 + j4.48</t>
-  </si>
-  <si>
-    <t>0 + j5.85</t>
-  </si>
-  <si>
-    <t>0 + j23.75</t>
-  </si>
-  <si>
-    <t>0 + j4.78</t>
-  </si>
-  <si>
-    <t>0 + j1.80</t>
-  </si>
-  <si>
-    <t>0 + j3.97</t>
-  </si>
-  <si>
-    <t>0 + j5.03</t>
-  </si>
-  <si>
-    <t>0 + j3.91</t>
-  </si>
-  <si>
-    <t>0 + j7.68</t>
-  </si>
-  <si>
-    <t>0 + j5.68</t>
-  </si>
-  <si>
-    <t>0 + j9.09</t>
-  </si>
-  <si>
-    <t>0 + j11.83</t>
-  </si>
-  <si>
-    <t>0 + j3.70</t>
-  </si>
-  <si>
-    <t>0 + j5.21</t>
-  </si>
-  <si>
-    <t>0 + j5.00</t>
-  </si>
-  <si>
-    <t>0 + j2.87</t>
-  </si>
-  <si>
-    <t>-21.3839570296806i</t>
-  </si>
-  <si>
-    <t>16.9004563123204i</t>
-  </si>
-  <si>
-    <t>4.48350071736012i</t>
-  </si>
-  <si>
-    <t>-33.3743257665262i</t>
-  </si>
-  <si>
-    <t>5.05127039450422i</t>
-  </si>
-  <si>
-    <t>5.67150635208711i</t>
-  </si>
-  <si>
-    <t>5.75109270761445i</t>
-  </si>
-  <si>
-    <t>-10.8981978341347i</t>
-  </si>
-  <si>
-    <t>5.84692743963047i</t>
-  </si>
-  <si>
-    <t>-41.8456846705837i</t>
-  </si>
-  <si>
-    <t>23.7473284255521i</t>
-  </si>
-  <si>
-    <t>4.78194338179036i</t>
-  </si>
-  <si>
-    <t>-37.9498609029828i</t>
-  </si>
-  <si>
-    <t>3.96793905245615i</t>
-  </si>
-  <si>
-    <t>-20.5811069359647i</t>
-  </si>
-  <si>
-    <t>-19.5490059482647i</t>
-  </si>
-  <si>
-    <t>5.67697984672154i</t>
-  </si>
-  <si>
-    <t>1.79797907152361i</t>
-  </si>
-  <si>
-    <t>9.09008271975275i</t>
-  </si>
-  <si>
-    <t>5.02765208647562i</t>
-  </si>
-  <si>
-    <t>3.90915132324772i</t>
-  </si>
-  <si>
-    <t>7.67636447378522i</t>
-  </si>
-  <si>
-    <t>-5.67697984672154i</t>
-  </si>
-  <si>
-    <t>-26.4208797275493i</t>
-  </si>
-  <si>
-    <t>11.8343195266272i</t>
-  </si>
-  <si>
-    <t>3.69849840964568i</t>
-  </si>
-  <si>
-    <t>-17.0407546804774i</t>
-  </si>
-  <si>
-    <t>5.20643515385016i</t>
-  </si>
-  <si>
-    <t>-10.2340872403258i</t>
-  </si>
-  <si>
-    <t>-8.91215312432837i</t>
-  </si>
-  <si>
-    <t>5.00300180108065i</t>
-  </si>
-  <si>
-    <t>-15.5527643554359i</t>
-  </si>
-  <si>
-    <t>2.87339808057008i</t>
-  </si>
-  <si>
-    <t>-6.57189649021577i</t>
-  </si>
-  <si>
     <t>something wrong with the way that Pto-from is calculated</t>
   </si>
   <si>
@@ -556,13 +258,22 @@
   </si>
   <si>
     <t>Created large res</t>
+  </si>
+  <si>
+    <t>P23</t>
+  </si>
+  <si>
+    <t>Q23</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000000000000000"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -599,6 +310,23 @@
       <strike/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1" tint="0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -659,7 +387,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -681,19 +409,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -702,19 +418,44 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1016,10 +757,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N36"/>
+  <dimension ref="A1:N46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="K41" sqref="K41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1029,20 +770,21 @@
     <col min="3" max="3" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
+      <c r="A1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
       <c r="I1" s="6" t="s">
         <v>1</v>
       </c>
@@ -1076,7 +818,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="8" t="s">
         <v>12</v>
       </c>
       <c r="J2" s="1">
@@ -1113,7 +855,7 @@
       <c r="G3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="8" t="s">
         <v>16</v>
       </c>
       <c r="J3" s="1">
@@ -1154,7 +896,7 @@
       <c r="G4" s="1">
         <v>0</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="I4" s="8" t="s">
         <v>18</v>
       </c>
       <c r="J4" s="1">
@@ -1195,7 +937,7 @@
       <c r="G5" s="1">
         <v>-1.2903313789999999E-7</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="I5" s="8" t="s">
         <v>20</v>
       </c>
       <c r="J5" s="1">
@@ -1236,7 +978,7 @@
       <c r="G6" s="1">
         <v>5.8433450400000004E-6</v>
       </c>
-      <c r="I6" s="10" t="s">
+      <c r="I6" s="8" t="s">
         <v>22</v>
       </c>
       <c r="J6" s="1">
@@ -1277,7 +1019,7 @@
       <c r="G7" s="1">
         <v>-2.10700941E-7</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="I7" s="8" t="s">
         <v>24</v>
       </c>
       <c r="J7" s="1">
@@ -1318,7 +1060,7 @@
       <c r="G8" s="1">
         <v>-8.7038090069999994E-9</v>
       </c>
-      <c r="I8" s="10" t="s">
+      <c r="I8" s="8" t="s">
         <v>26</v>
       </c>
       <c r="J8" s="1">
@@ -1359,7 +1101,7 @@
       <c r="G9" s="1">
         <v>3.2929260540000001E-6</v>
       </c>
-      <c r="I9" s="10" t="s">
+      <c r="I9" s="8" t="s">
         <v>28</v>
       </c>
       <c r="J9" s="1">
@@ -1395,15 +1137,15 @@
       <c r="N11" s="1"/>
     </row>
     <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
       <c r="I12" s="1"/>
       <c r="J12" s="6" t="s">
         <v>1</v>
@@ -1436,11 +1178,12 @@
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="I13" s="1"/>
-      <c r="J13" s="10" t="s">
+      <c r="J13" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="K13" s="1">
-        <v>0.48639810389999999</v>
+      <c r="K13" s="20">
+        <f>48.6441515966896/100</f>
+        <v>0.48644151596689605</v>
       </c>
       <c r="L13" s="1">
         <v>0.48125000969999998</v>
@@ -1471,11 +1214,12 @@
         <v>11</v>
       </c>
       <c r="I14" s="1"/>
-      <c r="J14" s="10" t="s">
+      <c r="J14" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="K14" s="1">
-        <v>0.41971020710000001</v>
+      <c r="K14" s="21">
+        <f>41.9683612159875/100</f>
+        <v>0.41968361215987499</v>
       </c>
       <c r="L14" s="1">
         <v>0.41874999619999997</v>
@@ -1510,10 +1254,11 @@
         <v>0</v>
       </c>
       <c r="I15" s="1"/>
-      <c r="J15" s="10" t="s">
+      <c r="J15" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="K15" s="1">
+      <c r="K15" s="20">
+        <f>-40/100</f>
         <v>-0.4</v>
       </c>
       <c r="L15" s="1">
@@ -1531,7 +1276,7 @@
         <v>19</v>
       </c>
       <c r="B16" s="1">
-        <v>-1.452558461E-2</v>
+        <v>-1.45245088402107E-2</v>
       </c>
       <c r="C16" s="1">
         <v>-1.453480387E-2</v>
@@ -1549,11 +1294,12 @@
         <v>-3.4400000000000003E-5</v>
       </c>
       <c r="I16" s="1"/>
-      <c r="J16" s="10" t="s">
+      <c r="J16" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K16" s="1">
-        <v>1.411757607E-2</v>
+      <c r="K16" s="21">
+        <f>1.44776824615491/100</f>
+        <v>1.44776824615491E-2</v>
       </c>
       <c r="L16" s="1">
         <v>0</v>
@@ -1570,7 +1316,7 @@
         <v>21</v>
       </c>
       <c r="B17" s="1">
-        <v>-2.1120212230000001E-2</v>
+        <v>-2.1118662608655699E-2</v>
       </c>
       <c r="C17" s="1">
         <v>-2.1131558979999999E-2</v>
@@ -1588,11 +1334,12 @@
         <v>2.7900000000000001E-2</v>
       </c>
       <c r="I17" s="1"/>
-      <c r="J17" s="10" t="s">
+      <c r="J17" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="K17" s="1">
-        <v>2.1200096990000002E-3</v>
+      <c r="K17" s="21">
+        <f>0.209417870761202/100</f>
+        <v>2.0941787076120201E-3</v>
       </c>
       <c r="L17" s="1">
         <v>0</v>
@@ -1609,7 +1356,7 @@
         <v>23</v>
       </c>
       <c r="B18" s="1">
-        <v>1.0000014189999999</v>
+        <v>0.999998359536033</v>
       </c>
       <c r="C18" s="1">
         <v>0.99971783469999997</v>
@@ -1627,10 +1374,10 @@
         <v>-1.14E-3</v>
       </c>
       <c r="I18" s="1"/>
-      <c r="J18" s="10" t="s">
+      <c r="J18" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="K18" s="1">
+      <c r="K18" s="20">
         <v>0</v>
       </c>
       <c r="L18" s="1">
@@ -1648,7 +1395,7 @@
         <v>25</v>
       </c>
       <c r="B19" s="1">
-        <v>0.99481623050000001</v>
+        <v>0.99480759668265895</v>
       </c>
       <c r="C19" s="1">
         <v>0.99453388529999998</v>
@@ -1666,10 +1413,10 @@
         <v>-1.15E-3</v>
       </c>
       <c r="I19" s="1"/>
-      <c r="J19" s="10" t="s">
+      <c r="J19" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="K19" s="1">
+      <c r="K19" s="20">
         <v>1</v>
       </c>
       <c r="L19" s="1">
@@ -1687,15 +1434,15 @@
         <v>27</v>
       </c>
       <c r="B20" s="1">
-        <v>0.99172445330000003</v>
+        <v>0.99171870097681902</v>
       </c>
       <c r="C20" s="1">
         <v>0.99143333180000004</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20" s="19">
         <v>-2.6933805729999998</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E20" s="23">
         <v>3.6848139049999999</v>
       </c>
       <c r="F20" s="3">
@@ -1705,11 +1452,11 @@
         <v>3.69</v>
       </c>
       <c r="I20" s="1"/>
-      <c r="J20" s="10" t="s">
+      <c r="J20" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="K20" s="1">
-        <v>0.99481745359999996</v>
+      <c r="K20" s="21">
+        <v>0.99480618409400001</v>
       </c>
       <c r="L20" s="1">
         <v>1</v>
@@ -1869,27 +1616,394 @@
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+    </row>
+    <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" s="16"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="16"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K32" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L32" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="M32" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="N32" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="K33" s="20">
+        <f>48.6441515966896/100</f>
+        <v>0.48644151596689605</v>
+      </c>
+      <c r="L33" s="1">
+        <v>0.48125000969999998</v>
+      </c>
+      <c r="M33" s="3">
+        <v>2.5799999999999999E-6</v>
+      </c>
+      <c r="N33" s="3">
+        <v>5.62E-9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="6"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I34" s="1"/>
+      <c r="J34" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="K34" s="21">
+        <f>41.9683612159875/100</f>
+        <v>0.41968361215987499</v>
+      </c>
+      <c r="L34" s="1">
+        <v>0.41874999619999997</v>
+      </c>
+      <c r="M34" s="3">
+        <v>-4.0200000000000003E-7</v>
+      </c>
+      <c r="N34" s="3">
+        <v>-2.5500000000000001E-9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35" s="1">
+        <v>0</v>
+      </c>
+      <c r="C35" s="1">
+        <v>0</v>
+      </c>
+      <c r="D35" s="1">
+        <v>0</v>
+      </c>
+      <c r="E35" s="1">
+        <v>0</v>
+      </c>
+      <c r="F35" s="1">
+        <v>0</v>
+      </c>
+      <c r="G35" s="1">
+        <v>0</v>
+      </c>
+      <c r="I35" s="1"/>
+      <c r="J35" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K35" s="20">
+        <f>-40/100</f>
+        <v>-0.4</v>
+      </c>
+      <c r="L35" s="1">
+        <v>-0.4</v>
+      </c>
+      <c r="M35" s="3">
+        <v>-7.8999999999999995E-7</v>
+      </c>
+      <c r="N35" s="3">
+        <v>6.3899999999999996E-9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B36" s="1">
+        <v>-1.45245088402107E-2</v>
+      </c>
+      <c r="C36" s="1">
+        <v>-1.453480387E-2</v>
+      </c>
+      <c r="D36" s="1">
+        <v>-1.449120355E-2</v>
+      </c>
+      <c r="E36" s="1">
+        <v>-4.3600324780000002E-5</v>
+      </c>
+      <c r="F36" s="3">
+        <v>9.2199999999999998E-6</v>
+      </c>
+      <c r="G36" s="3">
+        <v>-3.4400000000000003E-5</v>
+      </c>
+      <c r="I36" s="1"/>
+      <c r="J36" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K36" s="21">
+        <f>1.44776824615491/100</f>
+        <v>1.44776824615491E-2</v>
+      </c>
+      <c r="L36" s="1">
+        <v>0</v>
+      </c>
+      <c r="M36" s="3">
+        <v>-8.8800000000000004E-5</v>
+      </c>
+      <c r="N36" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B37" s="1">
+        <v>-2.1118662608655699E-2</v>
+      </c>
+      <c r="C37" s="1">
+        <v>-2.1131558979999999E-2</v>
+      </c>
+      <c r="D37" s="1">
+        <v>-4.9006550730000001E-2</v>
+      </c>
+      <c r="E37" s="1">
+        <v>2.7874991740000001E-2</v>
+      </c>
+      <c r="F37" s="3">
+        <v>1.13E-5</v>
+      </c>
+      <c r="G37" s="3">
+        <v>2.7900000000000001E-2</v>
+      </c>
+      <c r="I37" s="1"/>
+      <c r="J37" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K37" s="21">
+        <f>0.209417870761202/100</f>
+        <v>2.0941787076120201E-3</v>
+      </c>
+      <c r="L37" s="1">
+        <v>0</v>
+      </c>
+      <c r="M37" s="3">
+        <v>4.07E-5</v>
+      </c>
+      <c r="N37" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B38" s="1">
+        <v>0.999998359536033</v>
+      </c>
+      <c r="C38" s="1">
+        <v>0.99971783469999997</v>
+      </c>
+      <c r="D38" s="1">
+        <v>1.001140192</v>
+      </c>
+      <c r="E38" s="1">
+        <v>-1.422356891E-3</v>
+      </c>
+      <c r="F38" s="3">
+        <v>2.8400000000000002E-4</v>
+      </c>
+      <c r="G38" s="3">
+        <v>-1.14E-3</v>
+      </c>
+      <c r="I38" s="1"/>
+      <c r="J38" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K38" s="20">
+        <v>0</v>
+      </c>
+      <c r="L38" s="1">
+        <v>0</v>
+      </c>
+      <c r="M38" s="1">
+        <v>-1.016250469E-4</v>
+      </c>
+      <c r="N38" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B39" s="1">
+        <v>0.99480759668265895</v>
+      </c>
+      <c r="C39" s="1">
+        <v>0.99453388529999998</v>
+      </c>
+      <c r="D39" s="1">
+        <v>0.99596625130000005</v>
+      </c>
+      <c r="E39" s="1">
+        <v>-1.4323660430000001E-3</v>
+      </c>
+      <c r="F39" s="3">
+        <v>2.8200000000000002E-4</v>
+      </c>
+      <c r="G39" s="3">
+        <v>-1.15E-3</v>
+      </c>
+      <c r="I39" s="1"/>
+      <c r="J39" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="K39" s="20">
+        <v>1</v>
+      </c>
+      <c r="L39" s="1">
+        <v>1</v>
+      </c>
+      <c r="M39" s="3">
+        <v>-1.42E-6</v>
+      </c>
+      <c r="N39" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B40" s="1">
+        <v>0.99171870097681902</v>
+      </c>
+      <c r="C40" s="1">
+        <v>0.99143333180000004</v>
+      </c>
+      <c r="D40" s="19">
+        <v>-2.6933805729999998</v>
+      </c>
+      <c r="E40" s="23">
+        <v>3.6848139049999999</v>
+      </c>
+      <c r="F40" s="3">
+        <v>2.9100000000000003E-4</v>
+      </c>
+      <c r="G40" s="3">
+        <v>3.69</v>
+      </c>
+      <c r="I40" s="1"/>
+      <c r="J40" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K40" s="21">
+        <v>0.99480618409400001</v>
+      </c>
+      <c r="L40" s="1">
+        <v>1</v>
+      </c>
+      <c r="M40" s="3">
+        <v>1.2300000000000001E-6</v>
+      </c>
+      <c r="N40" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J41" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="K41">
+        <f>8.39887199942846/100</f>
+        <v>8.3988719994284602E-2</v>
+      </c>
+      <c r="L41" s="25"/>
+      <c r="M41" s="25"/>
+      <c r="N41" s="25"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J42" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="K42">
+        <f>0.711492512043611/100</f>
+        <v>7.1149251204361101E-3</v>
+      </c>
+      <c r="L42" s="25"/>
+      <c r="M42" s="25"/>
+      <c r="N42" s="25"/>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A12:G12"/>
+    <mergeCell ref="A32:G32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1897,8 +2011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P42" sqref="P42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1912,54 +2026,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="L1" s="15" t="s">
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="L1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="15" t="s">
+      <c r="M1" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="N1" s="15" t="s">
+      <c r="N1" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="O1" s="15" t="s">
+      <c r="O1" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="Q1" s="19" t="s">
+      <c r="Q1" s="22" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12" t="s">
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="L2" s="10" t="s">
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="L2" s="8" t="s">
         <v>42</v>
       </c>
       <c r="M2" s="1">
@@ -1972,37 +2086,37 @@
         <v>0</v>
       </c>
       <c r="Q2" t="s">
-        <v>175</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14" t="s">
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="J3" s="14" t="s">
+      <c r="J3" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="L3" s="8" t="s">
         <v>47</v>
       </c>
       <c r="M3" s="1">
@@ -2030,7 +2144,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-      <c r="L4" s="10" t="s">
+      <c r="L4" s="8" t="s">
         <v>48</v>
       </c>
       <c r="M4" s="1">
@@ -2069,7 +2183,7 @@
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
-      <c r="L5" s="10" t="s">
+      <c r="L5" s="8" t="s">
         <v>49</v>
       </c>
       <c r="M5" s="1">
@@ -2102,7 +2216,7 @@
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
-      <c r="L6" s="10" t="s">
+      <c r="L6" s="8" t="s">
         <v>50</v>
       </c>
       <c r="M6" s="1">
@@ -2142,15 +2256,15 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="L7" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="L7" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="M7" s="18">
+      <c r="M7" s="13">
         <v>62.339801271691996</v>
       </c>
-      <c r="N7" s="18">
+      <c r="N7" s="13">
         <f t="shared" si="0"/>
         <v>0.62339801271691997</v>
       </c>
@@ -2180,7 +2294,7 @@
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
-      <c r="L8" s="10" t="s">
+      <c r="L8" s="8" t="s">
         <v>52</v>
       </c>
       <c r="M8" s="1">
@@ -2218,7 +2332,7 @@
         <v>-2.8269438203140096E-3</v>
       </c>
       <c r="J9" s="1"/>
-      <c r="L9" s="10" t="s">
+      <c r="L9" s="8" t="s">
         <v>53</v>
       </c>
       <c r="M9" s="1">
@@ -2251,7 +2365,7 @@
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
-      <c r="L10" s="10" t="s">
+      <c r="L10" s="8" t="s">
         <v>54</v>
       </c>
       <c r="M10" s="1">
@@ -2285,9 +2399,9 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" t="s">
-        <v>176</v>
-      </c>
-      <c r="L11" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="L11" s="8" t="s">
         <v>55</v>
       </c>
       <c r="M11" s="1">
@@ -2325,7 +2439,7 @@
         <f>B12-F12</f>
         <v>-7.9849174164339787E-3</v>
       </c>
-      <c r="L12" s="10" t="s">
+      <c r="L12" s="8" t="s">
         <v>56</v>
       </c>
       <c r="M12" s="1">
@@ -2358,7 +2472,7 @@
         <f>B13-F13</f>
         <v>-8.0875207598860022E-3</v>
       </c>
-      <c r="L13" s="10" t="s">
+      <c r="L13" s="8" t="s">
         <v>57</v>
       </c>
       <c r="M13" s="1">
@@ -2397,7 +2511,7 @@
         <f>B14-F14</f>
         <v>-8.1104006401980233E-3</v>
       </c>
-      <c r="L14" s="10" t="s">
+      <c r="L14" s="8" t="s">
         <v>58</v>
       </c>
       <c r="M14" s="1">
@@ -2430,7 +2544,7 @@
         <v>-2.904198490876031E-3</v>
       </c>
       <c r="J15" s="1"/>
-      <c r="L15" s="10" t="s">
+      <c r="L15" s="8" t="s">
         <v>59</v>
       </c>
       <c r="M15" s="1">
@@ -2469,7 +2583,7 @@
         <f>B16-F16</f>
         <v>-8.4414517243280307E-3</v>
       </c>
-      <c r="L16" s="10" t="s">
+      <c r="L16" s="8" t="s">
         <v>60</v>
       </c>
       <c r="M16" s="1">
@@ -2508,7 +2622,7 @@
         <f>B17-F17</f>
         <v>-8.1301587412709875E-3</v>
       </c>
-      <c r="L17" s="10" t="s">
+      <c r="L17" s="8" t="s">
         <v>12</v>
       </c>
       <c r="M17" s="1">
@@ -2523,7 +2637,7 @@
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="L18" s="10" t="s">
+      <c r="L18" s="8" t="s">
         <v>61</v>
       </c>
       <c r="M18" s="1">
@@ -2538,7 +2652,7 @@
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="L19" s="10" t="s">
+      <c r="L19" s="8" t="s">
         <v>62</v>
       </c>
       <c r="M19" s="1">
@@ -2553,7 +2667,7 @@
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="L20" s="10" t="s">
+      <c r="L20" s="8" t="s">
         <v>63</v>
       </c>
       <c r="M20" s="1">
@@ -2568,7 +2682,7 @@
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="L21" s="10" t="s">
+      <c r="L21" s="8" t="s">
         <v>64</v>
       </c>
       <c r="M21" s="1">
@@ -2583,7 +2697,7 @@
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="L22" s="10" t="s">
+      <c r="L22" s="8" t="s">
         <v>65</v>
       </c>
       <c r="M22" s="1">
@@ -2598,7 +2712,7 @@
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="L23" s="10" t="s">
+      <c r="L23" s="8" t="s">
         <v>66</v>
       </c>
       <c r="M23" s="1">
@@ -2613,7 +2727,7 @@
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="L24" s="10" t="s">
+      <c r="L24" s="8" t="s">
         <v>67</v>
       </c>
       <c r="M24" s="1">
@@ -2628,7 +2742,7 @@
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="L25" s="10" t="s">
+      <c r="L25" s="8" t="s">
         <v>68</v>
       </c>
       <c r="M25" s="1">
@@ -2643,7 +2757,7 @@
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="L26" s="10" t="s">
+      <c r="L26" s="8" t="s">
         <v>52</v>
       </c>
       <c r="M26" s="1">
@@ -2658,7 +2772,7 @@
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="L27" s="10" t="s">
+      <c r="L27" s="8" t="s">
         <v>69</v>
       </c>
       <c r="M27" s="1">
@@ -2673,7 +2787,7 @@
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="L28" s="10" t="s">
+      <c r="L28" s="8" t="s">
         <v>16</v>
       </c>
       <c r="M28" s="1">
@@ -2688,7 +2802,7 @@
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="L29" s="10" t="s">
+      <c r="L29" s="8" t="s">
         <v>56</v>
       </c>
       <c r="M29" s="1">
@@ -2703,7 +2817,7 @@
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="L30" s="10" t="s">
+      <c r="L30" s="8" t="s">
         <v>70</v>
       </c>
       <c r="M30" s="1">
@@ -2718,7 +2832,7 @@
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="L31" s="10" t="s">
+      <c r="L31" s="8" t="s">
         <v>71</v>
       </c>
       <c r="M31" s="1">
@@ -2733,7 +2847,7 @@
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="L32" s="10" t="s">
+      <c r="L32" s="8" t="s">
         <v>72</v>
       </c>
       <c r="M32" s="1">
@@ -2751,51 +2865,51 @@
       <c r="O33" s="1"/>
     </row>
     <row r="35" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="13" t="s">
-        <v>178</v>
-      </c>
-      <c r="B35" s="13"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
-      <c r="H35" s="13"/>
-      <c r="I35" s="13"/>
-      <c r="J35" s="13"/>
-      <c r="L35" s="15" t="s">
+      <c r="A35" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="B35" s="17"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="17"/>
+      <c r="I35" s="17"/>
+      <c r="J35" s="17"/>
+      <c r="L35" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="M35" s="15" t="s">
+      <c r="M35" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="N35" s="15" t="s">
+      <c r="N35" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="O35" s="15" t="s">
+      <c r="O35" s="11" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="36" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="11" t="s">
+      <c r="A36" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="11" t="s">
+      <c r="B36" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C36" s="11" t="s">
+      <c r="C36" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D36" s="11"/>
-      <c r="E36" s="11"/>
-      <c r="F36" s="11"/>
-      <c r="G36" s="11" t="s">
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="H36" s="11"/>
-      <c r="I36" s="11"/>
-      <c r="J36" s="11"/>
-      <c r="L36" s="10" t="s">
+      <c r="H36" s="9"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="9"/>
+      <c r="L36" s="8" t="s">
         <v>47</v>
       </c>
       <c r="M36" s="1">
@@ -2805,38 +2919,38 @@
         <f>M36/100</f>
         <v>1.47880570388169</v>
       </c>
-      <c r="O36" s="20">
+      <c r="O36" s="14">
         <v>1.1932028856076501E-6</v>
       </c>
     </row>
     <row r="37" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="14"/>
-      <c r="B37" s="14"/>
-      <c r="C37" s="14" t="s">
+      <c r="A37" s="10"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D37" s="14" t="s">
+      <c r="D37" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E37" s="14" t="s">
+      <c r="E37" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="F37" s="14" t="s">
+      <c r="F37" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="G37" s="14" t="s">
+      <c r="G37" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="H37" s="14" t="s">
+      <c r="H37" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="I37" s="14" t="s">
+      <c r="I37" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="J37" s="14" t="s">
+      <c r="J37" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="L37" s="10" t="s">
+      <c r="L37" s="8" t="s">
         <v>48</v>
       </c>
       <c r="M37" s="1">
@@ -2866,7 +2980,7 @@
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
-      <c r="L38" s="10" t="s">
+      <c r="L38" s="8" t="s">
         <v>49</v>
       </c>
       <c r="M38" s="1">
@@ -2903,7 +3017,7 @@
       </c>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
-      <c r="L39" s="10" t="s">
+      <c r="L39" s="8" t="s">
         <v>50</v>
       </c>
       <c r="M39" s="1">
@@ -2928,10 +3042,13 @@
         <v>-7.6495960726050902E-2</v>
       </c>
       <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
+      <c r="H40" s="1">
+        <f>B40-D40</f>
+        <v>-0.14968301618653612</v>
+      </c>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
-      <c r="L40" s="10" t="s">
+      <c r="L40" s="8" t="s">
         <v>53</v>
       </c>
       <c r="M40" s="1">
@@ -2958,18 +3075,24 @@
       <c r="D41" s="1">
         <v>-3.4959843053773497E-2</v>
       </c>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
+      <c r="G41" s="1">
+        <f>B41-C41</f>
+        <v>4.0971035688744994E-2</v>
+      </c>
+      <c r="H41" s="1">
+        <f t="shared" ref="H41:H46" si="5">B41-D41</f>
+        <v>-0.14991593502174649</v>
+      </c>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
-      <c r="L41" s="10" t="s">
+      <c r="L41" s="8" t="s">
         <v>54</v>
       </c>
       <c r="M41" s="1">
         <v>28.985080382272201</v>
       </c>
       <c r="N41" s="1">
-        <f t="shared" ref="N41:N42" si="5">M41/100</f>
+        <f t="shared" ref="N41:N42" si="6">M41/100</f>
         <v>0.28985080382272199</v>
       </c>
       <c r="O41" s="3">
@@ -2989,18 +3112,24 @@
       <c r="D42" s="1">
         <v>-8.7151391052258404E-3</v>
       </c>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
+      <c r="G42" s="1">
+        <f t="shared" ref="G42:G43" si="7">B42-C42</f>
+        <v>-1.7271901644699827E-4</v>
+      </c>
+      <c r="H42" s="1">
+        <f t="shared" si="5"/>
+        <v>-0.14990931942679717</v>
+      </c>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
-      <c r="L42" s="10" t="s">
+      <c r="L42" s="8" t="s">
         <v>55</v>
       </c>
       <c r="M42" s="1">
         <v>0</v>
       </c>
       <c r="N42" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O42" s="3">
@@ -3021,11 +3150,17 @@
         <v>1.3950959767079701E-2</v>
       </c>
       <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
+      <c r="G43" s="1">
+        <f t="shared" si="7"/>
+        <v>-0.24691984520472629</v>
+      </c>
       <c r="H43" s="1"/>
-      <c r="I43" s="1"/>
+      <c r="I43" s="1">
+        <f>B43-E43</f>
+        <v>-0.2786347956288347</v>
+      </c>
       <c r="J43" s="1"/>
-      <c r="L43" s="10" t="s">
+      <c r="L43" s="8" t="s">
         <v>57</v>
       </c>
       <c r="M43" s="1">
@@ -3052,17 +3187,20 @@
       </c>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
+      <c r="H44" s="1">
+        <f t="shared" si="5"/>
+        <v>-0.15037987828394561</v>
+      </c>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
-      <c r="L44" s="10" t="s">
+      <c r="L44" s="8" t="s">
         <v>58</v>
       </c>
       <c r="M44" s="1">
         <v>7.5451451109037899</v>
       </c>
       <c r="N44" s="1">
-        <f t="shared" ref="N44:N47" si="6">M44/100</f>
+        <f t="shared" ref="N44:N47" si="8">M44/100</f>
         <v>7.5451451109037893E-2</v>
       </c>
       <c r="O44" s="3">
@@ -3082,17 +3220,20 @@
       </c>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
-      <c r="H45" s="1"/>
+      <c r="H45" s="1">
+        <f t="shared" si="5"/>
+        <v>-0.1505259037926529</v>
+      </c>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
-      <c r="L45" s="10" t="s">
+      <c r="L45" s="8" t="s">
         <v>59</v>
       </c>
       <c r="M45" s="1">
         <v>17.033691859918299</v>
       </c>
       <c r="N45" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.17033691859918298</v>
       </c>
       <c r="O45" s="3">
@@ -3114,17 +3255,23 @@
         <v>-2.07652454529514E-2</v>
       </c>
       <c r="G46" s="1"/>
-      <c r="H46" s="1"/>
+      <c r="H46" s="1">
+        <f t="shared" si="5"/>
+        <v>-0.15039408993572298</v>
+      </c>
       <c r="I46" s="1"/>
-      <c r="J46" s="1"/>
-      <c r="L46" s="10" t="s">
+      <c r="J46" s="1">
+        <f>B46-F46</f>
+        <v>-0.25661074561957059</v>
+      </c>
+      <c r="L46" s="8" t="s">
         <v>60</v>
       </c>
       <c r="M46" s="1">
         <v>1.44514504235841</v>
       </c>
       <c r="N46" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.4451450423584099E-2</v>
       </c>
       <c r="O46" s="3">
@@ -3146,15 +3293,18 @@
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
-      <c r="J47" s="1"/>
-      <c r="L47" s="10" t="s">
+      <c r="J47" s="1">
+        <f t="shared" ref="J47:J51" si="9">B47-F47</f>
+        <v>-0.25662297137373036</v>
+      </c>
+      <c r="L47" s="8" t="s">
         <v>12</v>
       </c>
       <c r="M47" s="1">
         <v>-6.1</v>
       </c>
       <c r="N47" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-6.0999999999999999E-2</v>
       </c>
       <c r="O47" s="3">
@@ -3178,9 +3328,15 @@
       </c>
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
-      <c r="I48" s="1"/>
-      <c r="J48" s="1"/>
-      <c r="L48" s="10" t="s">
+      <c r="I48" s="1">
+        <f t="shared" ref="I44:I51" si="10">B48-E48</f>
+        <v>-0.27861163064252253</v>
+      </c>
+      <c r="J48" s="1">
+        <f t="shared" si="9"/>
+        <v>-0.25664458905786991</v>
+      </c>
+      <c r="L48" s="8" t="s">
         <v>62</v>
       </c>
       <c r="M48" s="1">
@@ -3211,23 +3367,29 @@
       </c>
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
-      <c r="I49" s="1"/>
-      <c r="J49" s="1"/>
-      <c r="L49" s="10" t="s">
+      <c r="I49" s="1">
+        <f t="shared" si="10"/>
+        <v>-0.27870435248018355</v>
+      </c>
+      <c r="J49" s="1">
+        <f t="shared" si="9"/>
+        <v>-0.25388977416602609</v>
+      </c>
+      <c r="L49" s="8" t="s">
         <v>63</v>
       </c>
       <c r="M49" s="1">
         <v>9.9211640275555908</v>
       </c>
       <c r="N49" s="1">
-        <f t="shared" ref="N49:N54" si="7">M49/100</f>
+        <f t="shared" ref="N49:N54" si="11">M49/100</f>
         <v>9.9211640275555901E-2</v>
       </c>
       <c r="O49" s="3">
         <v>-1.38124769413772E-7</v>
       </c>
       <c r="P49" t="s">
-        <v>177</v>
+        <v>78</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
@@ -3244,16 +3406,19 @@
       </c>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
-      <c r="I50" s="1"/>
+      <c r="I50" s="1">
+        <f t="shared" si="10"/>
+        <v>-0.27868996527651574</v>
+      </c>
       <c r="J50" s="1"/>
-      <c r="L50" s="10" t="s">
+      <c r="L50" s="8" t="s">
         <v>64</v>
       </c>
       <c r="M50" s="1">
         <v>-7.6</v>
       </c>
       <c r="N50" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>-7.5999999999999998E-2</v>
       </c>
       <c r="O50" s="3">
@@ -3277,16 +3442,22 @@
       </c>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
-      <c r="I51" s="1"/>
-      <c r="J51" s="1"/>
-      <c r="L51" s="10" t="s">
+      <c r="I51" s="1">
+        <f t="shared" si="10"/>
+        <v>-0.27852421934355803</v>
+      </c>
+      <c r="J51" s="1">
+        <f t="shared" si="9"/>
+        <v>-0.25670105959310652</v>
+      </c>
+      <c r="L51" s="8" t="s">
         <v>65</v>
       </c>
       <c r="M51" s="1">
         <v>-62.339801271691996</v>
       </c>
       <c r="N51" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>-0.62339801271691997</v>
       </c>
       <c r="O51" s="3">
@@ -3294,14 +3465,14 @@
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L52" s="10" t="s">
+      <c r="L52" s="8" t="s">
         <v>66</v>
       </c>
       <c r="M52" s="1">
         <v>16.6313222291061</v>
       </c>
       <c r="N52" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0.16631322229106099</v>
       </c>
       <c r="O52" s="3">
@@ -3309,14 +3480,14 @@
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L53" s="10" t="s">
+      <c r="L53" s="8" t="s">
         <v>67</v>
       </c>
       <c r="M53" s="1">
         <v>28.985080382272098</v>
       </c>
       <c r="N53" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0.28985080382272099</v>
       </c>
       <c r="O53" s="3">
@@ -3324,14 +3495,14 @@
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L54" s="10" t="s">
+      <c r="L54" s="8" t="s">
         <v>68</v>
       </c>
       <c r="M54" s="1">
         <v>-94.2</v>
       </c>
       <c r="N54" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>-0.94200000000000006</v>
       </c>
       <c r="O54" s="3">
@@ -3339,7 +3510,7 @@
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L55" s="10" t="s">
+      <c r="L55" s="8" t="s">
         <v>69</v>
       </c>
       <c r="M55" s="1">
@@ -3354,7 +3525,7 @@
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L56" s="10" t="s">
+      <c r="L56" s="8" t="s">
         <v>16</v>
       </c>
       <c r="M56" s="1">
@@ -3369,7 +3540,7 @@
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L57" s="10" t="s">
+      <c r="L57" s="8" t="s">
         <v>70</v>
       </c>
       <c r="M57" s="1">
@@ -3384,7 +3555,7 @@
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L58" s="10" t="s">
+      <c r="L58" s="8" t="s">
         <v>71</v>
       </c>
       <c r="M58" s="1">
@@ -3432,636 +3603,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P32"/>
-  <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="9" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.42578125" customWidth="1"/>
-    <col min="11" max="16" width="18.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E2" t="s">
-        <v>81</v>
-      </c>
-      <c r="F2" t="s">
-        <v>82</v>
-      </c>
-      <c r="G2" t="s">
-        <v>83</v>
-      </c>
-      <c r="H2" t="s">
-        <v>84</v>
-      </c>
-      <c r="I2" t="s">
-        <v>85</v>
-      </c>
-      <c r="J2" t="s">
-        <v>86</v>
-      </c>
-      <c r="K2" t="s">
-        <v>87</v>
-      </c>
-      <c r="L2" t="s">
-        <v>88</v>
-      </c>
-      <c r="M2" t="s">
-        <v>89</v>
-      </c>
-      <c r="N2" t="s">
-        <v>90</v>
-      </c>
-      <c r="O2" t="s">
-        <v>91</v>
-      </c>
-      <c r="P2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="D3" t="s">
-        <v>121</v>
-      </c>
-      <c r="G3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C4" t="s">
-        <v>121</v>
-      </c>
-      <c r="D4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E4" t="s">
-        <v>122</v>
-      </c>
-      <c r="F4" t="s">
-        <v>123</v>
-      </c>
-      <c r="G4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>97</v>
-      </c>
-      <c r="D5" t="s">
-        <v>122</v>
-      </c>
-      <c r="E5" t="s">
-        <v>98</v>
-      </c>
-      <c r="F5" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>99</v>
-      </c>
-      <c r="D6" t="s">
-        <v>123</v>
-      </c>
-      <c r="E6" t="s">
-        <v>126</v>
-      </c>
-      <c r="F6" t="s">
-        <v>100</v>
-      </c>
-      <c r="G6" t="s">
-        <v>127</v>
-      </c>
-      <c r="I6" t="s">
-        <v>128</v>
-      </c>
-      <c r="K6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>101</v>
-      </c>
-      <c r="C7" t="s">
-        <v>125</v>
-      </c>
-      <c r="D7" t="s">
-        <v>124</v>
-      </c>
-      <c r="F7" t="s">
-        <v>127</v>
-      </c>
-      <c r="G7" t="s">
-        <v>102</v>
-      </c>
-      <c r="H7" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>103</v>
-      </c>
-      <c r="G8" t="s">
-        <v>130</v>
-      </c>
-      <c r="H8" t="s">
-        <v>104</v>
-      </c>
-      <c r="M8" t="s">
-        <v>131</v>
-      </c>
-      <c r="N8" t="s">
-        <v>132</v>
-      </c>
-      <c r="O8" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>105</v>
-      </c>
-      <c r="F9" t="s">
-        <v>128</v>
-      </c>
-      <c r="I9" t="s">
-        <v>106</v>
-      </c>
-      <c r="J9" t="s">
-        <v>134</v>
-      </c>
-      <c r="K9" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>107</v>
-      </c>
-      <c r="I10" t="s">
-        <v>134</v>
-      </c>
-      <c r="J10" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>109</v>
-      </c>
-      <c r="F11" t="s">
-        <v>129</v>
-      </c>
-      <c r="I11" t="s">
-        <v>135</v>
-      </c>
-      <c r="K11" t="s">
-        <v>110</v>
-      </c>
-      <c r="L11" t="s">
-        <v>136</v>
-      </c>
-      <c r="P11" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>111</v>
-      </c>
-      <c r="K12" t="s">
-        <v>136</v>
-      </c>
-      <c r="L12" t="s">
-        <v>112</v>
-      </c>
-      <c r="M12" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>113</v>
-      </c>
-      <c r="H13" t="s">
-        <v>131</v>
-      </c>
-      <c r="L13" t="s">
-        <v>138</v>
-      </c>
-      <c r="M13" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>115</v>
-      </c>
-      <c r="H14" t="s">
-        <v>132</v>
-      </c>
-      <c r="N14" t="s">
-        <v>116</v>
-      </c>
-      <c r="O14" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>117</v>
-      </c>
-      <c r="H15" t="s">
-        <v>133</v>
-      </c>
-      <c r="N15" t="s">
-        <v>139</v>
-      </c>
-      <c r="O15" t="s">
-        <v>118</v>
-      </c>
-      <c r="P15" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
-        <v>119</v>
-      </c>
-      <c r="K16" t="s">
-        <v>137</v>
-      </c>
-      <c r="O16" t="s">
-        <v>140</v>
-      </c>
-      <c r="P16" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>77</v>
-      </c>
-      <c r="B18" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>1</v>
-      </c>
-      <c r="B19" t="s">
-        <v>93</v>
-      </c>
-      <c r="C19" t="s">
-        <v>141</v>
-      </c>
-      <c r="D19" t="s">
-        <v>142</v>
-      </c>
-      <c r="G19" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>2</v>
-      </c>
-      <c r="B20" t="s">
-        <v>95</v>
-      </c>
-      <c r="C20" t="s">
-        <v>142</v>
-      </c>
-      <c r="D20" t="s">
-        <v>144</v>
-      </c>
-      <c r="E20" t="s">
-        <v>145</v>
-      </c>
-      <c r="F20" t="s">
-        <v>146</v>
-      </c>
-      <c r="G20" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>3</v>
-      </c>
-      <c r="B21" t="s">
-        <v>97</v>
-      </c>
-      <c r="D21" t="s">
-        <v>145</v>
-      </c>
-      <c r="E21" t="s">
-        <v>148</v>
-      </c>
-      <c r="F21" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>4</v>
-      </c>
-      <c r="B22" t="s">
-        <v>99</v>
-      </c>
-      <c r="D22" t="s">
-        <v>146</v>
-      </c>
-      <c r="E22" t="s">
-        <v>149</v>
-      </c>
-      <c r="F22" t="s">
-        <v>150</v>
-      </c>
-      <c r="G22" t="s">
-        <v>151</v>
-      </c>
-      <c r="I22" t="s">
-        <v>152</v>
-      </c>
-      <c r="K22" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>5</v>
-      </c>
-      <c r="B23" t="s">
-        <v>101</v>
-      </c>
-      <c r="C23" t="s">
-        <v>143</v>
-      </c>
-      <c r="D23" t="s">
-        <v>147</v>
-      </c>
-      <c r="F23" t="s">
-        <v>151</v>
-      </c>
-      <c r="G23" t="s">
-        <v>153</v>
-      </c>
-      <c r="H23" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>6</v>
-      </c>
-      <c r="B24" t="s">
-        <v>103</v>
-      </c>
-      <c r="G24" t="s">
-        <v>154</v>
-      </c>
-      <c r="H24" t="s">
-        <v>155</v>
-      </c>
-      <c r="M24" t="s">
-        <v>160</v>
-      </c>
-      <c r="N24" t="s">
-        <v>161</v>
-      </c>
-      <c r="O24" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>7</v>
-      </c>
-      <c r="B25" t="s">
-        <v>105</v>
-      </c>
-      <c r="F25" t="s">
-        <v>152</v>
-      </c>
-      <c r="I25" t="s">
-        <v>156</v>
-      </c>
-      <c r="J25" t="s">
-        <v>157</v>
-      </c>
-      <c r="K25" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>8</v>
-      </c>
-      <c r="B26" t="s">
-        <v>107</v>
-      </c>
-      <c r="I26" t="s">
-        <v>157</v>
-      </c>
-      <c r="J26" s="16" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>9</v>
-      </c>
-      <c r="B27" t="s">
-        <v>109</v>
-      </c>
-      <c r="F27" t="s">
-        <v>158</v>
-      </c>
-      <c r="I27" t="s">
-        <v>159</v>
-      </c>
-      <c r="K27" s="16" t="s">
-        <v>164</v>
-      </c>
-      <c r="L27" t="s">
-        <v>165</v>
-      </c>
-      <c r="P27" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>10</v>
-      </c>
-      <c r="B28" t="s">
-        <v>111</v>
-      </c>
-      <c r="K28" t="s">
-        <v>165</v>
-      </c>
-      <c r="L28" s="16" t="s">
-        <v>167</v>
-      </c>
-      <c r="M28" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>11</v>
-      </c>
-      <c r="B29" t="s">
-        <v>113</v>
-      </c>
-      <c r="H29" t="s">
-        <v>160</v>
-      </c>
-      <c r="L29" t="s">
-        <v>168</v>
-      </c>
-      <c r="M29" s="16" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>12</v>
-      </c>
-      <c r="B30" t="s">
-        <v>115</v>
-      </c>
-      <c r="H30" t="s">
-        <v>161</v>
-      </c>
-      <c r="N30" s="16" t="s">
-        <v>170</v>
-      </c>
-      <c r="O30" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>13</v>
-      </c>
-      <c r="B31" t="s">
-        <v>117</v>
-      </c>
-      <c r="H31" t="s">
-        <v>162</v>
-      </c>
-      <c r="N31" t="s">
-        <v>171</v>
-      </c>
-      <c r="O31" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="P31" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>14</v>
-      </c>
-      <c r="B32" t="s">
-        <v>119</v>
-      </c>
-      <c r="K32" t="s">
-        <v>166</v>
-      </c>
-      <c r="O32" t="s">
-        <v>173</v>
-      </c>
-      <c r="P32" s="16" t="s">
-        <v>174</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Created an even smaller 2 bus case
Created an even smaller 2 bus case from ECE 6320 notes, Module 3 SE
example. Removed a bunch of old files.
</commit_message>
<xml_diff>
--- a/DMASE - Test Results.xlsx
+++ b/DMASE - Test Results.xlsx
@@ -7,15 +7,16 @@
     <workbookView xWindow="360" yWindow="105" windowWidth="18195" windowHeight="7740"/>
   </bookViews>
   <sheets>
-    <sheet name="3 Bus" sheetId="1" r:id="rId1"/>
-    <sheet name="14 Bus DC" sheetId="2" r:id="rId2"/>
+    <sheet name="2 Bus" sheetId="4" r:id="rId1"/>
+    <sheet name="3 Bus" sheetId="1" r:id="rId2"/>
+    <sheet name="14 Bus DC" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="84">
   <si>
     <t>Abur 3-Bus Case Measurements (run through SE, rerun new estimate again)</t>
   </si>
@@ -104,9 +105,6 @@
     <t>V2</t>
   </si>
   <si>
-    <t>PowerWorld 3-Bus Power Flow (construct case, use PF results as measurements)</t>
-  </si>
-  <si>
     <t>PW AC Z</t>
   </si>
   <si>
@@ -260,10 +258,16 @@
     <t>Created large res</t>
   </si>
   <si>
-    <t>P23</t>
-  </si>
-  <si>
-    <t>Q23</t>
+    <t>PowerWorld 3-Bus Polar Power Flow (construct case, use PF results as measurements)</t>
+  </si>
+  <si>
+    <t>PowerWorld 3-Bus Rect Power Flow (construct case, use PF results as measurements)</t>
+  </si>
+  <si>
+    <t>Simple 2-Bus Case</t>
+  </si>
+  <si>
+    <t>Q1</t>
   </si>
 </sst>
 </file>
@@ -387,7 +391,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -452,10 +456,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -757,10 +768,311 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N46"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="K41" sqref="K41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="I1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="I2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2">
+        <f>103.26057736651/100</f>
+        <v>1.0326057736651</v>
+      </c>
+      <c r="K2" s="1"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+    </row>
+    <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3">
+        <f>14.3474275489088/100</f>
+        <v>0.143474275489088</v>
+      </c>
+      <c r="K3" s="1"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+    </row>
+    <row r="4" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="J4">
+        <f>103.260576725006/100</f>
+        <v>1.0326057672500601</v>
+      </c>
+      <c r="K4" s="1"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="1">
+        <v>-2.1773802320000001E-2</v>
+      </c>
+      <c r="C5" s="1">
+        <v>-2.1773937810000001E-2</v>
+      </c>
+      <c r="D5" s="1">
+        <v>-2.177367329E-2</v>
+      </c>
+      <c r="E5" s="1">
+        <v>-2.6452093980000002E-7</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1.354878019E-7</v>
+      </c>
+      <c r="G5" s="1">
+        <v>-1.2903313789999999E-7</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="J5">
+        <f>14.3474280834197/100</f>
+        <v>0.143474280834197</v>
+      </c>
+      <c r="K5" s="1"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="1"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="1">
+        <v>-4.7921796930000003E-2</v>
+      </c>
+      <c r="C6" s="1">
+        <v>-4.7924889909999997E-2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>-4.7927640270000002E-2</v>
+      </c>
+      <c r="E6" s="1">
+        <v>2.7503603419999999E-6</v>
+      </c>
+      <c r="F6" s="1">
+        <v>3.092984698E-6</v>
+      </c>
+      <c r="G6" s="1">
+        <v>5.8433450400000004E-6</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="1">
+        <f>-100/100</f>
+        <v>-1</v>
+      </c>
+      <c r="K6" s="1"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="1"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.99962925790000001</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.99962926860000001</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.99962946860000002</v>
+      </c>
+      <c r="E7" s="1">
+        <v>-1.999925691E-7</v>
+      </c>
+      <c r="F7" s="1">
+        <v>-1.0708371970000001E-8</v>
+      </c>
+      <c r="G7" s="1">
+        <v>-2.10700941E-7</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" s="1">
+        <f>-10/100</f>
+        <v>-0.1</v>
+      </c>
+      <c r="K7" s="1"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="1"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.97415607159999995</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.97415592419999997</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.9741560803</v>
+      </c>
+      <c r="E8" s="1">
+        <v>-1.5608798400000001E-7</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1.4738417499999999E-7</v>
+      </c>
+      <c r="G8" s="1">
+        <v>-8.7038090069999994E-9</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" s="1">
+        <v>1</v>
+      </c>
+      <c r="K8" s="1"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="1"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.94389038079999998</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.94388689830000005</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.94388708779999997</v>
+      </c>
+      <c r="E9" s="1">
+        <v>-1.8957620710000001E-7</v>
+      </c>
+      <c r="F9" s="1">
+        <v>3.4825022610000002E-6</v>
+      </c>
+      <c r="G9" s="1">
+        <v>3.2929260540000001E-6</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J9">
+        <v>0.96399318562929603</v>
+      </c>
+      <c r="K9" s="1"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N55"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -806,7 +1118,7 @@
     </row>
     <row r="2" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>8</v>
@@ -1138,7 +1450,7 @@
     </row>
     <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16" t="s">
-        <v>29</v>
+        <v>80</v>
       </c>
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
@@ -1151,27 +1463,27 @@
         <v>1</v>
       </c>
       <c r="K12" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="L12" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="L12" s="6" t="s">
+      <c r="M12" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="M12" s="6" t="s">
+      <c r="N12" s="6" t="s">
         <v>32</v>
-      </c>
-      <c r="N12" s="6" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
@@ -1470,10 +1782,10 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>9</v>
@@ -1625,9 +1937,18 @@
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
     </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+    </row>
     <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="16" t="s">
-        <v>29</v>
+        <v>81</v>
       </c>
       <c r="B32" s="16"/>
       <c r="C32" s="16"/>
@@ -1640,27 +1961,27 @@
         <v>1</v>
       </c>
       <c r="K32" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="L32" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="L32" s="6" t="s">
+      <c r="M32" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="M32" s="6" t="s">
+      <c r="N32" s="6" t="s">
         <v>32</v>
-      </c>
-      <c r="N32" s="6" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
@@ -1958,42 +2279,195 @@
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="J41" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="K41">
-        <f>8.39887199942846/100</f>
-        <v>8.3988719994284602E-2</v>
-      </c>
-      <c r="L41" s="25"/>
-      <c r="M41" s="25"/>
-      <c r="N41" s="25"/>
+      <c r="J41" s="8"/>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="J42" s="24" t="s">
-        <v>82</v>
-      </c>
-      <c r="K42">
-        <f>0.711492512043611/100</f>
-        <v>7.1149251204361101E-3</v>
-      </c>
-      <c r="L42" s="25"/>
-      <c r="M42" s="25"/>
-      <c r="N42" s="25"/>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="A42" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+      <c r="J42" s="8"/>
+    </row>
+    <row r="43" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="6"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G43" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B44" s="1">
+        <v>0</v>
+      </c>
+      <c r="C44" s="1">
+        <v>0</v>
+      </c>
+      <c r="D44" s="1">
+        <v>0</v>
+      </c>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B45" s="1">
+        <v>-1.443750012E-2</v>
+      </c>
+      <c r="C45" s="1">
+        <v>-1.443750029E-2</v>
+      </c>
+      <c r="D45" s="1">
+        <v>-1.443749678E-2</v>
+      </c>
+      <c r="E45" s="3">
+        <v>-3.5100000000000001E-9</v>
+      </c>
+      <c r="F45" s="3">
+        <v>1.6900000000000001E-10</v>
+      </c>
+      <c r="G45" s="3">
+        <v>-3.34E-9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B46" s="1">
+        <v>-2.093749994E-2</v>
+      </c>
+      <c r="C46" s="1">
+        <v>-2.0937501349999998E-2</v>
+      </c>
+      <c r="D46" s="1">
+        <v>-2.0937470489999999E-2</v>
+      </c>
+      <c r="E46" s="3">
+        <v>-3.0899999999999999E-8</v>
+      </c>
+      <c r="F46" s="3">
+        <v>1.4100000000000001E-9</v>
+      </c>
+      <c r="G46" s="3">
+        <v>-2.9499999999999999E-8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B47" s="1">
+        <v>1</v>
+      </c>
+      <c r="C47" s="1">
+        <v>1</v>
+      </c>
+      <c r="D47" s="1">
+        <v>1</v>
+      </c>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B48" s="1">
+        <v>1</v>
+      </c>
+      <c r="C48" s="1">
+        <v>1</v>
+      </c>
+      <c r="D48" s="1">
+        <v>1</v>
+      </c>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B49" s="1">
+        <v>1</v>
+      </c>
+      <c r="C49" s="1">
+        <v>1</v>
+      </c>
+      <c r="D49" s="1">
+        <v>1</v>
+      </c>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A51" s="24"/>
+      <c r="B51" s="24"/>
+      <c r="C51" s="24"/>
+      <c r="D51" s="24"/>
+      <c r="E51" s="24"/>
+      <c r="F51" s="24"/>
+      <c r="G51" s="24"/>
+      <c r="H51" s="24"/>
+      <c r="I51" s="24"/>
+      <c r="J51" s="26"/>
+      <c r="K51" s="25"/>
+      <c r="L51" s="27"/>
+      <c r="M51" s="28"/>
+      <c r="N51" s="27"/>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>39</v>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -2007,12 +2481,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2027,7 +2501,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
@@ -2042,16 +2516,16 @@
         <v>1</v>
       </c>
       <c r="M1" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N1" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O1" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q1" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -2068,13 +2542,13 @@
       <c r="E2" s="18"/>
       <c r="F2" s="18"/>
       <c r="G2" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H2" s="18"/>
       <c r="I2" s="18"/>
       <c r="J2" s="18"/>
       <c r="L2" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M2" s="1">
         <v>0</v>
@@ -2086,7 +2560,7 @@
         <v>0</v>
       </c>
       <c r="Q2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2099,10 +2573,10 @@
         <v>14</v>
       </c>
       <c r="E3" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="10" t="s">
         <v>43</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>44</v>
       </c>
       <c r="G3" s="10" t="s">
         <v>10</v>
@@ -2111,13 +2585,13 @@
         <v>11</v>
       </c>
       <c r="I3" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="J3" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="L3" s="8" t="s">
         <v>46</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>47</v>
       </c>
       <c r="M3" s="1">
         <v>147.88057038816899</v>
@@ -2145,7 +2619,7 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="L4" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M4" s="1">
         <v>71.119424158005401</v>
@@ -2184,7 +2658,7 @@
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="L5" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M5" s="1">
         <v>40.903974663241002</v>
@@ -2217,7 +2691,7 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="L6" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M6" s="1">
         <v>219</v>
@@ -2256,10 +2730,10 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L7" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M7" s="13">
         <v>62.339801271691996</v>
@@ -2295,7 +2769,7 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="L8" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M8" s="1">
         <v>-0.22617938916486699</v>
@@ -2333,7 +2807,7 @@
       </c>
       <c r="J9" s="1"/>
       <c r="L9" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M9" s="1">
         <v>-24.149760653480001</v>
@@ -2366,7 +2840,7 @@
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="L10" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M10" s="1">
         <v>28.985080382272201</v>
@@ -2399,10 +2873,10 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M11" s="1">
         <v>0</v>
@@ -2440,7 +2914,7 @@
         <v>-7.9849174164339787E-3</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M12" s="1">
         <v>-0.26468384711479698</v>
@@ -2473,7 +2947,7 @@
         <v>-8.0875207598860022E-3</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M13" s="1">
         <v>6.3047604774040904</v>
@@ -2512,7 +2986,7 @@
         <v>-8.1104006401980233E-3</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M14" s="1">
         <v>7.5451451109037899</v>
@@ -2545,7 +3019,7 @@
       </c>
       <c r="J15" s="1"/>
       <c r="L15" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M15" s="1">
         <v>17.033691859918299</v>
@@ -2584,7 +3058,7 @@
         <v>-8.4414517243280307E-3</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M16" s="1">
         <v>1.44514504235841</v>
@@ -2638,7 +3112,7 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L18" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M18" s="1">
         <v>-0.27737614157951601</v>
@@ -2653,7 +3127,7 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L19" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M19" s="1">
         <v>6.1952398951249403</v>
@@ -2668,7 +3142,7 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L20" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M20" s="1">
         <v>9.9211640275555908</v>
@@ -2683,7 +3157,7 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L21" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="M21" s="1">
         <v>-7.6</v>
@@ -2698,7 +3172,7 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L22" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M22" s="1">
         <v>-62.339801271691996</v>
@@ -2713,7 +3187,7 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L23" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M23" s="1">
         <v>16.6313222291061</v>
@@ -2728,7 +3202,7 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L24" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M24" s="1">
         <v>28.985080382272098</v>
@@ -2743,7 +3217,7 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L25" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M25" s="1">
         <v>-94.2</v>
@@ -2758,7 +3232,7 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L26" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M26" s="1">
         <v>-0.22617938916486699</v>
@@ -2773,7 +3247,7 @@
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L27" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M27" s="1">
         <v>4.9788363658350603</v>
@@ -2803,7 +3277,7 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L29" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M29" s="1">
         <v>-0.26468384711479698</v>
@@ -2818,7 +3292,7 @@
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L30" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M30" s="1">
         <v>-2.8047604625028999</v>
@@ -2833,7 +3307,7 @@
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L31" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M31" s="1">
         <v>-14.9</v>
@@ -2848,7 +3322,7 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L32" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M32" s="1">
         <v>-0.27737614157951601</v>
@@ -2866,7 +3340,7 @@
     </row>
     <row r="35" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B35" s="17"/>
       <c r="C35" s="17"/>
@@ -2881,13 +3355,13 @@
         <v>1</v>
       </c>
       <c r="M35" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N35" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O35" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -2904,13 +3378,13 @@
       <c r="E36" s="9"/>
       <c r="F36" s="9"/>
       <c r="G36" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H36" s="9"/>
       <c r="I36" s="9"/>
       <c r="J36" s="9"/>
       <c r="L36" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M36" s="1">
         <v>147.88057038816899</v>
@@ -2933,10 +3407,10 @@
         <v>14</v>
       </c>
       <c r="E37" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F37" s="10" t="s">
         <v>43</v>
-      </c>
-      <c r="F37" s="10" t="s">
-        <v>44</v>
       </c>
       <c r="G37" s="10" t="s">
         <v>10</v>
@@ -2945,13 +3419,13 @@
         <v>11</v>
       </c>
       <c r="I37" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="J37" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="J37" s="10" t="s">
-        <v>46</v>
-      </c>
       <c r="L37" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M37" s="1">
         <v>71.119424158005401</v>
@@ -2981,7 +3455,7 @@
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
       <c r="L38" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M38" s="1">
         <v>40.903974663241002</v>
@@ -3018,7 +3492,7 @@
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
       <c r="L39" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M39" s="1">
         <v>219</v>
@@ -3049,7 +3523,7 @@
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
       <c r="L40" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M40" s="1">
         <v>-24.149760653480001</v>
@@ -3086,7 +3560,7 @@
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
       <c r="L41" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M41" s="1">
         <v>28.985080382272201</v>
@@ -3123,7 +3597,7 @@
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
       <c r="L42" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M42" s="1">
         <v>0</v>
@@ -3161,7 +3635,7 @@
       </c>
       <c r="J43" s="1"/>
       <c r="L43" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M43" s="1">
         <v>6.3047604774040904</v>
@@ -3194,7 +3668,7 @@
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
       <c r="L44" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M44" s="1">
         <v>7.5451451109037899</v>
@@ -3227,7 +3701,7 @@
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
       <c r="L45" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M45" s="1">
         <v>17.033691859918299</v>
@@ -3265,7 +3739,7 @@
         <v>-0.25661074561957059</v>
       </c>
       <c r="L46" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M46" s="1">
         <v>1.44514504235841</v>
@@ -3337,7 +3811,7 @@
         <v>-0.25664458905786991</v>
       </c>
       <c r="L48" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M48" s="1">
         <v>6.1952398951249403</v>
@@ -3376,7 +3850,7 @@
         <v>-0.25388977416602609</v>
       </c>
       <c r="L49" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M49" s="1">
         <v>9.9211640275555908</v>
@@ -3389,7 +3863,7 @@
         <v>-1.38124769413772E-7</v>
       </c>
       <c r="P49" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
@@ -3412,7 +3886,7 @@
       </c>
       <c r="J50" s="1"/>
       <c r="L50" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="M50" s="1">
         <v>-7.6</v>
@@ -3451,7 +3925,7 @@
         <v>-0.25670105959310652</v>
       </c>
       <c r="L51" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M51" s="1">
         <v>-62.339801271691996</v>
@@ -3466,7 +3940,7 @@
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="L52" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M52" s="1">
         <v>16.6313222291061</v>
@@ -3481,7 +3955,7 @@
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="L53" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M53" s="1">
         <v>28.985080382272098</v>
@@ -3496,7 +3970,7 @@
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="L54" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M54" s="1">
         <v>-94.2</v>
@@ -3511,7 +3985,7 @@
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="L55" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M55" s="1">
         <v>4.9788363658350603</v>
@@ -3541,7 +4015,7 @@
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="L57" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M57" s="1">
         <v>-2.8047604625028999</v>
@@ -3556,7 +4030,7 @@
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="L58" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M58" s="1">
         <v>-14.9</v>

</xml_diff>

<commit_message>
Converted h vector formulation from polar to rectangular
Converted h vector from polar to rectangular. Not debugged yet. Also
updated the formulation in word and the results in DMASE - test
results.xlsx.
</commit_message>
<xml_diff>
--- a/DMASE - Test Results.xlsx
+++ b/DMASE - Test Results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="84">
   <si>
     <t>Abur 3-Bus Case Measurements (run through SE, rerun new estimate again)</t>
   </si>
@@ -771,7 +771,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -831,7 +831,9 @@
         <v>1.0326057736651</v>
       </c>
       <c r="K2" s="1"/>
-      <c r="L2" s="3"/>
+      <c r="L2" s="3">
+        <v>-4.09372882814729E-6</v>
+      </c>
       <c r="M2" s="3"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -860,7 +862,9 @@
         <v>0.143474275489088</v>
       </c>
       <c r="K3" s="1"/>
-      <c r="L3" s="3"/>
+      <c r="L3" s="3">
+        <v>-5.8479390156740401E-6</v>
+      </c>
       <c r="M3" s="3"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -893,7 +897,9 @@
         <v>1.0326057672500601</v>
       </c>
       <c r="K4" s="1"/>
-      <c r="L4" s="3"/>
+      <c r="L4" s="3">
+        <v>-4.1007288289485197E-6</v>
+      </c>
       <c r="M4" s="3"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -901,23 +907,13 @@
         <v>19</v>
       </c>
       <c r="B5" s="1">
-        <v>-2.1773802320000001E-2</v>
-      </c>
-      <c r="C5" s="1">
-        <v>-2.1773937810000001E-2</v>
-      </c>
-      <c r="D5" s="1">
-        <v>-2.177367329E-2</v>
-      </c>
-      <c r="E5" s="1">
-        <v>-2.6452093980000002E-7</v>
-      </c>
-      <c r="F5" s="1">
-        <v>1.354878019E-7</v>
-      </c>
-      <c r="G5" s="1">
-        <v>-1.2903313789999999E-7</v>
-      </c>
+        <v>-3.8391445791322899E-2</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
       <c r="I5" s="8" t="s">
         <v>83</v>
       </c>
@@ -926,31 +922,23 @@
         <v>0.143474280834197</v>
       </c>
       <c r="K5" s="1"/>
-      <c r="L5" s="3"/>
+      <c r="L5" s="3">
+        <v>-5.8419390149555601E-6</v>
+      </c>
       <c r="M5" s="1"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B6" s="1">
-        <v>-4.7921796930000003E-2</v>
-      </c>
-      <c r="C6" s="1">
-        <v>-4.7924889909999997E-2</v>
-      </c>
-      <c r="D6" s="1">
-        <v>-4.7927640270000002E-2</v>
-      </c>
-      <c r="E6" s="1">
-        <v>2.7503603419999999E-6</v>
-      </c>
-      <c r="F6" s="1">
-        <v>3.092984698E-6</v>
-      </c>
-      <c r="G6" s="1">
-        <v>5.8433450400000004E-6</v>
-      </c>
+        <v>1.00000000217498</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
       <c r="I6" s="8" t="s">
         <v>18</v>
       </c>
@@ -959,31 +947,23 @@
         <v>-1</v>
       </c>
       <c r="K6" s="1"/>
-      <c r="L6" s="3"/>
+      <c r="L6" s="3">
+        <v>3.76791437384227E-6</v>
+      </c>
       <c r="M6" s="1"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B7" s="1">
-        <v>0.99962925790000001</v>
-      </c>
-      <c r="C7" s="1">
-        <v>0.99962926860000001</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0.99962946860000002</v>
-      </c>
-      <c r="E7" s="1">
-        <v>-1.999925691E-7</v>
-      </c>
-      <c r="F7" s="1">
-        <v>-1.0708371970000001E-8</v>
-      </c>
-      <c r="G7" s="1">
-        <v>-2.10700941E-7</v>
-      </c>
+        <v>0.96399318557074398</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
       <c r="I7" s="8" t="s">
         <v>24</v>
       </c>
@@ -992,31 +972,19 @@
         <v>-0.1</v>
       </c>
       <c r="K7" s="1"/>
-      <c r="L7" s="3"/>
+      <c r="L7" s="3">
+        <v>5.3231864123454196E-6</v>
+      </c>
       <c r="M7" s="1"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="1">
-        <v>0.97415607159999995</v>
-      </c>
-      <c r="C8" s="1">
-        <v>0.97415592419999997</v>
-      </c>
-      <c r="D8" s="1">
-        <v>0.9741560803</v>
-      </c>
-      <c r="E8" s="1">
-        <v>-1.5608798400000001E-7</v>
-      </c>
-      <c r="F8" s="1">
-        <v>1.4738417499999999E-7</v>
-      </c>
-      <c r="G8" s="1">
-        <v>-8.7038090069999994E-9</v>
-      </c>
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
       <c r="I8" s="8" t="s">
         <v>26</v>
       </c>
@@ -1024,31 +992,12 @@
         <v>1</v>
       </c>
       <c r="K8" s="1"/>
-      <c r="L8" s="3"/>
+      <c r="L8" s="3">
+        <v>1.4224587097100299E-7</v>
+      </c>
       <c r="M8" s="1"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="1">
-        <v>0.94389038079999998</v>
-      </c>
-      <c r="C9" s="1">
-        <v>0.94388689830000005</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0.94388708779999997</v>
-      </c>
-      <c r="E9" s="1">
-        <v>-1.8957620710000001E-7</v>
-      </c>
-      <c r="F9" s="1">
-        <v>3.4825022610000002E-6</v>
-      </c>
-      <c r="G9" s="1">
-        <v>3.2929260540000001E-6</v>
-      </c>
       <c r="I9" s="8" t="s">
         <v>28</v>
       </c>
@@ -1056,7 +1005,9 @@
         <v>0.96399318562929603</v>
       </c>
       <c r="K9" s="1"/>
-      <c r="L9" s="3"/>
+      <c r="L9" s="3">
+        <v>5.0522178718370704E-7</v>
+      </c>
       <c r="M9" s="1"/>
     </row>
   </sheetData>
@@ -1064,6 +1015,7 @@
     <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Debug central rectangular SE by converting central polar SE results
Idea: to debug the centralized rectangular SE, take the measurements of
the central polar SE and convert them into rectangular form. Need to
first go back to the master branch though.
</commit_message>
<xml_diff>
--- a/DMASE - Test Results.xlsx
+++ b/DMASE - Test Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="18195" windowHeight="7740"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="18195" windowHeight="7740" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="2 Bus" sheetId="4" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="90">
   <si>
     <t>Abur 3-Bus Case Measurements (run through SE, rerun new estimate again)</t>
   </si>
@@ -268,6 +268,24 @@
   </si>
   <si>
     <t>Q1</t>
+  </si>
+  <si>
+    <t>e1</t>
+  </si>
+  <si>
+    <t>e2</t>
+  </si>
+  <si>
+    <t>e3</t>
+  </si>
+  <si>
+    <t>f1</t>
+  </si>
+  <si>
+    <t>f2</t>
+  </si>
+  <si>
+    <t>f3</t>
   </si>
 </sst>
 </file>
@@ -431,18 +449,6 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -465,6 +471,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="11" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -770,7 +788,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -784,15 +802,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
       <c r="I1" s="6" t="s">
         <v>1</v>
       </c>
@@ -1023,8 +1041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:N9"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1040,15 +1058,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
+      <c r="A1" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
       <c r="I1" s="6" t="s">
         <v>1</v>
       </c>
@@ -1401,15 +1419,15 @@
       <c r="N11" s="1"/>
     </row>
     <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
       <c r="I12" s="1"/>
       <c r="J12" s="6" t="s">
         <v>1</v>
@@ -1445,7 +1463,7 @@
       <c r="J13" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="K13" s="20">
+      <c r="K13" s="16">
         <f>48.6441515966896/100</f>
         <v>0.48644151596689605</v>
       </c>
@@ -1481,7 +1499,7 @@
       <c r="J14" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="K14" s="21">
+      <c r="K14" s="17">
         <f>41.9683612159875/100</f>
         <v>0.41968361215987499</v>
       </c>
@@ -1521,7 +1539,7 @@
       <c r="J15" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="K15" s="20">
+      <c r="K15" s="16">
         <f>-40/100</f>
         <v>-0.4</v>
       </c>
@@ -1561,7 +1579,7 @@
       <c r="J16" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K16" s="21">
+      <c r="K16" s="17">
         <f>1.44776824615491/100</f>
         <v>1.44776824615491E-2</v>
       </c>
@@ -1601,7 +1619,7 @@
       <c r="J17" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="K17" s="21">
+      <c r="K17" s="17">
         <f>0.209417870761202/100</f>
         <v>2.0941787076120201E-3</v>
       </c>
@@ -1641,7 +1659,7 @@
       <c r="J18" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="K18" s="20">
+      <c r="K18" s="16">
         <v>0</v>
       </c>
       <c r="L18" s="1">
@@ -1680,7 +1698,7 @@
       <c r="J19" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="K19" s="20">
+      <c r="K19" s="16">
         <v>1</v>
       </c>
       <c r="L19" s="1">
@@ -1703,10 +1721,10 @@
       <c r="C20" s="1">
         <v>0.99143333180000004</v>
       </c>
-      <c r="D20" s="19">
+      <c r="D20" s="15">
         <v>-2.6933805729999998</v>
       </c>
-      <c r="E20" s="23">
+      <c r="E20" s="19">
         <v>3.6848139049999999</v>
       </c>
       <c r="F20" s="3">
@@ -1719,7 +1737,7 @@
       <c r="J20" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="K20" s="21">
+      <c r="K20" s="17">
         <v>0.99480618409400001</v>
       </c>
       <c r="L20" s="1">
@@ -1899,15 +1917,15 @@
       <c r="G31" s="1"/>
     </row>
     <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="16" t="s">
+      <c r="A32" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="B32" s="16"/>
-      <c r="C32" s="16"/>
-      <c r="D32" s="16"/>
-      <c r="E32" s="16"/>
-      <c r="F32" s="16"/>
-      <c r="G32" s="16"/>
+      <c r="B32" s="26"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="26"/>
+      <c r="G32" s="26"/>
       <c r="I32" s="1"/>
       <c r="J32" s="6" t="s">
         <v>1</v>
@@ -1943,19 +1961,15 @@
       <c r="J33" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="K33" s="20">
+      <c r="K33" s="16">
         <f>48.6441515966896/100</f>
         <v>0.48644151596689605</v>
       </c>
       <c r="L33" s="1">
         <v>0.48125000969999998</v>
       </c>
-      <c r="M33" s="3">
-        <v>2.5799999999999999E-6</v>
-      </c>
-      <c r="N33" s="3">
-        <v>5.62E-9</v>
-      </c>
+      <c r="M33" s="3"/>
+      <c r="N33" s="3"/>
     </row>
     <row r="34" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="6"/>
@@ -1979,27 +1993,21 @@
       <c r="J34" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="K34" s="21">
+      <c r="K34" s="17">
         <f>41.9683612159875/100</f>
         <v>0.41968361215987499</v>
       </c>
       <c r="L34" s="1">
         <v>0.41874999619999997</v>
       </c>
-      <c r="M34" s="3">
-        <v>-4.0200000000000003E-7</v>
-      </c>
-      <c r="N34" s="3">
-        <v>-2.5500000000000001E-9</v>
-      </c>
+      <c r="M34" s="3"/>
+      <c r="N34" s="3"/>
     </row>
     <row r="35" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B35" s="1">
-        <v>0</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="B35" s="1"/>
       <c r="C35" s="1">
         <v>0</v>
       </c>
@@ -2019,216 +2027,134 @@
       <c r="J35" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="K35" s="20">
+      <c r="K35" s="16">
         <f>-40/100</f>
         <v>-0.4</v>
       </c>
       <c r="L35" s="1">
         <v>-0.4</v>
       </c>
-      <c r="M35" s="3">
-        <v>-7.8999999999999995E-7</v>
-      </c>
-      <c r="N35" s="3">
-        <v>6.3899999999999996E-9</v>
-      </c>
+      <c r="M35" s="3"/>
+      <c r="N35" s="3"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B36" s="1">
-        <v>-1.45245088402107E-2</v>
-      </c>
-      <c r="C36" s="1">
-        <v>-1.453480387E-2</v>
-      </c>
-      <c r="D36" s="1">
-        <v>-1.449120355E-2</v>
-      </c>
-      <c r="E36" s="1">
-        <v>-4.3600324780000002E-5</v>
-      </c>
-      <c r="F36" s="3">
-        <v>9.2199999999999998E-6</v>
-      </c>
-      <c r="G36" s="3">
-        <v>-3.4400000000000003E-5</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
       <c r="I36" s="1"/>
       <c r="J36" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K36" s="21">
+      <c r="K36" s="17">
         <f>1.44776824615491/100</f>
         <v>1.44776824615491E-2</v>
       </c>
       <c r="L36" s="1">
         <v>0</v>
       </c>
-      <c r="M36" s="3">
-        <v>-8.8800000000000004E-5</v>
-      </c>
-      <c r="N36" s="1">
-        <v>0</v>
-      </c>
+      <c r="M36" s="3"/>
+      <c r="N36" s="1"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B37" s="1">
-        <v>-2.1118662608655699E-2</v>
-      </c>
-      <c r="C37" s="1">
-        <v>-2.1131558979999999E-2</v>
-      </c>
-      <c r="D37" s="1">
-        <v>-4.9006550730000001E-2</v>
-      </c>
-      <c r="E37" s="1">
-        <v>2.7874991740000001E-2</v>
-      </c>
-      <c r="F37" s="3">
-        <v>1.13E-5</v>
-      </c>
-      <c r="G37" s="3">
-        <v>2.7900000000000001E-2</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
       <c r="I37" s="1"/>
       <c r="J37" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="K37" s="21">
+      <c r="K37" s="17">
         <f>0.209417870761202/100</f>
         <v>2.0941787076120201E-3</v>
       </c>
       <c r="L37" s="1">
         <v>0</v>
       </c>
-      <c r="M37" s="3">
-        <v>4.07E-5</v>
-      </c>
-      <c r="N37" s="1">
-        <v>0</v>
-      </c>
+      <c r="M37" s="3"/>
+      <c r="N37" s="1"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>23</v>
+        <v>87</v>
       </c>
       <c r="B38" s="1">
-        <v>0.999998359536033</v>
-      </c>
-      <c r="C38" s="1">
-        <v>0.99971783469999997</v>
-      </c>
-      <c r="D38" s="1">
-        <v>1.001140192</v>
-      </c>
-      <c r="E38" s="1">
-        <v>-1.422356891E-3</v>
-      </c>
-      <c r="F38" s="3">
-        <v>2.8400000000000002E-4</v>
-      </c>
-      <c r="G38" s="3">
-        <v>-1.14E-3</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
       <c r="I38" s="1"/>
       <c r="J38" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="K38" s="20">
+      <c r="K38" s="16">
         <v>0</v>
       </c>
       <c r="L38" s="1">
         <v>0</v>
       </c>
-      <c r="M38" s="1">
-        <v>-1.016250469E-4</v>
-      </c>
-      <c r="N38" s="1">
-        <v>0</v>
-      </c>
+      <c r="M38" s="1"/>
+      <c r="N38" s="1"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B39" s="1">
-        <v>0.99480759668265895</v>
-      </c>
-      <c r="C39" s="1">
-        <v>0.99453388529999998</v>
-      </c>
-      <c r="D39" s="1">
-        <v>0.99596625130000005</v>
-      </c>
-      <c r="E39" s="1">
-        <v>-1.4323660430000001E-3</v>
-      </c>
-      <c r="F39" s="3">
-        <v>2.8200000000000002E-4</v>
-      </c>
-      <c r="G39" s="3">
-        <v>-1.15E-3</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
       <c r="I39" s="1"/>
       <c r="J39" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="K39" s="20">
+      <c r="K39" s="16">
         <v>1</v>
       </c>
       <c r="L39" s="1">
         <v>1</v>
       </c>
-      <c r="M39" s="3">
-        <v>-1.42E-6</v>
-      </c>
-      <c r="N39" s="1">
-        <v>0</v>
-      </c>
+      <c r="M39" s="3"/>
+      <c r="N39" s="1"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B40" s="1">
-        <v>0.99171870097681902</v>
-      </c>
-      <c r="C40" s="1">
-        <v>0.99143333180000004</v>
-      </c>
-      <c r="D40" s="19">
-        <v>-2.6933805729999998</v>
-      </c>
-      <c r="E40" s="23">
-        <v>3.6848139049999999</v>
-      </c>
-      <c r="F40" s="3">
-        <v>2.9100000000000003E-4</v>
-      </c>
-      <c r="G40" s="3">
-        <v>3.69</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
       <c r="I40" s="1"/>
       <c r="J40" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="K40" s="21">
+      <c r="K40" s="17">
         <v>0.99480618409400001</v>
       </c>
       <c r="L40" s="1">
         <v>1</v>
       </c>
-      <c r="M40" s="3">
-        <v>1.2300000000000001E-6</v>
-      </c>
-      <c r="N40" s="1">
-        <v>0</v>
-      </c>
+      <c r="M40" s="3"/>
+      <c r="N40" s="1"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="J41" s="8"/>
@@ -2272,15 +2198,9 @@
       <c r="A44" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B44" s="1">
-        <v>0</v>
-      </c>
-      <c r="C44" s="1">
-        <v>0</v>
-      </c>
-      <c r="D44" s="1">
-        <v>0</v>
-      </c>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
@@ -2289,61 +2209,31 @@
       <c r="A45" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B45" s="1">
-        <v>-1.443750012E-2</v>
-      </c>
-      <c r="C45" s="1">
-        <v>-1.443750029E-2</v>
-      </c>
-      <c r="D45" s="1">
-        <v>-1.443749678E-2</v>
-      </c>
-      <c r="E45" s="3">
-        <v>-3.5100000000000001E-9</v>
-      </c>
-      <c r="F45" s="3">
-        <v>1.6900000000000001E-10</v>
-      </c>
-      <c r="G45" s="3">
-        <v>-3.34E-9</v>
-      </c>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B46" s="1">
-        <v>-2.093749994E-2</v>
-      </c>
-      <c r="C46" s="1">
-        <v>-2.0937501349999998E-2</v>
-      </c>
-      <c r="D46" s="1">
-        <v>-2.0937470489999999E-2</v>
-      </c>
-      <c r="E46" s="3">
-        <v>-3.0899999999999999E-8</v>
-      </c>
-      <c r="F46" s="3">
-        <v>1.4100000000000001E-9</v>
-      </c>
-      <c r="G46" s="3">
-        <v>-2.9499999999999999E-8</v>
-      </c>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B47" s="1">
-        <v>1</v>
-      </c>
-      <c r="C47" s="1">
-        <v>1</v>
-      </c>
-      <c r="D47" s="1">
-        <v>1</v>
-      </c>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
@@ -2352,15 +2242,9 @@
       <c r="A48" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B48" s="1">
-        <v>1</v>
-      </c>
-      <c r="C48" s="1">
-        <v>1</v>
-      </c>
-      <c r="D48" s="1">
-        <v>1</v>
-      </c>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
@@ -2369,15 +2253,9 @@
       <c r="A49" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B49" s="1">
-        <v>1</v>
-      </c>
-      <c r="C49" s="1">
-        <v>1</v>
-      </c>
-      <c r="D49" s="1">
-        <v>1</v>
-      </c>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
@@ -2392,20 +2270,20 @@
       <c r="G50" s="1"/>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A51" s="24"/>
-      <c r="B51" s="24"/>
-      <c r="C51" s="24"/>
-      <c r="D51" s="24"/>
-      <c r="E51" s="24"/>
-      <c r="F51" s="24"/>
-      <c r="G51" s="24"/>
-      <c r="H51" s="24"/>
-      <c r="I51" s="24"/>
-      <c r="J51" s="26"/>
-      <c r="K51" s="25"/>
-      <c r="L51" s="27"/>
-      <c r="M51" s="28"/>
-      <c r="N51" s="27"/>
+      <c r="A51" s="20"/>
+      <c r="B51" s="20"/>
+      <c r="C51" s="20"/>
+      <c r="D51" s="20"/>
+      <c r="E51" s="20"/>
+      <c r="F51" s="20"/>
+      <c r="G51" s="20"/>
+      <c r="H51" s="20"/>
+      <c r="I51" s="20"/>
+      <c r="J51" s="22"/>
+      <c r="K51" s="21"/>
+      <c r="L51" s="23"/>
+      <c r="M51" s="24"/>
+      <c r="N51" s="23"/>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
@@ -2452,18 +2330,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
       <c r="L1" s="11" t="s">
         <v>1</v>
       </c>
@@ -2476,7 +2354,7 @@
       <c r="O1" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="Q1" s="22" t="s">
+      <c r="Q1" s="18" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2487,18 +2365,18 @@
       <c r="B2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18" t="s">
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
       <c r="L2" s="8" t="s">
         <v>41</v>
       </c>
@@ -3291,18 +3169,18 @@
       <c r="O33" s="1"/>
     </row>
     <row r="35" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="17" t="s">
+      <c r="A35" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="B35" s="17"/>
-      <c r="C35" s="17"/>
-      <c r="D35" s="17"/>
-      <c r="E35" s="17"/>
-      <c r="F35" s="17"/>
-      <c r="G35" s="17"/>
-      <c r="H35" s="17"/>
-      <c r="I35" s="17"/>
-      <c r="J35" s="17"/>
+      <c r="B35" s="27"/>
+      <c r="C35" s="27"/>
+      <c r="D35" s="27"/>
+      <c r="E35" s="27"/>
+      <c r="F35" s="27"/>
+      <c r="G35" s="27"/>
+      <c r="H35" s="27"/>
+      <c r="I35" s="27"/>
+      <c r="J35" s="27"/>
       <c r="L35" s="11" t="s">
         <v>1</v>
       </c>
@@ -3755,7 +3633,7 @@
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
       <c r="I48" s="1">
-        <f t="shared" ref="I44:I51" si="10">B48-E48</f>
+        <f t="shared" ref="I48:I51" si="10">B48-E48</f>
         <v>-0.27861163064252253</v>
       </c>
       <c r="J48" s="1">

</xml_diff>

<commit_message>
Fixed h PF and QF; changed H PF and QF also
Confirmed that the h PF and QF functions are fixed, using what I know to
be correct values for the 3 bus case. Also derived the equations for the
H matrix, but haven't checked/debugged yet. Also need to type up the
rectangular derivations so that they're in the .docx.
</commit_message>
<xml_diff>
--- a/DMASE - Test Results.xlsx
+++ b/DMASE - Test Results.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="18195" windowHeight="7740" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="18195" windowHeight="7740" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="2 Bus" sheetId="4" r:id="rId1"/>
     <sheet name="3 Bus" sheetId="1" r:id="rId2"/>
     <sheet name="14 Bus DC" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="103">
   <si>
     <t>Abur 3-Bus Case Measurements (run through SE, rerun new estimate again)</t>
   </si>
@@ -286,6 +287,45 @@
   </si>
   <si>
     <t>f3</t>
+  </si>
+  <si>
+    <t>Polar 3 Bus SE Results</t>
+  </si>
+  <si>
+    <t>th1</t>
+  </si>
+  <si>
+    <t>th2</t>
+  </si>
+  <si>
+    <t>th3</t>
+  </si>
+  <si>
+    <t>V3</t>
+  </si>
+  <si>
+    <t>h1</t>
+  </si>
+  <si>
+    <t>h2</t>
+  </si>
+  <si>
+    <t>Iter 1</t>
+  </si>
+  <si>
+    <t>Iter 2</t>
+  </si>
+  <si>
+    <t>Iter 3</t>
+  </si>
+  <si>
+    <t>H1</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>Rectangular 3 Bus SE Results</t>
   </si>
 </sst>
 </file>
@@ -354,7 +394,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -367,8 +407,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -405,11 +451,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -483,6 +538,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1041,8 +1111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3907,4 +3977,783 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Y19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P24" sqref="P24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="F1" s="33" t="s">
+        <v>100</v>
+      </c>
+      <c r="G1" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="H1" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="I1" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="O1" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
+      <c r="T1" s="33" t="s">
+        <v>100</v>
+      </c>
+      <c r="U1" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="V1" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="W1" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="X1" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y1" s="34" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F2" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2">
+        <v>-30</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>10</v>
+      </c>
+      <c r="J2">
+        <v>-10</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="O2" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="T2" s="35" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A3" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="F3" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>-17.241379310344801</v>
+      </c>
+      <c r="I3">
+        <v>6.8965517241379297</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>-6.8965517241379297</v>
+      </c>
+      <c r="O3" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>1.0000159740000001</v>
+      </c>
+      <c r="R3">
+        <v>0.99999836200000003</v>
+      </c>
+      <c r="T3" s="35" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A4" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>-1.44481943076977E-2</v>
+      </c>
+      <c r="D4">
+        <v>-1.4524510647090099E-2</v>
+      </c>
+      <c r="F4" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4">
+        <v>40.958904109589</v>
+      </c>
+      <c r="H4">
+        <v>-10.958904109589</v>
+      </c>
+      <c r="I4">
+        <v>-10</v>
+      </c>
+      <c r="J4">
+        <v>14.1095890410959</v>
+      </c>
+      <c r="K4">
+        <v>-4.10958904109589</v>
+      </c>
+      <c r="O4" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4">
+        <v>0.99468638042393098</v>
+      </c>
+      <c r="R4">
+        <v>0.99470266483328695</v>
+      </c>
+      <c r="T4" s="35" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A5" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>-2.0940968386111598E-2</v>
+      </c>
+      <c r="D5">
+        <v>-2.11187041112352E-2</v>
+      </c>
+      <c r="F5" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5">
+        <v>10</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>30</v>
+      </c>
+      <c r="J5">
+        <v>-30</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="O5" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5">
+        <v>0.991243095267207</v>
+      </c>
+      <c r="R5">
+        <v>0.99149753812235297</v>
+      </c>
+      <c r="T5" s="35" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A6" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1.0000159739263801</v>
+      </c>
+      <c r="D6">
+        <v>0.999998361958229</v>
+      </c>
+      <c r="F6" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>6.8965517241379297</v>
+      </c>
+      <c r="I6">
+        <v>17.241379310344801</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>-17.241379310344801</v>
+      </c>
+      <c r="O6" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="T6" s="35" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A7" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>0.99479021016761804</v>
+      </c>
+      <c r="D7">
+        <v>0.99480759604436597</v>
+      </c>
+      <c r="F7" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7">
+        <v>-14.1095890410959</v>
+      </c>
+      <c r="H7">
+        <v>4.10958904109589</v>
+      </c>
+      <c r="I7">
+        <v>-30</v>
+      </c>
+      <c r="J7">
+        <v>40.958904109589</v>
+      </c>
+      <c r="K7">
+        <v>-10.958904109589</v>
+      </c>
+      <c r="O7" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>-1.43724218899485E-2</v>
+      </c>
+      <c r="R7">
+        <v>-1.44485858427847E-2</v>
+      </c>
+      <c r="T7" s="35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A8" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>0.99146047672768101</v>
+      </c>
+      <c r="D8">
+        <v>0.99171868270373598</v>
+      </c>
+      <c r="F8" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="O8" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>-2.0760624705304199E-2</v>
+      </c>
+      <c r="R8">
+        <v>-2.0942256529998499E-2</v>
+      </c>
+      <c r="T8" s="35" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="F9" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="T9" s="35" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F11" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="G11" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="H11" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="I11" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="J11" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="K11" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="T11" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="U11" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="V11" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="W11" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="X11" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y11" s="34" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A12" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0.48447633821146102</v>
+      </c>
+      <c r="F12" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12">
+        <v>-29.9847946068483</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>10.4846283386095</v>
+      </c>
+      <c r="J12">
+        <v>-9.5656783165009998</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="O12" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="T12" s="35" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A13" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0.41845110934032098</v>
+      </c>
+      <c r="F13" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>-17.233850201992599</v>
+      </c>
+      <c r="I13">
+        <v>7.3151063142873403</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>-6.5341192096312</v>
+      </c>
+      <c r="O13" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="T13" s="35" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A14" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>-0.39825059982490402</v>
+      </c>
+      <c r="F14" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14">
+        <v>40.532144770520901</v>
+      </c>
+      <c r="H14">
+        <v>-10.834803199321501</v>
+      </c>
+      <c r="I14">
+        <v>-10.3780364718241</v>
+      </c>
+      <c r="J14">
+        <v>13.635744779928901</v>
+      </c>
+      <c r="K14">
+        <v>-4.0173102798797702</v>
+      </c>
+      <c r="O14" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="T14" s="35" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A15" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>1.6163836389676299E-2</v>
+      </c>
+      <c r="F15" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15">
+        <v>9.51584314286786</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>30.016642795985302</v>
+      </c>
+      <c r="J15">
+        <v>-30.1418271916809</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="O15" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="T15" s="35" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A16" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>8.0799377993478992E-3</v>
+      </c>
+      <c r="F16" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>6.4783209465764502</v>
+      </c>
+      <c r="I16">
+        <v>17.2497345316017</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>-17.3822866433092</v>
+      </c>
+      <c r="O16" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="T16" s="35" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="31">
+        <v>1.7763568394002501E-15</v>
+      </c>
+      <c r="C17">
+        <v>1.0964776099249901E-3</v>
+      </c>
+      <c r="F17" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="G17">
+        <v>-14.361206615067299</v>
+      </c>
+      <c r="H17">
+        <v>3.9830043652526101</v>
+      </c>
+      <c r="I17">
+        <v>-29.696867195629</v>
+      </c>
+      <c r="J17">
+        <v>40.746619047357598</v>
+      </c>
+      <c r="K17">
+        <v>-10.928124169994</v>
+      </c>
+      <c r="O17" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="P17" s="31">
+        <v>1.7763568394002501E-15</v>
+      </c>
+      <c r="T17" s="35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>1.0000159739263801</v>
+      </c>
+      <c r="F18" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="O18" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="P18">
+        <v>1</v>
+      </c>
+      <c r="T18" s="35" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A19" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>0.99479021016761804</v>
+      </c>
+      <c r="F19" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="O19" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="P19">
+        <v>1</v>
+      </c>
+      <c r="T19" s="35" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="O1:R1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Central rectangular SE is now working.
Debugged H PF and QF functions. Also fixed H P and Q functions (ECE 6320
slides were correct). Remember to change measurements for V to V^2 when
dealing with rectangular coordinates. The centralized rectangular SE is
now working.
</commit_message>
<xml_diff>
--- a/DMASE - Test Results.xlsx
+++ b/DMASE - Test Results.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="113">
   <si>
     <t>Abur 3-Bus Case Measurements (run through SE, rerun new estimate again)</t>
   </si>
@@ -325,7 +325,37 @@
     <t>H2</t>
   </si>
   <si>
-    <t>Rectangular 3 Bus SE Results</t>
+    <t>Correct Rectangular 3 Bus SE Results</t>
+  </si>
+  <si>
+    <t>h3</t>
+  </si>
+  <si>
+    <t>Correct h's</t>
+  </si>
+  <si>
+    <t>H3</t>
+  </si>
+  <si>
+    <t>Actual Rectangular 3 Bus SE Results</t>
+  </si>
+  <si>
+    <t>Iter 4</t>
+  </si>
+  <si>
+    <t>Actual h's</t>
+  </si>
+  <si>
+    <t>Convert to Polar</t>
+  </si>
+  <si>
+    <t>V1^2</t>
+  </si>
+  <si>
+    <t>V2^2</t>
+  </si>
+  <si>
+    <t>H</t>
   </si>
 </sst>
 </file>
@@ -464,7 +494,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -531,15 +561,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -555,6 +576,29 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -872,15 +916,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
       <c r="I1" s="6" t="s">
         <v>1</v>
       </c>
@@ -1128,15 +1172,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
+      <c r="A1" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
       <c r="I1" s="6" t="s">
         <v>1</v>
       </c>
@@ -1489,15 +1533,15 @@
       <c r="N11" s="1"/>
     </row>
     <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="B12" s="26"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
       <c r="I12" s="1"/>
       <c r="J12" s="6" t="s">
         <v>1</v>
@@ -1987,15 +2031,15 @@
       <c r="G31" s="1"/>
     </row>
     <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="26" t="s">
+      <c r="A32" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="B32" s="26"/>
-      <c r="C32" s="26"/>
-      <c r="D32" s="26"/>
-      <c r="E32" s="26"/>
-      <c r="F32" s="26"/>
-      <c r="G32" s="26"/>
+      <c r="B32" s="34"/>
+      <c r="C32" s="34"/>
+      <c r="D32" s="34"/>
+      <c r="E32" s="34"/>
+      <c r="F32" s="34"/>
+      <c r="G32" s="34"/>
       <c r="I32" s="1"/>
       <c r="J32" s="6" t="s">
         <v>1</v>
@@ -2400,18 +2444,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
       <c r="L1" s="11" t="s">
         <v>1</v>
       </c>
@@ -2435,18 +2479,18 @@
       <c r="B2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28" t="s">
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
       <c r="L2" s="8" t="s">
         <v>41</v>
       </c>
@@ -3239,18 +3283,18 @@
       <c r="O33" s="1"/>
     </row>
     <row r="35" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="27" t="s">
+      <c r="A35" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="B35" s="27"/>
-      <c r="C35" s="27"/>
-      <c r="D35" s="27"/>
-      <c r="E35" s="27"/>
-      <c r="F35" s="27"/>
-      <c r="G35" s="27"/>
-      <c r="H35" s="27"/>
-      <c r="I35" s="27"/>
-      <c r="J35" s="27"/>
+      <c r="B35" s="35"/>
+      <c r="C35" s="35"/>
+      <c r="D35" s="35"/>
+      <c r="E35" s="35"/>
+      <c r="F35" s="35"/>
+      <c r="G35" s="35"/>
+      <c r="H35" s="35"/>
+      <c r="I35" s="35"/>
+      <c r="J35" s="35"/>
       <c r="L35" s="11" t="s">
         <v>1</v>
       </c>
@@ -3981,70 +4025,73 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y19"/>
+  <dimension ref="A1:AA61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P24" sqref="P24"/>
+      <selection activeCell="T22" sqref="T22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" style="2"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="F1" s="33" t="s">
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="G1" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="H1" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="I1" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="I1" s="34" t="s">
+      <c r="J1" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="J1" s="34" t="s">
+      <c r="K1" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="K1" s="34" t="s">
+      <c r="L1" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="O1" s="25" t="s">
-        <v>102</v>
-      </c>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="T1" s="33" t="s">
+      <c r="P1" s="33" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q1" s="33"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
+      <c r="T1" s="33"/>
+      <c r="V1" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="U1" s="34" t="s">
-        <v>92</v>
-      </c>
-      <c r="V1" s="34" t="s">
-        <v>93</v>
-      </c>
-      <c r="W1" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="X1" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="Y1" s="34" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="W1" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="X1" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="Y1" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA1" s="31" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A2" s="27" t="s">
         <v>37</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -4056,42 +4103,63 @@
       <c r="D2" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="F2" s="35" t="s">
+      <c r="E2" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G2" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>-30</v>
       </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
       <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
         <v>10</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>-10</v>
       </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="O2" s="30" t="s">
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="P2" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="T2" s="35" t="s">
+      <c r="T2" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="V2" s="32" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
+      <c r="W2">
+        <v>10</v>
+      </c>
+      <c r="X2">
+        <v>-10</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>-30</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
         <v>91</v>
       </c>
       <c r="B3">
@@ -4103,42 +4171,63 @@
       <c r="D3">
         <v>0</v>
       </c>
-      <c r="F3" s="35" t="s">
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
       <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
         <v>-17.241379310344801</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>6.8965517241379297</v>
       </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
       <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
         <v>-6.8965517241379297</v>
       </c>
-      <c r="O3" s="29" t="s">
+      <c r="P3" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>1</v>
       </c>
-      <c r="Q3">
-        <v>1.0000159740000001</v>
-      </c>
       <c r="R3">
-        <v>0.99999836200000003</v>
-      </c>
-      <c r="T3" s="35" t="s">
+        <v>1.0000226416499201</v>
+      </c>
+      <c r="S3">
+        <v>0.99999845433530399</v>
+      </c>
+      <c r="T3">
+        <v>0.99999845426357303</v>
+      </c>
+      <c r="V3" s="32" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
+      <c r="W3">
+        <v>6.8965517241379297</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <v>-6.8965517241379297</v>
+      </c>
+      <c r="Z3">
+        <v>0</v>
+      </c>
+      <c r="AA3">
+        <v>-17.241379310344801</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
         <v>92</v>
       </c>
       <c r="B4">
@@ -4150,42 +4239,63 @@
       <c r="D4">
         <v>-1.4524510647090099E-2</v>
       </c>
-      <c r="F4" s="35" t="s">
+      <c r="E4">
+        <v>-1.45245088402107E-2</v>
+      </c>
+      <c r="G4" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>40.958904109589</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>-10.958904109589</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>-10</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>14.1095890410959</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>-4.10958904109589</v>
       </c>
-      <c r="O4" s="29" t="s">
+      <c r="P4" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>1</v>
       </c>
-      <c r="Q4">
-        <v>0.99468638042393098</v>
-      </c>
       <c r="R4">
-        <v>0.99470266483328695</v>
-      </c>
-      <c r="T4" s="35" t="s">
+        <v>0.99479703030591204</v>
+      </c>
+      <c r="S4">
+        <v>0.99470275639643102</v>
+      </c>
+      <c r="T4">
+        <v>0.99470275148962295</v>
+      </c>
+      <c r="V4" s="32" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
+      <c r="W4">
+        <v>-10</v>
+      </c>
+      <c r="X4" s="38">
+        <v>14.1095890410959</v>
+      </c>
+      <c r="Y4">
+        <v>-4.10958904109589</v>
+      </c>
+      <c r="Z4">
+        <v>40.958904109589</v>
+      </c>
+      <c r="AA4">
+        <v>-10.958904109589</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
         <v>93</v>
       </c>
       <c r="B5">
@@ -4197,42 +4307,63 @@
       <c r="D5">
         <v>-2.11187041112352E-2</v>
       </c>
-      <c r="F5" s="35" t="s">
+      <c r="E5">
+        <v>-2.1118662608655699E-2</v>
+      </c>
+      <c r="G5" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>10</v>
       </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
       <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
         <v>30</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>-30</v>
       </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="O5" s="29" t="s">
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="P5" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>1</v>
       </c>
-      <c r="Q5">
-        <v>0.991243095267207</v>
-      </c>
       <c r="R5">
-        <v>0.99149753812235297</v>
-      </c>
-      <c r="T5" s="35" t="s">
+        <v>0.99146725876561503</v>
+      </c>
+      <c r="S5">
+        <v>0.99149764207917701</v>
+      </c>
+      <c r="T5">
+        <v>0.99149764559215503</v>
+      </c>
+      <c r="V5" s="32" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
+      <c r="W5">
+        <v>30</v>
+      </c>
+      <c r="X5">
+        <v>-30</v>
+      </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>10</v>
+      </c>
+      <c r="AA5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
         <v>26</v>
       </c>
       <c r="B6">
@@ -4244,42 +4375,63 @@
       <c r="D6">
         <v>0.999998361958229</v>
       </c>
-      <c r="F6" s="35" t="s">
+      <c r="E6">
+        <v>0.999998359536033</v>
+      </c>
+      <c r="G6" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
       <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
         <v>6.8965517241379297</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>17.241379310344801</v>
       </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
       <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
         <v>-17.241379310344801</v>
       </c>
-      <c r="O6" s="29" t="s">
+      <c r="P6" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
       <c r="Q6">
         <v>0</v>
       </c>
       <c r="R6">
         <v>0</v>
       </c>
-      <c r="T6" s="35" t="s">
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="V6" s="32" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A7" s="29" t="s">
+      <c r="W6">
+        <v>17.241379310344801</v>
+      </c>
+      <c r="X6">
+        <v>0</v>
+      </c>
+      <c r="Y6">
+        <v>-17.241379310344801</v>
+      </c>
+      <c r="Z6">
+        <v>0</v>
+      </c>
+      <c r="AA6">
+        <v>6.8965517241379297</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A7" s="26" t="s">
         <v>28</v>
       </c>
       <c r="B7">
@@ -4291,42 +4443,63 @@
       <c r="D7">
         <v>0.99480759604436597</v>
       </c>
-      <c r="F7" s="35" t="s">
+      <c r="E7">
+        <v>0.99480759668265895</v>
+      </c>
+      <c r="G7" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>-14.1095890410959</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>4.10958904109589</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>-30</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>40.958904109589</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>-10.958904109589</v>
       </c>
-      <c r="O7" s="29" t="s">
+      <c r="P7" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="P7">
-        <v>0</v>
-      </c>
       <c r="Q7">
-        <v>-1.43724218899485E-2</v>
+        <v>0</v>
       </c>
       <c r="R7">
-        <v>-1.44485858427847E-2</v>
-      </c>
-      <c r="T7" s="35" t="s">
+        <v>-1.44481943076977E-2</v>
+      </c>
+      <c r="S7">
+        <v>-1.4448582316564E-2</v>
+      </c>
+      <c r="T7">
+        <v>-1.44485822804116E-2</v>
+      </c>
+      <c r="V7" s="32" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
+      <c r="W7">
+        <v>-30</v>
+      </c>
+      <c r="X7" s="39">
+        <v>40.958904109589</v>
+      </c>
+      <c r="Y7">
+        <v>-10.958904109589</v>
+      </c>
+      <c r="Z7">
+        <v>-14.1095890410959</v>
+      </c>
+      <c r="AA7">
+        <v>4.10958904109589</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A8" s="26" t="s">
         <v>94</v>
       </c>
       <c r="B8">
@@ -4338,47 +4511,65 @@
       <c r="D8">
         <v>0.99171868270373598</v>
       </c>
-      <c r="F8" s="35" t="s">
+      <c r="E8">
+        <v>0.99171870097681902</v>
+      </c>
+      <c r="G8" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
       <c r="H8">
         <v>0</v>
       </c>
       <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
         <v>1</v>
       </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
       <c r="K8">
         <v>0</v>
       </c>
-      <c r="O8" s="29" t="s">
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="P8" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="P8">
-        <v>0</v>
-      </c>
       <c r="Q8">
-        <v>-2.0760624705304199E-2</v>
+        <v>0</v>
       </c>
       <c r="R8">
-        <v>-2.0942256529998499E-2</v>
-      </c>
-      <c r="T8" s="35" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="F9" s="35" t="s">
+        <v>-2.09409714756899E-2</v>
+      </c>
+      <c r="S8">
+        <v>-2.0942213484145999E-2</v>
+      </c>
+      <c r="T8">
+        <v>-2.0942213598037301E-2</v>
+      </c>
+      <c r="V8" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="W8" s="2">
+        <v>2</v>
+      </c>
+      <c r="X8">
+        <v>0</v>
+      </c>
+      <c r="Y8">
+        <v>0</v>
+      </c>
+      <c r="Z8">
+        <v>0</v>
+      </c>
+      <c r="AA8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="G9" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
       <c r="H9">
         <v>0</v>
       </c>
@@ -4386,67 +4577,100 @@
         <v>0</v>
       </c>
       <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
         <v>1</v>
       </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="T9" s="35" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="V9" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="W9">
+        <v>0</v>
+      </c>
+      <c r="X9" s="2">
+        <v>2</v>
+      </c>
+      <c r="Y9">
+        <v>0</v>
+      </c>
+      <c r="Z9">
+        <v>0</v>
+      </c>
+      <c r="AA9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="P10" s="33" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q10" s="33"/>
+      <c r="R10" s="33"/>
+      <c r="S10" s="33"/>
+      <c r="T10" s="25"/>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>95</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="F11" s="33" t="s">
+      <c r="D11" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G11" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="G11" s="34" t="s">
+      <c r="H11" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="H11" s="34" t="s">
+      <c r="I11" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="I11" s="34" t="s">
+      <c r="J11" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="J11" s="34" t="s">
+      <c r="K11" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="K11" s="34" t="s">
+      <c r="L11" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="P11" s="1" t="s">
+      <c r="Q11" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="Q11" s="1" t="s">
+      <c r="R11" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="T11" s="33" t="s">
+      <c r="S11" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="V11" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="U11" s="34" t="s">
-        <v>92</v>
-      </c>
-      <c r="V11" s="34" t="s">
-        <v>93</v>
-      </c>
-      <c r="W11" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="X11" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="Y11" s="34" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A12" s="32" t="s">
+      <c r="W11" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="X11" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="Y11" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z11" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA11" s="31" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A12" s="29" t="s">
         <v>12</v>
       </c>
       <c r="B12">
@@ -4455,36 +4679,60 @@
       <c r="C12">
         <v>0.48447633821146102</v>
       </c>
-      <c r="F12" s="35" t="s">
+      <c r="D12">
+        <v>0.48641373875914201</v>
+      </c>
+      <c r="G12" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>-29.9847946068483</v>
       </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
       <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
         <v>10.4846283386095</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>-9.5656783165009998</v>
       </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-      <c r="O12" s="32" t="s">
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="P12" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="P12">
-        <v>0</v>
-      </c>
-      <c r="T12" s="35" t="s">
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>0.48571293976437802</v>
+      </c>
+      <c r="S12">
+        <v>0.48641369705201498</v>
+      </c>
+      <c r="V12" s="32" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A13" s="32" t="s">
+      <c r="W12">
+        <v>10.485928359170201</v>
+      </c>
+      <c r="X12">
+        <v>-10.000226416499199</v>
+      </c>
+      <c r="Y12">
+        <v>0</v>
+      </c>
+      <c r="Z12">
+        <v>-30.000679249497601</v>
+      </c>
+      <c r="AA12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A13" s="29" t="s">
         <v>16</v>
       </c>
       <c r="B13">
@@ -4493,36 +4741,60 @@
       <c r="C13">
         <v>0.41845110934032098</v>
       </c>
-      <c r="F13" s="35" t="s">
+      <c r="D13">
+        <v>0.419699076096894</v>
+      </c>
+      <c r="G13" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
       <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
         <v>-17.233850201992599</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>7.3151063142873403</v>
       </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
       <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
         <v>-6.5341192096312</v>
       </c>
-      <c r="O13" s="32" t="s">
+      <c r="P13" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="P13">
-        <v>0</v>
-      </c>
-      <c r="T13" s="35" t="s">
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>0.42006338363364498</v>
+      </c>
+      <c r="S13">
+        <v>0.419698288986113</v>
+      </c>
+      <c r="V13" s="32" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A14" s="32" t="s">
+      <c r="W13">
+        <v>7.3167617463686403</v>
+      </c>
+      <c r="X13">
+        <v>0</v>
+      </c>
+      <c r="Y13">
+        <v>-6.8967078734477303</v>
+      </c>
+      <c r="Z13">
+        <v>0</v>
+      </c>
+      <c r="AA13">
+        <v>-17.2417696836193</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A14" s="29" t="s">
         <v>18</v>
       </c>
       <c r="B14">
@@ -4531,36 +4803,60 @@
       <c r="C14">
         <v>-0.39825059982490402</v>
       </c>
-      <c r="F14" s="35" t="s">
+      <c r="D14">
+        <v>-0.40003523389947299</v>
+      </c>
+      <c r="G14" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>40.532144770520901</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>-10.834803199321501</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>-10.3780364718241</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>13.635744779928901</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>-4.0173102798797702</v>
       </c>
-      <c r="O14" s="32" t="s">
+      <c r="P14" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="P14">
-        <v>0</v>
-      </c>
-      <c r="T14" s="35" t="s">
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>-0.39881435157154799</v>
+      </c>
+      <c r="S14">
+        <v>-0.40003567280852198</v>
+      </c>
+      <c r="V14" s="32" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A15" s="32" t="s">
+      <c r="W14">
+        <v>-10.381416132289999</v>
+      </c>
+      <c r="X14">
+        <v>14.227095254473999</v>
+      </c>
+      <c r="Y14">
+        <v>-4.2465433498346803</v>
+      </c>
+      <c r="Z14">
+        <v>40.544416484858502</v>
+      </c>
+      <c r="AA14">
+        <v>-10.842509122635899</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A15" s="29" t="s">
         <v>20</v>
       </c>
       <c r="B15">
@@ -4569,36 +4865,60 @@
       <c r="C15">
         <v>1.6163836389676299E-2</v>
       </c>
-      <c r="F15" s="35" t="s">
+      <c r="D15">
+        <v>1.43850337772129E-2</v>
+      </c>
+      <c r="G15" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>9.51584314286786</v>
       </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
       <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
         <v>30.016642795985302</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>-30.1418271916809</v>
       </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
-      <c r="O15" s="32" t="s">
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="P15" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="P15">
-        <v>0</v>
-      </c>
-      <c r="T15" s="35" t="s">
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>1.2286675427618099E-2</v>
+      </c>
+      <c r="S15">
+        <v>1.4385092766006E-2</v>
+      </c>
+      <c r="V15" s="32" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A16" s="32" t="s">
+      <c r="W15">
+        <v>30.012965646741002</v>
+      </c>
+      <c r="X15">
+        <v>-30.000679249497601</v>
+      </c>
+      <c r="Y15">
+        <v>0</v>
+      </c>
+      <c r="Z15">
+        <v>10.000226416499199</v>
+      </c>
+      <c r="AA15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A16" s="29" t="s">
         <v>22</v>
       </c>
       <c r="B16">
@@ -4607,74 +4927,122 @@
       <c r="C16">
         <v>8.0799377993478992E-3</v>
       </c>
-      <c r="F16" s="35" t="s">
+      <c r="D16">
+        <v>2.13657375520526E-3</v>
+      </c>
+      <c r="G16" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
       <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
         <v>6.4783209465764502</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>17.2497345316017</v>
       </c>
-      <c r="J16">
-        <v>0</v>
-      </c>
       <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
         <v>-17.3822866433092</v>
       </c>
-      <c r="O16" s="32" t="s">
+      <c r="P16" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="P16">
-        <v>0</v>
-      </c>
-      <c r="T16" s="35" t="s">
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <v>3.0861783923594199E-3</v>
+      </c>
+      <c r="S16">
+        <v>2.13666673998469E-3</v>
+      </c>
+      <c r="V16" s="32" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="32" t="s">
+      <c r="W16">
+        <v>17.244855792137098</v>
+      </c>
+      <c r="X16">
+        <v>0</v>
+      </c>
+      <c r="Y16">
+        <v>-17.2417696836193</v>
+      </c>
+      <c r="Z16">
+        <v>0</v>
+      </c>
+      <c r="AA16">
+        <v>6.8967078734477303</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A17" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="31">
+      <c r="B17" s="28">
         <v>1.7763568394002501E-15</v>
       </c>
       <c r="C17">
         <v>1.0964776099249901E-3</v>
       </c>
-      <c r="F17" s="35" t="s">
+      <c r="D17">
+        <v>-1.05718776926005E-4</v>
+      </c>
+      <c r="G17" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>-14.361206615067299</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>3.9830043652526101</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>-29.696867195629</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <v>40.746619047357598</v>
       </c>
-      <c r="K17">
+      <c r="L17">
         <v>-10.928124169994</v>
       </c>
-      <c r="O17" s="32" t="s">
+      <c r="P17" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="P17" s="31">
+      <c r="Q17" s="28">
         <v>1.7763568394002501E-15</v>
       </c>
-      <c r="T17" s="35" t="s">
+      <c r="R17">
+        <v>3.3262631497988399E-3</v>
+      </c>
+      <c r="S17">
+        <v>-1.05747606702557E-4</v>
+      </c>
+      <c r="V17" s="32" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="32" t="s">
+      <c r="W17">
+        <v>-29.699428966100399</v>
+      </c>
+      <c r="X17">
+        <v>40.539459692614003</v>
+      </c>
+      <c r="Y17">
+        <v>-10.842509122635899</v>
+      </c>
+      <c r="Z17">
+        <v>-15.0288237097754</v>
+      </c>
+      <c r="AA17">
+        <v>4.2465433498346803</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A18" s="29" t="s">
         <v>26</v>
       </c>
       <c r="B18">
@@ -4683,36 +5051,60 @@
       <c r="C18">
         <v>1.0000159739263801</v>
       </c>
-      <c r="F18" s="35" t="s">
+      <c r="D18">
+        <v>0.999998361958229</v>
+      </c>
+      <c r="G18" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
       <c r="H18">
         <v>0</v>
       </c>
       <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
         <v>1</v>
       </c>
-      <c r="J18">
-        <v>0</v>
-      </c>
       <c r="K18">
         <v>0</v>
       </c>
-      <c r="O18" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="P18">
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="P18" s="29" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q18">
         <v>1</v>
       </c>
-      <c r="T18" s="35" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="32" t="s">
+      <c r="R18">
+        <v>1.00004528381249</v>
+      </c>
+      <c r="S18">
+        <v>0.99999690867299795</v>
+      </c>
+      <c r="V18" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="W18">
+        <v>2.0000452832998401</v>
+      </c>
+      <c r="X18">
+        <v>0</v>
+      </c>
+      <c r="Y18">
+        <v>0</v>
+      </c>
+      <c r="Z18">
+        <v>0</v>
+      </c>
+      <c r="AA18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A19" s="29" t="s">
         <v>28</v>
       </c>
       <c r="B19">
@@ -4721,12 +5113,12 @@
       <c r="C19">
         <v>0.99479021016761804</v>
       </c>
-      <c r="F19" s="35" t="s">
+      <c r="D19">
+        <v>0.99480759604436597</v>
+      </c>
+      <c r="G19" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
       <c r="H19">
         <v>0</v>
       </c>
@@ -4734,25 +5126,1368 @@
         <v>0</v>
       </c>
       <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
         <v>1</v>
       </c>
-      <c r="K19">
-        <v>0</v>
-      </c>
-      <c r="O19" s="32" t="s">
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="P19" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q19">
+        <v>1</v>
+      </c>
+      <c r="R19">
+        <v>0.98982988182421405</v>
+      </c>
+      <c r="S19">
+        <v>0.98964233511361499</v>
+      </c>
+      <c r="V19" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="W19">
+        <v>0</v>
+      </c>
+      <c r="X19">
+        <v>1.9895940606118201</v>
+      </c>
+      <c r="Y19">
+        <v>0</v>
+      </c>
+      <c r="Z19">
+        <v>-2.8896388615395299E-2</v>
+      </c>
+      <c r="AA19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="G21" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="H21" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="I21" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="J21" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="K21" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="P19">
+      <c r="L21" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="T21" t="s">
+        <v>109</v>
+      </c>
+      <c r="V21" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="W21" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="X21" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="Y21" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z21" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA21" s="31" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="G22" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="H22">
+        <v>-29.985516683797002</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>10.4863981551088</v>
+      </c>
+      <c r="K22">
+        <v>-9.5632095475153402</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="P22" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="T22">
+        <f>ATAN(T6/T3)</f>
+        <v>0</v>
+      </c>
+      <c r="V22" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="W22">
+        <v>10.4863989922387</v>
+      </c>
+      <c r="X22">
+        <v>-9.9999845433530403</v>
+      </c>
+      <c r="Y22">
+        <v>0</v>
+      </c>
+      <c r="Z22">
+        <v>-29.9999536300591</v>
+      </c>
+      <c r="AA22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="G23" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>-17.239186252436902</v>
+      </c>
+      <c r="J23">
+        <v>7.3162401908807704</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>-6.5309146306713401</v>
+      </c>
+      <c r="P23" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="T23">
+        <f>ATAN(T7/T4)</f>
+        <v>-1.4524506154245323E-2</v>
+      </c>
+      <c r="V23" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="W23">
+        <v>7.3162400020813498</v>
+      </c>
+      <c r="X23">
+        <v>0</v>
+      </c>
+      <c r="Y23">
+        <v>-6.8965410643814096</v>
+      </c>
+      <c r="Z23">
+        <v>0</v>
+      </c>
+      <c r="AA23">
+        <v>-17.241352660953499</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="G24" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="H24">
+        <v>40.534763772355497</v>
+      </c>
+      <c r="I24">
+        <v>-10.8382183250586</v>
+      </c>
+      <c r="J24">
+        <v>-10.3804842135991</v>
+      </c>
+      <c r="K24">
+        <v>13.6342031350484</v>
+      </c>
+      <c r="L24">
+        <v>-4.0162721264518799</v>
+      </c>
+      <c r="P24" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="T24">
+        <f>ATAN(T8/T5)</f>
+        <v>-2.111865843078977E-2</v>
+      </c>
+      <c r="V24" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="W24">
+        <v>-10.3804850334612</v>
+      </c>
+      <c r="X24">
+        <v>14.2245655434992</v>
+      </c>
+      <c r="Y24">
+        <v>-4.2461601749613802</v>
+      </c>
+      <c r="Z24">
+        <v>40.544017988092897</v>
+      </c>
+      <c r="AA24">
+        <v>-10.841474389344899</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="G25" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="H25">
+        <v>9.5135535004322698</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>30.014335916087401</v>
+      </c>
+      <c r="K25">
+        <v>-30.142026260181201</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="P25" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="T25">
+        <f>SQRT(T3^2+T6^2)</f>
+        <v>0.99999845426357303</v>
+      </c>
+      <c r="V25" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="W25">
+        <v>30.0143387450597</v>
+      </c>
+      <c r="X25">
+        <v>-29.9999536300591</v>
+      </c>
+      <c r="Y25">
+        <v>0</v>
+      </c>
+      <c r="Z25">
+        <v>9.9999845433530403</v>
+      </c>
+      <c r="AA25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="G26" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>6.4768300543799402</v>
+      </c>
+      <c r="J26">
+        <v>17.243487645500299</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>-17.383141563328699</v>
+      </c>
+      <c r="P26" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="T26">
+        <f>SQRT(T4^2+T7^2)</f>
+        <v>0.99480768259545538</v>
+      </c>
+      <c r="V26" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="W26">
+        <v>17.243489330996098</v>
+      </c>
+      <c r="X26">
+        <v>0</v>
+      </c>
+      <c r="Y26">
+        <v>-17.241352660953499</v>
+      </c>
+      <c r="Z26">
+        <v>0</v>
+      </c>
+      <c r="AA26">
+        <v>6.8965410643814096</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="G27" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="H27">
+        <v>-14.363479312557001</v>
+      </c>
+      <c r="I27">
+        <v>3.9830121026245902</v>
+      </c>
+      <c r="J27">
+        <v>-29.696594091558602</v>
+      </c>
+      <c r="K27">
+        <v>40.746122663295303</v>
+      </c>
+      <c r="L27">
+        <v>-10.928722544089</v>
+      </c>
+      <c r="P27" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="T27">
+        <f>SQRT(T5^2+T8^2)</f>
+        <v>0.99171878953923853</v>
+      </c>
+      <c r="V27" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="W27">
+        <v>-29.696596868727301</v>
+      </c>
+      <c r="X27">
+        <v>40.532124528051398</v>
+      </c>
+      <c r="Y27">
+        <v>-10.841474389344899</v>
+      </c>
+      <c r="Z27">
+        <v>-15.028724873346</v>
+      </c>
+      <c r="AA27">
+        <v>4.2461601749613802</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="G28" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
         <v>1</v>
       </c>
-      <c r="T19" s="35" t="s">
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="V28" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="W28">
+        <v>1.99999690867061</v>
+      </c>
+      <c r="X28">
+        <v>0</v>
+      </c>
+      <c r="Y28">
+        <v>0</v>
+      </c>
+      <c r="Z28">
+        <v>0</v>
+      </c>
+      <c r="AA28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="G29" s="32" t="s">
         <v>28</v>
       </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <v>1</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="V29" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="W29">
+        <v>0</v>
+      </c>
+      <c r="X29">
+        <v>1.98940551279286</v>
+      </c>
+      <c r="Y29">
+        <v>0</v>
+      </c>
+      <c r="Z29">
+        <v>-2.8897164633128001E-2</v>
+      </c>
+      <c r="AA29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="P30" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>84</v>
+      </c>
+      <c r="R30" t="s">
+        <v>85</v>
+      </c>
+      <c r="S30" t="s">
+        <v>86</v>
+      </c>
+      <c r="T30" t="s">
+        <v>88</v>
+      </c>
+      <c r="U30" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="P31" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q31">
+        <v>10.484628332459099</v>
+      </c>
+      <c r="R31" s="2">
+        <v>-10.000159740000001</v>
+      </c>
+      <c r="S31">
+        <v>0</v>
+      </c>
+      <c r="T31" s="2">
+        <v>-30.000479219999999</v>
+      </c>
+      <c r="U31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="P32" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q32" s="40">
+        <v>7.3151063068693301</v>
+      </c>
+      <c r="R32" s="40">
+        <v>0</v>
+      </c>
+      <c r="S32" s="43">
+        <v>-6.8966618896551699</v>
+      </c>
+      <c r="T32" s="41">
+        <v>0</v>
+      </c>
+      <c r="U32" s="2">
+        <v>-17.241654724137899</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A33" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="B33" s="33"/>
+      <c r="C33" s="33"/>
+      <c r="D33" s="33"/>
+      <c r="F33" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="G33" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="H33" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="I33" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="J33" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="K33" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="P33" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q33" s="37">
+        <v>-10.3780364609378</v>
+      </c>
+      <c r="R33" s="44">
+        <v>14.222984299142199</v>
+      </c>
+      <c r="S33" s="44">
+        <v>-4.2452582416320297</v>
+      </c>
+      <c r="T33" s="45">
+        <v>40.543156953315901</v>
+      </c>
+      <c r="U33" s="2">
+        <v>-10.841607914687099</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A34" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F34" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="G34">
+        <v>10</v>
+      </c>
+      <c r="H34">
+        <v>-10</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <v>-30</v>
+      </c>
+      <c r="K34">
+        <v>0</v>
+      </c>
+      <c r="P34" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q34" s="37">
+        <v>30.016642808382599</v>
+      </c>
+      <c r="R34" s="45">
+        <v>-30.000479219999999</v>
+      </c>
+      <c r="S34" s="37">
+        <v>0</v>
+      </c>
+      <c r="T34" s="45">
+        <v>10.000159740000001</v>
+      </c>
+      <c r="U34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A35" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>1.0000159740000001</v>
+      </c>
+      <c r="D35">
+        <v>0.99999836200000003</v>
+      </c>
+      <c r="F35" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="G35">
+        <v>6.8965517241379297</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>-6.8965517241379297</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <v>-17.241379310344801</v>
+      </c>
+      <c r="P35" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q35" s="37">
+        <v>17.2497345319081</v>
+      </c>
+      <c r="R35" s="37">
+        <v>0</v>
+      </c>
+      <c r="S35" s="45">
+        <v>-17.241654724137899</v>
+      </c>
+      <c r="T35" s="41">
+        <v>0</v>
+      </c>
+      <c r="U35" s="2">
+        <v>6.8966618896551699</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A36" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>0.99468638042393098</v>
+      </c>
+      <c r="D36">
+        <v>0.99470266483328695</v>
+      </c>
+      <c r="F36" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="G36">
+        <v>-10</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <v>-4.10958904109589</v>
+      </c>
+      <c r="J36">
+        <v>40.958904109589</v>
+      </c>
+      <c r="K36">
+        <v>-10.958904109589</v>
+      </c>
+      <c r="P36" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q36" s="37">
+        <v>-29.696867193818498</v>
+      </c>
+      <c r="R36" s="45">
+        <v>40.533793263695202</v>
+      </c>
+      <c r="S36" s="45">
+        <v>-10.841607914687099</v>
+      </c>
+      <c r="T36" s="45">
+        <v>-15.023605105997399</v>
+      </c>
+      <c r="U36" s="2">
+        <v>4.2452582416320297</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A37" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <v>0.991243095267207</v>
+      </c>
+      <c r="D37">
+        <v>0.99149753812235297</v>
+      </c>
+      <c r="F37" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="G37">
+        <v>30</v>
+      </c>
+      <c r="H37">
+        <v>-30</v>
+      </c>
+      <c r="I37">
+        <v>0</v>
+      </c>
+      <c r="J37">
+        <v>10</v>
+      </c>
+      <c r="K37">
+        <v>0</v>
+      </c>
+      <c r="P37" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q37" s="42">
+        <v>2.0000319480000002</v>
+      </c>
+      <c r="R37" s="37">
+        <v>0</v>
+      </c>
+      <c r="S37" s="37">
+        <v>0</v>
+      </c>
+      <c r="T37" s="41">
+        <v>0</v>
+      </c>
+      <c r="U37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A38" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="F38" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="G38">
+        <v>17.241379310344801</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <v>-17.241379310344801</v>
+      </c>
+      <c r="J38">
+        <v>0</v>
+      </c>
+      <c r="K38">
+        <v>6.8965517241379297</v>
+      </c>
+      <c r="P38" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q38" s="37">
+        <v>0</v>
+      </c>
+      <c r="R38" s="37">
+        <v>1.98937276084786</v>
+      </c>
+      <c r="S38" s="37">
+        <v>0</v>
+      </c>
+      <c r="T38" s="41">
+        <v>-2.8744843779897101E-2</v>
+      </c>
+      <c r="U38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A39" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="B39">
+        <v>0</v>
+      </c>
+      <c r="C39">
+        <v>-1.43724218899485E-2</v>
+      </c>
+      <c r="D39">
+        <v>-1.44485858427847E-2</v>
+      </c>
+      <c r="F39" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="G39">
+        <v>-30</v>
+      </c>
+      <c r="H39" s="28">
+        <v>1.7763568394002501E-15</v>
+      </c>
+      <c r="I39">
+        <v>-10.958904109589</v>
+      </c>
+      <c r="J39">
+        <v>-14.1095890410959</v>
+      </c>
+      <c r="K39">
+        <v>4.10958904109589</v>
+      </c>
+      <c r="P39" s="37"/>
+      <c r="Q39" s="37"/>
+      <c r="R39" s="37"/>
+      <c r="S39" s="37"/>
+      <c r="T39" s="41"/>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A40" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <v>-2.0760624705304199E-2</v>
+      </c>
+      <c r="D40">
+        <v>-2.0942256529998499E-2</v>
+      </c>
+      <c r="F40" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G40">
+        <v>2</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F41" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>2</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="J41">
+        <v>0</v>
+      </c>
+      <c r="K41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A42" s="33" t="s">
+        <v>104</v>
+      </c>
+      <c r="B42" s="33"/>
+      <c r="C42" s="33"/>
+      <c r="D42" s="33"/>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B43" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D43" t="s">
+        <v>103</v>
+      </c>
+      <c r="F43" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="G43" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="H43" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="I43" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="J43" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="K43" s="31" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A44" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
+      <c r="C44">
+        <v>0.48447633136044399</v>
+      </c>
+      <c r="D44">
+        <v>0.48641375020364203</v>
+      </c>
+      <c r="F44" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="G44">
+        <v>10.461079280789701</v>
+      </c>
+      <c r="H44">
+        <v>-9.9969200982238906</v>
+      </c>
+      <c r="I44">
+        <v>0</v>
+      </c>
+      <c r="J44">
+        <v>-29.990760294671698</v>
+      </c>
+      <c r="K44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A45" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="B45">
+        <v>0</v>
+      </c>
+      <c r="C45">
+        <v>0.41845110144528402</v>
+      </c>
+      <c r="D45">
+        <v>0.41969907255002498</v>
+      </c>
+      <c r="F45" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="G45">
+        <v>7.25342409812494</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="I45">
+        <v>-6.8944276539475098</v>
+      </c>
+      <c r="J45">
+        <v>0</v>
+      </c>
+      <c r="K45">
+        <v>-17.236069134868799</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A46" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
+      <c r="C46">
+        <v>-0.39825059568029503</v>
+      </c>
+      <c r="D46">
+        <v>-0.40003525163856701</v>
+      </c>
+      <c r="F46" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="G46">
+        <v>-10.399652574119999</v>
+      </c>
+      <c r="H46">
+        <v>0.18493314273831599</v>
+      </c>
+      <c r="I46">
+        <v>-4.25403777798397</v>
+      </c>
+      <c r="J46">
+        <v>40.8318816208781</v>
+      </c>
+      <c r="K46">
+        <v>-10.862494264367299</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A47" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B47">
+        <v>0</v>
+      </c>
+      <c r="C47">
+        <v>1.6163846579749098E-2</v>
+      </c>
+      <c r="D47">
+        <v>1.4385033010819E-2</v>
+      </c>
+      <c r="F47" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="G47">
+        <v>29.938418411599201</v>
+      </c>
+      <c r="H47">
+        <v>-29.990760294671698</v>
+      </c>
+      <c r="I47">
+        <v>0</v>
+      </c>
+      <c r="J47">
+        <v>9.9969200982238906</v>
+      </c>
+      <c r="K47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A48" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="B48">
+        <v>0</v>
+      </c>
+      <c r="C48">
+        <v>8.0799368370503607E-3</v>
+      </c>
+      <c r="D48">
+        <v>2.1365700459448399E-3</v>
+      </c>
+      <c r="F48" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="G48">
+        <v>17.086310753645598</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48">
+        <v>-17.236069134868799</v>
+      </c>
+      <c r="J48">
+        <v>0</v>
+      </c>
+      <c r="K48">
+        <v>6.8944276539475098</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="B49" s="28">
+        <v>1.7763568394002501E-15</v>
+      </c>
+      <c r="C49">
+        <v>1.09646273687711E-3</v>
+      </c>
+      <c r="D49">
+        <v>-1.05719550862875E-4</v>
+      </c>
+      <c r="F49" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="G49">
+        <v>-29.754138291590198</v>
+      </c>
+      <c r="H49">
+        <v>-0.21524906492063101</v>
+      </c>
+      <c r="I49">
+        <v>-10.862494264367299</v>
+      </c>
+      <c r="J49">
+        <v>-14.468757209365601</v>
+      </c>
+      <c r="K49">
+        <v>4.25403777798397</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50">
+        <v>1.0000319482551701</v>
+      </c>
+      <c r="D50">
+        <v>0.99999672400268302</v>
+      </c>
+      <c r="F50" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G50">
+        <v>1.9993840196447801</v>
+      </c>
+      <c r="H50">
+        <v>0</v>
+      </c>
+      <c r="I50">
+        <v>0</v>
+      </c>
+      <c r="J50">
+        <v>0</v>
+      </c>
+      <c r="K50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51">
+        <v>0.98960756191184396</v>
+      </c>
+      <c r="D51">
+        <v>0.98964215305929903</v>
+      </c>
+      <c r="F51" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+      <c r="H51">
+        <v>1.99324134897781</v>
+      </c>
+      <c r="I51">
+        <v>0</v>
+      </c>
+      <c r="J51">
+        <v>-2.8896388615395299E-2</v>
+      </c>
+      <c r="K51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F53" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="G53" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="H53" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="I53" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="J53" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="K53" s="31" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F54" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="G54">
+        <v>10.5259569177432</v>
+      </c>
+      <c r="H54">
+        <v>-9.99676853213521</v>
+      </c>
+      <c r="I54">
+        <v>0</v>
+      </c>
+      <c r="J54">
+        <v>-29.990305596405602</v>
+      </c>
+      <c r="K54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F55" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="G55">
+        <v>7.2524947018006696</v>
+      </c>
+      <c r="H55">
+        <v>0</v>
+      </c>
+      <c r="I55">
+        <v>-6.89432312561049</v>
+      </c>
+      <c r="J55">
+        <v>0</v>
+      </c>
+      <c r="K55">
+        <v>-17.235807814026199</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F56" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="G56">
+        <v>-10.332861921678401</v>
+      </c>
+      <c r="H56">
+        <v>9.1523722926218895E-2</v>
+      </c>
+      <c r="I56">
+        <v>-4.2266263199785303</v>
+      </c>
+      <c r="J56">
+        <v>40.831633805081303</v>
+      </c>
+      <c r="K56">
+        <v>-10.7902914226365</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F57" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="G57">
+        <v>30.135734461311099</v>
+      </c>
+      <c r="H57">
+        <v>-29.990305596405602</v>
+      </c>
+      <c r="I57">
+        <v>0</v>
+      </c>
+      <c r="J57">
+        <v>9.99676853213521</v>
+      </c>
+      <c r="K57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F58" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="G58">
+        <v>17.0860762478206</v>
+      </c>
+      <c r="H58">
+        <v>0</v>
+      </c>
+      <c r="I58">
+        <v>-17.235807814026199</v>
+      </c>
+      <c r="J58">
+        <v>0</v>
+      </c>
+      <c r="K58">
+        <v>6.89432312561049</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F59" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="G59">
+        <v>-29.556449473116501</v>
+      </c>
+      <c r="H59">
+        <v>-0.48489290932829099</v>
+      </c>
+      <c r="I59">
+        <v>-10.7902914226365</v>
+      </c>
+      <c r="J59">
+        <v>-14.4679645187307</v>
+      </c>
+      <c r="K59">
+        <v>4.2266263199785303</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F60" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G60">
+        <v>1.9993537064270399</v>
+      </c>
+      <c r="H60">
+        <v>0</v>
+      </c>
+      <c r="I60">
+        <v>0</v>
+      </c>
+      <c r="J60">
+        <v>0</v>
+      </c>
+      <c r="K60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F61" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="G61">
+        <v>0</v>
+      </c>
+      <c r="H61">
+        <v>1.9800442068205599</v>
+      </c>
+      <c r="I61">
+        <v>0</v>
+      </c>
+      <c r="J61">
+        <v>-2.88427258383726E-2</v>
+      </c>
+      <c r="K61">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="O1:R1"/>
+  <mergeCells count="5">
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="P1:T1"/>
+    <mergeCell ref="P10:S10"/>
+    <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ADMM code is now working for 3 bus case.
ADMM SE seems to work for the 3-bus case. Changed myfun_Part1_AC and
Part2_AC to use h_rect and H_rect. May need to change them again for the
14 bus case.
</commit_message>
<xml_diff>
--- a/DMASE - Test Results.xlsx
+++ b/DMASE - Test Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="18195" windowHeight="7740" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="18195" windowHeight="7740" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="2 Bus" sheetId="4" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="114">
   <si>
     <t>Abur 3-Bus Case Measurements (run through SE, rerun new estimate again)</t>
   </si>
@@ -356,6 +356,9 @@
   </si>
   <si>
     <t>H</t>
+  </si>
+  <si>
+    <t>ADMM AC h (converge in 3 iter)</t>
   </si>
 </sst>
 </file>
@@ -365,7 +368,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000000000000000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -419,6 +422,12 @@
       <i/>
       <sz val="11"/>
       <color theme="1" tint="0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -494,7 +503,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -576,6 +585,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -588,17 +608,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -916,15 +928,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
       <c r="I1" s="6" t="s">
         <v>1</v>
       </c>
@@ -1155,15 +1167,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I9"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19.5703125" bestFit="1" customWidth="1"/>
@@ -1172,15 +1184,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
+      <c r="A1" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
       <c r="I1" s="6" t="s">
         <v>1</v>
       </c>
@@ -1533,15 +1545,15 @@
       <c r="N11" s="1"/>
     </row>
     <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="34" t="s">
+      <c r="A12" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="B12" s="34"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
       <c r="I12" s="1"/>
       <c r="J12" s="6" t="s">
         <v>1</v>
@@ -2031,15 +2043,15 @@
       <c r="G31" s="1"/>
     </row>
     <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="34" t="s">
+      <c r="A32" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="B32" s="34"/>
-      <c r="C32" s="34"/>
-      <c r="D32" s="34"/>
-      <c r="E32" s="34"/>
-      <c r="F32" s="34"/>
-      <c r="G32" s="34"/>
+      <c r="B32" s="43"/>
+      <c r="C32" s="43"/>
+      <c r="D32" s="43"/>
+      <c r="E32" s="43"/>
+      <c r="F32" s="43"/>
+      <c r="G32" s="43"/>
       <c r="I32" s="1"/>
       <c r="J32" s="6" t="s">
         <v>1</v>
@@ -2064,8 +2076,8 @@
       <c r="B33" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C33" s="7" t="s">
-        <v>39</v>
+      <c r="C33" s="46" t="s">
+        <v>113</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
@@ -2121,21 +2133,26 @@
       <c r="A35" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B35" s="1"/>
+      <c r="B35" s="1">
+        <v>0.99999845426357303</v>
+      </c>
       <c r="C35" s="1">
-        <v>0</v>
+        <v>0.99999999951187202</v>
       </c>
       <c r="D35" s="1">
-        <v>0</v>
+        <v>1.0000000057454399</v>
       </c>
       <c r="E35" s="1">
-        <v>0</v>
+        <f>C35-D35</f>
+        <v>-6.2335678840952369E-9</v>
       </c>
       <c r="F35" s="1">
-        <v>0</v>
+        <f>B35-C35</f>
+        <v>-1.5452482989841698E-6</v>
       </c>
       <c r="G35" s="1">
-        <v>0</v>
+        <f>B35-D35</f>
+        <v>-1.5514818668682651E-6</v>
       </c>
       <c r="I35" s="1"/>
       <c r="J35" s="8" t="s">
@@ -2155,12 +2172,27 @@
       <c r="A36" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
+      <c r="B36" s="1">
+        <v>0.99470275148962295</v>
+      </c>
+      <c r="C36" s="1">
+        <v>0.99470125387918296</v>
+      </c>
+      <c r="D36" s="1">
+        <v>0.99470126016887706</v>
+      </c>
+      <c r="E36" s="1">
+        <f t="shared" ref="E36:E37" si="0">C36-D36</f>
+        <v>-6.289694098882137E-9</v>
+      </c>
+      <c r="F36" s="1">
+        <f t="shared" ref="F36:F40" si="1">B36-C36</f>
+        <v>1.4976104399933021E-6</v>
+      </c>
+      <c r="G36" s="1">
+        <f t="shared" ref="G36:G40" si="2">B36-D36</f>
+        <v>1.49132074589442E-6</v>
+      </c>
       <c r="I36" s="1"/>
       <c r="J36" s="8" t="s">
         <v>20</v>
@@ -2179,12 +2211,27 @@
       <c r="A37" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
+      <c r="B37" s="1">
+        <v>0.99149764559215503</v>
+      </c>
+      <c r="C37" s="1">
+        <v>0.99150161828779304</v>
+      </c>
+      <c r="D37" s="1">
+        <v>0.99147831063616998</v>
+      </c>
+      <c r="E37" s="1">
+        <f t="shared" si="0"/>
+        <v>2.3307651623061254E-5</v>
+      </c>
+      <c r="F37" s="1">
+        <f t="shared" si="1"/>
+        <v>-3.9726956380103928E-6</v>
+      </c>
+      <c r="G37" s="1">
+        <f t="shared" si="2"/>
+        <v>1.9334955985050861E-5</v>
+      </c>
       <c r="I37" s="1"/>
       <c r="J37" s="8" t="s">
         <v>22</v>
@@ -2206,11 +2253,23 @@
       <c r="B38" s="1">
         <v>0</v>
       </c>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
+      <c r="C38" s="1">
+        <v>0</v>
+      </c>
+      <c r="D38" s="1">
+        <v>0</v>
+      </c>
+      <c r="E38" s="1">
+        <v>0</v>
+      </c>
+      <c r="F38" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G38" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="I38" s="1"/>
       <c r="J38" s="8" t="s">
         <v>24</v>
@@ -2228,12 +2287,27 @@
       <c r="A39" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
+      <c r="B39" s="1">
+        <v>-1.44485822804116E-2</v>
+      </c>
+      <c r="C39" s="1">
+        <v>-1.44484686620042E-2</v>
+      </c>
+      <c r="D39" s="1">
+        <v>-1.4448468599055299E-2</v>
+      </c>
+      <c r="E39" s="1">
+        <f>C39-D39</f>
+        <v>-6.2948901299875182E-11</v>
+      </c>
+      <c r="F39" s="1">
+        <f t="shared" si="1"/>
+        <v>-1.136184073994434E-7</v>
+      </c>
+      <c r="G39" s="1">
+        <f t="shared" si="2"/>
+        <v>-1.1368135630074327E-7</v>
+      </c>
       <c r="I39" s="1"/>
       <c r="J39" s="8" t="s">
         <v>26</v>
@@ -2251,12 +2325,27 @@
       <c r="A40" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="19"/>
-      <c r="E40" s="19"/>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
+      <c r="B40" s="1">
+        <v>-2.0942213598037301E-2</v>
+      </c>
+      <c r="C40" s="1">
+        <v>-2.0942297044494101E-2</v>
+      </c>
+      <c r="D40" s="1">
+        <v>-2.0940977170181601E-2</v>
+      </c>
+      <c r="E40" s="1">
+        <f>C40-D40</f>
+        <v>-1.3198743125004964E-6</v>
+      </c>
+      <c r="F40" s="1">
+        <f t="shared" si="1"/>
+        <v>8.3446456800029267E-8</v>
+      </c>
+      <c r="G40" s="1">
+        <f t="shared" si="2"/>
+        <v>-1.2364278557004671E-6</v>
+      </c>
       <c r="I40" s="1"/>
       <c r="J40" s="8" t="s">
         <v>28</v>
@@ -2430,7 +2519,7 @@
   <dimension ref="A1:Q66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2444,18 +2533,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
       <c r="L1" s="11" t="s">
         <v>1</v>
       </c>
@@ -2479,18 +2568,18 @@
       <c r="B2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36" t="s">
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45" t="s">
         <v>74</v>
       </c>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
       <c r="L2" s="8" t="s">
         <v>41</v>
       </c>
@@ -3283,18 +3372,18 @@
       <c r="O33" s="1"/>
     </row>
     <row r="35" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="35" t="s">
+      <c r="A35" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="B35" s="35"/>
-      <c r="C35" s="35"/>
-      <c r="D35" s="35"/>
-      <c r="E35" s="35"/>
-      <c r="F35" s="35"/>
-      <c r="G35" s="35"/>
-      <c r="H35" s="35"/>
-      <c r="I35" s="35"/>
-      <c r="J35" s="35"/>
+      <c r="B35" s="44"/>
+      <c r="C35" s="44"/>
+      <c r="D35" s="44"/>
+      <c r="E35" s="44"/>
+      <c r="F35" s="44"/>
+      <c r="G35" s="44"/>
+      <c r="H35" s="44"/>
+      <c r="I35" s="44"/>
+      <c r="J35" s="44"/>
       <c r="L35" s="11" t="s">
         <v>1</v>
       </c>
@@ -4027,25 +4116,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T22" sqref="T22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O31" sqref="O31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" style="2"/>
+    <col min="14" max="14" width="3.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="42" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
       <c r="G1" s="30" t="s">
         <v>100</v>
       </c>
@@ -4064,13 +4153,13 @@
       <c r="L1" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="P1" s="33" t="s">
+      <c r="P1" s="42" t="s">
         <v>106</v>
       </c>
-      <c r="Q1" s="33"/>
-      <c r="R1" s="33"/>
-      <c r="S1" s="33"/>
-      <c r="T1" s="33"/>
+      <c r="Q1" s="42"/>
+      <c r="R1" s="42"/>
+      <c r="S1" s="42"/>
+      <c r="T1" s="42"/>
       <c r="V1" s="30" t="s">
         <v>100</v>
       </c>
@@ -4281,7 +4370,7 @@
       <c r="W4">
         <v>-10</v>
       </c>
-      <c r="X4" s="38">
+      <c r="X4" s="34">
         <v>14.1095890410959</v>
       </c>
       <c r="Y4">
@@ -4485,7 +4574,7 @@
       <c r="W7">
         <v>-30</v>
       </c>
-      <c r="X7" s="39">
+      <c r="X7" s="35">
         <v>40.958904109589</v>
       </c>
       <c r="Y7">
@@ -4605,12 +4694,12 @@
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="P10" s="33" t="s">
+      <c r="P10" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="Q10" s="33"/>
-      <c r="R10" s="33"/>
-      <c r="S10" s="33"/>
+      <c r="Q10" s="42"/>
+      <c r="R10" s="42"/>
+      <c r="S10" s="42"/>
       <c r="T10" s="25"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
@@ -5609,16 +5698,16 @@
       <c r="P32" t="s">
         <v>16</v>
       </c>
-      <c r="Q32" s="40">
+      <c r="Q32" s="36">
         <v>7.3151063068693301</v>
       </c>
-      <c r="R32" s="40">
-        <v>0</v>
-      </c>
-      <c r="S32" s="43">
+      <c r="R32" s="36">
+        <v>0</v>
+      </c>
+      <c r="S32" s="39">
         <v>-6.8966618896551699</v>
       </c>
-      <c r="T32" s="41">
+      <c r="T32" s="37">
         <v>0</v>
       </c>
       <c r="U32" s="2">
@@ -5626,12 +5715,12 @@
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A33" s="33" t="s">
+      <c r="A33" s="42" t="s">
         <v>102</v>
       </c>
-      <c r="B33" s="33"/>
-      <c r="C33" s="33"/>
-      <c r="D33" s="33"/>
+      <c r="B33" s="42"/>
+      <c r="C33" s="42"/>
+      <c r="D33" s="42"/>
       <c r="F33" s="30" t="s">
         <v>100</v>
       </c>
@@ -5653,16 +5742,16 @@
       <c r="P33" t="s">
         <v>18</v>
       </c>
-      <c r="Q33" s="37">
+      <c r="Q33" s="33">
         <v>-10.3780364609378</v>
       </c>
-      <c r="R33" s="44">
+      <c r="R33" s="40">
         <v>14.222984299142199</v>
       </c>
-      <c r="S33" s="44">
+      <c r="S33" s="40">
         <v>-4.2452582416320297</v>
       </c>
-      <c r="T33" s="45">
+      <c r="T33" s="41">
         <v>40.543156953315901</v>
       </c>
       <c r="U33" s="2">
@@ -5703,16 +5792,16 @@
       <c r="P34" t="s">
         <v>20</v>
       </c>
-      <c r="Q34" s="37">
+      <c r="Q34" s="33">
         <v>30.016642808382599</v>
       </c>
-      <c r="R34" s="45">
+      <c r="R34" s="41">
         <v>-30.000479219999999</v>
       </c>
-      <c r="S34" s="37">
-        <v>0</v>
-      </c>
-      <c r="T34" s="45">
+      <c r="S34" s="33">
+        <v>0</v>
+      </c>
+      <c r="T34" s="41">
         <v>10.000159740000001</v>
       </c>
       <c r="U34">
@@ -5753,16 +5842,16 @@
       <c r="P35" t="s">
         <v>22</v>
       </c>
-      <c r="Q35" s="37">
+      <c r="Q35" s="33">
         <v>17.2497345319081</v>
       </c>
-      <c r="R35" s="37">
-        <v>0</v>
-      </c>
-      <c r="S35" s="45">
+      <c r="R35" s="33">
+        <v>0</v>
+      </c>
+      <c r="S35" s="41">
         <v>-17.241654724137899</v>
       </c>
-      <c r="T35" s="41">
+      <c r="T35" s="37">
         <v>0</v>
       </c>
       <c r="U35" s="2">
@@ -5803,16 +5892,16 @@
       <c r="P36" t="s">
         <v>24</v>
       </c>
-      <c r="Q36" s="37">
+      <c r="Q36" s="33">
         <v>-29.696867193818498</v>
       </c>
-      <c r="R36" s="45">
+      <c r="R36" s="41">
         <v>40.533793263695202</v>
       </c>
-      <c r="S36" s="45">
+      <c r="S36" s="41">
         <v>-10.841607914687099</v>
       </c>
-      <c r="T36" s="45">
+      <c r="T36" s="41">
         <v>-15.023605105997399</v>
       </c>
       <c r="U36" s="2">
@@ -5853,16 +5942,16 @@
       <c r="P37" t="s">
         <v>26</v>
       </c>
-      <c r="Q37" s="42">
+      <c r="Q37" s="38">
         <v>2.0000319480000002</v>
       </c>
-      <c r="R37" s="37">
-        <v>0</v>
-      </c>
-      <c r="S37" s="37">
-        <v>0</v>
-      </c>
-      <c r="T37" s="41">
+      <c r="R37" s="33">
+        <v>0</v>
+      </c>
+      <c r="S37" s="33">
+        <v>0</v>
+      </c>
+      <c r="T37" s="37">
         <v>0</v>
       </c>
       <c r="U37">
@@ -5903,16 +5992,16 @@
       <c r="P38" t="s">
         <v>28</v>
       </c>
-      <c r="Q38" s="37">
-        <v>0</v>
-      </c>
-      <c r="R38" s="37">
+      <c r="Q38" s="33">
+        <v>0</v>
+      </c>
+      <c r="R38" s="33">
         <v>1.98937276084786</v>
       </c>
-      <c r="S38" s="37">
-        <v>0</v>
-      </c>
-      <c r="T38" s="41">
+      <c r="S38" s="33">
+        <v>0</v>
+      </c>
+      <c r="T38" s="37">
         <v>-2.8744843779897101E-2</v>
       </c>
       <c r="U38">
@@ -5950,11 +6039,11 @@
       <c r="K39">
         <v>4.10958904109589</v>
       </c>
-      <c r="P39" s="37"/>
-      <c r="Q39" s="37"/>
-      <c r="R39" s="37"/>
-      <c r="S39" s="37"/>
-      <c r="T39" s="41"/>
+      <c r="P39" s="33"/>
+      <c r="Q39" s="33"/>
+      <c r="R39" s="33"/>
+      <c r="S39" s="33"/>
+      <c r="T39" s="37"/>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" s="26" t="s">
@@ -6009,12 +6098,12 @@
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A42" s="33" t="s">
+      <c r="A42" s="42" t="s">
         <v>104</v>
       </c>
-      <c r="B42" s="33"/>
-      <c r="C42" s="33"/>
-      <c r="D42" s="33"/>
+      <c r="B42" s="42"/>
+      <c r="C42" s="42"/>
+      <c r="D42" s="42"/>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">

</xml_diff>

<commit_message>
Created 14 bus AC case and SE results.
Adapted centralized 14-bus SE code to rectangular form. Used PowerWorld
to get the power flow results to use for the central SE measurements.
After running the code, the residuals are rather large for the case. Not
sure why yet. Possibly check on whether these measurements are right.
</commit_message>
<xml_diff>
--- a/DMASE - Test Results.xlsx
+++ b/DMASE - Test Results.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="18195" windowHeight="7740" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="18195" windowHeight="7740" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="2 Bus" sheetId="4" r:id="rId1"/>
     <sheet name="3 Bus" sheetId="1" r:id="rId2"/>
-    <sheet name="14 Bus DC" sheetId="2" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId4"/>
+    <sheet name="14 Bus AC" sheetId="6" r:id="rId3"/>
+    <sheet name="14 Bus DC" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="152">
   <si>
     <t>Abur 3-Bus Case Measurements (run through SE, rerun new estimate again)</t>
   </si>
@@ -359,14 +360,130 @@
   </si>
   <si>
     <t>ADMM AC h (converge in 3 iter)</t>
+  </si>
+  <si>
+    <t>V 6</t>
+  </si>
+  <si>
+    <t>V 9</t>
+  </si>
+  <si>
+    <t>PowerWorld IEEE 14-Bus Case (construct AC case, use ACPF results)</t>
+  </si>
+  <si>
+    <t>Q1-2</t>
+  </si>
+  <si>
+    <t>Q1-5</t>
+  </si>
+  <si>
+    <t>Q2-5</t>
+  </si>
+  <si>
+    <t>Q3-4</t>
+  </si>
+  <si>
+    <t>Q4-7</t>
+  </si>
+  <si>
+    <t>Q7-8</t>
+  </si>
+  <si>
+    <t>Q6-12</t>
+  </si>
+  <si>
+    <t>Q6-11</t>
+  </si>
+  <si>
+    <t>Q6-13</t>
+  </si>
+  <si>
+    <t>Q12-13</t>
+  </si>
+  <si>
+    <t>Q9-10</t>
+  </si>
+  <si>
+    <t>Q9-14</t>
+  </si>
+  <si>
+    <t>Q5</t>
+  </si>
+  <si>
+    <t>Q4-5</t>
+  </si>
+  <si>
+    <t>Q4-9</t>
+  </si>
+  <si>
+    <t>Q7-9</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>Q13-14</t>
+  </si>
+  <si>
+    <t>Q10-11</t>
+  </si>
+  <si>
+    <t>Q14</t>
+  </si>
+  <si>
+    <t>P5-4 created large res in DC case</t>
+  </si>
+  <si>
+    <t>Scaled PW AC Z</t>
+  </si>
+  <si>
+    <t>Area 1</t>
+  </si>
+  <si>
+    <t>Area 2</t>
+  </si>
+  <si>
+    <t>Area 3</t>
+  </si>
+  <si>
+    <t>Area 4</t>
+  </si>
+  <si>
+    <t>Boundary 1</t>
+  </si>
+  <si>
+    <t>Boundary 2</t>
+  </si>
+  <si>
+    <t>Boundary 3</t>
+  </si>
+  <si>
+    <t>Boundary 4</t>
+  </si>
+  <si>
+    <t>31:36</t>
+  </si>
+  <si>
+    <t>37:38</t>
+  </si>
+  <si>
+    <t>39:48</t>
+  </si>
+  <si>
+    <t>49:54</t>
+  </si>
+  <si>
+    <t>55:60</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000000000000000"/>
+    <numFmt numFmtId="166" formatCode="0.0000000000"/>
+    <numFmt numFmtId="167" formatCode="0.000E+00"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -503,7 +620,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -599,6 +716,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -608,7 +737,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -928,15 +1085,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
       <c r="I1" s="6" t="s">
         <v>1</v>
       </c>
@@ -1167,7 +1324,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
@@ -1184,15 +1341,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
+      <c r="A1" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
       <c r="I1" s="6" t="s">
         <v>1</v>
       </c>
@@ -1545,15 +1702,15 @@
       <c r="N11" s="1"/>
     </row>
     <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="43" t="s">
+      <c r="A12" s="47" t="s">
         <v>80</v>
       </c>
-      <c r="B12" s="43"/>
-      <c r="C12" s="43"/>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
+      <c r="B12" s="47"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="47"/>
+      <c r="G12" s="47"/>
       <c r="I12" s="1"/>
       <c r="J12" s="6" t="s">
         <v>1</v>
@@ -2043,15 +2200,15 @@
       <c r="G31" s="1"/>
     </row>
     <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="43" t="s">
+      <c r="A32" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="B32" s="43"/>
-      <c r="C32" s="43"/>
-      <c r="D32" s="43"/>
-      <c r="E32" s="43"/>
-      <c r="F32" s="43"/>
-      <c r="G32" s="43"/>
+      <c r="B32" s="47"/>
+      <c r="C32" s="47"/>
+      <c r="D32" s="47"/>
+      <c r="E32" s="47"/>
+      <c r="F32" s="47"/>
+      <c r="G32" s="47"/>
       <c r="I32" s="1"/>
       <c r="J32" s="6" t="s">
         <v>1</v>
@@ -2076,7 +2233,7 @@
       <c r="B33" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C33" s="46" t="s">
+      <c r="C33" s="45" t="s">
         <v>113</v>
       </c>
       <c r="D33" s="4"/>
@@ -2515,6 +2672,1520 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R86"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q50" sqref="Q50"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" customWidth="1"/>
+    <col min="12" max="12" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="48" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="43"/>
+      <c r="M1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="P1" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="R1" s="18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="49" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49" t="s">
+        <v>74</v>
+      </c>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="4"/>
+      <c r="L2" t="s">
+        <v>139</v>
+      </c>
+      <c r="M2" s="42" t="s">
+        <v>41</v>
+      </c>
+      <c r="N2" s="53">
+        <v>0</v>
+      </c>
+      <c r="O2" s="57">
+        <f>N2</f>
+        <v>0</v>
+      </c>
+      <c r="P2" s="61">
+        <v>0</v>
+      </c>
+      <c r="R2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="K3" s="4"/>
+      <c r="L3" s="58">
+        <v>4.8611111111111112E-2</v>
+      </c>
+      <c r="M3" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="N3" s="53">
+        <v>1.0599999427795399</v>
+      </c>
+      <c r="O3" s="57">
+        <f>N3</f>
+        <v>1.0599999427795399</v>
+      </c>
+      <c r="P3" s="61">
+        <v>-2.9953879373185301E-2</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="M4" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="N4" s="53">
+        <v>156.440731910842</v>
+      </c>
+      <c r="O4" s="1">
+        <f>N4/100</f>
+        <v>1.56440731910842</v>
+      </c>
+      <c r="P4" s="61">
+        <v>-8.6738403137775998E-6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="M5" s="42" t="s">
+        <v>117</v>
+      </c>
+      <c r="N5" s="53">
+        <v>-20.300935880694301</v>
+      </c>
+      <c r="O5" s="1">
+        <f t="shared" ref="O5:O11" si="0">N5/100</f>
+        <v>-0.20300935880694301</v>
+      </c>
+      <c r="P5" s="61">
+        <v>2.1648716178694401E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="M6" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="N6" s="53">
+        <v>75.916881283268793</v>
+      </c>
+      <c r="O6" s="1">
+        <f t="shared" si="0"/>
+        <v>0.75916881283268789</v>
+      </c>
+      <c r="P6" s="61">
+        <v>6.4758759358596297E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="M7" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="N7" s="53">
+        <v>-0.155506560051652</v>
+      </c>
+      <c r="O7" s="1">
+        <f t="shared" si="0"/>
+        <v>-1.55506560051652E-3</v>
+      </c>
+      <c r="P7" s="61">
+        <v>-1.47979634931223E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="M8" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="N8" s="53">
+        <v>41.338725991097199</v>
+      </c>
+      <c r="O8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.41338725991097197</v>
+      </c>
+      <c r="P8" s="61">
+        <v>6.8870384835700903E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="M9" s="42" t="s">
+        <v>119</v>
+      </c>
+      <c r="N9" s="53">
+        <v>-3.8398609004379098</v>
+      </c>
+      <c r="O9" s="1">
+        <f t="shared" si="0"/>
+        <v>-3.8398609004379101E-2</v>
+      </c>
+      <c r="P9" s="61">
+        <v>-1.3891657030102901E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>7</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="M10" s="42" t="s">
+        <v>49</v>
+      </c>
+      <c r="N10" s="53">
+        <v>232.35762119293199</v>
+      </c>
+      <c r="O10" s="1">
+        <f t="shared" si="0"/>
+        <v>2.32357621192932</v>
+      </c>
+      <c r="P10" s="61">
+        <v>6.3899375327158804E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="M11" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="N11" s="53">
+        <v>-20.456442236900301</v>
+      </c>
+      <c r="O11" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.20456442236900302</v>
+      </c>
+      <c r="P11" s="61">
+        <v>6.8507826856001298E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>9</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" t="s">
+        <v>140</v>
+      </c>
+      <c r="M12" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="N12" s="53">
+        <v>-0.22125272217770001</v>
+      </c>
+      <c r="O12" s="57">
+        <f>N12</f>
+        <v>-0.22125272217770001</v>
+      </c>
+      <c r="P12" s="62">
+        <v>-0.2212527222</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>10</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="58">
+        <v>0.47083333333333338</v>
+      </c>
+      <c r="M13" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="N13" s="53">
+        <v>1.0099999973080001</v>
+      </c>
+      <c r="O13" s="57">
+        <f>N13</f>
+        <v>1.0099999973080001</v>
+      </c>
+      <c r="P13" s="62">
+        <v>2.17540256007367E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>11</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="M14" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="N14" s="53">
+        <v>-23.569740833506799</v>
+      </c>
+      <c r="O14" s="1">
+        <f>N14/100</f>
+        <v>-0.235697408335068</v>
+      </c>
+      <c r="P14" s="61">
+        <v>-1.05523560178061E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>12</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="M15" s="42" t="s">
+        <v>120</v>
+      </c>
+      <c r="N15" s="53">
+        <v>0.96859150246414105</v>
+      </c>
+      <c r="O15" s="1">
+        <f t="shared" ref="O15:O19" si="1">N15/100</f>
+        <v>9.6859150246414102E-3</v>
+      </c>
+      <c r="P15" s="61">
+        <v>-2.2375145874756201E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>13</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="M16" s="42" t="s">
+        <v>53</v>
+      </c>
+      <c r="N16" s="53">
+        <v>29.247688021076399</v>
+      </c>
+      <c r="O16" s="1">
+        <f t="shared" si="1"/>
+        <v>0.29247688021076401</v>
+      </c>
+      <c r="P16" s="61">
+        <v>5.1585990707936401E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>14</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="M17" s="42" t="s">
+        <v>121</v>
+      </c>
+      <c r="N17" s="53">
+        <v>-10.134384235994199</v>
+      </c>
+      <c r="O17" s="1">
+        <f t="shared" si="1"/>
+        <v>-0.101343842359942</v>
+      </c>
+      <c r="P17" s="61">
+        <v>-2.7105327863768802E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M18" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="N18" s="53">
+        <v>4.9388912162000001E-5</v>
+      </c>
+      <c r="O18" s="1">
+        <f t="shared" si="1"/>
+        <v>4.9388912162000003E-7</v>
+      </c>
+      <c r="P18" s="61">
+        <v>6.5059278082477401E-7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M19" s="42" t="s">
+        <v>122</v>
+      </c>
+      <c r="N19" s="53">
+        <v>-23.1382548362844</v>
+      </c>
+      <c r="O19" s="1">
+        <f t="shared" si="1"/>
+        <v>-0.231382548362844</v>
+      </c>
+      <c r="P19" s="61">
+        <v>1.7465773008429299E-7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L20" t="s">
+        <v>141</v>
+      </c>
+      <c r="M20" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="N20" s="53">
+        <v>-0.25510563387813501</v>
+      </c>
+      <c r="O20" s="57">
+        <f>N20</f>
+        <v>-0.25510563387813501</v>
+      </c>
+      <c r="P20" s="62">
+        <v>-0.25510563390000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L21" s="58">
+        <v>0.8125</v>
+      </c>
+      <c r="M21" s="42" t="s">
+        <v>114</v>
+      </c>
+      <c r="N21" s="53">
+        <v>1.0385379019832599</v>
+      </c>
+      <c r="O21" s="57">
+        <f>N21</f>
+        <v>1.0385379019832599</v>
+      </c>
+      <c r="P21" s="62">
+        <v>-5.12238863404413E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M22" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="N22" s="53">
+        <v>6.4193752642371704</v>
+      </c>
+      <c r="O22" s="1">
+        <f>N22/100</f>
+        <v>6.4193752642371704E-2</v>
+      </c>
+      <c r="P22" s="61">
+        <v>1.2851248455257599E-4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M23" s="42" t="s">
+        <v>124</v>
+      </c>
+      <c r="N23" s="53">
+        <v>1.57798981550307</v>
+      </c>
+      <c r="O23" s="1">
+        <f t="shared" ref="O23:O31" si="2">N23/100</f>
+        <v>1.5779898155030701E-2</v>
+      </c>
+      <c r="P23" s="61">
+        <v>1.0767413611616999E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M24" s="42" t="s">
+        <v>57</v>
+      </c>
+      <c r="N24" s="53">
+        <v>7.6111237412808599</v>
+      </c>
+      <c r="O24" s="1">
+        <f t="shared" si="2"/>
+        <v>7.6111237412808605E-2</v>
+      </c>
+      <c r="P24" s="61">
+        <v>1.6297137374082799E-5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M25" s="42" t="s">
+        <v>123</v>
+      </c>
+      <c r="N25" s="53">
+        <v>2.2749299623984598</v>
+      </c>
+      <c r="O25" s="1">
+        <f t="shared" si="2"/>
+        <v>2.2749299623984597E-2</v>
+      </c>
+      <c r="P25" s="61">
+        <v>9.80565804585901E-5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M26" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="N26" s="53">
+        <v>17.236621109828601</v>
+      </c>
+      <c r="O26" s="1">
+        <f t="shared" si="2"/>
+        <v>0.17236621109828601</v>
+      </c>
+      <c r="P26" s="61">
+        <v>2.8072391037720099E-5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M27" s="42" t="s">
+        <v>125</v>
+      </c>
+      <c r="N27" s="53">
+        <v>6.2088690408799696</v>
+      </c>
+      <c r="O27" s="1">
+        <f t="shared" si="2"/>
+        <v>6.2088690408799697E-2</v>
+      </c>
+      <c r="P27" s="61">
+        <v>3.8053003130694002E-4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M28" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="N28" s="53">
+        <v>1.4392071686730901</v>
+      </c>
+      <c r="O28" s="1">
+        <f t="shared" si="2"/>
+        <v>1.4392071686730901E-2</v>
+      </c>
+      <c r="P28" s="61">
+        <v>3.3901950999533699E-5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M29" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="N29" s="53">
+        <v>0.52526799870488805</v>
+      </c>
+      <c r="O29" s="1">
+        <f t="shared" si="2"/>
+        <v>5.2526799870488807E-3</v>
+      </c>
+      <c r="P29" s="61">
+        <v>9.7871725652031802E-5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M30" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="N30" s="53">
+        <v>-6.1</v>
+      </c>
+      <c r="O30" s="1">
+        <f t="shared" si="2"/>
+        <v>-6.0999999999999999E-2</v>
+      </c>
+      <c r="P30" s="61">
+        <v>-5.5804864002167998E-6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M31" s="42" t="s">
+        <v>20</v>
+      </c>
+      <c r="N31" s="53">
+        <v>-1.6</v>
+      </c>
+      <c r="O31" s="1">
+        <f t="shared" si="2"/>
+        <v>-1.6E-2</v>
+      </c>
+      <c r="P31" s="61">
+        <v>5.2797756594065403E-5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L32" t="s">
+        <v>142</v>
+      </c>
+      <c r="M32" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="N32" s="53">
+        <v>-0.26806990591321</v>
+      </c>
+      <c r="O32" s="57">
+        <f>N32</f>
+        <v>-0.26806990591321</v>
+      </c>
+      <c r="P32" s="62">
+        <v>-0.26806990590000002</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L33" s="59" t="s">
+        <v>147</v>
+      </c>
+      <c r="M33" s="42" t="s">
+        <v>115</v>
+      </c>
+      <c r="N33" s="53">
+        <v>1.0349152577221601</v>
+      </c>
+      <c r="O33" s="57">
+        <f>N33</f>
+        <v>1.0349152577221601</v>
+      </c>
+      <c r="P33" s="62">
+        <v>-2.1765958813597698E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L34" s="50"/>
+      <c r="M34" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="N34" s="53">
+        <v>6.1481308294477897</v>
+      </c>
+      <c r="O34" s="1">
+        <f>N34/100</f>
+        <v>6.1481308294477899E-2</v>
+      </c>
+      <c r="P34" s="60">
+        <v>-1.88116567434796E-5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="52"/>
+      <c r="B35" s="52"/>
+      <c r="C35" s="52"/>
+      <c r="D35" s="52"/>
+      <c r="E35" s="52"/>
+      <c r="F35" s="52"/>
+      <c r="G35" s="52"/>
+      <c r="H35" s="52"/>
+      <c r="I35" s="52"/>
+      <c r="J35" s="52"/>
+      <c r="K35" s="52"/>
+      <c r="L35" s="50"/>
+      <c r="M35" s="42" t="s">
+        <v>127</v>
+      </c>
+      <c r="N35" s="53">
+        <v>6.1776975079165704</v>
+      </c>
+      <c r="O35" s="1">
+        <f t="shared" ref="O35:O47" si="3">N35/100</f>
+        <v>6.1776975079165707E-2</v>
+      </c>
+      <c r="P35" s="60">
+        <v>-4.4567340559324698E-4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A36" s="50"/>
+      <c r="B36" s="50"/>
+      <c r="C36" s="50"/>
+      <c r="D36" s="50"/>
+      <c r="E36" s="50"/>
+      <c r="F36" s="50"/>
+      <c r="G36" s="50"/>
+      <c r="H36" s="50"/>
+      <c r="I36" s="50"/>
+      <c r="J36" s="50"/>
+      <c r="K36" s="50"/>
+      <c r="L36" s="50"/>
+      <c r="M36" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="N36" s="53">
+        <v>10.1258308263922</v>
+      </c>
+      <c r="O36" s="1">
+        <f t="shared" si="3"/>
+        <v>0.101258308263922</v>
+      </c>
+      <c r="P36" s="61">
+        <v>-1.40656940313608E-4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A37" s="50"/>
+      <c r="B37" s="50"/>
+      <c r="C37" s="50"/>
+      <c r="D37" s="50"/>
+      <c r="E37" s="50"/>
+      <c r="F37" s="50"/>
+      <c r="G37" s="50"/>
+      <c r="H37" s="50"/>
+      <c r="I37" s="50"/>
+      <c r="J37" s="50"/>
+      <c r="K37" s="50"/>
+      <c r="L37" s="50"/>
+      <c r="M37" s="42" t="s">
+        <v>128</v>
+      </c>
+      <c r="N37" s="53">
+        <v>4.8779939913553596</v>
+      </c>
+      <c r="O37" s="1">
+        <f t="shared" si="3"/>
+        <v>4.8779939913553595E-2</v>
+      </c>
+      <c r="P37" s="60">
+        <v>-6.3339605935184401E-4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A38" s="50"/>
+      <c r="B38" s="50"/>
+      <c r="C38" s="50"/>
+      <c r="D38" s="50"/>
+      <c r="E38" s="50"/>
+      <c r="F38" s="50"/>
+      <c r="G38" s="50"/>
+      <c r="H38" s="50"/>
+      <c r="I38" s="50"/>
+      <c r="J38" s="50"/>
+      <c r="K38" s="50"/>
+      <c r="L38" t="s">
+        <v>143</v>
+      </c>
+      <c r="M38" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="N38" s="53">
+        <v>-7.6</v>
+      </c>
+      <c r="O38" s="1">
+        <f t="shared" si="3"/>
+        <v>-7.5999999999999998E-2</v>
+      </c>
+      <c r="P38" s="61">
+        <v>-1.4483820858600399E-4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+      <c r="L39" s="59" t="s">
+        <v>148</v>
+      </c>
+      <c r="M39" s="42" t="s">
+        <v>129</v>
+      </c>
+      <c r="N39" s="53">
+        <v>-1.6</v>
+      </c>
+      <c r="O39" s="1">
+        <f t="shared" si="3"/>
+        <v>-1.6E-2</v>
+      </c>
+      <c r="P39" s="61">
+        <v>-3.5573742834272E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+      <c r="K40" s="1"/>
+      <c r="L40" t="s">
+        <v>144</v>
+      </c>
+      <c r="M40" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="N40" s="54">
+        <v>-63.001699846354903</v>
+      </c>
+      <c r="O40" s="1">
+        <f t="shared" si="3"/>
+        <v>-0.63001699846354908</v>
+      </c>
+      <c r="P40" s="61">
+        <v>-9.5060452610995505E-4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+      <c r="L41" s="59" t="s">
+        <v>149</v>
+      </c>
+      <c r="M41" s="42" t="s">
+        <v>130</v>
+      </c>
+      <c r="N41" s="53">
+        <v>10.2039485868599</v>
+      </c>
+      <c r="O41" s="1">
+        <f t="shared" si="3"/>
+        <v>0.102039485868599</v>
+      </c>
+      <c r="P41" s="61">
+        <v>-5.1145973996759402E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1"/>
+      <c r="M42" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="N42" s="53">
+        <v>16.526211548050401</v>
+      </c>
+      <c r="O42" s="1">
+        <f t="shared" si="3"/>
+        <v>0.16526211548050401</v>
+      </c>
+      <c r="P42" s="61">
+        <v>3.0418249791705498E-4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="1"/>
+      <c r="M43" s="42" t="s">
+        <v>131</v>
+      </c>
+      <c r="N43" s="55">
+        <v>-1.34369314780613</v>
+      </c>
+      <c r="O43" s="1">
+        <f t="shared" si="3"/>
+        <v>-1.34369314780613E-2</v>
+      </c>
+      <c r="P43" s="61">
+        <v>-1.37670401876801E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
+      <c r="K44" s="1"/>
+      <c r="M44" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="N44" s="55">
+        <v>29.247637436823101</v>
+      </c>
+      <c r="O44" s="1">
+        <f t="shared" si="3"/>
+        <v>0.29247637436823104</v>
+      </c>
+      <c r="P44" s="61">
+        <v>2.2761940039589499E-4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
+      <c r="K45" s="1"/>
+      <c r="M45" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="N45" s="55">
+        <v>11.0919776937066</v>
+      </c>
+      <c r="O45" s="1">
+        <f t="shared" si="3"/>
+        <v>0.11091977693706599</v>
+      </c>
+      <c r="P45" s="61">
+        <v>-1.3983824680780001E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1"/>
+      <c r="K46" s="1"/>
+      <c r="M46" s="42" t="s">
+        <v>67</v>
+      </c>
+      <c r="N46" s="56">
+        <v>-94.199996999999996</v>
+      </c>
+      <c r="O46" s="1">
+        <f t="shared" si="3"/>
+        <v>-0.94199996999999991</v>
+      </c>
+      <c r="P46" s="61">
+        <v>-2.81965662445027E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+      <c r="K47" s="1"/>
+      <c r="M47" s="42" t="s">
+        <v>133</v>
+      </c>
+      <c r="N47">
+        <f>21.4613437652587-19</f>
+        <v>2.4613437652587002</v>
+      </c>
+      <c r="O47" s="1">
+        <f t="shared" si="3"/>
+        <v>2.4613437652587004E-2</v>
+      </c>
+      <c r="P47" s="61">
+        <v>-6.8701998242329402E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1"/>
+      <c r="K48" s="1"/>
+      <c r="M48" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="N48" s="55">
+        <v>-0.22125272217770001</v>
+      </c>
+      <c r="O48" s="57">
+        <f>N48</f>
+        <v>-0.22125272217770001</v>
+      </c>
+      <c r="P48" s="62">
+        <v>-0.2212527222</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1"/>
+      <c r="K49" s="1"/>
+      <c r="M49" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="N49" s="55">
+        <v>1.0099999973080001</v>
+      </c>
+      <c r="O49" s="57">
+        <f>N49</f>
+        <v>1.0099999973080001</v>
+      </c>
+      <c r="P49" s="62">
+        <v>2.17540256007367E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+      <c r="J50" s="1"/>
+      <c r="K50" s="1"/>
+      <c r="L50" t="s">
+        <v>145</v>
+      </c>
+      <c r="M50" s="42" t="s">
+        <v>68</v>
+      </c>
+      <c r="N50" s="55">
+        <v>4.9650161007164098</v>
+      </c>
+      <c r="O50" s="1">
+        <f>N50/100</f>
+        <v>4.9650161007164101E-2</v>
+      </c>
+      <c r="P50" s="61">
+        <v>1.15284947015369E-4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+      <c r="J51" s="1"/>
+      <c r="K51" s="1"/>
+      <c r="L51" s="59" t="s">
+        <v>150</v>
+      </c>
+      <c r="M51" s="42" t="s">
+        <v>134</v>
+      </c>
+      <c r="N51" s="55">
+        <v>0.52427629116916796</v>
+      </c>
+      <c r="O51" s="1">
+        <f t="shared" ref="O51:O53" si="4">N51/100</f>
+        <v>5.2427629116916794E-3</v>
+      </c>
+      <c r="P51" s="61">
+        <v>6.2348925580496799E-4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M52" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="N52" s="55">
+        <v>-13.5</v>
+      </c>
+      <c r="O52" s="1">
+        <f t="shared" si="4"/>
+        <v>-0.13500000000000001</v>
+      </c>
+      <c r="P52" s="61">
+        <v>-1.30914832287277E-5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M53" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="N53" s="55">
+        <v>-5.8</v>
+      </c>
+      <c r="O53" s="1">
+        <f t="shared" si="4"/>
+        <v>-5.7999999999999996E-2</v>
+      </c>
+      <c r="P53" s="61">
+        <v>1.15841086511394E-4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M54" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="N54" s="55">
+        <v>-0.25510563387813501</v>
+      </c>
+      <c r="O54" s="57">
+        <f>N54</f>
+        <v>-0.25510563387813501</v>
+      </c>
+      <c r="P54" s="62">
+        <v>-0.25510563390000002</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M55" s="42" t="s">
+        <v>114</v>
+      </c>
+      <c r="N55" s="55">
+        <v>1.0385379019832599</v>
+      </c>
+      <c r="O55" s="57">
+        <f>N55</f>
+        <v>1.0385379019832599</v>
+      </c>
+      <c r="P55" s="62">
+        <v>-5.12238863404413E-3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L56" t="s">
+        <v>146</v>
+      </c>
+      <c r="M56" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="N56" s="55">
+        <v>-2.8744036925517298</v>
+      </c>
+      <c r="O56" s="1">
+        <f>N56/100</f>
+        <v>-2.8744036925517299E-2</v>
+      </c>
+      <c r="P56" s="61">
+        <v>-9.7142222335186394E-5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L57" s="59" t="s">
+        <v>151</v>
+      </c>
+      <c r="M57" s="42" t="s">
+        <v>135</v>
+      </c>
+      <c r="N57" s="55">
+        <v>0.31779049296478201</v>
+      </c>
+      <c r="O57" s="1">
+        <f t="shared" ref="O57:O59" si="5">N57/100</f>
+        <v>3.1779049296478202E-3</v>
+      </c>
+      <c r="P57" s="61">
+        <v>-1.0332946463634299E-3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M58" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="N58" s="55">
+        <v>-14.9</v>
+      </c>
+      <c r="O58" s="1">
+        <f t="shared" si="5"/>
+        <v>-0.14899999999999999</v>
+      </c>
+      <c r="P58" s="61">
+        <v>-4.6294745534552998E-5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M59" s="42" t="s">
+        <v>136</v>
+      </c>
+      <c r="N59" s="55">
+        <v>-5</v>
+      </c>
+      <c r="O59" s="1">
+        <f t="shared" si="5"/>
+        <v>-0.05</v>
+      </c>
+      <c r="P59" s="61">
+        <v>-4.2582952991622499E-5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M60" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="N60" s="55">
+        <v>-0.26806990591321</v>
+      </c>
+      <c r="O60" s="57">
+        <f>N60</f>
+        <v>-0.26806990591321</v>
+      </c>
+      <c r="P60" s="62">
+        <v>-0.26806990590000002</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M61" s="42" t="s">
+        <v>115</v>
+      </c>
+      <c r="N61" s="55">
+        <v>1.0349152577221601</v>
+      </c>
+      <c r="O61" s="57">
+        <f>N61</f>
+        <v>1.0349152577221601</v>
+      </c>
+      <c r="P61" s="62">
+        <v>-2.1765958813597698E-3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O62" s="1"/>
+      <c r="P62" s="3"/>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M63" s="51"/>
+      <c r="N63" s="51"/>
+      <c r="O63" s="1"/>
+      <c r="P63" s="3"/>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M64" s="51"/>
+      <c r="N64" s="50"/>
+      <c r="P64" s="3"/>
+    </row>
+    <row r="65" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M65" s="51"/>
+      <c r="N65" s="50"/>
+      <c r="P65" s="3"/>
+    </row>
+    <row r="66" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M66" s="51"/>
+      <c r="N66" s="50"/>
+    </row>
+    <row r="67" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M67" s="42"/>
+      <c r="N67" s="1"/>
+    </row>
+    <row r="68" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M68" s="42"/>
+      <c r="N68" s="1"/>
+    </row>
+    <row r="69" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M69" s="42"/>
+      <c r="N69" s="1"/>
+    </row>
+    <row r="70" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M70" s="42"/>
+      <c r="N70" s="1"/>
+    </row>
+    <row r="71" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M71" s="42"/>
+      <c r="N71" s="1"/>
+    </row>
+    <row r="72" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M72" s="42"/>
+      <c r="N72" s="1"/>
+    </row>
+    <row r="73" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M73" s="42"/>
+      <c r="N73" s="1"/>
+    </row>
+    <row r="74" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M74" s="42"/>
+      <c r="N74" s="1"/>
+    </row>
+    <row r="75" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M75" s="42"/>
+      <c r="N75" s="1"/>
+    </row>
+    <row r="76" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M76" s="42"/>
+      <c r="N76" s="1"/>
+    </row>
+    <row r="77" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M77" s="42"/>
+      <c r="N77" s="1"/>
+    </row>
+    <row r="78" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M78" s="42"/>
+      <c r="N78" s="1"/>
+    </row>
+    <row r="79" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M79" s="42"/>
+      <c r="N79" s="1"/>
+    </row>
+    <row r="80" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M80" s="42"/>
+      <c r="N80" s="1"/>
+    </row>
+    <row r="81" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M81" s="42"/>
+      <c r="N81" s="1"/>
+    </row>
+    <row r="82" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M82" s="42"/>
+      <c r="N82" s="1"/>
+    </row>
+    <row r="83" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M83" s="42"/>
+      <c r="N83" s="1"/>
+    </row>
+    <row r="84" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M84" s="42"/>
+      <c r="N84" s="1"/>
+    </row>
+    <row r="85" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M85" s="42"/>
+      <c r="N85" s="1"/>
+    </row>
+    <row r="86" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M86" s="42"/>
+      <c r="N86" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:J2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q66"/>
   <sheetViews>
@@ -2533,18 +4204,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
       <c r="L1" s="11" t="s">
         <v>1</v>
       </c>
@@ -2568,18 +4239,18 @@
       <c r="B2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="45" t="s">
+      <c r="C2" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45" t="s">
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
       <c r="L2" s="8" t="s">
         <v>41</v>
       </c>
@@ -3372,18 +5043,18 @@
       <c r="O33" s="1"/>
     </row>
     <row r="35" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="44" t="s">
+      <c r="A35" s="48" t="s">
         <v>78</v>
       </c>
-      <c r="B35" s="44"/>
-      <c r="C35" s="44"/>
-      <c r="D35" s="44"/>
-      <c r="E35" s="44"/>
-      <c r="F35" s="44"/>
-      <c r="G35" s="44"/>
-      <c r="H35" s="44"/>
-      <c r="I35" s="44"/>
-      <c r="J35" s="44"/>
+      <c r="B35" s="48"/>
+      <c r="C35" s="48"/>
+      <c r="D35" s="48"/>
+      <c r="E35" s="48"/>
+      <c r="F35" s="48"/>
+      <c r="G35" s="48"/>
+      <c r="H35" s="48"/>
+      <c r="I35" s="48"/>
+      <c r="J35" s="48"/>
       <c r="L35" s="11" t="s">
         <v>1</v>
       </c>
@@ -4112,7 +5783,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA61"/>
   <sheetViews>
@@ -4128,13 +5799,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="46" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
       <c r="G1" s="30" t="s">
         <v>100</v>
       </c>
@@ -4153,13 +5824,13 @@
       <c r="L1" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="P1" s="42" t="s">
+      <c r="P1" s="46" t="s">
         <v>106</v>
       </c>
-      <c r="Q1" s="42"/>
-      <c r="R1" s="42"/>
-      <c r="S1" s="42"/>
-      <c r="T1" s="42"/>
+      <c r="Q1" s="46"/>
+      <c r="R1" s="46"/>
+      <c r="S1" s="46"/>
+      <c r="T1" s="46"/>
       <c r="V1" s="30" t="s">
         <v>100</v>
       </c>
@@ -4694,12 +6365,12 @@
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="P10" s="42" t="s">
+      <c r="P10" s="46" t="s">
         <v>108</v>
       </c>
-      <c r="Q10" s="42"/>
-      <c r="R10" s="42"/>
-      <c r="S10" s="42"/>
+      <c r="Q10" s="46"/>
+      <c r="R10" s="46"/>
+      <c r="S10" s="46"/>
       <c r="T10" s="25"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
@@ -5715,12 +7386,12 @@
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A33" s="42" t="s">
+      <c r="A33" s="46" t="s">
         <v>102</v>
       </c>
-      <c r="B33" s="42"/>
-      <c r="C33" s="42"/>
-      <c r="D33" s="42"/>
+      <c r="B33" s="46"/>
+      <c r="C33" s="46"/>
+      <c r="D33" s="46"/>
       <c r="F33" s="30" t="s">
         <v>100</v>
       </c>
@@ -6098,12 +7769,12 @@
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A42" s="42" t="s">
+      <c r="A42" s="46" t="s">
         <v>104</v>
       </c>
-      <c r="B42" s="42"/>
-      <c r="C42" s="42"/>
-      <c r="D42" s="42"/>
+      <c r="B42" s="46"/>
+      <c r="C42" s="46"/>
+      <c r="D42" s="46"/>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">

</xml_diff>

<commit_message>
Centralized 14 bus AC case works; began converting 14 bus ADMM to rectangular
Commented out the angle and V measurements from the 14 bus AC case. Then
the residuals are small for the centralized rectangular SE, and the
solution is as expected. Not sure how to incorporate PMU angles and
voltages (see Phadke book for more detail). Started working on
converting 14 bus ADMM from polar to rectangular.
</commit_message>
<xml_diff>
--- a/DMASE - Test Results.xlsx
+++ b/DMASE - Test Results.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leilei\Documents\GitHub\D-MASE\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="360" yWindow="105" windowWidth="18195" windowHeight="7740" activeTab="2"/>
   </bookViews>
@@ -13,12 +18,12 @@
     <sheet name="14 Bus DC" sheetId="2" r:id="rId4"/>
     <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="182">
   <si>
     <t>Abur 3-Bus Case Measurements (run through SE, rerun new estimate again)</t>
   </si>
@@ -474,6 +479,96 @@
   </si>
   <si>
     <t>55:60</t>
+  </si>
+  <si>
+    <t>e4</t>
+  </si>
+  <si>
+    <t>e5</t>
+  </si>
+  <si>
+    <t>e6</t>
+  </si>
+  <si>
+    <t>e7</t>
+  </si>
+  <si>
+    <t>e8</t>
+  </si>
+  <si>
+    <t>e9</t>
+  </si>
+  <si>
+    <t>e10</t>
+  </si>
+  <si>
+    <t>e11</t>
+  </si>
+  <si>
+    <t>e12</t>
+  </si>
+  <si>
+    <t>e13</t>
+  </si>
+  <si>
+    <t>e14</t>
+  </si>
+  <si>
+    <t>f4</t>
+  </si>
+  <si>
+    <t>f5</t>
+  </si>
+  <si>
+    <t>f6</t>
+  </si>
+  <si>
+    <t>f7</t>
+  </si>
+  <si>
+    <t>f8</t>
+  </si>
+  <si>
+    <t>f9</t>
+  </si>
+  <si>
+    <t>f10</t>
+  </si>
+  <si>
+    <t>f11</t>
+  </si>
+  <si>
+    <t>f12</t>
+  </si>
+  <si>
+    <t>f13</t>
+  </si>
+  <si>
+    <t>f14</t>
+  </si>
+  <si>
+    <t>1:8</t>
+  </si>
+  <si>
+    <t>9:14</t>
+  </si>
+  <si>
+    <t>15:24</t>
+  </si>
+  <si>
+    <t>25:28</t>
+  </si>
+  <si>
+    <t>29:30</t>
+  </si>
+  <si>
+    <t>31:38</t>
+  </si>
+  <si>
+    <t>39:42</t>
+  </si>
+  <si>
+    <t>43:46</t>
   </si>
 </sst>
 </file>
@@ -482,8 +577,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000000000000000"/>
-    <numFmt numFmtId="166" formatCode="0.0000000000"/>
-    <numFmt numFmtId="167" formatCode="0.000E+00"/>
+    <numFmt numFmtId="165" formatCode="0.0000000000"/>
+    <numFmt numFmtId="166" formatCode="0.000E+00"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -620,7 +715,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -728,6 +823,40 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -737,36 +866,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -777,6 +879,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -825,7 +930,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -860,7 +965,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1085,15 +1190,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="60" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
       <c r="I1" s="6" t="s">
         <v>1</v>
       </c>
@@ -1341,15 +1446,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
+      <c r="A1" s="60" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
       <c r="I1" s="6" t="s">
         <v>1</v>
       </c>
@@ -1702,15 +1807,15 @@
       <c r="N11" s="1"/>
     </row>
     <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="47" t="s">
+      <c r="A12" s="61" t="s">
         <v>80</v>
       </c>
-      <c r="B12" s="47"/>
-      <c r="C12" s="47"/>
-      <c r="D12" s="47"/>
-      <c r="E12" s="47"/>
-      <c r="F12" s="47"/>
-      <c r="G12" s="47"/>
+      <c r="B12" s="61"/>
+      <c r="C12" s="61"/>
+      <c r="D12" s="61"/>
+      <c r="E12" s="61"/>
+      <c r="F12" s="61"/>
+      <c r="G12" s="61"/>
       <c r="I12" s="1"/>
       <c r="J12" s="6" t="s">
         <v>1</v>
@@ -2200,15 +2305,15 @@
       <c r="G31" s="1"/>
     </row>
     <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="47" t="s">
+      <c r="A32" s="61" t="s">
         <v>81</v>
       </c>
-      <c r="B32" s="47"/>
-      <c r="C32" s="47"/>
-      <c r="D32" s="47"/>
-      <c r="E32" s="47"/>
-      <c r="F32" s="47"/>
-      <c r="G32" s="47"/>
+      <c r="B32" s="61"/>
+      <c r="C32" s="61"/>
+      <c r="D32" s="61"/>
+      <c r="E32" s="61"/>
+      <c r="F32" s="61"/>
+      <c r="G32" s="61"/>
       <c r="I32" s="1"/>
       <c r="J32" s="6" t="s">
         <v>1</v>
@@ -2673,10 +2778,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R86"/>
+  <dimension ref="A1:R134"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q50" sqref="Q50"/>
+    <sheetView tabSelected="1" topLeftCell="F34" workbookViewId="0">
+      <selection activeCell="L46" sqref="L46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2692,19 +2797,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="62" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
       <c r="K1" s="43"/>
+      <c r="L1" s="64"/>
       <c r="M1" s="11" t="s">
         <v>1</v>
       </c>
@@ -2722,40 +2828,38 @@
       </c>
     </row>
     <row r="2" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="44" t="s">
-        <v>7</v>
-      </c>
+      <c r="A2" s="44"/>
       <c r="B2" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49" t="s">
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63" t="s">
         <v>74</v>
       </c>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
       <c r="K2" s="4"/>
-      <c r="L2" t="s">
+      <c r="L2" s="64" t="s">
         <v>139</v>
       </c>
-      <c r="M2" s="42" t="s">
-        <v>41</v>
-      </c>
-      <c r="N2" s="53">
-        <v>0</v>
-      </c>
-      <c r="O2" s="57">
-        <f>N2</f>
-        <v>0</v>
-      </c>
-      <c r="P2" s="61">
-        <v>0</v>
+      <c r="M2" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="N2" s="50">
+        <v>156.440731910842</v>
+      </c>
+      <c r="O2" s="1">
+        <f>N2/100</f>
+        <v>1.56440731910842</v>
+      </c>
+      <c r="P2" s="58">
+        <v>1.06336745888669E-5</v>
       </c>
       <c r="R2" t="s">
         <v>75</v>
@@ -2789,32 +2893,32 @@
         <v>45</v>
       </c>
       <c r="K3" s="4"/>
-      <c r="L3" s="58">
-        <v>4.8611111111111112E-2</v>
-      </c>
-      <c r="M3" s="42" t="s">
-        <v>23</v>
-      </c>
-      <c r="N3" s="53">
-        <v>1.0599999427795399</v>
-      </c>
-      <c r="O3" s="57">
-        <f>N3</f>
-        <v>1.0599999427795399</v>
-      </c>
-      <c r="P3" s="61">
-        <v>-2.9953879373185301E-2</v>
+      <c r="L3" s="64" t="s">
+        <v>174</v>
+      </c>
+      <c r="M3" s="46" t="s">
+        <v>117</v>
+      </c>
+      <c r="N3" s="50">
+        <v>-20.300935880694301</v>
+      </c>
+      <c r="O3" s="1">
+        <f t="shared" ref="O3:O9" si="0">N3/100</f>
+        <v>-0.20300935880694301</v>
+      </c>
+      <c r="P3" s="58">
+        <v>4.3355679321677199E-5</v>
       </c>
       <c r="R3" s="2" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>1</v>
+      <c r="A4" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="B4" s="1">
-        <v>0</v>
+        <v>1.0599621403577</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -2824,25 +2928,28 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
-      <c r="M4" s="42" t="s">
-        <v>46</v>
-      </c>
-      <c r="N4" s="53">
-        <v>156.440731910842</v>
+      <c r="L4" s="64"/>
+      <c r="M4" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="N4" s="50">
+        <v>75.916881283268793</v>
       </c>
       <c r="O4" s="1">
-        <f>N4/100</f>
-        <v>1.56440731910842</v>
-      </c>
-      <c r="P4" s="61">
-        <v>-8.6738403137775998E-6</v>
+        <f t="shared" si="0"/>
+        <v>0.75916881283268789</v>
+      </c>
+      <c r="P4" s="58">
+        <v>1.3004902296165399E-6</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1.04103609065253</v>
+      </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -2851,25 +2958,28 @@
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
-      <c r="M5" s="42" t="s">
-        <v>117</v>
-      </c>
-      <c r="N5" s="53">
-        <v>-20.300935880694301</v>
+      <c r="L5" s="64"/>
+      <c r="M5" s="46" t="s">
+        <v>118</v>
+      </c>
+      <c r="N5" s="50">
+        <v>-0.155506560051652</v>
       </c>
       <c r="O5" s="1">
-        <f t="shared" ref="O5:O11" si="0">N5/100</f>
-        <v>-0.20300935880694301</v>
-      </c>
-      <c r="P5" s="61">
-        <v>2.1648716178694401E-3</v>
+        <f t="shared" si="0"/>
+        <v>-1.55506560051652E-3</v>
+      </c>
+      <c r="P5" s="58">
+        <v>1.94687132150312E-5</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>3</v>
-      </c>
-      <c r="B6" s="1"/>
+      <c r="A6" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.98533801740076798</v>
+      </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -2878,25 +2988,28 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
-      <c r="M6" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="N6" s="53">
-        <v>75.916881283268793</v>
+      <c r="L6" s="64"/>
+      <c r="M6" s="46" t="s">
+        <v>48</v>
+      </c>
+      <c r="N6" s="50">
+        <v>41.338725991097199</v>
       </c>
       <c r="O6" s="1">
         <f t="shared" si="0"/>
-        <v>0.75916881283268789</v>
-      </c>
-      <c r="P6" s="61">
-        <v>6.4758759358596297E-4</v>
+        <v>0.41338725991097197</v>
+      </c>
+      <c r="P6" s="58">
+        <v>6.7696186707433304E-6</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>4</v>
-      </c>
-      <c r="B7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1.00691238196979</v>
+      </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -2905,25 +3018,28 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
-      <c r="M7" s="42" t="s">
-        <v>118</v>
-      </c>
-      <c r="N7" s="53">
-        <v>-0.155506560051652</v>
+      <c r="L7" s="64"/>
+      <c r="M7" s="46" t="s">
+        <v>119</v>
+      </c>
+      <c r="N7" s="50">
+        <v>-3.8398609004379098</v>
       </c>
       <c r="O7" s="1">
         <f t="shared" si="0"/>
-        <v>-1.55506560051652E-3</v>
-      </c>
-      <c r="P7" s="61">
-        <v>-1.47979634931223E-3</v>
+        <v>-3.8398609004379101E-2</v>
+      </c>
+      <c r="P7" s="58">
+        <v>1.0256187421023299E-5</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>5</v>
-      </c>
-      <c r="B8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1.01577582353094</v>
+      </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -2932,25 +3048,28 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
-      <c r="M8" s="42" t="s">
-        <v>48</v>
-      </c>
-      <c r="N8" s="53">
-        <v>41.338725991097199</v>
+      <c r="L8" s="64"/>
+      <c r="M8" s="46" t="s">
+        <v>49</v>
+      </c>
+      <c r="N8" s="50">
+        <v>232.35762119293199</v>
       </c>
       <c r="O8" s="1">
         <f t="shared" si="0"/>
-        <v>0.41338725991097197</v>
-      </c>
-      <c r="P8" s="61">
-        <v>6.8870384835700903E-4</v>
+        <v>2.32357621192932</v>
+      </c>
+      <c r="P8" s="58">
+        <v>1.20141648185523E-5</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>6</v>
-      </c>
-      <c r="B9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1.0048890478609001</v>
+      </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -2958,25 +3077,28 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
-      <c r="M9" s="42" t="s">
-        <v>119</v>
-      </c>
-      <c r="N9" s="53">
-        <v>-3.8398609004379098</v>
+      <c r="L9" s="64"/>
+      <c r="M9" s="46" t="s">
+        <v>83</v>
+      </c>
+      <c r="N9" s="50">
+        <v>-20.456442236900301</v>
       </c>
       <c r="O9" s="1">
         <f t="shared" si="0"/>
-        <v>-3.8398609004379101E-2</v>
-      </c>
-      <c r="P9" s="61">
-        <v>-1.3891657030102901E-3</v>
+        <v>-0.20456442236900302</v>
+      </c>
+      <c r="P9" s="58">
+        <v>6.2827392531661404E-5</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>7</v>
-      </c>
-      <c r="B10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1.0165083916826201</v>
+      </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="F10" s="1"/>
@@ -2985,25 +3107,30 @@
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
-      <c r="M10" s="42" t="s">
-        <v>49</v>
-      </c>
-      <c r="N10" s="53">
-        <v>232.35762119293199</v>
+      <c r="L10" s="64" t="s">
+        <v>140</v>
+      </c>
+      <c r="M10" s="46" t="s">
+        <v>52</v>
+      </c>
+      <c r="N10" s="50">
+        <v>-23.569740833506799</v>
       </c>
       <c r="O10" s="1">
-        <f t="shared" si="0"/>
-        <v>2.32357621192932</v>
-      </c>
-      <c r="P10" s="61">
-        <v>6.3899375327158804E-4</v>
+        <f>N10/100</f>
+        <v>-0.235697408335068</v>
+      </c>
+      <c r="P10" s="58">
+        <v>-1.5324438971953099E-6</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>8</v>
-      </c>
-      <c r="B11" s="1"/>
+      <c r="A11" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1.05436901591651</v>
+      </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="F11" s="1"/>
@@ -3012,25 +3139,30 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
-      <c r="M11" s="42" t="s">
-        <v>83</v>
-      </c>
-      <c r="N11" s="53">
-        <v>-20.456442236900301</v>
+      <c r="L11" s="64" t="s">
+        <v>175</v>
+      </c>
+      <c r="M11" s="46" t="s">
+        <v>120</v>
+      </c>
+      <c r="N11" s="50">
+        <v>0.96859150246414105</v>
       </c>
       <c r="O11" s="1">
-        <f t="shared" si="0"/>
-        <v>-0.20456442236900302</v>
-      </c>
-      <c r="P11" s="61">
-        <v>6.8507826856001298E-4</v>
+        <f t="shared" ref="O11:O15" si="1">N11/100</f>
+        <v>9.6859150246414102E-3</v>
+      </c>
+      <c r="P11" s="58">
+        <v>-5.9967407733847699E-6</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>9</v>
-      </c>
-      <c r="B12" s="1"/>
+      <c r="A12" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0.99791127060776097</v>
+      </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="F12" s="1"/>
@@ -3039,28 +3171,28 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
-      <c r="L12" t="s">
-        <v>140</v>
-      </c>
-      <c r="M12" s="42" t="s">
-        <v>51</v>
-      </c>
-      <c r="N12" s="53">
-        <v>-0.22125272217770001</v>
-      </c>
-      <c r="O12" s="57">
-        <f>N12</f>
-        <v>-0.22125272217770001</v>
-      </c>
-      <c r="P12" s="62">
-        <v>-0.2212527222</v>
+      <c r="L12" s="64"/>
+      <c r="M12" s="46" t="s">
+        <v>53</v>
+      </c>
+      <c r="N12" s="50">
+        <v>29.247688021076399</v>
+      </c>
+      <c r="O12" s="1">
+        <f t="shared" si="1"/>
+        <v>0.29247688021076401</v>
+      </c>
+      <c r="P12" s="58">
+        <v>6.0811903938029496E-6</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>10</v>
-      </c>
-      <c r="B13" s="1"/>
+      <c r="A13" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0.99039833975510105</v>
+      </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="F13" s="1"/>
@@ -3069,28 +3201,28 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
-      <c r="L13" s="58">
-        <v>0.47083333333333338</v>
-      </c>
-      <c r="M13" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="N13" s="53">
-        <v>1.0099999973080001</v>
-      </c>
-      <c r="O13" s="57">
-        <f>N13</f>
-        <v>1.0099999973080001</v>
-      </c>
-      <c r="P13" s="62">
-        <v>2.17540256007367E-2</v>
+      <c r="L13" s="64"/>
+      <c r="M13" s="46" t="s">
+        <v>121</v>
+      </c>
+      <c r="N13" s="50">
+        <v>-10.134384235994199</v>
+      </c>
+      <c r="O13" s="1">
+        <f t="shared" si="1"/>
+        <v>-0.101343842359942</v>
+      </c>
+      <c r="P13" s="58">
+        <v>8.8204619878157198E-6</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>11</v>
-      </c>
-      <c r="B14" s="1"/>
+      <c r="A14" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0.99354407863493799</v>
+      </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -3100,25 +3232,28 @@
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
-      <c r="M14" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="N14" s="53">
-        <v>-23.569740833506799</v>
+      <c r="L14" s="64"/>
+      <c r="M14" s="46" t="s">
+        <v>54</v>
+      </c>
+      <c r="N14" s="50">
+        <v>4.9388912162000001E-5</v>
       </c>
       <c r="O14" s="1">
-        <f>N14/100</f>
-        <v>-0.235697408335068</v>
-      </c>
-      <c r="P14" s="61">
-        <v>-1.05523560178061E-3</v>
+        <f t="shared" si="1"/>
+        <v>4.9388912162000003E-7</v>
+      </c>
+      <c r="P14" s="58">
+        <v>7.3644127437410898E-6</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>12</v>
-      </c>
-      <c r="B15" s="1"/>
+      <c r="A15" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0.98670699585233201</v>
+      </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -3127,25 +3262,28 @@
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
-      <c r="M15" s="42" t="s">
-        <v>120</v>
-      </c>
-      <c r="N15" s="53">
-        <v>0.96859150246414105</v>
+      <c r="L15" s="64"/>
+      <c r="M15" s="46" t="s">
+        <v>122</v>
+      </c>
+      <c r="N15" s="50">
+        <v>-23.1382548362844</v>
       </c>
       <c r="O15" s="1">
-        <f t="shared" ref="O15:O19" si="1">N15/100</f>
-        <v>9.6859150246414102E-3</v>
-      </c>
-      <c r="P15" s="61">
-        <v>-2.2375145874756201E-3</v>
+        <f t="shared" si="1"/>
+        <v>-0.231382548362844</v>
+      </c>
+      <c r="P15" s="58">
+        <v>-1.3409001482223E-6</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>13</v>
-      </c>
-      <c r="B16" s="1"/>
+      <c r="A16" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0.98227711504043203</v>
+      </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -3155,25 +3293,30 @@
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
-      <c r="M16" s="42" t="s">
-        <v>53</v>
-      </c>
-      <c r="N16" s="53">
-        <v>29.247688021076399</v>
+      <c r="L16" s="64" t="s">
+        <v>141</v>
+      </c>
+      <c r="M16" s="46" t="s">
+        <v>56</v>
+      </c>
+      <c r="N16" s="50">
+        <v>6.4193752642371704</v>
       </c>
       <c r="O16" s="1">
-        <f t="shared" si="1"/>
-        <v>0.29247688021076401</v>
-      </c>
-      <c r="P16" s="61">
-        <v>5.1585990707936401E-4</v>
+        <f>N16/100</f>
+        <v>6.4193752642371704E-2</v>
+      </c>
+      <c r="P16" s="58">
+        <v>-1.70762709954253E-6</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>14</v>
-      </c>
-      <c r="B17" s="1"/>
+      <c r="A17" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0.96821859389559195</v>
+      </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -3183,396 +3326,491 @@
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
-      <c r="M17" s="42" t="s">
-        <v>121</v>
-      </c>
-      <c r="N17" s="53">
-        <v>-10.134384235994199</v>
+      <c r="L17" s="64" t="s">
+        <v>176</v>
+      </c>
+      <c r="M17" s="46" t="s">
+        <v>124</v>
+      </c>
+      <c r="N17" s="50">
+        <v>1.57798981550307</v>
       </c>
       <c r="O17" s="1">
-        <f t="shared" si="1"/>
-        <v>-0.101343842359942</v>
-      </c>
-      <c r="P17" s="61">
-        <v>-2.7105327863768802E-3</v>
+        <f t="shared" ref="O17:O25" si="2">N17/100</f>
+        <v>1.5779898155030701E-2</v>
+      </c>
+      <c r="P17" s="58">
+        <v>-3.39117996042693E-6</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="M18" s="42" t="s">
-        <v>54</v>
-      </c>
-      <c r="N18" s="53">
-        <v>4.9388912162000001E-5</v>
+      <c r="A18" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B18">
+        <v>-9.0498906725745204E-2</v>
+      </c>
+      <c r="L18" s="64"/>
+      <c r="M18" s="46" t="s">
+        <v>57</v>
+      </c>
+      <c r="N18" s="50">
+        <v>7.6111237412808599</v>
       </c>
       <c r="O18" s="1">
-        <f t="shared" si="1"/>
-        <v>4.9388912162000003E-7</v>
-      </c>
-      <c r="P18" s="61">
-        <v>6.5059278082477401E-7</v>
+        <f t="shared" si="2"/>
+        <v>7.6111237412808605E-2</v>
+      </c>
+      <c r="P18" s="58">
+        <v>-2.9288166818880502E-6</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="M19" s="42" t="s">
-        <v>122</v>
-      </c>
-      <c r="N19" s="53">
-        <v>-23.1382548362844</v>
+      <c r="A19" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B19">
+        <v>-0.22165365184591099</v>
+      </c>
+      <c r="L19" s="64"/>
+      <c r="M19" s="46" t="s">
+        <v>123</v>
+      </c>
+      <c r="N19" s="50">
+        <v>2.2749299623984598</v>
       </c>
       <c r="O19" s="1">
-        <f t="shared" si="1"/>
-        <v>-0.231382548362844</v>
-      </c>
-      <c r="P19" s="61">
-        <v>1.7465773008429299E-7</v>
+        <f t="shared" si="2"/>
+        <v>2.2749299623984597E-2</v>
+      </c>
+      <c r="P19" s="58">
+        <v>4.5373436844440403E-5</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L20" t="s">
-        <v>141</v>
-      </c>
-      <c r="M20" s="42" t="s">
-        <v>55</v>
-      </c>
-      <c r="N20" s="53">
-        <v>-0.25510563387813501</v>
-      </c>
-      <c r="O20" s="57">
-        <f>N20</f>
-        <v>-0.25510563387813501</v>
-      </c>
-      <c r="P20" s="62">
-        <v>-0.25510563390000002</v>
+      <c r="A20" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B20">
+        <v>-0.184493248459114</v>
+      </c>
+      <c r="L20" s="64"/>
+      <c r="M20" s="46" t="s">
+        <v>58</v>
+      </c>
+      <c r="N20" s="50">
+        <v>17.236621109828601</v>
+      </c>
+      <c r="O20" s="1">
+        <f t="shared" si="2"/>
+        <v>0.17236621109828601</v>
+      </c>
+      <c r="P20" s="58">
+        <v>-1.4699917021965299E-6</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L21" s="58">
-        <v>0.8125</v>
-      </c>
-      <c r="M21" s="42" t="s">
-        <v>114</v>
-      </c>
-      <c r="N21" s="53">
-        <v>1.0385379019832599</v>
-      </c>
-      <c r="O21" s="57">
-        <f>N21</f>
-        <v>1.0385379019832599</v>
-      </c>
-      <c r="P21" s="62">
-        <v>-5.12238863404413E-3</v>
+      <c r="A21" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B21">
+        <v>-0.15841659033345201</v>
+      </c>
+      <c r="L21" s="64"/>
+      <c r="M21" s="46" t="s">
+        <v>125</v>
+      </c>
+      <c r="N21" s="50">
+        <v>6.2088690408799696</v>
+      </c>
+      <c r="O21" s="1">
+        <f t="shared" si="2"/>
+        <v>6.2088690408799697E-2</v>
+      </c>
+      <c r="P21" s="58">
+        <v>6.9140064405080802E-5</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="M22" s="42" t="s">
-        <v>56</v>
-      </c>
-      <c r="N22" s="53">
-        <v>6.4193752642371704</v>
+      <c r="A22" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B22">
+        <v>-0.262083078069408</v>
+      </c>
+      <c r="L22" s="64"/>
+      <c r="M22" s="46" t="s">
+        <v>59</v>
+      </c>
+      <c r="N22" s="50">
+        <v>1.4392071686730901</v>
       </c>
       <c r="O22" s="1">
-        <f>N22/100</f>
-        <v>6.4193752642371704E-2</v>
-      </c>
-      <c r="P22" s="61">
-        <v>1.2851248455257599E-4</v>
+        <f t="shared" si="2"/>
+        <v>1.4392071686730901E-2</v>
+      </c>
+      <c r="P22" s="58">
+        <v>-3.0935268891200298E-6</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="M23" s="42" t="s">
-        <v>124</v>
-      </c>
-      <c r="N23" s="53">
-        <v>1.57798981550307</v>
+      <c r="A23" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B23">
+        <v>-0.24699463946439601</v>
+      </c>
+      <c r="L23" s="64"/>
+      <c r="M23" s="46" t="s">
+        <v>126</v>
+      </c>
+      <c r="N23" s="50">
+        <v>0.52526799870488805</v>
       </c>
       <c r="O23" s="1">
-        <f t="shared" ref="O23:O31" si="2">N23/100</f>
-        <v>1.5779898155030701E-2</v>
-      </c>
-      <c r="P23" s="61">
-        <v>1.0767413611616999E-3</v>
+        <f t="shared" si="2"/>
+        <v>5.2526799870488807E-3</v>
+      </c>
+      <c r="P23" s="58">
+        <v>-8.1203675952107E-6</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="M24" s="42" t="s">
-        <v>57</v>
-      </c>
-      <c r="N24" s="53">
-        <v>7.6111237412808599</v>
+      <c r="A24" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B24">
+        <v>-0.25619422730604202</v>
+      </c>
+      <c r="L24" s="64"/>
+      <c r="M24" s="46" t="s">
+        <v>12</v>
+      </c>
+      <c r="N24" s="50">
+        <v>-6.1</v>
       </c>
       <c r="O24" s="1">
         <f t="shared" si="2"/>
-        <v>7.6111237412808605E-2</v>
-      </c>
-      <c r="P24" s="61">
-        <v>1.6297137374082799E-5</v>
+        <v>-6.0999999999999999E-2</v>
+      </c>
+      <c r="P24" s="58">
+        <v>2.3373457752606801E-9</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="M25" s="42" t="s">
-        <v>123</v>
-      </c>
-      <c r="N25" s="53">
-        <v>2.2749299623984598</v>
+      <c r="A25" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B25">
+        <v>-0.274128496301564</v>
+      </c>
+      <c r="L25" s="64"/>
+      <c r="M25" s="46" t="s">
+        <v>20</v>
+      </c>
+      <c r="N25" s="50">
+        <v>-1.6</v>
       </c>
       <c r="O25" s="1">
         <f t="shared" si="2"/>
-        <v>2.2749299623984597E-2</v>
-      </c>
-      <c r="P25" s="61">
-        <v>9.80565804585901E-5</v>
+        <v>-1.6E-2</v>
+      </c>
+      <c r="P25" s="58">
+        <v>5.1566951013160001E-5</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="M26" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="N26" s="53">
-        <v>17.236621109828601</v>
+      <c r="A26" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B26">
+        <v>-0.27530156310841902</v>
+      </c>
+      <c r="L26" s="64" t="s">
+        <v>142</v>
+      </c>
+      <c r="M26" s="46" t="s">
+        <v>61</v>
+      </c>
+      <c r="N26" s="50">
+        <v>6.1481308294477897</v>
       </c>
       <c r="O26" s="1">
-        <f t="shared" si="2"/>
-        <v>0.17236621109828601</v>
-      </c>
-      <c r="P26" s="61">
-        <v>2.8072391037720099E-5</v>
+        <f>N26/100</f>
+        <v>6.1481308294477899E-2</v>
+      </c>
+      <c r="P26" s="57">
+        <v>-1.3131668610555401E-6</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="M27" s="42" t="s">
-        <v>125</v>
-      </c>
-      <c r="N27" s="53">
-        <v>6.2088690408799696</v>
+      <c r="A27" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B27">
+        <v>-0.27033852619593501</v>
+      </c>
+      <c r="L27" s="56" t="s">
+        <v>177</v>
+      </c>
+      <c r="M27" s="46" t="s">
+        <v>127</v>
+      </c>
+      <c r="N27" s="50">
+        <v>6.1776975079165704</v>
       </c>
       <c r="O27" s="1">
-        <f t="shared" si="2"/>
-        <v>6.2088690408799697E-2</v>
-      </c>
-      <c r="P27" s="61">
-        <v>3.8053003130694002E-4</v>
+        <f t="shared" ref="O27:O39" si="3">N27/100</f>
+        <v>6.1776975079165707E-2</v>
+      </c>
+      <c r="P27" s="57">
+        <v>4.8795271359383697E-6</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="M28" s="42" t="s">
-        <v>59</v>
-      </c>
-      <c r="N28" s="53">
-        <v>1.4392071686730901</v>
+      <c r="A28" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B28">
+        <v>-0.27393942115060799</v>
+      </c>
+      <c r="L28" s="65"/>
+      <c r="M28" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="N28" s="50">
+        <v>10.1258308263922</v>
       </c>
       <c r="O28" s="1">
-        <f t="shared" si="2"/>
-        <v>1.4392071686730901E-2</v>
-      </c>
-      <c r="P28" s="61">
-        <v>3.3901950999533699E-5</v>
+        <f t="shared" si="3"/>
+        <v>0.101258308263922</v>
+      </c>
+      <c r="P28" s="58">
+        <v>-1.22208074135322E-6</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="M29" s="42" t="s">
-        <v>126</v>
-      </c>
-      <c r="N29" s="53">
-        <v>0.52526799870488805</v>
+      <c r="A29" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B29">
+        <v>-0.274447646882094</v>
+      </c>
+      <c r="L29" s="65"/>
+      <c r="M29" s="46" t="s">
+        <v>128</v>
+      </c>
+      <c r="N29" s="50">
+        <v>4.8779939913553596</v>
       </c>
       <c r="O29" s="1">
-        <f t="shared" si="2"/>
-        <v>5.2526799870488807E-3</v>
-      </c>
-      <c r="P29" s="61">
-        <v>9.7871725652031802E-5</v>
+        <f t="shared" si="3"/>
+        <v>4.8779939913553595E-2</v>
+      </c>
+      <c r="P29" s="57">
+        <v>4.90141539373143E-5</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="M30" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="N30" s="53">
-        <v>-6.1</v>
+      <c r="A30" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B30">
+        <v>-0.28719972332980598</v>
+      </c>
+      <c r="L30" s="64" t="s">
+        <v>143</v>
+      </c>
+      <c r="M30" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="N30" s="50">
+        <v>-7.6</v>
       </c>
       <c r="O30" s="1">
-        <f t="shared" si="2"/>
-        <v>-6.0999999999999999E-2</v>
-      </c>
-      <c r="P30" s="61">
-        <v>-5.5804864002167998E-6</v>
+        <f t="shared" si="3"/>
+        <v>-7.5999999999999998E-2</v>
+      </c>
+      <c r="P30" s="58">
+        <v>4.3947993498549799E-7</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="M31" s="42" t="s">
-        <v>20</v>
-      </c>
-      <c r="N31" s="53">
+      <c r="L31" s="56" t="s">
+        <v>178</v>
+      </c>
+      <c r="M31" s="46" t="s">
+        <v>129</v>
+      </c>
+      <c r="N31" s="50">
         <v>-1.6</v>
       </c>
       <c r="O31" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-1.6E-2</v>
       </c>
-      <c r="P31" s="61">
-        <v>5.2797756594065403E-5</v>
+      <c r="P31" s="58">
+        <v>-1.14950706093311E-5</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L32" t="s">
-        <v>142</v>
-      </c>
-      <c r="M32" s="42" t="s">
-        <v>60</v>
-      </c>
-      <c r="N32" s="53">
-        <v>-0.26806990591321</v>
-      </c>
-      <c r="O32" s="57">
-        <f>N32</f>
-        <v>-0.26806990591321</v>
-      </c>
-      <c r="P32" s="62">
-        <v>-0.26806990590000002</v>
+      <c r="L32" s="64" t="s">
+        <v>144</v>
+      </c>
+      <c r="M32" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="N32" s="51">
+        <v>-63.001699846354903</v>
+      </c>
+      <c r="O32" s="1">
+        <f t="shared" si="3"/>
+        <v>-0.63001699846354908</v>
+      </c>
+      <c r="P32" s="58">
+        <v>-7.6439598420963202E-6</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L33" s="59" t="s">
-        <v>147</v>
-      </c>
-      <c r="M33" s="42" t="s">
-        <v>115</v>
-      </c>
-      <c r="N33" s="53">
-        <v>1.0349152577221601</v>
-      </c>
-      <c r="O33" s="57">
-        <f>N33</f>
-        <v>1.0349152577221601</v>
-      </c>
-      <c r="P33" s="62">
-        <v>-2.1765958813597698E-3</v>
+      <c r="L33" s="56" t="s">
+        <v>179</v>
+      </c>
+      <c r="M33" s="46" t="s">
+        <v>130</v>
+      </c>
+      <c r="N33" s="50">
+        <v>10.2039485868599</v>
+      </c>
+      <c r="O33" s="1">
+        <f t="shared" si="3"/>
+        <v>0.102039485868599</v>
+      </c>
+      <c r="P33" s="58">
+        <v>-1.95571751745866E-5</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L34" s="50"/>
-      <c r="M34" s="42" t="s">
-        <v>61</v>
-      </c>
-      <c r="N34" s="53">
-        <v>6.1481308294477897</v>
+      <c r="L34" s="64"/>
+      <c r="M34" s="46" t="s">
+        <v>65</v>
+      </c>
+      <c r="N34" s="50">
+        <v>16.526211548050401</v>
       </c>
       <c r="O34" s="1">
-        <f>N34/100</f>
-        <v>6.1481308294477899E-2</v>
-      </c>
-      <c r="P34" s="60">
-        <v>-1.88116567434796E-5</v>
+        <f t="shared" si="3"/>
+        <v>0.16526211548050401</v>
+      </c>
+      <c r="P34" s="58">
+        <v>-4.8466870822272401E-7</v>
       </c>
     </row>
     <row r="35" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="52"/>
-      <c r="B35" s="52"/>
-      <c r="C35" s="52"/>
-      <c r="D35" s="52"/>
-      <c r="E35" s="52"/>
-      <c r="F35" s="52"/>
-      <c r="G35" s="52"/>
-      <c r="H35" s="52"/>
-      <c r="I35" s="52"/>
-      <c r="J35" s="52"/>
-      <c r="K35" s="52"/>
-      <c r="L35" s="50"/>
-      <c r="M35" s="42" t="s">
-        <v>127</v>
-      </c>
-      <c r="N35" s="53">
-        <v>6.1776975079165704</v>
+      <c r="A35" s="49"/>
+      <c r="B35" s="49"/>
+      <c r="C35" s="49"/>
+      <c r="D35" s="49"/>
+      <c r="E35" s="49"/>
+      <c r="F35" s="49"/>
+      <c r="G35" s="49"/>
+      <c r="H35" s="49"/>
+      <c r="I35" s="49"/>
+      <c r="J35" s="49"/>
+      <c r="K35" s="49"/>
+      <c r="L35" s="64"/>
+      <c r="M35" s="46" t="s">
+        <v>131</v>
+      </c>
+      <c r="N35" s="52">
+        <v>-1.34369314780613</v>
       </c>
       <c r="O35" s="1">
-        <f t="shared" ref="O35:O47" si="3">N35/100</f>
-        <v>6.1776975079165707E-2</v>
-      </c>
-      <c r="P35" s="60">
-        <v>-4.4567340559324698E-4</v>
+        <f t="shared" si="3"/>
+        <v>-1.34369314780613E-2</v>
+      </c>
+      <c r="P35" s="58">
+        <v>5.79302350887934E-6</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A36" s="50"/>
-      <c r="B36" s="50"/>
-      <c r="C36" s="50"/>
-      <c r="D36" s="50"/>
-      <c r="E36" s="50"/>
-      <c r="F36" s="50"/>
-      <c r="G36" s="50"/>
-      <c r="H36" s="50"/>
-      <c r="I36" s="50"/>
-      <c r="J36" s="50"/>
-      <c r="K36" s="50"/>
-      <c r="L36" s="50"/>
-      <c r="M36" s="42" t="s">
-        <v>62</v>
-      </c>
-      <c r="N36" s="53">
-        <v>10.1258308263922</v>
+      <c r="A36" s="47"/>
+      <c r="B36" s="47"/>
+      <c r="C36" s="47"/>
+      <c r="D36" s="47"/>
+      <c r="E36" s="47"/>
+      <c r="F36" s="47"/>
+      <c r="G36" s="47"/>
+      <c r="H36" s="47"/>
+      <c r="I36" s="47"/>
+      <c r="J36" s="47"/>
+      <c r="K36" s="47"/>
+      <c r="L36" s="64"/>
+      <c r="M36" s="46" t="s">
+        <v>66</v>
+      </c>
+      <c r="N36" s="52">
+        <v>29.247637436823101</v>
       </c>
       <c r="O36" s="1">
         <f t="shared" si="3"/>
-        <v>0.101258308263922</v>
-      </c>
-      <c r="P36" s="61">
-        <v>-1.40656940313608E-4</v>
+        <v>0.29247637436823104</v>
+      </c>
+      <c r="P36" s="58">
+        <v>-9.6765970603040998E-7</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A37" s="50"/>
-      <c r="B37" s="50"/>
-      <c r="C37" s="50"/>
-      <c r="D37" s="50"/>
-      <c r="E37" s="50"/>
-      <c r="F37" s="50"/>
-      <c r="G37" s="50"/>
-      <c r="H37" s="50"/>
-      <c r="I37" s="50"/>
-      <c r="J37" s="50"/>
-      <c r="K37" s="50"/>
-      <c r="L37" s="50"/>
-      <c r="M37" s="42" t="s">
-        <v>128</v>
-      </c>
-      <c r="N37" s="53">
-        <v>4.8779939913553596</v>
+      <c r="A37" s="47"/>
+      <c r="B37" s="47"/>
+      <c r="C37" s="47"/>
+      <c r="D37" s="47"/>
+      <c r="E37" s="47"/>
+      <c r="F37" s="47"/>
+      <c r="G37" s="47"/>
+      <c r="H37" s="47"/>
+      <c r="I37" s="47"/>
+      <c r="J37" s="47"/>
+      <c r="K37" s="47"/>
+      <c r="L37" s="64"/>
+      <c r="M37" s="46" t="s">
+        <v>132</v>
+      </c>
+      <c r="N37" s="52">
+        <v>11.0919776937066</v>
       </c>
       <c r="O37" s="1">
         <f t="shared" si="3"/>
-        <v>4.8779939913553595E-2</v>
-      </c>
-      <c r="P37" s="60">
-        <v>-6.3339605935184401E-4</v>
+        <v>0.11091977693706599</v>
+      </c>
+      <c r="P37" s="58">
+        <v>1.05122553067938E-5</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A38" s="50"/>
-      <c r="B38" s="50"/>
-      <c r="C38" s="50"/>
-      <c r="D38" s="50"/>
-      <c r="E38" s="50"/>
-      <c r="F38" s="50"/>
-      <c r="G38" s="50"/>
-      <c r="H38" s="50"/>
-      <c r="I38" s="50"/>
-      <c r="J38" s="50"/>
-      <c r="K38" s="50"/>
-      <c r="L38" t="s">
-        <v>143</v>
-      </c>
-      <c r="M38" s="42" t="s">
-        <v>63</v>
+      <c r="A38" s="47"/>
+      <c r="B38" s="47"/>
+      <c r="C38" s="47"/>
+      <c r="D38" s="47"/>
+      <c r="E38" s="47"/>
+      <c r="F38" s="47"/>
+      <c r="G38" s="47"/>
+      <c r="H38" s="47"/>
+      <c r="I38" s="47"/>
+      <c r="J38" s="47"/>
+      <c r="K38" s="47"/>
+      <c r="L38" s="64"/>
+      <c r="M38" s="46" t="s">
+        <v>67</v>
       </c>
       <c r="N38" s="53">
-        <v>-7.6</v>
+        <v>-94.199996999999996</v>
       </c>
       <c r="O38" s="1">
         <f t="shared" si="3"/>
-        <v>-7.5999999999999998E-2</v>
-      </c>
-      <c r="P38" s="61">
-        <v>-1.4483820858600399E-4</v>
+        <v>-0.94199996999999991</v>
+      </c>
+      <c r="P38" s="58">
+        <v>-4.0078032588208899E-6</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
@@ -3585,21 +3823,20 @@
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
-      <c r="L39" s="59" t="s">
-        <v>148</v>
-      </c>
-      <c r="M39" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="N39" s="53">
-        <v>-1.6</v>
+      <c r="L39" s="64"/>
+      <c r="M39" s="46" t="s">
+        <v>133</v>
+      </c>
+      <c r="N39">
+        <f>21.4613437652587-19</f>
+        <v>2.4613437652587002</v>
       </c>
       <c r="O39" s="1">
         <f t="shared" si="3"/>
-        <v>-1.6E-2</v>
-      </c>
-      <c r="P39" s="61">
-        <v>-3.5573742834272E-3</v>
+        <v>2.4613437652587004E-2</v>
+      </c>
+      <c r="P39" s="58">
+        <v>-3.0646956959021199E-5</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
@@ -3611,21 +3848,21 @@
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
-      <c r="L40" t="s">
-        <v>144</v>
-      </c>
-      <c r="M40" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="N40" s="54">
-        <v>-63.001699846354903</v>
+      <c r="L40" s="64" t="s">
+        <v>145</v>
+      </c>
+      <c r="M40" s="46" t="s">
+        <v>68</v>
+      </c>
+      <c r="N40" s="52">
+        <v>4.9650161007164098</v>
       </c>
       <c r="O40" s="1">
-        <f t="shared" si="3"/>
-        <v>-0.63001699846354908</v>
-      </c>
-      <c r="P40" s="61">
-        <v>-9.5060452610995505E-4</v>
+        <f>N40/100</f>
+        <v>4.9650161007164101E-2</v>
+      </c>
+      <c r="P40" s="58">
+        <v>-1.8263251861869199E-6</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
@@ -3638,21 +3875,21 @@
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
-      <c r="L41" s="59" t="s">
-        <v>149</v>
-      </c>
-      <c r="M41" s="42" t="s">
-        <v>130</v>
-      </c>
-      <c r="N41" s="53">
-        <v>10.2039485868599</v>
+      <c r="L41" s="56" t="s">
+        <v>180</v>
+      </c>
+      <c r="M41" s="46" t="s">
+        <v>134</v>
+      </c>
+      <c r="N41" s="52">
+        <v>0.52427629116916796</v>
       </c>
       <c r="O41" s="1">
-        <f t="shared" si="3"/>
-        <v>0.102039485868599</v>
-      </c>
-      <c r="P41" s="61">
-        <v>-5.1145973996759402E-3</v>
+        <f t="shared" ref="O41:O43" si="4">N41/100</f>
+        <v>5.2427629116916794E-3</v>
+      </c>
+      <c r="P41" s="58">
+        <v>6.8227725995599298E-6</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
@@ -3665,18 +3902,19 @@
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
-      <c r="M42" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="N42" s="53">
-        <v>16.526211548050401</v>
+      <c r="L42" s="64"/>
+      <c r="M42" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="N42" s="52">
+        <v>-13.5</v>
       </c>
       <c r="O42" s="1">
-        <f t="shared" si="3"/>
-        <v>0.16526211548050401</v>
-      </c>
-      <c r="P42" s="61">
-        <v>3.0418249791705498E-4</v>
+        <f t="shared" si="4"/>
+        <v>-0.13500000000000001</v>
+      </c>
+      <c r="P42" s="58">
+        <v>3.1143046591852699E-6</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
@@ -3690,18 +3928,19 @@
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
-      <c r="M43" s="42" t="s">
-        <v>131</v>
-      </c>
-      <c r="N43" s="55">
-        <v>-1.34369314780613</v>
+      <c r="L43" s="64"/>
+      <c r="M43" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="N43" s="52">
+        <v>-5.8</v>
       </c>
       <c r="O43" s="1">
-        <f t="shared" si="3"/>
-        <v>-1.34369314780613E-2</v>
-      </c>
-      <c r="P43" s="61">
-        <v>-1.37670401876801E-3</v>
+        <f t="shared" si="4"/>
+        <v>-5.7999999999999996E-2</v>
+      </c>
+      <c r="P43" s="58">
+        <v>5.0234520724452802E-5</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
@@ -3715,18 +3954,21 @@
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
-      <c r="M44" s="42" t="s">
-        <v>66</v>
-      </c>
-      <c r="N44" s="55">
-        <v>29.247637436823101</v>
+      <c r="L44" s="64" t="s">
+        <v>146</v>
+      </c>
+      <c r="M44" s="46" t="s">
+        <v>69</v>
+      </c>
+      <c r="N44" s="52">
+        <v>-2.8744036925517298</v>
       </c>
       <c r="O44" s="1">
-        <f t="shared" si="3"/>
-        <v>0.29247637436823104</v>
-      </c>
-      <c r="P44" s="61">
-        <v>2.2761940039589499E-4</v>
+        <f>N44/100</f>
+        <v>-2.8744036925517299E-2</v>
+      </c>
+      <c r="P44" s="58">
+        <v>1.03396272051193E-6</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
@@ -3740,18 +3982,21 @@
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
-      <c r="M45" s="42" t="s">
-        <v>132</v>
-      </c>
-      <c r="N45" s="55">
-        <v>11.0919776937066</v>
+      <c r="L45" s="56" t="s">
+        <v>181</v>
+      </c>
+      <c r="M45" s="46" t="s">
+        <v>135</v>
+      </c>
+      <c r="N45" s="52">
+        <v>0.31779049296478201</v>
       </c>
       <c r="O45" s="1">
-        <f t="shared" si="3"/>
-        <v>0.11091977693706599</v>
-      </c>
-      <c r="P45" s="61">
-        <v>-1.3983824680780001E-3</v>
+        <f t="shared" ref="O45:O47" si="5">N45/100</f>
+        <v>3.1779049296478202E-3</v>
+      </c>
+      <c r="P45" s="58">
+        <v>4.5458701069499302E-6</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
@@ -3765,18 +4010,19 @@
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
-      <c r="M46" s="42" t="s">
-        <v>67</v>
-      </c>
-      <c r="N46" s="56">
-        <v>-94.199996999999996</v>
+      <c r="L46" s="64"/>
+      <c r="M46" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="N46" s="52">
+        <v>-14.9</v>
       </c>
       <c r="O46" s="1">
-        <f t="shared" si="3"/>
-        <v>-0.94199996999999991</v>
-      </c>
-      <c r="P46" s="61">
-        <v>-2.81965662445027E-3</v>
+        <f t="shared" si="5"/>
+        <v>-0.14899999999999999</v>
+      </c>
+      <c r="P46" s="58">
+        <v>3.11371443725839E-6</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
@@ -3790,19 +4036,19 @@
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
-      <c r="M47" s="42" t="s">
-        <v>133</v>
-      </c>
-      <c r="N47">
-        <f>21.4613437652587-19</f>
-        <v>2.4613437652587002</v>
+      <c r="L47" s="64"/>
+      <c r="M47" s="46" t="s">
+        <v>136</v>
+      </c>
+      <c r="N47" s="52">
+        <v>-5</v>
       </c>
       <c r="O47" s="1">
-        <f t="shared" si="3"/>
-        <v>2.4613437652587004E-2</v>
-      </c>
-      <c r="P47" s="61">
-        <v>-6.8701998242329402E-3</v>
+        <f t="shared" si="5"/>
+        <v>-0.05</v>
+      </c>
+      <c r="P47" s="58">
+        <v>4.6668128149698902E-5</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
@@ -3810,28 +4056,18 @@
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
-      <c r="M48" s="42" t="s">
-        <v>51</v>
-      </c>
-      <c r="N48" s="55">
-        <v>-0.22125272217770001</v>
-      </c>
-      <c r="O48" s="57">
-        <f>N48</f>
-        <v>-0.22125272217770001</v>
-      </c>
-      <c r="P48" s="62">
-        <v>-0.2212527222</v>
-      </c>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M48" s="46"/>
+      <c r="N48" s="52"/>
+      <c r="O48" s="1"/>
+      <c r="P48" s="58"/>
+    </row>
+    <row r="49" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -3843,46 +4079,46 @@
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
-      <c r="M49" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="N49" s="55">
-        <v>1.0099999973080001</v>
-      </c>
-      <c r="O49" s="57">
-        <f>N49</f>
-        <v>1.0099999973080001</v>
-      </c>
-      <c r="P49" s="62">
-        <v>2.17540256007367E-2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M49" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="N49" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="O49" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="P49" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
       <c r="L50" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="M50" s="42" t="s">
-        <v>68</v>
-      </c>
-      <c r="N50" s="55">
-        <v>4.9650161007164098</v>
-      </c>
-      <c r="O50" s="1">
-        <f>N50/100</f>
-        <v>4.9650161007164101E-2</v>
-      </c>
-      <c r="P50" s="61">
-        <v>1.15284947015369E-4</v>
+        <v>41</v>
+      </c>
+      <c r="N50" s="50">
+        <v>0</v>
+      </c>
+      <c r="O50" s="54">
+        <f>N50</f>
+        <v>0</v>
+      </c>
+      <c r="P50" s="58">
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
@@ -3891,288 +4127,1059 @@
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
-      <c r="F51" s="1"/>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
-      <c r="L51" s="59" t="s">
-        <v>150</v>
+      <c r="L51" s="55">
+        <v>4.8611111111111112E-2</v>
       </c>
       <c r="M51" s="42" t="s">
-        <v>134</v>
-      </c>
-      <c r="N51" s="55">
-        <v>0.52427629116916796</v>
-      </c>
-      <c r="O51" s="1">
-        <f t="shared" ref="O51:O53" si="4">N51/100</f>
-        <v>5.2427629116916794E-3</v>
-      </c>
-      <c r="P51" s="61">
-        <v>6.2348925580496799E-4</v>
+        <v>23</v>
+      </c>
+      <c r="N51" s="50">
+        <v>1.0599999427795399</v>
+      </c>
+      <c r="O51" s="54">
+        <f>N51</f>
+        <v>1.0599999427795399</v>
+      </c>
+      <c r="P51" s="58">
+        <v>-2.9953879373185301E-2</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
+      <c r="J52" s="1"/>
+      <c r="K52" s="1"/>
       <c r="M52" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="N52" s="55">
-        <v>-13.5</v>
+        <v>46</v>
+      </c>
+      <c r="N52" s="50">
+        <v>156.440731910842</v>
       </c>
       <c r="O52" s="1">
-        <f t="shared" si="4"/>
-        <v>-0.13500000000000001</v>
-      </c>
-      <c r="P52" s="61">
-        <v>-1.30914832287277E-5</v>
+        <f>N52/100</f>
+        <v>1.56440731910842</v>
+      </c>
+      <c r="P52" s="58">
+        <v>-8.6738403137775998E-6</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="M53" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="N53" s="55">
-        <v>-5.8</v>
+        <v>117</v>
+      </c>
+      <c r="N53" s="50">
+        <v>-20.300935880694301</v>
       </c>
       <c r="O53" s="1">
-        <f t="shared" si="4"/>
-        <v>-5.7999999999999996E-2</v>
-      </c>
-      <c r="P53" s="61">
-        <v>1.15841086511394E-4</v>
+        <f t="shared" ref="O53:O59" si="6">N53/100</f>
+        <v>-0.20300935880694301</v>
+      </c>
+      <c r="P53" s="58">
+        <v>2.1648716178694401E-3</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="M54" s="42" t="s">
-        <v>55</v>
-      </c>
-      <c r="N54" s="55">
-        <v>-0.25510563387813501</v>
-      </c>
-      <c r="O54" s="57">
-        <f>N54</f>
-        <v>-0.25510563387813501</v>
-      </c>
-      <c r="P54" s="62">
-        <v>-0.25510563390000002</v>
+        <v>47</v>
+      </c>
+      <c r="N54" s="50">
+        <v>75.916881283268793</v>
+      </c>
+      <c r="O54" s="1">
+        <f t="shared" si="6"/>
+        <v>0.75916881283268789</v>
+      </c>
+      <c r="P54" s="58">
+        <v>6.4758759358596297E-4</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="M55" s="42" t="s">
-        <v>114</v>
-      </c>
-      <c r="N55" s="55">
-        <v>1.0385379019832599</v>
-      </c>
-      <c r="O55" s="57">
-        <f>N55</f>
-        <v>1.0385379019832599</v>
-      </c>
-      <c r="P55" s="62">
-        <v>-5.12238863404413E-3</v>
+        <v>118</v>
+      </c>
+      <c r="N55" s="50">
+        <v>-0.155506560051652</v>
+      </c>
+      <c r="O55" s="1">
+        <f t="shared" si="6"/>
+        <v>-1.55506560051652E-3</v>
+      </c>
+      <c r="P55" s="58">
+        <v>-1.47979634931223E-3</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L56" t="s">
-        <v>146</v>
-      </c>
       <c r="M56" s="42" t="s">
-        <v>69</v>
-      </c>
-      <c r="N56" s="55">
-        <v>-2.8744036925517298</v>
+        <v>48</v>
+      </c>
+      <c r="N56" s="50">
+        <v>41.338725991097199</v>
       </c>
       <c r="O56" s="1">
-        <f>N56/100</f>
-        <v>-2.8744036925517299E-2</v>
-      </c>
-      <c r="P56" s="61">
-        <v>-9.7142222335186394E-5</v>
+        <f t="shared" si="6"/>
+        <v>0.41338725991097197</v>
+      </c>
+      <c r="P56" s="58">
+        <v>6.8870384835700903E-4</v>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L57" s="59" t="s">
-        <v>151</v>
-      </c>
       <c r="M57" s="42" t="s">
-        <v>135</v>
-      </c>
-      <c r="N57" s="55">
-        <v>0.31779049296478201</v>
+        <v>119</v>
+      </c>
+      <c r="N57" s="50">
+        <v>-3.8398609004379098</v>
       </c>
       <c r="O57" s="1">
-        <f t="shared" ref="O57:O59" si="5">N57/100</f>
-        <v>3.1779049296478202E-3</v>
-      </c>
-      <c r="P57" s="61">
-        <v>-1.0332946463634299E-3</v>
+        <f t="shared" si="6"/>
+        <v>-3.8398609004379101E-2</v>
+      </c>
+      <c r="P57" s="58">
+        <v>-1.3891657030102901E-3</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="M58" s="42" t="s">
-        <v>70</v>
-      </c>
-      <c r="N58" s="55">
-        <v>-14.9</v>
+        <v>49</v>
+      </c>
+      <c r="N58" s="50">
+        <v>232.35762119293199</v>
       </c>
       <c r="O58" s="1">
-        <f t="shared" si="5"/>
-        <v>-0.14899999999999999</v>
-      </c>
-      <c r="P58" s="61">
-        <v>-4.6294745534552998E-5</v>
+        <f t="shared" si="6"/>
+        <v>2.32357621192932</v>
+      </c>
+      <c r="P58" s="58">
+        <v>6.3899375327158804E-4</v>
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="M59" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="N59" s="50">
+        <v>-20.456442236900301</v>
+      </c>
+      <c r="O59" s="1">
+        <f t="shared" si="6"/>
+        <v>-0.20456442236900302</v>
+      </c>
+      <c r="P59" s="58">
+        <v>6.8507826856001298E-4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L60" t="s">
+        <v>140</v>
+      </c>
+      <c r="M60" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="N60" s="50">
+        <v>-0.22125272217770001</v>
+      </c>
+      <c r="O60" s="54">
+        <f>N60</f>
+        <v>-0.22125272217770001</v>
+      </c>
+      <c r="P60" s="59">
+        <v>-0.2212527222</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L61" s="55">
+        <v>0.47083333333333338</v>
+      </c>
+      <c r="M61" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="N61" s="50">
+        <v>1.0099999973080001</v>
+      </c>
+      <c r="O61" s="54">
+        <f>N61</f>
+        <v>1.0099999973080001</v>
+      </c>
+      <c r="P61" s="59">
+        <v>2.17540256007367E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M62" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="N62" s="50">
+        <v>-23.569740833506799</v>
+      </c>
+      <c r="O62" s="1">
+        <f>N62/100</f>
+        <v>-0.235697408335068</v>
+      </c>
+      <c r="P62" s="58">
+        <v>-1.05523560178061E-3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M63" s="42" t="s">
+        <v>120</v>
+      </c>
+      <c r="N63" s="50">
+        <v>0.96859150246414105</v>
+      </c>
+      <c r="O63" s="1">
+        <f t="shared" ref="O63:O67" si="7">N63/100</f>
+        <v>9.6859150246414102E-3</v>
+      </c>
+      <c r="P63" s="58">
+        <v>-2.2375145874756201E-3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M64" s="42" t="s">
+        <v>53</v>
+      </c>
+      <c r="N64" s="50">
+        <v>29.247688021076399</v>
+      </c>
+      <c r="O64" s="1">
+        <f t="shared" si="7"/>
+        <v>0.29247688021076401</v>
+      </c>
+      <c r="P64" s="58">
+        <v>5.1585990707936401E-4</v>
+      </c>
+    </row>
+    <row r="65" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M65" s="42" t="s">
+        <v>121</v>
+      </c>
+      <c r="N65" s="50">
+        <v>-10.134384235994199</v>
+      </c>
+      <c r="O65" s="1">
+        <f t="shared" si="7"/>
+        <v>-0.101343842359942</v>
+      </c>
+      <c r="P65" s="58">
+        <v>-2.7105327863768802E-3</v>
+      </c>
+    </row>
+    <row r="66" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M66" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="N66" s="50">
+        <v>4.9388912162000001E-5</v>
+      </c>
+      <c r="O66" s="1">
+        <f t="shared" si="7"/>
+        <v>4.9388912162000003E-7</v>
+      </c>
+      <c r="P66" s="58">
+        <v>6.5059278082477401E-7</v>
+      </c>
+    </row>
+    <row r="67" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M67" s="42" t="s">
+        <v>122</v>
+      </c>
+      <c r="N67" s="50">
+        <v>-23.1382548362844</v>
+      </c>
+      <c r="O67" s="1">
+        <f t="shared" si="7"/>
+        <v>-0.231382548362844</v>
+      </c>
+      <c r="P67" s="58">
+        <v>1.7465773008429299E-7</v>
+      </c>
+    </row>
+    <row r="68" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L68" t="s">
+        <v>141</v>
+      </c>
+      <c r="M68" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="N68" s="50">
+        <v>-0.25510563387813501</v>
+      </c>
+      <c r="O68" s="54">
+        <f>N68</f>
+        <v>-0.25510563387813501</v>
+      </c>
+      <c r="P68" s="59">
+        <v>-0.25510563390000002</v>
+      </c>
+    </row>
+    <row r="69" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L69" s="55">
+        <v>0.8125</v>
+      </c>
+      <c r="M69" s="42" t="s">
+        <v>114</v>
+      </c>
+      <c r="N69" s="50">
+        <v>1.0385379019832599</v>
+      </c>
+      <c r="O69" s="54">
+        <f>N69</f>
+        <v>1.0385379019832599</v>
+      </c>
+      <c r="P69" s="59">
+        <v>-5.12238863404413E-3</v>
+      </c>
+    </row>
+    <row r="70" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M70" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="N70" s="50">
+        <v>6.4193752642371704</v>
+      </c>
+      <c r="O70" s="1">
+        <f>N70/100</f>
+        <v>6.4193752642371704E-2</v>
+      </c>
+      <c r="P70" s="58">
+        <v>1.2851248455257599E-4</v>
+      </c>
+    </row>
+    <row r="71" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M71" s="42" t="s">
+        <v>124</v>
+      </c>
+      <c r="N71" s="50">
+        <v>1.57798981550307</v>
+      </c>
+      <c r="O71" s="1">
+        <f t="shared" ref="O71:O79" si="8">N71/100</f>
+        <v>1.5779898155030701E-2</v>
+      </c>
+      <c r="P71" s="58">
+        <v>1.0767413611616999E-3</v>
+      </c>
+    </row>
+    <row r="72" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M72" s="42" t="s">
+        <v>57</v>
+      </c>
+      <c r="N72" s="50">
+        <v>7.6111237412808599</v>
+      </c>
+      <c r="O72" s="1">
+        <f t="shared" si="8"/>
+        <v>7.6111237412808605E-2</v>
+      </c>
+      <c r="P72" s="58">
+        <v>1.6297137374082799E-5</v>
+      </c>
+    </row>
+    <row r="73" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M73" s="42" t="s">
+        <v>123</v>
+      </c>
+      <c r="N73" s="50">
+        <v>2.2749299623984598</v>
+      </c>
+      <c r="O73" s="1">
+        <f t="shared" si="8"/>
+        <v>2.2749299623984597E-2</v>
+      </c>
+      <c r="P73" s="58">
+        <v>9.80565804585901E-5</v>
+      </c>
+    </row>
+    <row r="74" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M74" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="N74" s="50">
+        <v>17.236621109828601</v>
+      </c>
+      <c r="O74" s="1">
+        <f t="shared" si="8"/>
+        <v>0.17236621109828601</v>
+      </c>
+      <c r="P74" s="58">
+        <v>2.8072391037720099E-5</v>
+      </c>
+    </row>
+    <row r="75" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M75" s="42" t="s">
+        <v>125</v>
+      </c>
+      <c r="N75" s="50">
+        <v>6.2088690408799696</v>
+      </c>
+      <c r="O75" s="1">
+        <f t="shared" si="8"/>
+        <v>6.2088690408799697E-2</v>
+      </c>
+      <c r="P75" s="58">
+        <v>3.8053003130694002E-4</v>
+      </c>
+    </row>
+    <row r="76" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M76" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="N76" s="50">
+        <v>1.4392071686730901</v>
+      </c>
+      <c r="O76" s="1">
+        <f t="shared" si="8"/>
+        <v>1.4392071686730901E-2</v>
+      </c>
+      <c r="P76" s="58">
+        <v>3.3901950999533699E-5</v>
+      </c>
+    </row>
+    <row r="77" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M77" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="N77" s="50">
+        <v>0.52526799870488805</v>
+      </c>
+      <c r="O77" s="1">
+        <f t="shared" si="8"/>
+        <v>5.2526799870488807E-3</v>
+      </c>
+      <c r="P77" s="58">
+        <v>9.7871725652031802E-5</v>
+      </c>
+    </row>
+    <row r="78" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M78" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="N78" s="50">
+        <v>-6.1</v>
+      </c>
+      <c r="O78" s="1">
+        <f t="shared" si="8"/>
+        <v>-6.0999999999999999E-2</v>
+      </c>
+      <c r="P78" s="58">
+        <v>-5.5804864002167998E-6</v>
+      </c>
+    </row>
+    <row r="79" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M79" s="42" t="s">
+        <v>20</v>
+      </c>
+      <c r="N79" s="50">
+        <v>-1.6</v>
+      </c>
+      <c r="O79" s="1">
+        <f t="shared" si="8"/>
+        <v>-1.6E-2</v>
+      </c>
+      <c r="P79" s="58">
+        <v>5.2797756594065403E-5</v>
+      </c>
+    </row>
+    <row r="80" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L80" t="s">
+        <v>142</v>
+      </c>
+      <c r="M80" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="N80" s="50">
+        <v>-0.26806990591321</v>
+      </c>
+      <c r="O80" s="54">
+        <f>N80</f>
+        <v>-0.26806990591321</v>
+      </c>
+      <c r="P80" s="59">
+        <v>-0.26806990590000002</v>
+      </c>
+    </row>
+    <row r="81" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L81" s="56" t="s">
+        <v>147</v>
+      </c>
+      <c r="M81" s="42" t="s">
+        <v>115</v>
+      </c>
+      <c r="N81" s="50">
+        <v>1.0349152577221601</v>
+      </c>
+      <c r="O81" s="54">
+        <f>N81</f>
+        <v>1.0349152577221601</v>
+      </c>
+      <c r="P81" s="59">
+        <v>-2.1765958813597698E-3</v>
+      </c>
+    </row>
+    <row r="82" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L82" s="47"/>
+      <c r="M82" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="N82" s="50">
+        <v>6.1481308294477897</v>
+      </c>
+      <c r="O82" s="1">
+        <f>N82/100</f>
+        <v>6.1481308294477899E-2</v>
+      </c>
+      <c r="P82" s="57">
+        <v>-1.88116567434796E-5</v>
+      </c>
+    </row>
+    <row r="83" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L83" s="47"/>
+      <c r="M83" s="42" t="s">
+        <v>127</v>
+      </c>
+      <c r="N83" s="50">
+        <v>6.1776975079165704</v>
+      </c>
+      <c r="O83" s="1">
+        <f t="shared" ref="O83:O95" si="9">N83/100</f>
+        <v>6.1776975079165707E-2</v>
+      </c>
+      <c r="P83" s="57">
+        <v>-4.4567340559324698E-4</v>
+      </c>
+    </row>
+    <row r="84" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L84" s="47"/>
+      <c r="M84" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="N84" s="50">
+        <v>10.1258308263922</v>
+      </c>
+      <c r="O84" s="1">
+        <f t="shared" si="9"/>
+        <v>0.101258308263922</v>
+      </c>
+      <c r="P84" s="58">
+        <v>-1.40656940313608E-4</v>
+      </c>
+    </row>
+    <row r="85" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L85" s="47"/>
+      <c r="M85" s="42" t="s">
+        <v>128</v>
+      </c>
+      <c r="N85" s="50">
+        <v>4.8779939913553596</v>
+      </c>
+      <c r="O85" s="1">
+        <f t="shared" si="9"/>
+        <v>4.8779939913553595E-2</v>
+      </c>
+      <c r="P85" s="57">
+        <v>-6.3339605935184401E-4</v>
+      </c>
+    </row>
+    <row r="86" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L86" t="s">
+        <v>143</v>
+      </c>
+      <c r="M86" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="N86" s="50">
+        <v>-7.6</v>
+      </c>
+      <c r="O86" s="1">
+        <f t="shared" si="9"/>
+        <v>-7.5999999999999998E-2</v>
+      </c>
+      <c r="P86" s="58">
+        <v>-1.4483820858600399E-4</v>
+      </c>
+    </row>
+    <row r="87" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L87" s="56" t="s">
+        <v>148</v>
+      </c>
+      <c r="M87" s="42" t="s">
+        <v>129</v>
+      </c>
+      <c r="N87" s="50">
+        <v>-1.6</v>
+      </c>
+      <c r="O87" s="1">
+        <f t="shared" si="9"/>
+        <v>-1.6E-2</v>
+      </c>
+      <c r="P87" s="58">
+        <v>-3.5573742834272E-3</v>
+      </c>
+    </row>
+    <row r="88" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L88" t="s">
+        <v>144</v>
+      </c>
+      <c r="M88" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="N88" s="51">
+        <v>-63.001699846354903</v>
+      </c>
+      <c r="O88" s="1">
+        <f t="shared" si="9"/>
+        <v>-0.63001699846354908</v>
+      </c>
+      <c r="P88" s="58">
+        <v>-9.5060452610995505E-4</v>
+      </c>
+    </row>
+    <row r="89" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L89" s="56" t="s">
+        <v>149</v>
+      </c>
+      <c r="M89" s="42" t="s">
+        <v>130</v>
+      </c>
+      <c r="N89" s="50">
+        <v>10.2039485868599</v>
+      </c>
+      <c r="O89" s="1">
+        <f t="shared" si="9"/>
+        <v>0.102039485868599</v>
+      </c>
+      <c r="P89" s="58">
+        <v>-5.1145973996759402E-3</v>
+      </c>
+    </row>
+    <row r="90" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M90" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="N90" s="50">
+        <v>16.526211548050401</v>
+      </c>
+      <c r="O90" s="1">
+        <f t="shared" si="9"/>
+        <v>0.16526211548050401</v>
+      </c>
+      <c r="P90" s="58">
+        <v>3.0418249791705498E-4</v>
+      </c>
+    </row>
+    <row r="91" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M91" s="42" t="s">
+        <v>131</v>
+      </c>
+      <c r="N91" s="52">
+        <v>-1.34369314780613</v>
+      </c>
+      <c r="O91" s="1">
+        <f t="shared" si="9"/>
+        <v>-1.34369314780613E-2</v>
+      </c>
+      <c r="P91" s="58">
+        <v>-1.37670401876801E-3</v>
+      </c>
+    </row>
+    <row r="92" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M92" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="N92" s="52">
+        <v>29.247637436823101</v>
+      </c>
+      <c r="O92" s="1">
+        <f t="shared" si="9"/>
+        <v>0.29247637436823104</v>
+      </c>
+      <c r="P92" s="58">
+        <v>2.2761940039589499E-4</v>
+      </c>
+    </row>
+    <row r="93" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M93" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="N93" s="52">
+        <v>11.0919776937066</v>
+      </c>
+      <c r="O93" s="1">
+        <f t="shared" si="9"/>
+        <v>0.11091977693706599</v>
+      </c>
+      <c r="P93" s="58">
+        <v>-1.3983824680780001E-3</v>
+      </c>
+    </row>
+    <row r="94" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M94" s="42" t="s">
+        <v>67</v>
+      </c>
+      <c r="N94" s="53">
+        <v>-94.199996999999996</v>
+      </c>
+      <c r="O94" s="1">
+        <f t="shared" si="9"/>
+        <v>-0.94199996999999991</v>
+      </c>
+      <c r="P94" s="58">
+        <v>-2.81965662445027E-3</v>
+      </c>
+    </row>
+    <row r="95" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M95" s="42" t="s">
+        <v>133</v>
+      </c>
+      <c r="N95">
+        <f>21.4613437652587-19</f>
+        <v>2.4613437652587002</v>
+      </c>
+      <c r="O95" s="1">
+        <f t="shared" si="9"/>
+        <v>2.4613437652587004E-2</v>
+      </c>
+      <c r="P95" s="58">
+        <v>-6.8701998242329402E-3</v>
+      </c>
+    </row>
+    <row r="96" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M96" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="N96" s="52">
+        <v>-0.22125272217770001</v>
+      </c>
+      <c r="O96" s="54">
+        <f>N96</f>
+        <v>-0.22125272217770001</v>
+      </c>
+      <c r="P96" s="59">
+        <v>-0.2212527222</v>
+      </c>
+    </row>
+    <row r="97" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M97" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="N97" s="52">
+        <v>1.0099999973080001</v>
+      </c>
+      <c r="O97" s="54">
+        <f>N97</f>
+        <v>1.0099999973080001</v>
+      </c>
+      <c r="P97" s="59">
+        <v>2.17540256007367E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L98" t="s">
+        <v>145</v>
+      </c>
+      <c r="M98" s="42" t="s">
+        <v>68</v>
+      </c>
+      <c r="N98" s="52">
+        <v>4.9650161007164098</v>
+      </c>
+      <c r="O98" s="1">
+        <f>N98/100</f>
+        <v>4.9650161007164101E-2</v>
+      </c>
+      <c r="P98" s="58">
+        <v>1.15284947015369E-4</v>
+      </c>
+    </row>
+    <row r="99" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L99" s="56" t="s">
+        <v>150</v>
+      </c>
+      <c r="M99" s="42" t="s">
+        <v>134</v>
+      </c>
+      <c r="N99" s="52">
+        <v>0.52427629116916796</v>
+      </c>
+      <c r="O99" s="1">
+        <f t="shared" ref="O99:O101" si="10">N99/100</f>
+        <v>5.2427629116916794E-3</v>
+      </c>
+      <c r="P99" s="58">
+        <v>6.2348925580496799E-4</v>
+      </c>
+    </row>
+    <row r="100" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M100" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="N100" s="52">
+        <v>-13.5</v>
+      </c>
+      <c r="O100" s="1">
+        <f t="shared" si="10"/>
+        <v>-0.13500000000000001</v>
+      </c>
+      <c r="P100" s="58">
+        <v>-1.30914832287277E-5</v>
+      </c>
+    </row>
+    <row r="101" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M101" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="N101" s="52">
+        <v>-5.8</v>
+      </c>
+      <c r="O101" s="1">
+        <f t="shared" si="10"/>
+        <v>-5.7999999999999996E-2</v>
+      </c>
+      <c r="P101" s="58">
+        <v>1.15841086511394E-4</v>
+      </c>
+    </row>
+    <row r="102" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M102" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="N102" s="52">
+        <v>-0.25510563387813501</v>
+      </c>
+      <c r="O102" s="54">
+        <f>N102</f>
+        <v>-0.25510563387813501</v>
+      </c>
+      <c r="P102" s="59">
+        <v>-0.25510563390000002</v>
+      </c>
+    </row>
+    <row r="103" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M103" s="42" t="s">
+        <v>114</v>
+      </c>
+      <c r="N103" s="52">
+        <v>1.0385379019832599</v>
+      </c>
+      <c r="O103" s="54">
+        <f>N103</f>
+        <v>1.0385379019832599</v>
+      </c>
+      <c r="P103" s="59">
+        <v>-5.12238863404413E-3</v>
+      </c>
+    </row>
+    <row r="104" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L104" t="s">
+        <v>146</v>
+      </c>
+      <c r="M104" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="N104" s="52">
+        <v>-2.8744036925517298</v>
+      </c>
+      <c r="O104" s="1">
+        <f>N104/100</f>
+        <v>-2.8744036925517299E-2</v>
+      </c>
+      <c r="P104" s="58">
+        <v>-9.7142222335186394E-5</v>
+      </c>
+    </row>
+    <row r="105" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L105" s="56" t="s">
+        <v>151</v>
+      </c>
+      <c r="M105" s="42" t="s">
+        <v>135</v>
+      </c>
+      <c r="N105" s="52">
+        <v>0.31779049296478201</v>
+      </c>
+      <c r="O105" s="1">
+        <f t="shared" ref="O105:O107" si="11">N105/100</f>
+        <v>3.1779049296478202E-3</v>
+      </c>
+      <c r="P105" s="58">
+        <v>-1.0332946463634299E-3</v>
+      </c>
+    </row>
+    <row r="106" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M106" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="N106" s="52">
+        <v>-14.9</v>
+      </c>
+      <c r="O106" s="1">
+        <f t="shared" si="11"/>
+        <v>-0.14899999999999999</v>
+      </c>
+      <c r="P106" s="58">
+        <v>-4.6294745534552998E-5</v>
+      </c>
+    </row>
+    <row r="107" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M107" s="42" t="s">
         <v>136</v>
       </c>
-      <c r="N59" s="55">
+      <c r="N107" s="52">
         <v>-5</v>
       </c>
-      <c r="O59" s="1">
-        <f t="shared" si="5"/>
+      <c r="O107" s="1">
+        <f t="shared" si="11"/>
         <v>-0.05</v>
       </c>
-      <c r="P59" s="61">
+      <c r="P107" s="58">
         <v>-4.2582952991622499E-5</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="M60" s="42" t="s">
+    <row r="108" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M108" s="42" t="s">
         <v>60</v>
       </c>
-      <c r="N60" s="55">
+      <c r="N108" s="52">
         <v>-0.26806990591321</v>
       </c>
-      <c r="O60" s="57">
-        <f>N60</f>
+      <c r="O108" s="54">
+        <f>N108</f>
         <v>-0.26806990591321</v>
       </c>
-      <c r="P60" s="62">
+      <c r="P108" s="59">
         <v>-0.26806990590000002</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="M61" s="42" t="s">
+    <row r="109" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M109" s="42" t="s">
         <v>115</v>
       </c>
-      <c r="N61" s="55">
+      <c r="N109" s="52">
         <v>1.0349152577221601</v>
       </c>
-      <c r="O61" s="57">
-        <f>N61</f>
+      <c r="O109" s="54">
+        <f>N109</f>
         <v>1.0349152577221601</v>
       </c>
-      <c r="P61" s="62">
+      <c r="P109" s="59">
         <v>-2.1765958813597698E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="O62" s="1"/>
-      <c r="P62" s="3"/>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="M63" s="51"/>
-      <c r="N63" s="51"/>
-      <c r="O63" s="1"/>
-      <c r="P63" s="3"/>
-    </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="M64" s="51"/>
-      <c r="N64" s="50"/>
-      <c r="P64" s="3"/>
-    </row>
-    <row r="65" spans="13:16" x14ac:dyDescent="0.25">
-      <c r="M65" s="51"/>
-      <c r="N65" s="50"/>
-      <c r="P65" s="3"/>
-    </row>
-    <row r="66" spans="13:16" x14ac:dyDescent="0.25">
-      <c r="M66" s="51"/>
-      <c r="N66" s="50"/>
-    </row>
-    <row r="67" spans="13:16" x14ac:dyDescent="0.25">
-      <c r="M67" s="42"/>
-      <c r="N67" s="1"/>
-    </row>
-    <row r="68" spans="13:16" x14ac:dyDescent="0.25">
-      <c r="M68" s="42"/>
-      <c r="N68" s="1"/>
-    </row>
-    <row r="69" spans="13:16" x14ac:dyDescent="0.25">
-      <c r="M69" s="42"/>
-      <c r="N69" s="1"/>
-    </row>
-    <row r="70" spans="13:16" x14ac:dyDescent="0.25">
-      <c r="M70" s="42"/>
-      <c r="N70" s="1"/>
-    </row>
-    <row r="71" spans="13:16" x14ac:dyDescent="0.25">
-      <c r="M71" s="42"/>
-      <c r="N71" s="1"/>
-    </row>
-    <row r="72" spans="13:16" x14ac:dyDescent="0.25">
-      <c r="M72" s="42"/>
-      <c r="N72" s="1"/>
-    </row>
-    <row r="73" spans="13:16" x14ac:dyDescent="0.25">
-      <c r="M73" s="42"/>
-      <c r="N73" s="1"/>
-    </row>
-    <row r="74" spans="13:16" x14ac:dyDescent="0.25">
-      <c r="M74" s="42"/>
-      <c r="N74" s="1"/>
-    </row>
-    <row r="75" spans="13:16" x14ac:dyDescent="0.25">
-      <c r="M75" s="42"/>
-      <c r="N75" s="1"/>
-    </row>
-    <row r="76" spans="13:16" x14ac:dyDescent="0.25">
-      <c r="M76" s="42"/>
-      <c r="N76" s="1"/>
-    </row>
-    <row r="77" spans="13:16" x14ac:dyDescent="0.25">
-      <c r="M77" s="42"/>
-      <c r="N77" s="1"/>
-    </row>
-    <row r="78" spans="13:16" x14ac:dyDescent="0.25">
-      <c r="M78" s="42"/>
-      <c r="N78" s="1"/>
-    </row>
-    <row r="79" spans="13:16" x14ac:dyDescent="0.25">
-      <c r="M79" s="42"/>
-      <c r="N79" s="1"/>
-    </row>
-    <row r="80" spans="13:16" x14ac:dyDescent="0.25">
-      <c r="M80" s="42"/>
-      <c r="N80" s="1"/>
-    </row>
-    <row r="81" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M81" s="42"/>
-      <c r="N81" s="1"/>
-    </row>
-    <row r="82" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M82" s="42"/>
-      <c r="N82" s="1"/>
-    </row>
-    <row r="83" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M83" s="42"/>
-      <c r="N83" s="1"/>
-    </row>
-    <row r="84" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M84" s="42"/>
-      <c r="N84" s="1"/>
-    </row>
-    <row r="85" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M85" s="42"/>
-      <c r="N85" s="1"/>
-    </row>
-    <row r="86" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M86" s="42"/>
-      <c r="N86" s="1"/>
+    <row r="110" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="O110" s="1"/>
+      <c r="P110" s="3"/>
+    </row>
+    <row r="111" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M111" s="48"/>
+      <c r="N111" s="48"/>
+      <c r="O111" s="1"/>
+      <c r="P111" s="3"/>
+    </row>
+    <row r="112" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M112" s="48"/>
+      <c r="N112" s="47"/>
+      <c r="P112" s="3"/>
+    </row>
+    <row r="113" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M113" s="48"/>
+      <c r="N113" s="47"/>
+      <c r="P113" s="3"/>
+    </row>
+    <row r="114" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M114" s="48"/>
+      <c r="N114" s="47"/>
+    </row>
+    <row r="115" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M115" s="42"/>
+      <c r="N115" s="1"/>
+    </row>
+    <row r="116" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M116" s="42"/>
+      <c r="N116" s="1"/>
+    </row>
+    <row r="117" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M117" s="42"/>
+      <c r="N117" s="1"/>
+    </row>
+    <row r="118" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M118" s="42"/>
+      <c r="N118" s="1"/>
+    </row>
+    <row r="119" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M119" s="42"/>
+      <c r="N119" s="1"/>
+    </row>
+    <row r="120" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M120" s="42"/>
+      <c r="N120" s="1"/>
+    </row>
+    <row r="121" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M121" s="42"/>
+      <c r="N121" s="1"/>
+    </row>
+    <row r="122" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M122" s="42"/>
+      <c r="N122" s="1"/>
+    </row>
+    <row r="123" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M123" s="42"/>
+      <c r="N123" s="1"/>
+    </row>
+    <row r="124" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M124" s="42"/>
+      <c r="N124" s="1"/>
+    </row>
+    <row r="125" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M125" s="42"/>
+      <c r="N125" s="1"/>
+    </row>
+    <row r="126" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M126" s="42"/>
+      <c r="N126" s="1"/>
+    </row>
+    <row r="127" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M127" s="42"/>
+      <c r="N127" s="1"/>
+    </row>
+    <row r="128" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M128" s="42"/>
+      <c r="N128" s="1"/>
+    </row>
+    <row r="129" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M129" s="42"/>
+      <c r="N129" s="1"/>
+    </row>
+    <row r="130" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M130" s="42"/>
+      <c r="N130" s="1"/>
+    </row>
+    <row r="131" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M131" s="42"/>
+      <c r="N131" s="1"/>
+    </row>
+    <row r="132" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M132" s="42"/>
+      <c r="N132" s="1"/>
+    </row>
+    <row r="133" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M133" s="42"/>
+      <c r="N133" s="1"/>
+    </row>
+    <row r="134" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M134" s="42"/>
+      <c r="N134" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4204,18 +5211,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="62" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
       <c r="L1" s="11" t="s">
         <v>1</v>
       </c>
@@ -4239,18 +5246,18 @@
       <c r="B2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49" t="s">
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63" t="s">
         <v>74</v>
       </c>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
       <c r="L2" s="8" t="s">
         <v>41</v>
       </c>
@@ -5043,18 +6050,18 @@
       <c r="O33" s="1"/>
     </row>
     <row r="35" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="48" t="s">
+      <c r="A35" s="62" t="s">
         <v>78</v>
       </c>
-      <c r="B35" s="48"/>
-      <c r="C35" s="48"/>
-      <c r="D35" s="48"/>
-      <c r="E35" s="48"/>
-      <c r="F35" s="48"/>
-      <c r="G35" s="48"/>
-      <c r="H35" s="48"/>
-      <c r="I35" s="48"/>
-      <c r="J35" s="48"/>
+      <c r="B35" s="62"/>
+      <c r="C35" s="62"/>
+      <c r="D35" s="62"/>
+      <c r="E35" s="62"/>
+      <c r="F35" s="62"/>
+      <c r="G35" s="62"/>
+      <c r="H35" s="62"/>
+      <c r="I35" s="62"/>
+      <c r="J35" s="62"/>
       <c r="L35" s="11" t="s">
         <v>1</v>
       </c>
@@ -5799,13 +6806,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="60" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
       <c r="G1" s="30" t="s">
         <v>100</v>
       </c>
@@ -5824,13 +6831,13 @@
       <c r="L1" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="P1" s="46" t="s">
+      <c r="P1" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="Q1" s="46"/>
-      <c r="R1" s="46"/>
-      <c r="S1" s="46"/>
-      <c r="T1" s="46"/>
+      <c r="Q1" s="60"/>
+      <c r="R1" s="60"/>
+      <c r="S1" s="60"/>
+      <c r="T1" s="60"/>
       <c r="V1" s="30" t="s">
         <v>100</v>
       </c>
@@ -6365,12 +7372,12 @@
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="P10" s="46" t="s">
+      <c r="P10" s="60" t="s">
         <v>108</v>
       </c>
-      <c r="Q10" s="46"/>
-      <c r="R10" s="46"/>
-      <c r="S10" s="46"/>
+      <c r="Q10" s="60"/>
+      <c r="R10" s="60"/>
+      <c r="S10" s="60"/>
       <c r="T10" s="25"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
@@ -7386,12 +8393,12 @@
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A33" s="46" t="s">
+      <c r="A33" s="60" t="s">
         <v>102</v>
       </c>
-      <c r="B33" s="46"/>
-      <c r="C33" s="46"/>
-      <c r="D33" s="46"/>
+      <c r="B33" s="60"/>
+      <c r="C33" s="60"/>
+      <c r="D33" s="60"/>
       <c r="F33" s="30" t="s">
         <v>100</v>
       </c>
@@ -7769,12 +8776,12 @@
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A42" s="46" t="s">
+      <c r="A42" s="60" t="s">
         <v>104</v>
       </c>
-      <c r="B42" s="46"/>
-      <c r="C42" s="46"/>
-      <c r="D42" s="46"/>
+      <c r="B42" s="60"/>
+      <c r="C42" s="60"/>
+      <c r="D42" s="60"/>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">

</xml_diff>

<commit_message>
myfun_Part1 works, but not myfun_Part2
myfun_Part1_overlap now works. Still need to finish debugging
myfun_Part2_overlap.m.
</commit_message>
<xml_diff>
--- a/DMASE - Test Results.xlsx
+++ b/DMASE - Test Results.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leilei\Documents\GitHub\D-MASE\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="360" yWindow="105" windowWidth="18195" windowHeight="7740" activeTab="2"/>
   </bookViews>
@@ -854,6 +849,10 @@
     <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -865,10 +864,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -930,7 +925,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -965,7 +960,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1190,15 +1185,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="62" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
       <c r="I1" s="6" t="s">
         <v>1</v>
       </c>
@@ -1427,10 +1422,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:N55"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="K40" sqref="K40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1446,15 +1444,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="60" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
+      <c r="A1" s="62" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
       <c r="I1" s="6" t="s">
         <v>1</v>
       </c>
@@ -1807,15 +1805,15 @@
       <c r="N11" s="1"/>
     </row>
     <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="61" t="s">
+      <c r="A12" s="63" t="s">
         <v>80</v>
       </c>
-      <c r="B12" s="61"/>
-      <c r="C12" s="61"/>
-      <c r="D12" s="61"/>
-      <c r="E12" s="61"/>
-      <c r="F12" s="61"/>
-      <c r="G12" s="61"/>
+      <c r="B12" s="63"/>
+      <c r="C12" s="63"/>
+      <c r="D12" s="63"/>
+      <c r="E12" s="63"/>
+      <c r="F12" s="63"/>
+      <c r="G12" s="63"/>
       <c r="I12" s="1"/>
       <c r="J12" s="6" t="s">
         <v>1</v>
@@ -2305,15 +2303,15 @@
       <c r="G31" s="1"/>
     </row>
     <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="61" t="s">
+      <c r="A32" s="63" t="s">
         <v>81</v>
       </c>
-      <c r="B32" s="61"/>
-      <c r="C32" s="61"/>
-      <c r="D32" s="61"/>
-      <c r="E32" s="61"/>
-      <c r="F32" s="61"/>
-      <c r="G32" s="61"/>
+      <c r="B32" s="63"/>
+      <c r="C32" s="63"/>
+      <c r="D32" s="63"/>
+      <c r="E32" s="63"/>
+      <c r="F32" s="63"/>
+      <c r="G32" s="63"/>
       <c r="I32" s="1"/>
       <c r="J32" s="6" t="s">
         <v>1</v>
@@ -2661,7 +2659,7 @@
     </row>
     <row r="44" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>17</v>
+        <v>84</v>
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -2672,7 +2670,7 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>19</v>
+        <v>85</v>
       </c>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -2683,7 +2681,7 @@
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>21</v>
+        <v>86</v>
       </c>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -2694,7 +2692,7 @@
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>23</v>
+        <v>87</v>
       </c>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -2705,7 +2703,7 @@
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>25</v>
+        <v>88</v>
       </c>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -2716,7 +2714,7 @@
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>27</v>
+        <v>89</v>
       </c>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -2772,16 +2770,19 @@
     <mergeCell ref="A32:G32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup scale="62" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:R134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F34" workbookViewId="0">
-      <selection activeCell="L46" sqref="L46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2797,20 +2798,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="64" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+      <c r="J1" s="64"/>
       <c r="K1" s="43"/>
-      <c r="L1" s="64"/>
+      <c r="L1" s="60"/>
       <c r="M1" s="11" t="s">
         <v>1</v>
       </c>
@@ -2832,20 +2833,20 @@
       <c r="B2" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="63" t="s">
+      <c r="C2" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63" t="s">
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65" t="s">
         <v>74</v>
       </c>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="63"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="65"/>
       <c r="K2" s="4"/>
-      <c r="L2" s="64" t="s">
+      <c r="L2" s="60" t="s">
         <v>139</v>
       </c>
       <c r="M2" s="46" t="s">
@@ -2893,7 +2894,7 @@
         <v>45</v>
       </c>
       <c r="K3" s="4"/>
-      <c r="L3" s="64" t="s">
+      <c r="L3" s="60" t="s">
         <v>174</v>
       </c>
       <c r="M3" s="46" t="s">
@@ -2928,7 +2929,7 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
-      <c r="L4" s="64"/>
+      <c r="L4" s="60"/>
       <c r="M4" s="46" t="s">
         <v>47</v>
       </c>
@@ -2958,7 +2959,7 @@
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
-      <c r="L5" s="64"/>
+      <c r="L5" s="60"/>
       <c r="M5" s="46" t="s">
         <v>118</v>
       </c>
@@ -2988,7 +2989,7 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
-      <c r="L6" s="64"/>
+      <c r="L6" s="60"/>
       <c r="M6" s="46" t="s">
         <v>48</v>
       </c>
@@ -3018,7 +3019,7 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
-      <c r="L7" s="64"/>
+      <c r="L7" s="60"/>
       <c r="M7" s="46" t="s">
         <v>119</v>
       </c>
@@ -3048,7 +3049,7 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
-      <c r="L8" s="64"/>
+      <c r="L8" s="60"/>
       <c r="M8" s="46" t="s">
         <v>49</v>
       </c>
@@ -3077,7 +3078,7 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
-      <c r="L9" s="64"/>
+      <c r="L9" s="60"/>
       <c r="M9" s="46" t="s">
         <v>83</v>
       </c>
@@ -3107,7 +3108,7 @@
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
-      <c r="L10" s="64" t="s">
+      <c r="L10" s="60" t="s">
         <v>140</v>
       </c>
       <c r="M10" s="46" t="s">
@@ -3139,7 +3140,7 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
-      <c r="L11" s="64" t="s">
+      <c r="L11" s="60" t="s">
         <v>175</v>
       </c>
       <c r="M11" s="46" t="s">
@@ -3171,7 +3172,7 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
-      <c r="L12" s="64"/>
+      <c r="L12" s="60"/>
       <c r="M12" s="46" t="s">
         <v>53</v>
       </c>
@@ -3201,7 +3202,7 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
-      <c r="L13" s="64"/>
+      <c r="L13" s="60"/>
       <c r="M13" s="46" t="s">
         <v>121</v>
       </c>
@@ -3232,7 +3233,7 @@
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
-      <c r="L14" s="64"/>
+      <c r="L14" s="60"/>
       <c r="M14" s="46" t="s">
         <v>54</v>
       </c>
@@ -3262,7 +3263,7 @@
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
-      <c r="L15" s="64"/>
+      <c r="L15" s="60"/>
       <c r="M15" s="46" t="s">
         <v>122</v>
       </c>
@@ -3293,7 +3294,7 @@
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
-      <c r="L16" s="64" t="s">
+      <c r="L16" s="60" t="s">
         <v>141</v>
       </c>
       <c r="M16" s="46" t="s">
@@ -3326,7 +3327,7 @@
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
-      <c r="L17" s="64" t="s">
+      <c r="L17" s="60" t="s">
         <v>176</v>
       </c>
       <c r="M17" s="46" t="s">
@@ -3350,7 +3351,7 @@
       <c r="B18">
         <v>-9.0498906725745204E-2</v>
       </c>
-      <c r="L18" s="64"/>
+      <c r="L18" s="60"/>
       <c r="M18" s="46" t="s">
         <v>57</v>
       </c>
@@ -3372,7 +3373,7 @@
       <c r="B19">
         <v>-0.22165365184591099</v>
       </c>
-      <c r="L19" s="64"/>
+      <c r="L19" s="60"/>
       <c r="M19" s="46" t="s">
         <v>123</v>
       </c>
@@ -3394,7 +3395,7 @@
       <c r="B20">
         <v>-0.184493248459114</v>
       </c>
-      <c r="L20" s="64"/>
+      <c r="L20" s="60"/>
       <c r="M20" s="46" t="s">
         <v>58</v>
       </c>
@@ -3416,7 +3417,7 @@
       <c r="B21">
         <v>-0.15841659033345201</v>
       </c>
-      <c r="L21" s="64"/>
+      <c r="L21" s="60"/>
       <c r="M21" s="46" t="s">
         <v>125</v>
       </c>
@@ -3438,7 +3439,7 @@
       <c r="B22">
         <v>-0.262083078069408</v>
       </c>
-      <c r="L22" s="64"/>
+      <c r="L22" s="60"/>
       <c r="M22" s="46" t="s">
         <v>59</v>
       </c>
@@ -3460,7 +3461,7 @@
       <c r="B23">
         <v>-0.24699463946439601</v>
       </c>
-      <c r="L23" s="64"/>
+      <c r="L23" s="60"/>
       <c r="M23" s="46" t="s">
         <v>126</v>
       </c>
@@ -3482,7 +3483,7 @@
       <c r="B24">
         <v>-0.25619422730604202</v>
       </c>
-      <c r="L24" s="64"/>
+      <c r="L24" s="60"/>
       <c r="M24" s="46" t="s">
         <v>12</v>
       </c>
@@ -3504,7 +3505,7 @@
       <c r="B25">
         <v>-0.274128496301564</v>
       </c>
-      <c r="L25" s="64"/>
+      <c r="L25" s="60"/>
       <c r="M25" s="46" t="s">
         <v>20</v>
       </c>
@@ -3526,7 +3527,7 @@
       <c r="B26">
         <v>-0.27530156310841902</v>
       </c>
-      <c r="L26" s="64" t="s">
+      <c r="L26" s="60" t="s">
         <v>142</v>
       </c>
       <c r="M26" s="46" t="s">
@@ -3574,7 +3575,7 @@
       <c r="B28">
         <v>-0.27393942115060799</v>
       </c>
-      <c r="L28" s="65"/>
+      <c r="L28" s="61"/>
       <c r="M28" s="46" t="s">
         <v>62</v>
       </c>
@@ -3596,7 +3597,7 @@
       <c r="B29">
         <v>-0.274447646882094</v>
       </c>
-      <c r="L29" s="65"/>
+      <c r="L29" s="61"/>
       <c r="M29" s="46" t="s">
         <v>128</v>
       </c>
@@ -3618,7 +3619,7 @@
       <c r="B30">
         <v>-0.28719972332980598</v>
       </c>
-      <c r="L30" s="64" t="s">
+      <c r="L30" s="60" t="s">
         <v>143</v>
       </c>
       <c r="M30" s="46" t="s">
@@ -3654,7 +3655,7 @@
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L32" s="64" t="s">
+      <c r="L32" s="60" t="s">
         <v>144</v>
       </c>
       <c r="M32" s="46" t="s">
@@ -3690,7 +3691,7 @@
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L34" s="64"/>
+      <c r="L34" s="60"/>
       <c r="M34" s="46" t="s">
         <v>65</v>
       </c>
@@ -3717,7 +3718,7 @@
       <c r="I35" s="49"/>
       <c r="J35" s="49"/>
       <c r="K35" s="49"/>
-      <c r="L35" s="64"/>
+      <c r="L35" s="60"/>
       <c r="M35" s="46" t="s">
         <v>131</v>
       </c>
@@ -3744,7 +3745,7 @@
       <c r="I36" s="47"/>
       <c r="J36" s="47"/>
       <c r="K36" s="47"/>
-      <c r="L36" s="64"/>
+      <c r="L36" s="60"/>
       <c r="M36" s="46" t="s">
         <v>66</v>
       </c>
@@ -3771,7 +3772,7 @@
       <c r="I37" s="47"/>
       <c r="J37" s="47"/>
       <c r="K37" s="47"/>
-      <c r="L37" s="64"/>
+      <c r="L37" s="60"/>
       <c r="M37" s="46" t="s">
         <v>132</v>
       </c>
@@ -3798,7 +3799,7 @@
       <c r="I38" s="47"/>
       <c r="J38" s="47"/>
       <c r="K38" s="47"/>
-      <c r="L38" s="64"/>
+      <c r="L38" s="60"/>
       <c r="M38" s="46" t="s">
         <v>67</v>
       </c>
@@ -3823,7 +3824,7 @@
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
-      <c r="L39" s="64"/>
+      <c r="L39" s="60"/>
       <c r="M39" s="46" t="s">
         <v>133</v>
       </c>
@@ -3848,7 +3849,7 @@
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
-      <c r="L40" s="64" t="s">
+      <c r="L40" s="60" t="s">
         <v>145</v>
       </c>
       <c r="M40" s="46" t="s">
@@ -3902,7 +3903,7 @@
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
-      <c r="L42" s="64"/>
+      <c r="L42" s="60"/>
       <c r="M42" s="46" t="s">
         <v>16</v>
       </c>
@@ -3928,7 +3929,7 @@
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
-      <c r="L43" s="64"/>
+      <c r="L43" s="60"/>
       <c r="M43" s="46" t="s">
         <v>22</v>
       </c>
@@ -3954,7 +3955,7 @@
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
-      <c r="L44" s="64" t="s">
+      <c r="L44" s="60" t="s">
         <v>146</v>
       </c>
       <c r="M44" s="46" t="s">
@@ -4010,7 +4011,7 @@
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
-      <c r="L46" s="64"/>
+      <c r="L46" s="60"/>
       <c r="M46" s="46" t="s">
         <v>70</v>
       </c>
@@ -4036,7 +4037,7 @@
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
-      <c r="L47" s="64"/>
+      <c r="L47" s="60"/>
       <c r="M47" s="46" t="s">
         <v>136</v>
       </c>
@@ -5188,7 +5189,7 @@
     <mergeCell ref="G2:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup scale="32" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5211,18 +5212,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="64" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+      <c r="J1" s="64"/>
       <c r="L1" s="11" t="s">
         <v>1</v>
       </c>
@@ -5246,18 +5247,18 @@
       <c r="B2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="63" t="s">
+      <c r="C2" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63" t="s">
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65" t="s">
         <v>74</v>
       </c>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="63"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="65"/>
       <c r="L2" s="8" t="s">
         <v>41</v>
       </c>
@@ -6050,18 +6051,18 @@
       <c r="O33" s="1"/>
     </row>
     <row r="35" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="62" t="s">
+      <c r="A35" s="64" t="s">
         <v>78</v>
       </c>
-      <c r="B35" s="62"/>
-      <c r="C35" s="62"/>
-      <c r="D35" s="62"/>
-      <c r="E35" s="62"/>
-      <c r="F35" s="62"/>
-      <c r="G35" s="62"/>
-      <c r="H35" s="62"/>
-      <c r="I35" s="62"/>
-      <c r="J35" s="62"/>
+      <c r="B35" s="64"/>
+      <c r="C35" s="64"/>
+      <c r="D35" s="64"/>
+      <c r="E35" s="64"/>
+      <c r="F35" s="64"/>
+      <c r="G35" s="64"/>
+      <c r="H35" s="64"/>
+      <c r="I35" s="64"/>
+      <c r="J35" s="64"/>
       <c r="L35" s="11" t="s">
         <v>1</v>
       </c>
@@ -6806,13 +6807,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="62" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
       <c r="G1" s="30" t="s">
         <v>100</v>
       </c>
@@ -6831,13 +6832,13 @@
       <c r="L1" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="P1" s="60" t="s">
+      <c r="P1" s="62" t="s">
         <v>106</v>
       </c>
-      <c r="Q1" s="60"/>
-      <c r="R1" s="60"/>
-      <c r="S1" s="60"/>
-      <c r="T1" s="60"/>
+      <c r="Q1" s="62"/>
+      <c r="R1" s="62"/>
+      <c r="S1" s="62"/>
+      <c r="T1" s="62"/>
       <c r="V1" s="30" t="s">
         <v>100</v>
       </c>
@@ -7372,12 +7373,12 @@
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="P10" s="60" t="s">
+      <c r="P10" s="62" t="s">
         <v>108</v>
       </c>
-      <c r="Q10" s="60"/>
-      <c r="R10" s="60"/>
-      <c r="S10" s="60"/>
+      <c r="Q10" s="62"/>
+      <c r="R10" s="62"/>
+      <c r="S10" s="62"/>
       <c r="T10" s="25"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
@@ -8393,12 +8394,12 @@
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A33" s="60" t="s">
+      <c r="A33" s="62" t="s">
         <v>102</v>
       </c>
-      <c r="B33" s="60"/>
-      <c r="C33" s="60"/>
-      <c r="D33" s="60"/>
+      <c r="B33" s="62"/>
+      <c r="C33" s="62"/>
+      <c r="D33" s="62"/>
       <c r="F33" s="30" t="s">
         <v>100</v>
       </c>
@@ -8776,12 +8777,12 @@
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A42" s="60" t="s">
+      <c r="A42" s="62" t="s">
         <v>104</v>
       </c>
-      <c r="B42" s="60"/>
-      <c r="C42" s="60"/>
-      <c r="D42" s="60"/>
+      <c r="B42" s="62"/>
+      <c r="C42" s="62"/>
+      <c r="D42" s="62"/>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">

</xml_diff>

<commit_message>
Verified createhvector and createHmatrix for 3 bus system
Verified new createhvector and createHmatrix functions by comparing the
results between the correct old test_3busADMM_overlap script and the new
results. Found that in summing up all buses' contributions for the bus
injection calculations, I forgot to account for the bus itself. Even
though the 3-bus system works, there are still issues with the 14 bus
system. For example, x2_k through x4_k are for some reason almost the
same? Also the way c_k is collected is wrong (needs to take into account
the f components).
</commit_message>
<xml_diff>
--- a/DMASE - Test Results.xlsx
+++ b/DMASE - Test Results.xlsx
@@ -9,16 +9,17 @@
   <sheets>
     <sheet name="2 Bus" sheetId="4" r:id="rId1"/>
     <sheet name="3 Bus" sheetId="1" r:id="rId2"/>
-    <sheet name="14 Bus AC" sheetId="6" r:id="rId3"/>
-    <sheet name="14 Bus DC" sheetId="2" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
+    <sheet name="3 Bus ADMM vs New Fcns" sheetId="7" r:id="rId3"/>
+    <sheet name="14 Bus AC" sheetId="6" r:id="rId4"/>
+    <sheet name="14 Bus DC" sheetId="2" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="184">
   <si>
     <t>Abur 3-Bus Case Measurements (run through SE, rerun new estimate again)</t>
   </si>
@@ -564,16 +565,24 @@
   </si>
   <si>
     <t>43:46</t>
+  </si>
+  <si>
+    <t>WRONG</t>
+  </si>
+  <si>
+    <t>CORRECT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.0000000000000000"/>
     <numFmt numFmtId="165" formatCode="0.0000000000"/>
     <numFmt numFmtId="166" formatCode="0.000E+00"/>
+    <numFmt numFmtId="167" formatCode="0.000000"/>
+    <numFmt numFmtId="168" formatCode="0.00000"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -710,7 +719,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -853,6 +862,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -865,6 +877,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1185,15 +1212,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="63" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
       <c r="I1" s="6" t="s">
         <v>1</v>
       </c>
@@ -1427,8 +1454,8 @@
   </sheetPr>
   <dimension ref="A1:N55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:N49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1444,15 +1471,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="62" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
+      <c r="A1" s="63" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
       <c r="I1" s="6" t="s">
         <v>1</v>
       </c>
@@ -1805,15 +1832,15 @@
       <c r="N11" s="1"/>
     </row>
     <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="63" t="s">
+      <c r="A12" s="64" t="s">
         <v>80</v>
       </c>
-      <c r="B12" s="63"/>
-      <c r="C12" s="63"/>
-      <c r="D12" s="63"/>
-      <c r="E12" s="63"/>
-      <c r="F12" s="63"/>
-      <c r="G12" s="63"/>
+      <c r="B12" s="64"/>
+      <c r="C12" s="64"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="64"/>
+      <c r="F12" s="64"/>
+      <c r="G12" s="64"/>
       <c r="I12" s="1"/>
       <c r="J12" s="6" t="s">
         <v>1</v>
@@ -2303,15 +2330,15 @@
       <c r="G31" s="1"/>
     </row>
     <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="63" t="s">
+      <c r="A32" s="64" t="s">
         <v>81</v>
       </c>
-      <c r="B32" s="63"/>
-      <c r="C32" s="63"/>
-      <c r="D32" s="63"/>
-      <c r="E32" s="63"/>
-      <c r="F32" s="63"/>
-      <c r="G32" s="63"/>
+      <c r="B32" s="64"/>
+      <c r="C32" s="64"/>
+      <c r="D32" s="64"/>
+      <c r="E32" s="64"/>
+      <c r="F32" s="64"/>
+      <c r="G32" s="64"/>
       <c r="I32" s="1"/>
       <c r="J32" s="6" t="s">
         <v>1</v>
@@ -2776,13 +2803,1084 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:W32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="W26" sqref="W26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="5"/>
+    <col min="11" max="11" width="9.85546875" style="5" customWidth="1"/>
+    <col min="12" max="14" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A1" s="64" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="4"/>
+      <c r="L1" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="O1" t="s">
+        <v>182</v>
+      </c>
+      <c r="S1" t="s">
+        <v>183</v>
+      </c>
+      <c r="V1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="45" t="s">
+        <v>113</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="67"/>
+      <c r="L2" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="S2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="62"/>
+      <c r="K3" s="69"/>
+      <c r="L3" s="4">
+        <v>0</v>
+      </c>
+      <c r="M3" s="70">
+        <v>0.486438997946261</v>
+      </c>
+      <c r="N3" s="68"/>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0.486438997946261</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0.48649675710267498</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0.48649675710267498</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.99999845426357303</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.99999999951187202</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1.0000000057454399</v>
+      </c>
+      <c r="E4" s="1">
+        <f>C4-D4</f>
+        <v>-6.2335678840952369E-9</v>
+      </c>
+      <c r="F4" s="1">
+        <f>B4-C4</f>
+        <v>-1.5452482989841698E-6</v>
+      </c>
+      <c r="G4" s="1">
+        <f>B4-D4</f>
+        <v>-1.5514818668682651E-6</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="J4" s="62"/>
+      <c r="K4" s="67"/>
+      <c r="L4" s="4">
+        <v>0</v>
+      </c>
+      <c r="M4" s="70">
+        <v>0.41968174773920602</v>
+      </c>
+      <c r="N4" s="68"/>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0.41968174773920602</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>-0.39792430931689898</v>
+      </c>
+      <c r="V4" s="2">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>-0.39792430931689898</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.99470275148962295</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.99470125387918296</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.99470126016887706</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" ref="E5:E6" si="0">C5-D5</f>
+        <v>-6.289694098882137E-9</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" ref="F5:F9" si="1">B5-C5</f>
+        <v>1.4976104399933021E-6</v>
+      </c>
+      <c r="G5" s="1">
+        <f t="shared" ref="G5:G9" si="2">B5-D5</f>
+        <v>1.49132074589442E-6</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="62"/>
+      <c r="K5" s="69"/>
+      <c r="L5" s="4">
+        <v>0</v>
+      </c>
+      <c r="M5" s="70">
+        <v>1.4478528373142899E-2</v>
+      </c>
+      <c r="N5" s="68"/>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>1.4478528373142899E-2</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>1.44809152293512E-2</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>1.44809152293512E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.99149764559215503</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.99150161828779304</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.99147831063616998</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="0"/>
+        <v>2.3307651623061254E-5</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" si="1"/>
+        <v>-3.9726956380103928E-6</v>
+      </c>
+      <c r="G6" s="1">
+        <f t="shared" si="2"/>
+        <v>1.9334955985050861E-5</v>
+      </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="62"/>
+      <c r="K6" s="69"/>
+      <c r="L6" s="4">
+        <v>0</v>
+      </c>
+      <c r="M6" s="70">
+        <v>2.0957195150350699E-3</v>
+      </c>
+      <c r="N6" s="4"/>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>2.0957195150350699E-3</v>
+      </c>
+      <c r="S6" s="28">
+        <v>1.7763568394002501E-15</v>
+      </c>
+      <c r="T6">
+        <v>5.7832243827587899E-3</v>
+      </c>
+      <c r="V6" s="72">
+        <v>1.7763568394002501E-15</v>
+      </c>
+      <c r="W6">
+        <v>5.7832243827587899E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I7" s="1"/>
+      <c r="J7" s="62"/>
+      <c r="K7" s="67"/>
+      <c r="L7" s="4">
+        <v>1</v>
+      </c>
+      <c r="M7" s="70">
+        <v>0.99998859049397604</v>
+      </c>
+      <c r="N7" s="4"/>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <v>0.99998859049397604</v>
+      </c>
+      <c r="S7">
+        <v>1</v>
+      </c>
+      <c r="T7">
+        <v>0.989863589625809</v>
+      </c>
+      <c r="V7">
+        <v>1</v>
+      </c>
+      <c r="W7">
+        <v>0.989863589625809</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" s="1">
+        <v>-1.44485822804116E-2</v>
+      </c>
+      <c r="C8" s="1">
+        <v>-1.44484686620042E-2</v>
+      </c>
+      <c r="D8" s="1">
+        <v>-1.4448468599055299E-2</v>
+      </c>
+      <c r="E8" s="1">
+        <f>C8-D8</f>
+        <v>-6.2948901299875182E-11</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="1"/>
+        <v>-1.136184073994434E-7</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="2"/>
+        <v>-1.1368135630074327E-7</v>
+      </c>
+      <c r="I8" s="1"/>
+      <c r="J8" s="62"/>
+      <c r="K8" s="67"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9" s="1">
+        <v>-2.0942213598037301E-2</v>
+      </c>
+      <c r="C9" s="1">
+        <v>-2.0942297044494101E-2</v>
+      </c>
+      <c r="D9" s="1">
+        <v>-2.0940977170181601E-2</v>
+      </c>
+      <c r="E9" s="1">
+        <f>C9-D9</f>
+        <v>-1.3198743125004964E-6</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" si="1"/>
+        <v>8.3446456800029267E-8</v>
+      </c>
+      <c r="G9" s="1">
+        <f t="shared" si="2"/>
+        <v>-1.2364278557004671E-6</v>
+      </c>
+      <c r="I9" s="1"/>
+      <c r="J9" s="62"/>
+      <c r="K9" s="69" t="s">
+        <v>183</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="M9" s="68"/>
+      <c r="N9" s="4"/>
+      <c r="S9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="J10" s="62"/>
+      <c r="L10" s="4">
+        <v>10</v>
+      </c>
+      <c r="M10" s="71">
+        <v>-10</v>
+      </c>
+      <c r="N10" s="4">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>-30</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>10</v>
+      </c>
+      <c r="T10">
+        <v>-10</v>
+      </c>
+      <c r="U10">
+        <v>0</v>
+      </c>
+      <c r="V10">
+        <v>-30</v>
+      </c>
+      <c r="W10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="J11" s="62"/>
+      <c r="L11" s="5">
+        <v>6.8965517241379297</v>
+      </c>
+      <c r="M11" s="5">
+        <v>0</v>
+      </c>
+      <c r="N11" s="5">
+        <v>-6.8965517241379297</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>-17.241379310344801</v>
+      </c>
+      <c r="S11">
+        <v>-10</v>
+      </c>
+      <c r="T11">
+        <v>14.1095890410959</v>
+      </c>
+      <c r="U11">
+        <v>-4.10958904109589</v>
+      </c>
+      <c r="V11">
+        <v>40.958904109589</v>
+      </c>
+      <c r="W11">
+        <v>-10.958904109589</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="L12" s="5">
+        <v>30</v>
+      </c>
+      <c r="M12" s="5">
+        <v>-30</v>
+      </c>
+      <c r="N12" s="5">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>10</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>30</v>
+      </c>
+      <c r="T12">
+        <v>-30</v>
+      </c>
+      <c r="U12">
+        <v>0</v>
+      </c>
+      <c r="V12">
+        <v>10</v>
+      </c>
+      <c r="W12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="L13" s="5">
+        <v>17.241379310344801</v>
+      </c>
+      <c r="M13" s="5">
+        <v>0</v>
+      </c>
+      <c r="N13" s="5">
+        <v>-17.241379310344801</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>6.8965517241379297</v>
+      </c>
+      <c r="S13">
+        <v>-30</v>
+      </c>
+      <c r="T13">
+        <v>40.958904109589</v>
+      </c>
+      <c r="U13">
+        <v>-10.958904109589</v>
+      </c>
+      <c r="V13">
+        <v>-14.1095890410959</v>
+      </c>
+      <c r="W13">
+        <v>4.10958904109589</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="L14" s="5">
+        <v>2</v>
+      </c>
+      <c r="M14" s="5">
+        <v>0</v>
+      </c>
+      <c r="N14" s="5">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <v>2</v>
+      </c>
+      <c r="U14">
+        <v>0</v>
+      </c>
+      <c r="V14">
+        <v>0</v>
+      </c>
+      <c r="W14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="L16" s="5">
+        <v>10.486384725291501</v>
+      </c>
+      <c r="M16" s="5">
+        <v>-9.9999429523071601</v>
+      </c>
+      <c r="N16" s="5">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>-29.9998288569215</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <v>10.487569561048501</v>
+      </c>
+      <c r="T16">
+        <v>-10.001127657953999</v>
+      </c>
+      <c r="U16">
+        <v>0</v>
+      </c>
+      <c r="V16">
+        <v>-30.0033829738619</v>
+      </c>
+      <c r="W16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="L17" s="5">
+        <v>7.3161965228419001</v>
+      </c>
+      <c r="M17" s="5">
+        <v>0</v>
+      </c>
+      <c r="N17" s="5">
+        <v>-6.8965123809014903</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>-17.2412809522537</v>
+      </c>
+      <c r="S17">
+        <v>-10.381593610952701</v>
+      </c>
+      <c r="T17">
+        <v>14.228210755774899</v>
+      </c>
+      <c r="U17">
+        <v>-4.2466159164624404</v>
+      </c>
+      <c r="V17">
+        <v>40.542624164467902</v>
+      </c>
+      <c r="W17">
+        <v>-10.842693634959099</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="L18" s="5">
+        <v>30.0143074678918</v>
+      </c>
+      <c r="M18" s="5">
+        <v>-29.9998288569215</v>
+      </c>
+      <c r="N18" s="5">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>9.9999429523071601</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <v>30.017862256323401</v>
+      </c>
+      <c r="T18">
+        <v>-30.0033829738619</v>
+      </c>
+      <c r="U18">
+        <v>0</v>
+      </c>
+      <c r="V18">
+        <v>10.001127657953999</v>
+      </c>
+      <c r="W18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="L19" s="5">
+        <v>17.243376683724399</v>
+      </c>
+      <c r="M19" s="5">
+        <v>0</v>
+      </c>
+      <c r="N19" s="5">
+        <v>-17.2412809522537</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>6.8965123809014903</v>
+      </c>
+      <c r="S19">
+        <v>-29.699934406035901</v>
+      </c>
+      <c r="T19">
+        <v>40.542631917522201</v>
+      </c>
+      <c r="U19">
+        <v>-10.842693634959099</v>
+      </c>
+      <c r="V19">
+        <v>-15.028208299055301</v>
+      </c>
+      <c r="W19">
+        <v>4.2466159164624404</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="L20" s="5">
+        <v>1.9999885904614301</v>
+      </c>
+      <c r="M20" s="5">
+        <v>0</v>
+      </c>
+      <c r="N20" s="5">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="S20">
+        <v>0</v>
+      </c>
+      <c r="T20">
+        <v>1.98962793658121</v>
+      </c>
+      <c r="U20">
+        <v>0</v>
+      </c>
+      <c r="V20">
+        <v>-2.88969285364425E-2</v>
+      </c>
+      <c r="W20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="K22" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="L22" s="5">
+        <v>10</v>
+      </c>
+      <c r="M22" s="5">
+        <v>-10</v>
+      </c>
+      <c r="N22" s="5">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>-30</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="R22" t="s">
+        <v>182</v>
+      </c>
+      <c r="S22">
+        <v>10.487569561048501</v>
+      </c>
+      <c r="T22">
+        <v>-10.001127657953999</v>
+      </c>
+      <c r="U22">
+        <v>0</v>
+      </c>
+      <c r="V22">
+        <v>-30.0033829738619</v>
+      </c>
+      <c r="W22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="L23" s="5">
+        <v>6.8965517241379297</v>
+      </c>
+      <c r="M23" s="5">
+        <v>0</v>
+      </c>
+      <c r="N23" s="5">
+        <v>-6.8965517241379297</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
+        <v>-17.241379310344801</v>
+      </c>
+      <c r="S23">
+        <v>-10.381593610952701</v>
+      </c>
+      <c r="T23" s="34">
+        <v>14.228210755774899</v>
+      </c>
+      <c r="U23">
+        <v>-4.2466159164624404</v>
+      </c>
+      <c r="V23" s="34">
+        <v>40.542624164467902</v>
+      </c>
+      <c r="W23">
+        <v>-10.842693634959099</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="L24" s="5">
+        <v>30</v>
+      </c>
+      <c r="M24" s="5">
+        <v>-30</v>
+      </c>
+      <c r="N24" s="5">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <v>10</v>
+      </c>
+      <c r="P24">
+        <v>0</v>
+      </c>
+      <c r="S24">
+        <v>30.017862256323401</v>
+      </c>
+      <c r="T24" s="34">
+        <v>-30.0033829738619</v>
+      </c>
+      <c r="U24">
+        <v>0</v>
+      </c>
+      <c r="V24">
+        <v>10.001127657953999</v>
+      </c>
+      <c r="W24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="L25" s="5">
+        <v>17.241379310344801</v>
+      </c>
+      <c r="M25" s="5">
+        <v>0</v>
+      </c>
+      <c r="N25" s="5">
+        <v>-17.241379310344801</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="P25">
+        <v>6.8965517241379297</v>
+      </c>
+      <c r="S25">
+        <v>-29.699934406035901</v>
+      </c>
+      <c r="T25" s="73">
+        <v>40.542631917522201</v>
+      </c>
+      <c r="U25">
+        <v>-10.842693634959099</v>
+      </c>
+      <c r="V25" s="34">
+        <v>-15.028208299055301</v>
+      </c>
+      <c r="W25">
+        <v>4.2466159164624404</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="L26" s="20">
+        <v>2</v>
+      </c>
+      <c r="M26" s="5">
+        <v>0</v>
+      </c>
+      <c r="N26" s="5">
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="P26">
+        <v>0</v>
+      </c>
+      <c r="S26">
+        <v>0</v>
+      </c>
+      <c r="T26">
+        <v>1.98962793658121</v>
+      </c>
+      <c r="U26">
+        <v>0</v>
+      </c>
+      <c r="V26">
+        <v>-2.88969285364425E-2</v>
+      </c>
+      <c r="W26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="L28" s="5">
+        <v>10.486384725291501</v>
+      </c>
+      <c r="M28" s="5">
+        <v>-9.9999429523071601</v>
+      </c>
+      <c r="N28" s="5">
+        <v>0</v>
+      </c>
+      <c r="O28">
+        <v>-29.9998288569215</v>
+      </c>
+      <c r="P28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="L29" s="5">
+        <v>7.3161965228419001</v>
+      </c>
+      <c r="M29" s="5">
+        <v>0</v>
+      </c>
+      <c r="N29" s="5">
+        <v>-6.8965123809014903</v>
+      </c>
+      <c r="O29">
+        <v>0</v>
+      </c>
+      <c r="P29">
+        <v>-17.2412809522537</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="L30" s="5">
+        <v>30.0143074678918</v>
+      </c>
+      <c r="M30" s="5">
+        <v>-29.9998288569215</v>
+      </c>
+      <c r="N30" s="5">
+        <v>0</v>
+      </c>
+      <c r="O30">
+        <v>9.9999429523071601</v>
+      </c>
+      <c r="P30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="L31" s="5">
+        <v>17.243376683724399</v>
+      </c>
+      <c r="M31" s="5">
+        <v>0</v>
+      </c>
+      <c r="N31" s="5">
+        <v>-17.2412809522537</v>
+      </c>
+      <c r="O31">
+        <v>0</v>
+      </c>
+      <c r="P31">
+        <v>6.8965123809014903</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="L32" s="5">
+        <v>1.9999885904614301</v>
+      </c>
+      <c r="M32" s="5">
+        <v>0</v>
+      </c>
+      <c r="N32" s="5">
+        <v>0</v>
+      </c>
+      <c r="O32">
+        <v>0</v>
+      </c>
+      <c r="P32">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:R134"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2798,18 +3896,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="65" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
-      <c r="J1" s="64"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
       <c r="K1" s="43"/>
       <c r="L1" s="60"/>
       <c r="M1" s="11" t="s">
@@ -2833,18 +3931,18 @@
       <c r="B2" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="65" t="s">
+      <c r="C2" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65" t="s">
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66" t="s">
         <v>74</v>
       </c>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="65"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="66"/>
       <c r="K2" s="4"/>
       <c r="L2" s="60" t="s">
         <v>139</v>
@@ -5193,7 +6291,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q66"/>
   <sheetViews>
@@ -5212,18 +6310,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="65" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
-      <c r="J1" s="64"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
       <c r="L1" s="11" t="s">
         <v>1</v>
       </c>
@@ -5247,18 +6345,18 @@
       <c r="B2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="65" t="s">
+      <c r="C2" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65" t="s">
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66" t="s">
         <v>74</v>
       </c>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="65"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="66"/>
       <c r="L2" s="8" t="s">
         <v>41</v>
       </c>
@@ -6051,18 +7149,18 @@
       <c r="O33" s="1"/>
     </row>
     <row r="35" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="64" t="s">
+      <c r="A35" s="65" t="s">
         <v>78</v>
       </c>
-      <c r="B35" s="64"/>
-      <c r="C35" s="64"/>
-      <c r="D35" s="64"/>
-      <c r="E35" s="64"/>
-      <c r="F35" s="64"/>
-      <c r="G35" s="64"/>
-      <c r="H35" s="64"/>
-      <c r="I35" s="64"/>
-      <c r="J35" s="64"/>
+      <c r="B35" s="65"/>
+      <c r="C35" s="65"/>
+      <c r="D35" s="65"/>
+      <c r="E35" s="65"/>
+      <c r="F35" s="65"/>
+      <c r="G35" s="65"/>
+      <c r="H35" s="65"/>
+      <c r="I35" s="65"/>
+      <c r="J35" s="65"/>
       <c r="L35" s="11" t="s">
         <v>1</v>
       </c>
@@ -6791,7 +7889,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA61"/>
   <sheetViews>
@@ -6807,13 +7905,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="63" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
       <c r="G1" s="30" t="s">
         <v>100</v>
       </c>
@@ -6832,13 +7930,13 @@
       <c r="L1" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="P1" s="62" t="s">
+      <c r="P1" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="Q1" s="62"/>
-      <c r="R1" s="62"/>
-      <c r="S1" s="62"/>
-      <c r="T1" s="62"/>
+      <c r="Q1" s="63"/>
+      <c r="R1" s="63"/>
+      <c r="S1" s="63"/>
+      <c r="T1" s="63"/>
       <c r="V1" s="30" t="s">
         <v>100</v>
       </c>
@@ -7373,12 +8471,12 @@
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="P10" s="62" t="s">
+      <c r="P10" s="63" t="s">
         <v>108</v>
       </c>
-      <c r="Q10" s="62"/>
-      <c r="R10" s="62"/>
-      <c r="S10" s="62"/>
+      <c r="Q10" s="63"/>
+      <c r="R10" s="63"/>
+      <c r="S10" s="63"/>
       <c r="T10" s="25"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
@@ -8394,12 +9492,12 @@
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A33" s="62" t="s">
+      <c r="A33" s="63" t="s">
         <v>102</v>
       </c>
-      <c r="B33" s="62"/>
-      <c r="C33" s="62"/>
-      <c r="D33" s="62"/>
+      <c r="B33" s="63"/>
+      <c r="C33" s="63"/>
+      <c r="D33" s="63"/>
       <c r="F33" s="30" t="s">
         <v>100</v>
       </c>
@@ -8777,12 +9875,12 @@
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A42" s="62" t="s">
+      <c r="A42" s="63" t="s">
         <v>104</v>
       </c>
-      <c r="B42" s="62"/>
-      <c r="C42" s="62"/>
-      <c r="D42" s="62"/>
+      <c r="B42" s="63"/>
+      <c r="C42" s="63"/>
+      <c r="D42" s="63"/>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">

</xml_diff>

<commit_message>
Should try adding a ton of measurements to the 14 bus ADMM system
I tried adding a few select measurements to Partition 1 in
example_14bus_IEEE_rectADMM, but they didn't seem to help the ADMM
convergence (in fact, made it worse). I also coded up an automatic way
to aggregate c_k, but it complicates how numPart is calculated... It
might be better to go back to yesterday's commit as a starting point.
The next thing to try is to probably add a ton more measurements to the
whole system.
</commit_message>
<xml_diff>
--- a/DMASE - Test Results.xlsx
+++ b/DMASE - Test Results.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="210">
   <si>
     <t>Abur 3-Bus Case Measurements (run through SE, rerun new estimate again)</t>
   </si>
@@ -631,6 +631,27 @@
   </si>
   <si>
     <t>Type</t>
+  </si>
+  <si>
+    <t>Extra Meas</t>
+  </si>
+  <si>
+    <t>Central AC Res</t>
+  </si>
+  <si>
+    <t>P5-6</t>
+  </si>
+  <si>
+    <t>Q5-6</t>
+  </si>
+  <si>
+    <t>P2-3</t>
+  </si>
+  <si>
+    <t>Q2-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V2 </t>
   </si>
 </sst>
 </file>
@@ -810,7 +831,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -983,6 +1004,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -991,6 +1015,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1309,15 +1336,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="80" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
       <c r="I1" s="6" t="s">
         <v>1</v>
       </c>
@@ -1568,15 +1595,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="79" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
+      <c r="A1" s="80" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
       <c r="I1" s="6" t="s">
         <v>1</v>
       </c>
@@ -1929,15 +1956,15 @@
       <c r="N11" s="1"/>
     </row>
     <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="80" t="s">
+      <c r="A12" s="81" t="s">
         <v>80</v>
       </c>
-      <c r="B12" s="80"/>
-      <c r="C12" s="80"/>
-      <c r="D12" s="80"/>
-      <c r="E12" s="80"/>
-      <c r="F12" s="80"/>
-      <c r="G12" s="80"/>
+      <c r="B12" s="81"/>
+      <c r="C12" s="81"/>
+      <c r="D12" s="81"/>
+      <c r="E12" s="81"/>
+      <c r="F12" s="81"/>
+      <c r="G12" s="81"/>
       <c r="I12" s="1"/>
       <c r="J12" s="6" t="s">
         <v>1</v>
@@ -2427,15 +2454,15 @@
       <c r="G31" s="1"/>
     </row>
     <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="80" t="s">
+      <c r="A32" s="81" t="s">
         <v>81</v>
       </c>
-      <c r="B32" s="80"/>
-      <c r="C32" s="80"/>
-      <c r="D32" s="80"/>
-      <c r="E32" s="80"/>
-      <c r="F32" s="80"/>
-      <c r="G32" s="80"/>
+      <c r="B32" s="81"/>
+      <c r="C32" s="81"/>
+      <c r="D32" s="81"/>
+      <c r="E32" s="81"/>
+      <c r="F32" s="81"/>
+      <c r="G32" s="81"/>
       <c r="I32" s="1"/>
       <c r="J32" s="6" t="s">
         <v>1</v>
@@ -2914,13 +2941,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="80" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
       <c r="G1" s="30" t="s">
         <v>100</v>
       </c>
@@ -2939,13 +2966,13 @@
       <c r="L1" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="P1" s="79" t="s">
+      <c r="P1" s="80" t="s">
         <v>106</v>
       </c>
-      <c r="Q1" s="79"/>
-      <c r="R1" s="79"/>
-      <c r="S1" s="79"/>
-      <c r="T1" s="79"/>
+      <c r="Q1" s="80"/>
+      <c r="R1" s="80"/>
+      <c r="S1" s="80"/>
+      <c r="T1" s="80"/>
       <c r="V1" s="30" t="s">
         <v>100</v>
       </c>
@@ -3480,12 +3507,12 @@
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="P10" s="79" t="s">
+      <c r="P10" s="80" t="s">
         <v>108</v>
       </c>
-      <c r="Q10" s="79"/>
-      <c r="R10" s="79"/>
-      <c r="S10" s="79"/>
+      <c r="Q10" s="80"/>
+      <c r="R10" s="80"/>
+      <c r="S10" s="80"/>
       <c r="T10" s="25"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
@@ -4501,12 +4528,12 @@
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A33" s="79" t="s">
+      <c r="A33" s="80" t="s">
         <v>102</v>
       </c>
-      <c r="B33" s="79"/>
-      <c r="C33" s="79"/>
-      <c r="D33" s="79"/>
+      <c r="B33" s="80"/>
+      <c r="C33" s="80"/>
+      <c r="D33" s="80"/>
       <c r="F33" s="30" t="s">
         <v>100</v>
       </c>
@@ -4884,12 +4911,12 @@
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A42" s="79" t="s">
+      <c r="A42" s="80" t="s">
         <v>104</v>
       </c>
-      <c r="B42" s="79"/>
-      <c r="C42" s="79"/>
-      <c r="D42" s="79"/>
+      <c r="B42" s="80"/>
+      <c r="C42" s="80"/>
+      <c r="D42" s="80"/>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
@@ -5388,15 +5415,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="81" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
       <c r="I1" s="1"/>
       <c r="J1" s="4"/>
       <c r="L1" s="4" t="s">
@@ -6444,10 +6471,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R134"/>
+  <dimension ref="A1:R140"/>
   <sheetViews>
-    <sheetView topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6463,18 +6490,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="82" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
-      <c r="F1" s="81"/>
-      <c r="G1" s="81"/>
-      <c r="H1" s="81"/>
-      <c r="I1" s="81"/>
-      <c r="J1" s="81"/>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
+      <c r="J1" s="82"/>
       <c r="K1" s="43"/>
       <c r="L1" s="60"/>
       <c r="M1" s="11" t="s">
@@ -6487,7 +6514,7 @@
         <v>138</v>
       </c>
       <c r="P1" s="11" t="s">
-        <v>40</v>
+        <v>204</v>
       </c>
       <c r="R1" s="18" t="s">
         <v>35</v>
@@ -6498,18 +6525,18 @@
       <c r="B2" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="82" t="s">
+      <c r="C2" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="82"/>
-      <c r="E2" s="82"/>
-      <c r="F2" s="82"/>
-      <c r="G2" s="82" t="s">
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="83" t="s">
         <v>74</v>
       </c>
-      <c r="H2" s="82"/>
-      <c r="I2" s="82"/>
-      <c r="J2" s="82"/>
+      <c r="H2" s="83"/>
+      <c r="I2" s="83"/>
+      <c r="J2" s="83"/>
       <c r="K2" s="4"/>
       <c r="L2" s="60" t="s">
         <v>139</v>
@@ -6524,9 +6551,7 @@
         <f>N2/100</f>
         <v>1.56440731910842</v>
       </c>
-      <c r="P2" s="58">
-        <v>1.06336745888669E-5</v>
-      </c>
+      <c r="P2" s="58"/>
       <c r="R2" t="s">
         <v>75</v>
       </c>
@@ -6572,9 +6597,7 @@
         <f t="shared" ref="O3:O9" si="0">N3/100</f>
         <v>-0.20300935880694301</v>
       </c>
-      <c r="P3" s="58">
-        <v>4.3355679321677199E-5</v>
-      </c>
+      <c r="P3" s="58"/>
       <c r="R3" s="2" t="s">
         <v>137</v>
       </c>
@@ -6585,6 +6608,9 @@
       </c>
       <c r="B4" s="1">
         <v>1.0599621403577</v>
+      </c>
+      <c r="C4" s="72">
+        <v>1.06046091821972</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -6605,9 +6631,7 @@
         <f t="shared" si="0"/>
         <v>0.75916881283268789</v>
       </c>
-      <c r="P4" s="58">
-        <v>1.3004902296165399E-6</v>
-      </c>
+      <c r="P4" s="58"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -6616,7 +6640,12 @@
       <c r="B5" s="1">
         <v>1.04103609065253</v>
       </c>
-      <c r="D5" s="1"/>
+      <c r="C5" s="72">
+        <v>1.0415317204627199</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1.0387512194945701</v>
+      </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -6635,9 +6664,7 @@
         <f t="shared" si="0"/>
         <v>-1.55506560051652E-3</v>
       </c>
-      <c r="P5" s="58">
-        <v>1.94687132150312E-5</v>
-      </c>
+      <c r="P5" s="58"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -6646,7 +6673,9 @@
       <c r="B6" s="1">
         <v>0.98533801740076798</v>
       </c>
-      <c r="D6" s="1"/>
+      <c r="D6" s="1">
+        <v>0.97941761721577303</v>
+      </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -6665,9 +6694,7 @@
         <f t="shared" si="0"/>
         <v>0.41338725991097197</v>
       </c>
-      <c r="P6" s="58">
-        <v>6.7696186707433304E-6</v>
-      </c>
+      <c r="P6" s="58"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -6676,7 +6703,12 @@
       <c r="B7" s="1">
         <v>1.00691238196979</v>
       </c>
-      <c r="D7" s="1"/>
+      <c r="C7" s="72">
+        <v>1.0045255871869501</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1.00185731587878</v>
+      </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -6695,9 +6727,7 @@
         <f t="shared" si="0"/>
         <v>-3.8398609004379101E-2</v>
       </c>
-      <c r="P7" s="58">
-        <v>1.0256187421023299E-5</v>
-      </c>
+      <c r="P7" s="58"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -6706,7 +6736,12 @@
       <c r="B8" s="1">
         <v>1.01577582353094</v>
       </c>
-      <c r="D8" s="1"/>
+      <c r="C8" s="72">
+        <v>1.01639383512379</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1.0114151980721</v>
+      </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -6725,9 +6760,7 @@
         <f t="shared" si="0"/>
         <v>2.32357621192932</v>
       </c>
-      <c r="P8" s="58">
-        <v>1.20141648185523E-5</v>
-      </c>
+      <c r="P8" s="58"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -6736,7 +6769,12 @@
       <c r="B9" s="1">
         <v>1.0048890478609001</v>
       </c>
-      <c r="E9" s="1"/>
+      <c r="C9" s="72">
+        <v>1.0130086495044099</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1.0219150296964401</v>
+      </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -6754,9 +6792,7 @@
         <f t="shared" si="0"/>
         <v>-0.20456442236900302</v>
       </c>
-      <c r="P9" s="58">
-        <v>6.2827392531661404E-5</v>
-      </c>
+      <c r="P9" s="58"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -6765,8 +6801,9 @@
       <c r="B10" s="1">
         <v>1.0165083916826201</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+      <c r="D10" s="72">
+        <v>1.0095485374987301</v>
+      </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -6786,9 +6823,7 @@
         <f>N10/100</f>
         <v>-0.235697408335068</v>
       </c>
-      <c r="P10" s="58">
-        <v>-1.5324438971953099E-6</v>
-      </c>
+      <c r="P10" s="58"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -6797,8 +6832,9 @@
       <c r="B11" s="1">
         <v>1.05436901591651</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+      <c r="D11" s="1">
+        <v>1.04711714761956</v>
+      </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -6818,9 +6854,7 @@
         <f t="shared" ref="O11:O15" si="1">N11/100</f>
         <v>9.6859150246414102E-3</v>
       </c>
-      <c r="P11" s="58">
-        <v>-5.9967407733847699E-6</v>
-      </c>
+      <c r="P11" s="58"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -6829,9 +6863,12 @@
       <c r="B12" s="1">
         <v>0.99791127060776097</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="F12" s="1"/>
+      <c r="D12" s="1">
+        <v>0.99022778494432395</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1.01864336835583</v>
+      </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
@@ -6848,9 +6885,7 @@
         <f t="shared" si="1"/>
         <v>0.29247688021076401</v>
       </c>
-      <c r="P12" s="58">
-        <v>6.0811903938029496E-6</v>
-      </c>
+      <c r="P12" s="58"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -6859,9 +6894,9 @@
       <c r="B13" s="1">
         <v>0.99039833975510105</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="F13" s="1"/>
+      <c r="F13" s="1">
+        <v>1.0112197070817699</v>
+      </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -6878,9 +6913,7 @@
         <f t="shared" si="1"/>
         <v>-0.101343842359942</v>
       </c>
-      <c r="P13" s="58">
-        <v>8.8204619878157198E-6</v>
-      </c>
+      <c r="P13" s="58"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -6890,9 +6923,12 @@
         <v>0.99354407863493799</v>
       </c>
       <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
+      <c r="E14" s="72">
+        <v>1.01121442717815</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1.0139243260461199</v>
+      </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
@@ -6909,9 +6945,7 @@
         <f t="shared" si="1"/>
         <v>4.9388912162000003E-7</v>
       </c>
-      <c r="P14" s="58">
-        <v>7.3644127437410898E-6</v>
-      </c>
+      <c r="P14" s="58"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -6921,8 +6955,9 @@
         <v>0.98670699585233201</v>
       </c>
       <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+      <c r="E15" s="72">
+        <v>1.0045674174936901</v>
+      </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
@@ -6939,9 +6974,7 @@
         <f t="shared" si="1"/>
         <v>-0.231382548362844</v>
       </c>
-      <c r="P15" s="58">
-        <v>-1.3409001482223E-6</v>
-      </c>
+      <c r="P15" s="58"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -6951,9 +6984,12 @@
         <v>0.98227711504043203</v>
       </c>
       <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
+      <c r="E16" s="72">
+        <v>1.00023502466276</v>
+      </c>
+      <c r="F16" s="72">
+        <v>1.0031611566719001</v>
+      </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
@@ -6972,9 +7008,7 @@
         <f>N16/100</f>
         <v>6.4193752642371704E-2</v>
       </c>
-      <c r="P16" s="58">
-        <v>-1.70762709954253E-6</v>
-      </c>
+      <c r="P16" s="58"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
@@ -6984,9 +7018,12 @@
         <v>0.96821859389559195</v>
       </c>
       <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
+      <c r="E17" s="72">
+        <v>0.98715606381157694</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0.99019975062743504</v>
+      </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
@@ -7005,9 +7042,7 @@
         <f t="shared" ref="O17:O25" si="2">N17/100</f>
         <v>1.5779898155030701E-2</v>
       </c>
-      <c r="P17" s="58">
-        <v>-3.39117996042693E-6</v>
-      </c>
+      <c r="P17" s="58"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
@@ -7016,6 +7051,12 @@
       <c r="B18">
         <v>-9.0498906725745204E-2</v>
       </c>
+      <c r="C18" s="72">
+        <v>-9.0453056678055102E-2</v>
+      </c>
+      <c r="D18" s="1">
+        <v>-0.11705687930061399</v>
+      </c>
       <c r="L18" s="60"/>
       <c r="M18" s="46" t="s">
         <v>57</v>
@@ -7027,9 +7068,7 @@
         <f t="shared" si="2"/>
         <v>7.6111237412808605E-2</v>
       </c>
-      <c r="P18" s="58">
-        <v>-2.9288166818880502E-6</v>
-      </c>
+      <c r="P18" s="58"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
@@ -7038,6 +7077,9 @@
       <c r="B19">
         <v>-0.22165365184591099</v>
       </c>
+      <c r="D19" s="1">
+        <v>-0.24696856648182799</v>
+      </c>
       <c r="L19" s="60"/>
       <c r="M19" s="46" t="s">
         <v>123</v>
@@ -7049,9 +7091,7 @@
         <f t="shared" si="2"/>
         <v>2.2749299623984597E-2</v>
       </c>
-      <c r="P19" s="58">
-        <v>4.5373436844440403E-5</v>
-      </c>
+      <c r="P19" s="58"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
@@ -7060,6 +7100,12 @@
       <c r="B20">
         <v>-0.184493248459114</v>
       </c>
+      <c r="C20" s="1">
+        <v>-0.18973189157605599</v>
+      </c>
+      <c r="D20" s="1">
+        <v>-0.210271602561001</v>
+      </c>
       <c r="L20" s="60"/>
       <c r="M20" s="46" t="s">
         <v>58</v>
@@ -7071,9 +7117,7 @@
         <f t="shared" si="2"/>
         <v>0.17236621109828601</v>
       </c>
-      <c r="P20" s="58">
-        <v>-1.4699917021965299E-6</v>
-      </c>
+      <c r="P20" s="58"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
@@ -7082,6 +7126,12 @@
       <c r="B21">
         <v>-0.15841659033345201</v>
       </c>
+      <c r="C21" s="1">
+        <v>-0.158348436134123</v>
+      </c>
+      <c r="D21" s="1">
+        <v>-0.184378898266429</v>
+      </c>
       <c r="L21" s="60"/>
       <c r="M21" s="46" t="s">
         <v>125</v>
@@ -7093,9 +7143,7 @@
         <f t="shared" si="2"/>
         <v>6.2088690408799697E-2</v>
       </c>
-      <c r="P21" s="58">
-        <v>6.9140064405080802E-5</v>
-      </c>
+      <c r="P21" s="58"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
@@ -7104,6 +7152,12 @@
       <c r="B22">
         <v>-0.262083078069408</v>
       </c>
+      <c r="C22" s="1">
+        <v>-0.227788998176361</v>
+      </c>
+      <c r="E22" s="1">
+        <v>-0.18643976635270701</v>
+      </c>
       <c r="L22" s="60"/>
       <c r="M22" s="46" t="s">
         <v>59</v>
@@ -7115,9 +7169,7 @@
         <f t="shared" si="2"/>
         <v>1.4392071686730901E-2</v>
       </c>
-      <c r="P22" s="58">
-        <v>-3.0935268891200298E-6</v>
-      </c>
+      <c r="P22" s="58"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
@@ -7126,6 +7178,9 @@
       <c r="B23">
         <v>-0.24699463946439601</v>
       </c>
+      <c r="D23" s="1">
+        <v>-0.27303668219411098</v>
+      </c>
       <c r="L23" s="60"/>
       <c r="M23" s="46" t="s">
         <v>126</v>
@@ -7137,9 +7192,7 @@
         <f t="shared" si="2"/>
         <v>5.2526799870488807E-3</v>
       </c>
-      <c r="P23" s="58">
-        <v>-8.1203675952107E-6</v>
-      </c>
+      <c r="P23" s="58"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
@@ -7148,6 +7201,9 @@
       <c r="B24">
         <v>-0.25619422730604202</v>
       </c>
+      <c r="D24" s="1">
+        <v>-0.28320201674479101</v>
+      </c>
       <c r="L24" s="60"/>
       <c r="M24" s="46" t="s">
         <v>12</v>
@@ -7159,9 +7215,7 @@
         <f t="shared" si="2"/>
         <v>-6.0999999999999999E-2</v>
       </c>
-      <c r="P24" s="58">
-        <v>2.3373457752606801E-9</v>
-      </c>
+      <c r="P24" s="58"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
@@ -7170,6 +7224,12 @@
       <c r="B25">
         <v>-0.274128496301564</v>
       </c>
+      <c r="D25" s="72">
+        <v>-0.29974357866110901</v>
+      </c>
+      <c r="F25" s="1">
+        <v>-0.18536451528078199</v>
+      </c>
       <c r="L25" s="60"/>
       <c r="M25" s="46" t="s">
         <v>20</v>
@@ -7181,9 +7241,7 @@
         <f t="shared" si="2"/>
         <v>-1.6E-2</v>
       </c>
-      <c r="P25" s="58">
-        <v>5.1566951013160001E-5</v>
-      </c>
+      <c r="P25" s="58"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
@@ -7192,6 +7250,9 @@
       <c r="B26">
         <v>-0.27530156310841902</v>
       </c>
+      <c r="F26" s="72">
+        <v>-0.18719102288282999</v>
+      </c>
       <c r="L26" s="60" t="s">
         <v>142</v>
       </c>
@@ -7205,9 +7266,7 @@
         <f>N26/100</f>
         <v>6.1481308294477899E-2</v>
       </c>
-      <c r="P26" s="57">
-        <v>-1.3131668610555401E-6</v>
-      </c>
+      <c r="P26" s="57"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
@@ -7216,6 +7275,12 @@
       <c r="B27">
         <v>-0.27033852619593501</v>
       </c>
+      <c r="E27" s="1">
+        <v>-0.19551994317777699</v>
+      </c>
+      <c r="F27" s="72">
+        <v>-0.18196005016786601</v>
+      </c>
       <c r="L27" s="56" t="s">
         <v>177</v>
       </c>
@@ -7229,9 +7294,7 @@
         <f t="shared" ref="O27:O39" si="3">N27/100</f>
         <v>6.1776975079165707E-2</v>
       </c>
-      <c r="P27" s="57">
-        <v>4.8795271359383697E-6</v>
-      </c>
+      <c r="P27" s="57"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
@@ -7240,6 +7303,9 @@
       <c r="B28">
         <v>-0.27393942115060799</v>
       </c>
+      <c r="E28" s="1">
+        <v>-0.19960947382823699</v>
+      </c>
       <c r="L28" s="61"/>
       <c r="M28" s="46" t="s">
         <v>62</v>
@@ -7251,9 +7317,7 @@
         <f t="shared" si="3"/>
         <v>0.101258308263922</v>
       </c>
-      <c r="P28" s="58">
-        <v>-1.22208074135322E-6</v>
-      </c>
+      <c r="P28" s="58"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
@@ -7262,6 +7326,12 @@
       <c r="B29">
         <v>-0.274447646882094</v>
       </c>
+      <c r="E29" s="1">
+        <v>-0.20045288832859101</v>
+      </c>
+      <c r="F29" s="72">
+        <v>-0.18699857554614599</v>
+      </c>
       <c r="L29" s="61"/>
       <c r="M29" s="46" t="s">
         <v>128</v>
@@ -7273,9 +7343,7 @@
         <f t="shared" si="3"/>
         <v>4.8779939913553595E-2</v>
       </c>
-      <c r="P29" s="57">
-        <v>4.90141539373143E-5</v>
-      </c>
+      <c r="P29" s="57"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
@@ -7284,6 +7352,12 @@
       <c r="B30">
         <v>-0.28719972332980598</v>
       </c>
+      <c r="E30" s="72">
+        <v>-0.214195311803524</v>
+      </c>
+      <c r="F30" s="72">
+        <v>-0.200990701503165</v>
+      </c>
       <c r="L30" s="60" t="s">
         <v>143</v>
       </c>
@@ -7297,9 +7371,7 @@
         <f t="shared" si="3"/>
         <v>-7.5999999999999998E-2</v>
       </c>
-      <c r="P30" s="58">
-        <v>4.3947993498549799E-7</v>
-      </c>
+      <c r="P30" s="58"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="L31" s="56" t="s">
@@ -7315,9 +7387,7 @@
         <f t="shared" si="3"/>
         <v>-1.6E-2</v>
       </c>
-      <c r="P31" s="58">
-        <v>-1.14950706093311E-5</v>
-      </c>
+      <c r="P31" s="58"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="L32" s="60" t="s">
@@ -7333,9 +7403,7 @@
         <f t="shared" si="3"/>
         <v>-0.63001699846354908</v>
       </c>
-      <c r="P32" s="58">
-        <v>-7.6439598420963202E-6</v>
-      </c>
+      <c r="P32" s="58"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="L33" s="56" t="s">
@@ -7351,9 +7419,7 @@
         <f t="shared" si="3"/>
         <v>0.102039485868599</v>
       </c>
-      <c r="P33" s="58">
-        <v>-1.95571751745866E-5</v>
-      </c>
+      <c r="P33" s="58"/>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="L34" s="60"/>
@@ -7367,9 +7433,7 @@
         <f t="shared" si="3"/>
         <v>0.16526211548050401</v>
       </c>
-      <c r="P34" s="58">
-        <v>-4.8466870822272401E-7</v>
-      </c>
+      <c r="P34" s="58"/>
     </row>
     <row r="35" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="49"/>
@@ -7394,9 +7458,7 @@
         <f t="shared" si="3"/>
         <v>-1.34369314780613E-2</v>
       </c>
-      <c r="P35" s="58">
-        <v>5.79302350887934E-6</v>
-      </c>
+      <c r="P35" s="58"/>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="47"/>
@@ -7421,9 +7483,7 @@
         <f t="shared" si="3"/>
         <v>0.29247637436823104</v>
       </c>
-      <c r="P36" s="58">
-        <v>-9.6765970603040998E-7</v>
-      </c>
+      <c r="P36" s="58"/>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="47"/>
@@ -7448,9 +7508,7 @@
         <f t="shared" si="3"/>
         <v>0.11091977693706599</v>
       </c>
-      <c r="P37" s="58">
-        <v>1.05122553067938E-5</v>
-      </c>
+      <c r="P37" s="58"/>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="47"/>
@@ -7475,9 +7533,7 @@
         <f t="shared" si="3"/>
         <v>-0.94199996999999991</v>
       </c>
-      <c r="P38" s="58">
-        <v>-4.0078032588208899E-6</v>
-      </c>
+      <c r="P38" s="58"/>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
@@ -7501,9 +7557,7 @@
         <f t="shared" si="3"/>
         <v>2.4613437652587004E-2</v>
       </c>
-      <c r="P39" s="58">
-        <v>-3.0646956959021199E-5</v>
-      </c>
+      <c r="P39" s="58"/>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
@@ -7527,9 +7581,7 @@
         <f>N40/100</f>
         <v>4.9650161007164101E-2</v>
       </c>
-      <c r="P40" s="58">
-        <v>-1.8263251861869199E-6</v>
-      </c>
+      <c r="P40" s="58"/>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
@@ -7554,9 +7606,7 @@
         <f t="shared" ref="O41:O43" si="4">N41/100</f>
         <v>5.2427629116916794E-3</v>
       </c>
-      <c r="P41" s="58">
-        <v>6.8227725995599298E-6</v>
-      </c>
+      <c r="P41" s="58"/>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
@@ -7579,9 +7629,7 @@
         <f t="shared" si="4"/>
         <v>-0.13500000000000001</v>
       </c>
-      <c r="P42" s="58">
-        <v>3.1143046591852699E-6</v>
-      </c>
+      <c r="P42" s="58"/>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
@@ -7605,15 +7653,14 @@
         <f t="shared" si="4"/>
         <v>-5.7999999999999996E-2</v>
       </c>
-      <c r="P43" s="58">
-        <v>5.0234520724452802E-5</v>
-      </c>
+      <c r="P43" s="58"/>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
+      <c r="E44" s="72"/>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
@@ -7633,15 +7680,14 @@
         <f>N44/100</f>
         <v>-2.8744036925517299E-2</v>
       </c>
-      <c r="P44" s="58">
-        <v>1.03396272051193E-6</v>
-      </c>
+      <c r="P44" s="58"/>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
+      <c r="E45" s="72"/>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
@@ -7658,18 +7704,17 @@
         <v>0.31779049296478201</v>
       </c>
       <c r="O45" s="1">
-        <f t="shared" ref="O45:O47" si="5">N45/100</f>
+        <f t="shared" ref="O45:O53" si="5">N45/100</f>
         <v>3.1779049296478202E-3</v>
       </c>
-      <c r="P45" s="58">
-        <v>4.5458701069499302E-6</v>
-      </c>
+      <c r="P45" s="58"/>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
+      <c r="E46" s="72"/>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
@@ -7687,9 +7732,7 @@
         <f t="shared" si="5"/>
         <v>-0.14899999999999999</v>
       </c>
-      <c r="P46" s="58">
-        <v>3.11371443725839E-6</v>
-      </c>
+      <c r="P46" s="58"/>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
@@ -7713,11 +7756,9 @@
         <f t="shared" si="5"/>
         <v>-0.05</v>
       </c>
-      <c r="P47" s="58">
-        <v>4.6668128149698902E-5</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P47" s="58"/>
+    </row>
+    <row r="48" spans="1:16" s="72" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -7728,1068 +7769,1183 @@
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
-      <c r="M48" s="46"/>
-      <c r="N48" s="52"/>
-      <c r="O48" s="1"/>
+      <c r="L48" s="60" t="s">
+        <v>203</v>
+      </c>
+      <c r="M48" s="79" t="s">
+        <v>207</v>
+      </c>
+      <c r="N48" s="84">
+        <v>72.934574594694098</v>
+      </c>
+      <c r="O48" s="1">
+        <f t="shared" si="5"/>
+        <v>0.72934574594694102</v>
+      </c>
       <c r="P48" s="58"/>
     </row>
-    <row r="49" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:16" s="72" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
-      <c r="M49" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="N49" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="O49" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="P49" s="11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="50" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="L49" s="60"/>
+      <c r="M49" s="79" t="s">
+        <v>208</v>
+      </c>
+      <c r="N49" s="72">
+        <v>3.5900360862934599</v>
+      </c>
+      <c r="O49" s="1">
+        <f>N49/100</f>
+        <v>3.5900360862934598E-2</v>
+      </c>
+      <c r="P49" s="58"/>
+    </row>
+    <row r="50" spans="1:16" s="72" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
-      <c r="L50" t="s">
-        <v>139</v>
-      </c>
-      <c r="M50" s="42" t="s">
-        <v>41</v>
-      </c>
-      <c r="N50" s="50">
-        <v>0</v>
-      </c>
-      <c r="O50" s="54">
-        <f>N50</f>
-        <v>0</v>
-      </c>
-      <c r="P50" s="58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L50" s="60"/>
+      <c r="M50" s="79" t="s">
+        <v>205</v>
+      </c>
+      <c r="N50" s="52">
+        <v>42.467165475154701</v>
+      </c>
+      <c r="O50" s="1">
+        <f t="shared" si="5"/>
+        <v>0.424671654751547</v>
+      </c>
+      <c r="P50" s="58"/>
+    </row>
+    <row r="51" spans="1:16" s="72" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
-      <c r="L51" s="55">
-        <v>4.8611111111111112E-2</v>
-      </c>
-      <c r="M51" s="42" t="s">
-        <v>23</v>
-      </c>
-      <c r="N51" s="50">
-        <v>1.0599999427795399</v>
-      </c>
-      <c r="O51" s="54">
-        <f>N51</f>
-        <v>1.0599999427795399</v>
-      </c>
-      <c r="P51" s="58">
-        <v>-2.9953879373185301E-2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L51" s="60"/>
+      <c r="M51" s="79" t="s">
+        <v>206</v>
+      </c>
+      <c r="N51" s="84">
+        <v>-2.12732489205733</v>
+      </c>
+      <c r="O51" s="1">
+        <f t="shared" si="5"/>
+        <v>-2.12732489205733E-2</v>
+      </c>
+      <c r="P51" s="58"/>
+    </row>
+    <row r="52" spans="1:16" s="72" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
-      <c r="M52" s="42" t="s">
+      <c r="L52" s="60"/>
+      <c r="M52" s="79" t="s">
+        <v>209</v>
+      </c>
+      <c r="N52" s="84">
+        <v>1.04499995797579</v>
+      </c>
+      <c r="O52" s="1">
+        <f>N52</f>
+        <v>1.04499995797579</v>
+      </c>
+      <c r="P52" s="58"/>
+    </row>
+    <row r="53" spans="1:16" s="72" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+      <c r="J53" s="1"/>
+      <c r="K53" s="1"/>
+      <c r="L53" s="60"/>
+      <c r="M53" s="79"/>
+      <c r="N53" s="52"/>
+      <c r="O53" s="1"/>
+      <c r="P53" s="58"/>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1"/>
+      <c r="K54" s="1"/>
+      <c r="M54" s="46"/>
+      <c r="N54" s="52"/>
+      <c r="O54" s="1"/>
+      <c r="P54" s="58"/>
+    </row>
+    <row r="55" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
+      <c r="J55" s="1"/>
+      <c r="K55" s="1"/>
+      <c r="M55" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="N55" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="O55" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="P55" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="1"/>
+      <c r="I56" s="1"/>
+      <c r="J56" s="1"/>
+      <c r="K56" s="1"/>
+      <c r="L56" t="s">
+        <v>139</v>
+      </c>
+      <c r="M56" s="42" t="s">
+        <v>41</v>
+      </c>
+      <c r="N56" s="50">
+        <v>0</v>
+      </c>
+      <c r="O56" s="54">
+        <f>N56</f>
+        <v>0</v>
+      </c>
+      <c r="P56" s="58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1"/>
+      <c r="I57" s="1"/>
+      <c r="J57" s="1"/>
+      <c r="K57" s="1"/>
+      <c r="L57" s="55">
+        <v>4.8611111111111112E-2</v>
+      </c>
+      <c r="M57" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="N57" s="50">
+        <v>1.0599999427795399</v>
+      </c>
+      <c r="O57" s="54">
+        <f>N57</f>
+        <v>1.0599999427795399</v>
+      </c>
+      <c r="P57" s="58">
+        <v>-2.9953879373185301E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="1"/>
+      <c r="I58" s="1"/>
+      <c r="J58" s="1"/>
+      <c r="K58" s="1"/>
+      <c r="M58" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="N52" s="50">
+      <c r="N58" s="50">
         <v>156.440731910842</v>
       </c>
-      <c r="O52" s="1">
-        <f>N52/100</f>
+      <c r="O58" s="1">
+        <f>N58/100</f>
         <v>1.56440731910842</v>
       </c>
-      <c r="P52" s="58">
+      <c r="P58" s="58">
         <v>-8.6738403137775998E-6</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="M53" s="42" t="s">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M59" s="42" t="s">
         <v>117</v>
       </c>
-      <c r="N53" s="50">
+      <c r="N59" s="50">
         <v>-20.300935880694301</v>
       </c>
-      <c r="O53" s="1">
-        <f t="shared" ref="O53:O59" si="6">N53/100</f>
+      <c r="O59" s="1">
+        <f t="shared" ref="O59:O65" si="6">N59/100</f>
         <v>-0.20300935880694301</v>
       </c>
-      <c r="P53" s="58">
+      <c r="P59" s="58">
         <v>2.1648716178694401E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="M54" s="42" t="s">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M60" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="N54" s="50">
+      <c r="N60" s="50">
         <v>75.916881283268793</v>
       </c>
-      <c r="O54" s="1">
+      <c r="O60" s="1">
         <f t="shared" si="6"/>
         <v>0.75916881283268789</v>
       </c>
-      <c r="P54" s="58">
+      <c r="P60" s="58">
         <v>6.4758759358596297E-4</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="M55" s="42" t="s">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M61" s="42" t="s">
         <v>118</v>
       </c>
-      <c r="N55" s="50">
+      <c r="N61" s="50">
         <v>-0.155506560051652</v>
       </c>
-      <c r="O55" s="1">
+      <c r="O61" s="1">
         <f t="shared" si="6"/>
         <v>-1.55506560051652E-3</v>
       </c>
-      <c r="P55" s="58">
+      <c r="P61" s="58">
         <v>-1.47979634931223E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="M56" s="42" t="s">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M62" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="N56" s="50">
+      <c r="N62" s="50">
         <v>41.338725991097199</v>
       </c>
-      <c r="O56" s="1">
+      <c r="O62" s="1">
         <f t="shared" si="6"/>
         <v>0.41338725991097197</v>
       </c>
-      <c r="P56" s="58">
+      <c r="P62" s="58">
         <v>6.8870384835700903E-4</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="M57" s="42" t="s">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M63" s="42" t="s">
         <v>119</v>
       </c>
-      <c r="N57" s="50">
+      <c r="N63" s="50">
         <v>-3.8398609004379098</v>
       </c>
-      <c r="O57" s="1">
+      <c r="O63" s="1">
         <f t="shared" si="6"/>
         <v>-3.8398609004379101E-2</v>
       </c>
-      <c r="P57" s="58">
+      <c r="P63" s="58">
         <v>-1.3891657030102901E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="M58" s="42" t="s">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M64" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="N58" s="50">
+      <c r="N64" s="50">
         <v>232.35762119293199</v>
       </c>
-      <c r="O58" s="1">
+      <c r="O64" s="1">
         <f t="shared" si="6"/>
         <v>2.32357621192932</v>
       </c>
-      <c r="P58" s="58">
+      <c r="P64" s="58">
         <v>6.3899375327158804E-4</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="M59" s="42" t="s">
+    <row r="65" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M65" s="42" t="s">
         <v>83</v>
       </c>
-      <c r="N59" s="50">
+      <c r="N65" s="50">
         <v>-20.456442236900301</v>
       </c>
-      <c r="O59" s="1">
+      <c r="O65" s="1">
         <f t="shared" si="6"/>
         <v>-0.20456442236900302</v>
       </c>
-      <c r="P59" s="58">
+      <c r="P65" s="58">
         <v>6.8507826856001298E-4</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L60" t="s">
+    <row r="66" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L66" t="s">
         <v>140</v>
       </c>
-      <c r="M60" s="42" t="s">
+      <c r="M66" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="N60" s="50">
+      <c r="N66" s="50">
         <v>-0.22125272217770001</v>
       </c>
-      <c r="O60" s="54">
-        <f>N60</f>
+      <c r="O66" s="54">
+        <f>N66</f>
         <v>-0.22125272217770001</v>
       </c>
-      <c r="P60" s="59">
+      <c r="P66" s="59">
         <v>-0.2212527222</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L61" s="55">
+    <row r="67" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L67" s="55">
         <v>0.47083333333333338</v>
       </c>
-      <c r="M61" s="42" t="s">
+      <c r="M67" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="N61" s="50">
+      <c r="N67" s="50">
         <v>1.0099999973080001</v>
       </c>
-      <c r="O61" s="54">
-        <f>N61</f>
+      <c r="O67" s="54">
+        <f>N67</f>
         <v>1.0099999973080001</v>
       </c>
-      <c r="P61" s="59">
+      <c r="P67" s="59">
         <v>2.17540256007367E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="M62" s="42" t="s">
+    <row r="68" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M68" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="N62" s="50">
+      <c r="N68" s="50">
         <v>-23.569740833506799</v>
       </c>
-      <c r="O62" s="1">
-        <f>N62/100</f>
+      <c r="O68" s="1">
+        <f>N68/100</f>
         <v>-0.235697408335068</v>
       </c>
-      <c r="P62" s="58">
+      <c r="P68" s="58">
         <v>-1.05523560178061E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="M63" s="42" t="s">
+    <row r="69" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M69" s="42" t="s">
         <v>120</v>
       </c>
-      <c r="N63" s="50">
+      <c r="N69" s="50">
         <v>0.96859150246414105</v>
       </c>
-      <c r="O63" s="1">
-        <f t="shared" ref="O63:O67" si="7">N63/100</f>
+      <c r="O69" s="1">
+        <f t="shared" ref="O69:O73" si="7">N69/100</f>
         <v>9.6859150246414102E-3</v>
       </c>
-      <c r="P63" s="58">
+      <c r="P69" s="58">
         <v>-2.2375145874756201E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="M64" s="42" t="s">
+    <row r="70" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M70" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="N64" s="50">
+      <c r="N70" s="50">
         <v>29.247688021076399</v>
       </c>
-      <c r="O64" s="1">
+      <c r="O70" s="1">
         <f t="shared" si="7"/>
         <v>0.29247688021076401</v>
       </c>
-      <c r="P64" s="58">
+      <c r="P70" s="58">
         <v>5.1585990707936401E-4</v>
       </c>
     </row>
-    <row r="65" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="M65" s="42" t="s">
+    <row r="71" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M71" s="42" t="s">
         <v>121</v>
       </c>
-      <c r="N65" s="50">
+      <c r="N71" s="50">
         <v>-10.134384235994199</v>
       </c>
-      <c r="O65" s="1">
+      <c r="O71" s="1">
         <f t="shared" si="7"/>
         <v>-0.101343842359942</v>
       </c>
-      <c r="P65" s="58">
+      <c r="P71" s="58">
         <v>-2.7105327863768802E-3</v>
       </c>
     </row>
-    <row r="66" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="M66" s="42" t="s">
+    <row r="72" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M72" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="N66" s="50">
+      <c r="N72" s="50">
         <v>4.9388912162000001E-5</v>
       </c>
-      <c r="O66" s="1">
+      <c r="O72" s="1">
         <f t="shared" si="7"/>
         <v>4.9388912162000003E-7</v>
       </c>
-      <c r="P66" s="58">
+      <c r="P72" s="58">
         <v>6.5059278082477401E-7</v>
       </c>
     </row>
-    <row r="67" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="M67" s="42" t="s">
+    <row r="73" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M73" s="42" t="s">
         <v>122</v>
       </c>
-      <c r="N67" s="50">
+      <c r="N73" s="50">
         <v>-23.1382548362844</v>
       </c>
-      <c r="O67" s="1">
+      <c r="O73" s="1">
         <f t="shared" si="7"/>
         <v>-0.231382548362844</v>
       </c>
-      <c r="P67" s="58">
+      <c r="P73" s="58">
         <v>1.7465773008429299E-7</v>
       </c>
     </row>
-    <row r="68" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="L68" t="s">
+    <row r="74" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L74" t="s">
         <v>141</v>
       </c>
-      <c r="M68" s="42" t="s">
+      <c r="M74" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="N68" s="50">
+      <c r="N74" s="50">
         <v>-0.25510563387813501</v>
       </c>
-      <c r="O68" s="54">
-        <f>N68</f>
+      <c r="O74" s="54">
+        <f>N74</f>
         <v>-0.25510563387813501</v>
       </c>
-      <c r="P68" s="59">
+      <c r="P74" s="59">
         <v>-0.25510563390000002</v>
       </c>
     </row>
-    <row r="69" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="L69" s="55">
+    <row r="75" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L75" s="55">
         <v>0.8125</v>
       </c>
-      <c r="M69" s="42" t="s">
+      <c r="M75" s="42" t="s">
         <v>114</v>
       </c>
-      <c r="N69" s="50">
+      <c r="N75" s="50">
         <v>1.0385379019832599</v>
       </c>
-      <c r="O69" s="54">
-        <f>N69</f>
+      <c r="O75" s="54">
+        <f>N75</f>
         <v>1.0385379019832599</v>
       </c>
-      <c r="P69" s="59">
+      <c r="P75" s="59">
         <v>-5.12238863404413E-3</v>
       </c>
     </row>
-    <row r="70" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="M70" s="42" t="s">
+    <row r="76" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M76" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="N70" s="50">
+      <c r="N76" s="50">
         <v>6.4193752642371704</v>
       </c>
-      <c r="O70" s="1">
-        <f>N70/100</f>
+      <c r="O76" s="1">
+        <f>N76/100</f>
         <v>6.4193752642371704E-2</v>
       </c>
-      <c r="P70" s="58">
+      <c r="P76" s="58">
         <v>1.2851248455257599E-4</v>
       </c>
     </row>
-    <row r="71" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="M71" s="42" t="s">
+    <row r="77" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M77" s="42" t="s">
         <v>124</v>
       </c>
-      <c r="N71" s="50">
+      <c r="N77" s="50">
         <v>1.57798981550307</v>
       </c>
-      <c r="O71" s="1">
-        <f t="shared" ref="O71:O79" si="8">N71/100</f>
+      <c r="O77" s="1">
+        <f t="shared" ref="O77:O85" si="8">N77/100</f>
         <v>1.5779898155030701E-2</v>
       </c>
-      <c r="P71" s="58">
+      <c r="P77" s="58">
         <v>1.0767413611616999E-3</v>
       </c>
     </row>
-    <row r="72" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="M72" s="42" t="s">
+    <row r="78" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M78" s="42" t="s">
         <v>57</v>
       </c>
-      <c r="N72" s="50">
+      <c r="N78" s="50">
         <v>7.6111237412808599</v>
       </c>
-      <c r="O72" s="1">
+      <c r="O78" s="1">
         <f t="shared" si="8"/>
         <v>7.6111237412808605E-2</v>
       </c>
-      <c r="P72" s="58">
+      <c r="P78" s="58">
         <v>1.6297137374082799E-5</v>
       </c>
     </row>
-    <row r="73" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="M73" s="42" t="s">
+    <row r="79" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M79" s="42" t="s">
         <v>123</v>
       </c>
-      <c r="N73" s="50">
+      <c r="N79" s="50">
         <v>2.2749299623984598</v>
       </c>
-      <c r="O73" s="1">
+      <c r="O79" s="1">
         <f t="shared" si="8"/>
         <v>2.2749299623984597E-2</v>
       </c>
-      <c r="P73" s="58">
+      <c r="P79" s="58">
         <v>9.80565804585901E-5</v>
       </c>
     </row>
-    <row r="74" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="M74" s="42" t="s">
+    <row r="80" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M80" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="N74" s="50">
+      <c r="N80" s="50">
         <v>17.236621109828601</v>
       </c>
-      <c r="O74" s="1">
+      <c r="O80" s="1">
         <f t="shared" si="8"/>
         <v>0.17236621109828601</v>
       </c>
-      <c r="P74" s="58">
+      <c r="P80" s="58">
         <v>2.8072391037720099E-5</v>
       </c>
     </row>
-    <row r="75" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="M75" s="42" t="s">
+    <row r="81" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M81" s="42" t="s">
         <v>125</v>
       </c>
-      <c r="N75" s="50">
+      <c r="N81" s="50">
         <v>6.2088690408799696</v>
       </c>
-      <c r="O75" s="1">
+      <c r="O81" s="1">
         <f t="shared" si="8"/>
         <v>6.2088690408799697E-2</v>
       </c>
-      <c r="P75" s="58">
+      <c r="P81" s="58">
         <v>3.8053003130694002E-4</v>
       </c>
     </row>
-    <row r="76" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="M76" s="42" t="s">
+    <row r="82" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M82" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="N76" s="50">
+      <c r="N82" s="50">
         <v>1.4392071686730901</v>
       </c>
-      <c r="O76" s="1">
+      <c r="O82" s="1">
         <f t="shared" si="8"/>
         <v>1.4392071686730901E-2</v>
       </c>
-      <c r="P76" s="58">
+      <c r="P82" s="58">
         <v>3.3901950999533699E-5</v>
       </c>
     </row>
-    <row r="77" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="M77" s="42" t="s">
+    <row r="83" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M83" s="42" t="s">
         <v>126</v>
       </c>
-      <c r="N77" s="50">
+      <c r="N83" s="50">
         <v>0.52526799870488805</v>
       </c>
-      <c r="O77" s="1">
+      <c r="O83" s="1">
         <f t="shared" si="8"/>
         <v>5.2526799870488807E-3</v>
       </c>
-      <c r="P77" s="58">
+      <c r="P83" s="58">
         <v>9.7871725652031802E-5</v>
       </c>
     </row>
-    <row r="78" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="M78" s="42" t="s">
+    <row r="84" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M84" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="N78" s="50">
+      <c r="N84" s="50">
         <v>-6.1</v>
       </c>
-      <c r="O78" s="1">
+      <c r="O84" s="1">
         <f t="shared" si="8"/>
         <v>-6.0999999999999999E-2</v>
       </c>
-      <c r="P78" s="58">
+      <c r="P84" s="58">
         <v>-5.5804864002167998E-6</v>
       </c>
     </row>
-    <row r="79" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="M79" s="42" t="s">
+    <row r="85" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M85" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="N79" s="50">
+      <c r="N85" s="50">
         <v>-1.6</v>
       </c>
-      <c r="O79" s="1">
+      <c r="O85" s="1">
         <f t="shared" si="8"/>
         <v>-1.6E-2</v>
       </c>
-      <c r="P79" s="58">
+      <c r="P85" s="58">
         <v>5.2797756594065403E-5</v>
       </c>
     </row>
-    <row r="80" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="L80" t="s">
+    <row r="86" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L86" t="s">
         <v>142</v>
       </c>
-      <c r="M80" s="42" t="s">
+      <c r="M86" s="42" t="s">
         <v>60</v>
       </c>
-      <c r="N80" s="50">
+      <c r="N86" s="50">
         <v>-0.26806990591321</v>
       </c>
-      <c r="O80" s="54">
-        <f>N80</f>
+      <c r="O86" s="54">
+        <f>N86</f>
         <v>-0.26806990591321</v>
       </c>
-      <c r="P80" s="59">
+      <c r="P86" s="59">
         <v>-0.26806990590000002</v>
       </c>
     </row>
-    <row r="81" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="L81" s="56" t="s">
+    <row r="87" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L87" s="56" t="s">
         <v>147</v>
       </c>
-      <c r="M81" s="42" t="s">
+      <c r="M87" s="42" t="s">
         <v>115</v>
       </c>
-      <c r="N81" s="50">
+      <c r="N87" s="50">
         <v>1.0349152577221601</v>
       </c>
-      <c r="O81" s="54">
-        <f>N81</f>
+      <c r="O87" s="54">
+        <f>N87</f>
         <v>1.0349152577221601</v>
       </c>
-      <c r="P81" s="59">
+      <c r="P87" s="59">
         <v>-2.1765958813597698E-3</v>
       </c>
     </row>
-    <row r="82" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="L82" s="47"/>
-      <c r="M82" s="42" t="s">
+    <row r="88" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L88" s="47"/>
+      <c r="M88" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="N82" s="50">
+      <c r="N88" s="50">
         <v>6.1481308294477897</v>
       </c>
-      <c r="O82" s="1">
-        <f>N82/100</f>
+      <c r="O88" s="1">
+        <f>N88/100</f>
         <v>6.1481308294477899E-2</v>
       </c>
-      <c r="P82" s="57">
+      <c r="P88" s="57">
         <v>-1.88116567434796E-5</v>
       </c>
     </row>
-    <row r="83" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="L83" s="47"/>
-      <c r="M83" s="42" t="s">
+    <row r="89" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L89" s="47"/>
+      <c r="M89" s="42" t="s">
         <v>127</v>
       </c>
-      <c r="N83" s="50">
+      <c r="N89" s="50">
         <v>6.1776975079165704</v>
       </c>
-      <c r="O83" s="1">
-        <f t="shared" ref="O83:O95" si="9">N83/100</f>
+      <c r="O89" s="1">
+        <f t="shared" ref="O89:O101" si="9">N89/100</f>
         <v>6.1776975079165707E-2</v>
       </c>
-      <c r="P83" s="57">
+      <c r="P89" s="57">
         <v>-4.4567340559324698E-4</v>
       </c>
     </row>
-    <row r="84" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="L84" s="47"/>
-      <c r="M84" s="42" t="s">
+    <row r="90" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L90" s="47"/>
+      <c r="M90" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="N84" s="50">
+      <c r="N90" s="50">
         <v>10.1258308263922</v>
       </c>
-      <c r="O84" s="1">
+      <c r="O90" s="1">
         <f t="shared" si="9"/>
         <v>0.101258308263922</v>
       </c>
-      <c r="P84" s="58">
+      <c r="P90" s="58">
         <v>-1.40656940313608E-4</v>
       </c>
     </row>
-    <row r="85" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="L85" s="47"/>
-      <c r="M85" s="42" t="s">
+    <row r="91" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L91" s="47"/>
+      <c r="M91" s="42" t="s">
         <v>128</v>
       </c>
-      <c r="N85" s="50">
+      <c r="N91" s="50">
         <v>4.8779939913553596</v>
       </c>
-      <c r="O85" s="1">
+      <c r="O91" s="1">
         <f t="shared" si="9"/>
         <v>4.8779939913553595E-2</v>
       </c>
-      <c r="P85" s="57">
+      <c r="P91" s="57">
         <v>-6.3339605935184401E-4</v>
       </c>
     </row>
-    <row r="86" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="L86" t="s">
+    <row r="92" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L92" t="s">
         <v>143</v>
       </c>
-      <c r="M86" s="42" t="s">
+      <c r="M92" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="N86" s="50">
+      <c r="N92" s="50">
         <v>-7.6</v>
       </c>
-      <c r="O86" s="1">
+      <c r="O92" s="1">
         <f t="shared" si="9"/>
         <v>-7.5999999999999998E-2</v>
       </c>
-      <c r="P86" s="58">
+      <c r="P92" s="58">
         <v>-1.4483820858600399E-4</v>
       </c>
     </row>
-    <row r="87" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="L87" s="56" t="s">
+    <row r="93" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L93" s="56" t="s">
         <v>148</v>
       </c>
-      <c r="M87" s="42" t="s">
+      <c r="M93" s="42" t="s">
         <v>129</v>
       </c>
-      <c r="N87" s="50">
+      <c r="N93" s="50">
         <v>-1.6</v>
       </c>
-      <c r="O87" s="1">
+      <c r="O93" s="1">
         <f t="shared" si="9"/>
         <v>-1.6E-2</v>
       </c>
-      <c r="P87" s="58">
+      <c r="P93" s="58">
         <v>-3.5573742834272E-3</v>
       </c>
     </row>
-    <row r="88" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="L88" t="s">
+    <row r="94" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L94" t="s">
         <v>144</v>
       </c>
-      <c r="M88" s="42" t="s">
+      <c r="M94" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="N88" s="51">
+      <c r="N94" s="51">
         <v>-63.001699846354903</v>
       </c>
-      <c r="O88" s="1">
+      <c r="O94" s="1">
         <f t="shared" si="9"/>
         <v>-0.63001699846354908</v>
       </c>
-      <c r="P88" s="58">
+      <c r="P94" s="58">
         <v>-9.5060452610995505E-4</v>
       </c>
     </row>
-    <row r="89" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="L89" s="56" t="s">
+    <row r="95" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L95" s="56" t="s">
         <v>149</v>
       </c>
-      <c r="M89" s="42" t="s">
+      <c r="M95" s="42" t="s">
         <v>130</v>
       </c>
-      <c r="N89" s="50">
+      <c r="N95" s="50">
         <v>10.2039485868599</v>
       </c>
-      <c r="O89" s="1">
+      <c r="O95" s="1">
         <f t="shared" si="9"/>
         <v>0.102039485868599</v>
       </c>
-      <c r="P89" s="58">
+      <c r="P95" s="58">
         <v>-5.1145973996759402E-3</v>
       </c>
     </row>
-    <row r="90" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="M90" s="42" t="s">
+    <row r="96" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M96" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="N90" s="50">
+      <c r="N96" s="50">
         <v>16.526211548050401</v>
       </c>
-      <c r="O90" s="1">
+      <c r="O96" s="1">
         <f t="shared" si="9"/>
         <v>0.16526211548050401</v>
       </c>
-      <c r="P90" s="58">
+      <c r="P96" s="58">
         <v>3.0418249791705498E-4</v>
       </c>
     </row>
-    <row r="91" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="M91" s="42" t="s">
+    <row r="97" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M97" s="42" t="s">
         <v>131</v>
       </c>
-      <c r="N91" s="52">
+      <c r="N97" s="52">
         <v>-1.34369314780613</v>
       </c>
-      <c r="O91" s="1">
+      <c r="O97" s="1">
         <f t="shared" si="9"/>
         <v>-1.34369314780613E-2</v>
       </c>
-      <c r="P91" s="58">
+      <c r="P97" s="58">
         <v>-1.37670401876801E-3</v>
       </c>
     </row>
-    <row r="92" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="M92" s="42" t="s">
+    <row r="98" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M98" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="N92" s="52">
+      <c r="N98" s="52">
         <v>29.247637436823101</v>
       </c>
-      <c r="O92" s="1">
+      <c r="O98" s="1">
         <f t="shared" si="9"/>
         <v>0.29247637436823104</v>
       </c>
-      <c r="P92" s="58">
+      <c r="P98" s="58">
         <v>2.2761940039589499E-4</v>
       </c>
     </row>
-    <row r="93" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="M93" s="42" t="s">
+    <row r="99" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M99" s="42" t="s">
         <v>132</v>
       </c>
-      <c r="N93" s="52">
+      <c r="N99" s="52">
         <v>11.0919776937066</v>
       </c>
-      <c r="O93" s="1">
+      <c r="O99" s="1">
         <f t="shared" si="9"/>
         <v>0.11091977693706599</v>
       </c>
-      <c r="P93" s="58">
+      <c r="P99" s="58">
         <v>-1.3983824680780001E-3</v>
       </c>
     </row>
-    <row r="94" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="M94" s="42" t="s">
+    <row r="100" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M100" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="N94" s="53">
+      <c r="N100" s="53">
         <v>-94.199996999999996</v>
       </c>
-      <c r="O94" s="1">
+      <c r="O100" s="1">
         <f t="shared" si="9"/>
         <v>-0.94199996999999991</v>
       </c>
-      <c r="P94" s="58">
+      <c r="P100" s="58">
         <v>-2.81965662445027E-3</v>
       </c>
     </row>
-    <row r="95" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="M95" s="42" t="s">
+    <row r="101" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M101" s="42" t="s">
         <v>133</v>
       </c>
-      <c r="N95">
+      <c r="N101">
         <f>21.4613437652587-19</f>
         <v>2.4613437652587002</v>
       </c>
-      <c r="O95" s="1">
+      <c r="O101" s="1">
         <f t="shared" si="9"/>
         <v>2.4613437652587004E-2</v>
       </c>
-      <c r="P95" s="58">
+      <c r="P101" s="58">
         <v>-6.8701998242329402E-3</v>
       </c>
     </row>
-    <row r="96" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="M96" s="42" t="s">
+    <row r="102" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M102" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="N96" s="52">
+      <c r="N102" s="52">
         <v>-0.22125272217770001</v>
       </c>
-      <c r="O96" s="54">
-        <f>N96</f>
+      <c r="O102" s="54">
+        <f>N102</f>
         <v>-0.22125272217770001</v>
       </c>
-      <c r="P96" s="59">
+      <c r="P102" s="59">
         <v>-0.2212527222</v>
       </c>
     </row>
-    <row r="97" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="M97" s="42" t="s">
+    <row r="103" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M103" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="N97" s="52">
+      <c r="N103" s="52">
         <v>1.0099999973080001</v>
       </c>
-      <c r="O97" s="54">
-        <f>N97</f>
+      <c r="O103" s="54">
+        <f>N103</f>
         <v>1.0099999973080001</v>
       </c>
-      <c r="P97" s="59">
+      <c r="P103" s="59">
         <v>2.17540256007367E-2</v>
       </c>
     </row>
-    <row r="98" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="L98" t="s">
+    <row r="104" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L104" t="s">
         <v>145</v>
       </c>
-      <c r="M98" s="42" t="s">
+      <c r="M104" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="N98" s="52">
+      <c r="N104" s="52">
         <v>4.9650161007164098</v>
       </c>
-      <c r="O98" s="1">
-        <f>N98/100</f>
+      <c r="O104" s="1">
+        <f>N104/100</f>
         <v>4.9650161007164101E-2</v>
       </c>
-      <c r="P98" s="58">
+      <c r="P104" s="58">
         <v>1.15284947015369E-4</v>
       </c>
     </row>
-    <row r="99" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="L99" s="56" t="s">
+    <row r="105" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L105" s="56" t="s">
         <v>150</v>
       </c>
-      <c r="M99" s="42" t="s">
+      <c r="M105" s="42" t="s">
         <v>134</v>
       </c>
-      <c r="N99" s="52">
+      <c r="N105" s="52">
         <v>0.52427629116916796</v>
       </c>
-      <c r="O99" s="1">
-        <f t="shared" ref="O99:O101" si="10">N99/100</f>
+      <c r="O105" s="1">
+        <f t="shared" ref="O105:O107" si="10">N105/100</f>
         <v>5.2427629116916794E-3</v>
       </c>
-      <c r="P99" s="58">
+      <c r="P105" s="58">
         <v>6.2348925580496799E-4</v>
       </c>
     </row>
-    <row r="100" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="M100" s="42" t="s">
+    <row r="106" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M106" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="N100" s="52">
+      <c r="N106" s="52">
         <v>-13.5</v>
       </c>
-      <c r="O100" s="1">
+      <c r="O106" s="1">
         <f t="shared" si="10"/>
         <v>-0.13500000000000001</v>
       </c>
-      <c r="P100" s="58">
+      <c r="P106" s="58">
         <v>-1.30914832287277E-5</v>
       </c>
     </row>
-    <row r="101" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="M101" s="42" t="s">
+    <row r="107" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M107" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="N101" s="52">
+      <c r="N107" s="52">
         <v>-5.8</v>
       </c>
-      <c r="O101" s="1">
+      <c r="O107" s="1">
         <f t="shared" si="10"/>
         <v>-5.7999999999999996E-2</v>
       </c>
-      <c r="P101" s="58">
+      <c r="P107" s="58">
         <v>1.15841086511394E-4</v>
       </c>
     </row>
-    <row r="102" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="M102" s="42" t="s">
+    <row r="108" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M108" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="N102" s="52">
+      <c r="N108" s="52">
         <v>-0.25510563387813501</v>
       </c>
-      <c r="O102" s="54">
-        <f>N102</f>
+      <c r="O108" s="54">
+        <f>N108</f>
         <v>-0.25510563387813501</v>
       </c>
-      <c r="P102" s="59">
+      <c r="P108" s="59">
         <v>-0.25510563390000002</v>
       </c>
     </row>
-    <row r="103" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="M103" s="42" t="s">
+    <row r="109" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M109" s="42" t="s">
         <v>114</v>
       </c>
-      <c r="N103" s="52">
+      <c r="N109" s="52">
         <v>1.0385379019832599</v>
       </c>
-      <c r="O103" s="54">
-        <f>N103</f>
+      <c r="O109" s="54">
+        <f>N109</f>
         <v>1.0385379019832599</v>
       </c>
-      <c r="P103" s="59">
+      <c r="P109" s="59">
         <v>-5.12238863404413E-3</v>
       </c>
     </row>
-    <row r="104" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="L104" t="s">
+    <row r="110" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L110" t="s">
         <v>146</v>
       </c>
-      <c r="M104" s="42" t="s">
+      <c r="M110" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="N104" s="52">
+      <c r="N110" s="52">
         <v>-2.8744036925517298</v>
       </c>
-      <c r="O104" s="1">
-        <f>N104/100</f>
+      <c r="O110" s="1">
+        <f>N110/100</f>
         <v>-2.8744036925517299E-2</v>
       </c>
-      <c r="P104" s="58">
+      <c r="P110" s="58">
         <v>-9.7142222335186394E-5</v>
       </c>
     </row>
-    <row r="105" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="L105" s="56" t="s">
+    <row r="111" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L111" s="56" t="s">
         <v>151</v>
       </c>
-      <c r="M105" s="42" t="s">
+      <c r="M111" s="42" t="s">
         <v>135</v>
       </c>
-      <c r="N105" s="52">
+      <c r="N111" s="52">
         <v>0.31779049296478201</v>
       </c>
-      <c r="O105" s="1">
-        <f t="shared" ref="O105:O107" si="11">N105/100</f>
+      <c r="O111" s="1">
+        <f t="shared" ref="O111:O113" si="11">N111/100</f>
         <v>3.1779049296478202E-3</v>
       </c>
-      <c r="P105" s="58">
+      <c r="P111" s="58">
         <v>-1.0332946463634299E-3</v>
       </c>
     </row>
-    <row r="106" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="M106" s="42" t="s">
+    <row r="112" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M112" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="N106" s="52">
+      <c r="N112" s="52">
         <v>-14.9</v>
       </c>
-      <c r="O106" s="1">
+      <c r="O112" s="1">
         <f t="shared" si="11"/>
         <v>-0.14899999999999999</v>
       </c>
-      <c r="P106" s="58">
+      <c r="P112" s="58">
         <v>-4.6294745534552998E-5</v>
       </c>
     </row>
-    <row r="107" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="M107" s="42" t="s">
+    <row r="113" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M113" s="42" t="s">
         <v>136</v>
       </c>
-      <c r="N107" s="52">
+      <c r="N113" s="52">
         <v>-5</v>
       </c>
-      <c r="O107" s="1">
+      <c r="O113" s="1">
         <f t="shared" si="11"/>
         <v>-0.05</v>
       </c>
-      <c r="P107" s="58">
+      <c r="P113" s="58">
         <v>-4.2582952991622499E-5</v>
       </c>
     </row>
-    <row r="108" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="M108" s="42" t="s">
+    <row r="114" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M114" s="42" t="s">
         <v>60</v>
       </c>
-      <c r="N108" s="52">
+      <c r="N114" s="52">
         <v>-0.26806990591321</v>
       </c>
-      <c r="O108" s="54">
-        <f>N108</f>
+      <c r="O114" s="54">
+        <f>N114</f>
         <v>-0.26806990591321</v>
       </c>
-      <c r="P108" s="59">
+      <c r="P114" s="59">
         <v>-0.26806990590000002</v>
       </c>
     </row>
-    <row r="109" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="M109" s="42" t="s">
+    <row r="115" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M115" s="42" t="s">
         <v>115</v>
       </c>
-      <c r="N109" s="52">
+      <c r="N115" s="52">
         <v>1.0349152577221601</v>
       </c>
-      <c r="O109" s="54">
-        <f>N109</f>
+      <c r="O115" s="54">
+        <f>N115</f>
         <v>1.0349152577221601</v>
       </c>
-      <c r="P109" s="59">
+      <c r="P115" s="59">
         <v>-2.1765958813597698E-3</v>
       </c>
     </row>
-    <row r="110" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="O110" s="1"/>
-      <c r="P110" s="3"/>
-    </row>
-    <row r="111" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="M111" s="48"/>
-      <c r="N111" s="48"/>
-      <c r="O111" s="1"/>
-      <c r="P111" s="3"/>
-    </row>
-    <row r="112" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="M112" s="48"/>
-      <c r="N112" s="47"/>
-      <c r="P112" s="3"/>
-    </row>
-    <row r="113" spans="13:16" x14ac:dyDescent="0.25">
-      <c r="M113" s="48"/>
-      <c r="N113" s="47"/>
-      <c r="P113" s="3"/>
-    </row>
-    <row r="114" spans="13:16" x14ac:dyDescent="0.25">
-      <c r="M114" s="48"/>
-      <c r="N114" s="47"/>
-    </row>
-    <row r="115" spans="13:16" x14ac:dyDescent="0.25">
-      <c r="M115" s="42"/>
-      <c r="N115" s="1"/>
-    </row>
     <row r="116" spans="13:16" x14ac:dyDescent="0.25">
-      <c r="M116" s="42"/>
-      <c r="N116" s="1"/>
+      <c r="O116" s="1"/>
+      <c r="P116" s="3"/>
     </row>
     <row r="117" spans="13:16" x14ac:dyDescent="0.25">
-      <c r="M117" s="42"/>
-      <c r="N117" s="1"/>
+      <c r="M117" s="48"/>
+      <c r="N117" s="48"/>
+      <c r="O117" s="1"/>
+      <c r="P117" s="3"/>
     </row>
     <row r="118" spans="13:16" x14ac:dyDescent="0.25">
-      <c r="M118" s="42"/>
-      <c r="N118" s="1"/>
+      <c r="M118" s="48"/>
+      <c r="N118" s="47"/>
+      <c r="P118" s="3"/>
     </row>
     <row r="119" spans="13:16" x14ac:dyDescent="0.25">
-      <c r="M119" s="42"/>
-      <c r="N119" s="1"/>
+      <c r="M119" s="48"/>
+      <c r="N119" s="47"/>
+      <c r="P119" s="3"/>
     </row>
     <row r="120" spans="13:16" x14ac:dyDescent="0.25">
-      <c r="M120" s="42"/>
-      <c r="N120" s="1"/>
+      <c r="M120" s="48"/>
+      <c r="N120" s="47"/>
     </row>
     <row r="121" spans="13:16" x14ac:dyDescent="0.25">
       <c r="M121" s="42"/>
@@ -8846,6 +9002,30 @@
     <row r="134" spans="13:14" x14ac:dyDescent="0.25">
       <c r="M134" s="42"/>
       <c r="N134" s="1"/>
+    </row>
+    <row r="135" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M135" s="42"/>
+      <c r="N135" s="1"/>
+    </row>
+    <row r="136" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M136" s="42"/>
+      <c r="N136" s="1"/>
+    </row>
+    <row r="137" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M137" s="42"/>
+      <c r="N137" s="1"/>
+    </row>
+    <row r="138" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M138" s="42"/>
+      <c r="N138" s="1"/>
+    </row>
+    <row r="139" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M139" s="42"/>
+      <c r="N139" s="1"/>
+    </row>
+    <row r="140" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M140" s="42"/>
+      <c r="N140" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -8877,18 +9057,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="82" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
-      <c r="F1" s="81"/>
-      <c r="G1" s="81"/>
-      <c r="H1" s="81"/>
-      <c r="I1" s="81"/>
-      <c r="J1" s="81"/>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
+      <c r="J1" s="82"/>
       <c r="L1" s="11" t="s">
         <v>1</v>
       </c>
@@ -8912,18 +9092,18 @@
       <c r="B2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="82" t="s">
+      <c r="C2" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="82"/>
-      <c r="E2" s="82"/>
-      <c r="F2" s="82"/>
-      <c r="G2" s="82" t="s">
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="83" t="s">
         <v>74</v>
       </c>
-      <c r="H2" s="82"/>
-      <c r="I2" s="82"/>
-      <c r="J2" s="82"/>
+      <c r="H2" s="83"/>
+      <c r="I2" s="83"/>
+      <c r="J2" s="83"/>
       <c r="L2" s="8" t="s">
         <v>41</v>
       </c>
@@ -9716,18 +9896,18 @@
       <c r="O33" s="1"/>
     </row>
     <row r="35" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="81" t="s">
+      <c r="A35" s="82" t="s">
         <v>78</v>
       </c>
-      <c r="B35" s="81"/>
-      <c r="C35" s="81"/>
-      <c r="D35" s="81"/>
-      <c r="E35" s="81"/>
-      <c r="F35" s="81"/>
-      <c r="G35" s="81"/>
-      <c r="H35" s="81"/>
-      <c r="I35" s="81"/>
-      <c r="J35" s="81"/>
+      <c r="B35" s="82"/>
+      <c r="C35" s="82"/>
+      <c r="D35" s="82"/>
+      <c r="E35" s="82"/>
+      <c r="F35" s="82"/>
+      <c r="G35" s="82"/>
+      <c r="H35" s="82"/>
+      <c r="I35" s="82"/>
+      <c r="J35" s="82"/>
       <c r="L35" s="11" t="s">
         <v>1</v>
       </c>
@@ -14563,8 +14743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q56"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="Q49" sqref="Q49"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O32" sqref="O32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16564,7 +16744,7 @@
   <dimension ref="A1:R47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Started adding new bus V measurements
Started adding in new measurements for bus voltages to make sure it's
not an observability issue
</commit_message>
<xml_diff>
--- a/DMASE - Test Results.xlsx
+++ b/DMASE - Test Results.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leilei\Documents\GitHub\D-MASE\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="18195" windowHeight="7740" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="2 Bus" sheetId="4" r:id="rId1"/>
@@ -17,7 +22,7 @@
     <sheet name="14 Bus ADMM H" sheetId="9" r:id="rId8"/>
     <sheet name="14 Bus h" sheetId="10" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -1004,6 +1009,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1016,9 +1024,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1028,6 +1033,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1076,7 +1084,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1111,7 +1119,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1336,15 +1344,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="81" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
       <c r="I1" s="6" t="s">
         <v>1</v>
       </c>
@@ -1595,15 +1603,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="80" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
+      <c r="A1" s="81" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
       <c r="I1" s="6" t="s">
         <v>1</v>
       </c>
@@ -1956,15 +1964,15 @@
       <c r="N11" s="1"/>
     </row>
     <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="81" t="s">
+      <c r="A12" s="82" t="s">
         <v>80</v>
       </c>
-      <c r="B12" s="81"/>
-      <c r="C12" s="81"/>
-      <c r="D12" s="81"/>
-      <c r="E12" s="81"/>
-      <c r="F12" s="81"/>
-      <c r="G12" s="81"/>
+      <c r="B12" s="82"/>
+      <c r="C12" s="82"/>
+      <c r="D12" s="82"/>
+      <c r="E12" s="82"/>
+      <c r="F12" s="82"/>
+      <c r="G12" s="82"/>
       <c r="I12" s="1"/>
       <c r="J12" s="6" t="s">
         <v>1</v>
@@ -2454,15 +2462,15 @@
       <c r="G31" s="1"/>
     </row>
     <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="81" t="s">
+      <c r="A32" s="82" t="s">
         <v>81</v>
       </c>
-      <c r="B32" s="81"/>
-      <c r="C32" s="81"/>
-      <c r="D32" s="81"/>
-      <c r="E32" s="81"/>
-      <c r="F32" s="81"/>
-      <c r="G32" s="81"/>
+      <c r="B32" s="82"/>
+      <c r="C32" s="82"/>
+      <c r="D32" s="82"/>
+      <c r="E32" s="82"/>
+      <c r="F32" s="82"/>
+      <c r="G32" s="82"/>
       <c r="I32" s="1"/>
       <c r="J32" s="6" t="s">
         <v>1</v>
@@ -2941,13 +2949,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="81" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
       <c r="G1" s="30" t="s">
         <v>100</v>
       </c>
@@ -2966,13 +2974,13 @@
       <c r="L1" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="P1" s="80" t="s">
+      <c r="P1" s="81" t="s">
         <v>106</v>
       </c>
-      <c r="Q1" s="80"/>
-      <c r="R1" s="80"/>
-      <c r="S1" s="80"/>
-      <c r="T1" s="80"/>
+      <c r="Q1" s="81"/>
+      <c r="R1" s="81"/>
+      <c r="S1" s="81"/>
+      <c r="T1" s="81"/>
       <c r="V1" s="30" t="s">
         <v>100</v>
       </c>
@@ -3507,12 +3515,12 @@
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="P10" s="80" t="s">
+      <c r="P10" s="81" t="s">
         <v>108</v>
       </c>
-      <c r="Q10" s="80"/>
-      <c r="R10" s="80"/>
-      <c r="S10" s="80"/>
+      <c r="Q10" s="81"/>
+      <c r="R10" s="81"/>
+      <c r="S10" s="81"/>
       <c r="T10" s="25"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
@@ -4528,12 +4536,12 @@
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A33" s="80" t="s">
+      <c r="A33" s="81" t="s">
         <v>102</v>
       </c>
-      <c r="B33" s="80"/>
-      <c r="C33" s="80"/>
-      <c r="D33" s="80"/>
+      <c r="B33" s="81"/>
+      <c r="C33" s="81"/>
+      <c r="D33" s="81"/>
       <c r="F33" s="30" t="s">
         <v>100</v>
       </c>
@@ -4911,12 +4919,12 @@
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A42" s="80" t="s">
+      <c r="A42" s="81" t="s">
         <v>104</v>
       </c>
-      <c r="B42" s="80"/>
-      <c r="C42" s="80"/>
-      <c r="D42" s="80"/>
+      <c r="B42" s="81"/>
+      <c r="C42" s="81"/>
+      <c r="D42" s="81"/>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
@@ -5415,15 +5423,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="82" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
-      <c r="F1" s="81"/>
-      <c r="G1" s="81"/>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
       <c r="I1" s="1"/>
       <c r="J1" s="4"/>
       <c r="L1" s="4" t="s">
@@ -6473,8 +6481,8 @@
   </sheetPr>
   <dimension ref="A1:R140"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="I10" workbookViewId="0">
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6490,18 +6498,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="83" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="83"/>
+      <c r="I1" s="83"/>
+      <c r="J1" s="83"/>
       <c r="K1" s="43"/>
       <c r="L1" s="60"/>
       <c r="M1" s="11" t="s">
@@ -6525,18 +6533,18 @@
       <c r="B2" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="83" t="s">
+      <c r="C2" s="84" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="83"/>
-      <c r="G2" s="83" t="s">
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84" t="s">
         <v>74</v>
       </c>
-      <c r="H2" s="83"/>
-      <c r="I2" s="83"/>
-      <c r="J2" s="83"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
       <c r="K2" s="4"/>
       <c r="L2" s="60" t="s">
         <v>139</v>
@@ -7704,7 +7712,7 @@
         <v>0.31779049296478201</v>
       </c>
       <c r="O45" s="1">
-        <f t="shared" ref="O45:O53" si="5">N45/100</f>
+        <f t="shared" ref="O45:O51" si="5">N45/100</f>
         <v>3.1779049296478202E-3</v>
       </c>
       <c r="P45" s="58"/>
@@ -7775,7 +7783,7 @@
       <c r="M48" s="79" t="s">
         <v>207</v>
       </c>
-      <c r="N48" s="84">
+      <c r="N48" s="80">
         <v>72.934574594694098</v>
       </c>
       <c r="O48" s="1">
@@ -7847,7 +7855,7 @@
       <c r="M51" s="79" t="s">
         <v>206</v>
       </c>
-      <c r="N51" s="84">
+      <c r="N51" s="80">
         <v>-2.12732489205733</v>
       </c>
       <c r="O51" s="1">
@@ -7871,7 +7879,7 @@
       <c r="M52" s="79" t="s">
         <v>209</v>
       </c>
-      <c r="N52" s="84">
+      <c r="N52" s="80">
         <v>1.04499995797579</v>
       </c>
       <c r="O52" s="1">
@@ -9057,18 +9065,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="83" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="83"/>
+      <c r="I1" s="83"/>
+      <c r="J1" s="83"/>
       <c r="L1" s="11" t="s">
         <v>1</v>
       </c>
@@ -9092,18 +9100,18 @@
       <c r="B2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="83" t="s">
+      <c r="C2" s="84" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="83"/>
-      <c r="G2" s="83" t="s">
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84" t="s">
         <v>74</v>
       </c>
-      <c r="H2" s="83"/>
-      <c r="I2" s="83"/>
-      <c r="J2" s="83"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
       <c r="L2" s="8" t="s">
         <v>41</v>
       </c>
@@ -9896,18 +9904,18 @@
       <c r="O33" s="1"/>
     </row>
     <row r="35" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="82" t="s">
+      <c r="A35" s="83" t="s">
         <v>78</v>
       </c>
-      <c r="B35" s="82"/>
-      <c r="C35" s="82"/>
-      <c r="D35" s="82"/>
-      <c r="E35" s="82"/>
-      <c r="F35" s="82"/>
-      <c r="G35" s="82"/>
-      <c r="H35" s="82"/>
-      <c r="I35" s="82"/>
-      <c r="J35" s="82"/>
+      <c r="B35" s="83"/>
+      <c r="C35" s="83"/>
+      <c r="D35" s="83"/>
+      <c r="E35" s="83"/>
+      <c r="F35" s="83"/>
+      <c r="G35" s="83"/>
+      <c r="H35" s="83"/>
+      <c r="I35" s="83"/>
+      <c r="J35" s="83"/>
       <c r="L35" s="11" t="s">
         <v>1</v>
       </c>
@@ -16743,8 +16751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N32" sqref="N32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Copied over bus V measurements from PowerWorld
Copied bus V measurements from PowerWorld via remote desktop
</commit_message>
<xml_diff>
--- a/DMASE - Test Results.xlsx
+++ b/DMASE - Test Results.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leilei\Documents\GitHub\D-MASE\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12240" windowHeight="9240" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="2 Bus" sheetId="4" r:id="rId1"/>
@@ -22,12 +17,12 @@
     <sheet name="14 Bus ADMM H" sheetId="9" r:id="rId8"/>
     <sheet name="14 Bus h" sheetId="10" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="212">
   <si>
     <t>Abur 3-Bus Case Measurements (run through SE, rerun new estimate again)</t>
   </si>
@@ -657,6 +652,12 @@
   </si>
   <si>
     <t xml:space="preserve">V2 </t>
+  </si>
+  <si>
+    <t>Bus Records</t>
+  </si>
+  <si>
+    <t>PU Volt</t>
   </si>
 </sst>
 </file>
@@ -1084,7 +1085,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1119,7 +1120,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -6481,8 +6482,8 @@
   </sheetPr>
   <dimension ref="A1:R140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I10" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+    <sheetView tabSelected="1" topLeftCell="H88" workbookViewId="0">
+      <selection activeCell="J90" sqref="J90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8371,7 +8372,7 @@
         <v>2.8072391037720099E-5</v>
       </c>
     </row>
-    <row r="81" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="81" spans="8:16" x14ac:dyDescent="0.25">
       <c r="M81" s="42" t="s">
         <v>125</v>
       </c>
@@ -8386,7 +8387,7 @@
         <v>3.8053003130694002E-4</v>
       </c>
     </row>
-    <row r="82" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="82" spans="8:16" x14ac:dyDescent="0.25">
       <c r="M82" s="42" t="s">
         <v>59</v>
       </c>
@@ -8401,7 +8402,7 @@
         <v>3.3901950999533699E-5</v>
       </c>
     </row>
-    <row r="83" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="83" spans="8:16" x14ac:dyDescent="0.25">
       <c r="M83" s="42" t="s">
         <v>126</v>
       </c>
@@ -8416,7 +8417,7 @@
         <v>9.7871725652031802E-5</v>
       </c>
     </row>
-    <row r="84" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="84" spans="8:16" x14ac:dyDescent="0.25">
       <c r="M84" s="42" t="s">
         <v>12</v>
       </c>
@@ -8431,7 +8432,7 @@
         <v>-5.5804864002167998E-6</v>
       </c>
     </row>
-    <row r="85" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="85" spans="8:16" x14ac:dyDescent="0.25">
       <c r="M85" s="42" t="s">
         <v>20</v>
       </c>
@@ -8446,7 +8447,7 @@
         <v>5.2797756594065403E-5</v>
       </c>
     </row>
-    <row r="86" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="86" spans="8:16" x14ac:dyDescent="0.25">
       <c r="L86" t="s">
         <v>142</v>
       </c>
@@ -8464,7 +8465,10 @@
         <v>-0.26806990590000002</v>
       </c>
     </row>
-    <row r="87" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="87" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="I87" s="72" t="s">
+        <v>210</v>
+      </c>
       <c r="L87" s="56" t="s">
         <v>147</v>
       </c>
@@ -8482,7 +8486,10 @@
         <v>-2.1765958813597698E-3</v>
       </c>
     </row>
-    <row r="88" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="88" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="I88" s="72" t="s">
+        <v>211</v>
+      </c>
       <c r="L88" s="47"/>
       <c r="M88" s="42" t="s">
         <v>61</v>
@@ -8498,7 +8505,13 @@
         <v>-1.88116567434796E-5</v>
       </c>
     </row>
-    <row r="89" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="89" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="H89">
+        <v>1</v>
+      </c>
+      <c r="I89" s="72">
+        <v>1.0599999427795399</v>
+      </c>
       <c r="L89" s="47"/>
       <c r="M89" s="42" t="s">
         <v>127</v>
@@ -8514,7 +8527,13 @@
         <v>-4.4567340559324698E-4</v>
       </c>
     </row>
-    <row r="90" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="90" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="H90">
+        <v>2</v>
+      </c>
+      <c r="I90" s="72">
+        <v>1.04499995797579</v>
+      </c>
       <c r="L90" s="47"/>
       <c r="M90" s="42" t="s">
         <v>62</v>
@@ -8530,7 +8549,13 @@
         <v>-1.40656940313608E-4</v>
       </c>
     </row>
-    <row r="91" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="91" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="H91">
+        <v>3</v>
+      </c>
+      <c r="I91" s="72">
+        <v>1.0099999973080001</v>
+      </c>
       <c r="L91" s="47"/>
       <c r="M91" s="42" t="s">
         <v>128</v>
@@ -8546,7 +8571,13 @@
         <v>-6.3339605935184401E-4</v>
       </c>
     </row>
-    <row r="92" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="92" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="H92">
+        <v>4</v>
+      </c>
+      <c r="I92" s="72">
+        <v>1.02371286456331</v>
+      </c>
       <c r="L92" t="s">
         <v>143</v>
       </c>
@@ -8564,7 +8595,13 @@
         <v>-1.4483820858600399E-4</v>
       </c>
     </row>
-    <row r="93" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="93" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="H93">
+        <v>5</v>
+      </c>
+      <c r="I93" s="72">
+        <v>1.0280925147905799</v>
+      </c>
       <c r="L93" s="56" t="s">
         <v>148</v>
       </c>
@@ -8582,7 +8619,13 @@
         <v>-3.5573742834272E-3</v>
       </c>
     </row>
-    <row r="94" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="94" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="H94">
+        <v>6</v>
+      </c>
+      <c r="I94" s="72">
+        <v>1.0385379019832599</v>
+      </c>
       <c r="L94" t="s">
         <v>144</v>
       </c>
@@ -8600,7 +8643,13 @@
         <v>-9.5060452610995505E-4</v>
       </c>
     </row>
-    <row r="95" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="95" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="H95">
+        <v>7</v>
+      </c>
+      <c r="I95" s="72">
+        <v>1.04612245201456</v>
+      </c>
       <c r="L95" s="56" t="s">
         <v>149</v>
       </c>
@@ -8618,7 +8667,13 @@
         <v>-5.1145973996759402E-3</v>
       </c>
     </row>
-    <row r="96" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="96" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="H96">
+        <v>8</v>
+      </c>
+      <c r="I96" s="72">
+        <v>1.0850835071553799</v>
+      </c>
       <c r="M96" s="42" t="s">
         <v>65</v>
       </c>
@@ -8633,7 +8688,13 @@
         <v>3.0418249791705498E-4</v>
       </c>
     </row>
-    <row r="97" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="97" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="H97">
+        <v>9</v>
+      </c>
+      <c r="I97" s="72">
+        <v>1.0349152577221601</v>
+      </c>
       <c r="M97" s="42" t="s">
         <v>131</v>
       </c>
@@ -8648,7 +8709,13 @@
         <v>-1.37670401876801E-3</v>
       </c>
     </row>
-    <row r="98" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="98" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="H98">
+        <v>10</v>
+      </c>
+      <c r="I98" s="72">
+        <v>1.02798621556374</v>
+      </c>
       <c r="M98" s="42" t="s">
         <v>66</v>
       </c>
@@ -8663,7 +8730,13 @@
         <v>2.2761940039589499E-4</v>
       </c>
     </row>
-    <row r="99" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="99" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="H99">
+        <v>11</v>
+      </c>
+      <c r="I99" s="72">
+        <v>1.02970205350408</v>
+      </c>
       <c r="M99" s="42" t="s">
         <v>132</v>
       </c>
@@ -8678,7 +8751,13 @@
         <v>-1.3983824680780001E-3</v>
       </c>
     </row>
-    <row r="100" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="100" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="H100">
+        <v>12</v>
+      </c>
+      <c r="I100" s="72">
+        <v>1.0240525230119499</v>
+      </c>
       <c r="M100" s="42" t="s">
         <v>67</v>
       </c>
@@ -8693,7 +8772,13 @@
         <v>-2.81965662445027E-3</v>
       </c>
     </row>
-    <row r="101" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="101" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="H101">
+        <v>13</v>
+      </c>
+      <c r="I101" s="72">
+        <v>1.01992383631813</v>
+      </c>
       <c r="M101" s="42" t="s">
         <v>133</v>
       </c>
@@ -8709,7 +8794,13 @@
         <v>-6.8701998242329402E-3</v>
       </c>
     </row>
-    <row r="102" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="102" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="H102">
+        <v>14</v>
+      </c>
+      <c r="I102" s="72">
+        <v>1.00994172446495</v>
+      </c>
       <c r="M102" s="42" t="s">
         <v>51</v>
       </c>
@@ -8724,7 +8815,7 @@
         <v>-0.2212527222</v>
       </c>
     </row>
-    <row r="103" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="103" spans="8:16" x14ac:dyDescent="0.25">
       <c r="M103" s="42" t="s">
         <v>27</v>
       </c>
@@ -8739,7 +8830,7 @@
         <v>2.17540256007367E-2</v>
       </c>
     </row>
-    <row r="104" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="104" spans="8:16" x14ac:dyDescent="0.25">
       <c r="L104" t="s">
         <v>145</v>
       </c>
@@ -8757,7 +8848,7 @@
         <v>1.15284947015369E-4</v>
       </c>
     </row>
-    <row r="105" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="105" spans="8:16" x14ac:dyDescent="0.25">
       <c r="L105" s="56" t="s">
         <v>150</v>
       </c>
@@ -8775,7 +8866,7 @@
         <v>6.2348925580496799E-4</v>
       </c>
     </row>
-    <row r="106" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="106" spans="8:16" x14ac:dyDescent="0.25">
       <c r="M106" s="42" t="s">
         <v>16</v>
       </c>
@@ -8790,7 +8881,7 @@
         <v>-1.30914832287277E-5</v>
       </c>
     </row>
-    <row r="107" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="107" spans="8:16" x14ac:dyDescent="0.25">
       <c r="M107" s="42" t="s">
         <v>22</v>
       </c>
@@ -8805,7 +8896,7 @@
         <v>1.15841086511394E-4</v>
       </c>
     </row>
-    <row r="108" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="108" spans="8:16" x14ac:dyDescent="0.25">
       <c r="M108" s="42" t="s">
         <v>55</v>
       </c>
@@ -8820,7 +8911,7 @@
         <v>-0.25510563390000002</v>
       </c>
     </row>
-    <row r="109" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="109" spans="8:16" x14ac:dyDescent="0.25">
       <c r="M109" s="42" t="s">
         <v>114</v>
       </c>
@@ -8835,7 +8926,7 @@
         <v>-5.12238863404413E-3</v>
       </c>
     </row>
-    <row r="110" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="110" spans="8:16" x14ac:dyDescent="0.25">
       <c r="L110" t="s">
         <v>146</v>
       </c>
@@ -8853,7 +8944,7 @@
         <v>-9.7142222335186394E-5</v>
       </c>
     </row>
-    <row r="111" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="111" spans="8:16" x14ac:dyDescent="0.25">
       <c r="L111" s="56" t="s">
         <v>151</v>
       </c>
@@ -8871,7 +8962,7 @@
         <v>-1.0332946463634299E-3</v>
       </c>
     </row>
-    <row r="112" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="112" spans="8:16" x14ac:dyDescent="0.25">
       <c r="M112" s="42" t="s">
         <v>70</v>
       </c>

</xml_diff>

<commit_message>
Added a bunch of bus V measurements, mostly to Partitions 1 and 2
Added a bunch of bus V measurements, mostly to Partitions 1 and 2, not
very many to Partitions 3 and 4. The difference between the ADMM
solution and the centralized solution is reasonably small for Partition
1 but large for Partitions 2-4. Should look at intermediate calculations
tomorrow. Also, global observability ~=> local observability.
</commit_message>
<xml_diff>
--- a/DMASE - Test Results.xlsx
+++ b/DMASE - Test Results.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leilei\Documents\GitHub\D-MASE\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12240" windowHeight="9240" activeTab="4"/>
   </bookViews>
@@ -17,12 +22,12 @@
     <sheet name="14 Bus ADMM H" sheetId="9" r:id="rId8"/>
     <sheet name="14 Bus h" sheetId="10" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="222">
   <si>
     <t>Abur 3-Bus Case Measurements (run through SE, rerun new estimate again)</t>
   </si>
@@ -372,9 +377,6 @@
     <t>V 9</t>
   </si>
   <si>
-    <t>PowerWorld IEEE 14-Bus Case (construct AC case, use ACPF results)</t>
-  </si>
-  <si>
     <t>Q1-2</t>
   </si>
   <si>
@@ -651,13 +653,46 @@
     <t>Q2-3</t>
   </si>
   <si>
-    <t xml:space="preserve">V2 </t>
-  </si>
-  <si>
     <t>Bus Records</t>
   </si>
   <si>
     <t>PU Volt</t>
+  </si>
+  <si>
+    <t>V5</t>
+  </si>
+  <si>
+    <t>V8</t>
+  </si>
+  <si>
+    <t>V12</t>
+  </si>
+  <si>
+    <t>V13</t>
+  </si>
+  <si>
+    <t>V10</t>
+  </si>
+  <si>
+    <t>V9</t>
+  </si>
+  <si>
+    <t>47:58</t>
+  </si>
+  <si>
+    <t>Partition 2</t>
+  </si>
+  <si>
+    <t>Partition 1</t>
+  </si>
+  <si>
+    <t>Partition 3</t>
+  </si>
+  <si>
+    <t>Partition 4</t>
+  </si>
+  <si>
+    <t>PowerWorld IEEE 14-Bus Case (construct AC case, use ACPF results) - Doesn't converge in 10 iterations</t>
   </si>
 </sst>
 </file>
@@ -837,7 +872,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1016,6 +1051,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1085,7 +1123,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1120,7 +1158,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1345,15 +1383,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="82" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
-      <c r="F1" s="81"/>
-      <c r="G1" s="81"/>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
       <c r="I1" s="6" t="s">
         <v>1</v>
       </c>
@@ -1604,15 +1642,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="81" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
-      <c r="F1" s="81"/>
-      <c r="G1" s="81"/>
+      <c r="A1" s="82" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
       <c r="I1" s="6" t="s">
         <v>1</v>
       </c>
@@ -1965,15 +2003,15 @@
       <c r="N11" s="1"/>
     </row>
     <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="82" t="s">
+      <c r="A12" s="83" t="s">
         <v>80</v>
       </c>
-      <c r="B12" s="82"/>
-      <c r="C12" s="82"/>
-      <c r="D12" s="82"/>
-      <c r="E12" s="82"/>
-      <c r="F12" s="82"/>
-      <c r="G12" s="82"/>
+      <c r="B12" s="83"/>
+      <c r="C12" s="83"/>
+      <c r="D12" s="83"/>
+      <c r="E12" s="83"/>
+      <c r="F12" s="83"/>
+      <c r="G12" s="83"/>
       <c r="I12" s="1"/>
       <c r="J12" s="6" t="s">
         <v>1</v>
@@ -2463,15 +2501,15 @@
       <c r="G31" s="1"/>
     </row>
     <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="82" t="s">
+      <c r="A32" s="83" t="s">
         <v>81</v>
       </c>
-      <c r="B32" s="82"/>
-      <c r="C32" s="82"/>
-      <c r="D32" s="82"/>
-      <c r="E32" s="82"/>
-      <c r="F32" s="82"/>
-      <c r="G32" s="82"/>
+      <c r="B32" s="83"/>
+      <c r="C32" s="83"/>
+      <c r="D32" s="83"/>
+      <c r="E32" s="83"/>
+      <c r="F32" s="83"/>
+      <c r="G32" s="83"/>
       <c r="I32" s="1"/>
       <c r="J32" s="6" t="s">
         <v>1</v>
@@ -2950,13 +2988,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="82" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
       <c r="G1" s="30" t="s">
         <v>100</v>
       </c>
@@ -2975,13 +3013,13 @@
       <c r="L1" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="P1" s="81" t="s">
+      <c r="P1" s="82" t="s">
         <v>106</v>
       </c>
-      <c r="Q1" s="81"/>
-      <c r="R1" s="81"/>
-      <c r="S1" s="81"/>
-      <c r="T1" s="81"/>
+      <c r="Q1" s="82"/>
+      <c r="R1" s="82"/>
+      <c r="S1" s="82"/>
+      <c r="T1" s="82"/>
       <c r="V1" s="30" t="s">
         <v>100</v>
       </c>
@@ -3516,12 +3554,12 @@
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="P10" s="81" t="s">
+      <c r="P10" s="82" t="s">
         <v>108</v>
       </c>
-      <c r="Q10" s="81"/>
-      <c r="R10" s="81"/>
-      <c r="S10" s="81"/>
+      <c r="Q10" s="82"/>
+      <c r="R10" s="82"/>
+      <c r="S10" s="82"/>
       <c r="T10" s="25"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
@@ -4537,12 +4575,12 @@
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A33" s="81" t="s">
+      <c r="A33" s="82" t="s">
         <v>102</v>
       </c>
-      <c r="B33" s="81"/>
-      <c r="C33" s="81"/>
-      <c r="D33" s="81"/>
+      <c r="B33" s="82"/>
+      <c r="C33" s="82"/>
+      <c r="D33" s="82"/>
       <c r="F33" s="30" t="s">
         <v>100</v>
       </c>
@@ -4920,12 +4958,12 @@
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A42" s="81" t="s">
+      <c r="A42" s="82" t="s">
         <v>104</v>
       </c>
-      <c r="B42" s="81"/>
-      <c r="C42" s="81"/>
-      <c r="D42" s="81"/>
+      <c r="B42" s="82"/>
+      <c r="C42" s="82"/>
+      <c r="D42" s="82"/>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
@@ -5424,28 +5462,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="83" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
       <c r="I1" s="1"/>
       <c r="J1" s="4"/>
       <c r="L1" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="O1" t="s">
+        <v>181</v>
+      </c>
+      <c r="S1" t="s">
         <v>182</v>
       </c>
-      <c r="S1" t="s">
-        <v>183</v>
-      </c>
       <c r="V1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
@@ -5796,7 +5834,7 @@
       <c r="I9" s="1"/>
       <c r="J9" s="62"/>
       <c r="K9" s="65" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L9" s="4" t="s">
         <v>100</v>
@@ -6217,7 +6255,7 @@
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="K22" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="L22" s="5">
         <v>10</v>
@@ -6235,7 +6273,7 @@
         <v>0</v>
       </c>
       <c r="R22" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="S22">
         <v>10.487569561048501</v>
@@ -6480,10 +6518,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R140"/>
+  <dimension ref="A1:R146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H88" workbookViewId="0">
-      <selection activeCell="J90" sqref="J90"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6499,18 +6537,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="83" t="s">
-        <v>116</v>
-      </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="83"/>
-      <c r="G1" s="83"/>
-      <c r="H1" s="83"/>
-      <c r="I1" s="83"/>
-      <c r="J1" s="83"/>
+      <c r="A1" s="84" t="s">
+        <v>221</v>
+      </c>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
       <c r="K1" s="43"/>
       <c r="L1" s="60"/>
       <c r="M1" s="11" t="s">
@@ -6520,10 +6558,10 @@
         <v>29</v>
       </c>
       <c r="O1" s="11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="P1" s="11" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="R1" s="18" t="s">
         <v>35</v>
@@ -6534,21 +6572,21 @@
       <c r="B2" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="84" t="s">
+      <c r="C2" s="85" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84" t="s">
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85" t="s">
         <v>74</v>
       </c>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
       <c r="K2" s="4"/>
       <c r="L2" s="60" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="M2" s="46" t="s">
         <v>46</v>
@@ -6594,10 +6632,10 @@
       </c>
       <c r="K3" s="4"/>
       <c r="L3" s="60" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="M3" s="46" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="N3" s="50">
         <v>-20.300935880694301</v>
@@ -6608,7 +6646,7 @@
       </c>
       <c r="P3" s="58"/>
       <c r="R3" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -6616,15 +6654,17 @@
         <v>84</v>
       </c>
       <c r="B4" s="1">
-        <v>1.0599621403577</v>
+        <v>1.05999768165375</v>
       </c>
       <c r="C4" s="72">
-        <v>1.06046091821972</v>
+        <v>1.0594758722195099</v>
       </c>
       <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
+      <c r="G4" s="1">
+        <f>B4-C4</f>
+        <v>5.2180943424007253E-4</v>
+      </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -6647,24 +6687,29 @@
         <v>85</v>
       </c>
       <c r="B5" s="1">
-        <v>1.04103609065253</v>
+        <v>1.0410720611633699</v>
       </c>
       <c r="C5" s="72">
-        <v>1.0415317204627199</v>
+        <v>1.04054088963373</v>
       </c>
       <c r="D5" s="1">
-        <v>1.0387512194945701</v>
-      </c>
-      <c r="E5" s="1"/>
+        <v>1.03872090033057</v>
+      </c>
       <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
+      <c r="G5" s="1">
+        <f t="shared" ref="G5:G30" si="1">B5-C5</f>
+        <v>5.3117152963988445E-4</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" ref="H5:H30" si="2">B5-D5</f>
+        <v>2.3511608327999589E-3</v>
+      </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="60"/>
       <c r="M5" s="46" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N5" s="50">
         <v>-0.155506560051652</v>
@@ -6680,15 +6725,17 @@
         <v>86</v>
       </c>
       <c r="B6" s="1">
-        <v>0.98533801740076798</v>
+        <v>0.98537777124357495</v>
       </c>
       <c r="D6" s="1">
-        <v>0.97941761721577303</v>
-      </c>
-      <c r="E6" s="1"/>
+        <v>0.97983761929261803</v>
+      </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
+      <c r="H6" s="1">
+        <f t="shared" si="2"/>
+        <v>5.5401519509569175E-3</v>
+      </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
@@ -6707,27 +6754,32 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B7" s="1">
-        <v>1.00691238196979</v>
+        <v>1.00695008061588</v>
       </c>
       <c r="C7" s="72">
-        <v>1.0045255871869501</v>
+        <v>1.0064523876518101</v>
       </c>
       <c r="D7" s="1">
-        <v>1.00185731587878</v>
-      </c>
-      <c r="E7" s="1"/>
+        <v>1.00234717655369</v>
+      </c>
       <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
+      <c r="G7" s="1">
+        <f t="shared" si="1"/>
+        <v>4.9769296406987351E-4</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" si="2"/>
+        <v>4.6029040621899941E-3</v>
+      </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="60"/>
       <c r="M7" s="46" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="N7" s="50">
         <v>-3.8398609004379098</v>
@@ -6740,21 +6792,26 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B8" s="1">
-        <v>1.01577582353094</v>
+        <v>1.01581292033021</v>
       </c>
       <c r="C8" s="72">
-        <v>1.01639383512379</v>
+        <v>1.01530256145714</v>
       </c>
       <c r="D8" s="1">
-        <v>1.0114151980721</v>
-      </c>
-      <c r="E8" s="1"/>
+        <v>1.0118429049491899</v>
+      </c>
       <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
+      <c r="G8" s="1">
+        <f t="shared" si="1"/>
+        <v>5.1035887306993821E-4</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" si="2"/>
+        <v>3.9700153810200423E-3</v>
+      </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -6773,21 +6830,27 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B9" s="1">
-        <v>1.0048890478609001</v>
+        <v>1.0049243733889699</v>
       </c>
       <c r="C9" s="72">
-        <v>1.0130086495044099</v>
+        <v>1.0043986845670301</v>
       </c>
       <c r="E9" s="1">
-        <v>1.0219150296964401</v>
+        <v>1.0211400459242399</v>
       </c>
       <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+      <c r="G9" s="1">
+        <f t="shared" si="1"/>
+        <v>5.2568882193981814E-4</v>
+      </c>
       <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
+      <c r="I9" s="1">
+        <f>B9-E9</f>
+        <v>-1.6215672535270009E-2</v>
+      </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="60"/>
@@ -6805,22 +6868,25 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B10" s="1">
-        <v>1.0165083916826201</v>
+        <v>1.01654592268694</v>
       </c>
       <c r="D10" s="72">
-        <v>1.0095485374987301</v>
+        <v>1.0104617162685099</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
+      <c r="H10" s="1">
+        <f t="shared" si="2"/>
+        <v>6.0842064184301048E-3</v>
+      </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="60" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M10" s="46" t="s">
         <v>52</v>
@@ -6836,52 +6902,61 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B11" s="1">
-        <v>1.05436901591651</v>
-      </c>
-      <c r="D11" s="1">
-        <v>1.04711714761956</v>
+        <v>1.0544057013008099</v>
+      </c>
+      <c r="D11" s="72">
+        <v>1.0481605437678101</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
+      <c r="H11" s="1">
+        <f t="shared" si="2"/>
+        <v>6.2451575329998121E-3</v>
+      </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="60" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M11" s="46" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="N11" s="50">
         <v>0.96859150246414105</v>
       </c>
       <c r="O11" s="1">
-        <f t="shared" ref="O11:O15" si="1">N11/100</f>
+        <f t="shared" ref="O11:O15" si="3">N11/100</f>
         <v>9.6859150246414102E-3</v>
       </c>
       <c r="P11" s="58"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B12" s="1">
-        <v>0.99791127060776097</v>
+        <v>0.99794960680741096</v>
       </c>
       <c r="D12" s="1">
-        <v>0.99022778494432395</v>
+        <v>0.991234454626438</v>
       </c>
       <c r="F12" s="1">
-        <v>1.01864336835583</v>
+        <v>1.01906777725339</v>
       </c>
       <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
+      <c r="H12" s="1">
+        <f t="shared" si="2"/>
+        <v>6.7151521809729608E-3</v>
+      </c>
       <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
+      <c r="J12" s="1">
+        <f>B12-F12</f>
+        <v>-2.1118170445979079E-2</v>
+      </c>
       <c r="K12" s="1"/>
       <c r="L12" s="60"/>
       <c r="M12" s="46" t="s">
@@ -6891,57 +6966,66 @@
         <v>29.247688021076399</v>
       </c>
       <c r="O12" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.29247688021076401</v>
       </c>
       <c r="P12" s="58"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B13" s="1">
-        <v>0.99039833975510105</v>
+        <v>0.990436803259924</v>
       </c>
       <c r="F13" s="1">
-        <v>1.0112197070817699</v>
+        <v>1.01168045459334</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
+      <c r="J13" s="1">
+        <f t="shared" ref="J13:J30" si="4">B13-F13</f>
+        <v>-2.1243651333415992E-2</v>
+      </c>
       <c r="K13" s="1"/>
       <c r="L13" s="60"/>
       <c r="M13" s="46" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="N13" s="50">
         <v>-10.134384235994199</v>
       </c>
       <c r="O13" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-0.101343842359942</v>
       </c>
       <c r="P13" s="58"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B14" s="1">
-        <v>0.99354407863493799</v>
+        <v>0.99358117274512303</v>
       </c>
       <c r="C14" s="1"/>
-      <c r="E14" s="72">
-        <v>1.01121442717815</v>
+      <c r="E14" s="1">
+        <v>1.01040246678996</v>
       </c>
       <c r="F14" s="1">
-        <v>1.0139243260461199</v>
+        <v>1.0143603439878</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
+      <c r="I14" s="1">
+        <f t="shared" ref="I10:I30" si="5">B14-E14</f>
+        <v>-1.682129404483701E-2</v>
+      </c>
+      <c r="J14" s="1">
+        <f t="shared" si="4"/>
+        <v>-2.0779171242676919E-2</v>
+      </c>
       <c r="K14" s="1"/>
       <c r="L14" s="60"/>
       <c r="M14" s="46" t="s">
@@ -6951,61 +7035,70 @@
         <v>4.9388912162000001E-5</v>
       </c>
       <c r="O14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4.9388912162000003E-7</v>
       </c>
       <c r="P14" s="58"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B15" s="1">
-        <v>0.98670699585233201</v>
+        <v>0.98674259047048396</v>
       </c>
       <c r="C15" s="1"/>
-      <c r="E15" s="72">
-        <v>1.0045674174936901</v>
+      <c r="E15" s="1">
+        <v>1.00379748711045</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
+      <c r="I15" s="1">
+        <f t="shared" si="5"/>
+        <v>-1.7054896639966066E-2</v>
+      </c>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="60"/>
       <c r="M15" s="46" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="N15" s="50">
         <v>-23.1382548362844</v>
       </c>
       <c r="O15" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-0.231382548362844</v>
       </c>
       <c r="P15" s="58"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B16" s="1">
-        <v>0.98227711504043203</v>
+        <v>0.98231334549872895</v>
       </c>
       <c r="C16" s="1"/>
-      <c r="E16" s="72">
-        <v>1.00023502466276</v>
+      <c r="E16" s="1">
+        <v>0.99944316216807905</v>
       </c>
       <c r="F16" s="72">
-        <v>1.0031611566719001</v>
+        <v>1.00355759692244</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
+      <c r="I16" s="1">
+        <f t="shared" si="5"/>
+        <v>-1.7129816669350095E-2</v>
+      </c>
+      <c r="J16" s="1">
+        <f t="shared" si="4"/>
+        <v>-2.1244251423711003E-2</v>
+      </c>
       <c r="K16" s="1"/>
       <c r="L16" s="60" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="M16" s="46" t="s">
         <v>56</v>
@@ -7021,34 +7114,40 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B17" s="1">
-        <v>0.96821859389559195</v>
+        <v>0.96825697606458705</v>
       </c>
       <c r="C17" s="1"/>
-      <c r="E17" s="72">
-        <v>0.98715606381157694</v>
-      </c>
-      <c r="F17" s="1">
-        <v>0.99019975062743504</v>
+      <c r="E17" s="1">
+        <v>0.986336641110657</v>
+      </c>
+      <c r="F17" s="72">
+        <v>0.99068950600852101</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
+      <c r="I17" s="1">
+        <f t="shared" si="5"/>
+        <v>-1.8079665046069948E-2</v>
+      </c>
+      <c r="J17" s="1">
+        <f t="shared" si="4"/>
+        <v>-2.2432529943933965E-2</v>
+      </c>
       <c r="K17" s="1"/>
       <c r="L17" s="60" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="M17" s="46" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="N17" s="50">
         <v>1.57798981550307</v>
       </c>
       <c r="O17" s="1">
-        <f t="shared" ref="O17:O25" si="2">N17/100</f>
+        <f t="shared" ref="O17:O25" si="6">N17/100</f>
         <v>1.5779898155030701E-2</v>
       </c>
       <c r="P17" s="58"/>
@@ -7057,15 +7156,25 @@
       <c r="A18" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B18">
-        <v>-9.0498906725745204E-2</v>
+      <c r="B18" s="72">
+        <v>-9.0495834798616795E-2</v>
       </c>
       <c r="C18" s="72">
-        <v>-9.0453056678055102E-2</v>
+        <v>-9.0540985536805701E-2</v>
       </c>
       <c r="D18" s="1">
-        <v>-0.11705687930061399</v>
-      </c>
+        <v>-0.114895605675454</v>
+      </c>
+      <c r="G18" s="1">
+        <f t="shared" si="1"/>
+        <v>4.5150738188906581E-5</v>
+      </c>
+      <c r="H18" s="1">
+        <f t="shared" si="2"/>
+        <v>2.4399770876837201E-2</v>
+      </c>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
       <c r="L18" s="60"/>
       <c r="M18" s="46" t="s">
         <v>57</v>
@@ -7074,7 +7183,7 @@
         <v>7.6111237412808599</v>
       </c>
       <c r="O18" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>7.6111237412808605E-2</v>
       </c>
       <c r="P18" s="58"/>
@@ -7083,38 +7192,55 @@
       <c r="A19" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B19">
-        <v>-0.22165365184591099</v>
-      </c>
-      <c r="D19" s="1">
-        <v>-0.24696856648182799</v>
-      </c>
+      <c r="B19" s="72">
+        <v>-0.22164655627270699</v>
+      </c>
+      <c r="D19" s="72">
+        <v>-0.24495373472907001</v>
+      </c>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1">
+        <f t="shared" si="2"/>
+        <v>2.3307178456363015E-2</v>
+      </c>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
       <c r="L19" s="60"/>
       <c r="M19" s="46" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="N19" s="50">
         <v>2.2749299623984598</v>
       </c>
       <c r="O19" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>2.2749299623984597E-2</v>
       </c>
       <c r="P19" s="58"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="B20">
-        <v>-0.184493248459114</v>
-      </c>
-      <c r="C20" s="1">
-        <v>-0.18973189157605599</v>
-      </c>
-      <c r="D20" s="1">
-        <v>-0.210271602561001</v>
-      </c>
+        <v>162</v>
+      </c>
+      <c r="B20" s="72">
+        <v>-0.18448701889772101</v>
+      </c>
+      <c r="C20" s="72">
+        <v>-0.18457225505352301</v>
+      </c>
+      <c r="D20" s="72">
+        <v>-0.20824399700225299</v>
+      </c>
+      <c r="G20" s="1">
+        <f t="shared" si="1"/>
+        <v>8.5236155801998725E-5</v>
+      </c>
+      <c r="H20" s="1">
+        <f t="shared" si="2"/>
+        <v>2.3756978104531978E-2</v>
+      </c>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
       <c r="L20" s="60"/>
       <c r="M20" s="46" t="s">
         <v>58</v>
@@ -7123,50 +7249,70 @@
         <v>17.236621109828601</v>
       </c>
       <c r="O20" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.17236621109828601</v>
       </c>
       <c r="P20" s="58"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="B21">
-        <v>-0.15841659033345201</v>
-      </c>
-      <c r="C21" s="1">
-        <v>-0.158348436134123</v>
-      </c>
-      <c r="D21" s="1">
-        <v>-0.184378898266429</v>
-      </c>
+        <v>163</v>
+      </c>
+      <c r="B21" s="72">
+        <v>-0.158411156268046</v>
+      </c>
+      <c r="C21" s="72">
+        <v>-0.15848142142271501</v>
+      </c>
+      <c r="D21" s="72">
+        <v>-0.18233334454932901</v>
+      </c>
+      <c r="G21" s="1">
+        <f t="shared" si="1"/>
+        <v>7.0265154669013619E-5</v>
+      </c>
+      <c r="H21" s="1">
+        <f t="shared" si="2"/>
+        <v>2.3922188281283008E-2</v>
+      </c>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
       <c r="L21" s="60"/>
       <c r="M21" s="46" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="N21" s="50">
         <v>6.2088690408799696</v>
       </c>
       <c r="O21" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>6.2088690408799697E-2</v>
       </c>
       <c r="P21" s="58"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="B22">
-        <v>-0.262083078069408</v>
-      </c>
-      <c r="C22" s="1">
-        <v>-0.227788998176361</v>
+        <v>164</v>
+      </c>
+      <c r="B22" s="72">
+        <v>-0.26207372353015002</v>
+      </c>
+      <c r="C22" s="72">
+        <v>-0.26216969055655398</v>
       </c>
       <c r="E22" s="1">
-        <v>-0.18643976635270701</v>
-      </c>
+        <v>-0.19034602137735601</v>
+      </c>
+      <c r="G22" s="1">
+        <f t="shared" si="1"/>
+        <v>9.5967026403964706E-5</v>
+      </c>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1">
+        <f t="shared" si="5"/>
+        <v>-7.1727702152794004E-2</v>
+      </c>
+      <c r="J22" s="1"/>
       <c r="L22" s="60"/>
       <c r="M22" s="46" t="s">
         <v>59</v>
@@ -7175,44 +7321,58 @@
         <v>1.4392071686730901</v>
       </c>
       <c r="O22" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1.4392071686730901E-2</v>
       </c>
       <c r="P22" s="58"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="B23">
-        <v>-0.24699463946439601</v>
-      </c>
-      <c r="D23" s="1">
-        <v>-0.27303668219411098</v>
-      </c>
+        <v>165</v>
+      </c>
+      <c r="B23" s="72">
+        <v>-0.246986077730002</v>
+      </c>
+      <c r="D23" s="72">
+        <v>-0.27106672253693198</v>
+      </c>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1">
+        <f t="shared" si="2"/>
+        <v>2.4080644806929979E-2</v>
+      </c>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
       <c r="L23" s="60"/>
       <c r="M23" s="46" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="N23" s="50">
         <v>0.52526799870488805</v>
       </c>
       <c r="O23" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>5.2526799870488807E-3</v>
       </c>
       <c r="P23" s="58"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="B24">
-        <v>-0.25619422730604202</v>
-      </c>
-      <c r="D24" s="1">
-        <v>-0.28320201674479101</v>
-      </c>
+        <v>166</v>
+      </c>
+      <c r="B24" s="72">
+        <v>-0.25618480157818402</v>
+      </c>
+      <c r="D24" s="72">
+        <v>-0.28118399233407798</v>
+      </c>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1">
+        <f t="shared" si="2"/>
+        <v>2.4999190755893963E-2</v>
+      </c>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
       <c r="L24" s="60"/>
       <c r="M24" s="46" t="s">
         <v>12</v>
@@ -7221,23 +7381,33 @@
         <v>-6.1</v>
       </c>
       <c r="O24" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-6.0999999999999999E-2</v>
       </c>
       <c r="P24" s="58"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B25">
-        <v>-0.274128496301564</v>
-      </c>
-      <c r="D25" s="72">
-        <v>-0.29974357866110901</v>
+        <v>167</v>
+      </c>
+      <c r="B25" s="72">
+        <v>-0.27411931344698798</v>
+      </c>
+      <c r="D25" s="1">
+        <v>-0.29781202630382703</v>
       </c>
       <c r="F25" s="1">
-        <v>-0.18536451528078199</v>
+        <v>-0.18023948589966499</v>
+      </c>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1">
+        <f t="shared" si="2"/>
+        <v>2.3692712856839049E-2</v>
+      </c>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1">
+        <f t="shared" si="4"/>
+        <v>-9.3879827547322992E-2</v>
       </c>
       <c r="L25" s="60"/>
       <c r="M25" s="46" t="s">
@@ -7247,23 +7417,30 @@
         <v>-1.6</v>
       </c>
       <c r="O25" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-1.6E-2</v>
       </c>
       <c r="P25" s="58"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="B26">
-        <v>-0.27530156310841902</v>
+        <v>168</v>
+      </c>
+      <c r="B26" s="72">
+        <v>-0.27529246082033898</v>
       </c>
       <c r="F26" s="72">
-        <v>-0.18719102288282999</v>
+        <v>-0.182108887845847</v>
+      </c>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1">
+        <f t="shared" si="4"/>
+        <v>-9.3183572974491979E-2</v>
       </c>
       <c r="L26" s="60" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="M26" s="46" t="s">
         <v>61</v>
@@ -7279,42 +7456,59 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="B27">
-        <v>-0.27033852619593501</v>
-      </c>
-      <c r="E27" s="1">
-        <v>-0.19551994317777699</v>
+        <v>169</v>
+      </c>
+      <c r="B27" s="72">
+        <v>-0.27032933293769501</v>
+      </c>
+      <c r="E27" s="72">
+        <v>-0.19938713356909199</v>
       </c>
       <c r="F27" s="72">
-        <v>-0.18196005016786601</v>
+        <v>-0.176862385318663</v>
+      </c>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1">
+        <f t="shared" si="5"/>
+        <v>-7.0942199368603021E-2</v>
+      </c>
+      <c r="J27" s="1">
+        <f t="shared" si="4"/>
+        <v>-9.3466947619032015E-2</v>
       </c>
       <c r="L27" s="56" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M27" s="46" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="N27" s="50">
         <v>6.1776975079165704</v>
       </c>
       <c r="O27" s="1">
-        <f t="shared" ref="O27:O39" si="3">N27/100</f>
+        <f t="shared" ref="O27:O39" si="7">N27/100</f>
         <v>6.1776975079165707E-2</v>
       </c>
       <c r="P27" s="57"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="B28">
-        <v>-0.27393942115060799</v>
-      </c>
-      <c r="E28" s="1">
-        <v>-0.19960947382823699</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="B28" s="72">
+        <v>-0.27392983143629202</v>
+      </c>
+      <c r="E28" s="72">
+        <v>-0.20346909670597699</v>
+      </c>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1">
+        <f t="shared" si="5"/>
+        <v>-7.0460734730315028E-2</v>
+      </c>
+      <c r="J28" s="1"/>
       <c r="L28" s="61"/>
       <c r="M28" s="46" t="s">
         <v>62</v>
@@ -7323,52 +7517,72 @@
         <v>10.1258308263922</v>
       </c>
       <c r="O28" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0.101258308263922</v>
       </c>
       <c r="P28" s="58"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="B29">
-        <v>-0.274447646882094</v>
-      </c>
-      <c r="E29" s="1">
-        <v>-0.20045288832859101</v>
+        <v>171</v>
+      </c>
+      <c r="B29" s="72">
+        <v>-0.27443829599560998</v>
+      </c>
+      <c r="E29" s="72">
+        <v>-0.20428985760073801</v>
       </c>
       <c r="F29" s="72">
-        <v>-0.18699857554614599</v>
+        <v>-0.18192834943927999</v>
+      </c>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1">
+        <f t="shared" si="5"/>
+        <v>-7.0148438394871976E-2</v>
+      </c>
+      <c r="J29" s="1">
+        <f t="shared" si="4"/>
+        <v>-9.2509946556329992E-2</v>
       </c>
       <c r="L29" s="61"/>
       <c r="M29" s="46" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N29" s="50">
         <v>4.8779939913553596</v>
       </c>
       <c r="O29" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>4.8779939913553595E-2</v>
       </c>
       <c r="P29" s="57"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="B30">
-        <v>-0.28719972332980598</v>
+        <v>172</v>
+      </c>
+      <c r="B30" s="72">
+        <v>-0.287190454321613</v>
       </c>
       <c r="E30" s="72">
-        <v>-0.214195311803524</v>
+        <v>-0.21798641515405301</v>
       </c>
       <c r="F30" s="72">
-        <v>-0.200990701503165</v>
+        <v>-0.196013663332814</v>
+      </c>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1">
+        <f t="shared" si="5"/>
+        <v>-6.9204039167559989E-2</v>
+      </c>
+      <c r="J30" s="1">
+        <f t="shared" si="4"/>
+        <v>-9.1176790988798995E-2</v>
       </c>
       <c r="L30" s="60" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M30" s="46" t="s">
         <v>63</v>
@@ -7377,30 +7591,30 @@
         <v>-7.6</v>
       </c>
       <c r="O30" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-7.5999999999999998E-2</v>
       </c>
       <c r="P30" s="58"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="L31" s="56" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M31" s="46" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N31" s="50">
         <v>-1.6</v>
       </c>
       <c r="O31" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-1.6E-2</v>
       </c>
       <c r="P31" s="58"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="L32" s="60" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="M32" s="46" t="s">
         <v>64</v>
@@ -7409,23 +7623,23 @@
         <v>-63.001699846354903</v>
       </c>
       <c r="O32" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-0.63001699846354908</v>
       </c>
       <c r="P32" s="58"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="L33" s="56" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M33" s="46" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N33" s="50">
         <v>10.2039485868599</v>
       </c>
       <c r="O33" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0.102039485868599</v>
       </c>
       <c r="P33" s="58"/>
@@ -7439,7 +7653,7 @@
         <v>16.526211548050401</v>
       </c>
       <c r="O34" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0.16526211548050401</v>
       </c>
       <c r="P34" s="58"/>
@@ -7458,13 +7672,13 @@
       <c r="K35" s="49"/>
       <c r="L35" s="60"/>
       <c r="M35" s="46" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="N35" s="52">
         <v>-1.34369314780613</v>
       </c>
       <c r="O35" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-1.34369314780613E-2</v>
       </c>
       <c r="P35" s="58"/>
@@ -7489,7 +7703,7 @@
         <v>29.247637436823101</v>
       </c>
       <c r="O36" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0.29247637436823104</v>
       </c>
       <c r="P36" s="58"/>
@@ -7508,13 +7722,13 @@
       <c r="K37" s="47"/>
       <c r="L37" s="60"/>
       <c r="M37" s="46" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N37" s="52">
         <v>11.0919776937066</v>
       </c>
       <c r="O37" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0.11091977693706599</v>
       </c>
       <c r="P37" s="58"/>
@@ -7539,7 +7753,7 @@
         <v>-94.199996999999996</v>
       </c>
       <c r="O38" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-0.94199996999999991</v>
       </c>
       <c r="P38" s="58"/>
@@ -7556,14 +7770,14 @@
       <c r="K39" s="1"/>
       <c r="L39" s="60"/>
       <c r="M39" s="46" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="N39">
         <f>21.4613437652587-19</f>
         <v>2.4613437652587002</v>
       </c>
       <c r="O39" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2.4613437652587004E-2</v>
       </c>
       <c r="P39" s="58"/>
@@ -7578,7 +7792,7 @@
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
       <c r="L40" s="60" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="M40" s="46" t="s">
         <v>68</v>
@@ -7603,16 +7817,16 @@
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
       <c r="L41" s="56" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="M41" s="46" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N41" s="52">
         <v>0.52427629116916796</v>
       </c>
       <c r="O41" s="1">
-        <f t="shared" ref="O41:O43" si="4">N41/100</f>
+        <f t="shared" ref="O41:O43" si="8">N41/100</f>
         <v>5.2427629116916794E-3</v>
       </c>
       <c r="P41" s="58"/>
@@ -7635,7 +7849,7 @@
         <v>-13.5</v>
       </c>
       <c r="O42" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-0.13500000000000001</v>
       </c>
       <c r="P42" s="58"/>
@@ -7659,7 +7873,7 @@
         <v>-5.8</v>
       </c>
       <c r="O43" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-5.7999999999999996E-2</v>
       </c>
       <c r="P43" s="58"/>
@@ -7677,7 +7891,7 @@
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
       <c r="L44" s="60" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="M44" s="46" t="s">
         <v>69</v>
@@ -7704,16 +7918,16 @@
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
       <c r="L45" s="56" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M45" s="46" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N45" s="52">
         <v>0.31779049296478201</v>
       </c>
       <c r="O45" s="1">
-        <f t="shared" ref="O45:O51" si="5">N45/100</f>
+        <f t="shared" ref="O45:O51" si="9">N45/100</f>
         <v>3.1779049296478202E-3</v>
       </c>
       <c r="P45" s="58"/>
@@ -7738,7 +7952,7 @@
         <v>-14.9</v>
       </c>
       <c r="O46" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>-0.14899999999999999</v>
       </c>
       <c r="P46" s="58"/>
@@ -7756,13 +7970,13 @@
       <c r="K47" s="1"/>
       <c r="L47" s="60"/>
       <c r="M47" s="46" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N47" s="52">
         <v>-5</v>
       </c>
       <c r="O47" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>-0.05</v>
       </c>
       <c r="P47" s="58"/>
@@ -7779,19 +7993,21 @@
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
       <c r="L48" s="60" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="M48" s="79" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="N48" s="80">
         <v>72.934574594694098</v>
       </c>
       <c r="O48" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0.72934574594694102</v>
       </c>
-      <c r="P48" s="58"/>
+      <c r="P48" s="58" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="49" spans="1:16" s="72" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
@@ -7804,9 +8020,11 @@
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
-      <c r="L49" s="60"/>
+      <c r="L49" s="60" t="s">
+        <v>216</v>
+      </c>
       <c r="M49" s="79" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="N49" s="72">
         <v>3.5900360862934599</v>
@@ -7815,7 +8033,9 @@
         <f>N49/100</f>
         <v>3.5900360862934598E-2</v>
       </c>
-      <c r="P49" s="58"/>
+      <c r="P49" s="58" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="50" spans="1:16" s="72" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
@@ -7830,16 +8050,18 @@
       <c r="K50" s="1"/>
       <c r="L50" s="60"/>
       <c r="M50" s="79" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="N50" s="52">
         <v>42.467165475154701</v>
       </c>
       <c r="O50" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0.424671654751547</v>
       </c>
-      <c r="P50" s="58"/>
+      <c r="P50" s="58" t="s">
+        <v>218</v>
+      </c>
     </row>
     <row r="51" spans="1:16" s="72" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
@@ -7854,16 +8076,18 @@
       <c r="K51" s="1"/>
       <c r="L51" s="60"/>
       <c r="M51" s="79" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="N51" s="80">
         <v>-2.12732489205733</v>
       </c>
       <c r="O51" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>-2.12732489205733E-2</v>
       </c>
-      <c r="P51" s="58"/>
+      <c r="P51" s="58" t="s">
+        <v>218</v>
+      </c>
     </row>
     <row r="52" spans="1:16" s="72" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
@@ -7878,16 +8102,18 @@
       <c r="K52" s="1"/>
       <c r="L52" s="60"/>
       <c r="M52" s="79" t="s">
-        <v>209</v>
+        <v>26</v>
       </c>
       <c r="N52" s="80">
-        <v>1.04499995797579</v>
+        <v>1.059999943</v>
       </c>
       <c r="O52" s="1">
         <f>N52</f>
-        <v>1.04499995797579</v>
-      </c>
-      <c r="P52" s="58"/>
+        <v>1.059999943</v>
+      </c>
+      <c r="P52" s="58" t="s">
+        <v>218</v>
+      </c>
     </row>
     <row r="53" spans="1:16" s="72" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
@@ -7897,16 +8123,24 @@
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
-      <c r="I53" s="1"/>
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
       <c r="L53" s="60"/>
-      <c r="M53" s="79"/>
-      <c r="N53" s="52"/>
-      <c r="O53" s="1"/>
-      <c r="P53" s="58"/>
-    </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M53" s="81" t="s">
+        <v>210</v>
+      </c>
+      <c r="N53" s="80">
+        <v>1.028092515</v>
+      </c>
+      <c r="O53" s="1">
+        <f>N53</f>
+        <v>1.028092515</v>
+      </c>
+      <c r="P53" s="58" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" s="72" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -7914,1167 +8148,1293 @@
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>
-      <c r="I54" s="1"/>
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
-      <c r="M54" s="46"/>
-      <c r="N54" s="52"/>
-      <c r="O54" s="1"/>
-      <c r="P54" s="58"/>
-    </row>
-    <row r="55" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L54" s="60"/>
+      <c r="M54" s="81" t="s">
+        <v>94</v>
+      </c>
+      <c r="N54" s="80">
+        <v>1.009999997</v>
+      </c>
+      <c r="O54" s="1">
+        <f t="shared" ref="O54:O59" si="10">N54</f>
+        <v>1.009999997</v>
+      </c>
+      <c r="P54" s="58" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" s="72" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
-      <c r="I55" s="1"/>
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
-      <c r="M55" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="N55" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="O55" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="P55" s="11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="56" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="L55" s="60"/>
+      <c r="M55" s="81" t="s">
+        <v>211</v>
+      </c>
+      <c r="N55" s="80">
+        <v>1.085083507</v>
+      </c>
+      <c r="O55" s="1">
+        <f t="shared" si="10"/>
+        <v>1.085083507</v>
+      </c>
+      <c r="P55" s="58" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" s="72" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
-      <c r="I56" s="1"/>
       <c r="J56" s="1"/>
       <c r="K56" s="1"/>
-      <c r="L56" t="s">
-        <v>139</v>
-      </c>
-      <c r="M56" s="42" t="s">
-        <v>41</v>
-      </c>
-      <c r="N56" s="50">
-        <v>0</v>
-      </c>
-      <c r="O56" s="54">
-        <f>N56</f>
-        <v>0</v>
-      </c>
-      <c r="P56" s="58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L56" s="60"/>
+      <c r="M56" s="81" t="s">
+        <v>212</v>
+      </c>
+      <c r="N56" s="80">
+        <v>1.0240525229999999</v>
+      </c>
+      <c r="O56" s="1">
+        <f t="shared" si="10"/>
+        <v>1.0240525229999999</v>
+      </c>
+      <c r="P56" s="58" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" s="72" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
-      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
-      <c r="I57" s="1"/>
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
-      <c r="L57" s="55">
-        <v>4.8611111111111112E-2</v>
-      </c>
-      <c r="M57" s="42" t="s">
-        <v>23</v>
-      </c>
-      <c r="N57" s="50">
-        <v>1.0599999427795399</v>
-      </c>
-      <c r="O57" s="54">
-        <f>N57</f>
-        <v>1.0599999427795399</v>
-      </c>
-      <c r="P57" s="58">
-        <v>-2.9953879373185301E-2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L57" s="60"/>
+      <c r="M57" s="81" t="s">
+        <v>213</v>
+      </c>
+      <c r="N57" s="80">
+        <v>1.019923836</v>
+      </c>
+      <c r="O57" s="1">
+        <f t="shared" si="10"/>
+        <v>1.019923836</v>
+      </c>
+      <c r="P57" s="58" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" s="72" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
-      <c r="E58" s="1"/>
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
       <c r="H58" s="1"/>
-      <c r="I58" s="1"/>
       <c r="J58" s="1"/>
       <c r="K58" s="1"/>
-      <c r="M58" s="42" t="s">
+      <c r="L58" s="60"/>
+      <c r="M58" s="81" t="s">
+        <v>214</v>
+      </c>
+      <c r="N58" s="80">
+        <v>1.027986216</v>
+      </c>
+      <c r="O58" s="1">
+        <f t="shared" si="10"/>
+        <v>1.027986216</v>
+      </c>
+      <c r="P58" s="58" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" s="72" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1"/>
+      <c r="H59" s="1"/>
+      <c r="J59" s="1"/>
+      <c r="K59" s="1"/>
+      <c r="L59" s="60"/>
+      <c r="M59" s="81" t="s">
+        <v>215</v>
+      </c>
+      <c r="N59" s="80">
+        <v>1.0349152580000001</v>
+      </c>
+      <c r="O59" s="1">
+        <f t="shared" si="10"/>
+        <v>1.0349152580000001</v>
+      </c>
+      <c r="P59" s="58" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
+      <c r="H60" s="1"/>
+      <c r="I60" s="1"/>
+      <c r="J60" s="1"/>
+      <c r="K60" s="1"/>
+      <c r="M60" s="46"/>
+      <c r="N60" s="52"/>
+      <c r="O60" s="1"/>
+      <c r="P60" s="58"/>
+    </row>
+    <row r="61" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1"/>
+      <c r="H61" s="1"/>
+      <c r="I61" s="1"/>
+      <c r="J61" s="1"/>
+      <c r="K61" s="1"/>
+      <c r="M61" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="N61" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="O61" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="P61" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="1"/>
+      <c r="B62" s="1"/>
+      <c r="C62" s="1"/>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+      <c r="F62" s="1"/>
+      <c r="G62" s="1"/>
+      <c r="H62" s="1"/>
+      <c r="I62" s="1"/>
+      <c r="J62" s="1"/>
+      <c r="K62" s="1"/>
+      <c r="L62" t="s">
+        <v>138</v>
+      </c>
+      <c r="M62" s="42" t="s">
+        <v>41</v>
+      </c>
+      <c r="N62" s="50">
+        <v>0</v>
+      </c>
+      <c r="O62" s="54">
+        <f>N62</f>
+        <v>0</v>
+      </c>
+      <c r="P62" s="58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+      <c r="G63" s="1"/>
+      <c r="H63" s="1"/>
+      <c r="I63" s="1"/>
+      <c r="J63" s="1"/>
+      <c r="K63" s="1"/>
+      <c r="L63" s="55">
+        <v>4.8611111111111112E-2</v>
+      </c>
+      <c r="M63" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="N63" s="50">
+        <v>1.0599999427795399</v>
+      </c>
+      <c r="O63" s="54">
+        <f>N63</f>
+        <v>1.0599999427795399</v>
+      </c>
+      <c r="P63" s="58">
+        <v>-2.9953879373185301E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A64" s="1"/>
+      <c r="B64" s="1"/>
+      <c r="C64" s="1"/>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+      <c r="F64" s="1"/>
+      <c r="G64" s="1"/>
+      <c r="H64" s="1"/>
+      <c r="I64" s="1"/>
+      <c r="J64" s="1"/>
+      <c r="K64" s="1"/>
+      <c r="M64" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="N58" s="50">
+      <c r="N64" s="50">
         <v>156.440731910842</v>
       </c>
-      <c r="O58" s="1">
-        <f>N58/100</f>
+      <c r="O64" s="1">
+        <f>N64/100</f>
         <v>1.56440731910842</v>
       </c>
-      <c r="P58" s="58">
+      <c r="P64" s="58">
         <v>-8.6738403137775998E-6</v>
-      </c>
-    </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="M59" s="42" t="s">
-        <v>117</v>
-      </c>
-      <c r="N59" s="50">
-        <v>-20.300935880694301</v>
-      </c>
-      <c r="O59" s="1">
-        <f t="shared" ref="O59:O65" si="6">N59/100</f>
-        <v>-0.20300935880694301</v>
-      </c>
-      <c r="P59" s="58">
-        <v>2.1648716178694401E-3</v>
-      </c>
-    </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="M60" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="N60" s="50">
-        <v>75.916881283268793</v>
-      </c>
-      <c r="O60" s="1">
-        <f t="shared" si="6"/>
-        <v>0.75916881283268789</v>
-      </c>
-      <c r="P60" s="58">
-        <v>6.4758759358596297E-4</v>
-      </c>
-    </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="M61" s="42" t="s">
-        <v>118</v>
-      </c>
-      <c r="N61" s="50">
-        <v>-0.155506560051652</v>
-      </c>
-      <c r="O61" s="1">
-        <f t="shared" si="6"/>
-        <v>-1.55506560051652E-3</v>
-      </c>
-      <c r="P61" s="58">
-        <v>-1.47979634931223E-3</v>
-      </c>
-    </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="M62" s="42" t="s">
-        <v>48</v>
-      </c>
-      <c r="N62" s="50">
-        <v>41.338725991097199</v>
-      </c>
-      <c r="O62" s="1">
-        <f t="shared" si="6"/>
-        <v>0.41338725991097197</v>
-      </c>
-      <c r="P62" s="58">
-        <v>6.8870384835700903E-4</v>
-      </c>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="M63" s="42" t="s">
-        <v>119</v>
-      </c>
-      <c r="N63" s="50">
-        <v>-3.8398609004379098</v>
-      </c>
-      <c r="O63" s="1">
-        <f t="shared" si="6"/>
-        <v>-3.8398609004379101E-2</v>
-      </c>
-      <c r="P63" s="58">
-        <v>-1.3891657030102901E-3</v>
-      </c>
-    </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="M64" s="42" t="s">
-        <v>49</v>
-      </c>
-      <c r="N64" s="50">
-        <v>232.35762119293199</v>
-      </c>
-      <c r="O64" s="1">
-        <f t="shared" si="6"/>
-        <v>2.32357621192932</v>
-      </c>
-      <c r="P64" s="58">
-        <v>6.3899375327158804E-4</v>
       </c>
     </row>
     <row r="65" spans="12:16" x14ac:dyDescent="0.25">
       <c r="M65" s="42" t="s">
-        <v>83</v>
+        <v>116</v>
       </c>
       <c r="N65" s="50">
-        <v>-20.456442236900301</v>
+        <v>-20.300935880694301</v>
       </c>
       <c r="O65" s="1">
-        <f t="shared" si="6"/>
-        <v>-0.20456442236900302</v>
+        <f t="shared" ref="O65:O71" si="11">N65/100</f>
+        <v>-0.20300935880694301</v>
       </c>
       <c r="P65" s="58">
-        <v>6.8507826856001298E-4</v>
+        <v>2.1648716178694401E-3</v>
       </c>
     </row>
     <row r="66" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="L66" t="s">
-        <v>140</v>
-      </c>
       <c r="M66" s="42" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="N66" s="50">
-        <v>-0.22125272217770001</v>
-      </c>
-      <c r="O66" s="54">
-        <f>N66</f>
-        <v>-0.22125272217770001</v>
-      </c>
-      <c r="P66" s="59">
-        <v>-0.2212527222</v>
+        <v>75.916881283268793</v>
+      </c>
+      <c r="O66" s="1">
+        <f t="shared" si="11"/>
+        <v>0.75916881283268789</v>
+      </c>
+      <c r="P66" s="58">
+        <v>6.4758759358596297E-4</v>
       </c>
     </row>
     <row r="67" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="L67" s="55">
-        <v>0.47083333333333338</v>
-      </c>
       <c r="M67" s="42" t="s">
-        <v>27</v>
+        <v>117</v>
       </c>
       <c r="N67" s="50">
-        <v>1.0099999973080001</v>
-      </c>
-      <c r="O67" s="54">
-        <f>N67</f>
-        <v>1.0099999973080001</v>
-      </c>
-      <c r="P67" s="59">
-        <v>2.17540256007367E-2</v>
+        <v>-0.155506560051652</v>
+      </c>
+      <c r="O67" s="1">
+        <f t="shared" si="11"/>
+        <v>-1.55506560051652E-3</v>
+      </c>
+      <c r="P67" s="58">
+        <v>-1.47979634931223E-3</v>
       </c>
     </row>
     <row r="68" spans="12:16" x14ac:dyDescent="0.25">
       <c r="M68" s="42" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="N68" s="50">
-        <v>-23.569740833506799</v>
+        <v>41.338725991097199</v>
       </c>
       <c r="O68" s="1">
-        <f>N68/100</f>
-        <v>-0.235697408335068</v>
+        <f t="shared" si="11"/>
+        <v>0.41338725991097197</v>
       </c>
       <c r="P68" s="58">
-        <v>-1.05523560178061E-3</v>
+        <v>6.8870384835700903E-4</v>
       </c>
     </row>
     <row r="69" spans="12:16" x14ac:dyDescent="0.25">
       <c r="M69" s="42" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="N69" s="50">
-        <v>0.96859150246414105</v>
+        <v>-3.8398609004379098</v>
       </c>
       <c r="O69" s="1">
-        <f t="shared" ref="O69:O73" si="7">N69/100</f>
-        <v>9.6859150246414102E-3</v>
+        <f t="shared" si="11"/>
+        <v>-3.8398609004379101E-2</v>
       </c>
       <c r="P69" s="58">
-        <v>-2.2375145874756201E-3</v>
+        <v>-1.3891657030102901E-3</v>
       </c>
     </row>
     <row r="70" spans="12:16" x14ac:dyDescent="0.25">
       <c r="M70" s="42" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="N70" s="50">
-        <v>29.247688021076399</v>
+        <v>232.35762119293199</v>
       </c>
       <c r="O70" s="1">
-        <f t="shared" si="7"/>
-        <v>0.29247688021076401</v>
+        <f t="shared" si="11"/>
+        <v>2.32357621192932</v>
       </c>
       <c r="P70" s="58">
-        <v>5.1585990707936401E-4</v>
+        <v>6.3899375327158804E-4</v>
       </c>
     </row>
     <row r="71" spans="12:16" x14ac:dyDescent="0.25">
       <c r="M71" s="42" t="s">
-        <v>121</v>
+        <v>83</v>
       </c>
       <c r="N71" s="50">
-        <v>-10.134384235994199</v>
+        <v>-20.456442236900301</v>
       </c>
       <c r="O71" s="1">
-        <f t="shared" si="7"/>
-        <v>-0.101343842359942</v>
+        <f t="shared" si="11"/>
+        <v>-0.20456442236900302</v>
       </c>
       <c r="P71" s="58">
-        <v>-2.7105327863768802E-3</v>
+        <v>6.8507826856001298E-4</v>
       </c>
     </row>
     <row r="72" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L72" t="s">
+        <v>139</v>
+      </c>
       <c r="M72" s="42" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="N72" s="50">
-        <v>4.9388912162000001E-5</v>
-      </c>
-      <c r="O72" s="1">
-        <f t="shared" si="7"/>
-        <v>4.9388912162000003E-7</v>
-      </c>
-      <c r="P72" s="58">
-        <v>6.5059278082477401E-7</v>
+        <v>-0.22125272217770001</v>
+      </c>
+      <c r="O72" s="54">
+        <f>N72</f>
+        <v>-0.22125272217770001</v>
+      </c>
+      <c r="P72" s="59">
+        <v>-0.2212527222</v>
       </c>
     </row>
     <row r="73" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L73" s="55">
+        <v>0.47083333333333338</v>
+      </c>
       <c r="M73" s="42" t="s">
-        <v>122</v>
+        <v>27</v>
       </c>
       <c r="N73" s="50">
-        <v>-23.1382548362844</v>
-      </c>
-      <c r="O73" s="1">
-        <f t="shared" si="7"/>
-        <v>-0.231382548362844</v>
-      </c>
-      <c r="P73" s="58">
-        <v>1.7465773008429299E-7</v>
+        <v>1.0099999973080001</v>
+      </c>
+      <c r="O73" s="54">
+        <f>N73</f>
+        <v>1.0099999973080001</v>
+      </c>
+      <c r="P73" s="59">
+        <v>2.17540256007367E-2</v>
       </c>
     </row>
     <row r="74" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="L74" t="s">
-        <v>141</v>
-      </c>
       <c r="M74" s="42" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="N74" s="50">
-        <v>-0.25510563387813501</v>
-      </c>
-      <c r="O74" s="54">
-        <f>N74</f>
-        <v>-0.25510563387813501</v>
-      </c>
-      <c r="P74" s="59">
-        <v>-0.25510563390000002</v>
+        <v>-23.569740833506799</v>
+      </c>
+      <c r="O74" s="1">
+        <f>N74/100</f>
+        <v>-0.235697408335068</v>
+      </c>
+      <c r="P74" s="58">
+        <v>-1.05523560178061E-3</v>
       </c>
     </row>
     <row r="75" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="L75" s="55">
-        <v>0.8125</v>
-      </c>
       <c r="M75" s="42" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="N75" s="50">
-        <v>1.0385379019832599</v>
-      </c>
-      <c r="O75" s="54">
-        <f>N75</f>
-        <v>1.0385379019832599</v>
-      </c>
-      <c r="P75" s="59">
-        <v>-5.12238863404413E-3</v>
+        <v>0.96859150246414105</v>
+      </c>
+      <c r="O75" s="1">
+        <f t="shared" ref="O75:O79" si="12">N75/100</f>
+        <v>9.6859150246414102E-3</v>
+      </c>
+      <c r="P75" s="58">
+        <v>-2.2375145874756201E-3</v>
       </c>
     </row>
     <row r="76" spans="12:16" x14ac:dyDescent="0.25">
       <c r="M76" s="42" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="N76" s="50">
-        <v>6.4193752642371704</v>
+        <v>29.247688021076399</v>
       </c>
       <c r="O76" s="1">
-        <f>N76/100</f>
-        <v>6.4193752642371704E-2</v>
+        <f t="shared" si="12"/>
+        <v>0.29247688021076401</v>
       </c>
       <c r="P76" s="58">
-        <v>1.2851248455257599E-4</v>
+        <v>5.1585990707936401E-4</v>
       </c>
     </row>
     <row r="77" spans="12:16" x14ac:dyDescent="0.25">
       <c r="M77" s="42" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="N77" s="50">
-        <v>1.57798981550307</v>
+        <v>-10.134384235994199</v>
       </c>
       <c r="O77" s="1">
-        <f t="shared" ref="O77:O85" si="8">N77/100</f>
-        <v>1.5779898155030701E-2</v>
+        <f t="shared" si="12"/>
+        <v>-0.101343842359942</v>
       </c>
       <c r="P77" s="58">
-        <v>1.0767413611616999E-3</v>
+        <v>-2.7105327863768802E-3</v>
       </c>
     </row>
     <row r="78" spans="12:16" x14ac:dyDescent="0.25">
       <c r="M78" s="42" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="N78" s="50">
-        <v>7.6111237412808599</v>
+        <v>4.9388912162000001E-5</v>
       </c>
       <c r="O78" s="1">
-        <f t="shared" si="8"/>
-        <v>7.6111237412808605E-2</v>
+        <f t="shared" si="12"/>
+        <v>4.9388912162000003E-7</v>
       </c>
       <c r="P78" s="58">
-        <v>1.6297137374082799E-5</v>
+        <v>6.5059278082477401E-7</v>
       </c>
     </row>
     <row r="79" spans="12:16" x14ac:dyDescent="0.25">
       <c r="M79" s="42" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="N79" s="50">
-        <v>2.2749299623984598</v>
+        <v>-23.1382548362844</v>
       </c>
       <c r="O79" s="1">
-        <f t="shared" si="8"/>
-        <v>2.2749299623984597E-2</v>
+        <f t="shared" si="12"/>
+        <v>-0.231382548362844</v>
       </c>
       <c r="P79" s="58">
-        <v>9.80565804585901E-5</v>
+        <v>1.7465773008429299E-7</v>
       </c>
     </row>
     <row r="80" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L80" t="s">
+        <v>140</v>
+      </c>
       <c r="M80" s="42" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="N80" s="50">
-        <v>17.236621109828601</v>
-      </c>
-      <c r="O80" s="1">
-        <f t="shared" si="8"/>
-        <v>0.17236621109828601</v>
-      </c>
-      <c r="P80" s="58">
-        <v>2.8072391037720099E-5</v>
+        <v>-0.25510563387813501</v>
+      </c>
+      <c r="O80" s="54">
+        <f>N80</f>
+        <v>-0.25510563387813501</v>
+      </c>
+      <c r="P80" s="59">
+        <v>-0.25510563390000002</v>
       </c>
     </row>
     <row r="81" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="L81" s="55">
+        <v>0.8125</v>
+      </c>
       <c r="M81" s="42" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="N81" s="50">
-        <v>6.2088690408799696</v>
-      </c>
-      <c r="O81" s="1">
-        <f t="shared" si="8"/>
-        <v>6.2088690408799697E-2</v>
-      </c>
-      <c r="P81" s="58">
-        <v>3.8053003130694002E-4</v>
+        <v>1.0385379019832599</v>
+      </c>
+      <c r="O81" s="54">
+        <f>N81</f>
+        <v>1.0385379019832599</v>
+      </c>
+      <c r="P81" s="59">
+        <v>-5.12238863404413E-3</v>
       </c>
     </row>
     <row r="82" spans="8:16" x14ac:dyDescent="0.25">
       <c r="M82" s="42" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="N82" s="50">
-        <v>1.4392071686730901</v>
+        <v>6.4193752642371704</v>
       </c>
       <c r="O82" s="1">
-        <f t="shared" si="8"/>
-        <v>1.4392071686730901E-2</v>
+        <f>N82/100</f>
+        <v>6.4193752642371704E-2</v>
       </c>
       <c r="P82" s="58">
-        <v>3.3901950999533699E-5</v>
+        <v>1.2851248455257599E-4</v>
       </c>
     </row>
     <row r="83" spans="8:16" x14ac:dyDescent="0.25">
       <c r="M83" s="42" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="N83" s="50">
-        <v>0.52526799870488805</v>
+        <v>1.57798981550307</v>
       </c>
       <c r="O83" s="1">
-        <f t="shared" si="8"/>
-        <v>5.2526799870488807E-3</v>
+        <f t="shared" ref="O83:O91" si="13">N83/100</f>
+        <v>1.5779898155030701E-2</v>
       </c>
       <c r="P83" s="58">
-        <v>9.7871725652031802E-5</v>
+        <v>1.0767413611616999E-3</v>
       </c>
     </row>
     <row r="84" spans="8:16" x14ac:dyDescent="0.25">
       <c r="M84" s="42" t="s">
-        <v>12</v>
+        <v>57</v>
       </c>
       <c r="N84" s="50">
-        <v>-6.1</v>
+        <v>7.6111237412808599</v>
       </c>
       <c r="O84" s="1">
-        <f t="shared" si="8"/>
-        <v>-6.0999999999999999E-2</v>
+        <f t="shared" si="13"/>
+        <v>7.6111237412808605E-2</v>
       </c>
       <c r="P84" s="58">
-        <v>-5.5804864002167998E-6</v>
+        <v>1.6297137374082799E-5</v>
       </c>
     </row>
     <row r="85" spans="8:16" x14ac:dyDescent="0.25">
       <c r="M85" s="42" t="s">
+        <v>122</v>
+      </c>
+      <c r="N85" s="50">
+        <v>2.2749299623984598</v>
+      </c>
+      <c r="O85" s="1">
+        <f t="shared" si="13"/>
+        <v>2.2749299623984597E-2</v>
+      </c>
+      <c r="P85" s="58">
+        <v>9.80565804585901E-5</v>
+      </c>
+    </row>
+    <row r="86" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="M86" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="N86" s="50">
+        <v>17.236621109828601</v>
+      </c>
+      <c r="O86" s="1">
+        <f t="shared" si="13"/>
+        <v>0.17236621109828601</v>
+      </c>
+      <c r="P86" s="58">
+        <v>2.8072391037720099E-5</v>
+      </c>
+    </row>
+    <row r="87" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="M87" s="42" t="s">
+        <v>124</v>
+      </c>
+      <c r="N87" s="50">
+        <v>6.2088690408799696</v>
+      </c>
+      <c r="O87" s="1">
+        <f t="shared" si="13"/>
+        <v>6.2088690408799697E-2</v>
+      </c>
+      <c r="P87" s="58">
+        <v>3.8053003130694002E-4</v>
+      </c>
+    </row>
+    <row r="88" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="M88" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="N88" s="50">
+        <v>1.4392071686730901</v>
+      </c>
+      <c r="O88" s="1">
+        <f t="shared" si="13"/>
+        <v>1.4392071686730901E-2</v>
+      </c>
+      <c r="P88" s="58">
+        <v>3.3901950999533699E-5</v>
+      </c>
+    </row>
+    <row r="89" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="M89" s="42" t="s">
+        <v>125</v>
+      </c>
+      <c r="N89" s="50">
+        <v>0.52526799870488805</v>
+      </c>
+      <c r="O89" s="1">
+        <f t="shared" si="13"/>
+        <v>5.2526799870488807E-3</v>
+      </c>
+      <c r="P89" s="58">
+        <v>9.7871725652031802E-5</v>
+      </c>
+    </row>
+    <row r="90" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="M90" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="N90" s="50">
+        <v>-6.1</v>
+      </c>
+      <c r="O90" s="1">
+        <f t="shared" si="13"/>
+        <v>-6.0999999999999999E-2</v>
+      </c>
+      <c r="P90" s="58">
+        <v>-5.5804864002167998E-6</v>
+      </c>
+    </row>
+    <row r="91" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="M91" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="N85" s="50">
+      <c r="N91" s="50">
         <v>-1.6</v>
       </c>
-      <c r="O85" s="1">
-        <f t="shared" si="8"/>
+      <c r="O91" s="1">
+        <f t="shared" si="13"/>
         <v>-1.6E-2</v>
       </c>
-      <c r="P85" s="58">
+      <c r="P91" s="58">
         <v>5.2797756594065403E-5</v>
       </c>
     </row>
-    <row r="86" spans="8:16" x14ac:dyDescent="0.25">
-      <c r="L86" t="s">
-        <v>142</v>
-      </c>
-      <c r="M86" s="42" t="s">
+    <row r="92" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="L92" t="s">
+        <v>141</v>
+      </c>
+      <c r="M92" s="42" t="s">
         <v>60</v>
       </c>
-      <c r="N86" s="50">
+      <c r="N92" s="50">
         <v>-0.26806990591321</v>
       </c>
-      <c r="O86" s="54">
-        <f>N86</f>
+      <c r="O92" s="54">
+        <f>N92</f>
         <v>-0.26806990591321</v>
       </c>
-      <c r="P86" s="59">
+      <c r="P92" s="59">
         <v>-0.26806990590000002</v>
       </c>
     </row>
-    <row r="87" spans="8:16" x14ac:dyDescent="0.25">
-      <c r="I87" s="72" t="s">
-        <v>210</v>
-      </c>
-      <c r="L87" s="56" t="s">
-        <v>147</v>
-      </c>
-      <c r="M87" s="42" t="s">
+    <row r="93" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="I93" s="72" t="s">
+        <v>208</v>
+      </c>
+      <c r="L93" s="56" t="s">
+        <v>146</v>
+      </c>
+      <c r="M93" s="42" t="s">
         <v>115</v>
       </c>
-      <c r="N87" s="50">
+      <c r="N93" s="50">
         <v>1.0349152577221601</v>
       </c>
-      <c r="O87" s="54">
-        <f>N87</f>
+      <c r="O93" s="54">
+        <f>N93</f>
         <v>1.0349152577221601</v>
       </c>
-      <c r="P87" s="59">
+      <c r="P93" s="59">
         <v>-2.1765958813597698E-3</v>
       </c>
     </row>
-    <row r="88" spans="8:16" x14ac:dyDescent="0.25">
-      <c r="I88" s="72" t="s">
-        <v>211</v>
-      </c>
-      <c r="L88" s="47"/>
-      <c r="M88" s="42" t="s">
+    <row r="94" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="I94" s="72" t="s">
+        <v>209</v>
+      </c>
+      <c r="L94" s="47"/>
+      <c r="M94" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="N88" s="50">
+      <c r="N94" s="50">
         <v>6.1481308294477897</v>
       </c>
-      <c r="O88" s="1">
-        <f>N88/100</f>
+      <c r="O94" s="1">
+        <f>N94/100</f>
         <v>6.1481308294477899E-2</v>
       </c>
-      <c r="P88" s="57">
+      <c r="P94" s="57">
         <v>-1.88116567434796E-5</v>
-      </c>
-    </row>
-    <row r="89" spans="8:16" x14ac:dyDescent="0.25">
-      <c r="H89">
-        <v>1</v>
-      </c>
-      <c r="I89" s="72">
-        <v>1.0599999427795399</v>
-      </c>
-      <c r="L89" s="47"/>
-      <c r="M89" s="42" t="s">
-        <v>127</v>
-      </c>
-      <c r="N89" s="50">
-        <v>6.1776975079165704</v>
-      </c>
-      <c r="O89" s="1">
-        <f t="shared" ref="O89:O101" si="9">N89/100</f>
-        <v>6.1776975079165707E-2</v>
-      </c>
-      <c r="P89" s="57">
-        <v>-4.4567340559324698E-4</v>
-      </c>
-    </row>
-    <row r="90" spans="8:16" x14ac:dyDescent="0.25">
-      <c r="H90">
-        <v>2</v>
-      </c>
-      <c r="I90" s="72">
-        <v>1.04499995797579</v>
-      </c>
-      <c r="L90" s="47"/>
-      <c r="M90" s="42" t="s">
-        <v>62</v>
-      </c>
-      <c r="N90" s="50">
-        <v>10.1258308263922</v>
-      </c>
-      <c r="O90" s="1">
-        <f t="shared" si="9"/>
-        <v>0.101258308263922</v>
-      </c>
-      <c r="P90" s="58">
-        <v>-1.40656940313608E-4</v>
-      </c>
-    </row>
-    <row r="91" spans="8:16" x14ac:dyDescent="0.25">
-      <c r="H91">
-        <v>3</v>
-      </c>
-      <c r="I91" s="72">
-        <v>1.0099999973080001</v>
-      </c>
-      <c r="L91" s="47"/>
-      <c r="M91" s="42" t="s">
-        <v>128</v>
-      </c>
-      <c r="N91" s="50">
-        <v>4.8779939913553596</v>
-      </c>
-      <c r="O91" s="1">
-        <f t="shared" si="9"/>
-        <v>4.8779939913553595E-2</v>
-      </c>
-      <c r="P91" s="57">
-        <v>-6.3339605935184401E-4</v>
-      </c>
-    </row>
-    <row r="92" spans="8:16" x14ac:dyDescent="0.25">
-      <c r="H92">
-        <v>4</v>
-      </c>
-      <c r="I92" s="72">
-        <v>1.02371286456331</v>
-      </c>
-      <c r="L92" t="s">
-        <v>143</v>
-      </c>
-      <c r="M92" s="42" t="s">
-        <v>63</v>
-      </c>
-      <c r="N92" s="50">
-        <v>-7.6</v>
-      </c>
-      <c r="O92" s="1">
-        <f t="shared" si="9"/>
-        <v>-7.5999999999999998E-2</v>
-      </c>
-      <c r="P92" s="58">
-        <v>-1.4483820858600399E-4</v>
-      </c>
-    </row>
-    <row r="93" spans="8:16" x14ac:dyDescent="0.25">
-      <c r="H93">
-        <v>5</v>
-      </c>
-      <c r="I93" s="72">
-        <v>1.0280925147905799</v>
-      </c>
-      <c r="L93" s="56" t="s">
-        <v>148</v>
-      </c>
-      <c r="M93" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="N93" s="50">
-        <v>-1.6</v>
-      </c>
-      <c r="O93" s="1">
-        <f t="shared" si="9"/>
-        <v>-1.6E-2</v>
-      </c>
-      <c r="P93" s="58">
-        <v>-3.5573742834272E-3</v>
-      </c>
-    </row>
-    <row r="94" spans="8:16" x14ac:dyDescent="0.25">
-      <c r="H94">
-        <v>6</v>
-      </c>
-      <c r="I94" s="72">
-        <v>1.0385379019832599</v>
-      </c>
-      <c r="L94" t="s">
-        <v>144</v>
-      </c>
-      <c r="M94" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="N94" s="51">
-        <v>-63.001699846354903</v>
-      </c>
-      <c r="O94" s="1">
-        <f t="shared" si="9"/>
-        <v>-0.63001699846354908</v>
-      </c>
-      <c r="P94" s="58">
-        <v>-9.5060452610995505E-4</v>
       </c>
     </row>
     <row r="95" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H95">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="I95" s="72">
-        <v>1.04612245201456</v>
-      </c>
-      <c r="L95" s="56" t="s">
-        <v>149</v>
-      </c>
+        <v>1.0599999427795399</v>
+      </c>
+      <c r="L95" s="47"/>
       <c r="M95" s="42" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="N95" s="50">
-        <v>10.2039485868599</v>
+        <v>6.1776975079165704</v>
       </c>
       <c r="O95" s="1">
-        <f t="shared" si="9"/>
-        <v>0.102039485868599</v>
-      </c>
-      <c r="P95" s="58">
-        <v>-5.1145973996759402E-3</v>
+        <f t="shared" ref="O95:O107" si="14">N95/100</f>
+        <v>6.1776975079165707E-2</v>
+      </c>
+      <c r="P95" s="57">
+        <v>-4.4567340559324698E-4</v>
       </c>
     </row>
     <row r="96" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H96">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="I96" s="72">
-        <v>1.0850835071553799</v>
-      </c>
+        <v>1.04499995797579</v>
+      </c>
+      <c r="L96" s="47"/>
       <c r="M96" s="42" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="N96" s="50">
-        <v>16.526211548050401</v>
+        <v>10.1258308263922</v>
       </c>
       <c r="O96" s="1">
-        <f t="shared" si="9"/>
-        <v>0.16526211548050401</v>
+        <f t="shared" si="14"/>
+        <v>0.101258308263922</v>
       </c>
       <c r="P96" s="58">
-        <v>3.0418249791705498E-4</v>
+        <v>-1.40656940313608E-4</v>
       </c>
     </row>
     <row r="97" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H97">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="I97" s="72">
-        <v>1.0349152577221601</v>
-      </c>
+        <v>1.0099999973080001</v>
+      </c>
+      <c r="L97" s="47"/>
       <c r="M97" s="42" t="s">
-        <v>131</v>
-      </c>
-      <c r="N97" s="52">
-        <v>-1.34369314780613</v>
+        <v>127</v>
+      </c>
+      <c r="N97" s="50">
+        <v>4.8779939913553596</v>
       </c>
       <c r="O97" s="1">
-        <f t="shared" si="9"/>
-        <v>-1.34369314780613E-2</v>
-      </c>
-      <c r="P97" s="58">
-        <v>-1.37670401876801E-3</v>
+        <f t="shared" si="14"/>
+        <v>4.8779939913553595E-2</v>
+      </c>
+      <c r="P97" s="57">
+        <v>-6.3339605935184401E-4</v>
       </c>
     </row>
     <row r="98" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H98">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="I98" s="72">
-        <v>1.02798621556374</v>
+        <v>1.02371286456331</v>
+      </c>
+      <c r="L98" t="s">
+        <v>142</v>
       </c>
       <c r="M98" s="42" t="s">
-        <v>66</v>
-      </c>
-      <c r="N98" s="52">
-        <v>29.247637436823101</v>
+        <v>63</v>
+      </c>
+      <c r="N98" s="50">
+        <v>-7.6</v>
       </c>
       <c r="O98" s="1">
-        <f t="shared" si="9"/>
-        <v>0.29247637436823104</v>
+        <f t="shared" si="14"/>
+        <v>-7.5999999999999998E-2</v>
       </c>
       <c r="P98" s="58">
-        <v>2.2761940039589499E-4</v>
+        <v>-1.4483820858600399E-4</v>
       </c>
     </row>
     <row r="99" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H99">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="I99" s="72">
-        <v>1.02970205350408</v>
+        <v>1.0280925147905799</v>
+      </c>
+      <c r="L99" s="56" t="s">
+        <v>147</v>
       </c>
       <c r="M99" s="42" t="s">
-        <v>132</v>
-      </c>
-      <c r="N99" s="52">
-        <v>11.0919776937066</v>
+        <v>128</v>
+      </c>
+      <c r="N99" s="50">
+        <v>-1.6</v>
       </c>
       <c r="O99" s="1">
-        <f t="shared" si="9"/>
-        <v>0.11091977693706599</v>
+        <f t="shared" si="14"/>
+        <v>-1.6E-2</v>
       </c>
       <c r="P99" s="58">
-        <v>-1.3983824680780001E-3</v>
+        <v>-3.5573742834272E-3</v>
       </c>
     </row>
     <row r="100" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H100">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="I100" s="72">
-        <v>1.0240525230119499</v>
+        <v>1.0385379019832599</v>
+      </c>
+      <c r="L100" t="s">
+        <v>143</v>
       </c>
       <c r="M100" s="42" t="s">
-        <v>67</v>
-      </c>
-      <c r="N100" s="53">
-        <v>-94.199996999999996</v>
+        <v>64</v>
+      </c>
+      <c r="N100" s="51">
+        <v>-63.001699846354903</v>
       </c>
       <c r="O100" s="1">
-        <f t="shared" si="9"/>
-        <v>-0.94199996999999991</v>
+        <f t="shared" si="14"/>
+        <v>-0.63001699846354908</v>
       </c>
       <c r="P100" s="58">
-        <v>-2.81965662445027E-3</v>
+        <v>-9.5060452610995505E-4</v>
       </c>
     </row>
     <row r="101" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H101">
+        <v>7</v>
+      </c>
+      <c r="I101" s="72">
+        <v>1.04612245201456</v>
+      </c>
+      <c r="L101" s="56" t="s">
+        <v>148</v>
+      </c>
+      <c r="M101" s="42" t="s">
+        <v>129</v>
+      </c>
+      <c r="N101" s="50">
+        <v>10.2039485868599</v>
+      </c>
+      <c r="O101" s="1">
+        <f t="shared" si="14"/>
+        <v>0.102039485868599</v>
+      </c>
+      <c r="P101" s="58">
+        <v>-5.1145973996759402E-3</v>
+      </c>
+    </row>
+    <row r="102" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="H102">
+        <v>8</v>
+      </c>
+      <c r="I102" s="72">
+        <v>1.0850835071553799</v>
+      </c>
+      <c r="M102" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="N102" s="50">
+        <v>16.526211548050401</v>
+      </c>
+      <c r="O102" s="1">
+        <f t="shared" si="14"/>
+        <v>0.16526211548050401</v>
+      </c>
+      <c r="P102" s="58">
+        <v>3.0418249791705498E-4</v>
+      </c>
+    </row>
+    <row r="103" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="H103">
+        <v>9</v>
+      </c>
+      <c r="I103" s="72">
+        <v>1.0349152577221601</v>
+      </c>
+      <c r="M103" s="42" t="s">
+        <v>130</v>
+      </c>
+      <c r="N103" s="52">
+        <v>-1.34369314780613</v>
+      </c>
+      <c r="O103" s="1">
+        <f t="shared" si="14"/>
+        <v>-1.34369314780613E-2</v>
+      </c>
+      <c r="P103" s="58">
+        <v>-1.37670401876801E-3</v>
+      </c>
+    </row>
+    <row r="104" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="H104">
+        <v>10</v>
+      </c>
+      <c r="I104" s="72">
+        <v>1.02798621556374</v>
+      </c>
+      <c r="M104" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="N104" s="52">
+        <v>29.247637436823101</v>
+      </c>
+      <c r="O104" s="1">
+        <f t="shared" si="14"/>
+        <v>0.29247637436823104</v>
+      </c>
+      <c r="P104" s="58">
+        <v>2.2761940039589499E-4</v>
+      </c>
+    </row>
+    <row r="105" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="H105">
+        <v>11</v>
+      </c>
+      <c r="I105" s="72">
+        <v>1.02970205350408</v>
+      </c>
+      <c r="M105" s="42" t="s">
+        <v>131</v>
+      </c>
+      <c r="N105" s="52">
+        <v>11.0919776937066</v>
+      </c>
+      <c r="O105" s="1">
+        <f t="shared" si="14"/>
+        <v>0.11091977693706599</v>
+      </c>
+      <c r="P105" s="58">
+        <v>-1.3983824680780001E-3</v>
+      </c>
+    </row>
+    <row r="106" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="H106">
+        <v>12</v>
+      </c>
+      <c r="I106" s="72">
+        <v>1.0240525230119499</v>
+      </c>
+      <c r="M106" s="42" t="s">
+        <v>67</v>
+      </c>
+      <c r="N106" s="53">
+        <v>-94.199996999999996</v>
+      </c>
+      <c r="O106" s="1">
+        <f t="shared" si="14"/>
+        <v>-0.94199996999999991</v>
+      </c>
+      <c r="P106" s="58">
+        <v>-2.81965662445027E-3</v>
+      </c>
+    </row>
+    <row r="107" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="H107">
         <v>13</v>
       </c>
-      <c r="I101" s="72">
+      <c r="I107" s="72">
         <v>1.01992383631813</v>
       </c>
-      <c r="M101" s="42" t="s">
-        <v>133</v>
-      </c>
-      <c r="N101">
+      <c r="M107" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="N107">
         <f>21.4613437652587-19</f>
         <v>2.4613437652587002</v>
       </c>
-      <c r="O101" s="1">
-        <f t="shared" si="9"/>
+      <c r="O107" s="1">
+        <f t="shared" si="14"/>
         <v>2.4613437652587004E-2</v>
       </c>
-      <c r="P101" s="58">
+      <c r="P107" s="58">
         <v>-6.8701998242329402E-3</v>
       </c>
     </row>
-    <row r="102" spans="8:16" x14ac:dyDescent="0.25">
-      <c r="H102">
+    <row r="108" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="H108">
         <v>14</v>
       </c>
-      <c r="I102" s="72">
+      <c r="I108" s="72">
         <v>1.00994172446495</v>
       </c>
-      <c r="M102" s="42" t="s">
+      <c r="M108" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="N102" s="52">
+      <c r="N108" s="52">
         <v>-0.22125272217770001</v>
-      </c>
-      <c r="O102" s="54">
-        <f>N102</f>
-        <v>-0.22125272217770001</v>
-      </c>
-      <c r="P102" s="59">
-        <v>-0.2212527222</v>
-      </c>
-    </row>
-    <row r="103" spans="8:16" x14ac:dyDescent="0.25">
-      <c r="M103" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="N103" s="52">
-        <v>1.0099999973080001</v>
-      </c>
-      <c r="O103" s="54">
-        <f>N103</f>
-        <v>1.0099999973080001</v>
-      </c>
-      <c r="P103" s="59">
-        <v>2.17540256007367E-2</v>
-      </c>
-    </row>
-    <row r="104" spans="8:16" x14ac:dyDescent="0.25">
-      <c r="L104" t="s">
-        <v>145</v>
-      </c>
-      <c r="M104" s="42" t="s">
-        <v>68</v>
-      </c>
-      <c r="N104" s="52">
-        <v>4.9650161007164098</v>
-      </c>
-      <c r="O104" s="1">
-        <f>N104/100</f>
-        <v>4.9650161007164101E-2</v>
-      </c>
-      <c r="P104" s="58">
-        <v>1.15284947015369E-4</v>
-      </c>
-    </row>
-    <row r="105" spans="8:16" x14ac:dyDescent="0.25">
-      <c r="L105" s="56" t="s">
-        <v>150</v>
-      </c>
-      <c r="M105" s="42" t="s">
-        <v>134</v>
-      </c>
-      <c r="N105" s="52">
-        <v>0.52427629116916796</v>
-      </c>
-      <c r="O105" s="1">
-        <f t="shared" ref="O105:O107" si="10">N105/100</f>
-        <v>5.2427629116916794E-3</v>
-      </c>
-      <c r="P105" s="58">
-        <v>6.2348925580496799E-4</v>
-      </c>
-    </row>
-    <row r="106" spans="8:16" x14ac:dyDescent="0.25">
-      <c r="M106" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="N106" s="52">
-        <v>-13.5</v>
-      </c>
-      <c r="O106" s="1">
-        <f t="shared" si="10"/>
-        <v>-0.13500000000000001</v>
-      </c>
-      <c r="P106" s="58">
-        <v>-1.30914832287277E-5</v>
-      </c>
-    </row>
-    <row r="107" spans="8:16" x14ac:dyDescent="0.25">
-      <c r="M107" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="N107" s="52">
-        <v>-5.8</v>
-      </c>
-      <c r="O107" s="1">
-        <f t="shared" si="10"/>
-        <v>-5.7999999999999996E-2</v>
-      </c>
-      <c r="P107" s="58">
-        <v>1.15841086511394E-4</v>
-      </c>
-    </row>
-    <row r="108" spans="8:16" x14ac:dyDescent="0.25">
-      <c r="M108" s="42" t="s">
-        <v>55</v>
-      </c>
-      <c r="N108" s="52">
-        <v>-0.25510563387813501</v>
       </c>
       <c r="O108" s="54">
         <f>N108</f>
-        <v>-0.25510563387813501</v>
+        <v>-0.22125272217770001</v>
       </c>
       <c r="P108" s="59">
-        <v>-0.25510563390000002</v>
+        <v>-0.2212527222</v>
       </c>
     </row>
     <row r="109" spans="8:16" x14ac:dyDescent="0.25">
       <c r="M109" s="42" t="s">
-        <v>114</v>
+        <v>27</v>
       </c>
       <c r="N109" s="52">
-        <v>1.0385379019832599</v>
+        <v>1.0099999973080001</v>
       </c>
       <c r="O109" s="54">
         <f>N109</f>
-        <v>1.0385379019832599</v>
+        <v>1.0099999973080001</v>
       </c>
       <c r="P109" s="59">
-        <v>-5.12238863404413E-3</v>
+        <v>2.17540256007367E-2</v>
       </c>
     </row>
     <row r="110" spans="8:16" x14ac:dyDescent="0.25">
       <c r="L110" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="M110" s="42" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="N110" s="52">
-        <v>-2.8744036925517298</v>
+        <v>4.9650161007164098</v>
       </c>
       <c r="O110" s="1">
         <f>N110/100</f>
-        <v>-2.8744036925517299E-2</v>
+        <v>4.9650161007164101E-2</v>
       </c>
       <c r="P110" s="58">
-        <v>-9.7142222335186394E-5</v>
+        <v>1.15284947015369E-4</v>
       </c>
     </row>
     <row r="111" spans="8:16" x14ac:dyDescent="0.25">
       <c r="L111" s="56" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="M111" s="42" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="N111" s="52">
-        <v>0.31779049296478201</v>
+        <v>0.52427629116916796</v>
       </c>
       <c r="O111" s="1">
-        <f t="shared" ref="O111:O113" si="11">N111/100</f>
-        <v>3.1779049296478202E-3</v>
+        <f t="shared" ref="O111:O113" si="15">N111/100</f>
+        <v>5.2427629116916794E-3</v>
       </c>
       <c r="P111" s="58">
-        <v>-1.0332946463634299E-3</v>
+        <v>6.2348925580496799E-4</v>
       </c>
     </row>
     <row r="112" spans="8:16" x14ac:dyDescent="0.25">
       <c r="M112" s="42" t="s">
-        <v>70</v>
+        <v>16</v>
       </c>
       <c r="N112" s="52">
-        <v>-14.9</v>
+        <v>-13.5</v>
       </c>
       <c r="O112" s="1">
-        <f t="shared" si="11"/>
-        <v>-0.14899999999999999</v>
+        <f t="shared" si="15"/>
+        <v>-0.13500000000000001</v>
       </c>
       <c r="P112" s="58">
-        <v>-4.6294745534552998E-5</v>
-      </c>
-    </row>
-    <row r="113" spans="13:16" x14ac:dyDescent="0.25">
+        <v>-1.30914832287277E-5</v>
+      </c>
+    </row>
+    <row r="113" spans="12:16" x14ac:dyDescent="0.25">
       <c r="M113" s="42" t="s">
-        <v>136</v>
+        <v>22</v>
       </c>
       <c r="N113" s="52">
-        <v>-5</v>
+        <v>-5.8</v>
       </c>
       <c r="O113" s="1">
-        <f t="shared" si="11"/>
-        <v>-0.05</v>
+        <f t="shared" si="15"/>
+        <v>-5.7999999999999996E-2</v>
       </c>
       <c r="P113" s="58">
-        <v>-4.2582952991622499E-5</v>
-      </c>
-    </row>
-    <row r="114" spans="13:16" x14ac:dyDescent="0.25">
+        <v>1.15841086511394E-4</v>
+      </c>
+    </row>
+    <row r="114" spans="12:16" x14ac:dyDescent="0.25">
       <c r="M114" s="42" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="N114" s="52">
-        <v>-0.26806990591321</v>
+        <v>-0.25510563387813501</v>
       </c>
       <c r="O114" s="54">
         <f>N114</f>
-        <v>-0.26806990591321</v>
+        <v>-0.25510563387813501</v>
       </c>
       <c r="P114" s="59">
-        <v>-0.26806990590000002</v>
-      </c>
-    </row>
-    <row r="115" spans="13:16" x14ac:dyDescent="0.25">
+        <v>-0.25510563390000002</v>
+      </c>
+    </row>
+    <row r="115" spans="12:16" x14ac:dyDescent="0.25">
       <c r="M115" s="42" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="N115" s="52">
-        <v>1.0349152577221601</v>
+        <v>1.0385379019832599</v>
       </c>
       <c r="O115" s="54">
         <f>N115</f>
+        <v>1.0385379019832599</v>
+      </c>
+      <c r="P115" s="59">
+        <v>-5.12238863404413E-3</v>
+      </c>
+    </row>
+    <row r="116" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L116" t="s">
+        <v>145</v>
+      </c>
+      <c r="M116" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="N116" s="52">
+        <v>-2.8744036925517298</v>
+      </c>
+      <c r="O116" s="1">
+        <f>N116/100</f>
+        <v>-2.8744036925517299E-2</v>
+      </c>
+      <c r="P116" s="58">
+        <v>-9.7142222335186394E-5</v>
+      </c>
+    </row>
+    <row r="117" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L117" s="56" t="s">
+        <v>150</v>
+      </c>
+      <c r="M117" s="42" t="s">
+        <v>134</v>
+      </c>
+      <c r="N117" s="52">
+        <v>0.31779049296478201</v>
+      </c>
+      <c r="O117" s="1">
+        <f t="shared" ref="O117:O119" si="16">N117/100</f>
+        <v>3.1779049296478202E-3</v>
+      </c>
+      <c r="P117" s="58">
+        <v>-1.0332946463634299E-3</v>
+      </c>
+    </row>
+    <row r="118" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M118" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="N118" s="52">
+        <v>-14.9</v>
+      </c>
+      <c r="O118" s="1">
+        <f t="shared" si="16"/>
+        <v>-0.14899999999999999</v>
+      </c>
+      <c r="P118" s="58">
+        <v>-4.6294745534552998E-5</v>
+      </c>
+    </row>
+    <row r="119" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M119" s="42" t="s">
+        <v>135</v>
+      </c>
+      <c r="N119" s="52">
+        <v>-5</v>
+      </c>
+      <c r="O119" s="1">
+        <f t="shared" si="16"/>
+        <v>-0.05</v>
+      </c>
+      <c r="P119" s="58">
+        <v>-4.2582952991622499E-5</v>
+      </c>
+    </row>
+    <row r="120" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M120" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="N120" s="52">
+        <v>-0.26806990591321</v>
+      </c>
+      <c r="O120" s="54">
+        <f>N120</f>
+        <v>-0.26806990591321</v>
+      </c>
+      <c r="P120" s="59">
+        <v>-0.26806990590000002</v>
+      </c>
+    </row>
+    <row r="121" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M121" s="42" t="s">
+        <v>115</v>
+      </c>
+      <c r="N121" s="52">
         <v>1.0349152577221601</v>
       </c>
-      <c r="P115" s="59">
+      <c r="O121" s="54">
+        <f>N121</f>
+        <v>1.0349152577221601</v>
+      </c>
+      <c r="P121" s="59">
         <v>-2.1765958813597698E-3</v>
       </c>
     </row>
-    <row r="116" spans="13:16" x14ac:dyDescent="0.25">
-      <c r="O116" s="1"/>
-      <c r="P116" s="3"/>
-    </row>
-    <row r="117" spans="13:16" x14ac:dyDescent="0.25">
-      <c r="M117" s="48"/>
-      <c r="N117" s="48"/>
-      <c r="O117" s="1"/>
-      <c r="P117" s="3"/>
-    </row>
-    <row r="118" spans="13:16" x14ac:dyDescent="0.25">
-      <c r="M118" s="48"/>
-      <c r="N118" s="47"/>
-      <c r="P118" s="3"/>
-    </row>
-    <row r="119" spans="13:16" x14ac:dyDescent="0.25">
-      <c r="M119" s="48"/>
-      <c r="N119" s="47"/>
-      <c r="P119" s="3"/>
-    </row>
-    <row r="120" spans="13:16" x14ac:dyDescent="0.25">
-      <c r="M120" s="48"/>
-      <c r="N120" s="47"/>
-    </row>
-    <row r="121" spans="13:16" x14ac:dyDescent="0.25">
-      <c r="M121" s="42"/>
-      <c r="N121" s="1"/>
-    </row>
-    <row r="122" spans="13:16" x14ac:dyDescent="0.25">
-      <c r="M122" s="42"/>
-      <c r="N122" s="1"/>
-    </row>
-    <row r="123" spans="13:16" x14ac:dyDescent="0.25">
-      <c r="M123" s="42"/>
-      <c r="N123" s="1"/>
-    </row>
-    <row r="124" spans="13:16" x14ac:dyDescent="0.25">
-      <c r="M124" s="42"/>
-      <c r="N124" s="1"/>
-    </row>
-    <row r="125" spans="13:16" x14ac:dyDescent="0.25">
-      <c r="M125" s="42"/>
-      <c r="N125" s="1"/>
-    </row>
-    <row r="126" spans="13:16" x14ac:dyDescent="0.25">
-      <c r="M126" s="42"/>
-      <c r="N126" s="1"/>
-    </row>
-    <row r="127" spans="13:16" x14ac:dyDescent="0.25">
+    <row r="122" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="O122" s="1"/>
+      <c r="P122" s="3"/>
+    </row>
+    <row r="123" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M123" s="48"/>
+      <c r="N123" s="48"/>
+      <c r="O123" s="1"/>
+      <c r="P123" s="3"/>
+    </row>
+    <row r="124" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M124" s="48"/>
+      <c r="N124" s="47"/>
+      <c r="P124" s="3"/>
+    </row>
+    <row r="125" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M125" s="48"/>
+      <c r="N125" s="47"/>
+      <c r="P125" s="3"/>
+    </row>
+    <row r="126" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M126" s="48"/>
+      <c r="N126" s="47"/>
+    </row>
+    <row r="127" spans="12:16" x14ac:dyDescent="0.25">
       <c r="M127" s="42"/>
       <c r="N127" s="1"/>
     </row>
-    <row r="128" spans="13:16" x14ac:dyDescent="0.25">
+    <row r="128" spans="12:16" x14ac:dyDescent="0.25">
       <c r="M128" s="42"/>
       <c r="N128" s="1"/>
     </row>
@@ -9125,6 +9485,30 @@
     <row r="140" spans="13:14" x14ac:dyDescent="0.25">
       <c r="M140" s="42"/>
       <c r="N140" s="1"/>
+    </row>
+    <row r="141" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M141" s="42"/>
+      <c r="N141" s="1"/>
+    </row>
+    <row r="142" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M142" s="42"/>
+      <c r="N142" s="1"/>
+    </row>
+    <row r="143" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M143" s="42"/>
+      <c r="N143" s="1"/>
+    </row>
+    <row r="144" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M144" s="42"/>
+      <c r="N144" s="1"/>
+    </row>
+    <row r="145" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M145" s="42"/>
+      <c r="N145" s="1"/>
+    </row>
+    <row r="146" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M146" s="42"/>
+      <c r="N146" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -9156,18 +9540,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="84" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="83"/>
-      <c r="G1" s="83"/>
-      <c r="H1" s="83"/>
-      <c r="I1" s="83"/>
-      <c r="J1" s="83"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
       <c r="L1" s="11" t="s">
         <v>1</v>
       </c>
@@ -9191,18 +9575,18 @@
       <c r="B2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="84" t="s">
+      <c r="C2" s="85" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84" t="s">
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85" t="s">
         <v>74</v>
       </c>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
       <c r="L2" s="8" t="s">
         <v>41</v>
       </c>
@@ -9995,18 +10379,18 @@
       <c r="O33" s="1"/>
     </row>
     <row r="35" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="83" t="s">
+      <c r="A35" s="84" t="s">
         <v>78</v>
       </c>
-      <c r="B35" s="83"/>
-      <c r="C35" s="83"/>
-      <c r="D35" s="83"/>
-      <c r="E35" s="83"/>
-      <c r="F35" s="83"/>
-      <c r="G35" s="83"/>
-      <c r="H35" s="83"/>
-      <c r="I35" s="83"/>
-      <c r="J35" s="83"/>
+      <c r="B35" s="84"/>
+      <c r="C35" s="84"/>
+      <c r="D35" s="84"/>
+      <c r="E35" s="84"/>
+      <c r="F35" s="84"/>
+      <c r="G35" s="84"/>
+      <c r="H35" s="84"/>
+      <c r="I35" s="84"/>
+      <c r="J35" s="84"/>
       <c r="L35" s="11" t="s">
         <v>1</v>
       </c>
@@ -14854,7 +15238,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="73" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B1" s="77">
         <v>1</v>
@@ -14888,7 +15272,7 @@
       <c r="N1" s="74"/>
       <c r="O1" s="74"/>
       <c r="Q1" s="74" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -15263,7 +15647,7 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="73" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B14" s="77">
         <v>2</v>
@@ -15308,7 +15692,7 @@
         <v>9</v>
       </c>
       <c r="Q14" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -15971,7 +16355,7 @@
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="73" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B31" s="77">
         <v>6</v>
@@ -16004,7 +16388,7 @@
         <v>14</v>
       </c>
       <c r="Q31" s="72" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
@@ -16511,7 +16895,7 @@
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="73" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B48" s="77">
         <v>9</v>
@@ -16544,7 +16928,7 @@
         <v>14</v>
       </c>
       <c r="Q48" s="72" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
@@ -16860,46 +17244,46 @@
   <sheetData>
     <row r="1" spans="1:18" s="72" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="72" t="s">
+        <v>187</v>
+      </c>
+      <c r="B1" s="72" t="s">
+        <v>186</v>
+      </c>
+      <c r="D1" s="72" t="s">
+        <v>187</v>
+      </c>
+      <c r="E1" s="72" t="s">
         <v>188</v>
       </c>
-      <c r="B1" s="72" t="s">
+      <c r="F1" s="72" t="s">
+        <v>201</v>
+      </c>
+      <c r="H1" s="72" t="s">
         <v>187</v>
       </c>
-      <c r="D1" s="72" t="s">
-        <v>188</v>
-      </c>
-      <c r="E1" s="72" t="s">
+      <c r="I1" s="72" t="s">
         <v>189</v>
       </c>
-      <c r="F1" s="72" t="s">
-        <v>202</v>
-      </c>
-      <c r="H1" s="72" t="s">
-        <v>188</v>
-      </c>
-      <c r="I1" s="72" t="s">
+      <c r="J1" s="72" t="s">
+        <v>201</v>
+      </c>
+      <c r="L1" s="72" t="s">
+        <v>187</v>
+      </c>
+      <c r="M1" s="72" t="s">
         <v>190</v>
       </c>
-      <c r="J1" s="72" t="s">
-        <v>202</v>
-      </c>
-      <c r="L1" s="72" t="s">
-        <v>188</v>
-      </c>
-      <c r="M1" s="72" t="s">
+      <c r="N1" s="72" t="s">
+        <v>201</v>
+      </c>
+      <c r="P1" s="72" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q1" s="72" t="s">
         <v>191</v>
       </c>
-      <c r="N1" s="72" t="s">
-        <v>202</v>
-      </c>
-      <c r="P1" s="72" t="s">
-        <v>188</v>
-      </c>
-      <c r="Q1" s="72" t="s">
-        <v>192</v>
-      </c>
       <c r="R1" s="72" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -16918,7 +17302,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="72" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H2" s="72">
         <v>9</v>
@@ -16927,7 +17311,7 @@
         <v>0</v>
       </c>
       <c r="J2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L2" s="72">
         <v>15</v>
@@ -16936,7 +17320,7 @@
         <v>0</v>
       </c>
       <c r="N2" s="72" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="P2" s="72">
         <v>25</v>
@@ -16945,7 +17329,7 @@
         <v>0</v>
       </c>
       <c r="R2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -16964,7 +17348,7 @@
         <v>-2.64000000000006E-2</v>
       </c>
       <c r="F3" s="72" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H3" s="72">
         <f t="shared" ref="H3:H15" si="0">H2+1</f>
@@ -16974,7 +17358,7 @@
         <v>-6.4000000000001799E-3</v>
       </c>
       <c r="J3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L3" s="72">
         <f t="shared" ref="L3:L15" si="1">L2+1</f>
@@ -16984,7 +17368,7 @@
         <v>0</v>
       </c>
       <c r="N3" s="72" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="P3" s="72">
         <f t="shared" ref="P3:P9" si="2">P2+1</f>
@@ -16994,7 +17378,7 @@
         <v>0</v>
       </c>
       <c r="R3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -17013,7 +17397,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="72" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H4" s="72">
         <f t="shared" si="0"/>
@@ -17023,7 +17407,7 @@
         <v>0</v>
       </c>
       <c r="J4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L4" s="72">
         <f t="shared" si="1"/>
@@ -17033,7 +17417,7 @@
         <v>0</v>
       </c>
       <c r="N4" s="72" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="P4" s="72">
         <f t="shared" si="2"/>
@@ -17043,7 +17427,7 @@
         <v>0</v>
       </c>
       <c r="R4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -17062,7 +17446,7 @@
         <v>-2.4600000000000399E-2</v>
       </c>
       <c r="F5" s="72" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H5" s="72">
         <f t="shared" si="0"/>
@@ -17072,7 +17456,7 @@
         <v>0</v>
       </c>
       <c r="J5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L5" s="72">
         <f t="shared" si="1"/>
@@ -17082,7 +17466,7 @@
         <v>0</v>
       </c>
       <c r="N5" s="72" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="P5" s="72">
         <f t="shared" si="2"/>
@@ -17092,7 +17476,7 @@
         <v>0</v>
       </c>
       <c r="R5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -17111,7 +17495,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="72" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H6" s="72">
         <f t="shared" si="0"/>
@@ -17121,7 +17505,7 @@
         <v>0</v>
       </c>
       <c r="J6" s="72" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L6" s="72">
         <f t="shared" si="1"/>
@@ -17131,7 +17515,7 @@
         <v>0</v>
       </c>
       <c r="N6" s="72" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="P6" s="72">
         <v>43</v>
@@ -17140,7 +17524,7 @@
         <v>0</v>
       </c>
       <c r="R6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -17159,7 +17543,7 @@
         <v>-1.7299999999999701E-2</v>
       </c>
       <c r="F7" s="72" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H7" s="72">
         <f t="shared" si="0"/>
@@ -17169,7 +17553,7 @@
         <v>0</v>
       </c>
       <c r="J7" s="72" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L7" s="72">
         <f t="shared" si="1"/>
@@ -17179,7 +17563,7 @@
         <v>0</v>
       </c>
       <c r="N7" s="72" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="P7" s="72">
         <f t="shared" si="2"/>
@@ -17189,7 +17573,7 @@
         <v>0</v>
       </c>
       <c r="R7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -17208,7 +17592,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H8" s="72">
         <v>31</v>
@@ -17217,7 +17601,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="72" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L8" s="72">
         <f t="shared" si="1"/>
@@ -17227,7 +17611,7 @@
         <v>0</v>
       </c>
       <c r="N8" s="72" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="P8" s="72">
         <f t="shared" si="2"/>
@@ -17237,7 +17621,7 @@
         <v>0</v>
       </c>
       <c r="R8" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -17256,7 +17640,7 @@
         <v>-5.1000000000001003E-2</v>
       </c>
       <c r="F9" s="72" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H9" s="72">
         <f t="shared" si="0"/>
@@ -17266,7 +17650,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="72" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L9" s="72">
         <f t="shared" si="1"/>
@@ -17276,7 +17660,7 @@
         <v>0</v>
       </c>
       <c r="N9" s="72" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="P9" s="72">
         <f t="shared" si="2"/>
@@ -17286,7 +17670,7 @@
         <v>-9.9999999999766901E-5</v>
       </c>
       <c r="R9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -17304,7 +17688,7 @@
         <v>-1.7763568394002501E-15</v>
       </c>
       <c r="F10" s="68" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H10" s="72">
         <f t="shared" si="0"/>
@@ -17314,7 +17698,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="72" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L10" s="72">
         <f t="shared" si="1"/>
@@ -17324,7 +17708,7 @@
         <v>0</v>
       </c>
       <c r="N10" s="72" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -17343,7 +17727,7 @@
         <v>-4.18999999999983E-2</v>
       </c>
       <c r="F11" s="72" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H11" s="72">
         <f t="shared" si="0"/>
@@ -17353,7 +17737,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="72" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L11" s="72">
         <f t="shared" si="1"/>
@@ -17363,7 +17747,7 @@
         <v>-9.9999999999766901E-5</v>
       </c>
       <c r="N11" s="68" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
@@ -17382,7 +17766,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="72" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L12" s="72">
         <v>39</v>
@@ -17391,7 +17775,7 @@
         <v>0</v>
       </c>
       <c r="N12" s="72" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -17410,7 +17794,7 @@
         <v>0</v>
       </c>
       <c r="J13" s="72" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L13" s="72">
         <f t="shared" si="1"/>
@@ -17420,7 +17804,7 @@
         <v>0</v>
       </c>
       <c r="N13" s="72" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
@@ -17439,7 +17823,7 @@
         <v>0</v>
       </c>
       <c r="J14" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="L14" s="72">
         <f t="shared" si="1"/>
@@ -17449,7 +17833,7 @@
         <v>4.4408920985006301E-16</v>
       </c>
       <c r="N14" s="68" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
@@ -17468,7 +17852,7 @@
         <v>-2.83000000000007E-2</v>
       </c>
       <c r="J15" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L15" s="72">
         <f t="shared" si="1"/>
@@ -17478,7 +17862,7 @@
         <v>-1.00000000000211E-4</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added meas for line 2-5. SE results for small partition is not the same as for overall system.
Added measurements for line 2-5. For some reason, the SE results for the
entire system is not the same as the SE results for the small individual
systems. Does that make sense?
</commit_message>
<xml_diff>
--- a/DMASE - Test Results.xlsx
+++ b/DMASE - Test Results.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="938" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="941" uniqueCount="274">
   <si>
     <t>Abur 3-Bus Case Measurements (run through SE, rerun new estimate again)</t>
   </si>
@@ -839,6 +839,12 @@
   </si>
   <si>
     <t>P5-4 = -P4-5</t>
+  </si>
+  <si>
+    <t>x2+slack2</t>
+  </si>
+  <si>
+    <t>Central - (x2+slack2)</t>
   </si>
 </sst>
 </file>
@@ -1265,6 +1271,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1286,10 +1296,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1610,15 +1616,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="86" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
+      <c r="B1" s="86"/>
+      <c r="C1" s="86"/>
+      <c r="D1" s="86"/>
+      <c r="E1" s="86"/>
+      <c r="F1" s="86"/>
+      <c r="G1" s="86"/>
       <c r="I1" s="6" t="s">
         <v>1</v>
       </c>
@@ -1847,10 +1853,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S57"/>
+  <dimension ref="A1:S59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1877,78 +1883,78 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="90" t="s">
         <v>222</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
-      <c r="D1" s="88"/>
-      <c r="F1" s="86" t="s">
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="92"/>
+      <c r="F1" s="90" t="s">
         <v>228</v>
       </c>
-      <c r="G1" s="87"/>
-      <c r="H1" s="87"/>
-      <c r="I1" s="88"/>
-      <c r="K1" s="86" t="s">
+      <c r="G1" s="91"/>
+      <c r="H1" s="91"/>
+      <c r="I1" s="92"/>
+      <c r="K1" s="90" t="s">
         <v>229</v>
       </c>
-      <c r="L1" s="87"/>
-      <c r="M1" s="87"/>
-      <c r="N1" s="88"/>
-      <c r="P1" s="86" t="s">
+      <c r="L1" s="91"/>
+      <c r="M1" s="91"/>
+      <c r="N1" s="92"/>
+      <c r="P1" s="90" t="s">
         <v>230</v>
       </c>
-      <c r="Q1" s="87"/>
-      <c r="R1" s="87"/>
-      <c r="S1" s="88"/>
+      <c r="Q1" s="91"/>
+      <c r="R1" s="91"/>
+      <c r="S1" s="92"/>
     </row>
     <row r="2" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="89" t="s">
+      <c r="A2" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="90" t="s">
+      <c r="B2" s="83" t="s">
         <v>223</v>
       </c>
-      <c r="C2" s="90" t="s">
+      <c r="C2" s="83" t="s">
         <v>224</v>
       </c>
-      <c r="D2" s="91" t="s">
+      <c r="D2" s="84" t="s">
         <v>225</v>
       </c>
-      <c r="F2" s="89" t="s">
+      <c r="F2" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="90" t="s">
+      <c r="G2" s="83" t="s">
         <v>223</v>
       </c>
-      <c r="H2" s="90" t="s">
+      <c r="H2" s="83" t="s">
         <v>224</v>
       </c>
-      <c r="I2" s="91" t="s">
+      <c r="I2" s="84" t="s">
         <v>225</v>
       </c>
-      <c r="K2" s="89" t="s">
+      <c r="K2" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="90" t="s">
+      <c r="L2" s="83" t="s">
         <v>223</v>
       </c>
-      <c r="M2" s="90" t="s">
+      <c r="M2" s="83" t="s">
         <v>224</v>
       </c>
-      <c r="N2" s="91" t="s">
+      <c r="N2" s="84" t="s">
         <v>225</v>
       </c>
-      <c r="P2" s="89" t="s">
+      <c r="P2" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="Q2" s="90" t="s">
+      <c r="Q2" s="83" t="s">
         <v>223</v>
       </c>
-      <c r="R2" s="90" t="s">
+      <c r="R2" s="83" t="s">
         <v>224</v>
       </c>
-      <c r="S2" s="91" t="s">
+      <c r="S2" s="84" t="s">
         <v>225</v>
       </c>
     </row>
@@ -2129,15 +2135,15 @@
       </c>
     </row>
     <row r="7" spans="1:19" s="72" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="74" t="s">
-        <v>26</v>
+      <c r="A7" s="20" t="s">
+        <v>48</v>
       </c>
       <c r="B7" s="72">
-        <v>1.0599999427795399</v>
+        <v>41.338725991097199</v>
       </c>
       <c r="C7" s="20">
-        <f>B7</f>
-        <v>1.0599999427795399</v>
+        <f>B7/100</f>
+        <v>0.41338725991097197</v>
       </c>
       <c r="D7" s="74"/>
       <c r="F7" s="20" t="s">
@@ -2173,15 +2179,15 @@
       </c>
     </row>
     <row r="8" spans="1:19" s="72" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="74" t="s">
-        <v>28</v>
+      <c r="A8" s="20" t="s">
+        <v>118</v>
       </c>
       <c r="B8" s="72">
-        <v>1.04499995797579</v>
+        <v>-3.8398609004379098</v>
       </c>
       <c r="C8" s="20">
-        <f t="shared" ref="C8:C9" si="4">B8</f>
-        <v>1.04499995797579</v>
+        <f>B8/100</f>
+        <v>-3.8398609004379101E-2</v>
       </c>
       <c r="D8" s="74"/>
       <c r="F8" s="20" t="s">
@@ -2212,20 +2218,20 @@
         <v>1.02798621556374</v>
       </c>
       <c r="R8" s="72">
-        <f t="shared" ref="R8:R9" si="5">Q8</f>
+        <f t="shared" ref="R8:R9" si="4">Q8</f>
         <v>1.02798621556374</v>
       </c>
     </row>
     <row r="9" spans="1:19" s="72" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="74" t="s">
-        <v>210</v>
+        <v>26</v>
       </c>
       <c r="B9" s="72">
-        <v>1.0280925147905799</v>
+        <v>1.0599999427795399</v>
       </c>
       <c r="C9" s="20">
-        <f t="shared" si="4"/>
-        <v>1.0280925147905799</v>
+        <f>B9</f>
+        <v>1.0599999427795399</v>
       </c>
       <c r="D9" s="74"/>
       <c r="F9" s="20" t="s">
@@ -2256,20 +2262,20 @@
         <v>1.00994172446495</v>
       </c>
       <c r="R9" s="72">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.00994172446495</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="74" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="B10" s="72">
-        <v>232.35762119293199</v>
-      </c>
-      <c r="C10" s="74">
-        <f>B10/100</f>
-        <v>2.32357621192932</v>
+        <v>1.04499995797579</v>
+      </c>
+      <c r="C10" s="20">
+        <f t="shared" ref="C10:C11" si="5">B10</f>
+        <v>1.04499995797579</v>
       </c>
       <c r="D10" s="74"/>
       <c r="F10" s="20" t="s">
@@ -2306,14 +2312,14 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="74" t="s">
-        <v>83</v>
+        <v>210</v>
       </c>
       <c r="B11" s="72">
-        <v>-20.456442236900301</v>
-      </c>
-      <c r="C11" s="74">
-        <f t="shared" ref="C11:C21" si="8">B11/100</f>
-        <v>-0.20456442236900302</v>
+        <v>1.0280925147905799</v>
+      </c>
+      <c r="C11" s="20">
+        <f t="shared" si="5"/>
+        <v>1.0280925147905799</v>
       </c>
       <c r="D11" s="74"/>
       <c r="F11" s="20" t="s">
@@ -2344,21 +2350,20 @@
         <v>-16.599999</v>
       </c>
       <c r="R11" s="72">
-        <f t="shared" ref="R11:R21" si="9">Q11/100</f>
+        <f t="shared" ref="R11:R21" si="8">Q11/100</f>
         <v>-0.16599999000000001</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="74" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="B12" s="72">
-        <f>40.0000005960464-21.699999</f>
-        <v>18.3000015960464</v>
+        <v>232.35762119293199</v>
       </c>
       <c r="C12" s="74">
-        <f t="shared" si="8"/>
-        <v>0.183000015960464</v>
+        <f>B12/100</f>
+        <v>2.32357621192932</v>
       </c>
       <c r="D12" s="74"/>
       <c r="F12" s="20" t="s">
@@ -2389,21 +2394,20 @@
         <v>-9</v>
       </c>
       <c r="R12" s="72">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>-0.09</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="74" t="s">
-        <v>24</v>
+        <v>83</v>
       </c>
       <c r="B13" s="72">
-        <f>34.8948746919631-12.7</f>
-        <v>22.194874691963104</v>
+        <v>-20.456442236900301</v>
       </c>
       <c r="C13" s="74">
-        <f t="shared" si="8"/>
-        <v>0.22194874691963104</v>
+        <f t="shared" ref="C13:C23" si="9">B13/100</f>
+        <v>-0.20456442236900302</v>
       </c>
       <c r="D13" s="74"/>
       <c r="F13" s="20" t="s">
@@ -2434,20 +2438,21 @@
         <v>-5.8</v>
       </c>
       <c r="R13" s="72">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>-5.7999999999999996E-2</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="74" t="s">
-        <v>63</v>
-      </c>
-      <c r="B14" s="74">
-        <v>-7.6</v>
+        <v>18</v>
+      </c>
+      <c r="B14" s="72">
+        <f>40.0000005960464-21.699999</f>
+        <v>18.3000015960464</v>
       </c>
       <c r="C14" s="74">
-        <f t="shared" si="8"/>
-        <v>-7.5999999999999998E-2</v>
+        <f t="shared" si="9"/>
+        <v>0.183000015960464</v>
       </c>
       <c r="D14" s="74"/>
       <c r="F14" s="20" t="s">
@@ -2480,20 +2485,21 @@
         <v>-14.9</v>
       </c>
       <c r="R14" s="72">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>-0.14899999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="74" t="s">
-        <v>128</v>
-      </c>
-      <c r="B15" s="20">
-        <v>-1.6</v>
+        <v>24</v>
+      </c>
+      <c r="B15" s="72">
+        <f>34.8948746919631-12.7</f>
+        <v>22.194874691963104</v>
       </c>
       <c r="C15" s="74">
-        <f t="shared" si="8"/>
-        <v>-1.6E-2</v>
+        <f t="shared" si="9"/>
+        <v>0.22194874691963104</v>
       </c>
       <c r="D15" s="74"/>
       <c r="F15" s="20" t="s">
@@ -2524,24 +2530,22 @@
         <v>-5</v>
       </c>
       <c r="R15" s="72">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>-0.05</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="74" t="s">
-        <v>206</v>
-      </c>
-      <c r="B16" s="72">
-        <v>72.934574594694098</v>
+        <v>63</v>
+      </c>
+      <c r="B16" s="74">
+        <v>-7.6</v>
       </c>
       <c r="C16" s="74">
-        <f t="shared" si="8"/>
-        <v>0.72934574594694102</v>
-      </c>
-      <c r="D16" s="74" t="s">
-        <v>227</v>
-      </c>
+        <f t="shared" si="9"/>
+        <v>-7.5999999999999998E-2</v>
+      </c>
+      <c r="D16" s="74"/>
       <c r="F16" s="20" t="s">
         <v>234</v>
       </c>
@@ -2570,7 +2574,7 @@
         <v>-29.247637436823101</v>
       </c>
       <c r="R16" s="72">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>-0.29247637436823104</v>
       </c>
       <c r="S16" s="74" t="s">
@@ -2579,18 +2583,16 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="74" t="s">
-        <v>207</v>
-      </c>
-      <c r="B17" s="72">
-        <v>3.5900360862934599</v>
+        <v>128</v>
+      </c>
+      <c r="B17" s="20">
+        <v>-1.6</v>
       </c>
       <c r="C17" s="74">
-        <f t="shared" si="8"/>
-        <v>3.5900360862934598E-2</v>
-      </c>
-      <c r="D17" s="74" t="s">
-        <v>227</v>
-      </c>
+        <f t="shared" si="9"/>
+        <v>-1.6E-2</v>
+      </c>
+      <c r="D17" s="74"/>
       <c r="F17" s="20" t="s">
         <v>235</v>
       </c>
@@ -2619,7 +2621,7 @@
         <v>-11.0919776937066</v>
       </c>
       <c r="R17" s="72">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>-0.11091977693706599</v>
       </c>
       <c r="S17" s="74" t="s">
@@ -2627,17 +2629,17 @@
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18" s="92" t="s">
-        <v>50</v>
-      </c>
-      <c r="B18" s="2">
-        <v>63.520589529047797</v>
-      </c>
-      <c r="C18" s="92">
-        <f>B18/100</f>
-        <v>0.635205895290478</v>
-      </c>
-      <c r="D18" s="92" t="s">
+      <c r="A18" s="74" t="s">
+        <v>206</v>
+      </c>
+      <c r="B18" s="72">
+        <v>72.934574594694098</v>
+      </c>
+      <c r="C18" s="74">
+        <f t="shared" si="9"/>
+        <v>0.72934574594694102</v>
+      </c>
+      <c r="D18" s="74" t="s">
         <v>227</v>
       </c>
       <c r="F18" s="20" t="s">
@@ -2668,7 +2670,7 @@
         <v>-2.8744036925517298</v>
       </c>
       <c r="R18" s="72">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>-2.8744036925517299E-2</v>
       </c>
       <c r="S18" s="74" t="s">
@@ -2676,17 +2678,17 @@
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="92" t="s">
-        <v>226</v>
-      </c>
-      <c r="B19" s="2">
-        <v>-8.5672111358111902</v>
-      </c>
-      <c r="C19" s="92">
-        <f>B19/100</f>
-        <v>-8.5672111358111896E-2</v>
-      </c>
-      <c r="D19" s="92" t="s">
+      <c r="A19" s="74" t="s">
+        <v>207</v>
+      </c>
+      <c r="B19" s="72">
+        <v>3.5900360862934599</v>
+      </c>
+      <c r="C19" s="74">
+        <f t="shared" si="9"/>
+        <v>3.5900360862934598E-2</v>
+      </c>
+      <c r="D19" s="74" t="s">
         <v>227</v>
       </c>
       <c r="F19" s="20" t="s">
@@ -2717,7 +2719,7 @@
         <v>0.31779049296478201</v>
       </c>
       <c r="R19" s="72">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>3.1779049296478202E-3</v>
       </c>
       <c r="S19" s="74" t="s">
@@ -2725,17 +2727,17 @@
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="74" t="s">
-        <v>204</v>
-      </c>
-      <c r="B20" s="72">
-        <v>42.467165475154701</v>
-      </c>
-      <c r="C20" s="74">
-        <f t="shared" si="8"/>
-        <v>0.424671654751547</v>
-      </c>
-      <c r="D20" s="74" t="s">
+      <c r="A20" s="85" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="2">
+        <v>63.520589529047797</v>
+      </c>
+      <c r="C20" s="85">
+        <f>B20/100</f>
+        <v>0.635205895290478</v>
+      </c>
+      <c r="D20" s="85" t="s">
         <v>227</v>
       </c>
       <c r="F20" s="20" t="s">
@@ -2766,51 +2768,51 @@
         <v>-4.9650161007164098</v>
       </c>
       <c r="R20" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>-4.9650161007164101E-2</v>
       </c>
-      <c r="S20" s="92" t="s">
+      <c r="S20" s="85" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" s="74" t="s">
-        <v>205</v>
-      </c>
-      <c r="B21" s="72">
-        <v>-2.12732489205733</v>
-      </c>
-      <c r="C21" s="74">
-        <f t="shared" si="8"/>
-        <v>-2.12732489205733E-2</v>
-      </c>
-      <c r="D21" s="74" t="s">
+      <c r="A21" s="85" t="s">
+        <v>226</v>
+      </c>
+      <c r="B21" s="2">
+        <v>-8.5672111358111902</v>
+      </c>
+      <c r="C21" s="85">
+        <f>B21/100</f>
+        <v>-8.5672111358111896E-2</v>
+      </c>
+      <c r="D21" s="85" t="s">
         <v>227</v>
       </c>
-      <c r="F21" s="92" t="s">
+      <c r="F21" s="85" t="s">
         <v>239</v>
       </c>
       <c r="G21" s="2">
         <v>-70.630210315105003</v>
       </c>
-      <c r="H21" s="92">
+      <c r="H21" s="85">
         <f>G21/100</f>
         <v>-0.70630210315105002</v>
       </c>
-      <c r="I21" s="92" t="s">
+      <c r="I21" s="85" t="s">
         <v>227</v>
       </c>
       <c r="K21" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="L21" s="72">
+      <c r="L21" s="2">
         <v>2.8808971477310599</v>
       </c>
       <c r="M21" s="2">
         <f>L21/100</f>
         <v>2.88089714773106E-2</v>
       </c>
-      <c r="N21" s="92" t="s">
+      <c r="N21" s="85" t="s">
         <v>227</v>
       </c>
       <c r="P21" s="2" t="s">
@@ -2820,42 +2822,68 @@
         <v>-0.52427629116916796</v>
       </c>
       <c r="R21" s="2">
+        <f t="shared" si="8"/>
+        <v>-5.2427629116916794E-3</v>
+      </c>
+      <c r="S21" s="85" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A22" s="74" t="s">
+        <v>204</v>
+      </c>
+      <c r="B22" s="72">
+        <v>42.467165475154701</v>
+      </c>
+      <c r="C22" s="74">
         <f t="shared" si="9"/>
-        <v>-5.2427629116916794E-3</v>
-      </c>
-      <c r="S21" s="92" t="s">
+        <v>0.424671654751547</v>
+      </c>
+      <c r="D22" s="74" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="F22" s="92" t="s">
+      <c r="F22" s="85" t="s">
         <v>257</v>
       </c>
       <c r="G22" s="2">
         <v>1.49275268307195</v>
       </c>
-      <c r="H22" s="92">
+      <c r="H22" s="85">
         <f>G22/100</f>
         <v>1.49275268307195E-2</v>
       </c>
-      <c r="I22" s="92" t="s">
+      <c r="I22" s="85" t="s">
         <v>227</v>
       </c>
       <c r="K22" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="L22" s="72">
+      <c r="L22" s="2">
         <v>-0.30259003060574602</v>
       </c>
       <c r="M22" s="2">
         <f>L22/100</f>
         <v>-3.0259003060574604E-3</v>
       </c>
-      <c r="N22" s="92" t="s">
+      <c r="N22" s="85" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A23" s="74" t="s">
+        <v>205</v>
+      </c>
+      <c r="B23" s="72">
+        <v>-2.12732489205733</v>
+      </c>
+      <c r="C23" s="74">
+        <f t="shared" si="9"/>
+        <v>-2.12732489205733E-2</v>
+      </c>
+      <c r="D23" s="74" t="s">
+        <v>227</v>
+      </c>
       <c r="F23" s="20" t="s">
         <v>64</v>
       </c>
@@ -2884,9 +2912,6 @@
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A24" s="72" t="s">
-        <v>271</v>
-      </c>
       <c r="F24" s="20" t="s">
         <v>129</v>
       </c>
@@ -2915,7 +2940,6 @@
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A25" s="72"/>
       <c r="F25" s="20" t="s">
         <v>66</v>
       </c>
@@ -2933,6 +2957,9 @@
       <c r="Q25" s="72"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A26" s="72" t="s">
+        <v>271</v>
+      </c>
       <c r="F26" s="20" t="s">
         <v>131</v>
       </c>
@@ -2955,6 +2982,7 @@
       <c r="Q26" s="72"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A27" s="72"/>
       <c r="K27" t="s">
         <v>259</v>
       </c>
@@ -2964,28 +2992,11 @@
       <c r="Q27" s="72"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A28" s="72"/>
-      <c r="B28" s="72"/>
       <c r="K28" s="72"/>
       <c r="L28" s="72"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A29" s="72"/>
-      <c r="B29" s="72" t="s">
-        <v>8</v>
-      </c>
-      <c r="C29" s="72" t="s">
-        <v>13</v>
-      </c>
-      <c r="D29" s="72" t="s">
-        <v>14</v>
-      </c>
-      <c r="E29" s="72" t="s">
-        <v>42</v>
-      </c>
-      <c r="F29" t="s">
-        <v>43</v>
-      </c>
+      <c r="E29" s="72"/>
       <c r="G29" s="72"/>
       <c r="H29" s="72"/>
       <c r="L29" s="72"/>
@@ -2993,82 +3004,113 @@
       <c r="Q29" s="72"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A30" s="72" t="s">
-        <v>91</v>
-      </c>
-      <c r="B30" s="72">
-        <v>0</v>
-      </c>
-      <c r="C30" s="72">
-        <v>0</v>
-      </c>
-      <c r="D30" s="72"/>
+      <c r="A30" s="72"/>
+      <c r="B30" s="72"/>
       <c r="E30" s="72"/>
       <c r="G30" s="72"/>
       <c r="H30" s="72"/>
       <c r="Q30" s="72"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>92</v>
-      </c>
-      <c r="B31" s="72">
-        <v>-8.6707362007295993E-2</v>
-      </c>
-      <c r="C31" s="72">
-        <v>-9.0628250293378898E-2</v>
-      </c>
-      <c r="D31" s="72"/>
+      <c r="A31" s="72"/>
+      <c r="B31" s="72" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="72" t="s">
+        <v>13</v>
+      </c>
+      <c r="D31" s="72" t="s">
+        <v>10</v>
+      </c>
       <c r="E31" s="72"/>
+      <c r="F31" t="s">
+        <v>14</v>
+      </c>
+      <c r="G31" t="s">
+        <v>272</v>
+      </c>
+      <c r="H31" s="72" t="s">
+        <v>273</v>
+      </c>
+      <c r="I31" s="72"/>
       <c r="L31" s="72"/>
       <c r="Q31" s="72"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>93</v>
+      <c r="A32" s="72" t="s">
+        <v>91</v>
       </c>
       <c r="B32" s="72">
-        <v>-0.22125272217770001</v>
+        <v>0</v>
       </c>
       <c r="C32" s="72">
-        <v>-0.231574865264149</v>
-      </c>
-      <c r="D32" s="72"/>
+        <v>0</v>
+      </c>
+      <c r="D32" s="2">
+        <f>B32-C32</f>
+        <v>0</v>
+      </c>
       <c r="E32" s="72"/>
+      <c r="H32" s="72"/>
+      <c r="I32" s="72"/>
       <c r="L32" s="72"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="72" t="s">
-        <v>261</v>
+      <c r="A33" t="s">
+        <v>92</v>
       </c>
       <c r="B33" s="72">
-        <v>-0.18120346048303301</v>
+        <v>-8.6707362007295993E-2</v>
       </c>
       <c r="C33" s="72">
-        <v>-0.18943967096190201</v>
-      </c>
-      <c r="D33" s="72"/>
+        <v>-9.0560143656216105E-2</v>
+      </c>
+      <c r="D33" s="2">
+        <f t="shared" ref="D33:D37" si="12">B33-C33</f>
+        <v>3.8527816489201117E-3</v>
+      </c>
       <c r="E33" s="72"/>
-      <c r="H33" s="72"/>
-      <c r="I33" s="72"/>
+      <c r="F33" s="72">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <f>F33+$B$33</f>
+        <v>-8.6707362007295993E-2</v>
+      </c>
+      <c r="H33">
+        <f>B33-G33</f>
+        <v>0</v>
+      </c>
       <c r="J33" s="72"/>
       <c r="K33" s="72"/>
       <c r="L33" s="72"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="72" t="s">
-        <v>262</v>
+      <c r="A34" t="s">
+        <v>93</v>
       </c>
       <c r="B34" s="72">
-        <v>-0.15469869726819899</v>
+        <v>-0.22125272217770001</v>
       </c>
       <c r="C34" s="72">
-        <v>-0.16173717771688301</v>
-      </c>
-      <c r="D34" s="72"/>
+        <v>-0.2313578436489</v>
+      </c>
+      <c r="D34" s="72">
+        <f t="shared" si="12"/>
+        <v>1.010512147119999E-2</v>
+      </c>
       <c r="E34" s="72"/>
-      <c r="G34" s="72"/>
-      <c r="H34" s="72"/>
+      <c r="F34" s="72">
+        <v>-0.13921611092296601</v>
+      </c>
+      <c r="G34" s="72">
+        <f t="shared" ref="G34:G40" si="13">F34+$B$33</f>
+        <v>-0.22592347293026199</v>
+      </c>
+      <c r="H34" s="72">
+        <f t="shared" ref="H34:H40" si="14">B34-G34</f>
+        <v>4.6707507525619862E-3</v>
+      </c>
       <c r="I34" s="72"/>
       <c r="J34" s="72"/>
       <c r="K34" s="72"/>
@@ -3076,210 +3118,378 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="72" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B35" s="72">
-        <v>-0.25510563387813501</v>
+        <v>-0.18120346048303301</v>
       </c>
       <c r="C35" s="72">
-        <v>-0.26673372422283498</v>
-      </c>
-      <c r="G35" s="72"/>
-      <c r="H35" s="72"/>
+        <v>-0.18930389483374499</v>
+      </c>
+      <c r="D35" s="72">
+        <f t="shared" si="12"/>
+        <v>8.1004343507119769E-3</v>
+      </c>
+      <c r="F35" s="72">
+        <v>-9.7341403915477701E-2</v>
+      </c>
+      <c r="G35" s="72">
+        <f t="shared" si="13"/>
+        <v>-0.18404876592277369</v>
+      </c>
+      <c r="H35" s="72">
+        <f t="shared" si="14"/>
+        <v>2.8453054397406807E-3</v>
+      </c>
       <c r="J35" s="72"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="72" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B36" s="72">
-        <v>-0.238346440923459</v>
-      </c>
-      <c r="C36" s="72"/>
+        <v>-0.15469869726819899</v>
+      </c>
+      <c r="C36" s="72">
+        <v>-0.161598663395048</v>
+      </c>
+      <c r="D36" s="2">
+        <f t="shared" si="12"/>
+        <v>6.8999661268490109E-3</v>
+      </c>
+      <c r="F36" s="72">
+        <v>-6.9820700644162195E-2</v>
+      </c>
+      <c r="G36" s="72">
+        <f t="shared" si="13"/>
+        <v>-0.15652806265145819</v>
+      </c>
+      <c r="H36" s="72">
+        <f t="shared" si="14"/>
+        <v>1.8293653832592016E-3</v>
+      </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="72" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B37" s="72">
-        <v>-0.23834653794917299</v>
+        <v>-0.25510563387813501</v>
+      </c>
+      <c r="C37" s="72">
+        <v>-0.26608376679888901</v>
+      </c>
+      <c r="D37" s="72">
+        <f t="shared" si="12"/>
+        <v>1.0978132920754002E-2</v>
+      </c>
+      <c r="F37" s="72"/>
+      <c r="G37" s="72"/>
+      <c r="H37" s="72">
+        <f t="shared" si="14"/>
+        <v>-0.25510563387813501</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="72" t="s">
-        <v>71</v>
+        <v>264</v>
       </c>
       <c r="B38" s="72">
-        <v>-0.26806990591321</v>
+        <v>-0.238346440923459</v>
+      </c>
+      <c r="C38" s="72"/>
+      <c r="F38" s="72">
+        <v>-0.15697103903670701</v>
+      </c>
+      <c r="G38" s="72">
+        <f t="shared" si="13"/>
+        <v>-0.24367840104400301</v>
+      </c>
+      <c r="H38" s="72">
+        <f t="shared" si="14"/>
+        <v>5.3319601205440159E-3</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="72" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B39" s="72">
-        <v>-0.27110601345129198</v>
+        <v>-0.23834653794917299</v>
+      </c>
+      <c r="F39" s="72">
+        <v>-0.15697631350866401</v>
+      </c>
+      <c r="G39" s="72">
+        <f t="shared" si="13"/>
+        <v>-0.24368367551595999</v>
+      </c>
+      <c r="H39" s="72">
+        <f t="shared" si="14"/>
+        <v>5.337137566786998E-3</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="72" t="s">
-        <v>267</v>
+        <v>71</v>
       </c>
       <c r="B40" s="72">
-        <v>-0.26564400434675201</v>
+        <v>-0.26806990591321</v>
+      </c>
+      <c r="F40" s="72">
+        <v>-0.18806468644843799</v>
+      </c>
+      <c r="G40" s="72">
+        <f t="shared" si="13"/>
+        <v>-0.274772048455734</v>
+      </c>
+      <c r="H40" s="72">
+        <f t="shared" si="14"/>
+        <v>6.7021425425239922E-3</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="72" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B41" s="72">
-        <v>-0.27078434534196499</v>
+        <v>-0.27110601345129198</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="72" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B42" s="72">
-        <v>-0.272427561300289</v>
+        <v>-0.26564400434675201</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="72" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B43" s="72">
-        <v>-0.28833317446325502</v>
+        <v>-0.27078434534196499</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>26</v>
+      <c r="A44" s="72" t="s">
+        <v>269</v>
       </c>
       <c r="B44" s="72">
-        <v>1.0599999427795399</v>
-      </c>
-      <c r="C44" s="72">
-        <v>1.03719630406032</v>
+        <v>-0.272427561300289</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="72" t="s">
-        <v>28</v>
+        <v>270</v>
       </c>
       <c r="B45" s="72">
-        <v>1.04499995797579</v>
-      </c>
-      <c r="C45" s="72">
-        <v>1.0221355493891</v>
+        <v>-0.28833317446325502</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A46" s="72" t="s">
-        <v>94</v>
+      <c r="A46" t="s">
+        <v>26</v>
       </c>
       <c r="B46" s="72">
-        <v>1.0099999973080001</v>
+        <v>1.0599999427795399</v>
       </c>
       <c r="C46" s="72">
-        <v>0.98671261750101302</v>
+        <v>1.03755066623056</v>
+      </c>
+      <c r="D46" s="2">
+        <f>B46-C46</f>
+        <v>2.244927654897988E-2</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="72" t="s">
-        <v>231</v>
+        <v>28</v>
       </c>
       <c r="B47" s="72">
-        <v>1.02371286456331</v>
+        <v>1.04499995797579</v>
       </c>
       <c r="C47" s="72">
-        <v>1.0021122211514</v>
+        <v>1.0224496733022901</v>
+      </c>
+      <c r="D47" s="2">
+        <f t="shared" ref="D47:D51" si="15">B47-C47</f>
+        <v>2.2550284673499954E-2</v>
+      </c>
+      <c r="F47" s="72">
+        <v>1.02806731578837</v>
+      </c>
+      <c r="H47">
+        <f>B47-F47</f>
+        <v>1.6932642187420077E-2</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="72" t="s">
+        <v>94</v>
+      </c>
+      <c r="B48" s="72">
+        <v>1.0099999973080001</v>
+      </c>
+      <c r="C48" s="72">
+        <v>0.98752731394708704</v>
+      </c>
+      <c r="D48" s="72">
+        <f t="shared" si="15"/>
+        <v>2.2472683360913015E-2</v>
+      </c>
+      <c r="F48" s="72">
+        <v>0.99108591538372603</v>
+      </c>
+      <c r="H48" s="72">
+        <f t="shared" ref="H48:H54" si="16">B48-F48</f>
+        <v>1.8914081924274018E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="72" t="s">
+        <v>231</v>
+      </c>
+      <c r="B49" s="72">
+        <v>1.02371286456331</v>
+      </c>
+      <c r="C49" s="72">
+        <v>1.0016333989946899</v>
+      </c>
+      <c r="D49" s="72">
+        <f t="shared" si="15"/>
+        <v>2.207946556862006E-2</v>
+      </c>
+      <c r="F49" s="72">
+        <v>1.0037548576348501</v>
+      </c>
+      <c r="H49" s="72">
+        <f t="shared" si="16"/>
+        <v>1.9958006928459948E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="72" t="s">
         <v>210</v>
       </c>
-      <c r="B48" s="72">
+      <c r="B50" s="72">
         <v>1.0280925147905799</v>
       </c>
-      <c r="C48" s="72">
-        <v>1.0058453108706</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="72" t="s">
+      <c r="C50" s="72">
+        <v>1.0058936235173901</v>
+      </c>
+      <c r="D50" s="72">
+        <f t="shared" si="15"/>
+        <v>2.2198891273189858E-2</v>
+      </c>
+      <c r="F50" s="72">
+        <v>1.0082505743316901</v>
+      </c>
+      <c r="H50" s="72">
+        <f t="shared" si="16"/>
+        <v>1.9841940458889873E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="72" t="s">
         <v>240</v>
       </c>
-      <c r="B49" s="72">
+      <c r="B51" s="72">
         <v>1.0385379019832599</v>
       </c>
-      <c r="C49" s="72">
-        <v>1.0167525042054999</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="72" t="s">
+      <c r="C51" s="72">
+        <v>1.0178223709630601</v>
+      </c>
+      <c r="D51" s="72">
+        <f t="shared" si="15"/>
+        <v>2.0715531020199851E-2</v>
+      </c>
+      <c r="F51" s="72"/>
+      <c r="H51" s="72"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="72" t="s">
         <v>232</v>
       </c>
-      <c r="B50" s="72">
+      <c r="B52" s="72">
         <v>1.04612245201456</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="72" t="s">
+      <c r="F52" s="72">
+        <v>1.0235939390642299</v>
+      </c>
+      <c r="H52" s="72">
+        <f t="shared" si="16"/>
+        <v>2.2528512950330093E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="72" t="s">
         <v>211</v>
       </c>
-      <c r="B51" s="72">
+      <c r="B53" s="72">
         <v>1.0850835071553799</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="72" t="s">
+      <c r="F53" s="72">
+        <v>1.0619005149699601</v>
+      </c>
+      <c r="H53" s="72">
+        <f t="shared" si="16"/>
+        <v>2.318299218541986E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="72" t="s">
         <v>215</v>
       </c>
-      <c r="B52" s="72">
+      <c r="B54" s="72">
         <v>1.0349152577221601</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="72" t="s">
+      <c r="F54" s="72">
+        <v>1.0118554130617501</v>
+      </c>
+      <c r="H54" s="72">
+        <f t="shared" si="16"/>
+        <v>2.305984466041E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="72" t="s">
         <v>214</v>
       </c>
-      <c r="B53" s="72">
+      <c r="B55" s="72">
         <v>1.02798621556374</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="72" t="s">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="72" t="s">
         <v>241</v>
       </c>
-      <c r="B54" s="72">
+      <c r="B56" s="72">
         <v>1.02970205350408</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="72" t="s">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="72" t="s">
         <v>212</v>
       </c>
-      <c r="B55" s="72">
+      <c r="B57" s="72">
         <v>1.0240525230119499</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="72" t="s">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="72" t="s">
         <v>213</v>
       </c>
-      <c r="B56" s="72">
+      <c r="B58" s="72">
         <v>1.01992383631813</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="72" t="s">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="72" t="s">
         <v>248</v>
       </c>
-      <c r="B57" s="72">
+      <c r="B59" s="72">
         <v>1.00994172446495</v>
       </c>
     </row>
@@ -3319,15 +3529,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="82" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
+      <c r="A1" s="86" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="86"/>
+      <c r="C1" s="86"/>
+      <c r="D1" s="86"/>
+      <c r="E1" s="86"/>
+      <c r="F1" s="86"/>
+      <c r="G1" s="86"/>
       <c r="I1" s="6" t="s">
         <v>1</v>
       </c>
@@ -3680,15 +3890,15 @@
       <c r="N11" s="1"/>
     </row>
     <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="83" t="s">
+      <c r="A12" s="87" t="s">
         <v>80</v>
       </c>
-      <c r="B12" s="83"/>
-      <c r="C12" s="83"/>
-      <c r="D12" s="83"/>
-      <c r="E12" s="83"/>
-      <c r="F12" s="83"/>
-      <c r="G12" s="83"/>
+      <c r="B12" s="87"/>
+      <c r="C12" s="87"/>
+      <c r="D12" s="87"/>
+      <c r="E12" s="87"/>
+      <c r="F12" s="87"/>
+      <c r="G12" s="87"/>
       <c r="I12" s="1"/>
       <c r="J12" s="6" t="s">
         <v>1</v>
@@ -4178,15 +4388,15 @@
       <c r="G31" s="1"/>
     </row>
     <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="83" t="s">
+      <c r="A32" s="87" t="s">
         <v>81</v>
       </c>
-      <c r="B32" s="83"/>
-      <c r="C32" s="83"/>
-      <c r="D32" s="83"/>
-      <c r="E32" s="83"/>
-      <c r="F32" s="83"/>
-      <c r="G32" s="83"/>
+      <c r="B32" s="87"/>
+      <c r="C32" s="87"/>
+      <c r="D32" s="87"/>
+      <c r="E32" s="87"/>
+      <c r="F32" s="87"/>
+      <c r="G32" s="87"/>
       <c r="I32" s="1"/>
       <c r="J32" s="6" t="s">
         <v>1</v>
@@ -4665,13 +4875,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="86" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
+      <c r="B1" s="86"/>
+      <c r="C1" s="86"/>
+      <c r="D1" s="86"/>
+      <c r="E1" s="86"/>
       <c r="G1" s="30" t="s">
         <v>100</v>
       </c>
@@ -4690,13 +4900,13 @@
       <c r="L1" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="P1" s="82" t="s">
+      <c r="P1" s="86" t="s">
         <v>106</v>
       </c>
-      <c r="Q1" s="82"/>
-      <c r="R1" s="82"/>
-      <c r="S1" s="82"/>
-      <c r="T1" s="82"/>
+      <c r="Q1" s="86"/>
+      <c r="R1" s="86"/>
+      <c r="S1" s="86"/>
+      <c r="T1" s="86"/>
       <c r="V1" s="30" t="s">
         <v>100</v>
       </c>
@@ -5231,12 +5441,12 @@
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="P10" s="82" t="s">
+      <c r="P10" s="86" t="s">
         <v>108</v>
       </c>
-      <c r="Q10" s="82"/>
-      <c r="R10" s="82"/>
-      <c r="S10" s="82"/>
+      <c r="Q10" s="86"/>
+      <c r="R10" s="86"/>
+      <c r="S10" s="86"/>
       <c r="T10" s="25"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
@@ -6252,12 +6462,12 @@
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A33" s="82" t="s">
+      <c r="A33" s="86" t="s">
         <v>102</v>
       </c>
-      <c r="B33" s="82"/>
-      <c r="C33" s="82"/>
-      <c r="D33" s="82"/>
+      <c r="B33" s="86"/>
+      <c r="C33" s="86"/>
+      <c r="D33" s="86"/>
       <c r="F33" s="30" t="s">
         <v>100</v>
       </c>
@@ -6635,12 +6845,12 @@
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A42" s="82" t="s">
+      <c r="A42" s="86" t="s">
         <v>104</v>
       </c>
-      <c r="B42" s="82"/>
-      <c r="C42" s="82"/>
-      <c r="D42" s="82"/>
+      <c r="B42" s="86"/>
+      <c r="C42" s="86"/>
+      <c r="D42" s="86"/>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
@@ -7139,15 +7349,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="87" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="83"/>
-      <c r="G1" s="83"/>
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
       <c r="I1" s="1"/>
       <c r="J1" s="4"/>
       <c r="L1" s="4" t="s">
@@ -8209,18 +8419,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="88" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84"/>
-      <c r="I1" s="84"/>
-      <c r="J1" s="84"/>
+      <c r="B1" s="88"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="88"/>
+      <c r="G1" s="88"/>
+      <c r="H1" s="88"/>
+      <c r="I1" s="88"/>
+      <c r="J1" s="88"/>
       <c r="L1" s="11" t="s">
         <v>1</v>
       </c>
@@ -8244,18 +8454,18 @@
       <c r="B2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="85" t="s">
+      <c r="C2" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85" t="s">
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89" t="s">
         <v>74</v>
       </c>
-      <c r="H2" s="85"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="85"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="89"/>
       <c r="L2" s="8" t="s">
         <v>41</v>
       </c>
@@ -9048,18 +9258,18 @@
       <c r="O33" s="1"/>
     </row>
     <row r="35" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="84" t="s">
+      <c r="A35" s="88" t="s">
         <v>78</v>
       </c>
-      <c r="B35" s="84"/>
-      <c r="C35" s="84"/>
-      <c r="D35" s="84"/>
-      <c r="E35" s="84"/>
-      <c r="F35" s="84"/>
-      <c r="G35" s="84"/>
-      <c r="H35" s="84"/>
-      <c r="I35" s="84"/>
-      <c r="J35" s="84"/>
+      <c r="B35" s="88"/>
+      <c r="C35" s="88"/>
+      <c r="D35" s="88"/>
+      <c r="E35" s="88"/>
+      <c r="F35" s="88"/>
+      <c r="G35" s="88"/>
+      <c r="H35" s="88"/>
+      <c r="I35" s="88"/>
+      <c r="J35" s="88"/>
       <c r="L35" s="11" t="s">
         <v>1</v>
       </c>
@@ -16851,18 +17061,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="88" t="s">
         <v>221</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84"/>
-      <c r="I1" s="84"/>
-      <c r="J1" s="84"/>
+      <c r="B1" s="88"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="88"/>
+      <c r="G1" s="88"/>
+      <c r="H1" s="88"/>
+      <c r="I1" s="88"/>
+      <c r="J1" s="88"/>
       <c r="K1" s="43"/>
       <c r="L1" s="60"/>
       <c r="M1" s="11" t="s">
@@ -16886,18 +17096,18 @@
       <c r="B2" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="85" t="s">
+      <c r="C2" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85" t="s">
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89" t="s">
         <v>74</v>
       </c>
-      <c r="H2" s="85"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="85"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="89"/>
       <c r="K2" s="4"/>
       <c r="L2" s="60" t="s">
         <v>138</v>

</xml_diff>

<commit_message>
Modified partition measurements to be V^2 and realized that each partition should have its own slack bus
Found why Partition 1 central SE results don't match overall 14 bus SE
results - V measurements should be V^2. Also realized that each
partition should have its own slack bus and then be looked at with
reference to a system wide slack bus. Currently, there are still
problems with getting Partitions 2-4 to match central results.
</commit_message>
<xml_diff>
--- a/DMASE - Test Results.xlsx
+++ b/DMASE - Test Results.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="941" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="940" uniqueCount="272">
   <si>
     <t>Abur 3-Bus Case Measurements (run through SE, rerun new estimate again)</t>
   </si>
@@ -839,12 +839,6 @@
   </si>
   <si>
     <t>P5-4 = -P4-5</t>
-  </si>
-  <si>
-    <t>x2+slack2</t>
-  </si>
-  <si>
-    <t>Central - (x2+slack2)</t>
   </si>
 </sst>
 </file>
@@ -1855,8 +1849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3019,19 +3013,17 @@
       <c r="C31" s="72" t="s">
         <v>13</v>
       </c>
-      <c r="D31" s="72" t="s">
-        <v>10</v>
+      <c r="D31" s="34" t="s">
+        <v>14</v>
       </c>
       <c r="E31" s="72"/>
       <c r="F31" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G31" t="s">
-        <v>272</v>
-      </c>
-      <c r="H31" s="72" t="s">
-        <v>273</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="H31" s="72"/>
       <c r="I31" s="72"/>
       <c r="L31" s="72"/>
       <c r="Q31" s="72"/>
@@ -3046,10 +3038,7 @@
       <c r="C32" s="72">
         <v>0</v>
       </c>
-      <c r="D32" s="2">
-        <f>B32-C32</f>
-        <v>0</v>
-      </c>
+      <c r="D32" s="34"/>
       <c r="E32" s="72"/>
       <c r="H32" s="72"/>
       <c r="I32" s="72"/>
@@ -3063,23 +3052,16 @@
         <v>-8.6707362007295993E-2</v>
       </c>
       <c r="C33" s="72">
-        <v>-9.0560143656216105E-2</v>
-      </c>
-      <c r="D33" s="2">
-        <f t="shared" ref="D33:D37" si="12">B33-C33</f>
-        <v>3.8527816489201117E-3</v>
+        <v>-8.6708237100475705E-2</v>
+      </c>
+      <c r="D33" s="34">
+        <f>0.884088158942101+$B$34</f>
+        <v>0.66283543676440104</v>
       </c>
       <c r="E33" s="72"/>
       <c r="F33" s="72">
-        <v>0</v>
-      </c>
-      <c r="G33">
-        <f>F33+$B$33</f>
-        <v>-8.6707362007295993E-2</v>
-      </c>
-      <c r="H33">
-        <f>B33-G33</f>
-        <v>0</v>
+        <f>B33-D33</f>
+        <v>-0.74954279877169705</v>
       </c>
       <c r="J33" s="72"/>
       <c r="K33" s="72"/>
@@ -3093,24 +3075,19 @@
         <v>-0.22125272217770001</v>
       </c>
       <c r="C34" s="72">
-        <v>-0.2313578436489</v>
-      </c>
-      <c r="D34" s="72">
-        <f t="shared" si="12"/>
-        <v>1.010512147119999E-2</v>
+        <v>-0.22124896604786901</v>
+      </c>
+      <c r="D34" s="34">
+        <f>0+$B$34</f>
+        <v>-0.22125272217770001</v>
       </c>
       <c r="E34" s="72"/>
       <c r="F34" s="72">
-        <v>-0.13921611092296601</v>
-      </c>
-      <c r="G34" s="72">
-        <f t="shared" ref="G34:G40" si="13">F34+$B$33</f>
-        <v>-0.22592347293026199</v>
-      </c>
-      <c r="H34" s="72">
-        <f t="shared" ref="H34:H40" si="14">B34-G34</f>
-        <v>4.6707507525619862E-3</v>
-      </c>
+        <f t="shared" ref="F34:F40" si="12">B34-D34</f>
+        <v>0</v>
+      </c>
+      <c r="G34" s="72"/>
+      <c r="H34" s="72"/>
       <c r="I34" s="72"/>
       <c r="J34" s="72"/>
       <c r="K34" s="72"/>
@@ -3124,23 +3101,18 @@
         <v>-0.18120346048303301</v>
       </c>
       <c r="C35" s="72">
-        <v>-0.18930389483374499</v>
-      </c>
-      <c r="D35" s="72">
+        <v>-0.18120036659231001</v>
+      </c>
+      <c r="D35" s="34">
+        <f>0.040048851584724+$B$34</f>
+        <v>-0.18120387059297599</v>
+      </c>
+      <c r="F35" s="72">
         <f t="shared" si="12"/>
-        <v>8.1004343507119769E-3</v>
-      </c>
-      <c r="F35" s="72">
-        <v>-9.7341403915477701E-2</v>
-      </c>
-      <c r="G35" s="72">
-        <f t="shared" si="13"/>
-        <v>-0.18404876592277369</v>
-      </c>
-      <c r="H35" s="72">
-        <f t="shared" si="14"/>
-        <v>2.8453054397406807E-3</v>
-      </c>
+        <v>4.1010994297763226E-7</v>
+      </c>
+      <c r="G35" s="72"/>
+      <c r="H35" s="72"/>
       <c r="J35" s="72"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
@@ -3151,23 +3123,18 @@
         <v>-0.15469869726819899</v>
       </c>
       <c r="C36" s="72">
-        <v>-0.161598663395048</v>
-      </c>
-      <c r="D36" s="2">
+        <v>-0.15469627337389699</v>
+      </c>
+      <c r="D36" s="34">
+        <f>0.066553618443497+$B$34</f>
+        <v>-0.15469910373420301</v>
+      </c>
+      <c r="F36" s="72">
         <f t="shared" si="12"/>
-        <v>6.8999661268490109E-3</v>
-      </c>
-      <c r="F36" s="72">
-        <v>-6.9820700644162195E-2</v>
-      </c>
-      <c r="G36" s="72">
-        <f t="shared" si="13"/>
-        <v>-0.15652806265145819</v>
-      </c>
-      <c r="H36" s="72">
-        <f t="shared" si="14"/>
-        <v>1.8293653832592016E-3</v>
-      </c>
+        <v>4.0646600402149957E-7</v>
+      </c>
+      <c r="G36" s="72"/>
+      <c r="H36" s="72"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="72" t="s">
@@ -3177,18 +3144,14 @@
         <v>-0.25510563387813501</v>
       </c>
       <c r="C37" s="72">
-        <v>-0.26608376679888901</v>
-      </c>
-      <c r="D37" s="72">
-        <f t="shared" si="12"/>
-        <v>1.0978132920754002E-2</v>
+        <v>-0.255101990043542</v>
       </c>
       <c r="F37" s="72"/>
-      <c r="G37" s="72"/>
-      <c r="H37" s="72">
-        <f t="shared" si="14"/>
+      <c r="G37" s="72">
+        <f>0+B37</f>
         <v>-0.25510563387813501</v>
       </c>
+      <c r="H37" s="72"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="72" t="s">
@@ -3198,17 +3161,19 @@
         <v>-0.238346440923459</v>
       </c>
       <c r="C38" s="72"/>
+      <c r="D38" s="72">
+        <f>-0.0170943075250511+$B$34</f>
+        <v>-0.2383470297027511</v>
+      </c>
       <c r="F38" s="72">
-        <v>-0.15697103903670701</v>
+        <f t="shared" si="12"/>
+        <v>5.8877929209888435E-7</v>
       </c>
       <c r="G38" s="72">
-        <f t="shared" si="13"/>
-        <v>-0.24367840104400301</v>
-      </c>
-      <c r="H38" s="72">
-        <f t="shared" si="14"/>
-        <v>5.3319601205440159E-3</v>
-      </c>
+        <f>0.00525434884790097+B37</f>
+        <v>-0.24985128503023404</v>
+      </c>
+      <c r="H38" s="72"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="72" t="s">
@@ -3217,17 +3182,18 @@
       <c r="B39" s="72">
         <v>-0.23834653794917299</v>
       </c>
+      <c r="D39" s="34">
+        <f>-0.0170943114208884+$B$34</f>
+        <v>-0.23834703359858841</v>
+      </c>
       <c r="F39" s="72">
-        <v>-0.15697631350866401</v>
+        <f t="shared" si="12"/>
+        <v>4.9564941542734609E-7</v>
       </c>
       <c r="G39" s="72">
-        <f t="shared" si="13"/>
-        <v>-0.24368367551595999</v>
-      </c>
-      <c r="H39" s="72">
-        <f t="shared" si="14"/>
-        <v>5.337137566786998E-3</v>
-      </c>
+        <v>3.7900965250991601E-3</v>
+      </c>
+      <c r="H39" s="72"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="72" t="s">
@@ -3236,17 +3202,18 @@
       <c r="B40" s="72">
         <v>-0.26806990591321</v>
       </c>
+      <c r="D40" s="34">
+        <f>-0.0468176408310144+$B$34</f>
+        <v>-0.2680703630087144</v>
+      </c>
       <c r="F40" s="72">
-        <v>-0.18806468644843799</v>
+        <f t="shared" si="12"/>
+        <v>4.5709550439143598E-7</v>
       </c>
       <c r="G40" s="72">
-        <f t="shared" si="13"/>
-        <v>-0.274772048455734</v>
-      </c>
-      <c r="H40" s="72">
-        <f t="shared" si="14"/>
-        <v>6.7021425425239922E-3</v>
-      </c>
+        <v>3.8658936106577501E-3</v>
+      </c>
+      <c r="H40" s="72"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="72" t="s">
@@ -3255,6 +3222,10 @@
       <c r="B41" s="72">
         <v>-0.27110601345129198</v>
       </c>
+      <c r="D41" s="34"/>
+      <c r="G41" s="72">
+        <v>5.1455717794403602E-3</v>
+      </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="72" t="s">
@@ -3263,6 +3234,10 @@
       <c r="B42" s="72">
         <v>-0.26564400434675201</v>
       </c>
+      <c r="D42" s="34"/>
+      <c r="G42" s="72">
+        <v>2.18618035355134E-2</v>
+      </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="72" t="s">
@@ -3271,6 +3246,7 @@
       <c r="B43" s="72">
         <v>-0.27078434534196499</v>
       </c>
+      <c r="D43" s="34"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="72" t="s">
@@ -3279,6 +3255,7 @@
       <c r="B44" s="72">
         <v>-0.272427561300289</v>
       </c>
+      <c r="D44" s="34"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="72" t="s">
@@ -3287,6 +3264,7 @@
       <c r="B45" s="72">
         <v>-0.28833317446325502</v>
       </c>
+      <c r="D45" s="34"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
@@ -3296,12 +3274,9 @@
         <v>1.0599999427795399</v>
       </c>
       <c r="C46" s="72">
-        <v>1.03755066623056</v>
-      </c>
-      <c r="D46" s="2">
-        <f>B46-C46</f>
-        <v>2.244927654897988E-2</v>
-      </c>
+        <v>1.05999978718632</v>
+      </c>
+      <c r="D46" s="34"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="72" t="s">
@@ -3311,18 +3286,14 @@
         <v>1.04499995797579</v>
       </c>
       <c r="C47" s="72">
-        <v>1.0224496733022901</v>
-      </c>
-      <c r="D47" s="2">
-        <f t="shared" ref="D47:D51" si="15">B47-C47</f>
-        <v>2.2550284673499954E-2</v>
+        <v>1.04499963862116</v>
+      </c>
+      <c r="D47" s="34">
+        <v>1.6333803303629399</v>
       </c>
       <c r="F47" s="72">
-        <v>1.02806731578837</v>
-      </c>
-      <c r="H47">
-        <f>B47-F47</f>
-        <v>1.6932642187420077E-2</v>
+        <f>B47-D47</f>
+        <v>-0.58838037238714991</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
@@ -3333,19 +3304,16 @@
         <v>1.0099999973080001</v>
       </c>
       <c r="C48" s="72">
-        <v>0.98752731394708704</v>
-      </c>
-      <c r="D48" s="72">
-        <f t="shared" si="15"/>
-        <v>2.2472683360913015E-2</v>
+        <v>1.0100010595292099</v>
+      </c>
+      <c r="D48" s="34">
+        <v>1.0099999154299499</v>
       </c>
       <c r="F48" s="72">
-        <v>0.99108591538372603</v>
-      </c>
-      <c r="H48" s="72">
-        <f t="shared" ref="H48:H54" si="16">B48-F48</f>
-        <v>1.8914081924274018E-2</v>
-      </c>
+        <f t="shared" ref="F48:F54" si="13">B48-D48</f>
+        <v>8.1878050117722978E-8</v>
+      </c>
+      <c r="H48" s="72"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="72" t="s">
@@ -3355,19 +3323,16 @@
         <v>1.02371286456331</v>
       </c>
       <c r="C49" s="72">
-        <v>1.0016333989946899</v>
-      </c>
-      <c r="D49" s="72">
-        <f t="shared" si="15"/>
-        <v>2.207946556862006E-2</v>
+        <v>1.0237139016294901</v>
+      </c>
+      <c r="D49" s="34">
+        <v>1.0237127741001699</v>
       </c>
       <c r="F49" s="72">
-        <v>1.0037548576348501</v>
-      </c>
-      <c r="H49" s="72">
-        <f t="shared" si="16"/>
-        <v>1.9958006928459948E-2</v>
-      </c>
+        <f t="shared" si="13"/>
+        <v>9.0463140089980243E-8</v>
+      </c>
+      <c r="H49" s="72"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="72" t="s">
@@ -3377,19 +3342,16 @@
         <v>1.0280925147905799</v>
       </c>
       <c r="C50" s="72">
-        <v>1.0058936235173901</v>
-      </c>
-      <c r="D50" s="72">
-        <f t="shared" si="15"/>
-        <v>2.2198891273189858E-2</v>
+        <v>1.0280934274068501</v>
+      </c>
+      <c r="D50" s="34">
+        <v>1.0280924499320001</v>
       </c>
       <c r="F50" s="72">
-        <v>1.0082505743316901</v>
-      </c>
-      <c r="H50" s="72">
-        <f t="shared" si="16"/>
-        <v>1.9841940458889873E-2</v>
-      </c>
+        <f t="shared" si="13"/>
+        <v>6.4858579840176844E-8</v>
+      </c>
+      <c r="H50" s="72"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="72" t="s">
@@ -3399,14 +3361,16 @@
         <v>1.0385379019832599</v>
       </c>
       <c r="C51" s="72">
-        <v>1.0178223709630601</v>
-      </c>
-      <c r="D51" s="72">
-        <f t="shared" si="15"/>
-        <v>2.0715531020199851E-2</v>
+        <v>1.03853856918465</v>
       </c>
       <c r="F51" s="72"/>
-      <c r="H51" s="72"/>
+      <c r="G51" s="72">
+        <v>1.0340843666464401</v>
+      </c>
+      <c r="H51" s="72">
+        <f>B51-G51</f>
+        <v>4.4535353368198027E-3</v>
+      </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="72" t="s">
@@ -3415,13 +3379,14 @@
       <c r="B52" s="72">
         <v>1.04612245201456</v>
       </c>
+      <c r="D52" s="72">
+        <v>1.04612260923001</v>
+      </c>
       <c r="F52" s="72">
-        <v>1.0235939390642299</v>
-      </c>
-      <c r="H52" s="72">
-        <f t="shared" si="16"/>
-        <v>2.2528512950330093E-2</v>
-      </c>
+        <f t="shared" si="13"/>
+        <v>-1.5721544999180992E-7</v>
+      </c>
+      <c r="H52" s="72"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="72" t="s">
@@ -3430,13 +3395,14 @@
       <c r="B53" s="72">
         <v>1.0850835071553799</v>
       </c>
+      <c r="D53" s="34">
+        <v>1.0850835263671801</v>
+      </c>
       <c r="F53" s="72">
-        <v>1.0619005149699601</v>
-      </c>
-      <c r="H53" s="72">
-        <f t="shared" si="16"/>
-        <v>2.318299218541986E-2</v>
-      </c>
+        <f t="shared" si="13"/>
+        <v>-1.921180015074242E-8</v>
+      </c>
+      <c r="H53" s="72"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="72" t="s">
@@ -3445,13 +3411,14 @@
       <c r="B54" s="72">
         <v>1.0349152577221601</v>
       </c>
+      <c r="D54" s="72">
+        <v>1.03491546996032</v>
+      </c>
       <c r="F54" s="72">
-        <v>1.0118554130617501</v>
-      </c>
-      <c r="H54" s="72">
-        <f t="shared" si="16"/>
-        <v>2.305984466041E-2</v>
-      </c>
+        <f t="shared" si="13"/>
+        <v>-2.1223815993565154E-7</v>
+      </c>
+      <c r="H54" s="72"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="72" t="s">
@@ -3460,6 +3427,13 @@
       <c r="B55" s="72">
         <v>1.02798621556374</v>
       </c>
+      <c r="G55" s="72">
+        <v>1.02971162455886</v>
+      </c>
+      <c r="H55" s="72">
+        <f t="shared" ref="H52:H59" si="14">B55-G55</f>
+        <v>-1.7254089951199703E-3</v>
+      </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="72" t="s">
@@ -3468,6 +3442,13 @@
       <c r="B56" s="72">
         <v>1.02970205350408</v>
       </c>
+      <c r="G56" s="72">
+        <v>1.02966763377662</v>
+      </c>
+      <c r="H56" s="72">
+        <f t="shared" si="14"/>
+        <v>3.4419727459988891E-5</v>
+      </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="72" t="s">
@@ -3476,6 +3457,13 @@
       <c r="B57" s="72">
         <v>1.0240525230119499</v>
       </c>
+      <c r="G57" s="72">
+        <v>1.0257083598498999</v>
+      </c>
+      <c r="H57" s="72">
+        <f t="shared" si="14"/>
+        <v>-1.6558368379500088E-3</v>
+      </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="72" t="s">
@@ -3484,6 +3472,13 @@
       <c r="B58" s="72">
         <v>1.01992383631813</v>
       </c>
+      <c r="G58" s="72">
+        <v>1.0228316776611599</v>
+      </c>
+      <c r="H58" s="72">
+        <f t="shared" si="14"/>
+        <v>-2.9078413430299044E-3</v>
+      </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="72" t="s">
@@ -3491,6 +3486,13 @@
       </c>
       <c r="B59" s="72">
         <v>1.00994172446495</v>
+      </c>
+      <c r="G59" s="72">
+        <v>1.0220031485954399</v>
+      </c>
+      <c r="H59" s="72">
+        <f t="shared" si="14"/>
+        <v>-1.2061424130489939E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Central Partition 2 results now match overall system results.
Central Partition 2 results now match overall central system results.
Original error was due to an error in the way x was mapped to f. Check
that in the future if there are errors for other partitions.
</commit_message>
<xml_diff>
--- a/DMASE - Test Results.xlsx
+++ b/DMASE - Test Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12240" windowHeight="9240" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12240" windowHeight="9240" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="2 Bus" sheetId="4" r:id="rId1"/>
@@ -17,13 +17,14 @@
     <sheet name="14 Bus h" sheetId="10" r:id="rId8"/>
     <sheet name="14 Bus AC" sheetId="6" r:id="rId9"/>
     <sheet name="Sheet1" sheetId="11" r:id="rId10"/>
+    <sheet name="Sheet2" sheetId="12" r:id="rId11"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="940" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="939" uniqueCount="274">
   <si>
     <t>Abur 3-Bus Case Measurements (run through SE, rerun new estimate again)</t>
   </si>
@@ -839,6 +840,12 @@
   </si>
   <si>
     <t>P5-4 = -P4-5</t>
+  </si>
+  <si>
+    <t>x2 (unscaled)</t>
+  </si>
+  <si>
+    <t>x2 + th3</t>
   </si>
 </sst>
 </file>
@@ -1849,8 +1856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3006,86 +3013,28 @@
       <c r="Q30" s="72"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A31" s="72"/>
-      <c r="B31" s="72" t="s">
-        <v>8</v>
-      </c>
-      <c r="C31" s="72" t="s">
-        <v>13</v>
-      </c>
-      <c r="D31" s="34" t="s">
-        <v>14</v>
-      </c>
       <c r="E31" s="72"/>
-      <c r="F31" t="s">
-        <v>11</v>
-      </c>
-      <c r="G31" t="s">
-        <v>42</v>
-      </c>
       <c r="H31" s="72"/>
       <c r="I31" s="72"/>
       <c r="L31" s="72"/>
       <c r="Q31" s="72"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A32" s="72" t="s">
-        <v>91</v>
-      </c>
-      <c r="B32" s="72">
-        <v>0</v>
-      </c>
-      <c r="C32" s="72">
-        <v>0</v>
-      </c>
-      <c r="D32" s="34"/>
       <c r="E32" s="72"/>
       <c r="H32" s="72"/>
       <c r="I32" s="72"/>
       <c r="L32" s="72"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>92</v>
-      </c>
-      <c r="B33" s="72">
-        <v>-8.6707362007295993E-2</v>
-      </c>
-      <c r="C33" s="72">
-        <v>-8.6708237100475705E-2</v>
-      </c>
-      <c r="D33" s="34">
-        <f>0.884088158942101+$B$34</f>
-        <v>0.66283543676440104</v>
-      </c>
+    <row r="33" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E33" s="72"/>
-      <c r="F33" s="72">
-        <f>B33-D33</f>
-        <v>-0.74954279877169705</v>
-      </c>
+      <c r="F33" s="72"/>
       <c r="J33" s="72"/>
       <c r="K33" s="72"/>
       <c r="L33" s="72"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>93</v>
-      </c>
-      <c r="B34" s="72">
-        <v>-0.22125272217770001</v>
-      </c>
-      <c r="C34" s="72">
-        <v>-0.22124896604786901</v>
-      </c>
-      <c r="D34" s="34">
-        <f>0+$B$34</f>
-        <v>-0.22125272217770001</v>
-      </c>
+    <row r="34" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E34" s="72"/>
-      <c r="F34" s="72">
-        <f t="shared" ref="F34:F40" si="12">B34-D34</f>
-        <v>0</v>
-      </c>
+      <c r="F34" s="72"/>
       <c r="G34" s="72"/>
       <c r="H34" s="72"/>
       <c r="I34" s="72"/>
@@ -3093,407 +3042,94 @@
       <c r="K34" s="72"/>
       <c r="L34" s="72"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="72" t="s">
-        <v>261</v>
-      </c>
-      <c r="B35" s="72">
-        <v>-0.18120346048303301</v>
-      </c>
-      <c r="C35" s="72">
-        <v>-0.18120036659231001</v>
-      </c>
-      <c r="D35" s="34">
-        <f>0.040048851584724+$B$34</f>
-        <v>-0.18120387059297599</v>
-      </c>
-      <c r="F35" s="72">
-        <f t="shared" si="12"/>
-        <v>4.1010994297763226E-7</v>
-      </c>
+    <row r="35" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="F35" s="72"/>
       <c r="G35" s="72"/>
       <c r="H35" s="72"/>
       <c r="J35" s="72"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="72" t="s">
-        <v>262</v>
-      </c>
-      <c r="B36" s="72">
-        <v>-0.15469869726819899</v>
-      </c>
-      <c r="C36" s="72">
-        <v>-0.15469627337389699</v>
-      </c>
-      <c r="D36" s="34">
-        <f>0.066553618443497+$B$34</f>
-        <v>-0.15469910373420301</v>
-      </c>
-      <c r="F36" s="72">
-        <f t="shared" si="12"/>
-        <v>4.0646600402149957E-7</v>
-      </c>
+    <row r="36" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="F36" s="72"/>
       <c r="G36" s="72"/>
       <c r="H36" s="72"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="72" t="s">
-        <v>263</v>
-      </c>
-      <c r="B37" s="72">
-        <v>-0.25510563387813501</v>
-      </c>
-      <c r="C37" s="72">
-        <v>-0.255101990043542</v>
-      </c>
+    <row r="37" spans="5:12" x14ac:dyDescent="0.25">
       <c r="F37" s="72"/>
-      <c r="G37" s="72">
-        <f>0+B37</f>
-        <v>-0.25510563387813501</v>
-      </c>
+      <c r="G37" s="72"/>
       <c r="H37" s="72"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="72" t="s">
-        <v>264</v>
-      </c>
-      <c r="B38" s="72">
-        <v>-0.238346440923459</v>
-      </c>
-      <c r="C38" s="72"/>
-      <c r="D38" s="72">
-        <f>-0.0170943075250511+$B$34</f>
-        <v>-0.2383470297027511</v>
-      </c>
-      <c r="F38" s="72">
-        <f t="shared" si="12"/>
-        <v>5.8877929209888435E-7</v>
-      </c>
-      <c r="G38" s="72">
-        <f>0.00525434884790097+B37</f>
-        <v>-0.24985128503023404</v>
-      </c>
+    <row r="38" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="F38" s="72"/>
+      <c r="G38" s="72"/>
       <c r="H38" s="72"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="72" t="s">
-        <v>265</v>
-      </c>
-      <c r="B39" s="72">
-        <v>-0.23834653794917299</v>
-      </c>
-      <c r="D39" s="34">
-        <f>-0.0170943114208884+$B$34</f>
-        <v>-0.23834703359858841</v>
-      </c>
-      <c r="F39" s="72">
-        <f t="shared" si="12"/>
-        <v>4.9564941542734609E-7</v>
-      </c>
-      <c r="G39" s="72">
-        <v>3.7900965250991601E-3</v>
-      </c>
+    <row r="39" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="F39" s="72"/>
+      <c r="G39" s="72"/>
       <c r="H39" s="72"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="72" t="s">
-        <v>71</v>
-      </c>
-      <c r="B40" s="72">
-        <v>-0.26806990591321</v>
-      </c>
-      <c r="D40" s="34">
-        <f>-0.0468176408310144+$B$34</f>
-        <v>-0.2680703630087144</v>
-      </c>
-      <c r="F40" s="72">
-        <f t="shared" si="12"/>
-        <v>4.5709550439143598E-7</v>
-      </c>
-      <c r="G40" s="72">
-        <v>3.8658936106577501E-3</v>
-      </c>
+    <row r="40" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="F40" s="72"/>
+      <c r="G40" s="72"/>
       <c r="H40" s="72"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="72" t="s">
-        <v>266</v>
-      </c>
-      <c r="B41" s="72">
-        <v>-0.27110601345129198</v>
-      </c>
-      <c r="D41" s="34"/>
-      <c r="G41" s="72">
-        <v>5.1455717794403602E-3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" s="72" t="s">
-        <v>267</v>
-      </c>
-      <c r="B42" s="72">
-        <v>-0.26564400434675201</v>
-      </c>
-      <c r="D42" s="34"/>
-      <c r="G42" s="72">
-        <v>2.18618035355134E-2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" s="72" t="s">
-        <v>268</v>
-      </c>
-      <c r="B43" s="72">
-        <v>-0.27078434534196499</v>
-      </c>
-      <c r="D43" s="34"/>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" s="72" t="s">
-        <v>269</v>
-      </c>
-      <c r="B44" s="72">
-        <v>-0.272427561300289</v>
-      </c>
-      <c r="D44" s="34"/>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" s="72" t="s">
-        <v>270</v>
-      </c>
-      <c r="B45" s="72">
-        <v>-0.28833317446325502</v>
-      </c>
-      <c r="D45" s="34"/>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>26</v>
-      </c>
-      <c r="B46" s="72">
-        <v>1.0599999427795399</v>
-      </c>
-      <c r="C46" s="72">
-        <v>1.05999978718632</v>
-      </c>
-      <c r="D46" s="34"/>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A47" s="72" t="s">
-        <v>28</v>
-      </c>
-      <c r="B47" s="72">
-        <v>1.04499995797579</v>
-      </c>
-      <c r="C47" s="72">
-        <v>1.04499963862116</v>
-      </c>
-      <c r="D47" s="34">
-        <v>1.6333803303629399</v>
-      </c>
-      <c r="F47" s="72">
-        <f>B47-D47</f>
-        <v>-0.58838037238714991</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A48" s="72" t="s">
-        <v>94</v>
-      </c>
-      <c r="B48" s="72">
-        <v>1.0099999973080001</v>
-      </c>
-      <c r="C48" s="72">
-        <v>1.0100010595292099</v>
-      </c>
-      <c r="D48" s="34">
-        <v>1.0099999154299499</v>
-      </c>
-      <c r="F48" s="72">
-        <f t="shared" ref="F48:F54" si="13">B48-D48</f>
-        <v>8.1878050117722978E-8</v>
-      </c>
+    <row r="41" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="G41" s="72"/>
+    </row>
+    <row r="42" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="G42" s="72"/>
+    </row>
+    <row r="47" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="F47" s="72"/>
+    </row>
+    <row r="48" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="F48" s="72"/>
       <c r="H48" s="72"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="72" t="s">
-        <v>231</v>
-      </c>
-      <c r="B49" s="72">
-        <v>1.02371286456331</v>
-      </c>
-      <c r="C49" s="72">
-        <v>1.0237139016294901</v>
-      </c>
-      <c r="D49" s="34">
-        <v>1.0237127741001699</v>
-      </c>
-      <c r="F49" s="72">
-        <f t="shared" si="13"/>
-        <v>9.0463140089980243E-8</v>
-      </c>
+    <row r="49" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F49" s="72"/>
       <c r="H49" s="72"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="72" t="s">
-        <v>210</v>
-      </c>
-      <c r="B50" s="72">
-        <v>1.0280925147905799</v>
-      </c>
-      <c r="C50" s="72">
-        <v>1.0280934274068501</v>
-      </c>
-      <c r="D50" s="34">
-        <v>1.0280924499320001</v>
-      </c>
-      <c r="F50" s="72">
-        <f t="shared" si="13"/>
-        <v>6.4858579840176844E-8</v>
-      </c>
+    <row r="50" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F50" s="72"/>
       <c r="H50" s="72"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="72" t="s">
-        <v>240</v>
-      </c>
-      <c r="B51" s="72">
-        <v>1.0385379019832599</v>
-      </c>
-      <c r="C51" s="72">
-        <v>1.03853856918465</v>
-      </c>
+    <row r="51" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F51" s="72"/>
-      <c r="G51" s="72">
-        <v>1.0340843666464401</v>
-      </c>
-      <c r="H51" s="72">
-        <f>B51-G51</f>
-        <v>4.4535353368198027E-3</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="72" t="s">
-        <v>232</v>
-      </c>
-      <c r="B52" s="72">
-        <v>1.04612245201456</v>
-      </c>
-      <c r="D52" s="72">
-        <v>1.04612260923001</v>
-      </c>
-      <c r="F52" s="72">
-        <f t="shared" si="13"/>
-        <v>-1.5721544999180992E-7</v>
-      </c>
+      <c r="G51" s="72"/>
+      <c r="H51" s="72"/>
+    </row>
+    <row r="52" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F52" s="72"/>
       <c r="H52" s="72"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="72" t="s">
-        <v>211</v>
-      </c>
-      <c r="B53" s="72">
-        <v>1.0850835071553799</v>
-      </c>
-      <c r="D53" s="34">
-        <v>1.0850835263671801</v>
-      </c>
-      <c r="F53" s="72">
-        <f t="shared" si="13"/>
-        <v>-1.921180015074242E-8</v>
-      </c>
+    <row r="53" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F53" s="72"/>
       <c r="H53" s="72"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="72" t="s">
-        <v>215</v>
-      </c>
-      <c r="B54" s="72">
-        <v>1.0349152577221601</v>
-      </c>
-      <c r="D54" s="72">
-        <v>1.03491546996032</v>
-      </c>
-      <c r="F54" s="72">
-        <f t="shared" si="13"/>
-        <v>-2.1223815993565154E-7</v>
-      </c>
+    <row r="54" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F54" s="72"/>
       <c r="H54" s="72"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="72" t="s">
-        <v>214</v>
-      </c>
-      <c r="B55" s="72">
-        <v>1.02798621556374</v>
-      </c>
-      <c r="G55" s="72">
-        <v>1.02971162455886</v>
-      </c>
-      <c r="H55" s="72">
-        <f t="shared" ref="H52:H59" si="14">B55-G55</f>
-        <v>-1.7254089951199703E-3</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="72" t="s">
-        <v>241</v>
-      </c>
-      <c r="B56" s="72">
-        <v>1.02970205350408</v>
-      </c>
-      <c r="G56" s="72">
-        <v>1.02966763377662</v>
-      </c>
-      <c r="H56" s="72">
-        <f t="shared" si="14"/>
-        <v>3.4419727459988891E-5</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="72" t="s">
-        <v>212</v>
-      </c>
-      <c r="B57" s="72">
-        <v>1.0240525230119499</v>
-      </c>
-      <c r="G57" s="72">
-        <v>1.0257083598498999</v>
-      </c>
-      <c r="H57" s="72">
-        <f t="shared" si="14"/>
-        <v>-1.6558368379500088E-3</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="72" t="s">
-        <v>213</v>
-      </c>
-      <c r="B58" s="72">
-        <v>1.01992383631813</v>
-      </c>
-      <c r="G58" s="72">
-        <v>1.0228316776611599</v>
-      </c>
-      <c r="H58" s="72">
-        <f t="shared" si="14"/>
-        <v>-2.9078413430299044E-3</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="72" t="s">
-        <v>248</v>
-      </c>
-      <c r="B59" s="72">
-        <v>1.00994172446495</v>
-      </c>
-      <c r="G59" s="72">
-        <v>1.0220031485954399</v>
-      </c>
-      <c r="H59" s="72">
-        <f t="shared" si="14"/>
-        <v>-1.2061424130489939E-2</v>
-      </c>
+    <row r="55" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="G55" s="72"/>
+      <c r="H55" s="72"/>
+    </row>
+    <row r="56" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="G56" s="72"/>
+      <c r="H56" s="72"/>
+    </row>
+    <row r="57" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="G57" s="72"/>
+      <c r="H57" s="72"/>
+    </row>
+    <row r="58" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="G58" s="72"/>
+      <c r="H58" s="72"/>
+    </row>
+    <row r="59" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="G59" s="72"/>
+      <c r="H59" s="72"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3504,6 +3140,409 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="72"/>
+      <c r="B1" s="72" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="72" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="34" t="s">
+        <v>272</v>
+      </c>
+      <c r="E1" s="34" t="s">
+        <v>273</v>
+      </c>
+      <c r="F1" s="34"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="72" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="72">
+        <v>0</v>
+      </c>
+      <c r="C2" s="72">
+        <v>0</v>
+      </c>
+      <c r="D2" s="34"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="72">
+        <v>-8.6707362007295993E-2</v>
+      </c>
+      <c r="C3" s="72">
+        <v>-8.6708237100475705E-2</v>
+      </c>
+      <c r="D3" s="34">
+        <v>0.13454518661145601</v>
+      </c>
+      <c r="E3" s="72">
+        <f>$B$4+D3</f>
+        <v>-8.6707535566243998E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" s="72">
+        <v>-0.22125272217770001</v>
+      </c>
+      <c r="C4" s="72">
+        <v>-0.22124896604786901</v>
+      </c>
+      <c r="D4" s="34">
+        <v>0</v>
+      </c>
+      <c r="E4" s="72">
+        <f t="shared" ref="E4:E10" si="0">$B$4+D4</f>
+        <v>-0.22125272217770001</v>
+      </c>
+      <c r="F4" s="72"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="72" t="s">
+        <v>261</v>
+      </c>
+      <c r="B5" s="72">
+        <v>-0.18120346048303301</v>
+      </c>
+      <c r="C5" s="72">
+        <v>-0.18120036659231001</v>
+      </c>
+      <c r="D5" s="34">
+        <v>4.0048858036497499E-2</v>
+      </c>
+      <c r="E5" s="72">
+        <f t="shared" si="0"/>
+        <v>-0.18120386414120251</v>
+      </c>
+      <c r="F5" s="72"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="72" t="s">
+        <v>262</v>
+      </c>
+      <c r="B6" s="72">
+        <v>-0.15469869726819899</v>
+      </c>
+      <c r="C6" s="72">
+        <v>-0.15469627337389699</v>
+      </c>
+      <c r="D6" s="34">
+        <v>6.6553625884739995E-2</v>
+      </c>
+      <c r="E6" s="72">
+        <f t="shared" si="0"/>
+        <v>-0.15469909629296003</v>
+      </c>
+      <c r="F6" s="72"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="72" t="s">
+        <v>263</v>
+      </c>
+      <c r="B7" s="72">
+        <v>-0.25510563387813501</v>
+      </c>
+      <c r="C7" s="72">
+        <v>-0.255101990043542</v>
+      </c>
+      <c r="E7" s="72"/>
+      <c r="F7" s="72"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="72" t="s">
+        <v>264</v>
+      </c>
+      <c r="B8" s="72">
+        <v>-0.238346440923459</v>
+      </c>
+      <c r="C8" s="72"/>
+      <c r="D8" s="72">
+        <v>-1.7094294986265499E-2</v>
+      </c>
+      <c r="E8" s="72">
+        <f t="shared" si="0"/>
+        <v>-0.2383470171639655</v>
+      </c>
+      <c r="F8" s="72"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="72" t="s">
+        <v>265</v>
+      </c>
+      <c r="B9" s="72">
+        <v>-0.23834653794917299</v>
+      </c>
+      <c r="D9" s="72">
+        <v>-1.7094298065348599E-2</v>
+      </c>
+      <c r="E9" s="72">
+        <f t="shared" si="0"/>
+        <v>-0.2383470202430486</v>
+      </c>
+      <c r="F9" s="72"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="72" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" s="72">
+        <v>-0.26806990591321</v>
+      </c>
+      <c r="D10" s="34">
+        <v>-4.6817626498101603E-2</v>
+      </c>
+      <c r="E10" s="72">
+        <f t="shared" si="0"/>
+        <v>-0.2680703486758016</v>
+      </c>
+      <c r="F10" s="72"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="72" t="s">
+        <v>266</v>
+      </c>
+      <c r="B11" s="72">
+        <v>-0.27110601345129198</v>
+      </c>
+      <c r="D11" s="34"/>
+      <c r="F11" s="72"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="72" t="s">
+        <v>267</v>
+      </c>
+      <c r="B12" s="72">
+        <v>-0.26564400434675201</v>
+      </c>
+      <c r="D12" s="34"/>
+      <c r="F12" s="72"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="72" t="s">
+        <v>268</v>
+      </c>
+      <c r="B13" s="72">
+        <v>-0.27078434534196499</v>
+      </c>
+      <c r="D13" s="34"/>
+      <c r="F13" s="72"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="72" t="s">
+        <v>269</v>
+      </c>
+      <c r="B14" s="72">
+        <v>-0.272427561300289</v>
+      </c>
+      <c r="D14" s="34"/>
+      <c r="F14" s="72"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="72" t="s">
+        <v>270</v>
+      </c>
+      <c r="B15" s="72">
+        <v>-0.28833317446325502</v>
+      </c>
+      <c r="D15" s="34"/>
+      <c r="F15" s="72"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="72">
+        <v>1.0599999427795399</v>
+      </c>
+      <c r="C16" s="72">
+        <v>1.05999978718632</v>
+      </c>
+      <c r="D16" s="34"/>
+      <c r="F16" s="72"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="72" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="72">
+        <v>1.04499995797579</v>
+      </c>
+      <c r="C17" s="72">
+        <v>1.04499963862116</v>
+      </c>
+      <c r="D17" s="34"/>
+      <c r="E17">
+        <v>1.04499906313014</v>
+      </c>
+      <c r="F17" s="72"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="72" t="s">
+        <v>94</v>
+      </c>
+      <c r="B18" s="72">
+        <v>1.0099999973080001</v>
+      </c>
+      <c r="C18" s="72">
+        <v>1.0100010595292099</v>
+      </c>
+      <c r="D18" s="34"/>
+      <c r="E18">
+        <v>1.0099998991758801</v>
+      </c>
+      <c r="F18" s="72"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="72" t="s">
+        <v>231</v>
+      </c>
+      <c r="B19" s="72">
+        <v>1.02371286456331</v>
+      </c>
+      <c r="C19" s="72">
+        <v>1.0237139016294901</v>
+      </c>
+      <c r="D19" s="34"/>
+      <c r="E19">
+        <v>1.0237127697133499</v>
+      </c>
+      <c r="F19" s="72"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="72" t="s">
+        <v>210</v>
+      </c>
+      <c r="B20" s="72">
+        <v>1.0280925147905799</v>
+      </c>
+      <c r="C20" s="72">
+        <v>1.0280934274068501</v>
+      </c>
+      <c r="D20" s="34"/>
+      <c r="E20">
+        <v>1.0280924472289901</v>
+      </c>
+      <c r="F20" s="72"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="72" t="s">
+        <v>240</v>
+      </c>
+      <c r="B21" s="72">
+        <v>1.0385379019832599</v>
+      </c>
+      <c r="C21" s="72">
+        <v>1.03853856918465</v>
+      </c>
+      <c r="F21" s="72"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="72" t="s">
+        <v>232</v>
+      </c>
+      <c r="B22" s="72">
+        <v>1.04612245201456</v>
+      </c>
+      <c r="D22" s="72"/>
+      <c r="E22">
+        <v>1.04612261065483</v>
+      </c>
+      <c r="F22" s="72"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="72" t="s">
+        <v>211</v>
+      </c>
+      <c r="B23" s="72">
+        <v>1.0850835071553799</v>
+      </c>
+      <c r="D23" s="34"/>
+      <c r="E23">
+        <v>1.08508352833644</v>
+      </c>
+      <c r="F23" s="72"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="72" t="s">
+        <v>215</v>
+      </c>
+      <c r="B24" s="72">
+        <v>1.0349152577221601</v>
+      </c>
+      <c r="D24" s="72"/>
+      <c r="E24">
+        <v>1.0349154728988099</v>
+      </c>
+      <c r="F24" s="72"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="72" t="s">
+        <v>214</v>
+      </c>
+      <c r="B25" s="72">
+        <v>1.02798621556374</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="72" t="s">
+        <v>241</v>
+      </c>
+      <c r="B26" s="72">
+        <v>1.02970205350408</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="72" t="s">
+        <v>212</v>
+      </c>
+      <c r="B27" s="72">
+        <v>1.0240525230119499</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="72" t="s">
+        <v>213</v>
+      </c>
+      <c r="B28" s="72">
+        <v>1.01992383631813</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="72" t="s">
+        <v>248</v>
+      </c>
+      <c r="B29" s="72">
+        <v>1.00994172446495</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Central Partition 3 results work.
Central Partition 3 results worked after adding measurements for P/Q6-13
and P/Q6-5.
</commit_message>
<xml_diff>
--- a/DMASE - Test Results.xlsx
+++ b/DMASE - Test Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12240" windowHeight="9240" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12240" windowHeight="9240" firstSheet="3" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="2 Bus" sheetId="4" r:id="rId1"/>
@@ -16,7 +16,7 @@
     <sheet name="14 Bus ADMM H" sheetId="9" r:id="rId7"/>
     <sheet name="14 Bus h" sheetId="10" r:id="rId8"/>
     <sheet name="14 Bus AC" sheetId="6" r:id="rId9"/>
-    <sheet name="Sheet1" sheetId="11" r:id="rId10"/>
+    <sheet name="14 Bus Partitions" sheetId="11" r:id="rId10"/>
     <sheet name="Sheet2" sheetId="12" r:id="rId11"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="939" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="278">
   <si>
     <t>Abur 3-Bus Case Measurements (run through SE, rerun new estimate again)</t>
   </si>
@@ -800,12 +800,6 @@
     <t>Q3-2</t>
   </si>
   <si>
-    <t>P6-5?</t>
-  </si>
-  <si>
-    <t>Q6-5?</t>
-  </si>
-  <si>
     <t>P9-4?</t>
   </si>
   <si>
@@ -839,13 +833,31 @@
     <t>th14</t>
   </si>
   <si>
-    <t>P5-4 = -P4-5</t>
-  </si>
-  <si>
     <t>x2 (unscaled)</t>
   </si>
   <si>
     <t>x2 + th3</t>
+  </si>
+  <si>
+    <t>x3 + th6</t>
+  </si>
+  <si>
+    <t>x4 (unscaled)</t>
+  </si>
+  <si>
+    <t>x3 (unscaled)</t>
+  </si>
+  <si>
+    <t>x4 + th9</t>
+  </si>
+  <si>
+    <t>P5-4 does not equal -P4-5</t>
+  </si>
+  <si>
+    <t>P6-5</t>
+  </si>
+  <si>
+    <t>Q6-5</t>
   </si>
 </sst>
 </file>
@@ -1093,7 +1105,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1297,6 +1309,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1856,8 +1869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S59"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:D59"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2159,14 +2172,14 @@
       </c>
       <c r="I7" s="74"/>
       <c r="K7" s="72" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L7" s="72">
-        <v>1.4392071686730901</v>
+        <v>17.236621109828601</v>
       </c>
       <c r="M7" s="72">
         <f t="shared" si="2"/>
-        <v>1.4392071686730901E-2</v>
+        <v>0.17236621109828601</v>
       </c>
       <c r="P7" s="72" t="s">
         <v>215</v>
@@ -2203,14 +2216,14 @@
       </c>
       <c r="I8" s="74"/>
       <c r="K8" s="72" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L8" s="72">
-        <v>0.52526799870488805</v>
+        <v>6.2088690408799696</v>
       </c>
       <c r="M8" s="72">
         <f t="shared" si="2"/>
-        <v>5.2526799870488807E-3</v>
+        <v>6.2088690408799697E-2</v>
       </c>
       <c r="P8" s="72" t="s">
         <v>214</v>
@@ -2247,14 +2260,14 @@
       </c>
       <c r="I9" s="74"/>
       <c r="K9" s="72" t="s">
-        <v>240</v>
+        <v>59</v>
       </c>
       <c r="L9" s="72">
-        <v>1.0385379019832599</v>
+        <v>1.4392071686730901</v>
       </c>
       <c r="M9" s="72">
-        <f>L9</f>
-        <v>1.0385379019832599</v>
+        <f>L9/100</f>
+        <v>1.4392071686730901E-2</v>
       </c>
       <c r="P9" s="72" t="s">
         <v>248</v>
@@ -2290,16 +2303,17 @@
         <v>1.02371286456331</v>
       </c>
       <c r="I10" s="74"/>
-      <c r="K10" t="s">
-        <v>241</v>
+      <c r="K10" s="72" t="s">
+        <v>125</v>
       </c>
       <c r="L10" s="72">
-        <v>1.02970205350408</v>
+        <v>0.52526799870488805</v>
       </c>
       <c r="M10" s="72">
-        <f t="shared" ref="M10:M12" si="7">L10</f>
-        <v>1.02970205350408</v>
-      </c>
+        <f>L10/100</f>
+        <v>5.2526799870488807E-3</v>
+      </c>
+      <c r="N10" s="72"/>
       <c r="P10" t="s">
         <v>249</v>
       </c>
@@ -2334,16 +2348,17 @@
         <v>1.04612245201456</v>
       </c>
       <c r="I11" s="74"/>
-      <c r="K11" t="s">
-        <v>212</v>
+      <c r="K11" s="72" t="s">
+        <v>240</v>
       </c>
       <c r="L11" s="72">
-        <v>1.0240525230119499</v>
+        <v>1.0385379019832599</v>
       </c>
       <c r="M11" s="72">
-        <f t="shared" si="7"/>
-        <v>1.0240525230119499</v>
-      </c>
+        <f>L11</f>
+        <v>1.0385379019832599</v>
+      </c>
+      <c r="N11" s="72"/>
       <c r="P11" t="s">
         <v>250</v>
       </c>
@@ -2351,7 +2366,7 @@
         <v>-16.599999</v>
       </c>
       <c r="R11" s="72">
-        <f t="shared" ref="R11:R21" si="8">Q11/100</f>
+        <f t="shared" ref="R11:R23" si="7">Q11/100</f>
         <v>-0.16599999000000001</v>
       </c>
     </row>
@@ -2379,14 +2394,14 @@
       </c>
       <c r="I12" s="74"/>
       <c r="K12" t="s">
-        <v>213</v>
+        <v>241</v>
       </c>
       <c r="L12" s="72">
-        <v>1.01992383631813</v>
+        <v>1.02970205350408</v>
       </c>
       <c r="M12" s="72">
-        <f t="shared" si="7"/>
-        <v>1.01992383631813</v>
+        <f t="shared" ref="M12:M14" si="8">L12</f>
+        <v>1.02970205350408</v>
       </c>
       <c r="P12" t="s">
         <v>251</v>
@@ -2395,7 +2410,7 @@
         <v>-9</v>
       </c>
       <c r="R12" s="72">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>-0.09</v>
       </c>
     </row>
@@ -2423,14 +2438,14 @@
       </c>
       <c r="I13" s="74"/>
       <c r="K13" t="s">
-        <v>242</v>
-      </c>
-      <c r="L13">
-        <v>-11.2</v>
-      </c>
-      <c r="M13">
-        <f>L13/100</f>
-        <v>-0.11199999999999999</v>
+        <v>212</v>
+      </c>
+      <c r="L13" s="72">
+        <v>1.0240525230119499</v>
+      </c>
+      <c r="M13" s="72">
+        <f t="shared" si="8"/>
+        <v>1.0240525230119499</v>
       </c>
       <c r="P13" t="s">
         <v>252</v>
@@ -2439,7 +2454,7 @@
         <v>-5.8</v>
       </c>
       <c r="R13" s="72">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>-5.7999999999999996E-2</v>
       </c>
     </row>
@@ -2469,15 +2484,14 @@
       </c>
       <c r="I14" s="74"/>
       <c r="K14" t="s">
-        <v>243</v>
+        <v>213</v>
       </c>
       <c r="L14" s="72">
-        <f>23.9999994635581-7.5</f>
-        <v>16.499999463558101</v>
+        <v>1.01992383631813</v>
       </c>
       <c r="M14" s="72">
-        <f t="shared" ref="M14:M24" si="11">L14/100</f>
-        <v>0.16499999463558102</v>
+        <f t="shared" si="8"/>
+        <v>1.01992383631813</v>
       </c>
       <c r="P14" t="s">
         <v>70</v>
@@ -2486,7 +2500,7 @@
         <v>-14.9</v>
       </c>
       <c r="R14" s="72">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>-0.14899999999999999</v>
       </c>
     </row>
@@ -2515,14 +2529,14 @@
       </c>
       <c r="I15" s="74"/>
       <c r="K15" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="L15">
-        <v>-3.5</v>
-      </c>
-      <c r="M15" s="72">
-        <f t="shared" si="11"/>
-        <v>-3.5000000000000003E-2</v>
+        <v>-11.2</v>
+      </c>
+      <c r="M15">
+        <f>L15/100</f>
+        <v>-0.11199999999999999</v>
       </c>
       <c r="P15" t="s">
         <v>135</v>
@@ -2531,7 +2545,7 @@
         <v>-5</v>
       </c>
       <c r="R15" s="72">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>-0.05</v>
       </c>
     </row>
@@ -2559,28 +2573,27 @@
       </c>
       <c r="I16" s="74"/>
       <c r="K16" t="s">
-        <v>245</v>
-      </c>
-      <c r="L16">
-        <v>-1.8</v>
+        <v>243</v>
+      </c>
+      <c r="L16" s="72">
+        <f>23.9999994635581-7.5</f>
+        <v>16.499999463558101</v>
       </c>
       <c r="M16" s="72">
-        <f t="shared" si="11"/>
-        <v>-1.8000000000000002E-2</v>
-      </c>
-      <c r="P16" t="s">
-        <v>253</v>
+        <f t="shared" ref="M16:M26" si="11">L16/100</f>
+        <v>0.16499999463558102</v>
+      </c>
+      <c r="P16" s="72" t="s">
+        <v>258</v>
       </c>
       <c r="Q16" s="72">
-        <v>-29.247637436823101</v>
+        <v>-16.079815706198001</v>
       </c>
       <c r="R16" s="72">
-        <f t="shared" si="8"/>
-        <v>-0.29247637436823104</v>
-      </c>
-      <c r="S16" s="74" t="s">
-        <v>227</v>
-      </c>
+        <f>Q16/100</f>
+        <v>-0.16079815706198</v>
+      </c>
+      <c r="S16" s="72"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="74" t="s">
@@ -2606,28 +2619,26 @@
       </c>
       <c r="I17" s="74"/>
       <c r="K17" t="s">
-        <v>12</v>
+        <v>244</v>
       </c>
       <c r="L17">
-        <v>-6.1</v>
+        <v>-3.5</v>
       </c>
       <c r="M17" s="72">
         <f t="shared" si="11"/>
-        <v>-6.0999999999999999E-2</v>
-      </c>
-      <c r="P17" t="s">
-        <v>254</v>
+        <v>-3.5000000000000003E-2</v>
+      </c>
+      <c r="P17" s="72" t="s">
+        <v>258</v>
       </c>
       <c r="Q17" s="72">
-        <v>-11.0919776937066</v>
+        <v>1.7323809918499999</v>
       </c>
       <c r="R17" s="72">
-        <f t="shared" si="8"/>
-        <v>-0.11091977693706599</v>
-      </c>
-      <c r="S17" s="74" t="s">
-        <v>227</v>
-      </c>
+        <f>Q17/100</f>
+        <v>1.7323809918500001E-2</v>
+      </c>
+      <c r="S17" s="72"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="74" t="s">
@@ -2655,26 +2666,26 @@
       </c>
       <c r="I18" s="74"/>
       <c r="K18" t="s">
-        <v>20</v>
+        <v>245</v>
       </c>
       <c r="L18">
-        <v>-1.6</v>
+        <v>-1.8</v>
       </c>
       <c r="M18" s="72">
         <f t="shared" si="11"/>
-        <v>-1.6E-2</v>
-      </c>
-      <c r="P18" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q18" s="72">
-        <v>-2.8744036925517298</v>
-      </c>
-      <c r="R18" s="72">
-        <f t="shared" si="8"/>
-        <v>-2.8744036925517299E-2</v>
-      </c>
-      <c r="S18" s="74" t="s">
+        <v>-1.8000000000000002E-2</v>
+      </c>
+      <c r="P18" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="Q18" s="2">
+        <v>-29.247637436823101</v>
+      </c>
+      <c r="R18" s="2">
+        <f t="shared" si="7"/>
+        <v>-0.29247637436823104</v>
+      </c>
+      <c r="S18" s="85" t="s">
         <v>227</v>
       </c>
     </row>
@@ -2704,26 +2715,26 @@
       </c>
       <c r="I19" s="74"/>
       <c r="K19" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="L19">
-        <v>-13.5</v>
+        <v>-6.1</v>
       </c>
       <c r="M19" s="72">
         <f t="shared" si="11"/>
-        <v>-0.13500000000000001</v>
-      </c>
-      <c r="P19" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q19" s="72">
-        <v>0.31779049296478201</v>
-      </c>
-      <c r="R19" s="72">
-        <f t="shared" si="8"/>
-        <v>3.1779049296478202E-3</v>
-      </c>
-      <c r="S19" s="74" t="s">
+        <v>-6.0999999999999999E-2</v>
+      </c>
+      <c r="P19" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="Q19" s="2">
+        <v>-11.0919776937066</v>
+      </c>
+      <c r="R19" s="2">
+        <f t="shared" si="7"/>
+        <v>-0.11091977693706599</v>
+      </c>
+      <c r="S19" s="85" t="s">
         <v>227</v>
       </c>
     </row>
@@ -2753,26 +2764,26 @@
       </c>
       <c r="I20" s="74"/>
       <c r="K20" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L20">
-        <v>-5.8</v>
+        <v>-1.6</v>
       </c>
       <c r="M20" s="72">
         <f t="shared" si="11"/>
-        <v>-5.7999999999999996E-2</v>
-      </c>
-      <c r="P20" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="Q20" s="2">
-        <v>-4.9650161007164098</v>
-      </c>
-      <c r="R20" s="2">
-        <f t="shared" si="8"/>
-        <v>-4.9650161007164101E-2</v>
-      </c>
-      <c r="S20" s="85" t="s">
+        <v>-1.6E-2</v>
+      </c>
+      <c r="P20" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q20" s="72">
+        <v>-2.8744036925517298</v>
+      </c>
+      <c r="R20" s="72">
+        <f t="shared" si="7"/>
+        <v>-2.8744036925517299E-2</v>
+      </c>
+      <c r="S20" s="74" t="s">
         <v>227</v>
       </c>
     </row>
@@ -2803,30 +2814,27 @@
       <c r="I21" s="85" t="s">
         <v>227</v>
       </c>
-      <c r="K21" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="L21" s="2">
-        <v>2.8808971477310599</v>
-      </c>
-      <c r="M21" s="2">
-        <f>L21/100</f>
-        <v>2.88089714773106E-2</v>
-      </c>
-      <c r="N21" s="85" t="s">
-        <v>227</v>
-      </c>
-      <c r="P21" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="Q21" s="2">
-        <v>-0.52427629116916796</v>
-      </c>
-      <c r="R21" s="2">
-        <f t="shared" si="8"/>
-        <v>-5.2427629116916794E-3</v>
-      </c>
-      <c r="S21" s="85" t="s">
+      <c r="K21" t="s">
+        <v>16</v>
+      </c>
+      <c r="L21">
+        <v>-13.5</v>
+      </c>
+      <c r="M21" s="72">
+        <f t="shared" si="11"/>
+        <v>-0.13500000000000001</v>
+      </c>
+      <c r="P21" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q21" s="72">
+        <v>0.31779049296478201</v>
+      </c>
+      <c r="R21" s="72">
+        <f t="shared" si="7"/>
+        <v>3.1779049296478202E-3</v>
+      </c>
+      <c r="S21" s="74" t="s">
         <v>227</v>
       </c>
     </row>
@@ -2857,17 +2865,27 @@
       <c r="I22" s="85" t="s">
         <v>227</v>
       </c>
-      <c r="K22" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="L22" s="2">
-        <v>-0.30259003060574602</v>
-      </c>
-      <c r="M22" s="2">
-        <f>L22/100</f>
-        <v>-3.0259003060574604E-3</v>
-      </c>
-      <c r="N22" s="85" t="s">
+      <c r="K22" t="s">
+        <v>22</v>
+      </c>
+      <c r="L22">
+        <v>-5.8</v>
+      </c>
+      <c r="M22" s="72">
+        <f t="shared" si="11"/>
+        <v>-5.7999999999999996E-2</v>
+      </c>
+      <c r="P22" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="Q22" s="2">
+        <v>-4.9650161007164098</v>
+      </c>
+      <c r="R22" s="2">
+        <f t="shared" si="7"/>
+        <v>-4.9650161007164101E-2</v>
+      </c>
+      <c r="S22" s="85" t="s">
         <v>227</v>
       </c>
     </row>
@@ -2898,17 +2916,30 @@
       <c r="I23" s="74" t="s">
         <v>227</v>
       </c>
-      <c r="K23" t="s">
-        <v>68</v>
-      </c>
-      <c r="L23" s="72">
-        <v>4.9650161007164098</v>
-      </c>
-      <c r="M23" s="72">
-        <f t="shared" si="11"/>
-        <v>4.9650161007164101E-2</v>
-      </c>
-      <c r="N23" s="74" t="s">
+      <c r="K23" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="L23" s="2">
+        <v>-42.467163764624999</v>
+      </c>
+      <c r="M23" s="2">
+        <f>L23/100</f>
+        <v>-0.42467163764624999</v>
+      </c>
+      <c r="N23" s="85" t="s">
+        <v>227</v>
+      </c>
+      <c r="P23" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="Q23" s="2">
+        <v>-0.52427629116916796</v>
+      </c>
+      <c r="R23" s="2">
+        <f t="shared" si="7"/>
+        <v>-5.2427629116916794E-3</v>
+      </c>
+      <c r="S23" s="85" t="s">
         <v>227</v>
       </c>
     </row>
@@ -2926,17 +2957,17 @@
       <c r="I24" s="74" t="s">
         <v>227</v>
       </c>
-      <c r="K24" t="s">
-        <v>133</v>
-      </c>
-      <c r="L24" s="72">
-        <v>0.52427629116916796</v>
-      </c>
-      <c r="M24" s="72">
-        <f t="shared" si="11"/>
-        <v>5.2427629116916794E-3</v>
-      </c>
-      <c r="N24" s="74" t="s">
+      <c r="K24" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="L24" s="2">
+        <v>6.4382015347410002</v>
+      </c>
+      <c r="M24" s="2">
+        <f>L24/100</f>
+        <v>6.4382015347410004E-2</v>
+      </c>
+      <c r="N24" s="85" t="s">
         <v>227</v>
       </c>
     </row>
@@ -2954,12 +2985,23 @@
       <c r="I25" s="74" t="s">
         <v>227</v>
       </c>
-      <c r="P25" s="72"/>
-      <c r="Q25" s="72"/>
+      <c r="K25" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="L25" s="2">
+        <v>2.8808971477310599</v>
+      </c>
+      <c r="M25" s="2">
+        <f>L25/100</f>
+        <v>2.88089714773106E-2</v>
+      </c>
+      <c r="N25" s="85" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="72" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="F26" s="20" t="s">
         <v>131</v>
@@ -2974,34 +3016,60 @@
       <c r="I26" s="74" t="s">
         <v>227</v>
       </c>
-      <c r="K26" t="s">
-        <v>258</v>
-      </c>
-      <c r="P26" s="72" t="s">
-        <v>260</v>
-      </c>
-      <c r="Q26" s="72"/>
+      <c r="K26" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="L26" s="2">
+        <v>-0.30259003060574602</v>
+      </c>
+      <c r="M26" s="2">
+        <f>L26/100</f>
+        <v>-3.0259003060574604E-3</v>
+      </c>
+      <c r="N26" s="85" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="72"/>
       <c r="K27" t="s">
-        <v>259</v>
-      </c>
-      <c r="P27" t="s">
-        <v>260</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="L27" s="72">
+        <v>4.9650161007164098</v>
+      </c>
+      <c r="M27" s="72">
+        <f>L27/100</f>
+        <v>4.9650161007164101E-2</v>
+      </c>
+      <c r="N27" s="74" t="s">
+        <v>227</v>
+      </c>
+      <c r="P27" s="72"/>
       <c r="Q27" s="72"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="K28" s="72"/>
-      <c r="L28" s="72"/>
+      <c r="K28" t="s">
+        <v>133</v>
+      </c>
+      <c r="L28" s="72">
+        <v>0.52427629116916796</v>
+      </c>
+      <c r="M28" s="72">
+        <f>L28/100</f>
+        <v>5.2427629116916794E-3</v>
+      </c>
+      <c r="N28" s="74" t="s">
+        <v>227</v>
+      </c>
+      <c r="P28" s="72"/>
+      <c r="Q28" s="72"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E29" s="72"/>
       <c r="G29" s="72"/>
       <c r="H29" s="72"/>
-      <c r="L29" s="72"/>
-      <c r="M29" s="72"/>
+      <c r="P29" s="72"/>
       <c r="Q29" s="72"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
@@ -3010,79 +3078,86 @@
       <c r="E30" s="72"/>
       <c r="G30" s="72"/>
       <c r="H30" s="72"/>
-      <c r="Q30" s="72"/>
+      <c r="K30" s="72"/>
+      <c r="L30" s="72"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E31" s="72"/>
       <c r="H31" s="72"/>
       <c r="I31" s="72"/>
+      <c r="K31" s="72"/>
       <c r="L31" s="72"/>
+      <c r="M31" s="72"/>
       <c r="Q31" s="72"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E32" s="72"/>
       <c r="H32" s="72"/>
       <c r="I32" s="72"/>
+      <c r="K32" s="72"/>
       <c r="L32" s="72"/>
-    </row>
-    <row r="33" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="Q32" s="72"/>
+    </row>
+    <row r="33" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E33" s="72"/>
       <c r="F33" s="72"/>
       <c r="J33" s="72"/>
-      <c r="K33" s="72"/>
-      <c r="L33" s="72"/>
-    </row>
-    <row r="34" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="Q33" s="72"/>
+    </row>
+    <row r="34" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E34" s="72"/>
       <c r="F34" s="72"/>
       <c r="G34" s="72"/>
       <c r="H34" s="72"/>
       <c r="I34" s="72"/>
       <c r="J34" s="72"/>
-      <c r="K34" s="72"/>
       <c r="L34" s="72"/>
     </row>
-    <row r="35" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="5:17" x14ac:dyDescent="0.25">
       <c r="F35" s="72"/>
       <c r="G35" s="72"/>
       <c r="H35" s="72"/>
       <c r="J35" s="72"/>
-    </row>
-    <row r="36" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="K35" s="72"/>
+      <c r="L35" s="72"/>
+    </row>
+    <row r="36" spans="5:17" x14ac:dyDescent="0.25">
       <c r="F36" s="72"/>
       <c r="G36" s="72"/>
       <c r="H36" s="72"/>
-    </row>
-    <row r="37" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="K36" s="72"/>
+      <c r="L36" s="72"/>
+    </row>
+    <row r="37" spans="5:17" x14ac:dyDescent="0.25">
       <c r="F37" s="72"/>
       <c r="G37" s="72"/>
       <c r="H37" s="72"/>
     </row>
-    <row r="38" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="5:17" x14ac:dyDescent="0.25">
       <c r="F38" s="72"/>
       <c r="G38" s="72"/>
       <c r="H38" s="72"/>
     </row>
-    <row r="39" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="5:17" x14ac:dyDescent="0.25">
       <c r="F39" s="72"/>
       <c r="G39" s="72"/>
       <c r="H39" s="72"/>
     </row>
-    <row r="40" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="5:17" x14ac:dyDescent="0.25">
       <c r="F40" s="72"/>
       <c r="G40" s="72"/>
       <c r="H40" s="72"/>
     </row>
-    <row r="41" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="5:17" x14ac:dyDescent="0.25">
       <c r="G41" s="72"/>
     </row>
-    <row r="42" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="5:17" x14ac:dyDescent="0.25">
       <c r="G42" s="72"/>
     </row>
-    <row r="47" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="5:17" x14ac:dyDescent="0.25">
       <c r="F47" s="72"/>
     </row>
-    <row r="48" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="5:17" x14ac:dyDescent="0.25">
       <c r="F48" s="72"/>
       <c r="H48" s="72"/>
     </row>
@@ -3145,20 +3220,28 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:Q29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="R29" sqref="R29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="72" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="72" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="72"/>
+    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="72"/>
       <c r="B1" s="72" t="s">
         <v>8</v>
@@ -3166,15 +3249,41 @@
       <c r="C1" s="72" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="E1" s="34" t="s">
+        <v>269</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>270</v>
+      </c>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34" t="s">
+        <v>273</v>
+      </c>
+      <c r="I1" s="34" t="s">
+        <v>271</v>
+      </c>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34" t="s">
         <v>272</v>
       </c>
-      <c r="E1" s="34" t="s">
-        <v>273</v>
-      </c>
-      <c r="F1" s="34"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="L1" s="34" t="s">
+        <v>274</v>
+      </c>
+      <c r="M1" s="93"/>
+      <c r="N1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="72" t="s">
         <v>91</v>
       </c>
@@ -3184,361 +3293,840 @@
       <c r="C2" s="72">
         <v>0</v>
       </c>
-      <c r="D2" s="34"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E2" s="34"/>
+      <c r="M2" s="93"/>
+      <c r="N2">
+        <f>B2-C2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>92</v>
       </c>
       <c r="B3" s="72">
-        <v>-8.6707362007295993E-2</v>
+        <v>-8.6669791486718703E-2</v>
       </c>
       <c r="C3" s="72">
         <v>-8.6708237100475705E-2</v>
       </c>
-      <c r="D3" s="34">
+      <c r="E3" s="34">
         <v>0.13454518661145601</v>
       </c>
-      <c r="E3" s="72">
-        <f>$B$4+D3</f>
-        <v>-8.6707535566243998E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F3" s="72">
+        <f>$B$4+E3</f>
+        <v>-8.6616927051581E-2</v>
+      </c>
+      <c r="M3" s="93"/>
+      <c r="N3" s="72">
+        <f>B3-C3</f>
+        <v>3.8445613757001618E-5</v>
+      </c>
+      <c r="O3">
+        <f>B3-F3</f>
+        <v>-5.2864435137703336E-5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>93</v>
       </c>
       <c r="B4" s="72">
-        <v>-0.22125272217770001</v>
+        <v>-0.22116211366303701</v>
       </c>
       <c r="C4" s="72">
         <v>-0.22124896604786901</v>
       </c>
-      <c r="D4" s="34">
-        <v>0</v>
-      </c>
-      <c r="E4" s="72">
-        <f t="shared" ref="E4:E10" si="0">$B$4+D4</f>
-        <v>-0.22125272217770001</v>
-      </c>
-      <c r="F4" s="72"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E4" s="34">
+        <v>0</v>
+      </c>
+      <c r="F4" s="72">
+        <f t="shared" ref="F4:F10" si="0">$B$4+E4</f>
+        <v>-0.22116211366303701</v>
+      </c>
+      <c r="H4" s="72"/>
+      <c r="M4" s="93"/>
+      <c r="N4" s="72">
+        <f>B4-C4</f>
+        <v>8.6852384831997975E-5</v>
+      </c>
+      <c r="O4" s="72">
+        <f t="shared" ref="O4:O10" si="1">B4-F4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="72" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B5" s="72">
-        <v>-0.18120346048303301</v>
+        <v>-0.18108637306068801</v>
       </c>
       <c r="C5" s="72">
         <v>-0.18120036659231001</v>
       </c>
-      <c r="D5" s="34">
+      <c r="E5" s="34">
         <v>4.0048858036497499E-2</v>
       </c>
-      <c r="E5" s="72">
+      <c r="F5" s="72">
         <f t="shared" si="0"/>
-        <v>-0.18120386414120251</v>
-      </c>
-      <c r="F5" s="72"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>-0.18111325562653952</v>
+      </c>
+      <c r="H5" s="72"/>
+      <c r="K5">
+        <v>8.4777565687419704E-2</v>
+      </c>
+      <c r="L5">
+        <f>$B$10+K5</f>
+        <v>-0.18304977592106428</v>
+      </c>
+      <c r="M5" s="93"/>
+      <c r="N5" s="72">
+        <f>B5-C5</f>
+        <v>1.139935316220031E-4</v>
+      </c>
+      <c r="O5" s="72">
+        <f t="shared" si="1"/>
+        <v>2.6882565851510387E-5</v>
+      </c>
+      <c r="Q5">
+        <f>B5-L5</f>
+        <v>1.9634028603762732E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="72" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B6" s="72">
-        <v>-0.15469869726819899</v>
+        <v>-0.15459540540712</v>
       </c>
       <c r="C6" s="72">
         <v>-0.15469627337389699</v>
       </c>
-      <c r="D6" s="34">
+      <c r="E6" s="34">
         <v>6.6553625884739995E-2</v>
       </c>
-      <c r="E6" s="72">
+      <c r="F6" s="72">
         <f t="shared" si="0"/>
-        <v>-0.15469909629296003</v>
-      </c>
-      <c r="F6" s="72"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>-0.154608487778297</v>
+      </c>
+      <c r="H6" s="72">
+        <v>0.10040928822293101</v>
+      </c>
+      <c r="I6" s="72">
+        <f>$B$7+H6</f>
+        <v>-0.15449621523418899</v>
+      </c>
+      <c r="L6" s="72"/>
+      <c r="M6" s="93"/>
+      <c r="N6" s="72">
+        <f>B6-C6</f>
+        <v>1.0086796677699628E-4</v>
+      </c>
+      <c r="O6" s="72">
+        <f t="shared" si="1"/>
+        <v>1.3082371177003393E-5</v>
+      </c>
+      <c r="P6">
+        <f>B6-I6</f>
+        <v>-9.9190172931001852E-5</v>
+      </c>
+      <c r="Q6" s="72"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="72" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B7" s="72">
-        <v>-0.25510563387813501</v>
+        <v>-0.25490550345711999</v>
       </c>
       <c r="C7" s="72">
         <v>-0.255101990043542</v>
       </c>
-      <c r="E7" s="72"/>
       <c r="F7" s="72"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H7" s="72">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <f>$B$7+H7</f>
+        <v>-0.25490550345711999</v>
+      </c>
+      <c r="L7" s="72"/>
+      <c r="M7" s="93"/>
+      <c r="N7" s="72">
+        <f>B7-C7</f>
+        <v>1.9648658642201777E-4</v>
+      </c>
+      <c r="O7" s="72"/>
+      <c r="P7" s="72">
+        <f>B7-I7</f>
+        <v>0</v>
+      </c>
+      <c r="Q7" s="72"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="72" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B8" s="72">
-        <v>-0.238346440923459</v>
+        <v>-0.238124828874305</v>
       </c>
       <c r="C8" s="72"/>
-      <c r="D8" s="72">
+      <c r="E8" s="72">
         <v>-1.7094294986265499E-2</v>
       </c>
-      <c r="E8" s="72">
+      <c r="F8" s="72">
         <f t="shared" si="0"/>
-        <v>-0.2383470171639655</v>
-      </c>
-      <c r="F8" s="72"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>-0.2382564086493025</v>
+      </c>
+      <c r="I8" s="72"/>
+      <c r="K8">
+        <v>2.9803356989265999E-2</v>
+      </c>
+      <c r="L8" s="72">
+        <f t="shared" ref="L6:L15" si="2">$B$10+K8</f>
+        <v>-0.23802398461921798</v>
+      </c>
+      <c r="M8" s="93"/>
+      <c r="N8" s="72"/>
+      <c r="O8" s="72">
+        <f t="shared" si="1"/>
+        <v>1.315797749975034E-4</v>
+      </c>
+      <c r="Q8" s="72">
+        <f t="shared" ref="Q6:Q29" si="3">B8-L8</f>
+        <v>-1.0084425508702366E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="72" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B9" s="72">
-        <v>-0.23834653794917299</v>
-      </c>
-      <c r="D9" s="72">
+        <v>-0.23811416408082101</v>
+      </c>
+      <c r="E9" s="72">
         <v>-1.7094298065348599E-2</v>
       </c>
-      <c r="E9" s="72">
+      <c r="F9" s="72">
         <f t="shared" si="0"/>
-        <v>-0.2383470202430486</v>
-      </c>
-      <c r="F9" s="72"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>-0.2382564117283856</v>
+      </c>
+      <c r="I9" s="72"/>
+      <c r="L9" s="72"/>
+      <c r="M9" s="93"/>
+      <c r="N9" s="72"/>
+      <c r="O9" s="72">
+        <f t="shared" si="1"/>
+        <v>1.4224764756459729E-4</v>
+      </c>
+      <c r="Q9" s="72"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="72" t="s">
         <v>71</v>
       </c>
       <c r="B10" s="72">
-        <v>-0.26806990591321</v>
-      </c>
-      <c r="D10" s="34">
+        <v>-0.26782734160848398</v>
+      </c>
+      <c r="E10" s="34">
         <v>-4.6817626498101603E-2</v>
       </c>
-      <c r="E10" s="72">
+      <c r="F10" s="72">
         <f t="shared" si="0"/>
-        <v>-0.2680703486758016</v>
-      </c>
-      <c r="F10" s="72"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>-0.26797974016113862</v>
+      </c>
+      <c r="I10" s="72"/>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10" s="72">
+        <f t="shared" si="2"/>
+        <v>-0.26782734160848398</v>
+      </c>
+      <c r="M10" s="93"/>
+      <c r="N10" s="72"/>
+      <c r="O10" s="72">
+        <f t="shared" si="1"/>
+        <v>1.5239855265464231E-4</v>
+      </c>
+      <c r="Q10" s="72">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="72" t="s">
+        <v>264</v>
+      </c>
+      <c r="B11" s="72">
+        <v>-0.27082639634655098</v>
+      </c>
+      <c r="E11" s="34"/>
+      <c r="H11">
+        <v>-1.59962164357162E-2</v>
+      </c>
+      <c r="I11" s="72">
+        <f t="shared" ref="I11:I15" si="4">$B$7+H11</f>
+        <v>-0.27090171989283618</v>
+      </c>
+      <c r="K11">
+        <v>-2.8854192291146198E-3</v>
+      </c>
+      <c r="L11" s="72">
+        <f t="shared" si="2"/>
+        <v>-0.2707127608375986</v>
+      </c>
+      <c r="M11" s="93"/>
+      <c r="N11" s="72"/>
+      <c r="P11">
+        <f>B11-I11</f>
+        <v>7.5323546285199772E-5</v>
+      </c>
+      <c r="Q11" s="72">
+        <f t="shared" si="3"/>
+        <v>-1.1363550895238106E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="72" t="s">
+        <v>265</v>
+      </c>
+      <c r="B12" s="72">
+        <v>-0.26537530725671299</v>
+      </c>
+      <c r="E12" s="34"/>
+      <c r="H12">
+        <v>-1.05354439253986E-2</v>
+      </c>
+      <c r="I12" s="72">
+        <f t="shared" si="4"/>
+        <v>-0.26544094738251861</v>
+      </c>
+      <c r="K12">
+        <v>2.76657675401411E-3</v>
+      </c>
+      <c r="L12" s="72">
+        <f t="shared" si="2"/>
+        <v>-0.26506076485446989</v>
+      </c>
+      <c r="M12" s="93"/>
+      <c r="N12" s="72"/>
+      <c r="P12" s="72">
+        <f t="shared" ref="P12:P15" si="5">B12-I12</f>
+        <v>6.5640125805621619E-5</v>
+      </c>
+      <c r="Q12" s="72">
+        <f t="shared" si="3"/>
+        <v>-3.1454240224310093E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="72" t="s">
         <v>266</v>
       </c>
-      <c r="B11" s="72">
-        <v>-0.27110601345129198</v>
-      </c>
-      <c r="D11" s="34"/>
-      <c r="F11" s="72"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="72" t="s">
+      <c r="B13" s="72">
+        <v>-0.27056740976696902</v>
+      </c>
+      <c r="E13" s="34"/>
+      <c r="H13">
+        <v>-1.5681481070227099E-2</v>
+      </c>
+      <c r="I13" s="72">
+        <f t="shared" si="4"/>
+        <v>-0.27058698452734709</v>
+      </c>
+      <c r="L13" s="72"/>
+      <c r="M13" s="93"/>
+      <c r="N13" s="72"/>
+      <c r="P13" s="72">
+        <f t="shared" si="5"/>
+        <v>1.9574760378060496E-5</v>
+      </c>
+      <c r="Q13" s="72"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="72" t="s">
         <v>267</v>
       </c>
-      <c r="B12" s="72">
-        <v>-0.26564400434675201</v>
-      </c>
-      <c r="D12" s="34"/>
-      <c r="F12" s="72"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="72" t="s">
+      <c r="B14" s="72">
+        <v>-0.272193451087546</v>
+      </c>
+      <c r="E14" s="34"/>
+      <c r="H14" s="72">
+        <v>-1.73222072322563E-2</v>
+      </c>
+      <c r="I14" s="72">
+        <f t="shared" si="4"/>
+        <v>-0.27222771068937629</v>
+      </c>
+      <c r="K14">
+        <v>-3.4089835958288602E-3</v>
+      </c>
+      <c r="L14" s="72">
+        <f t="shared" si="2"/>
+        <v>-0.27123632520431284</v>
+      </c>
+      <c r="M14" s="93"/>
+      <c r="N14" s="72"/>
+      <c r="P14" s="72">
+        <f t="shared" si="5"/>
+        <v>3.4259601830288755E-5</v>
+      </c>
+      <c r="Q14" s="72">
+        <f t="shared" si="3"/>
+        <v>-9.5712588323315639E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="72" t="s">
         <v>268</v>
       </c>
-      <c r="B13" s="72">
-        <v>-0.27078434534196499</v>
-      </c>
-      <c r="D13" s="34"/>
-      <c r="F13" s="72"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="72" t="s">
-        <v>269</v>
-      </c>
-      <c r="B14" s="72">
-        <v>-0.272427561300289</v>
-      </c>
-      <c r="D14" s="34"/>
-      <c r="F14" s="72"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="72" t="s">
-        <v>270</v>
-      </c>
       <c r="B15" s="72">
-        <v>-0.28833317446325502</v>
-      </c>
-      <c r="D15" s="34"/>
-      <c r="F15" s="72"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>-0.28803193308711</v>
+      </c>
+      <c r="E15" s="34"/>
+      <c r="H15" s="72">
+        <v>-3.32188944082469E-2</v>
+      </c>
+      <c r="I15" s="72">
+        <f t="shared" si="4"/>
+        <v>-0.28812439786536687</v>
+      </c>
+      <c r="K15">
+        <v>-1.9713877950687402E-2</v>
+      </c>
+      <c r="L15" s="72">
+        <f t="shared" si="2"/>
+        <v>-0.28754121955917139</v>
+      </c>
+      <c r="M15" s="93"/>
+      <c r="N15" s="72"/>
+      <c r="P15" s="72">
+        <f t="shared" si="5"/>
+        <v>9.2464778256862168E-5</v>
+      </c>
+      <c r="Q15" s="72">
+        <f t="shared" si="3"/>
+        <v>-4.9071352793861323E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>26</v>
       </c>
       <c r="B16" s="72">
-        <v>1.0599999427795399</v>
+        <v>1.06021182972759</v>
       </c>
       <c r="C16" s="72">
         <v>1.05999978718632</v>
       </c>
-      <c r="D16" s="34"/>
-      <c r="F16" s="72"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E16" s="34"/>
+      <c r="H16" s="72"/>
+      <c r="M16" s="93"/>
+      <c r="N16" s="72">
+        <f>B16-C16</f>
+        <v>2.1204254126994115E-4</v>
+      </c>
+      <c r="Q16" s="72"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="72" t="s">
         <v>28</v>
       </c>
       <c r="B17" s="72">
-        <v>1.04499995797579</v>
+        <v>1.04521069537303</v>
       </c>
       <c r="C17" s="72">
         <v>1.04499963862116</v>
       </c>
-      <c r="D17" s="34"/>
-      <c r="E17">
+      <c r="E17" s="72">
         <v>1.04499906313014</v>
       </c>
-      <c r="F17" s="72"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <v>1.04499906313014</v>
+      </c>
+      <c r="H17" s="72"/>
+      <c r="M17" s="93"/>
+      <c r="N17" s="72">
+        <f>B17-C17</f>
+        <v>2.1105675187005346E-4</v>
+      </c>
+      <c r="O17">
+        <f>B17-F17</f>
+        <v>2.1163224289000304E-4</v>
+      </c>
+      <c r="Q17" s="72"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="72" t="s">
         <v>94</v>
       </c>
       <c r="B18" s="72">
-        <v>1.0099999973080001</v>
+        <v>1.0102223344885899</v>
       </c>
       <c r="C18" s="72">
         <v>1.0100010595292099</v>
       </c>
-      <c r="D18" s="34"/>
-      <c r="E18">
+      <c r="E18" s="72">
         <v>1.0099998991758801</v>
       </c>
-      <c r="F18" s="72"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <v>1.0099998991758801</v>
+      </c>
+      <c r="H18" s="72"/>
+      <c r="M18" s="93"/>
+      <c r="N18" s="72">
+        <f>B18-C18</f>
+        <v>2.2127495937995789E-4</v>
+      </c>
+      <c r="O18" s="72">
+        <f t="shared" ref="O18:O24" si="6">B18-F18</f>
+        <v>2.2243531270982331E-4</v>
+      </c>
+      <c r="Q18" s="72"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="72" t="s">
         <v>231</v>
       </c>
       <c r="B19" s="72">
-        <v>1.02371286456331</v>
+        <v>1.0238916772678499</v>
       </c>
       <c r="C19" s="72">
         <v>1.0237139016294901</v>
       </c>
-      <c r="D19" s="34"/>
-      <c r="E19">
+      <c r="E19" s="72">
         <v>1.0237127697133499</v>
       </c>
-      <c r="F19" s="72"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <v>1.0237127697133499</v>
+      </c>
+      <c r="H19" s="72"/>
+      <c r="K19">
+        <v>1.0267750886447</v>
+      </c>
+      <c r="L19">
+        <f>K19</f>
+        <v>1.0267750886447</v>
+      </c>
+      <c r="M19" s="93"/>
+      <c r="N19" s="72">
+        <f>B19-C19</f>
+        <v>1.777756383598561E-4</v>
+      </c>
+      <c r="O19" s="72">
+        <f t="shared" si="6"/>
+        <v>1.7890755450000739E-4</v>
+      </c>
+      <c r="Q19" s="72">
+        <f t="shared" si="3"/>
+        <v>-2.8834113768501091E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="72" t="s">
         <v>210</v>
       </c>
       <c r="B20" s="72">
-        <v>1.0280925147905799</v>
+        <v>1.02827099057284</v>
       </c>
       <c r="C20" s="72">
         <v>1.0280934274068501</v>
       </c>
-      <c r="D20" s="34"/>
-      <c r="E20">
+      <c r="E20" s="72">
         <v>1.0280924472289901</v>
       </c>
-      <c r="F20" s="72"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <v>1.0280924472289901</v>
+      </c>
+      <c r="H20" s="72">
+        <v>1.0280804768676</v>
+      </c>
+      <c r="I20" s="72">
+        <v>1.0280804768676</v>
+      </c>
+      <c r="L20" s="72"/>
+      <c r="M20" s="93"/>
+      <c r="N20" s="72">
+        <f>B20-C20</f>
+        <v>1.7756316598993571E-4</v>
+      </c>
+      <c r="O20" s="72">
+        <f t="shared" si="6"/>
+        <v>1.7854334384992399E-4</v>
+      </c>
+      <c r="P20">
+        <f>B20-I20</f>
+        <v>1.905137052400363E-4</v>
+      </c>
+      <c r="Q20" s="72"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="72" t="s">
         <v>240</v>
       </c>
       <c r="B21" s="72">
-        <v>1.0385379019832599</v>
+        <v>1.0384892284060301</v>
       </c>
       <c r="C21" s="72">
         <v>1.03853856918465</v>
       </c>
-      <c r="F21" s="72"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E21" s="72"/>
+      <c r="H21" s="72">
+        <v>1.03853803524227</v>
+      </c>
+      <c r="I21" s="72">
+        <v>1.03853803524227</v>
+      </c>
+      <c r="L21" s="72"/>
+      <c r="M21" s="93"/>
+      <c r="N21" s="72">
+        <f>B21-C21</f>
+        <v>-4.9340778619955117E-5</v>
+      </c>
+      <c r="O21" s="72"/>
+      <c r="P21" s="72">
+        <f t="shared" ref="P21:P29" si="7">B21-I21</f>
+        <v>-4.8806836239867479E-5</v>
+      </c>
+      <c r="Q21" s="72"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="72" t="s">
         <v>232</v>
       </c>
       <c r="B22" s="72">
-        <v>1.04612245201456</v>
-      </c>
-      <c r="D22" s="72"/>
-      <c r="E22">
+        <v>1.0461591070376699</v>
+      </c>
+      <c r="E22" s="72">
         <v>1.04612261065483</v>
       </c>
-      <c r="F22" s="72"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F22">
+        <v>1.04612261065483</v>
+      </c>
+      <c r="I22" s="72"/>
+      <c r="K22">
+        <v>1.04677077937396</v>
+      </c>
+      <c r="L22" s="72">
+        <f t="shared" ref="L20:L29" si="8">K22</f>
+        <v>1.04677077937396</v>
+      </c>
+      <c r="M22" s="93"/>
+      <c r="N22" s="72"/>
+      <c r="O22" s="72">
+        <f t="shared" si="6"/>
+        <v>3.6496382839867891E-5</v>
+      </c>
+      <c r="P22" s="72"/>
+      <c r="Q22" s="72">
+        <f t="shared" si="3"/>
+        <v>-6.1167233629011442E-4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="72" t="s">
         <v>211</v>
       </c>
       <c r="B23" s="72">
-        <v>1.0850835071553799</v>
-      </c>
-      <c r="D23" s="34"/>
-      <c r="E23">
+        <v>1.08522332015065</v>
+      </c>
+      <c r="E23" s="72">
         <v>1.08508352833644</v>
       </c>
-      <c r="F23" s="72"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F23">
+        <v>1.08508352833644</v>
+      </c>
+      <c r="I23" s="72"/>
+      <c r="L23" s="72"/>
+      <c r="M23" s="93"/>
+      <c r="N23" s="72"/>
+      <c r="O23" s="72">
+        <f t="shared" si="6"/>
+        <v>1.3979181421008846E-4</v>
+      </c>
+      <c r="P23" s="72"/>
+      <c r="Q23" s="72"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="72" t="s">
         <v>215</v>
       </c>
       <c r="B24" s="72">
-        <v>1.0349152577221601</v>
-      </c>
-      <c r="D24" s="72"/>
-      <c r="E24">
+        <v>1.0346562939178801</v>
+      </c>
+      <c r="E24" s="72">
         <v>1.0349154728988099</v>
       </c>
-      <c r="F24" s="72"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F24">
+        <v>1.0349154728988099</v>
+      </c>
+      <c r="I24" s="72"/>
+      <c r="K24">
+        <v>1.03503957660164</v>
+      </c>
+      <c r="L24" s="72">
+        <f t="shared" si="8"/>
+        <v>1.03503957660164</v>
+      </c>
+      <c r="M24" s="93"/>
+      <c r="N24" s="72"/>
+      <c r="O24" s="72">
+        <f t="shared" si="6"/>
+        <v>-2.5917898092986391E-4</v>
+      </c>
+      <c r="P24" s="72"/>
+      <c r="Q24" s="72">
+        <f t="shared" si="3"/>
+        <v>-3.8328268375997787E-4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="72" t="s">
         <v>214</v>
       </c>
       <c r="B25" s="72">
-        <v>1.02798621556374</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1.0276736347300599</v>
+      </c>
+      <c r="H25">
+        <v>1.02797790645934</v>
+      </c>
+      <c r="I25" s="72">
+        <v>1.02797790645934</v>
+      </c>
+      <c r="K25">
+        <v>1.02786440451723</v>
+      </c>
+      <c r="L25" s="72">
+        <f t="shared" si="8"/>
+        <v>1.02786440451723</v>
+      </c>
+      <c r="M25" s="93"/>
+      <c r="N25" s="72"/>
+      <c r="P25" s="72">
+        <f t="shared" si="7"/>
+        <v>-3.0427172928004786E-4</v>
+      </c>
+      <c r="Q25" s="72">
+        <f t="shared" si="3"/>
+        <v>-1.9076978717014192E-4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="72" t="s">
         <v>241</v>
       </c>
       <c r="B26" s="72">
-        <v>1.02970205350408</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1.0294797148790999</v>
+      </c>
+      <c r="H26">
+        <v>1.0296965694578899</v>
+      </c>
+      <c r="I26" s="72">
+        <v>1.0296965694578899</v>
+      </c>
+      <c r="K26">
+        <v>1.02930548527036</v>
+      </c>
+      <c r="L26" s="72">
+        <f t="shared" si="8"/>
+        <v>1.02930548527036</v>
+      </c>
+      <c r="M26" s="93"/>
+      <c r="N26" s="72"/>
+      <c r="P26" s="72">
+        <f t="shared" si="7"/>
+        <v>-2.1685457878994896E-4</v>
+      </c>
+      <c r="Q26" s="72">
+        <f t="shared" si="3"/>
+        <v>1.7422960873991755E-4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="72" t="s">
         <v>212</v>
       </c>
       <c r="B27" s="72">
-        <v>1.0240525230119499</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1.0240118665753799</v>
+      </c>
+      <c r="H27">
+        <v>1.02405678356367</v>
+      </c>
+      <c r="I27" s="72">
+        <v>1.02405678356367</v>
+      </c>
+      <c r="L27" s="72"/>
+      <c r="M27" s="93"/>
+      <c r="N27" s="72"/>
+      <c r="P27" s="72">
+        <f t="shared" si="7"/>
+        <v>-4.4916988290122362E-5</v>
+      </c>
+      <c r="Q27" s="72"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="72" t="s">
         <v>213</v>
       </c>
       <c r="B28" s="72">
-        <v>1.01992383631813</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1.0198403758847501</v>
+      </c>
+      <c r="H28" s="72">
+        <v>1.0199247903486901</v>
+      </c>
+      <c r="I28" s="72">
+        <v>1.0199247903486901</v>
+      </c>
+      <c r="K28">
+        <v>1.0192462123467401</v>
+      </c>
+      <c r="L28" s="72">
+        <f t="shared" si="8"/>
+        <v>1.0192462123467401</v>
+      </c>
+      <c r="M28" s="93"/>
+      <c r="N28" s="72"/>
+      <c r="P28" s="72">
+        <f t="shared" si="7"/>
+        <v>-8.441446394003016E-5</v>
+      </c>
+      <c r="Q28" s="72">
+        <f t="shared" si="3"/>
+        <v>5.9416353801000632E-4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="72" t="s">
         <v>248</v>
       </c>
       <c r="B29" s="72">
-        <v>1.00994172446495</v>
+        <v>1.0096275188231001</v>
+      </c>
+      <c r="H29" s="72">
+        <v>1.00992321157402</v>
+      </c>
+      <c r="I29" s="72">
+        <v>1.00992321157402</v>
+      </c>
+      <c r="K29">
+        <v>1.0094717121613901</v>
+      </c>
+      <c r="L29" s="72">
+        <f t="shared" si="8"/>
+        <v>1.0094717121613901</v>
+      </c>
+      <c r="M29" s="93"/>
+      <c r="N29" s="72"/>
+      <c r="P29" s="72">
+        <f t="shared" si="7"/>
+        <v>-2.9569275091989589E-4</v>
+      </c>
+      <c r="Q29" s="72">
+        <f t="shared" si="3"/>
+        <v>1.5580666171000068E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Started trying to debug 14 bus ADMM.
I think all 4 partitions work now, but I'm not 100% sure. Started trying
to get the 14 bus ADMM to work. Vectorized the way that c1 and c2 mapped
to c, which seems to work. Should find an automatic way to calculate
numPart and also calculate c_k.
</commit_message>
<xml_diff>
--- a/DMASE - Test Results.xlsx
+++ b/DMASE - Test Results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="279">
   <si>
     <t>Abur 3-Bus Case Measurements (run through SE, rerun new estimate again)</t>
   </si>
@@ -858,6 +858,9 @@
   </si>
   <si>
     <t>Q6-5</t>
+  </si>
+  <si>
+    <t>Uses small Ybus for each partition, which is slightly different from using the Ybus for the overall system</t>
   </si>
 </sst>
 </file>
@@ -1105,7 +1108,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1288,6 +1291,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1309,7 +1313,9 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1630,15 +1636,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="87" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="86"/>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
-      <c r="F1" s="86"/>
-      <c r="G1" s="86"/>
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
       <c r="I1" s="6" t="s">
         <v>1</v>
       </c>
@@ -1897,30 +1903,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="90" t="s">
+      <c r="A1" s="91" t="s">
         <v>222</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
-      <c r="D1" s="92"/>
-      <c r="F1" s="90" t="s">
+      <c r="B1" s="92"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="93"/>
+      <c r="F1" s="91" t="s">
         <v>228</v>
       </c>
-      <c r="G1" s="91"/>
-      <c r="H1" s="91"/>
-      <c r="I1" s="92"/>
-      <c r="K1" s="90" t="s">
+      <c r="G1" s="92"/>
+      <c r="H1" s="92"/>
+      <c r="I1" s="93"/>
+      <c r="K1" s="91" t="s">
         <v>229</v>
       </c>
-      <c r="L1" s="91"/>
-      <c r="M1" s="91"/>
-      <c r="N1" s="92"/>
-      <c r="P1" s="90" t="s">
+      <c r="L1" s="92"/>
+      <c r="M1" s="92"/>
+      <c r="N1" s="93"/>
+      <c r="P1" s="91" t="s">
         <v>230</v>
       </c>
-      <c r="Q1" s="91"/>
-      <c r="R1" s="91"/>
-      <c r="S1" s="92"/>
+      <c r="Q1" s="92"/>
+      <c r="R1" s="92"/>
+      <c r="S1" s="93"/>
     </row>
     <row r="2" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="82" t="s">
@@ -2580,7 +2586,7 @@
         <v>16.499999463558101</v>
       </c>
       <c r="M16" s="72">
-        <f t="shared" ref="M16:M26" si="11">L16/100</f>
+        <f t="shared" ref="M16:M22" si="11">L16/100</f>
         <v>0.16499999463558102</v>
       </c>
       <c r="P16" s="72" t="s">
@@ -2923,7 +2929,7 @@
         <v>-42.467163764624999</v>
       </c>
       <c r="M23" s="2">
-        <f>L23/100</f>
+        <f t="shared" ref="M23:M28" si="12">L23/100</f>
         <v>-0.42467163764624999</v>
       </c>
       <c r="N23" s="85" t="s">
@@ -2964,7 +2970,7 @@
         <v>6.4382015347410002</v>
       </c>
       <c r="M24" s="2">
-        <f>L24/100</f>
+        <f t="shared" si="12"/>
         <v>6.4382015347410004E-2</v>
       </c>
       <c r="N24" s="85" t="s">
@@ -2992,7 +2998,7 @@
         <v>2.8808971477310599</v>
       </c>
       <c r="M25" s="2">
-        <f>L25/100</f>
+        <f t="shared" si="12"/>
         <v>2.88089714773106E-2</v>
       </c>
       <c r="N25" s="85" t="s">
@@ -3023,7 +3029,7 @@
         <v>-0.30259003060574602</v>
       </c>
       <c r="M26" s="2">
-        <f>L26/100</f>
+        <f t="shared" si="12"/>
         <v>-3.0259003060574604E-3</v>
       </c>
       <c r="N26" s="85" t="s">
@@ -3039,7 +3045,7 @@
         <v>4.9650161007164098</v>
       </c>
       <c r="M27" s="72">
-        <f>L27/100</f>
+        <f t="shared" si="12"/>
         <v>4.9650161007164101E-2</v>
       </c>
       <c r="N27" s="74" t="s">
@@ -3056,7 +3062,7 @@
         <v>0.52427629116916796</v>
       </c>
       <c r="M28" s="72">
-        <f>L28/100</f>
+        <f t="shared" si="12"/>
         <v>5.2427629116916794E-3</v>
       </c>
       <c r="N28" s="74" t="s">
@@ -3220,10 +3226,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q29"/>
+  <dimension ref="A1:Q63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R29" sqref="R29"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="O45" sqref="O45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3241,895 +3247,1370 @@
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="72"/>
-      <c r="B1" s="72" t="s">
+    <row r="1" spans="1:17" s="72" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="94" t="s">
+        <v>278</v>
+      </c>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
+      <c r="G1" s="94"/>
+      <c r="H1" s="94"/>
+      <c r="I1" s="94"/>
+      <c r="J1" s="94"/>
+      <c r="K1" s="94"/>
+      <c r="L1" s="94"/>
+      <c r="M1" s="94"/>
+      <c r="N1" s="94"/>
+      <c r="O1" s="94"/>
+      <c r="P1" s="94"/>
+      <c r="Q1" s="94"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="72"/>
+      <c r="B2" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="72" t="s">
+      <c r="C2" s="72" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E2" s="34" t="s">
         <v>269</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="F2" s="34" t="s">
         <v>270</v>
       </c>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34" t="s">
+      <c r="G2" s="34"/>
+      <c r="H2" s="34" t="s">
         <v>273</v>
       </c>
-      <c r="I1" s="34" t="s">
+      <c r="I2" s="34" t="s">
         <v>271</v>
       </c>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34" t="s">
+      <c r="J2" s="34"/>
+      <c r="K2" s="34" t="s">
         <v>272</v>
       </c>
-      <c r="L1" s="34" t="s">
+      <c r="L2" s="34" t="s">
         <v>274</v>
       </c>
-      <c r="M1" s="93"/>
-      <c r="N1" t="s">
+      <c r="M2" s="86"/>
+      <c r="N2" t="s">
         <v>10</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O2" t="s">
         <v>11</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P2" t="s">
         <v>44</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="72" t="s">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="72" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="72">
-        <v>0</v>
-      </c>
-      <c r="C2" s="72">
-        <v>0</v>
-      </c>
-      <c r="E2" s="34"/>
-      <c r="M2" s="93"/>
-      <c r="N2">
-        <f>B2-C2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>92</v>
-      </c>
       <c r="B3" s="72">
-        <v>-8.6669791486718703E-2</v>
+        <v>0</v>
       </c>
       <c r="C3" s="72">
-        <v>-8.6708237100475705E-2</v>
-      </c>
-      <c r="E3" s="34">
-        <v>0.13454518661145601</v>
-      </c>
-      <c r="F3" s="72">
-        <f>$B$4+E3</f>
-        <v>-8.6616927051581E-2</v>
-      </c>
-      <c r="M3" s="93"/>
-      <c r="N3" s="72">
-        <f>B3-C3</f>
-        <v>3.8445613757001618E-5</v>
-      </c>
-      <c r="O3">
-        <f>B3-F3</f>
-        <v>-5.2864435137703336E-5</v>
+        <v>0</v>
+      </c>
+      <c r="E3" s="34"/>
+      <c r="M3" s="86"/>
+      <c r="N3" s="2">
+        <f t="shared" ref="N3:N8" si="0">B3-C3</f>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" s="72">
+        <v>-8.6669791486718703E-2</v>
+      </c>
+      <c r="C4" s="72">
+        <v>-8.6708237100475705E-2</v>
+      </c>
+      <c r="E4" s="34">
+        <v>0.13454518661145601</v>
+      </c>
+      <c r="F4" s="72">
+        <f>$B$5+E4</f>
+        <v>-8.6616927051581E-2</v>
+      </c>
+      <c r="M4" s="86"/>
+      <c r="N4" s="2">
+        <f t="shared" si="0"/>
+        <v>3.8445613757001618E-5</v>
+      </c>
+      <c r="O4">
+        <f>B4-F4</f>
+        <v>-5.2864435137703336E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>93</v>
       </c>
-      <c r="B4" s="72">
+      <c r="B5" s="72">
         <v>-0.22116211366303701</v>
       </c>
-      <c r="C4" s="72">
+      <c r="C5" s="72">
         <v>-0.22124896604786901</v>
       </c>
-      <c r="E4" s="34">
-        <v>0</v>
-      </c>
-      <c r="F4" s="72">
-        <f t="shared" ref="F4:F10" si="0">$B$4+E4</f>
+      <c r="E5" s="34">
+        <v>0</v>
+      </c>
+      <c r="F5" s="72">
+        <f t="shared" ref="F5:F11" si="1">$B$5+E5</f>
         <v>-0.22116211366303701</v>
       </c>
-      <c r="H4" s="72"/>
-      <c r="M4" s="93"/>
-      <c r="N4" s="72">
-        <f>B4-C4</f>
+      <c r="H5" s="72"/>
+      <c r="M5" s="86"/>
+      <c r="N5" s="72">
+        <f t="shared" si="0"/>
         <v>8.6852384831997975E-5</v>
       </c>
-      <c r="O4" s="72">
-        <f t="shared" ref="O4:O10" si="1">B4-F4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="72" t="s">
-        <v>259</v>
-      </c>
-      <c r="B5" s="72">
-        <v>-0.18108637306068801</v>
-      </c>
-      <c r="C5" s="72">
-        <v>-0.18120036659231001</v>
-      </c>
-      <c r="E5" s="34">
-        <v>4.0048858036497499E-2</v>
-      </c>
-      <c r="F5" s="72">
-        <f t="shared" si="0"/>
-        <v>-0.18111325562653952</v>
-      </c>
-      <c r="H5" s="72"/>
-      <c r="K5">
-        <v>8.4777565687419704E-2</v>
-      </c>
-      <c r="L5">
-        <f>$B$10+K5</f>
-        <v>-0.18304977592106428</v>
-      </c>
-      <c r="M5" s="93"/>
-      <c r="N5" s="72">
-        <f>B5-C5</f>
-        <v>1.139935316220031E-4</v>
-      </c>
-      <c r="O5" s="72">
-        <f t="shared" si="1"/>
-        <v>2.6882565851510387E-5</v>
-      </c>
-      <c r="Q5">
-        <f>B5-L5</f>
-        <v>1.9634028603762732E-3</v>
+      <c r="O5" s="2">
+        <f t="shared" ref="O5:O11" si="2">B5-F5</f>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="72" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B6" s="72">
-        <v>-0.15459540540712</v>
+        <v>-0.18108637306068801</v>
       </c>
       <c r="C6" s="72">
-        <v>-0.15469627337389699</v>
+        <v>-0.18120036659231001</v>
       </c>
       <c r="E6" s="34">
-        <v>6.6553625884739995E-2</v>
+        <v>4.0048858036497499E-2</v>
       </c>
       <c r="F6" s="72">
+        <f t="shared" si="1"/>
+        <v>-0.18111325562653952</v>
+      </c>
+      <c r="H6" s="72"/>
+      <c r="K6">
+        <v>8.4777565687419704E-2</v>
+      </c>
+      <c r="L6">
+        <f>$B$11+K6</f>
+        <v>-0.18304977592106428</v>
+      </c>
+      <c r="M6" s="86"/>
+      <c r="N6" s="72">
         <f t="shared" si="0"/>
-        <v>-0.154608487778297</v>
-      </c>
-      <c r="H6" s="72">
-        <v>0.10040928822293101</v>
-      </c>
-      <c r="I6" s="72">
-        <f>$B$7+H6</f>
-        <v>-0.15449621523418899</v>
-      </c>
-      <c r="L6" s="72"/>
-      <c r="M6" s="93"/>
-      <c r="N6" s="72">
-        <f>B6-C6</f>
-        <v>1.0086796677699628E-4</v>
-      </c>
-      <c r="O6" s="72">
-        <f t="shared" si="1"/>
-        <v>1.3082371177003393E-5</v>
-      </c>
-      <c r="P6">
-        <f>B6-I6</f>
-        <v>-9.9190172931001852E-5</v>
-      </c>
-      <c r="Q6" s="72"/>
+        <v>1.139935316220031E-4</v>
+      </c>
+      <c r="O6" s="2">
+        <f t="shared" si="2"/>
+        <v>2.6882565851510387E-5</v>
+      </c>
+      <c r="Q6">
+        <f>B6-L6</f>
+        <v>1.9634028603762732E-3</v>
+      </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="72" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B7" s="72">
-        <v>-0.25490550345711999</v>
+        <v>-0.15459540540712</v>
       </c>
       <c r="C7" s="72">
-        <v>-0.255101990043542</v>
-      </c>
-      <c r="F7" s="72"/>
+        <v>-0.15469627337389699</v>
+      </c>
+      <c r="E7" s="34">
+        <v>6.6553625884739995E-2</v>
+      </c>
+      <c r="F7" s="72">
+        <f t="shared" si="1"/>
+        <v>-0.154608487778297</v>
+      </c>
       <c r="H7" s="72">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <f>$B$7+H7</f>
-        <v>-0.25490550345711999</v>
+        <v>0.10040928822293101</v>
+      </c>
+      <c r="I7" s="72">
+        <f>$B$8+H7</f>
+        <v>-0.15449621523418899</v>
       </c>
       <c r="L7" s="72"/>
-      <c r="M7" s="93"/>
-      <c r="N7" s="72">
-        <f>B7-C7</f>
-        <v>1.9648658642201777E-4</v>
-      </c>
-      <c r="O7" s="72"/>
-      <c r="P7" s="72">
+      <c r="M7" s="86"/>
+      <c r="N7" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0086796677699628E-4</v>
+      </c>
+      <c r="O7" s="72">
+        <f t="shared" si="2"/>
+        <v>1.3082371177003393E-5</v>
+      </c>
+      <c r="P7">
         <f>B7-I7</f>
-        <v>0</v>
+        <v>-9.9190172931001852E-5</v>
       </c>
       <c r="Q7" s="72"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="72" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B8" s="72">
-        <v>-0.238124828874305</v>
-      </c>
-      <c r="C8" s="72"/>
-      <c r="E8" s="72">
-        <v>-1.7094294986265499E-2</v>
-      </c>
-      <c r="F8" s="72">
+        <v>-0.25490550345711999</v>
+      </c>
+      <c r="C8" s="72">
+        <v>-0.255101990043542</v>
+      </c>
+      <c r="F8" s="72"/>
+      <c r="H8" s="72">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <f>$B$8+H8</f>
+        <v>-0.25490550345711999</v>
+      </c>
+      <c r="L8" s="72"/>
+      <c r="M8" s="86"/>
+      <c r="N8" s="72">
         <f t="shared" si="0"/>
-        <v>-0.2382564086493025</v>
-      </c>
-      <c r="I8" s="72"/>
-      <c r="K8">
-        <v>2.9803356989265999E-2</v>
-      </c>
-      <c r="L8" s="72">
-        <f t="shared" ref="L6:L15" si="2">$B$10+K8</f>
-        <v>-0.23802398461921798</v>
-      </c>
-      <c r="M8" s="93"/>
-      <c r="N8" s="72"/>
-      <c r="O8" s="72">
-        <f t="shared" si="1"/>
-        <v>1.315797749975034E-4</v>
-      </c>
-      <c r="Q8" s="72">
-        <f t="shared" ref="Q6:Q29" si="3">B8-L8</f>
-        <v>-1.0084425508702366E-4</v>
-      </c>
+        <v>1.9648658642201777E-4</v>
+      </c>
+      <c r="O8" s="72"/>
+      <c r="P8" s="2">
+        <f>B8-I8</f>
+        <v>0</v>
+      </c>
+      <c r="Q8" s="72"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="72" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B9" s="72">
-        <v>-0.23811416408082101</v>
-      </c>
+        <v>-0.238124828874305</v>
+      </c>
+      <c r="C9" s="72"/>
       <c r="E9" s="72">
-        <v>-1.7094298065348599E-2</v>
+        <v>-1.7094294986265499E-2</v>
       </c>
       <c r="F9" s="72">
-        <f t="shared" si="0"/>
-        <v>-0.2382564117283856</v>
+        <f t="shared" si="1"/>
+        <v>-0.2382564086493025</v>
       </c>
       <c r="I9" s="72"/>
-      <c r="L9" s="72"/>
-      <c r="M9" s="93"/>
+      <c r="K9">
+        <v>2.9803356989265999E-2</v>
+      </c>
+      <c r="L9" s="72">
+        <f>$B$11+K9</f>
+        <v>-0.23802398461921798</v>
+      </c>
+      <c r="M9" s="86"/>
       <c r="N9" s="72"/>
-      <c r="O9" s="72">
-        <f t="shared" si="1"/>
-        <v>1.4224764756459729E-4</v>
-      </c>
-      <c r="Q9" s="72"/>
+      <c r="O9" s="2">
+        <f t="shared" si="2"/>
+        <v>1.315797749975034E-4</v>
+      </c>
+      <c r="Q9" s="72">
+        <f t="shared" ref="Q9:Q30" si="3">B9-L9</f>
+        <v>-1.0084425508702366E-4</v>
+      </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="72" t="s">
-        <v>71</v>
+        <v>263</v>
       </c>
       <c r="B10" s="72">
-        <v>-0.26782734160848398</v>
-      </c>
-      <c r="E10" s="34">
-        <v>-4.6817626498101603E-2</v>
+        <v>-0.23811416408082101</v>
+      </c>
+      <c r="E10" s="72">
+        <v>-1.7094298065348599E-2</v>
       </c>
       <c r="F10" s="72">
-        <f t="shared" si="0"/>
-        <v>-0.26797974016113862</v>
+        <f t="shared" si="1"/>
+        <v>-0.2382564117283856</v>
       </c>
       <c r="I10" s="72"/>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10" s="72">
+      <c r="L10" s="72"/>
+      <c r="M10" s="86"/>
+      <c r="N10" s="72"/>
+      <c r="O10" s="2">
         <f t="shared" si="2"/>
-        <v>-0.26782734160848398</v>
-      </c>
-      <c r="M10" s="93"/>
-      <c r="N10" s="72"/>
-      <c r="O10" s="72">
-        <f t="shared" si="1"/>
-        <v>1.5239855265464231E-4</v>
-      </c>
-      <c r="Q10" s="72">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
+        <v>1.4224764756459729E-4</v>
+      </c>
+      <c r="Q10" s="72"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="72" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11" s="72">
+        <v>-0.26782734160848398</v>
+      </c>
+      <c r="E11" s="34">
+        <v>-4.6817626498101603E-2</v>
+      </c>
+      <c r="F11" s="72">
+        <f t="shared" si="1"/>
+        <v>-0.26797974016113862</v>
+      </c>
+      <c r="I11" s="72"/>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11" s="72">
+        <f>$B$11+K11</f>
+        <v>-0.26782734160848398</v>
+      </c>
+      <c r="M11" s="86"/>
+      <c r="N11" s="72"/>
+      <c r="O11" s="72">
+        <f t="shared" si="2"/>
+        <v>1.5239855265464231E-4</v>
+      </c>
+      <c r="Q11" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="72" t="s">
         <v>264</v>
       </c>
-      <c r="B11" s="72">
+      <c r="B12" s="72">
         <v>-0.27082639634655098</v>
       </c>
-      <c r="E11" s="34"/>
-      <c r="H11">
+      <c r="E12" s="34"/>
+      <c r="H12">
         <v>-1.59962164357162E-2</v>
       </c>
-      <c r="I11" s="72">
-        <f t="shared" ref="I11:I15" si="4">$B$7+H11</f>
+      <c r="I12" s="72">
+        <f t="shared" ref="I12:I16" si="4">$B$8+H12</f>
         <v>-0.27090171989283618</v>
       </c>
-      <c r="K11">
+      <c r="K12">
         <v>-2.8854192291146198E-3</v>
       </c>
-      <c r="L11" s="72">
-        <f t="shared" si="2"/>
+      <c r="L12" s="72">
+        <f>$B$11+K12</f>
         <v>-0.2707127608375986</v>
       </c>
-      <c r="M11" s="93"/>
-      <c r="N11" s="72"/>
-      <c r="P11">
-        <f>B11-I11</f>
+      <c r="M12" s="86"/>
+      <c r="N12" s="72"/>
+      <c r="P12">
+        <f>B12-I12</f>
         <v>7.5323546285199772E-5</v>
       </c>
-      <c r="Q11" s="72">
+      <c r="Q12" s="2">
         <f t="shared" si="3"/>
         <v>-1.1363550895238106E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="72" t="s">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="72" t="s">
         <v>265</v>
       </c>
-      <c r="B12" s="72">
+      <c r="B13" s="72">
         <v>-0.26537530725671299</v>
       </c>
-      <c r="E12" s="34"/>
-      <c r="H12">
+      <c r="E13" s="34"/>
+      <c r="H13">
         <v>-1.05354439253986E-2</v>
       </c>
-      <c r="I12" s="72">
+      <c r="I13" s="72">
         <f t="shared" si="4"/>
         <v>-0.26544094738251861</v>
       </c>
-      <c r="K12">
+      <c r="K13">
         <v>2.76657675401411E-3</v>
       </c>
-      <c r="L12" s="72">
-        <f t="shared" si="2"/>
+      <c r="L13" s="72">
+        <f>$B$11+K13</f>
         <v>-0.26506076485446989</v>
       </c>
-      <c r="M12" s="93"/>
-      <c r="N12" s="72"/>
-      <c r="P12" s="72">
-        <f t="shared" ref="P12:P15" si="5">B12-I12</f>
+      <c r="M13" s="86"/>
+      <c r="N13" s="72"/>
+      <c r="P13" s="2">
+        <f t="shared" ref="P13:P16" si="5">B13-I13</f>
         <v>6.5640125805621619E-5</v>
       </c>
-      <c r="Q12" s="72">
+      <c r="Q13" s="72">
         <f t="shared" si="3"/>
         <v>-3.1454240224310093E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="72" t="s">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="72" t="s">
         <v>266</v>
       </c>
-      <c r="B13" s="72">
+      <c r="B14" s="72">
         <v>-0.27056740976696902</v>
       </c>
-      <c r="E13" s="34"/>
-      <c r="H13">
+      <c r="E14" s="34"/>
+      <c r="H14">
         <v>-1.5681481070227099E-2</v>
       </c>
-      <c r="I13" s="72">
+      <c r="I14" s="72">
         <f t="shared" si="4"/>
         <v>-0.27058698452734709</v>
       </c>
-      <c r="L13" s="72"/>
-      <c r="M13" s="93"/>
-      <c r="N13" s="72"/>
-      <c r="P13" s="72">
+      <c r="L14" s="72"/>
+      <c r="M14" s="86"/>
+      <c r="N14" s="72"/>
+      <c r="P14" s="2">
         <f t="shared" si="5"/>
         <v>1.9574760378060496E-5</v>
       </c>
-      <c r="Q13" s="72"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="72" t="s">
+      <c r="Q14" s="72"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="72" t="s">
         <v>267</v>
       </c>
-      <c r="B14" s="72">
+      <c r="B15" s="72">
         <v>-0.272193451087546</v>
       </c>
-      <c r="E14" s="34"/>
-      <c r="H14" s="72">
+      <c r="E15" s="34"/>
+      <c r="H15" s="72">
         <v>-1.73222072322563E-2</v>
       </c>
-      <c r="I14" s="72">
+      <c r="I15" s="72">
         <f t="shared" si="4"/>
         <v>-0.27222771068937629</v>
       </c>
-      <c r="K14">
+      <c r="K15">
         <v>-3.4089835958288602E-3</v>
       </c>
-      <c r="L14" s="72">
-        <f t="shared" si="2"/>
+      <c r="L15" s="72">
+        <f>$B$11+K15</f>
         <v>-0.27123632520431284</v>
       </c>
-      <c r="M14" s="93"/>
-      <c r="N14" s="72"/>
-      <c r="P14" s="72">
+      <c r="M15" s="86"/>
+      <c r="N15" s="72"/>
+      <c r="P15" s="2">
         <f t="shared" si="5"/>
         <v>3.4259601830288755E-5</v>
       </c>
-      <c r="Q14" s="72">
+      <c r="Q15" s="72">
         <f t="shared" si="3"/>
         <v>-9.5712588323315639E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="72" t="s">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="72" t="s">
         <v>268</v>
       </c>
-      <c r="B15" s="72">
+      <c r="B16" s="72">
         <v>-0.28803193308711</v>
       </c>
-      <c r="E15" s="34"/>
-      <c r="H15" s="72">
+      <c r="E16" s="34"/>
+      <c r="H16" s="72">
         <v>-3.32188944082469E-2</v>
       </c>
-      <c r="I15" s="72">
+      <c r="I16" s="72">
         <f t="shared" si="4"/>
         <v>-0.28812439786536687</v>
       </c>
-      <c r="K15">
+      <c r="K16">
         <v>-1.9713877950687402E-2</v>
       </c>
-      <c r="L15" s="72">
-        <f t="shared" si="2"/>
+      <c r="L16" s="72">
+        <f>$B$11+K16</f>
         <v>-0.28754121955917139</v>
       </c>
-      <c r="M15" s="93"/>
-      <c r="N15" s="72"/>
-      <c r="P15" s="72">
+      <c r="M16" s="86"/>
+      <c r="N16" s="72"/>
+      <c r="P16" s="72">
         <f t="shared" si="5"/>
         <v>9.2464778256862168E-5</v>
       </c>
-      <c r="Q15" s="72">
+      <c r="Q16" s="2">
         <f t="shared" si="3"/>
         <v>-4.9071352793861323E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="72">
+      <c r="B17" s="72">
         <v>1.06021182972759</v>
       </c>
-      <c r="C16" s="72">
+      <c r="C17" s="72">
         <v>1.05999978718632</v>
       </c>
-      <c r="E16" s="34"/>
-      <c r="H16" s="72"/>
-      <c r="M16" s="93"/>
-      <c r="N16" s="72">
-        <f>B16-C16</f>
+      <c r="E17" s="34"/>
+      <c r="H17" s="72"/>
+      <c r="M17" s="86"/>
+      <c r="N17" s="2">
+        <f t="shared" ref="N17:N22" si="6">B17-C17</f>
         <v>2.1204254126994115E-4</v>
-      </c>
-      <c r="Q16" s="72"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="72" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="72">
-        <v>1.04521069537303</v>
-      </c>
-      <c r="C17" s="72">
-        <v>1.04499963862116</v>
-      </c>
-      <c r="E17" s="72">
-        <v>1.04499906313014</v>
-      </c>
-      <c r="F17">
-        <v>1.04499906313014</v>
-      </c>
-      <c r="H17" s="72"/>
-      <c r="M17" s="93"/>
-      <c r="N17" s="72">
-        <f>B17-C17</f>
-        <v>2.1105675187005346E-4</v>
-      </c>
-      <c r="O17">
-        <f>B17-F17</f>
-        <v>2.1163224289000304E-4</v>
       </c>
       <c r="Q17" s="72"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="72" t="s">
-        <v>94</v>
+        <v>28</v>
       </c>
       <c r="B18" s="72">
-        <v>1.0102223344885899</v>
+        <v>1.04521069537303</v>
       </c>
       <c r="C18" s="72">
-        <v>1.0100010595292099</v>
+        <v>1.04499963862116</v>
       </c>
       <c r="E18" s="72">
-        <v>1.0099998991758801</v>
+        <v>1.04499906313014</v>
       </c>
       <c r="F18">
-        <v>1.0099998991758801</v>
+        <v>1.04499906313014</v>
       </c>
       <c r="H18" s="72"/>
-      <c r="M18" s="93"/>
-      <c r="N18" s="72">
-        <f>B18-C18</f>
-        <v>2.2127495937995789E-4</v>
-      </c>
-      <c r="O18" s="72">
-        <f t="shared" ref="O18:O24" si="6">B18-F18</f>
-        <v>2.2243531270982331E-4</v>
+      <c r="M18" s="86"/>
+      <c r="N18" s="2">
+        <f t="shared" si="6"/>
+        <v>2.1105675187005346E-4</v>
+      </c>
+      <c r="O18">
+        <f>B18-F18</f>
+        <v>2.1163224289000304E-4</v>
       </c>
       <c r="Q18" s="72"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="72" t="s">
+        <v>94</v>
+      </c>
+      <c r="B19" s="72">
+        <v>1.0102223344885899</v>
+      </c>
+      <c r="C19" s="72">
+        <v>1.0100010595292099</v>
+      </c>
+      <c r="E19" s="72">
+        <v>1.0099998991758801</v>
+      </c>
+      <c r="F19">
+        <v>1.0099998991758801</v>
+      </c>
+      <c r="H19" s="72"/>
+      <c r="M19" s="86"/>
+      <c r="N19" s="72">
+        <f t="shared" si="6"/>
+        <v>2.2127495937995789E-4</v>
+      </c>
+      <c r="O19" s="2">
+        <f t="shared" ref="O19:O25" si="7">B19-F19</f>
+        <v>2.2243531270982331E-4</v>
+      </c>
+      <c r="Q19" s="72"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" s="72" t="s">
         <v>231</v>
       </c>
-      <c r="B19" s="72">
+      <c r="B20" s="72">
         <v>1.0238916772678499</v>
       </c>
-      <c r="C19" s="72">
+      <c r="C20" s="72">
         <v>1.0237139016294901</v>
       </c>
-      <c r="E19" s="72">
+      <c r="E20" s="72">
         <v>1.0237127697133499</v>
       </c>
-      <c r="F19">
+      <c r="F20">
         <v>1.0237127697133499</v>
       </c>
-      <c r="H19" s="72"/>
-      <c r="K19">
+      <c r="H20" s="72"/>
+      <c r="K20">
         <v>1.0267750886447</v>
       </c>
-      <c r="L19">
-        <f>K19</f>
+      <c r="L20">
+        <f>K20</f>
         <v>1.0267750886447</v>
       </c>
-      <c r="M19" s="93"/>
-      <c r="N19" s="72">
-        <f>B19-C19</f>
+      <c r="M20" s="86"/>
+      <c r="N20" s="72">
+        <f t="shared" si="6"/>
         <v>1.777756383598561E-4</v>
       </c>
-      <c r="O19" s="72">
-        <f t="shared" si="6"/>
+      <c r="O20" s="2">
+        <f t="shared" si="7"/>
         <v>1.7890755450000739E-4</v>
       </c>
-      <c r="Q19" s="72">
+      <c r="Q20" s="72">
         <f t="shared" si="3"/>
         <v>-2.8834113768501091E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="72" t="s">
-        <v>210</v>
-      </c>
-      <c r="B20" s="72">
-        <v>1.02827099057284</v>
-      </c>
-      <c r="C20" s="72">
-        <v>1.0280934274068501</v>
-      </c>
-      <c r="E20" s="72">
-        <v>1.0280924472289901</v>
-      </c>
-      <c r="F20">
-        <v>1.0280924472289901</v>
-      </c>
-      <c r="H20" s="72">
-        <v>1.0280804768676</v>
-      </c>
-      <c r="I20" s="72">
-        <v>1.0280804768676</v>
-      </c>
-      <c r="L20" s="72"/>
-      <c r="M20" s="93"/>
-      <c r="N20" s="72">
-        <f>B20-C20</f>
-        <v>1.7756316598993571E-4</v>
-      </c>
-      <c r="O20" s="72">
-        <f t="shared" si="6"/>
-        <v>1.7854334384992399E-4</v>
-      </c>
-      <c r="P20">
-        <f>B20-I20</f>
-        <v>1.905137052400363E-4</v>
-      </c>
-      <c r="Q20" s="72"/>
-    </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="72" t="s">
-        <v>240</v>
+        <v>210</v>
       </c>
       <c r="B21" s="72">
-        <v>1.0384892284060301</v>
+        <v>1.02827099057284</v>
       </c>
       <c r="C21" s="72">
-        <v>1.03853856918465</v>
-      </c>
-      <c r="E21" s="72"/>
+        <v>1.0280934274068501</v>
+      </c>
+      <c r="E21" s="72">
+        <v>1.0280924472289901</v>
+      </c>
+      <c r="F21">
+        <v>1.0280924472289901</v>
+      </c>
       <c r="H21" s="72">
-        <v>1.03853803524227</v>
+        <v>1.0280804768676</v>
       </c>
       <c r="I21" s="72">
-        <v>1.03853803524227</v>
+        <v>1.0280804768676</v>
       </c>
       <c r="L21" s="72"/>
-      <c r="M21" s="93"/>
-      <c r="N21" s="72">
-        <f>B21-C21</f>
-        <v>-4.9340778619955117E-5</v>
-      </c>
-      <c r="O21" s="72"/>
-      <c r="P21" s="72">
-        <f t="shared" ref="P21:P29" si="7">B21-I21</f>
-        <v>-4.8806836239867479E-5</v>
+      <c r="M21" s="86"/>
+      <c r="N21" s="2">
+        <f t="shared" si="6"/>
+        <v>1.7756316598993571E-4</v>
+      </c>
+      <c r="O21" s="72">
+        <f t="shared" si="7"/>
+        <v>1.7854334384992399E-4</v>
+      </c>
+      <c r="P21">
+        <f>B21-I21</f>
+        <v>1.905137052400363E-4</v>
       </c>
       <c r="Q21" s="72"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="72" t="s">
+        <v>240</v>
+      </c>
+      <c r="B22" s="72">
+        <v>1.0384892284060301</v>
+      </c>
+      <c r="C22" s="72">
+        <v>1.03853856918465</v>
+      </c>
+      <c r="E22" s="72"/>
+      <c r="H22" s="72">
+        <v>1.03853803524227</v>
+      </c>
+      <c r="I22" s="72">
+        <v>1.03853803524227</v>
+      </c>
+      <c r="L22" s="72"/>
+      <c r="M22" s="86"/>
+      <c r="N22" s="72">
+        <f t="shared" si="6"/>
+        <v>-4.9340778619955117E-5</v>
+      </c>
+      <c r="O22" s="72"/>
+      <c r="P22" s="2">
+        <f t="shared" ref="P22:P30" si="8">B22-I22</f>
+        <v>-4.8806836239867479E-5</v>
+      </c>
+      <c r="Q22" s="72"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" s="72" t="s">
         <v>232</v>
       </c>
-      <c r="B22" s="72">
+      <c r="B23" s="72">
         <v>1.0461591070376699</v>
       </c>
-      <c r="E22" s="72">
+      <c r="E23" s="72">
         <v>1.04612261065483</v>
       </c>
-      <c r="F22">
+      <c r="F23">
         <v>1.04612261065483</v>
       </c>
-      <c r="I22" s="72"/>
-      <c r="K22">
+      <c r="I23" s="72"/>
+      <c r="K23">
         <v>1.04677077937396</v>
       </c>
-      <c r="L22" s="72">
-        <f t="shared" ref="L20:L29" si="8">K22</f>
+      <c r="L23" s="72">
+        <f t="shared" ref="L23:L30" si="9">K23</f>
         <v>1.04677077937396</v>
       </c>
-      <c r="M22" s="93"/>
-      <c r="N22" s="72"/>
-      <c r="O22" s="72">
-        <f t="shared" si="6"/>
+      <c r="M23" s="86"/>
+      <c r="N23" s="72"/>
+      <c r="O23" s="2">
+        <f t="shared" si="7"/>
         <v>3.6496382839867891E-5</v>
       </c>
-      <c r="P22" s="72"/>
-      <c r="Q22" s="72">
+      <c r="P23" s="72"/>
+      <c r="Q23" s="72">
         <f t="shared" si="3"/>
         <v>-6.1167233629011442E-4</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" s="72" t="s">
-        <v>211</v>
-      </c>
-      <c r="B23" s="72">
-        <v>1.08522332015065</v>
-      </c>
-      <c r="E23" s="72">
-        <v>1.08508352833644</v>
-      </c>
-      <c r="F23">
-        <v>1.08508352833644</v>
-      </c>
-      <c r="I23" s="72"/>
-      <c r="L23" s="72"/>
-      <c r="M23" s="93"/>
-      <c r="N23" s="72"/>
-      <c r="O23" s="72">
-        <f t="shared" si="6"/>
-        <v>1.3979181421008846E-4</v>
-      </c>
-      <c r="P23" s="72"/>
-      <c r="Q23" s="72"/>
-    </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="72" t="s">
+        <v>211</v>
+      </c>
+      <c r="B24" s="72">
+        <v>1.08522332015065</v>
+      </c>
+      <c r="E24" s="72">
+        <v>1.08508352833644</v>
+      </c>
+      <c r="F24">
+        <v>1.08508352833644</v>
+      </c>
+      <c r="I24" s="72"/>
+      <c r="L24" s="72"/>
+      <c r="M24" s="86"/>
+      <c r="N24" s="72"/>
+      <c r="O24" s="2">
+        <f t="shared" si="7"/>
+        <v>1.3979181421008846E-4</v>
+      </c>
+      <c r="P24" s="72"/>
+      <c r="Q24" s="72"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" s="72" t="s">
         <v>215</v>
       </c>
-      <c r="B24" s="72">
+      <c r="B25" s="72">
         <v>1.0346562939178801</v>
       </c>
-      <c r="E24" s="72">
+      <c r="E25" s="72">
         <v>1.0349154728988099</v>
       </c>
-      <c r="F24">
+      <c r="F25">
         <v>1.0349154728988099</v>
       </c>
-      <c r="I24" s="72"/>
-      <c r="K24">
+      <c r="I25" s="72"/>
+      <c r="K25">
         <v>1.03503957660164</v>
       </c>
-      <c r="L24" s="72">
-        <f t="shared" si="8"/>
+      <c r="L25" s="72">
+        <f t="shared" si="9"/>
         <v>1.03503957660164</v>
       </c>
-      <c r="M24" s="93"/>
-      <c r="N24" s="72"/>
-      <c r="O24" s="72">
-        <f t="shared" si="6"/>
+      <c r="M25" s="86"/>
+      <c r="N25" s="72"/>
+      <c r="O25" s="72">
+        <f t="shared" si="7"/>
         <v>-2.5917898092986391E-4</v>
       </c>
-      <c r="P24" s="72"/>
-      <c r="Q24" s="72">
+      <c r="P25" s="72"/>
+      <c r="Q25" s="2">
         <f t="shared" si="3"/>
         <v>-3.8328268375997787E-4</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" s="72" t="s">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26" s="72" t="s">
         <v>214</v>
       </c>
-      <c r="B25" s="72">
+      <c r="B26" s="72">
         <v>1.0276736347300599</v>
       </c>
-      <c r="H25">
+      <c r="H26">
         <v>1.02797790645934</v>
       </c>
-      <c r="I25" s="72">
+      <c r="I26" s="72">
         <v>1.02797790645934</v>
       </c>
-      <c r="K25">
+      <c r="K26">
         <v>1.02786440451723</v>
       </c>
-      <c r="L25" s="72">
+      <c r="L26" s="72">
+        <f t="shared" si="9"/>
+        <v>1.02786440451723</v>
+      </c>
+      <c r="M26" s="86"/>
+      <c r="N26" s="72"/>
+      <c r="P26" s="72">
         <f t="shared" si="8"/>
-        <v>1.02786440451723</v>
-      </c>
-      <c r="M25" s="93"/>
-      <c r="N25" s="72"/>
-      <c r="P25" s="72">
-        <f t="shared" si="7"/>
         <v>-3.0427172928004786E-4</v>
       </c>
-      <c r="Q25" s="72">
+      <c r="Q26" s="2">
         <f t="shared" si="3"/>
         <v>-1.9076978717014192E-4</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" s="72" t="s">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A27" s="72" t="s">
         <v>241</v>
       </c>
-      <c r="B26" s="72">
+      <c r="B27" s="72">
         <v>1.0294797148790999</v>
       </c>
-      <c r="H26">
+      <c r="H27">
         <v>1.0296965694578899</v>
       </c>
-      <c r="I26" s="72">
+      <c r="I27" s="72">
         <v>1.0296965694578899</v>
       </c>
-      <c r="K26">
+      <c r="K27">
         <v>1.02930548527036</v>
       </c>
-      <c r="L26" s="72">
+      <c r="L27" s="72">
+        <f t="shared" si="9"/>
+        <v>1.02930548527036</v>
+      </c>
+      <c r="M27" s="86"/>
+      <c r="N27" s="72"/>
+      <c r="P27" s="2">
         <f t="shared" si="8"/>
-        <v>1.02930548527036</v>
-      </c>
-      <c r="M26" s="93"/>
-      <c r="N26" s="72"/>
-      <c r="P26" s="72">
-        <f t="shared" si="7"/>
         <v>-2.1685457878994896E-4</v>
       </c>
-      <c r="Q26" s="72">
+      <c r="Q27" s="72">
         <f t="shared" si="3"/>
         <v>1.7422960873991755E-4</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A27" s="72" t="s">
-        <v>212</v>
-      </c>
-      <c r="B27" s="72">
-        <v>1.0240118665753799</v>
-      </c>
-      <c r="H27">
-        <v>1.02405678356367</v>
-      </c>
-      <c r="I27" s="72">
-        <v>1.02405678356367</v>
-      </c>
-      <c r="L27" s="72"/>
-      <c r="M27" s="93"/>
-      <c r="N27" s="72"/>
-      <c r="P27" s="72">
-        <f t="shared" si="7"/>
-        <v>-4.4916988290122362E-5</v>
-      </c>
-      <c r="Q27" s="72"/>
-    </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="72" t="s">
+        <v>212</v>
+      </c>
+      <c r="B28" s="72">
+        <v>1.0240118665753799</v>
+      </c>
+      <c r="H28">
+        <v>1.02405678356367</v>
+      </c>
+      <c r="I28" s="72">
+        <v>1.02405678356367</v>
+      </c>
+      <c r="L28" s="72"/>
+      <c r="M28" s="86"/>
+      <c r="N28" s="72"/>
+      <c r="P28" s="2">
+        <f t="shared" si="8"/>
+        <v>-4.4916988290122362E-5</v>
+      </c>
+      <c r="Q28" s="72"/>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A29" s="72" t="s">
         <v>213</v>
       </c>
-      <c r="B28" s="72">
+      <c r="B29" s="72">
         <v>1.0198403758847501</v>
       </c>
-      <c r="H28" s="72">
+      <c r="H29" s="72">
         <v>1.0199247903486901</v>
       </c>
-      <c r="I28" s="72">
+      <c r="I29" s="72">
         <v>1.0199247903486901</v>
       </c>
-      <c r="K28">
+      <c r="K29">
         <v>1.0192462123467401</v>
       </c>
-      <c r="L28" s="72">
+      <c r="L29" s="72">
+        <f t="shared" si="9"/>
+        <v>1.0192462123467401</v>
+      </c>
+      <c r="M29" s="86"/>
+      <c r="N29" s="72"/>
+      <c r="P29" s="2">
         <f t="shared" si="8"/>
-        <v>1.0192462123467401</v>
-      </c>
-      <c r="M28" s="93"/>
-      <c r="N28" s="72"/>
-      <c r="P28" s="72">
-        <f t="shared" si="7"/>
         <v>-8.441446394003016E-5</v>
       </c>
-      <c r="Q28" s="72">
+      <c r="Q29" s="72">
         <f t="shared" si="3"/>
         <v>5.9416353801000632E-4</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A29" s="72" t="s">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30" s="72" t="s">
         <v>248</v>
       </c>
-      <c r="B29" s="72">
+      <c r="B30" s="72">
         <v>1.0096275188231001</v>
       </c>
-      <c r="H29" s="72">
+      <c r="H30" s="72">
         <v>1.00992321157402</v>
       </c>
-      <c r="I29" s="72">
+      <c r="I30" s="72">
         <v>1.00992321157402</v>
       </c>
-      <c r="K29">
+      <c r="K30">
         <v>1.0094717121613901</v>
       </c>
-      <c r="L29" s="72">
+      <c r="L30" s="72">
+        <f t="shared" si="9"/>
+        <v>1.0094717121613901</v>
+      </c>
+      <c r="M30" s="86"/>
+      <c r="N30" s="72"/>
+      <c r="P30" s="72">
         <f t="shared" si="8"/>
-        <v>1.0094717121613901</v>
-      </c>
-      <c r="M29" s="93"/>
-      <c r="N29" s="72"/>
-      <c r="P29" s="72">
-        <f t="shared" si="7"/>
         <v>-2.9569275091989589E-4</v>
       </c>
-      <c r="Q29" s="72">
+      <c r="Q30" s="2">
         <f t="shared" si="3"/>
         <v>1.5580666171000068E-4</v>
       </c>
     </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A35" s="72"/>
+      <c r="B35" s="72" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" s="72" t="s">
+        <v>13</v>
+      </c>
+      <c r="E35" s="34" t="s">
+        <v>269</v>
+      </c>
+      <c r="F35" s="34" t="s">
+        <v>270</v>
+      </c>
+      <c r="G35" s="34"/>
+      <c r="H35" s="34" t="s">
+        <v>273</v>
+      </c>
+      <c r="I35" s="34" t="s">
+        <v>271</v>
+      </c>
+      <c r="J35" s="34"/>
+      <c r="K35" s="34" t="s">
+        <v>272</v>
+      </c>
+      <c r="L35" s="34" t="s">
+        <v>274</v>
+      </c>
+      <c r="M35" s="86"/>
+      <c r="N35" s="72" t="s">
+        <v>10</v>
+      </c>
+      <c r="O35" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="P35" s="72" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q35" s="72" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A36" s="72" t="s">
+        <v>91</v>
+      </c>
+      <c r="B36" s="72">
+        <v>0</v>
+      </c>
+      <c r="M36" s="86"/>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A37" s="72" t="s">
+        <v>92</v>
+      </c>
+      <c r="B37" s="72">
+        <v>-8.6669791486718703E-2</v>
+      </c>
+      <c r="E37" s="72">
+        <v>0.13454518661145601</v>
+      </c>
+      <c r="F37">
+        <f>$B$38+E37</f>
+        <v>-8.6616927051581E-2</v>
+      </c>
+      <c r="M37" s="86"/>
+      <c r="O37">
+        <f>B37-F37</f>
+        <v>-5.2864435137703336E-5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A38" s="72" t="s">
+        <v>93</v>
+      </c>
+      <c r="B38" s="72">
+        <v>-0.22116211366303701</v>
+      </c>
+      <c r="E38" s="72">
+        <v>0</v>
+      </c>
+      <c r="F38" s="72">
+        <f t="shared" ref="F38:F44" si="10">$B$38+E38</f>
+        <v>-0.22116211366303701</v>
+      </c>
+      <c r="M38" s="86"/>
+      <c r="O38" s="72">
+        <f t="shared" ref="O38:O58" si="11">B38-F38</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A39" s="72" t="s">
+        <v>259</v>
+      </c>
+      <c r="B39" s="72">
+        <v>-0.18108637306068801</v>
+      </c>
+      <c r="E39" s="72">
+        <v>4.0048858036497499E-2</v>
+      </c>
+      <c r="F39" s="72">
+        <f t="shared" si="10"/>
+        <v>-0.18111325562653952</v>
+      </c>
+      <c r="M39" s="86"/>
+      <c r="O39" s="72">
+        <f t="shared" si="11"/>
+        <v>2.6882565851510387E-5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A40" s="72" t="s">
+        <v>260</v>
+      </c>
+      <c r="B40" s="72">
+        <v>-0.15459540540712</v>
+      </c>
+      <c r="E40" s="72">
+        <v>6.6553625884739995E-2</v>
+      </c>
+      <c r="F40" s="72">
+        <f t="shared" si="10"/>
+        <v>-0.154608487778297</v>
+      </c>
+      <c r="M40" s="86"/>
+      <c r="O40" s="72">
+        <f t="shared" si="11"/>
+        <v>1.3082371177003393E-5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A41" s="72" t="s">
+        <v>261</v>
+      </c>
+      <c r="B41" s="72">
+        <v>-0.25490550345711999</v>
+      </c>
+      <c r="F41" s="72"/>
+      <c r="M41" s="86"/>
+      <c r="O41" s="72"/>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A42" s="72" t="s">
+        <v>262</v>
+      </c>
+      <c r="B42" s="72">
+        <v>-0.238124828874305</v>
+      </c>
+      <c r="E42" s="72">
+        <v>-1.7094294986265499E-2</v>
+      </c>
+      <c r="F42" s="72">
+        <f t="shared" si="10"/>
+        <v>-0.2382564086493025</v>
+      </c>
+      <c r="M42" s="86"/>
+      <c r="O42" s="72">
+        <f t="shared" si="11"/>
+        <v>1.315797749975034E-4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A43" s="72" t="s">
+        <v>263</v>
+      </c>
+      <c r="B43" s="72">
+        <v>-0.23811416408082101</v>
+      </c>
+      <c r="E43" s="72">
+        <v>-1.7094298065348599E-2</v>
+      </c>
+      <c r="F43" s="72">
+        <f t="shared" si="10"/>
+        <v>-0.2382564117283856</v>
+      </c>
+      <c r="M43" s="86"/>
+      <c r="O43" s="72">
+        <f t="shared" si="11"/>
+        <v>1.4224764756459729E-4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A44" s="72" t="s">
+        <v>71</v>
+      </c>
+      <c r="B44" s="72">
+        <v>-0.26782734160848398</v>
+      </c>
+      <c r="E44" s="72">
+        <v>-4.6817626498101603E-2</v>
+      </c>
+      <c r="F44" s="72">
+        <f t="shared" si="10"/>
+        <v>-0.26797974016113862</v>
+      </c>
+      <c r="M44" s="86"/>
+      <c r="O44" s="72">
+        <f t="shared" si="11"/>
+        <v>1.5239855265464231E-4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A45" s="72" t="s">
+        <v>264</v>
+      </c>
+      <c r="B45" s="72">
+        <v>-0.27082639634655098</v>
+      </c>
+      <c r="M45" s="86"/>
+      <c r="O45" s="72"/>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A46" s="72" t="s">
+        <v>265</v>
+      </c>
+      <c r="B46" s="72">
+        <v>-0.26537530725671299</v>
+      </c>
+      <c r="M46" s="86"/>
+      <c r="O46" s="72"/>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A47" s="72" t="s">
+        <v>266</v>
+      </c>
+      <c r="B47" s="72">
+        <v>-0.27056740976696902</v>
+      </c>
+      <c r="M47" s="86"/>
+      <c r="O47" s="72"/>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A48" s="72" t="s">
+        <v>267</v>
+      </c>
+      <c r="B48" s="72">
+        <v>-0.272193451087546</v>
+      </c>
+      <c r="M48" s="86"/>
+      <c r="O48" s="72"/>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A49" s="72" t="s">
+        <v>268</v>
+      </c>
+      <c r="B49" s="72">
+        <v>-0.28803193308711</v>
+      </c>
+      <c r="M49" s="86"/>
+      <c r="O49" s="72"/>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A50" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="B50" s="72">
+        <v>1.06021182972759</v>
+      </c>
+      <c r="M50" s="86"/>
+      <c r="O50" s="72"/>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A51" s="72" t="s">
+        <v>28</v>
+      </c>
+      <c r="B51" s="72">
+        <v>1.04521069537303</v>
+      </c>
+      <c r="E51" s="72">
+        <v>1.04499906313014</v>
+      </c>
+      <c r="F51" s="72">
+        <v>1.04499906313014</v>
+      </c>
+      <c r="M51" s="86"/>
+      <c r="O51" s="72">
+        <f t="shared" si="11"/>
+        <v>2.1163224289000304E-4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A52" s="72" t="s">
+        <v>94</v>
+      </c>
+      <c r="B52" s="72">
+        <v>1.0102223344885899</v>
+      </c>
+      <c r="E52" s="72">
+        <v>1.0099998991758801</v>
+      </c>
+      <c r="F52" s="72">
+        <v>1.0099998991758801</v>
+      </c>
+      <c r="M52" s="86"/>
+      <c r="O52" s="72">
+        <f t="shared" si="11"/>
+        <v>2.2243531270982331E-4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A53" s="72" t="s">
+        <v>231</v>
+      </c>
+      <c r="B53" s="72">
+        <v>1.0238916772678499</v>
+      </c>
+      <c r="E53" s="72">
+        <v>1.0237127697133499</v>
+      </c>
+      <c r="F53" s="72">
+        <v>1.0237127697133499</v>
+      </c>
+      <c r="M53" s="86"/>
+      <c r="O53" s="72">
+        <f t="shared" si="11"/>
+        <v>1.7890755450000739E-4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A54" s="72" t="s">
+        <v>210</v>
+      </c>
+      <c r="B54" s="72">
+        <v>1.02827099057284</v>
+      </c>
+      <c r="E54" s="72">
+        <v>1.0280924472289901</v>
+      </c>
+      <c r="F54" s="72">
+        <v>1.0280924472289901</v>
+      </c>
+      <c r="M54" s="86"/>
+      <c r="O54" s="72">
+        <f t="shared" si="11"/>
+        <v>1.7854334384992399E-4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A55" s="72" t="s">
+        <v>240</v>
+      </c>
+      <c r="B55" s="72">
+        <v>1.0384892284060301</v>
+      </c>
+      <c r="F55" s="72"/>
+      <c r="M55" s="86"/>
+      <c r="O55" s="72"/>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A56" s="72" t="s">
+        <v>232</v>
+      </c>
+      <c r="B56" s="72">
+        <v>1.0461591070376699</v>
+      </c>
+      <c r="E56" s="72">
+        <v>1.04612261065483</v>
+      </c>
+      <c r="F56" s="72">
+        <v>1.04612261065483</v>
+      </c>
+      <c r="M56" s="86"/>
+      <c r="O56" s="72">
+        <f t="shared" si="11"/>
+        <v>3.6496382839867891E-5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A57" s="72" t="s">
+        <v>211</v>
+      </c>
+      <c r="B57" s="72">
+        <v>1.08522332015065</v>
+      </c>
+      <c r="E57" s="72">
+        <v>1.08508352833644</v>
+      </c>
+      <c r="F57" s="72">
+        <v>1.08508352833644</v>
+      </c>
+      <c r="M57" s="86"/>
+      <c r="O57" s="72">
+        <f t="shared" si="11"/>
+        <v>1.3979181421008846E-4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A58" s="72" t="s">
+        <v>215</v>
+      </c>
+      <c r="B58" s="72">
+        <v>1.0346562939178801</v>
+      </c>
+      <c r="E58" s="72">
+        <v>1.0349154728988099</v>
+      </c>
+      <c r="F58" s="72">
+        <v>1.0349154728988099</v>
+      </c>
+      <c r="M58" s="86"/>
+      <c r="O58" s="72">
+        <f t="shared" si="11"/>
+        <v>-2.5917898092986391E-4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A59" s="72" t="s">
+        <v>214</v>
+      </c>
+      <c r="B59" s="72">
+        <v>1.0276736347300599</v>
+      </c>
+      <c r="M59" s="86"/>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A60" s="72" t="s">
+        <v>241</v>
+      </c>
+      <c r="B60" s="72">
+        <v>1.0294797148790999</v>
+      </c>
+      <c r="M60" s="86"/>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A61" s="72" t="s">
+        <v>212</v>
+      </c>
+      <c r="B61" s="72">
+        <v>1.0240118665753799</v>
+      </c>
+      <c r="M61" s="86"/>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A62" s="72" t="s">
+        <v>213</v>
+      </c>
+      <c r="B62" s="72">
+        <v>1.0198403758847501</v>
+      </c>
+      <c r="M62" s="86"/>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A63" s="72" t="s">
+        <v>248</v>
+      </c>
+      <c r="B63" s="72">
+        <v>1.0096275188231001</v>
+      </c>
+      <c r="M63" s="86"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:Q1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4158,15 +4639,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="86" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="86"/>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
-      <c r="F1" s="86"/>
-      <c r="G1" s="86"/>
+      <c r="A1" s="87" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
       <c r="I1" s="6" t="s">
         <v>1</v>
       </c>
@@ -4519,15 +5000,15 @@
       <c r="N11" s="1"/>
     </row>
     <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="87" t="s">
+      <c r="A12" s="88" t="s">
         <v>80</v>
       </c>
-      <c r="B12" s="87"/>
-      <c r="C12" s="87"/>
-      <c r="D12" s="87"/>
-      <c r="E12" s="87"/>
-      <c r="F12" s="87"/>
-      <c r="G12" s="87"/>
+      <c r="B12" s="88"/>
+      <c r="C12" s="88"/>
+      <c r="D12" s="88"/>
+      <c r="E12" s="88"/>
+      <c r="F12" s="88"/>
+      <c r="G12" s="88"/>
       <c r="I12" s="1"/>
       <c r="J12" s="6" t="s">
         <v>1</v>
@@ -5017,15 +5498,15 @@
       <c r="G31" s="1"/>
     </row>
     <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="87" t="s">
+      <c r="A32" s="88" t="s">
         <v>81</v>
       </c>
-      <c r="B32" s="87"/>
-      <c r="C32" s="87"/>
-      <c r="D32" s="87"/>
-      <c r="E32" s="87"/>
-      <c r="F32" s="87"/>
-      <c r="G32" s="87"/>
+      <c r="B32" s="88"/>
+      <c r="C32" s="88"/>
+      <c r="D32" s="88"/>
+      <c r="E32" s="88"/>
+      <c r="F32" s="88"/>
+      <c r="G32" s="88"/>
       <c r="I32" s="1"/>
       <c r="J32" s="6" t="s">
         <v>1</v>
@@ -5504,13 +5985,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="87" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="86"/>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
       <c r="G1" s="30" t="s">
         <v>100</v>
       </c>
@@ -5529,13 +6010,13 @@
       <c r="L1" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="P1" s="86" t="s">
+      <c r="P1" s="87" t="s">
         <v>106</v>
       </c>
-      <c r="Q1" s="86"/>
-      <c r="R1" s="86"/>
-      <c r="S1" s="86"/>
-      <c r="T1" s="86"/>
+      <c r="Q1" s="87"/>
+      <c r="R1" s="87"/>
+      <c r="S1" s="87"/>
+      <c r="T1" s="87"/>
       <c r="V1" s="30" t="s">
         <v>100</v>
       </c>
@@ -6070,12 +6551,12 @@
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="P10" s="86" t="s">
+      <c r="P10" s="87" t="s">
         <v>108</v>
       </c>
-      <c r="Q10" s="86"/>
-      <c r="R10" s="86"/>
-      <c r="S10" s="86"/>
+      <c r="Q10" s="87"/>
+      <c r="R10" s="87"/>
+      <c r="S10" s="87"/>
       <c r="T10" s="25"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
@@ -7091,12 +7572,12 @@
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A33" s="86" t="s">
+      <c r="A33" s="87" t="s">
         <v>102</v>
       </c>
-      <c r="B33" s="86"/>
-      <c r="C33" s="86"/>
-      <c r="D33" s="86"/>
+      <c r="B33" s="87"/>
+      <c r="C33" s="87"/>
+      <c r="D33" s="87"/>
       <c r="F33" s="30" t="s">
         <v>100</v>
       </c>
@@ -7474,12 +7955,12 @@
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A42" s="86" t="s">
+      <c r="A42" s="87" t="s">
         <v>104</v>
       </c>
-      <c r="B42" s="86"/>
-      <c r="C42" s="86"/>
-      <c r="D42" s="86"/>
+      <c r="B42" s="87"/>
+      <c r="C42" s="87"/>
+      <c r="D42" s="87"/>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
@@ -7978,15 +8459,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="88" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="87"/>
-      <c r="G1" s="87"/>
+      <c r="B1" s="88"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="88"/>
+      <c r="G1" s="88"/>
       <c r="I1" s="1"/>
       <c r="J1" s="4"/>
       <c r="L1" s="4" t="s">
@@ -9048,18 +9529,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="89" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="88"/>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
-      <c r="F1" s="88"/>
-      <c r="G1" s="88"/>
-      <c r="H1" s="88"/>
-      <c r="I1" s="88"/>
-      <c r="J1" s="88"/>
+      <c r="B1" s="89"/>
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="89"/>
+      <c r="H1" s="89"/>
+      <c r="I1" s="89"/>
+      <c r="J1" s="89"/>
       <c r="L1" s="11" t="s">
         <v>1</v>
       </c>
@@ -9083,18 +9564,18 @@
       <c r="B2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="89" t="s">
+      <c r="C2" s="90" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89" t="s">
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90" t="s">
         <v>74</v>
       </c>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
       <c r="L2" s="8" t="s">
         <v>41</v>
       </c>
@@ -9887,18 +10368,18 @@
       <c r="O33" s="1"/>
     </row>
     <row r="35" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="88" t="s">
+      <c r="A35" s="89" t="s">
         <v>78</v>
       </c>
-      <c r="B35" s="88"/>
-      <c r="C35" s="88"/>
-      <c r="D35" s="88"/>
-      <c r="E35" s="88"/>
-      <c r="F35" s="88"/>
-      <c r="G35" s="88"/>
-      <c r="H35" s="88"/>
-      <c r="I35" s="88"/>
-      <c r="J35" s="88"/>
+      <c r="B35" s="89"/>
+      <c r="C35" s="89"/>
+      <c r="D35" s="89"/>
+      <c r="E35" s="89"/>
+      <c r="F35" s="89"/>
+      <c r="G35" s="89"/>
+      <c r="H35" s="89"/>
+      <c r="I35" s="89"/>
+      <c r="J35" s="89"/>
       <c r="L35" s="11" t="s">
         <v>1</v>
       </c>
@@ -17690,18 +18171,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="89" t="s">
         <v>221</v>
       </c>
-      <c r="B1" s="88"/>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
-      <c r="F1" s="88"/>
-      <c r="G1" s="88"/>
-      <c r="H1" s="88"/>
-      <c r="I1" s="88"/>
-      <c r="J1" s="88"/>
+      <c r="B1" s="89"/>
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="89"/>
+      <c r="H1" s="89"/>
+      <c r="I1" s="89"/>
+      <c r="J1" s="89"/>
       <c r="K1" s="43"/>
       <c r="L1" s="60"/>
       <c r="M1" s="11" t="s">
@@ -17725,18 +18206,18 @@
       <c r="B2" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="89" t="s">
+      <c r="C2" s="90" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89" t="s">
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90" t="s">
         <v>74</v>
       </c>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
       <c r="K2" s="4"/>
       <c r="L2" s="60" t="s">
         <v>138</v>

</xml_diff>

<commit_message>
The way c_k is calculated is broken.
I started changing the way that c_k is calculated, but then realized
that each partition has its own slack bus and there's no way to know
what the difference in the slack bus angles are. To know the difference,
you would already need to know the centralized solution.

Also, I think the reason why the mini centralized SE results don't 100%
agree with the overall 14 bus centralized results is due to the fact
that the central Ybus(i,i) != the individual central Ybus(i,i). What I
should probably do instead is actually form a Ybus(i,i) that's purely
the size of the partition's state vector (not including the overlapped
buses) and then input the extra line parameters to calculate those
values in h.
</commit_message>
<xml_diff>
--- a/DMASE - Test Results.xlsx
+++ b/DMASE - Test Results.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leilei\Documents\GitHub\D-MASE\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12240" windowHeight="9240" firstSheet="3" activeTab="10"/>
   </bookViews>
@@ -18,13 +23,14 @@
     <sheet name="14 Bus AC" sheetId="6" r:id="rId9"/>
     <sheet name="14 Bus Partitions" sheetId="11" r:id="rId10"/>
     <sheet name="Sheet2" sheetId="12" r:id="rId11"/>
+    <sheet name="Sheet1" sheetId="13" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="296">
   <si>
     <t>Abur 3-Bus Case Measurements (run through SE, rerun new estimate again)</t>
   </si>
@@ -861,6 +867,57 @@
   </si>
   <si>
     <t>Uses small Ybus for each partition, which is slightly different from using the Ybus for the overall system</t>
+  </si>
+  <si>
+    <t>6.02500000000000 - 19.4471000000000i</t>
+  </si>
+  <si>
+    <t>-4.99910000000000 + 15.2631000000000i</t>
+  </si>
+  <si>
+    <t>0.00000000000000 + 0.00000000000000i</t>
+  </si>
+  <si>
+    <t>-1.02590000000000 + 4.23500000000000i</t>
+  </si>
+  <si>
+    <t>9.52130000000000 - 30.2721000000000i</t>
+  </si>
+  <si>
+    <t>-1.13500000000000 + 4.78190000000000i</t>
+  </si>
+  <si>
+    <t>-1.68600000000000 + 5.11580000000000i</t>
+  </si>
+  <si>
+    <t>-1.70110000000000 + 5.19390000000000i</t>
+  </si>
+  <si>
+    <t>3.12100000000000 - 9.82240000000000i</t>
+  </si>
+  <si>
+    <t>-1.98600000000000 + 5.06880000000000i</t>
+  </si>
+  <si>
+    <t>10.5130000000000 - 31.7398000000000i</t>
+  </si>
+  <si>
+    <t>-6.84100000000000 + 21.5786000000000i</t>
+  </si>
+  <si>
+    <t>9.56800000000000 - 34.9335000000000i</t>
+  </si>
+  <si>
+    <t>0.00000000000000 + 3.96790000000000i</t>
+  </si>
+  <si>
+    <t>0.00000000000000 - 3.96790000000000i</t>
+  </si>
+  <si>
+    <t>10.5130000000000 - 38.3197000000000i</t>
+  </si>
+  <si>
+    <t>6.57990000000000 - 17.3407000000000i</t>
   </si>
 </sst>
 </file>
@@ -1376,7 +1433,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1411,7 +1468,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1876,7 +1933,7 @@
   <dimension ref="A1:S59"/>
   <sheetViews>
     <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="P23" sqref="P23"/>
+      <selection activeCell="S29" sqref="S29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3228,8 +3285,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="O45" sqref="O45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4611,6 +4668,196 @@
   <mergeCells count="1">
     <mergeCell ref="A1:Q1"/>
   </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:G15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="6" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>279</v>
+      </c>
+      <c r="C2" t="s">
+        <v>280</v>
+      </c>
+      <c r="F2" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>280</v>
+      </c>
+      <c r="C3" t="s">
+        <v>283</v>
+      </c>
+      <c r="D3" t="s">
+        <v>284</v>
+      </c>
+      <c r="E3" t="s">
+        <v>285</v>
+      </c>
+      <c r="F3" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>284</v>
+      </c>
+      <c r="D4" t="s">
+        <v>287</v>
+      </c>
+      <c r="E4" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>285</v>
+      </c>
+      <c r="D5" t="s">
+        <v>288</v>
+      </c>
+      <c r="E5" t="s">
+        <v>289</v>
+      </c>
+      <c r="F5" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>282</v>
+      </c>
+      <c r="C6" t="s">
+        <v>286</v>
+      </c>
+      <c r="E6" t="s">
+        <v>290</v>
+      </c>
+      <c r="F6" t="s">
+        <v>291</v>
+      </c>
+      <c r="G6" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>292</v>
+      </c>
+      <c r="G7" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>279</v>
+      </c>
+      <c r="C10" t="s">
+        <v>280</v>
+      </c>
+      <c r="F10" t="s">
+        <v>282</v>
+      </c>
+      <c r="G10" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>280</v>
+      </c>
+      <c r="C11" t="s">
+        <v>283</v>
+      </c>
+      <c r="D11" t="s">
+        <v>284</v>
+      </c>
+      <c r="E11" t="s">
+        <v>285</v>
+      </c>
+      <c r="F11" t="s">
+        <v>286</v>
+      </c>
+      <c r="G11" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>284</v>
+      </c>
+      <c r="D12" t="s">
+        <v>287</v>
+      </c>
+      <c r="E12" t="s">
+        <v>288</v>
+      </c>
+      <c r="F12" t="s">
+        <v>281</v>
+      </c>
+      <c r="G12" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>285</v>
+      </c>
+      <c r="D13" t="s">
+        <v>288</v>
+      </c>
+      <c r="E13" t="s">
+        <v>294</v>
+      </c>
+      <c r="F13" t="s">
+        <v>290</v>
+      </c>
+      <c r="G13" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>282</v>
+      </c>
+      <c r="C14" t="s">
+        <v>286</v>
+      </c>
+      <c r="E14" t="s">
+        <v>290</v>
+      </c>
+      <c r="F14" t="s">
+        <v>291</v>
+      </c>
+      <c r="G14" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>292</v>
+      </c>
+      <c r="G15" t="s">
+        <v>295</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
How to reference areas with different slack buses to the same global slack bus
One way to reference all of the areas to the same slack bus is to look
at common buses measured between the area of interest and the area with
the global slack bus. Then take the angle(s) of the area with the global
slack bus and subtract from it the angle(s) of the area of interest.
Then take the average of all the angles and add that to the area of
interest's state vector.
</commit_message>
<xml_diff>
--- a/DMASE - Test Results.xlsx
+++ b/DMASE - Test Results.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leilei\Documents\GitHub\D-MASE\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12240" windowHeight="9240" firstSheet="3" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12240" windowHeight="9240" firstSheet="3" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="2 Bus" sheetId="4" r:id="rId1"/>
@@ -24,13 +19,14 @@
     <sheet name="14 Bus Partitions" sheetId="11" r:id="rId10"/>
     <sheet name="Sheet2" sheetId="12" r:id="rId11"/>
     <sheet name="Sheet1" sheetId="13" r:id="rId12"/>
+    <sheet name="Sheet3" sheetId="14" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1121" uniqueCount="314">
   <si>
     <t>Abur 3-Bus Case Measurements (run through SE, rerun new estimate again)</t>
   </si>
@@ -918,6 +914,60 @@
   </si>
   <si>
     <t>6.57990000000000 - 17.3407000000000i</t>
+  </si>
+  <si>
+    <t>Area1</t>
+  </si>
+  <si>
+    <t>Area2 (unscaled)</t>
+  </si>
+  <si>
+    <t>Area3 (unscaled)</t>
+  </si>
+  <si>
+    <t>Area4 (unscaled)</t>
+  </si>
+  <si>
+    <t>first iteration x_k</t>
+  </si>
+  <si>
+    <t>Issues to consider in implementing ADMM-based MASE</t>
+  </si>
+  <si>
+    <t>1. rectangular form of power flow</t>
+  </si>
+  <si>
+    <t>2. slack bus reconciliation</t>
+  </si>
+  <si>
+    <t>3. division of partitions/overlap boundaries</t>
+  </si>
+  <si>
+    <t>Choose global reference slack bus</t>
+  </si>
+  <si>
+    <t>In this case, let's say area 1</t>
+  </si>
+  <si>
+    <t>AVG DIFF</t>
+  </si>
+  <si>
+    <t>Area 1 - Area 2</t>
+  </si>
+  <si>
+    <t>Area 1 - Area 3</t>
+  </si>
+  <si>
+    <t>Area 1 - Area 4</t>
+  </si>
+  <si>
+    <t>Area 2 (scaled)</t>
+  </si>
+  <si>
+    <t>Area 3 (scaled)</t>
+  </si>
+  <si>
+    <t>Area 4 (scaled)</t>
   </si>
 </sst>
 </file>
@@ -1433,7 +1483,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1468,7 +1518,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1932,7 +1982,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S59"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S29" sqref="S29"/>
     </sheetView>
   </sheetViews>
@@ -3285,8 +3335,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4677,7 +4727,7 @@
   <dimension ref="B2:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4822,7 +4872,7 @@
       <c r="D13" t="s">
         <v>288</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="2" t="s">
         <v>294</v>
       </c>
       <c r="F13" t="s">
@@ -4853,11 +4903,940 @@
       <c r="F15" t="s">
         <v>292</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="2" t="s">
         <v>295</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="5" width="16" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="72"/>
+    <col min="11" max="11" width="9.140625" customWidth="1"/>
+    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="16" style="72" customWidth="1"/>
+    <col min="15" max="15" width="16" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="16" style="72" customWidth="1"/>
+    <col min="18" max="18" width="16" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" s="72" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="94" t="s">
+        <v>300</v>
+      </c>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="I1" s="94" t="s">
+        <v>300</v>
+      </c>
+      <c r="J1" s="94"/>
+      <c r="K1" s="94"/>
+      <c r="L1" s="94"/>
+      <c r="M1" s="94"/>
+      <c r="N1" s="94"/>
+      <c r="O1" s="94"/>
+      <c r="P1" s="94"/>
+      <c r="Q1" s="94"/>
+      <c r="R1" s="94"/>
+      <c r="U1" s="72" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>296</v>
+      </c>
+      <c r="C2" t="s">
+        <v>297</v>
+      </c>
+      <c r="D2" s="72" t="s">
+        <v>298</v>
+      </c>
+      <c r="E2" s="72" t="s">
+        <v>299</v>
+      </c>
+      <c r="I2" s="72"/>
+      <c r="J2" s="72" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="72" t="s">
+        <v>296</v>
+      </c>
+      <c r="L2" s="72" t="s">
+        <v>297</v>
+      </c>
+      <c r="M2" s="72" t="s">
+        <v>308</v>
+      </c>
+      <c r="N2" s="72" t="s">
+        <v>311</v>
+      </c>
+      <c r="O2" s="72" t="s">
+        <v>298</v>
+      </c>
+      <c r="P2" s="72" t="s">
+        <v>309</v>
+      </c>
+      <c r="Q2" s="72" t="s">
+        <v>312</v>
+      </c>
+      <c r="R2" s="72" t="s">
+        <v>299</v>
+      </c>
+      <c r="S2" t="s">
+        <v>310</v>
+      </c>
+      <c r="T2" t="s">
+        <v>313</v>
+      </c>
+      <c r="U2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="72" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3">
+        <v>1.06528940064943</v>
+      </c>
+      <c r="I3" s="72" t="s">
+        <v>91</v>
+      </c>
+      <c r="J3" s="72">
+        <v>0</v>
+      </c>
+      <c r="K3" s="72">
+        <v>0</v>
+      </c>
+      <c r="L3" s="72"/>
+      <c r="O3" s="72"/>
+      <c r="R3" s="72"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="72" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4">
+        <v>1.0460411087171999</v>
+      </c>
+      <c r="C4">
+        <v>1.0366520373714401</v>
+      </c>
+      <c r="I4" s="72" t="s">
+        <v>92</v>
+      </c>
+      <c r="J4" s="72">
+        <v>-8.6669791486718703E-2</v>
+      </c>
+      <c r="K4" s="72">
+        <v>-9.1290585578995304E-2</v>
+      </c>
+      <c r="L4" s="72">
+        <v>0.13604529735975701</v>
+      </c>
+      <c r="M4" s="72">
+        <f>K4-L4</f>
+        <v>-0.22733588293875232</v>
+      </c>
+      <c r="N4" s="72">
+        <f>L4+$M$32</f>
+        <v>-9.5084673299724309E-2</v>
+      </c>
+      <c r="O4" s="72"/>
+      <c r="R4" s="72"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="72" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5">
+        <v>0.99202295652386696</v>
+      </c>
+      <c r="C5">
+        <v>1.01080492498633</v>
+      </c>
+      <c r="I5" s="72" t="s">
+        <v>93</v>
+      </c>
+      <c r="J5" s="72">
+        <v>-0.22116211366303701</v>
+      </c>
+      <c r="K5" s="72">
+        <v>-0.235459843805775</v>
+      </c>
+      <c r="L5" s="72">
+        <v>0</v>
+      </c>
+      <c r="M5" s="72">
+        <f>K5-L5</f>
+        <v>-0.235459843805775</v>
+      </c>
+      <c r="N5" s="72">
+        <f t="shared" ref="N5:N7" si="0">L5+$M$32</f>
+        <v>-0.23112997065948132</v>
+      </c>
+      <c r="O5" s="72"/>
+      <c r="R5" s="72"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="72" t="s">
+        <v>151</v>
+      </c>
+      <c r="B6">
+        <v>1.01449687116911</v>
+      </c>
+      <c r="C6">
+        <v>1.0237650685834301</v>
+      </c>
+      <c r="E6" s="72">
+        <v>1.02266696072011</v>
+      </c>
+      <c r="I6" s="72" t="s">
+        <v>259</v>
+      </c>
+      <c r="J6" s="72">
+        <v>-0.18108637306068801</v>
+      </c>
+      <c r="K6" s="72">
+        <v>-0.19120119080043499</v>
+      </c>
+      <c r="L6" s="72">
+        <v>4.0056113513174202E-2</v>
+      </c>
+      <c r="M6" s="72">
+        <f>K6-L6</f>
+        <v>-0.23125730431360919</v>
+      </c>
+      <c r="N6" s="72">
+        <f t="shared" si="0"/>
+        <v>-0.19107385714630712</v>
+      </c>
+      <c r="O6" s="72"/>
+      <c r="R6" s="72">
+        <v>8.7666838686665693E-2</v>
+      </c>
+      <c r="S6">
+        <f>K6-R6</f>
+        <v>-0.27886802948710065</v>
+      </c>
+      <c r="T6">
+        <f>R6+$S$32</f>
+        <v>-0.19120119080043496</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="72" t="s">
+        <v>152</v>
+      </c>
+      <c r="B7">
+        <v>1.0218931452171001</v>
+      </c>
+      <c r="C7">
+        <v>1.02789838928665</v>
+      </c>
+      <c r="D7" s="72">
+        <v>1.0227107597990099</v>
+      </c>
+      <c r="I7" s="72" t="s">
+        <v>260</v>
+      </c>
+      <c r="J7" s="72">
+        <v>-0.15459540540712</v>
+      </c>
+      <c r="K7" s="72">
+        <v>-0.163466853701174</v>
+      </c>
+      <c r="L7" s="72">
+        <v>6.69999978786147E-2</v>
+      </c>
+      <c r="M7" s="72">
+        <f>K7-L7</f>
+        <v>-0.23046685157978869</v>
+      </c>
+      <c r="N7" s="72">
+        <f t="shared" si="0"/>
+        <v>-0.16412997278086661</v>
+      </c>
+      <c r="O7" s="72">
+        <v>0.104196486471622</v>
+      </c>
+      <c r="P7" s="72">
+        <f>K7-O7</f>
+        <v>-0.26766334017279603</v>
+      </c>
+      <c r="Q7" s="72">
+        <f>O7+$P$32</f>
+        <v>-0.15385036613490921</v>
+      </c>
+      <c r="T7" s="72"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="72" t="s">
+        <v>153</v>
+      </c>
+      <c r="B8">
+        <v>1.01563267653981</v>
+      </c>
+      <c r="D8" s="72">
+        <v>1.0391282933224899</v>
+      </c>
+      <c r="I8" s="72" t="s">
+        <v>261</v>
+      </c>
+      <c r="J8" s="72">
+        <v>-0.25490550345711999</v>
+      </c>
+      <c r="K8" s="72">
+        <v>-0.267926663489854</v>
+      </c>
+      <c r="O8" s="72">
+        <v>0</v>
+      </c>
+      <c r="P8" s="72">
+        <f>K8-O8</f>
+        <v>-0.267926663489854</v>
+      </c>
+      <c r="Q8" s="72">
+        <f>O8+$P$32</f>
+        <v>-0.25804685260653121</v>
+      </c>
+      <c r="T8" s="72"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="72" t="s">
+        <v>154</v>
+      </c>
+      <c r="C9">
+        <v>1.0465513528972901</v>
+      </c>
+      <c r="E9" s="72">
+        <v>1.04697591826057</v>
+      </c>
+      <c r="I9" s="72" t="s">
+        <v>262</v>
+      </c>
+      <c r="J9" s="72">
+        <v>-0.238124828874305</v>
+      </c>
+      <c r="K9" s="72"/>
+      <c r="L9" s="72">
+        <v>-1.9000290946371599E-2</v>
+      </c>
+      <c r="R9" s="72">
+        <v>3.0814112406048599E-2</v>
+      </c>
+      <c r="T9" s="72">
+        <f t="shared" ref="T7:T16" si="1">R9+$S$32</f>
+        <v>-0.24805391708105207</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" s="72" t="s">
+        <v>155</v>
+      </c>
+      <c r="C10">
+        <v>1.0875611278507999</v>
+      </c>
+      <c r="I10" s="72" t="s">
+        <v>263</v>
+      </c>
+      <c r="J10" s="72">
+        <v>-0.23811416408082101</v>
+      </c>
+      <c r="K10" s="72"/>
+      <c r="L10" s="72">
+        <v>-1.8255514956707498E-2</v>
+      </c>
+      <c r="T10" s="72"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" s="72" t="s">
+        <v>156</v>
+      </c>
+      <c r="C11">
+        <v>1.03363463574681</v>
+      </c>
+      <c r="E11" s="72">
+        <v>1.0353437154263301</v>
+      </c>
+      <c r="I11" s="72" t="s">
+        <v>71</v>
+      </c>
+      <c r="J11" s="72">
+        <v>-0.26782734160848398</v>
+      </c>
+      <c r="K11" s="72"/>
+      <c r="L11" s="72">
+        <v>-5.0260940165644002E-2</v>
+      </c>
+      <c r="R11" s="72">
+        <v>0</v>
+      </c>
+      <c r="T11" s="72">
+        <f t="shared" si="1"/>
+        <v>-0.27886802948710065</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" s="72" t="s">
+        <v>157</v>
+      </c>
+      <c r="D12" s="72">
+        <v>1.0279410767585999</v>
+      </c>
+      <c r="E12" s="72">
+        <v>1.02791715563223</v>
+      </c>
+      <c r="I12" s="72" t="s">
+        <v>264</v>
+      </c>
+      <c r="J12" s="72">
+        <v>-0.27082639634655098</v>
+      </c>
+      <c r="K12" s="72"/>
+      <c r="L12" s="72"/>
+      <c r="O12" s="72">
+        <v>-1.6600304727115101E-2</v>
+      </c>
+      <c r="P12" s="72">
+        <f>J12-O12</f>
+        <v>-0.25422609161943588</v>
+      </c>
+      <c r="Q12" s="72">
+        <f t="shared" ref="Q8:Q16" si="2">O12+$P$32</f>
+        <v>-0.27464715733364631</v>
+      </c>
+      <c r="R12" s="72">
+        <v>-2.9904912760974301E-3</v>
+      </c>
+      <c r="T12" s="72">
+        <f t="shared" si="1"/>
+        <v>-0.28185852076319806</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="72" t="s">
+        <v>158</v>
+      </c>
+      <c r="D13" s="72">
+        <v>1.02984990508254</v>
+      </c>
+      <c r="E13" s="72">
+        <v>1.0293026657978499</v>
+      </c>
+      <c r="I13" s="72" t="s">
+        <v>265</v>
+      </c>
+      <c r="J13" s="72">
+        <v>-0.26537530725671299</v>
+      </c>
+      <c r="K13" s="72"/>
+      <c r="L13" s="72"/>
+      <c r="O13" s="72">
+        <v>-1.0947560823407299E-2</v>
+      </c>
+      <c r="P13" s="72">
+        <f t="shared" ref="P13:P16" si="3">J13-O13</f>
+        <v>-0.25442774643330568</v>
+      </c>
+      <c r="Q13" s="72">
+        <f t="shared" si="2"/>
+        <v>-0.26899441342993852</v>
+      </c>
+      <c r="R13" s="72">
+        <v>2.8179192054674602E-3</v>
+      </c>
+      <c r="T13" s="72">
+        <f t="shared" si="1"/>
+        <v>-0.27605011028163318</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" s="72" t="s">
+        <v>159</v>
+      </c>
+      <c r="D14" s="72">
+        <v>1.02406093645796</v>
+      </c>
+      <c r="I14" s="72" t="s">
+        <v>266</v>
+      </c>
+      <c r="J14" s="72">
+        <v>-0.27056740976696902</v>
+      </c>
+      <c r="K14" s="72"/>
+      <c r="L14" s="72"/>
+      <c r="O14" s="72">
+        <v>-1.6267059612644099E-2</v>
+      </c>
+      <c r="P14" s="72">
+        <f t="shared" si="3"/>
+        <v>-0.25430035015432495</v>
+      </c>
+      <c r="Q14" s="72">
+        <f t="shared" si="2"/>
+        <v>-0.27431391221917528</v>
+      </c>
+      <c r="T14" s="72"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" s="72" t="s">
+        <v>160</v>
+      </c>
+      <c r="D15" s="72">
+        <v>1.0198149779104799</v>
+      </c>
+      <c r="E15" s="72">
+        <v>1.0182381308847801</v>
+      </c>
+      <c r="I15" s="72" t="s">
+        <v>267</v>
+      </c>
+      <c r="J15" s="72">
+        <v>-0.272193451087546</v>
+      </c>
+      <c r="K15" s="72"/>
+      <c r="L15" s="72"/>
+      <c r="O15" s="72">
+        <v>-1.7998913484384298E-2</v>
+      </c>
+      <c r="P15" s="72">
+        <f t="shared" si="3"/>
+        <v>-0.25419453760316169</v>
+      </c>
+      <c r="Q15" s="72">
+        <f t="shared" si="2"/>
+        <v>-0.27604576609091552</v>
+      </c>
+      <c r="R15" s="72">
+        <v>-3.7762002123430498E-3</v>
+      </c>
+      <c r="T15" s="72">
+        <f t="shared" si="1"/>
+        <v>-0.28264422969944369</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="72" t="s">
+        <v>161</v>
+      </c>
+      <c r="D16" s="72">
+        <v>1.0087683120630799</v>
+      </c>
+      <c r="E16" s="72">
+        <v>1.0090207852464499</v>
+      </c>
+      <c r="I16" s="72" t="s">
+        <v>268</v>
+      </c>
+      <c r="J16" s="72">
+        <v>-0.28803193308711</v>
+      </c>
+      <c r="K16" s="72"/>
+      <c r="L16" s="72"/>
+      <c r="O16" s="72">
+        <v>-3.4442694314269398E-2</v>
+      </c>
+      <c r="P16" s="72">
+        <f t="shared" si="3"/>
+        <v>-0.25358923877284062</v>
+      </c>
+      <c r="Q16" s="72">
+        <f t="shared" si="2"/>
+        <v>-0.29248954692080059</v>
+      </c>
+      <c r="R16" s="72">
+        <v>-2.0422237393388699E-2</v>
+      </c>
+      <c r="T16" s="72">
+        <f t="shared" si="1"/>
+        <v>-0.29929026688048938</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17" s="72" t="s">
+        <v>87</v>
+      </c>
+      <c r="I17" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="J17" s="72">
+        <v>1.06021182972759</v>
+      </c>
+      <c r="K17" s="72">
+        <v>1.06528940064943</v>
+      </c>
+      <c r="L17" s="72"/>
+      <c r="O17" s="72"/>
+      <c r="R17" s="72"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18" s="72" t="s">
+        <v>88</v>
+      </c>
+      <c r="B18">
+        <v>-9.5759873274871996E-2</v>
+      </c>
+      <c r="C18">
+        <v>0.14190821118581601</v>
+      </c>
+      <c r="I18" s="72" t="s">
+        <v>28</v>
+      </c>
+      <c r="J18" s="72">
+        <v>1.04521069537303</v>
+      </c>
+      <c r="K18" s="72">
+        <v>1.05041513434258</v>
+      </c>
+      <c r="L18" s="72">
+        <v>1.04631992573415</v>
+      </c>
+      <c r="O18" s="72"/>
+      <c r="R18" s="72"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A19" s="72" t="s">
+        <v>89</v>
+      </c>
+      <c r="B19">
+        <v>-0.23799618884858001</v>
+      </c>
+      <c r="I19" s="72" t="s">
+        <v>94</v>
+      </c>
+      <c r="J19" s="72">
+        <v>1.0102223344885899</v>
+      </c>
+      <c r="K19" s="72">
+        <v>1.0201724031637001</v>
+      </c>
+      <c r="L19" s="72">
+        <v>1.01080492498633</v>
+      </c>
+      <c r="O19" s="72"/>
+      <c r="R19" s="72"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A20" s="72" t="s">
+        <v>162</v>
+      </c>
+      <c r="B20">
+        <v>-0.19637184279346301</v>
+      </c>
+      <c r="C20">
+        <v>4.1029996249025397E-2</v>
+      </c>
+      <c r="E20" s="72">
+        <v>8.9884365546254993E-2</v>
+      </c>
+      <c r="I20" s="72" t="s">
+        <v>231</v>
+      </c>
+      <c r="J20" s="72">
+        <v>1.0238916772678499</v>
+      </c>
+      <c r="K20" s="72">
+        <v>1.0333275387088099</v>
+      </c>
+      <c r="L20" s="72">
+        <v>1.0245869295690999</v>
+      </c>
+      <c r="O20" s="72"/>
+      <c r="R20" s="72">
+        <v>1.0266094251068201</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A21" s="72" t="s">
+        <v>163</v>
+      </c>
+      <c r="B21">
+        <v>-0.16854963328528999</v>
+      </c>
+      <c r="C21">
+        <v>6.8972426535251805E-2</v>
+      </c>
+      <c r="D21" s="72">
+        <v>0.106950197760304</v>
+      </c>
+      <c r="I21" s="72" t="s">
+        <v>210</v>
+      </c>
+      <c r="J21" s="72">
+        <v>1.02827099057284</v>
+      </c>
+      <c r="K21" s="72">
+        <v>1.03570004302515</v>
+      </c>
+      <c r="L21" s="72">
+        <v>1.0302098302386</v>
+      </c>
+      <c r="O21" s="72">
+        <v>1.0282877238446599</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A22" s="72" t="s">
+        <v>164</v>
+      </c>
+      <c r="B22">
+        <v>-0.27881886491819902</v>
+      </c>
+      <c r="I22" s="72" t="s">
+        <v>240</v>
+      </c>
+      <c r="J22" s="72">
+        <v>1.0384892284060301</v>
+      </c>
+      <c r="K22" s="72">
+        <v>1.0532092351900899</v>
+      </c>
+      <c r="O22" s="72">
+        <v>1.0391282933224899</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A23" s="72" t="s">
+        <v>165</v>
+      </c>
+      <c r="C23">
+        <v>-1.98871734161255E-2</v>
+      </c>
+      <c r="E23" s="72">
+        <v>3.2271848420798298E-2</v>
+      </c>
+      <c r="I23" s="72" t="s">
+        <v>232</v>
+      </c>
+      <c r="J23" s="72">
+        <v>1.0461591070376699</v>
+      </c>
+      <c r="K23" s="72"/>
+      <c r="L23" s="72">
+        <v>1.0467402896218501</v>
+      </c>
+      <c r="R23" s="72">
+        <v>1.0474731717891701</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A24" s="72" t="s">
+        <v>166</v>
+      </c>
+      <c r="C24">
+        <v>-1.9856194268582199E-2</v>
+      </c>
+      <c r="I24" s="72" t="s">
+        <v>211</v>
+      </c>
+      <c r="J24" s="72">
+        <v>1.08522332015065</v>
+      </c>
+      <c r="K24" s="72"/>
+      <c r="L24" s="72">
+        <v>1.0877423754101601</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A25" s="72" t="s">
+        <v>167</v>
+      </c>
+      <c r="C25">
+        <v>-5.1995238756297503E-2</v>
+      </c>
+      <c r="I25" s="72" t="s">
+        <v>215</v>
+      </c>
+      <c r="J25" s="72">
+        <v>1.0346562939178801</v>
+      </c>
+      <c r="K25" s="72"/>
+      <c r="L25" s="72">
+        <v>1.03494157567892</v>
+      </c>
+      <c r="R25" s="72">
+        <v>1.0353437154263301</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A26" s="72" t="s">
+        <v>168</v>
+      </c>
+      <c r="D26" s="72">
+        <v>-1.7065702743745501E-2</v>
+      </c>
+      <c r="E26" s="72">
+        <v>-3.0739864500671501E-3</v>
+      </c>
+      <c r="I26" s="72" t="s">
+        <v>214</v>
+      </c>
+      <c r="J26" s="72">
+        <v>1.0276736347300599</v>
+      </c>
+      <c r="K26" s="72"/>
+      <c r="L26" s="72"/>
+      <c r="O26" s="72">
+        <v>1.02808272794449</v>
+      </c>
+      <c r="R26" s="72">
+        <v>1.02792175200049</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A27" s="72" t="s">
+        <v>169</v>
+      </c>
+      <c r="D27" s="72">
+        <v>-1.1274794903099E-2</v>
+      </c>
+      <c r="E27" s="72">
+        <v>2.9004994274963E-3</v>
+      </c>
+      <c r="I27" s="72" t="s">
+        <v>241</v>
+      </c>
+      <c r="J27" s="72">
+        <v>1.0294797148790999</v>
+      </c>
+      <c r="K27" s="72"/>
+      <c r="L27" s="72"/>
+      <c r="O27" s="72">
+        <v>1.02991162145042</v>
+      </c>
+      <c r="R27" s="72">
+        <v>1.02930675248708</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A28" s="72" t="s">
+        <v>170</v>
+      </c>
+      <c r="D28" s="72">
+        <v>-1.6659929827751802E-2</v>
+      </c>
+      <c r="I28" s="72" t="s">
+        <v>212</v>
+      </c>
+      <c r="J28" s="72">
+        <v>1.0240118665753799</v>
+      </c>
+      <c r="K28" s="72"/>
+      <c r="L28" s="72"/>
+      <c r="O28" s="72">
+        <v>1.02419644348192</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A29" s="72" t="s">
+        <v>171</v>
+      </c>
+      <c r="D29" s="72">
+        <v>-1.83575439757129E-2</v>
+      </c>
+      <c r="E29" s="72">
+        <v>-3.8450893226716801E-3</v>
+      </c>
+      <c r="I29" s="72" t="s">
+        <v>213</v>
+      </c>
+      <c r="J29" s="72">
+        <v>1.0198403758847501</v>
+      </c>
+      <c r="K29" s="72"/>
+      <c r="L29" s="72"/>
+      <c r="O29" s="72">
+        <v>1.0199801902936001</v>
+      </c>
+      <c r="R29" s="72">
+        <v>1.01824539080697</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A30" s="72" t="s">
+        <v>172</v>
+      </c>
+      <c r="D30" s="72">
+        <v>-3.4758444331587403E-2</v>
+      </c>
+      <c r="E30" s="72">
+        <v>-2.0609327252956802E-2</v>
+      </c>
+      <c r="I30" s="72" t="s">
+        <v>248</v>
+      </c>
+      <c r="J30" s="72">
+        <v>1.0096275188231001</v>
+      </c>
+      <c r="K30" s="72"/>
+      <c r="L30" s="72"/>
+      <c r="O30" s="72">
+        <v>1.0093669584818701</v>
+      </c>
+      <c r="R30" s="72">
+        <v>1.0092312368477301</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="L32" t="s">
+        <v>307</v>
+      </c>
+      <c r="M32" s="72">
+        <f>AVERAGE(M4:M7)</f>
+        <v>-0.23112997065948132</v>
+      </c>
+      <c r="P32" s="72">
+        <f>AVERAGE(P7:P16)</f>
+        <v>-0.25804685260653121</v>
+      </c>
+      <c r="S32">
+        <f>S6</f>
+        <v>-0.27886802948710065</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>304</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="I1:R1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
How to calculate the slack bus shift
Calculated (and documented) how to do the slack bus shift. First take
Area 1 overlap angles - Area X overlap angles (angles of the buses
shared between the two areas' state vectors). Then convert them from
polar into rectangular form (using trig identities, see .docx), and add
them back to the original rectangular states. Next step is to figure out
the process flow. Does this need to be done for every iteration of ADMM?
Also need to finish editing how c_k works. Don't worry about the
automatic calculation yet.
</commit_message>
<xml_diff>
--- a/DMASE - Test Results.xlsx
+++ b/DMASE - Test Results.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1121" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1123" uniqueCount="316">
   <si>
     <t>Abur 3-Bus Case Measurements (run through SE, rerun new estimate again)</t>
   </si>
@@ -968,6 +968,12 @@
   </si>
   <si>
     <t>Area 4 (scaled)</t>
+  </si>
+  <si>
+    <t>Calculated</t>
+  </si>
+  <si>
+    <t>4. observability (I think it requires local observability to converge, which is more strict than global observability)</t>
   </si>
 </sst>
 </file>
@@ -4914,27 +4920,29 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U37"/>
+  <dimension ref="A1:V38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="72"/>
-    <col min="11" max="11" width="9.140625" customWidth="1"/>
-    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="16" style="72" customWidth="1"/>
-    <col min="15" max="15" width="16" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="16" style="72" customWidth="1"/>
-    <col min="18" max="18" width="16" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" style="72" customWidth="1"/>
+    <col min="5" max="6" width="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="72"/>
+    <col min="12" max="12" width="9.140625" customWidth="1"/>
+    <col min="13" max="13" width="16" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="16" style="72" customWidth="1"/>
+    <col min="16" max="16" width="16" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="16" style="72" customWidth="1"/>
+    <col min="19" max="19" width="16" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" s="72" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="94" t="s">
         <v>300</v>
       </c>
@@ -4942,10 +4950,10 @@
       <c r="C1" s="94"/>
       <c r="D1" s="94"/>
       <c r="E1" s="94"/>
-      <c r="I1" s="94" t="s">
+      <c r="F1" s="94"/>
+      <c r="J1" s="94" t="s">
         <v>300</v>
       </c>
-      <c r="J1" s="94"/>
       <c r="K1" s="94"/>
       <c r="L1" s="94"/>
       <c r="M1" s="94"/>
@@ -4954,11 +4962,12 @@
       <c r="P1" s="94"/>
       <c r="Q1" s="94"/>
       <c r="R1" s="94"/>
-      <c r="U1" s="72" t="s">
+      <c r="S1" s="94"/>
+      <c r="V1" s="72" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>296</v>
       </c>
@@ -4966,70 +4975,76 @@
         <v>297</v>
       </c>
       <c r="D2" s="72" t="s">
+        <v>314</v>
+      </c>
+      <c r="E2" s="72" t="s">
         <v>298</v>
       </c>
-      <c r="E2" s="72" t="s">
+      <c r="F2" s="72" t="s">
         <v>299</v>
       </c>
-      <c r="I2" s="72"/>
-      <c r="J2" s="72" t="s">
+      <c r="J2" s="72"/>
+      <c r="K2" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="72" t="s">
+      <c r="L2" s="72" t="s">
         <v>296</v>
       </c>
-      <c r="L2" s="72" t="s">
+      <c r="M2" s="72" t="s">
         <v>297</v>
       </c>
-      <c r="M2" s="72" t="s">
+      <c r="N2" s="72" t="s">
         <v>308</v>
       </c>
-      <c r="N2" s="72" t="s">
+      <c r="O2" s="72" t="s">
         <v>311</v>
       </c>
-      <c r="O2" s="72" t="s">
+      <c r="P2" s="72" t="s">
         <v>298</v>
       </c>
-      <c r="P2" s="72" t="s">
+      <c r="Q2" s="72" t="s">
         <v>309</v>
       </c>
-      <c r="Q2" s="72" t="s">
+      <c r="R2" s="72" t="s">
         <v>312</v>
       </c>
-      <c r="R2" s="72" t="s">
+      <c r="S2" s="72" t="s">
         <v>299</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>310</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>313</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="72" t="s">
         <v>84</v>
       </c>
       <c r="B3">
         <v>1.06528940064943</v>
       </c>
-      <c r="I3" s="72" t="s">
+      <c r="D3" s="72">
+        <v>0</v>
+      </c>
+      <c r="J3" s="72" t="s">
         <v>91</v>
       </c>
-      <c r="J3" s="72">
-        <v>0</v>
-      </c>
       <c r="K3" s="72">
         <v>0</v>
       </c>
-      <c r="L3" s="72"/>
-      <c r="O3" s="72"/>
-      <c r="R3" s="72"/>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="L3" s="72">
+        <v>0</v>
+      </c>
+      <c r="M3" s="72"/>
+      <c r="P3" s="72"/>
+      <c r="S3" s="72"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="72" t="s">
         <v>85</v>
       </c>
@@ -5039,30 +5054,33 @@
       <c r="C4">
         <v>1.0366520373714401</v>
       </c>
-      <c r="I4" s="72" t="s">
+      <c r="D4" s="72">
+        <v>1.04159354933772</v>
+      </c>
+      <c r="J4" s="72" t="s">
         <v>92</v>
       </c>
-      <c r="J4" s="72">
+      <c r="K4" s="72">
         <v>-8.6669791486718703E-2</v>
       </c>
-      <c r="K4" s="72">
+      <c r="L4" s="72">
         <v>-9.1290585578995304E-2</v>
       </c>
-      <c r="L4" s="72">
+      <c r="M4" s="72">
         <v>0.13604529735975701</v>
       </c>
-      <c r="M4" s="72">
-        <f>K4-L4</f>
+      <c r="N4" s="72">
+        <f>L4-M4</f>
         <v>-0.22733588293875232</v>
       </c>
-      <c r="N4" s="72">
-        <f>L4+$M$32</f>
+      <c r="O4" s="72">
+        <f>M4+$N$32</f>
         <v>-9.5084673299724309E-2</v>
       </c>
-      <c r="O4" s="72"/>
-      <c r="R4" s="72"/>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="P4" s="72"/>
+      <c r="S4" s="72"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="72" t="s">
         <v>86</v>
       </c>
@@ -5072,30 +5090,34 @@
       <c r="C5">
         <v>1.01080492498633</v>
       </c>
-      <c r="I5" s="72" t="s">
+      <c r="D5" s="72">
+        <v>0.98392576775238405</v>
+      </c>
+      <c r="G5" s="72"/>
+      <c r="J5" s="72" t="s">
         <v>93</v>
       </c>
-      <c r="J5" s="72">
+      <c r="K5" s="72">
         <v>-0.22116211366303701</v>
       </c>
-      <c r="K5" s="72">
+      <c r="L5" s="72">
         <v>-0.235459843805775</v>
       </c>
-      <c r="L5" s="72">
-        <v>0</v>
-      </c>
       <c r="M5" s="72">
-        <f>K5-L5</f>
+        <v>0</v>
+      </c>
+      <c r="N5" s="72">
+        <f>L5-M5</f>
         <v>-0.235459843805775</v>
       </c>
-      <c r="N5" s="72">
-        <f t="shared" ref="N5:N7" si="0">L5+$M$32</f>
+      <c r="O5" s="72">
+        <f>M5+$N$32</f>
         <v>-0.23112997065948132</v>
       </c>
-      <c r="O5" s="72"/>
-      <c r="R5" s="72"/>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="P5" s="72"/>
+      <c r="S5" s="72"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="72" t="s">
         <v>151</v>
       </c>
@@ -5105,43 +5127,47 @@
       <c r="C6">
         <v>1.0237650685834301</v>
       </c>
-      <c r="E6" s="72">
+      <c r="D6" s="72">
+        <v>1.0059403301057199</v>
+      </c>
+      <c r="F6" s="72">
         <v>1.02266696072011</v>
       </c>
-      <c r="I6" s="72" t="s">
+      <c r="G6" s="72"/>
+      <c r="J6" s="72" t="s">
         <v>259</v>
       </c>
-      <c r="J6" s="72">
+      <c r="K6" s="72">
         <v>-0.18108637306068801</v>
       </c>
-      <c r="K6" s="72">
+      <c r="L6" s="72">
         <v>-0.19120119080043499</v>
       </c>
-      <c r="L6" s="72">
+      <c r="M6" s="72">
         <v>4.0056113513174202E-2</v>
       </c>
-      <c r="M6" s="72">
-        <f>K6-L6</f>
+      <c r="N6" s="72">
+        <f>L6-M6</f>
         <v>-0.23125730431360919</v>
       </c>
-      <c r="N6" s="72">
-        <f t="shared" si="0"/>
+      <c r="O6" s="72">
+        <f>M6+$N$32</f>
         <v>-0.19107385714630712</v>
       </c>
-      <c r="O6" s="72"/>
-      <c r="R6" s="72">
+      <c r="P6" s="72"/>
+      <c r="S6" s="72">
         <v>8.7666838686665693E-2</v>
       </c>
-      <c r="S6">
-        <f>K6-R6</f>
+      <c r="T6">
+        <f>L6-S6</f>
         <v>-0.27886802948710065</v>
       </c>
-      <c r="T6">
-        <f>R6+$S$32</f>
+      <c r="U6">
+        <f>S6+$T$32</f>
         <v>-0.19120119080043496</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="72" t="s">
         <v>152</v>
       </c>
@@ -5152,42 +5178,46 @@
         <v>1.02789838928665</v>
       </c>
       <c r="D7" s="72">
+        <v>1.01636472287964</v>
+      </c>
+      <c r="E7" s="72">
         <v>1.0227107597990099</v>
       </c>
-      <c r="I7" s="72" t="s">
+      <c r="G7" s="72"/>
+      <c r="J7" s="72" t="s">
         <v>260</v>
       </c>
-      <c r="J7" s="72">
+      <c r="K7" s="72">
         <v>-0.15459540540712</v>
       </c>
-      <c r="K7" s="72">
+      <c r="L7" s="72">
         <v>-0.163466853701174</v>
       </c>
-      <c r="L7" s="72">
+      <c r="M7" s="72">
         <v>6.69999978786147E-2</v>
       </c>
-      <c r="M7" s="72">
-        <f>K7-L7</f>
+      <c r="N7" s="72">
+        <f>L7-M7</f>
         <v>-0.23046685157978869</v>
       </c>
-      <c r="N7" s="72">
-        <f t="shared" si="0"/>
+      <c r="O7" s="72">
+        <f>M7+$N$32</f>
         <v>-0.16412997278086661</v>
       </c>
-      <c r="O7" s="72">
+      <c r="P7" s="72">
         <v>0.104196486471622</v>
       </c>
-      <c r="P7" s="72">
-        <f>K7-O7</f>
+      <c r="Q7" s="72">
+        <f>L7-P7</f>
         <v>-0.26766334017279603</v>
       </c>
-      <c r="Q7" s="72">
-        <f>O7+$P$32</f>
-        <v>-0.15385036613490921</v>
-      </c>
-      <c r="T7" s="72"/>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="R7" s="72">
+        <f>P7+$Q$32</f>
+        <v>-0.16359851535970299</v>
+      </c>
+      <c r="U7" s="72"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="72" t="s">
         <v>153</v>
       </c>
@@ -5195,299 +5225,322 @@
         <v>1.01563267653981</v>
       </c>
       <c r="D8" s="72">
+        <v>0</v>
+      </c>
+      <c r="E8" s="72">
         <v>1.0391282933224899</v>
       </c>
-      <c r="I8" s="72" t="s">
+      <c r="H8" s="72"/>
+      <c r="J8" s="72" t="s">
         <v>261</v>
       </c>
-      <c r="J8" s="72">
+      <c r="K8" s="72">
         <v>-0.25490550345711999</v>
       </c>
-      <c r="K8" s="72">
+      <c r="L8" s="72">
         <v>-0.267926663489854</v>
       </c>
-      <c r="O8" s="72">
-        <v>0</v>
-      </c>
       <c r="P8" s="72">
-        <f>K8-O8</f>
+        <v>0</v>
+      </c>
+      <c r="Q8" s="72">
+        <f>L8-P8</f>
         <v>-0.267926663489854</v>
       </c>
-      <c r="Q8" s="72">
-        <f>O8+$P$32</f>
-        <v>-0.25804685260653121</v>
-      </c>
-      <c r="T8" s="72"/>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="R8" s="72">
+        <f>P8+$Q$32</f>
+        <v>-0.26779500183132499</v>
+      </c>
+      <c r="U8" s="72"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="72" t="s">
         <v>154</v>
       </c>
       <c r="C9">
         <v>1.0465513528972901</v>
       </c>
-      <c r="E9" s="72">
+      <c r="D9" s="72">
+        <v>1.0141659267677701</v>
+      </c>
+      <c r="F9" s="72">
         <v>1.04697591826057</v>
       </c>
-      <c r="I9" s="72" t="s">
+      <c r="J9" s="72" t="s">
         <v>262</v>
       </c>
-      <c r="J9" s="72">
+      <c r="K9" s="72">
         <v>-0.238124828874305</v>
       </c>
-      <c r="K9" s="72"/>
-      <c r="L9" s="72">
+      <c r="L9" s="72"/>
+      <c r="M9" s="72">
         <v>-1.9000290946371599E-2</v>
       </c>
-      <c r="R9" s="72">
+      <c r="O9" s="72">
+        <f>M9+$N$32</f>
+        <v>-0.25013026160585294</v>
+      </c>
+      <c r="S9" s="72">
         <v>3.0814112406048599E-2</v>
       </c>
-      <c r="T9" s="72">
-        <f t="shared" ref="T7:T16" si="1">R9+$S$32</f>
+      <c r="U9" s="72">
+        <f t="shared" ref="U9:U16" si="0">S9+$T$32</f>
         <v>-0.24805391708105207</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="72" t="s">
         <v>155</v>
       </c>
       <c r="C10">
         <v>1.0875611278507999</v>
       </c>
-      <c r="I10" s="72" t="s">
+      <c r="D10" s="72">
+        <v>1.0540922732031099</v>
+      </c>
+      <c r="J10" s="72" t="s">
         <v>263</v>
       </c>
-      <c r="J10" s="72">
+      <c r="K10" s="72">
         <v>-0.23811416408082101</v>
       </c>
-      <c r="K10" s="72"/>
-      <c r="L10" s="72">
+      <c r="L10" s="72"/>
+      <c r="M10" s="72">
         <v>-1.8255514956707498E-2</v>
       </c>
-      <c r="T10" s="72"/>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="O10" s="72">
+        <f>M10+$N$32</f>
+        <v>-0.24938548561618881</v>
+      </c>
+      <c r="U10" s="72"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="72" t="s">
         <v>156</v>
       </c>
       <c r="C11">
         <v>1.03363463574681</v>
       </c>
-      <c r="E11" s="72">
+      <c r="D11" s="72">
+        <v>0.99423745052268397</v>
+      </c>
+      <c r="F11" s="72">
         <v>1.0353437154263301</v>
       </c>
-      <c r="I11" s="72" t="s">
+      <c r="J11" s="72" t="s">
         <v>71</v>
       </c>
-      <c r="J11" s="72">
+      <c r="K11" s="72">
         <v>-0.26782734160848398</v>
       </c>
-      <c r="K11" s="72"/>
-      <c r="L11" s="72">
+      <c r="L11" s="72"/>
+      <c r="M11" s="72">
         <v>-5.0260940165644002E-2</v>
       </c>
-      <c r="R11" s="72">
-        <v>0</v>
-      </c>
-      <c r="T11" s="72">
-        <f t="shared" si="1"/>
+      <c r="O11" s="72">
+        <f>M11+$N$32</f>
+        <v>-0.28139091082512535</v>
+      </c>
+      <c r="S11" s="72">
+        <v>0</v>
+      </c>
+      <c r="U11" s="72">
+        <f t="shared" si="0"/>
         <v>-0.27886802948710065</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="72" t="s">
         <v>157</v>
       </c>
       <c r="D12" s="72">
+        <v>0</v>
+      </c>
+      <c r="E12" s="72">
         <v>1.0279410767585999</v>
       </c>
-      <c r="E12" s="72">
+      <c r="F12" s="72">
         <v>1.02791715563223</v>
       </c>
-      <c r="I12" s="72" t="s">
+      <c r="J12" s="72" t="s">
         <v>264</v>
       </c>
-      <c r="J12" s="72">
+      <c r="K12" s="72">
         <v>-0.27082639634655098</v>
       </c>
-      <c r="K12" s="72"/>
       <c r="L12" s="72"/>
-      <c r="O12" s="72">
+      <c r="M12" s="72"/>
+      <c r="P12" s="72">
         <v>-1.6600304727115101E-2</v>
       </c>
-      <c r="P12" s="72">
-        <f>J12-O12</f>
-        <v>-0.25422609161943588</v>
-      </c>
-      <c r="Q12" s="72">
-        <f t="shared" ref="Q8:Q16" si="2">O12+$P$32</f>
-        <v>-0.27464715733364631</v>
-      </c>
       <c r="R12" s="72">
+        <f t="shared" ref="R12:R16" si="1">P12+$Q$32</f>
+        <v>-0.28439530655844009</v>
+      </c>
+      <c r="S12" s="72">
         <v>-2.9904912760974301E-3</v>
       </c>
-      <c r="T12" s="72">
-        <f t="shared" si="1"/>
+      <c r="U12" s="72">
+        <f t="shared" si="0"/>
         <v>-0.28185852076319806</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="72" t="s">
         <v>158</v>
       </c>
       <c r="D13" s="72">
+        <v>0</v>
+      </c>
+      <c r="E13" s="72">
         <v>1.02984990508254</v>
       </c>
-      <c r="E13" s="72">
+      <c r="F13" s="72">
         <v>1.0293026657978499</v>
       </c>
-      <c r="I13" s="72" t="s">
+      <c r="J13" s="72" t="s">
         <v>265</v>
       </c>
-      <c r="J13" s="72">
+      <c r="K13" s="72">
         <v>-0.26537530725671299</v>
       </c>
-      <c r="K13" s="72"/>
       <c r="L13" s="72"/>
-      <c r="O13" s="72">
+      <c r="M13" s="72"/>
+      <c r="P13" s="72">
         <v>-1.0947560823407299E-2</v>
       </c>
-      <c r="P13" s="72">
-        <f t="shared" ref="P13:P16" si="3">J13-O13</f>
-        <v>-0.25442774643330568</v>
-      </c>
-      <c r="Q13" s="72">
-        <f t="shared" si="2"/>
-        <v>-0.26899441342993852</v>
-      </c>
       <c r="R13" s="72">
+        <f t="shared" si="1"/>
+        <v>-0.2787425626547323</v>
+      </c>
+      <c r="S13" s="72">
         <v>2.8179192054674602E-3</v>
       </c>
-      <c r="T13" s="72">
-        <f t="shared" si="1"/>
+      <c r="U13" s="72">
+        <f t="shared" si="0"/>
         <v>-0.27605011028163318</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="72" t="s">
         <v>159</v>
       </c>
       <c r="D14" s="72">
+        <v>0</v>
+      </c>
+      <c r="E14" s="72">
         <v>1.02406093645796</v>
       </c>
-      <c r="I14" s="72" t="s">
+      <c r="J14" s="72" t="s">
         <v>266</v>
       </c>
-      <c r="J14" s="72">
+      <c r="K14" s="72">
         <v>-0.27056740976696902</v>
       </c>
-      <c r="K14" s="72"/>
       <c r="L14" s="72"/>
-      <c r="O14" s="72">
+      <c r="M14" s="72"/>
+      <c r="P14" s="72">
         <v>-1.6267059612644099E-2</v>
       </c>
-      <c r="P14" s="72">
-        <f t="shared" si="3"/>
-        <v>-0.25430035015432495</v>
-      </c>
-      <c r="Q14" s="72">
-        <f t="shared" si="2"/>
-        <v>-0.27431391221917528</v>
-      </c>
-      <c r="T14" s="72"/>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="R14" s="72">
+        <f t="shared" si="1"/>
+        <v>-0.28406206144396906</v>
+      </c>
+      <c r="U14" s="72"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="72" t="s">
         <v>160</v>
       </c>
       <c r="D15" s="72">
+        <v>0</v>
+      </c>
+      <c r="E15" s="72">
         <v>1.0198149779104799</v>
       </c>
-      <c r="E15" s="72">
+      <c r="F15" s="72">
         <v>1.0182381308847801</v>
       </c>
-      <c r="I15" s="72" t="s">
+      <c r="J15" s="72" t="s">
         <v>267</v>
       </c>
-      <c r="J15" s="72">
+      <c r="K15" s="72">
         <v>-0.272193451087546</v>
       </c>
-      <c r="K15" s="72"/>
       <c r="L15" s="72"/>
-      <c r="O15" s="72">
+      <c r="M15" s="72"/>
+      <c r="P15" s="72">
         <v>-1.7998913484384298E-2</v>
       </c>
-      <c r="P15" s="72">
-        <f t="shared" si="3"/>
-        <v>-0.25419453760316169</v>
-      </c>
-      <c r="Q15" s="72">
-        <f t="shared" si="2"/>
-        <v>-0.27604576609091552</v>
-      </c>
       <c r="R15" s="72">
+        <f t="shared" si="1"/>
+        <v>-0.2857939153157093</v>
+      </c>
+      <c r="S15" s="72">
         <v>-3.7762002123430498E-3</v>
       </c>
-      <c r="T15" s="72">
-        <f t="shared" si="1"/>
+      <c r="U15" s="72">
+        <f t="shared" si="0"/>
         <v>-0.28264422969944369</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="72" t="s">
         <v>161</v>
       </c>
       <c r="D16" s="72">
+        <v>0</v>
+      </c>
+      <c r="E16" s="72">
         <v>1.0087683120630799</v>
       </c>
-      <c r="E16" s="72">
+      <c r="F16" s="72">
         <v>1.0090207852464499</v>
       </c>
-      <c r="I16" s="72" t="s">
+      <c r="J16" s="72" t="s">
         <v>268</v>
       </c>
-      <c r="J16" s="72">
+      <c r="K16" s="72">
         <v>-0.28803193308711</v>
       </c>
-      <c r="K16" s="72"/>
       <c r="L16" s="72"/>
-      <c r="O16" s="72">
+      <c r="M16" s="72"/>
+      <c r="P16" s="72">
         <v>-3.4442694314269398E-2</v>
       </c>
-      <c r="P16" s="72">
-        <f t="shared" si="3"/>
-        <v>-0.25358923877284062</v>
-      </c>
-      <c r="Q16" s="72">
-        <f t="shared" si="2"/>
-        <v>-0.29248954692080059</v>
-      </c>
       <c r="R16" s="72">
+        <f t="shared" si="1"/>
+        <v>-0.30223769614559437</v>
+      </c>
+      <c r="S16" s="72">
         <v>-2.0422237393388699E-2</v>
       </c>
-      <c r="T16" s="72">
-        <f t="shared" si="1"/>
+      <c r="U16" s="72">
+        <f t="shared" si="0"/>
         <v>-0.29929026688048938</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="72" t="s">
         <v>87</v>
       </c>
-      <c r="I17" s="72" t="s">
+      <c r="D17" s="72">
+        <v>0</v>
+      </c>
+      <c r="J17" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="J17" s="72">
+      <c r="K17" s="72">
         <v>1.06021182972759</v>
       </c>
-      <c r="K17" s="72">
+      <c r="L17" s="72">
         <v>1.06528940064943</v>
       </c>
-      <c r="L17" s="72"/>
-      <c r="O17" s="72"/>
-      <c r="R17" s="72"/>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="M17" s="72"/>
+      <c r="P17" s="72"/>
+      <c r="S17" s="72"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="72" t="s">
         <v>88</v>
       </c>
@@ -5497,44 +5550,59 @@
       <c r="C18">
         <v>0.14190821118581601</v>
       </c>
-      <c r="I18" s="72" t="s">
+      <c r="D18" s="72">
+        <v>-9.9339141159860006E-2</v>
+      </c>
+      <c r="G18" s="72"/>
+      <c r="J18" s="72" t="s">
         <v>28</v>
       </c>
-      <c r="J18" s="72">
+      <c r="K18" s="72">
         <v>1.04521069537303</v>
       </c>
-      <c r="K18" s="72">
+      <c r="L18" s="72">
         <v>1.05041513434258</v>
       </c>
-      <c r="L18" s="72">
+      <c r="M18" s="72">
         <v>1.04631992573415</v>
       </c>
-      <c r="O18" s="72"/>
-      <c r="R18" s="72"/>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="O18" s="72">
+        <v>1.04631992573415</v>
+      </c>
+      <c r="P18" s="72"/>
+      <c r="S18" s="72"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="72" t="s">
         <v>89</v>
       </c>
       <c r="B19">
         <v>-0.23799618884858001</v>
       </c>
-      <c r="I19" s="72" t="s">
+      <c r="C19" s="72"/>
+      <c r="D19" s="72">
+        <v>-0.23155275841479001</v>
+      </c>
+      <c r="G19" s="72"/>
+      <c r="J19" s="72" t="s">
         <v>94</v>
       </c>
-      <c r="J19" s="72">
+      <c r="K19" s="72">
         <v>1.0102223344885899</v>
       </c>
-      <c r="K19" s="72">
+      <c r="L19" s="72">
         <v>1.0201724031637001</v>
       </c>
-      <c r="L19" s="72">
+      <c r="M19" s="72">
         <v>1.01080492498633</v>
       </c>
-      <c r="O19" s="72"/>
-      <c r="R19" s="72"/>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="O19" s="72">
+        <v>1.01080492498633</v>
+      </c>
+      <c r="P19" s="72"/>
+      <c r="S19" s="72"/>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="72" t="s">
         <v>162</v>
       </c>
@@ -5544,27 +5612,34 @@
       <c r="C20">
         <v>4.1029996249025397E-2</v>
       </c>
-      <c r="E20" s="72">
+      <c r="D20" s="72">
+        <v>-0.19458270352378901</v>
+      </c>
+      <c r="F20" s="72">
         <v>8.9884365546254993E-2</v>
       </c>
-      <c r="I20" s="72" t="s">
+      <c r="G20" s="72"/>
+      <c r="J20" s="72" t="s">
         <v>231</v>
       </c>
-      <c r="J20" s="72">
+      <c r="K20" s="72">
         <v>1.0238916772678499</v>
       </c>
-      <c r="K20" s="72">
+      <c r="L20" s="72">
         <v>1.0333275387088099</v>
       </c>
-      <c r="L20" s="72">
+      <c r="M20" s="72">
         <v>1.0245869295690999</v>
       </c>
-      <c r="O20" s="72"/>
-      <c r="R20" s="72">
+      <c r="O20" s="72">
+        <v>1.0245869295690999</v>
+      </c>
+      <c r="P20" s="72"/>
+      <c r="S20" s="72">
         <v>1.0266094251068201</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="72" t="s">
         <v>163</v>
       </c>
@@ -5575,240 +5650,286 @@
         <v>6.8972426535251805E-2</v>
       </c>
       <c r="D21" s="72">
+        <v>-0.16833016487261601</v>
+      </c>
+      <c r="E21" s="72">
         <v>0.106950197760304</v>
       </c>
-      <c r="I21" s="72" t="s">
+      <c r="G21" s="72"/>
+      <c r="J21" s="72" t="s">
         <v>210</v>
       </c>
-      <c r="J21" s="72">
+      <c r="K21" s="72">
         <v>1.02827099057284</v>
       </c>
-      <c r="K21" s="72">
+      <c r="L21" s="72">
         <v>1.03570004302515</v>
       </c>
-      <c r="L21" s="72">
+      <c r="M21" s="72">
         <v>1.0302098302386</v>
       </c>
       <c r="O21" s="72">
+        <v>1.0302098302386</v>
+      </c>
+      <c r="P21" s="72">
         <v>1.0282877238446599</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="72" t="s">
         <v>164</v>
       </c>
       <c r="B22">
         <v>-0.27881886491819902</v>
       </c>
-      <c r="I22" s="72" t="s">
+      <c r="D22" s="72">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="J22" s="72" t="s">
         <v>240</v>
       </c>
-      <c r="J22" s="72">
+      <c r="K22" s="72">
         <v>1.0384892284060301</v>
       </c>
-      <c r="K22" s="72">
+      <c r="L22" s="72">
         <v>1.0532092351900899</v>
       </c>
-      <c r="O22" s="72">
+      <c r="P22" s="72">
         <v>1.0391282933224899</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="72" t="s">
         <v>165</v>
       </c>
       <c r="C23">
         <v>-1.98871734161255E-2</v>
       </c>
-      <c r="E23" s="72">
+      <c r="D23" s="72">
+        <v>-0.25909980104373398</v>
+      </c>
+      <c r="F23" s="72">
         <v>3.2271848420798298E-2</v>
       </c>
-      <c r="I23" s="72" t="s">
+      <c r="J23" s="72" t="s">
         <v>232</v>
       </c>
-      <c r="J23" s="72">
+      <c r="K23" s="72">
         <v>1.0461591070376699</v>
       </c>
-      <c r="K23" s="72"/>
-      <c r="L23" s="72">
+      <c r="L23" s="72"/>
+      <c r="M23" s="72">
         <v>1.0467402896218501</v>
       </c>
-      <c r="R23" s="72">
+      <c r="O23" s="72">
+        <v>1.0467402896218501</v>
+      </c>
+      <c r="S23" s="72">
         <v>1.0474731717891701</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="72" t="s">
         <v>166</v>
       </c>
       <c r="C24">
         <v>-1.9856194268582199E-2</v>
       </c>
-      <c r="I24" s="72" t="s">
+      <c r="D24" s="72">
+        <v>-0.268464066192176</v>
+      </c>
+      <c r="J24" s="72" t="s">
         <v>211</v>
       </c>
-      <c r="J24" s="72">
+      <c r="K24" s="72">
         <v>1.08522332015065</v>
       </c>
-      <c r="K24" s="72"/>
-      <c r="L24" s="72">
+      <c r="L24" s="72"/>
+      <c r="M24" s="72">
         <v>1.0877423754101601</v>
       </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="O24" s="72">
+        <v>1.0877423754101601</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="72" t="s">
         <v>167</v>
       </c>
       <c r="C25">
         <v>-5.1995238756297503E-2</v>
       </c>
-      <c r="I25" s="72" t="s">
+      <c r="D25" s="72">
+        <v>-0.287395123561481</v>
+      </c>
+      <c r="J25" s="72" t="s">
         <v>215</v>
       </c>
-      <c r="J25" s="72">
+      <c r="K25" s="72">
         <v>1.0346562939178801</v>
       </c>
-      <c r="K25" s="72"/>
-      <c r="L25" s="72">
+      <c r="L25" s="72"/>
+      <c r="M25" s="72">
         <v>1.03494157567892</v>
       </c>
-      <c r="R25" s="72">
+      <c r="O25" s="72">
+        <v>1.03494157567892</v>
+      </c>
+      <c r="S25" s="72">
         <v>1.0353437154263301</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="72" t="s">
         <v>168</v>
       </c>
       <c r="D26" s="72">
+        <v>0</v>
+      </c>
+      <c r="E26" s="72">
         <v>-1.7065702743745501E-2</v>
       </c>
-      <c r="E26" s="72">
+      <c r="F26" s="72">
         <v>-3.0739864500671501E-3</v>
       </c>
-      <c r="I26" s="72" t="s">
+      <c r="J26" s="72" t="s">
         <v>214</v>
       </c>
-      <c r="J26" s="72">
+      <c r="K26" s="72">
         <v>1.0276736347300599</v>
       </c>
-      <c r="K26" s="72"/>
       <c r="L26" s="72"/>
-      <c r="O26" s="72">
+      <c r="M26" s="72"/>
+      <c r="P26" s="72">
         <v>1.02808272794449</v>
       </c>
-      <c r="R26" s="72">
+      <c r="S26" s="72">
         <v>1.02792175200049</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="72" t="s">
         <v>169</v>
       </c>
       <c r="D27" s="72">
+        <v>0</v>
+      </c>
+      <c r="E27" s="72">
         <v>-1.1274794903099E-2</v>
       </c>
-      <c r="E27" s="72">
+      <c r="F27" s="72">
         <v>2.9004994274963E-3</v>
       </c>
-      <c r="I27" s="72" t="s">
+      <c r="J27" s="72" t="s">
         <v>241</v>
       </c>
-      <c r="J27" s="72">
+      <c r="K27" s="72">
         <v>1.0294797148790999</v>
       </c>
-      <c r="K27" s="72"/>
       <c r="L27" s="72"/>
-      <c r="O27" s="72">
+      <c r="M27" s="72"/>
+      <c r="P27" s="72">
         <v>1.02991162145042</v>
       </c>
-      <c r="R27" s="72">
+      <c r="S27" s="72">
         <v>1.02930675248708</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="72" t="s">
         <v>170</v>
       </c>
       <c r="D28" s="72">
+        <v>0</v>
+      </c>
+      <c r="E28" s="72">
         <v>-1.6659929827751802E-2</v>
       </c>
-      <c r="I28" s="72" t="s">
+      <c r="J28" s="72" t="s">
         <v>212</v>
       </c>
-      <c r="J28" s="72">
+      <c r="K28" s="72">
         <v>1.0240118665753799</v>
       </c>
-      <c r="K28" s="72"/>
       <c r="L28" s="72"/>
-      <c r="O28" s="72">
+      <c r="M28" s="72"/>
+      <c r="P28" s="72">
         <v>1.02419644348192</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="72" t="s">
         <v>171</v>
       </c>
       <c r="D29" s="72">
+        <v>0</v>
+      </c>
+      <c r="E29" s="72">
         <v>-1.83575439757129E-2</v>
       </c>
-      <c r="E29" s="72">
+      <c r="F29" s="72">
         <v>-3.8450893226716801E-3</v>
       </c>
-      <c r="I29" s="72" t="s">
+      <c r="J29" s="72" t="s">
         <v>213</v>
       </c>
-      <c r="J29" s="72">
+      <c r="K29" s="72">
         <v>1.0198403758847501</v>
       </c>
-      <c r="K29" s="72"/>
       <c r="L29" s="72"/>
-      <c r="O29" s="72">
+      <c r="M29" s="72"/>
+      <c r="P29" s="72">
         <v>1.0199801902936001</v>
       </c>
-      <c r="R29" s="72">
+      <c r="S29" s="72">
         <v>1.01824539080697</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="72" t="s">
         <v>172</v>
       </c>
       <c r="D30" s="72">
+        <v>0</v>
+      </c>
+      <c r="E30" s="72">
         <v>-3.4758444331587403E-2</v>
       </c>
-      <c r="E30" s="72">
+      <c r="F30" s="72">
         <v>-2.0609327252956802E-2</v>
       </c>
-      <c r="I30" s="72" t="s">
+      <c r="J30" s="72" t="s">
         <v>248</v>
       </c>
-      <c r="J30" s="72">
+      <c r="K30" s="72">
         <v>1.0096275188231001</v>
       </c>
-      <c r="K30" s="72"/>
       <c r="L30" s="72"/>
-      <c r="O30" s="72">
+      <c r="M30" s="72"/>
+      <c r="P30" s="72">
         <v>1.0093669584818701</v>
       </c>
-      <c r="R30" s="72">
+      <c r="S30" s="72">
         <v>1.0092312368477301</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="L32" t="s">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="M32" t="s">
         <v>307</v>
       </c>
-      <c r="M32" s="72">
-        <f>AVERAGE(M4:M7)</f>
+      <c r="N32" s="72">
+        <f>AVERAGE(N4:N7)</f>
         <v>-0.23112997065948132</v>
       </c>
-      <c r="P32" s="72">
-        <f>AVERAGE(P7:P16)</f>
-        <v>-0.25804685260653121</v>
-      </c>
-      <c r="S32">
-        <f>S6</f>
+      <c r="Q32" s="72">
+        <f>AVERAGE(Q7:Q16)</f>
+        <v>-0.26779500183132499</v>
+      </c>
+      <c r="T32">
+        <f>T6</f>
         <v>-0.27886802948710065</v>
       </c>
     </row>
@@ -5832,12 +5953,18 @@
         <v>304</v>
       </c>
     </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>315</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="I1:R1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="J1:S1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Fixed the slack bus shift issue and how c_k is calculated.
It seems that the 14 bus ADMM code almost works now. There are a few
minor issues with Areas 2-4 (especially Area 4 - see .xls), because
central - x4_k is sort of large, around 1e-3 vs 1e-5 for the other
areas. Also, the normres_r is still nonzero, although it does get
smaller. I need to take a closer look at how normres_r and normres_s are
calculated.
</commit_message>
<xml_diff>
--- a/DMASE - Test Results.xlsx
+++ b/DMASE - Test Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12240" windowHeight="9240" firstSheet="2" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12240" windowHeight="9240" firstSheet="2" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="2 Bus" sheetId="4" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="301">
   <si>
     <t>Abur 3-Bus Case Measurements (run through SE, rerun new estimate again)</t>
   </si>
@@ -925,6 +925,9 @@
   </si>
   <si>
     <t>delta Area 1 - Area 2</t>
+  </si>
+  <si>
+    <t>ADMM AC h</t>
   </si>
 </sst>
 </file>
@@ -1209,7 +1212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1398,6 +1401,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1419,14 +1432,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1749,15 +1761,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="91" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="87"/>
-      <c r="G1" s="87"/>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
+      <c r="G1" s="91"/>
       <c r="I1" s="6" t="s">
         <v>1</v>
       </c>
@@ -2009,26 +2021,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" s="72" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="98" t="s">
         <v>276</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="J1" s="94" t="s">
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
+      <c r="J1" s="98" t="s">
         <v>276</v>
       </c>
-      <c r="K1" s="94"/>
-      <c r="L1" s="94"/>
-      <c r="M1" s="94"/>
-      <c r="N1" s="94"/>
-      <c r="O1" s="94"/>
-      <c r="P1" s="94"/>
-      <c r="Q1" s="94"/>
-      <c r="R1" s="94"/>
-      <c r="S1" s="94"/>
+      <c r="K1" s="98"/>
+      <c r="L1" s="98"/>
+      <c r="M1" s="98"/>
+      <c r="N1" s="98"/>
+      <c r="O1" s="98"/>
+      <c r="P1" s="98"/>
+      <c r="Q1" s="98"/>
+      <c r="R1" s="98"/>
+      <c r="S1" s="98"/>
       <c r="V1" s="72" t="s">
         <v>281</v>
       </c>
@@ -3044,10 +3056,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S146"/>
+  <dimension ref="A1:S147"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3055,29 +3067,30 @@
     <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" style="72" customWidth="1"/>
-    <col min="6" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" style="72" customWidth="1"/>
     <col min="12" max="12" width="12.7109375" customWidth="1"/>
     <col min="13" max="13" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="89" t="s">
+      <c r="A1" s="93" t="s">
         <v>221</v>
       </c>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="89"/>
-      <c r="F1" s="89"/>
-      <c r="G1" s="89"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="89"/>
-      <c r="J1" s="89"/>
-      <c r="K1" s="89"/>
+      <c r="B1" s="93"/>
+      <c r="C1" s="93"/>
+      <c r="D1" s="93"/>
+      <c r="E1" s="93"/>
+      <c r="F1" s="93"/>
+      <c r="G1" s="93"/>
+      <c r="H1" s="93"/>
+      <c r="I1" s="93"/>
+      <c r="J1" s="93"/>
+      <c r="K1" s="88"/>
       <c r="L1" s="43"/>
       <c r="M1" s="60"/>
       <c r="N1" s="11" t="s">
@@ -3101,19 +3114,19 @@
       <c r="B2" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="90" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90" t="s">
+      <c r="C2" s="94" t="s">
+        <v>300</v>
+      </c>
+      <c r="D2" s="94"/>
+      <c r="E2" s="94"/>
+      <c r="F2" s="94"/>
+      <c r="G2" s="94"/>
+      <c r="H2" s="94" t="s">
         <v>74</v>
       </c>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
-      <c r="K2" s="90"/>
+      <c r="I2" s="94"/>
+      <c r="J2" s="94"/>
+      <c r="K2" s="4"/>
       <c r="L2" s="4"/>
       <c r="M2" s="60" t="s">
         <v>138</v>
@@ -3142,41 +3155,40 @@
       <c r="D3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="10"/>
+      <c r="E3" s="10" t="s">
+        <v>42</v>
+      </c>
       <c r="F3" s="10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>43</v>
+        <v>10</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="K3" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="L3" s="4"/>
-      <c r="M3" s="60" t="s">
+      <c r="K3" s="4"/>
+      <c r="L3" s="60" t="s">
         <v>173</v>
       </c>
-      <c r="N3" s="46" t="s">
+      <c r="M3" s="46" t="s">
         <v>116</v>
       </c>
-      <c r="O3" s="50">
+      <c r="N3" s="50">
         <v>-20.300935880694301</v>
       </c>
-      <c r="P3" s="1">
-        <f t="shared" ref="P3:P9" si="0">O3/100</f>
+      <c r="O3" s="1">
+        <f t="shared" ref="O3:O9" si="0">N3/100</f>
         <v>-0.20300935880694301</v>
       </c>
-      <c r="Q3" s="58"/>
-      <c r="S3" s="2" t="s">
+      <c r="P3" s="58"/>
+      <c r="R3" s="2" t="s">
         <v>136</v>
       </c>
     </row>
@@ -3188,33 +3200,31 @@
         <v>1.05999768165375</v>
       </c>
       <c r="C4" s="72">
-        <v>1.0596099876699601</v>
+        <v>1.0599997511008601</v>
       </c>
       <c r="D4" s="1"/>
-      <c r="E4" s="72">
-        <v>0</v>
-      </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1">
+      <c r="E4"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1">
         <f>B4-C4</f>
-        <v>3.8769398378990516E-4</v>
-      </c>
+        <v>-2.0694471101201373E-6</v>
+      </c>
+      <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="60"/>
-      <c r="N4" s="46" t="s">
+      <c r="K4" s="89"/>
+      <c r="L4" s="60"/>
+      <c r="M4" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="O4" s="50">
+      <c r="N4" s="50">
         <v>75.916881283268793</v>
       </c>
-      <c r="P4" s="1">
+      <c r="O4" s="1">
         <f t="shared" si="0"/>
         <v>0.75916881283268789</v>
       </c>
-      <c r="Q4" s="58"/>
+      <c r="P4" s="58"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -3224,38 +3234,36 @@
         <v>1.0410720611633699</v>
       </c>
       <c r="C5" s="72">
-        <v>1.040680470326</v>
-      </c>
-      <c r="D5" s="86">
-        <v>1.01075701619514</v>
-      </c>
-      <c r="E5" s="72">
-        <v>1.04159354933772</v>
-      </c>
-      <c r="G5" s="1"/>
+        <v>1.0410737422161001</v>
+      </c>
+      <c r="D5" s="89">
+        <v>1.04107313245226</v>
+      </c>
+      <c r="E5"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="89">
+        <f t="shared" ref="G5:G23" si="1">B5-C5</f>
+        <v>-1.6810527301291955E-6</v>
+      </c>
       <c r="H5" s="1">
-        <f t="shared" ref="H5:H9" si="1">B5-C5</f>
-        <v>3.9159083736994837E-4</v>
-      </c>
-      <c r="I5" s="1">
-        <f t="shared" ref="I5:I8" si="2">B5-D5</f>
-        <v>3.0315044968229898E-2</v>
-      </c>
+        <f>B5-D5</f>
+        <v>-1.0712888900421547E-6</v>
+      </c>
+      <c r="I5" s="1"/>
       <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="60"/>
-      <c r="N5" s="46" t="s">
+      <c r="K5" s="89"/>
+      <c r="L5" s="60"/>
+      <c r="M5" s="46" t="s">
         <v>117</v>
       </c>
-      <c r="O5" s="50">
+      <c r="N5" s="50">
         <v>-0.155506560051652</v>
       </c>
-      <c r="P5" s="1">
+      <c r="O5" s="1">
         <f t="shared" si="0"/>
         <v>-1.55506560051652E-3</v>
       </c>
-      <c r="Q5" s="58"/>
+      <c r="P5" s="58"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -3265,35 +3273,36 @@
         <v>0.98537777124357495</v>
       </c>
       <c r="C6" s="72">
-        <v>0.98496964587221503</v>
-      </c>
-      <c r="D6" s="86">
-        <v>1.0147683638791001</v>
-      </c>
-      <c r="E6" s="72">
-        <v>0.98392576775238405</v>
-      </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1">
-        <f t="shared" si="2"/>
-        <v>-2.9390592635525126E-2</v>
-      </c>
+        <v>0.98538136281301902</v>
+      </c>
+      <c r="D6" s="89">
+        <v>0.98537952175389198</v>
+      </c>
+      <c r="E6"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="89">
+        <f t="shared" si="1"/>
+        <v>-3.5915694440724621E-6</v>
+      </c>
+      <c r="H6" s="89">
+        <f t="shared" ref="H6:H26" si="2">B6-D6</f>
+        <v>-1.750510317033438E-6</v>
+      </c>
+      <c r="I6" s="1"/>
       <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="60"/>
-      <c r="N6" s="46" t="s">
+      <c r="K6" s="89"/>
+      <c r="L6" s="60"/>
+      <c r="M6" s="46" t="s">
         <v>48</v>
       </c>
-      <c r="O6" s="50">
+      <c r="N6" s="50">
         <v>41.338725991097199</v>
       </c>
-      <c r="P6" s="1">
+      <c r="O6" s="1">
         <f t="shared" si="0"/>
         <v>0.41338725991097197</v>
       </c>
-      <c r="Q6" s="58"/>
+      <c r="P6" s="58"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -3303,38 +3312,41 @@
         <v>1.00695008061588</v>
       </c>
       <c r="C7" s="72">
-        <v>1.00655458784489</v>
-      </c>
-      <c r="D7" s="86">
-        <v>0.99778459206162395</v>
-      </c>
-      <c r="E7" s="72">
-        <v>1.0059403301057199</v>
-      </c>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1">
+        <v>1.0069537044419401</v>
+      </c>
+      <c r="D7" s="89">
+        <v>1.00695177443619</v>
+      </c>
+      <c r="E7"/>
+      <c r="F7" s="89">
+        <v>1.00996354489964</v>
+      </c>
+      <c r="G7" s="89">
         <f t="shared" si="1"/>
-        <v>3.9549277098993585E-4</v>
-      </c>
-      <c r="I7" s="1">
+        <v>-3.6238260601173522E-6</v>
+      </c>
+      <c r="H7" s="89">
         <f t="shared" si="2"/>
-        <v>9.1654885542560294E-3</v>
-      </c>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="60"/>
-      <c r="N7" s="46" t="s">
+        <v>-1.693820310011418E-6</v>
+      </c>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1">
+        <f>B7-F7</f>
+        <v>-3.0134642837600367E-3</v>
+      </c>
+      <c r="K7" s="89"/>
+      <c r="L7" s="60"/>
+      <c r="M7" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="O7" s="50">
+      <c r="N7" s="50">
         <v>-3.8398609004379098</v>
       </c>
-      <c r="P7" s="1">
+      <c r="O7" s="1">
         <f t="shared" si="0"/>
         <v>-3.8398609004379101E-2</v>
       </c>
-      <c r="Q7" s="58"/>
+      <c r="P7" s="58"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -3344,38 +3356,40 @@
         <v>1.01581292033021</v>
       </c>
       <c r="C8" s="72">
-        <v>1.0154201531468201</v>
-      </c>
-      <c r="D8" s="86">
-        <v>1.00482662710487</v>
+        <v>1.0158162823742001</v>
+      </c>
+      <c r="D8" s="89">
+        <v>1.01581467096329</v>
       </c>
       <c r="E8" s="72">
-        <v>1.01636472287964</v>
-      </c>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1">
+        <v>1.0158028020538401</v>
+      </c>
+      <c r="G8" s="89">
         <f t="shared" si="1"/>
-        <v>3.9276718338987493E-4</v>
+        <v>-3.3620439900960974E-6</v>
+      </c>
+      <c r="H8" s="89">
+        <f t="shared" si="2"/>
+        <v>-1.7506330800554082E-6</v>
       </c>
       <c r="I8" s="1">
-        <f t="shared" si="2"/>
-        <v>1.0986293225339949E-2</v>
-      </c>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="60"/>
-      <c r="N8" s="46" t="s">
+        <f>B8-E8</f>
+        <v>1.0118276369874835E-5</v>
+      </c>
+      <c r="J8" s="89"/>
+      <c r="K8" s="89"/>
+      <c r="L8" s="60"/>
+      <c r="M8" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="O8" s="50">
+      <c r="N8" s="50">
         <v>232.35762119293199</v>
       </c>
-      <c r="P8" s="1">
+      <c r="O8" s="1">
         <f t="shared" si="0"/>
         <v>2.32357621192932</v>
       </c>
-      <c r="Q8" s="58"/>
+      <c r="P8" s="58"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -3385,36 +3399,34 @@
         <v>1.0049243733889699</v>
       </c>
       <c r="C9" s="72">
-        <v>1.00453299329137</v>
-      </c>
-      <c r="E9" s="72">
-        <v>0</v>
-      </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1">
+        <v>1.00492888606756</v>
+      </c>
+      <c r="E9" s="89">
+        <v>1.00492719711304</v>
+      </c>
+      <c r="G9" s="89">
         <f t="shared" si="1"/>
-        <v>3.9138009759986936E-4</v>
-      </c>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1">
-        <f>B9-F9</f>
-        <v>1.0049243733889699</v>
-      </c>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="60"/>
-      <c r="N9" s="46" t="s">
+        <v>-4.5126785901405952E-6</v>
+      </c>
+      <c r="H9" s="89"/>
+      <c r="I9" s="89">
+        <f t="shared" ref="I9:I31" si="3">B9-E9</f>
+        <v>-2.8237240701223243E-6</v>
+      </c>
+      <c r="J9" s="89"/>
+      <c r="K9" s="89"/>
+      <c r="L9" s="60"/>
+      <c r="M9" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="O9" s="50">
+      <c r="N9" s="50">
         <v>-20.456442236900301</v>
       </c>
-      <c r="P9" s="1">
+      <c r="O9" s="1">
         <f t="shared" si="0"/>
         <v>-0.20456442236900302</v>
       </c>
-      <c r="Q9" s="58"/>
+      <c r="P9" s="58"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -3424,34 +3436,36 @@
         <v>1.01654592268694</v>
       </c>
       <c r="D10" s="72">
-        <v>0.99772698571068097</v>
-      </c>
-      <c r="E10" s="72">
-        <v>1.0141659267677701</v>
-      </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1">
-        <f>B10-D25</f>
-        <v>1.315675948146771</v>
-      </c>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="60" t="s">
+        <v>1.0165481591655401</v>
+      </c>
+      <c r="F10" s="72">
+        <v>1.0177118977556301</v>
+      </c>
+      <c r="G10" s="89"/>
+      <c r="H10" s="89">
+        <f t="shared" si="2"/>
+        <v>-2.236478600092795E-6</v>
+      </c>
+      <c r="I10" s="89"/>
+      <c r="J10" s="89">
+        <f t="shared" ref="J8:J31" si="4">B10-F10</f>
+        <v>-1.1659750686900949E-3</v>
+      </c>
+      <c r="K10" s="89"/>
+      <c r="L10" s="60" t="s">
         <v>139</v>
       </c>
-      <c r="N10" s="46" t="s">
+      <c r="M10" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="O10" s="50">
+      <c r="N10" s="50">
         <v>-23.569740833506799</v>
       </c>
-      <c r="P10" s="1">
-        <f>O10/100</f>
+      <c r="O10" s="1">
+        <f>N10/100</f>
         <v>-0.235697408335068</v>
       </c>
-      <c r="Q10" s="58"/>
+      <c r="P10" s="58"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -3461,34 +3475,30 @@
         <v>1.0544057013008099</v>
       </c>
       <c r="D11" s="72">
-        <v>1.02907233816918</v>
-      </c>
-      <c r="E11" s="72">
-        <v>1.0540922732031099</v>
-      </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1" t="e">
-        <f>B11-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="60" t="s">
+        <v>1.05440764654987</v>
+      </c>
+      <c r="G11" s="89"/>
+      <c r="H11" s="89">
+        <f t="shared" si="2"/>
+        <v>-1.9452490600535555E-6</v>
+      </c>
+      <c r="I11" s="89"/>
+      <c r="J11" s="89"/>
+      <c r="K11" s="89"/>
+      <c r="L11" s="60" t="s">
         <v>174</v>
       </c>
-      <c r="N11" s="46" t="s">
+      <c r="M11" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="O11" s="50">
+      <c r="N11" s="50">
         <v>0.96859150246414105</v>
       </c>
-      <c r="P11" s="1">
-        <f t="shared" ref="P11:P15" si="3">O11/100</f>
+      <c r="O11" s="1">
+        <f t="shared" ref="O11:O15" si="5">N11/100</f>
         <v>9.6859150246414102E-3</v>
       </c>
-      <c r="Q11" s="58"/>
+      <c r="P11" s="58"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -3498,35 +3508,34 @@
         <v>0.99794960680741096</v>
       </c>
       <c r="D12" s="72">
-        <v>0.96561621774548401</v>
-      </c>
-      <c r="E12" s="72">
-        <v>0.99423745052268397</v>
-      </c>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1" t="e">
-        <f>B12-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1">
-        <f>B12-G12</f>
-        <v>0.99794960680741096</v>
-      </c>
-      <c r="L12" s="1"/>
-      <c r="M12" s="60"/>
-      <c r="N12" s="46" t="s">
+        <v>0.99795213754072598</v>
+      </c>
+      <c r="F12" s="72">
+        <v>0.99864274324894997</v>
+      </c>
+      <c r="G12" s="89"/>
+      <c r="H12" s="89">
+        <f t="shared" si="2"/>
+        <v>-2.5307333150204059E-6</v>
+      </c>
+      <c r="I12" s="89"/>
+      <c r="J12" s="89">
+        <f t="shared" si="4"/>
+        <v>-6.9313644153901066E-4</v>
+      </c>
+      <c r="K12" s="89"/>
+      <c r="L12" s="60"/>
+      <c r="M12" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="O12" s="50">
+      <c r="N12" s="50">
         <v>29.247688021076399</v>
       </c>
-      <c r="P12" s="1">
-        <f t="shared" si="3"/>
+      <c r="O12" s="1">
+        <f t="shared" si="5"/>
         <v>0.29247688021076401</v>
       </c>
-      <c r="Q12" s="58"/>
+      <c r="P12" s="58"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -3536,29 +3545,34 @@
         <v>0.990436803259924</v>
       </c>
       <c r="E13" s="72">
-        <v>0</v>
-      </c>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1">
-        <f t="shared" ref="K13:K30" si="4">B13-G13</f>
-        <v>0.990436803259924</v>
-      </c>
-      <c r="L13" s="1"/>
-      <c r="M13" s="60"/>
-      <c r="N13" s="46" t="s">
+        <v>0.990432185290816</v>
+      </c>
+      <c r="F13" s="72">
+        <v>0.99093622037218698</v>
+      </c>
+      <c r="G13" s="89"/>
+      <c r="H13" s="89"/>
+      <c r="I13" s="89">
+        <f t="shared" si="3"/>
+        <v>4.617969108000608E-6</v>
+      </c>
+      <c r="J13" s="89">
+        <f t="shared" si="4"/>
+        <v>-4.9941711226297869E-4</v>
+      </c>
+      <c r="K13" s="89"/>
+      <c r="L13" s="60"/>
+      <c r="M13" s="46" t="s">
         <v>120</v>
       </c>
-      <c r="O13" s="50">
+      <c r="N13" s="50">
         <v>-10.134384235994199</v>
       </c>
-      <c r="P13" s="1">
-        <f t="shared" si="3"/>
+      <c r="O13" s="1">
+        <f t="shared" si="5"/>
         <v>-0.101343842359942</v>
       </c>
-      <c r="Q13" s="58"/>
+      <c r="P13" s="58"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -3568,33 +3582,34 @@
         <v>0.99358117274512303</v>
       </c>
       <c r="E14" s="72">
-        <v>0</v>
-      </c>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1">
-        <f t="shared" ref="J14:J30" si="5">B14-F14</f>
-        <v>0.99358117274512303</v>
-      </c>
-      <c r="K14" s="1">
+        <v>0.99357908633896896</v>
+      </c>
+      <c r="F14" s="72">
+        <v>0.99385505357405401</v>
+      </c>
+      <c r="G14" s="89"/>
+      <c r="H14" s="89"/>
+      <c r="I14" s="89">
+        <f t="shared" si="3"/>
+        <v>2.0864061540670775E-6</v>
+      </c>
+      <c r="J14" s="89">
         <f t="shared" si="4"/>
-        <v>0.99358117274512303</v>
-      </c>
-      <c r="L14" s="1"/>
-      <c r="M14" s="60"/>
-      <c r="N14" s="46" t="s">
+        <v>-2.7388082893098353E-4</v>
+      </c>
+      <c r="K14" s="89"/>
+      <c r="L14" s="60"/>
+      <c r="M14" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="O14" s="50">
+      <c r="N14" s="50">
         <v>4.9388912162000001E-5</v>
       </c>
-      <c r="P14" s="1">
-        <f t="shared" si="3"/>
+      <c r="O14" s="1">
+        <f t="shared" si="5"/>
         <v>4.9388912162000003E-7</v>
       </c>
-      <c r="Q14" s="58"/>
+      <c r="P14" s="58"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -3603,31 +3618,29 @@
       <c r="B15" s="1">
         <v>0.98674259047048396</v>
       </c>
-      <c r="C15" s="1"/>
       <c r="E15" s="72">
-        <v>0</v>
-      </c>
-      <c r="F15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1">
+        <v>0.98674065776487996</v>
+      </c>
+      <c r="G15" s="89"/>
+      <c r="H15" s="89"/>
+      <c r="I15" s="89">
+        <f t="shared" si="3"/>
+        <v>1.9327056040019386E-6</v>
+      </c>
+      <c r="J15" s="89"/>
+      <c r="K15" s="89"/>
+      <c r="L15" s="60"/>
+      <c r="M15" s="46" t="s">
+        <v>121</v>
+      </c>
+      <c r="N15" s="50">
+        <v>-23.1382548362844</v>
+      </c>
+      <c r="O15" s="1">
         <f t="shared" si="5"/>
-        <v>0.98674259047048396</v>
-      </c>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="60"/>
-      <c r="N15" s="46" t="s">
-        <v>121</v>
-      </c>
-      <c r="O15" s="50">
-        <v>-23.1382548362844</v>
-      </c>
-      <c r="P15" s="1">
-        <f t="shared" si="3"/>
         <v>-0.231382548362844</v>
       </c>
-      <c r="Q15" s="58"/>
+      <c r="P15" s="58"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -3638,35 +3651,36 @@
       </c>
       <c r="C16" s="1"/>
       <c r="E16" s="72">
-        <v>0</v>
-      </c>
-      <c r="F16" s="1"/>
-      <c r="G16" s="72"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1">
-        <f t="shared" si="5"/>
-        <v>0.98231334549872895</v>
-      </c>
-      <c r="K16" s="1">
+        <v>0.98231019425810095</v>
+      </c>
+      <c r="F16" s="72">
+        <v>0.98248572663218803</v>
+      </c>
+      <c r="G16" s="89"/>
+      <c r="H16" s="89"/>
+      <c r="I16" s="89">
+        <f t="shared" si="3"/>
+        <v>3.1512406279965433E-6</v>
+      </c>
+      <c r="J16" s="89">
         <f t="shared" si="4"/>
-        <v>0.98231334549872895</v>
-      </c>
-      <c r="L16" s="1"/>
-      <c r="M16" s="60" t="s">
+        <v>-1.7238113345907635E-4</v>
+      </c>
+      <c r="K16" s="89"/>
+      <c r="L16" s="60" t="s">
         <v>140</v>
       </c>
-      <c r="N16" s="46" t="s">
+      <c r="M16" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="O16" s="50">
+      <c r="N16" s="50">
         <v>6.4193752642371704</v>
       </c>
-      <c r="P16" s="1">
-        <f>O16/100</f>
+      <c r="O16" s="1">
+        <f>N16/100</f>
         <v>6.4193752642371704E-2</v>
       </c>
-      <c r="Q16" s="58"/>
+      <c r="P16" s="58"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
@@ -3675,601 +3689,637 @@
       <c r="B17" s="1">
         <v>0.96825697606458705</v>
       </c>
-      <c r="C17" s="1"/>
+      <c r="C17" s="72"/>
       <c r="E17" s="72">
-        <v>0</v>
-      </c>
-      <c r="F17" s="1"/>
-      <c r="G17" s="72"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1">
-        <f t="shared" si="5"/>
-        <v>0.96825697606458705</v>
-      </c>
-      <c r="K17" s="1">
+        <v>0.96823482800318095</v>
+      </c>
+      <c r="F17" s="89">
+        <v>0.96855419296839496</v>
+      </c>
+      <c r="G17" s="89"/>
+      <c r="H17" s="89"/>
+      <c r="I17" s="89">
+        <f t="shared" si="3"/>
+        <v>2.2148061406102038E-5</v>
+      </c>
+      <c r="J17" s="89">
         <f t="shared" si="4"/>
-        <v>0.96825697606458705</v>
-      </c>
-      <c r="L17" s="1"/>
-      <c r="M17" s="60" t="s">
+        <v>-2.9721690380790644E-4</v>
+      </c>
+      <c r="K17" s="89"/>
+      <c r="L17" s="60" t="s">
         <v>175</v>
       </c>
-      <c r="N17" s="46" t="s">
+      <c r="M17" s="46" t="s">
         <v>123</v>
       </c>
-      <c r="O17" s="50">
+      <c r="N17" s="50">
         <v>1.57798981550307</v>
       </c>
-      <c r="P17" s="1">
-        <f t="shared" ref="P17:P25" si="6">O17/100</f>
+      <c r="O17" s="1">
+        <f t="shared" ref="O17:O26" si="6">N17/100</f>
         <v>1.5779898155030701E-2</v>
       </c>
-      <c r="Q17" s="58"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="P17" s="58"/>
+    </row>
+    <row r="18" spans="1:17" s="72" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="89" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" s="89">
+        <v>0</v>
+      </c>
+      <c r="C18" s="72">
+        <v>0</v>
+      </c>
+      <c r="G18" s="89">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H18" s="89"/>
+      <c r="I18" s="89"/>
+      <c r="J18" s="89"/>
+      <c r="K18" s="89"/>
+      <c r="L18" s="60"/>
+      <c r="M18" s="87"/>
+      <c r="N18" s="50"/>
+      <c r="O18" s="89"/>
+      <c r="P18" s="58"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B18" s="72">
+      <c r="B19" s="72">
         <v>-9.0495834798616795E-2</v>
       </c>
-      <c r="C18" s="72">
-        <v>-9.0529272892522994E-2</v>
-      </c>
-      <c r="D18" s="72">
-        <v>-0.124554431030527</v>
-      </c>
-      <c r="E18" s="72">
-        <v>-9.9339141159860006E-2</v>
-      </c>
-      <c r="H18" s="1" t="e">
-        <f>B18-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I18" s="1" t="e">
-        <f>B18-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="M18" s="60"/>
-      <c r="N18" s="46" t="s">
+      <c r="C19" s="72">
+        <v>-9.0496583187875498E-2</v>
+      </c>
+      <c r="D19" s="72">
+        <v>-9.0492639023846799E-2</v>
+      </c>
+      <c r="G19" s="89">
+        <f t="shared" si="1"/>
+        <v>7.4838925870346351E-7</v>
+      </c>
+      <c r="H19" s="89">
+        <f t="shared" si="2"/>
+        <v>-3.1957747699956629E-6</v>
+      </c>
+      <c r="I19" s="89"/>
+      <c r="J19" s="89"/>
+      <c r="K19" s="89"/>
+      <c r="L19" s="60"/>
+      <c r="M19" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="O18" s="50">
+      <c r="N19" s="50">
         <v>7.6111237412808599</v>
       </c>
-      <c r="P18" s="1">
+      <c r="O19" s="1">
         <f t="shared" si="6"/>
         <v>7.6111237412808605E-2</v>
       </c>
-      <c r="Q18" s="58"/>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="P19" s="58"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B19" s="72">
+      <c r="B20" s="72">
         <v>-0.22164655627270699</v>
       </c>
-      <c r="C19" s="72">
-        <v>-0.22171218760252401</v>
-      </c>
-      <c r="D19" s="72">
-        <v>-4.2210794417888997E-2</v>
-      </c>
-      <c r="E19" s="72">
-        <v>-0.23155275841479001</v>
-      </c>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1" t="e">
-        <f>B19-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="M19" s="60"/>
-      <c r="N19" s="46" t="s">
+      <c r="C20" s="72">
+        <v>-0.22164303678837699</v>
+      </c>
+      <c r="D20" s="72">
+        <v>-0.22164370984260501</v>
+      </c>
+      <c r="G20" s="89">
+        <f t="shared" si="1"/>
+        <v>-3.5194843300001555E-6</v>
+      </c>
+      <c r="H20" s="89">
+        <f t="shared" si="2"/>
+        <v>-2.8464301019825999E-6</v>
+      </c>
+      <c r="I20" s="89"/>
+      <c r="J20" s="89"/>
+      <c r="K20" s="89"/>
+      <c r="L20" s="60"/>
+      <c r="M20" s="46" t="s">
         <v>122</v>
       </c>
-      <c r="O19" s="50">
+      <c r="N20" s="50">
         <v>2.2749299623984598</v>
       </c>
-      <c r="P19" s="1">
+      <c r="O20" s="1">
         <f t="shared" si="6"/>
         <v>2.2749299623984597E-2</v>
       </c>
-      <c r="Q19" s="58"/>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="P20" s="58"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B20" s="72">
+      <c r="B21" s="72">
         <v>-0.18448701889772101</v>
       </c>
-      <c r="C20" s="72">
-        <v>-0.18455446908089501</v>
-      </c>
-      <c r="D20" s="72">
-        <v>-0.26529410521504199</v>
-      </c>
-      <c r="E20" s="72">
-        <v>-0.19458270352378901</v>
-      </c>
-      <c r="H20" s="1" t="e">
-        <f>B20-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I20" s="1" t="e">
-        <f>B20-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="M20" s="60"/>
-      <c r="N20" s="46" t="s">
+      <c r="C21" s="72">
+        <v>-0.18448391547260901</v>
+      </c>
+      <c r="D21" s="72">
+        <v>-0.184485283589502</v>
+      </c>
+      <c r="F21" s="72">
+        <v>-0.18503534812550401</v>
+      </c>
+      <c r="G21" s="89">
+        <f t="shared" si="1"/>
+        <v>-3.1034251120054535E-6</v>
+      </c>
+      <c r="H21" s="89">
+        <f t="shared" si="2"/>
+        <v>-1.73530821900858E-6</v>
+      </c>
+      <c r="I21" s="89"/>
+      <c r="J21" s="89">
+        <f t="shared" si="4"/>
+        <v>5.4832922778300097E-4</v>
+      </c>
+      <c r="K21" s="89"/>
+      <c r="L21" s="60"/>
+      <c r="M21" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="O20" s="50">
+      <c r="N21" s="50">
         <v>17.236621109828601</v>
       </c>
-      <c r="P20" s="1">
+      <c r="O21" s="1">
         <f t="shared" si="6"/>
         <v>0.17236621109828601</v>
       </c>
-      <c r="Q20" s="58"/>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="P21" s="58"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B21" s="72">
+      <c r="B22" s="72">
         <v>-0.158411156268046</v>
       </c>
-      <c r="C21" s="72">
-        <v>-0.158467957369227</v>
-      </c>
-      <c r="D21" s="72">
-        <v>-0.224988393624065</v>
-      </c>
-      <c r="E21" s="72">
-        <v>-0.16833016487261601</v>
-      </c>
-      <c r="H21" s="1" t="e">
-        <f>B21-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I21" s="1" t="e">
-        <f>B21-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="M21" s="60"/>
-      <c r="N21" s="46" t="s">
+      <c r="C22" s="72">
+        <v>-0.15840864797552401</v>
+      </c>
+      <c r="D22" s="72">
+        <v>-0.158409442565668</v>
+      </c>
+      <c r="E22" s="72">
+        <v>-0.158404611844949</v>
+      </c>
+      <c r="G22" s="89">
+        <f t="shared" si="1"/>
+        <v>-2.508292521991029E-6</v>
+      </c>
+      <c r="H22" s="89">
+        <f t="shared" si="2"/>
+        <v>-1.71370237800339E-6</v>
+      </c>
+      <c r="I22" s="89">
+        <f t="shared" si="3"/>
+        <v>-6.5444230969990969E-6</v>
+      </c>
+      <c r="J22" s="89"/>
+      <c r="K22" s="89"/>
+      <c r="L22" s="60"/>
+      <c r="M22" s="46" t="s">
         <v>124</v>
       </c>
-      <c r="O21" s="50">
+      <c r="N22" s="50">
         <v>6.2088690408799696</v>
       </c>
-      <c r="P21" s="1">
+      <c r="O22" s="1">
         <f t="shared" si="6"/>
         <v>6.2088690408799697E-2</v>
       </c>
-      <c r="Q21" s="58"/>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="P22" s="58"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="B22" s="72">
+      <c r="B23" s="72">
         <v>-0.26207372353015002</v>
       </c>
-      <c r="C22" s="72">
-        <v>-0.26215071828858399</v>
-      </c>
-      <c r="E22" s="72">
-        <v>0</v>
-      </c>
-      <c r="F22" s="1"/>
-      <c r="H22" s="1" t="e">
-        <f>B22-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1">
-        <f t="shared" si="5"/>
-        <v>-0.26207372353015002</v>
-      </c>
-      <c r="K22" s="1"/>
-      <c r="M22" s="60"/>
-      <c r="N22" s="46" t="s">
+      <c r="C23" s="72">
+        <v>-0.26206908569225601</v>
+      </c>
+      <c r="E23" s="72">
+        <v>-0.262070640122187</v>
+      </c>
+      <c r="G23" s="89">
+        <f t="shared" si="1"/>
+        <v>-4.6378378940059584E-6</v>
+      </c>
+      <c r="H23" s="89"/>
+      <c r="I23" s="89">
+        <f t="shared" si="3"/>
+        <v>-3.0834079630115419E-6</v>
+      </c>
+      <c r="J23" s="89"/>
+      <c r="K23" s="89"/>
+      <c r="L23" s="60"/>
+      <c r="M23" s="46" t="s">
         <v>59</v>
       </c>
-      <c r="O22" s="50">
+      <c r="N23" s="50">
         <v>1.4392071686730901</v>
       </c>
-      <c r="P22" s="1">
+      <c r="O23" s="1">
         <f t="shared" si="6"/>
         <v>1.4392071686730901E-2</v>
       </c>
-      <c r="Q22" s="58"/>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="P23" s="58"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B23" s="72">
+      <c r="B24" s="72">
         <v>-0.246986077730002</v>
       </c>
-      <c r="D23" s="72">
-        <v>-0.198495031973627</v>
-      </c>
-      <c r="E23" s="72">
-        <v>-0.25909980104373398</v>
-      </c>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1" t="e">
-        <f>B23-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="M23" s="60"/>
-      <c r="N23" s="46" t="s">
+      <c r="D24" s="72">
+        <v>-0.24698548709700099</v>
+      </c>
+      <c r="F24" s="72">
+        <v>-0.24492655820126599</v>
+      </c>
+      <c r="G24" s="1"/>
+      <c r="H24" s="89">
+        <f t="shared" si="2"/>
+        <v>-5.9063300100747895E-7</v>
+      </c>
+      <c r="I24" s="89"/>
+      <c r="J24" s="89">
+        <f t="shared" si="4"/>
+        <v>-2.0595195287360091E-3</v>
+      </c>
+      <c r="K24" s="89"/>
+      <c r="L24" s="60"/>
+      <c r="M24" s="46" t="s">
         <v>125</v>
       </c>
-      <c r="O23" s="50">
+      <c r="N24" s="50">
         <v>0.52526799870488805</v>
       </c>
-      <c r="P23" s="1">
+      <c r="O24" s="1">
         <f t="shared" si="6"/>
         <v>5.2526799870488807E-3</v>
       </c>
-      <c r="Q23" s="58"/>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="P24" s="58"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B24" s="72">
+      <c r="B25" s="72">
         <v>-0.25618480157818402</v>
       </c>
-      <c r="D24" s="72">
-        <v>-0.29265337611138798</v>
-      </c>
-      <c r="E24" s="72">
-        <v>-0.268464066192176</v>
-      </c>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1" t="e">
-        <f>B24-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="M24" s="60"/>
-      <c r="N24" s="46" t="s">
+      <c r="D25" s="72">
+        <v>-0.25618433392062101</v>
+      </c>
+      <c r="G25" s="1"/>
+      <c r="H25" s="89">
+        <f t="shared" si="2"/>
+        <v>-4.6765756300803929E-7</v>
+      </c>
+      <c r="I25" s="89"/>
+      <c r="J25" s="89"/>
+      <c r="K25" s="89"/>
+      <c r="L25" s="60"/>
+      <c r="M25" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="O24" s="50">
+      <c r="N25" s="50">
         <v>-6.1</v>
       </c>
-      <c r="P24" s="1">
+      <c r="O25" s="1">
         <f t="shared" si="6"/>
         <v>-6.0999999999999999E-2</v>
       </c>
-      <c r="Q24" s="58"/>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="P25" s="58"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="B25" s="72">
+      <c r="B26" s="72">
         <v>-0.27411931344698798</v>
       </c>
-      <c r="D25" s="72">
-        <v>-0.29913002545983097</v>
-      </c>
-      <c r="E25" s="72">
-        <v>-0.287395123561481</v>
-      </c>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1" t="e">
-        <f>B25-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1">
+      <c r="D26" s="72">
+        <v>-0.274119032775341</v>
+      </c>
+      <c r="F26" s="89">
+        <v>-0.27206131194628702</v>
+      </c>
+      <c r="G26" s="1"/>
+      <c r="H26" s="89">
+        <f t="shared" si="2"/>
+        <v>-2.8067164697942459E-7</v>
+      </c>
+      <c r="I26" s="89"/>
+      <c r="J26" s="89">
         <f t="shared" si="4"/>
-        <v>-0.27411931344698798</v>
-      </c>
-      <c r="M25" s="60"/>
-      <c r="N25" s="46" t="s">
+        <v>-2.0580015007009567E-3</v>
+      </c>
+      <c r="K26" s="89"/>
+      <c r="L26" s="60"/>
+      <c r="M26" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="O25" s="50">
+      <c r="N26" s="50">
         <v>-1.6</v>
       </c>
-      <c r="P25" s="1">
+      <c r="O26" s="1">
         <f t="shared" si="6"/>
         <v>-1.6E-2</v>
       </c>
-      <c r="Q25" s="58"/>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B26" s="72">
-        <v>-0.27529246082033898</v>
-      </c>
-      <c r="G26" s="72"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1">
-        <f t="shared" si="4"/>
-        <v>-0.27529246082033898</v>
-      </c>
-      <c r="M26" s="60" t="s">
-        <v>141</v>
-      </c>
-      <c r="N26" s="46" t="s">
-        <v>61</v>
-      </c>
-      <c r="O26" s="50">
-        <v>6.1481308294477897</v>
-      </c>
-      <c r="P26" s="1">
-        <f>O26/100</f>
-        <v>6.1481308294477899E-2</v>
-      </c>
-      <c r="Q26" s="57"/>
+      <c r="P26" s="58"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B27" s="72">
-        <v>-0.27032933293769501</v>
-      </c>
-      <c r="F27" s="72"/>
-      <c r="G27" s="72"/>
+        <v>-0.27529246082033898</v>
+      </c>
+      <c r="E27" s="72">
+        <v>-0.27528456522628397</v>
+      </c>
+      <c r="F27" s="89">
+        <v>-0.273035701817684</v>
+      </c>
+      <c r="G27" s="1"/>
       <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1">
-        <f t="shared" si="5"/>
-        <v>-0.27032933293769501</v>
-      </c>
-      <c r="K27" s="1">
+      <c r="I27" s="89">
+        <f t="shared" si="3"/>
+        <v>-7.8955940550073933E-6</v>
+      </c>
+      <c r="J27" s="89">
         <f t="shared" si="4"/>
-        <v>-0.27032933293769501</v>
-      </c>
-      <c r="M27" s="56" t="s">
-        <v>176</v>
-      </c>
-      <c r="N27" s="46" t="s">
-        <v>126</v>
-      </c>
-      <c r="O27" s="50">
-        <v>6.1776975079165704</v>
-      </c>
-      <c r="P27" s="1">
-        <f t="shared" ref="P27:P39" si="7">O27/100</f>
-        <v>6.1776975079165707E-2</v>
-      </c>
-      <c r="Q27" s="57"/>
+        <v>-2.2567590026549844E-3</v>
+      </c>
+      <c r="K27" s="89"/>
+      <c r="L27" s="60" t="s">
+        <v>141</v>
+      </c>
+      <c r="M27" s="46" t="s">
+        <v>61</v>
+      </c>
+      <c r="N27" s="50">
+        <v>6.1481308294477897</v>
+      </c>
+      <c r="O27" s="1">
+        <f>N27/100</f>
+        <v>6.1481308294477899E-2</v>
+      </c>
+      <c r="P27" s="57"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B28" s="72">
+        <v>-0.27032933293769501</v>
+      </c>
+      <c r="E28" s="72">
+        <v>-0.27032264406406797</v>
+      </c>
+      <c r="F28" s="72">
+        <v>-0.267805813851972</v>
+      </c>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="89">
+        <f t="shared" si="3"/>
+        <v>-6.6888736270365179E-6</v>
+      </c>
+      <c r="J28" s="89">
+        <f t="shared" si="4"/>
+        <v>-2.5235190857230139E-3</v>
+      </c>
+      <c r="K28" s="89"/>
+      <c r="L28" s="56" t="s">
+        <v>176</v>
+      </c>
+      <c r="M28" s="46" t="s">
+        <v>126</v>
+      </c>
+      <c r="N28" s="50">
+        <v>6.1776975079165704</v>
+      </c>
+      <c r="O28" s="1">
+        <f t="shared" ref="O28:P40" si="7">N28/100</f>
+        <v>6.1776975079165707E-2</v>
+      </c>
+      <c r="P28" s="57"/>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="B28" s="72">
+      <c r="B29" s="72">
         <v>-0.27392983143629202</v>
       </c>
-      <c r="F28" s="72"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1">
-        <f t="shared" si="5"/>
-        <v>-0.27392983143629202</v>
-      </c>
-      <c r="K28" s="1"/>
-      <c r="M28" s="61"/>
-      <c r="N28" s="46" t="s">
+      <c r="E29" s="72">
+        <v>-0.27392304691536401</v>
+      </c>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="89">
+        <f t="shared" si="3"/>
+        <v>-6.7845209280048557E-6</v>
+      </c>
+      <c r="J29" s="89"/>
+      <c r="K29" s="89"/>
+      <c r="L29" s="61"/>
+      <c r="M29" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="O28" s="50">
+      <c r="N29" s="50">
         <v>10.1258308263922</v>
       </c>
-      <c r="P28" s="1">
+      <c r="O29" s="1">
         <f t="shared" si="7"/>
         <v>0.101258308263922</v>
       </c>
-      <c r="Q28" s="58"/>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+      <c r="P29" s="58"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="B29" s="72">
+      <c r="B30" s="72">
         <v>-0.27443829599560998</v>
       </c>
-      <c r="F29" s="72"/>
-      <c r="G29" s="72"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1">
-        <f t="shared" si="5"/>
-        <v>-0.27443829599560998</v>
-      </c>
-      <c r="K29" s="1">
+      <c r="E30" s="72">
+        <v>-0.27443001849145199</v>
+      </c>
+      <c r="F30" s="72">
+        <v>-0.27126408666823298</v>
+      </c>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="89">
+        <f t="shared" si="3"/>
+        <v>-8.2775041579941089E-6</v>
+      </c>
+      <c r="J30" s="89">
         <f t="shared" si="4"/>
-        <v>-0.27443829599560998</v>
-      </c>
-      <c r="M29" s="61"/>
-      <c r="N29" s="46" t="s">
+        <v>-3.1742093273769978E-3</v>
+      </c>
+      <c r="K30" s="89"/>
+      <c r="L30" s="61"/>
+      <c r="M30" s="46" t="s">
         <v>127</v>
       </c>
-      <c r="O29" s="50">
+      <c r="N30" s="50">
         <v>4.8779939913553596</v>
       </c>
-      <c r="P29" s="1">
+      <c r="O30" s="1">
         <f t="shared" si="7"/>
         <v>4.8779939913553595E-2</v>
       </c>
-      <c r="Q29" s="57"/>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+      <c r="P30" s="57"/>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="B30" s="72">
+      <c r="B31" s="72">
         <v>-0.287190454321613</v>
       </c>
-      <c r="F30" s="72"/>
-      <c r="G30" s="72"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1">
-        <f t="shared" si="5"/>
-        <v>-0.287190454321613</v>
-      </c>
-      <c r="K30" s="1">
+      <c r="E31" s="72">
+        <v>-0.28716765031181002</v>
+      </c>
+      <c r="F31" s="72">
+        <v>-0.28449010818014198</v>
+      </c>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="89">
+        <f t="shared" si="3"/>
+        <v>-2.2804009802979142E-5</v>
+      </c>
+      <c r="J31" s="89">
         <f t="shared" si="4"/>
-        <v>-0.287190454321613</v>
-      </c>
-      <c r="M30" s="60" t="s">
+        <v>-2.7003461414710217E-3</v>
+      </c>
+      <c r="K31" s="89"/>
+      <c r="L31" s="60" t="s">
         <v>142</v>
       </c>
-      <c r="N30" s="46" t="s">
+      <c r="M31" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="O30" s="50">
+      <c r="N31" s="50">
         <v>-7.6</v>
       </c>
-      <c r="P30" s="1">
+      <c r="O31" s="1">
         <f t="shared" si="7"/>
         <v>-7.5999999999999998E-2</v>
       </c>
-      <c r="Q30" s="58"/>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="M31" s="56" t="s">
+      <c r="P31" s="58"/>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M32" s="56" t="s">
         <v>177</v>
       </c>
-      <c r="N31" s="46" t="s">
+      <c r="N32" s="46" t="s">
         <v>128</v>
       </c>
-      <c r="O31" s="50">
+      <c r="O32" s="50">
         <v>-1.6</v>
       </c>
-      <c r="P31" s="1">
+      <c r="P32" s="1">
         <f t="shared" si="7"/>
         <v>-1.6E-2</v>
       </c>
-      <c r="Q31" s="58"/>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="M32" s="60" t="s">
+      <c r="Q32" s="58"/>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M33" s="60" t="s">
         <v>143</v>
       </c>
-      <c r="N32" s="46" t="s">
+      <c r="N33" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="O32" s="51">
+      <c r="O33" s="51">
         <v>-63.001699846354903</v>
       </c>
-      <c r="P32" s="1">
+      <c r="P33" s="1">
         <f t="shared" si="7"/>
         <v>-0.63001699846354908</v>
       </c>
-      <c r="Q32" s="58"/>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="M33" s="56" t="s">
+      <c r="Q33" s="58"/>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M34" s="56" t="s">
         <v>178</v>
       </c>
-      <c r="N33" s="46" t="s">
+      <c r="N34" s="46" t="s">
         <v>129</v>
       </c>
-      <c r="O33" s="50">
+      <c r="O34" s="50">
         <v>10.2039485868599</v>
       </c>
-      <c r="P33" s="1">
+      <c r="P34" s="1">
         <f t="shared" si="7"/>
         <v>0.102039485868599</v>
       </c>
-      <c r="Q33" s="58"/>
-    </row>
-    <row r="34" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E34" s="49"/>
-      <c r="M34" s="60"/>
-      <c r="N34" s="46" t="s">
+      <c r="Q34" s="58"/>
+    </row>
+    <row r="35" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D35" s="49"/>
+      <c r="E35" s="49"/>
+      <c r="M35" s="60"/>
+      <c r="N35" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="O34" s="50">
+      <c r="O35" s="50">
         <v>16.526211548050401</v>
       </c>
-      <c r="P34" s="1">
+      <c r="P35" s="1">
         <f t="shared" si="7"/>
         <v>0.16526211548050401</v>
       </c>
-      <c r="Q34" s="58"/>
-    </row>
-    <row r="35" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="49"/>
-      <c r="B35" s="49"/>
-      <c r="C35" s="49"/>
-      <c r="D35" s="49"/>
-      <c r="E35" s="47"/>
-      <c r="F35" s="49"/>
-      <c r="G35" s="49"/>
-      <c r="H35" s="49"/>
-      <c r="I35" s="49"/>
-      <c r="J35" s="49"/>
-      <c r="K35" s="49"/>
-      <c r="L35" s="49"/>
-      <c r="M35" s="60"/>
-      <c r="N35" s="46" t="s">
+      <c r="Q35" s="58"/>
+    </row>
+    <row r="36" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="49"/>
+      <c r="B36" s="49"/>
+      <c r="C36" s="49"/>
+      <c r="D36" s="47"/>
+      <c r="E36" s="47"/>
+      <c r="F36" s="49"/>
+      <c r="G36" s="49"/>
+      <c r="H36" s="49"/>
+      <c r="I36" s="49"/>
+      <c r="J36" s="49"/>
+      <c r="K36" s="49"/>
+      <c r="L36" s="49"/>
+      <c r="M36" s="60"/>
+      <c r="N36" s="46" t="s">
         <v>130</v>
       </c>
-      <c r="O35" s="52">
+      <c r="O36" s="52">
         <v>-1.34369314780613</v>
       </c>
-      <c r="P35" s="1">
+      <c r="P36" s="1">
         <f t="shared" si="7"/>
         <v>-1.34369314780613E-2</v>
-      </c>
-      <c r="Q35" s="58"/>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A36" s="47"/>
-      <c r="B36" s="47"/>
-      <c r="C36" s="47"/>
-      <c r="D36" s="47"/>
-      <c r="E36" s="47"/>
-      <c r="F36" s="47"/>
-      <c r="G36" s="47"/>
-      <c r="H36" s="47"/>
-      <c r="I36" s="47"/>
-      <c r="J36" s="47"/>
-      <c r="K36" s="47"/>
-      <c r="L36" s="47"/>
-      <c r="M36" s="60"/>
-      <c r="N36" s="46" t="s">
-        <v>66</v>
-      </c>
-      <c r="O36" s="52">
-        <v>29.247637436823101</v>
-      </c>
-      <c r="P36" s="1">
-        <f t="shared" si="7"/>
-        <v>0.29247637436823104</v>
       </c>
       <c r="Q36" s="58"/>
     </row>
@@ -4288,14 +4338,14 @@
       <c r="L37" s="47"/>
       <c r="M37" s="60"/>
       <c r="N37" s="46" t="s">
-        <v>131</v>
+        <v>66</v>
       </c>
       <c r="O37" s="52">
-        <v>11.0919776937066</v>
+        <v>29.247637436823101</v>
       </c>
       <c r="P37" s="1">
         <f t="shared" si="7"/>
-        <v>0.11091977693706599</v>
+        <v>0.29247637436823104</v>
       </c>
       <c r="Q37" s="58"/>
     </row>
@@ -4304,7 +4354,7 @@
       <c r="B38" s="47"/>
       <c r="C38" s="47"/>
       <c r="D38" s="47"/>
-      <c r="E38" s="86"/>
+      <c r="E38" s="47"/>
       <c r="F38" s="47"/>
       <c r="G38" s="47"/>
       <c r="H38" s="47"/>
@@ -4314,90 +4364,90 @@
       <c r="L38" s="47"/>
       <c r="M38" s="60"/>
       <c r="N38" s="46" t="s">
-        <v>67</v>
-      </c>
-      <c r="O38" s="53">
-        <v>-94.199996999999996</v>
+        <v>131</v>
+      </c>
+      <c r="O38" s="52">
+        <v>11.0919776937066</v>
       </c>
       <c r="P38" s="1">
         <f t="shared" si="7"/>
-        <v>-0.94199996999999991</v>
+        <v>0.11091977693706599</v>
       </c>
       <c r="Q38" s="58"/>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
+      <c r="A39" s="47"/>
+      <c r="B39" s="47"/>
+      <c r="C39" s="47"/>
       <c r="D39" s="1"/>
       <c r="E39" s="86"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
-      <c r="K39" s="1"/>
-      <c r="L39" s="1"/>
+      <c r="F39" s="47"/>
+      <c r="G39" s="47"/>
+      <c r="H39" s="47"/>
+      <c r="I39" s="47"/>
+      <c r="J39" s="47"/>
+      <c r="K39" s="47"/>
+      <c r="L39" s="47"/>
       <c r="M39" s="60"/>
       <c r="N39" s="46" t="s">
-        <v>132</v>
-      </c>
-      <c r="O39">
-        <f>21.4613437652587-19</f>
-        <v>2.4613437652587002</v>
+        <v>67</v>
+      </c>
+      <c r="O39" s="53">
+        <v>-94.199996999999996</v>
       </c>
       <c r="P39" s="1">
         <f t="shared" si="7"/>
-        <v>2.4613437652587004E-2</v>
+        <v>-0.94199996999999991</v>
       </c>
       <c r="Q39" s="58"/>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="86"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
-      <c r="K40" s="1"/>
+      <c r="K40" s="89"/>
       <c r="L40" s="1"/>
-      <c r="M40" s="60" t="s">
-        <v>144</v>
-      </c>
+      <c r="M40" s="60"/>
       <c r="N40" s="46" t="s">
-        <v>68</v>
-      </c>
-      <c r="O40" s="52">
-        <v>4.9650161007164098</v>
+        <v>132</v>
+      </c>
+      <c r="O40">
+        <f>21.4613437652587-19</f>
+        <v>2.4613437652587002</v>
       </c>
       <c r="P40" s="1">
-        <f>O40/100</f>
-        <v>4.9650161007164101E-2</v>
+        <f t="shared" si="7"/>
+        <v>2.4613437652587004E-2</v>
       </c>
       <c r="Q40" s="58"/>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="86"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
-      <c r="K41" s="1"/>
+      <c r="K41" s="89"/>
       <c r="L41" s="1"/>
-      <c r="M41" s="56" t="s">
-        <v>179</v>
+      <c r="M41" s="60" t="s">
+        <v>144</v>
       </c>
       <c r="N41" s="46" t="s">
-        <v>133</v>
+        <v>68</v>
       </c>
       <c r="O41" s="52">
-        <v>0.52427629116916796</v>
+        <v>4.9650161007164098</v>
       </c>
       <c r="P41" s="1">
-        <f t="shared" ref="P41:P43" si="8">O41/100</f>
-        <v>5.2427629116916794E-3</v>
+        <f>O41/100</f>
+        <v>4.9650161007164101E-2</v>
       </c>
       <c r="Q41" s="58"/>
     </row>
@@ -4406,21 +4456,24 @@
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
+      <c r="E42" s="86"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
-      <c r="K42" s="1"/>
+      <c r="K42" s="89"/>
       <c r="L42" s="1"/>
-      <c r="M42" s="60"/>
+      <c r="M42" s="56" t="s">
+        <v>179</v>
+      </c>
       <c r="N42" s="46" t="s">
-        <v>16</v>
+        <v>133</v>
       </c>
       <c r="O42" s="52">
-        <v>-13.5</v>
+        <v>0.52427629116916796</v>
       </c>
       <c r="P42" s="1">
-        <f t="shared" si="8"/>
-        <v>-0.13500000000000001</v>
+        <f t="shared" ref="P42:P44" si="8">O42/100</f>
+        <v>5.2427629116916794E-3</v>
       </c>
       <c r="Q42" s="58"/>
     </row>
@@ -4428,24 +4481,21 @@
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
-      <c r="E43" s="86"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
-      <c r="K43" s="1"/>
+      <c r="K43" s="89"/>
       <c r="L43" s="1"/>
       <c r="M43" s="60"/>
       <c r="N43" s="46" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="O43" s="52">
-        <v>-5.8</v>
+        <v>-13.5</v>
       </c>
       <c r="P43" s="1">
         <f t="shared" si="8"/>
-        <v>-5.7999999999999996E-2</v>
+        <v>-0.13500000000000001</v>
       </c>
       <c r="Q43" s="58"/>
     </row>
@@ -4455,25 +4505,23 @@
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44" s="86"/>
-      <c r="F44" s="72"/>
+      <c r="F44" s="1"/>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
-      <c r="K44" s="1"/>
+      <c r="K44" s="89"/>
       <c r="L44" s="1"/>
-      <c r="M44" s="60" t="s">
-        <v>145</v>
-      </c>
+      <c r="M44" s="60"/>
       <c r="N44" s="46" t="s">
-        <v>69</v>
+        <v>22</v>
       </c>
       <c r="O44" s="52">
-        <v>-2.8744036925517298</v>
+        <v>-5.8</v>
       </c>
       <c r="P44" s="1">
-        <f>O44/100</f>
-        <v>-2.8744036925517299E-2</v>
+        <f t="shared" si="8"/>
+        <v>-5.7999999999999996E-2</v>
       </c>
       <c r="Q44" s="58"/>
     </row>
@@ -4488,20 +4536,20 @@
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
-      <c r="K45" s="1"/>
+      <c r="K45" s="89"/>
       <c r="L45" s="1"/>
-      <c r="M45" s="56" t="s">
-        <v>180</v>
+      <c r="M45" s="60" t="s">
+        <v>145</v>
       </c>
       <c r="N45" s="46" t="s">
-        <v>134</v>
+        <v>69</v>
       </c>
       <c r="O45" s="52">
-        <v>0.31779049296478201</v>
+        <v>-2.8744036925517298</v>
       </c>
       <c r="P45" s="1">
-        <f t="shared" ref="P45:P51" si="9">O45/100</f>
-        <v>3.1779049296478202E-3</v>
+        <f>O45/100</f>
+        <v>-2.8744036925517299E-2</v>
       </c>
       <c r="Q45" s="58"/>
     </row>
@@ -4516,18 +4564,20 @@
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
-      <c r="K46" s="1"/>
+      <c r="K46" s="89"/>
       <c r="L46" s="1"/>
-      <c r="M46" s="60"/>
+      <c r="M46" s="56" t="s">
+        <v>180</v>
+      </c>
       <c r="N46" s="46" t="s">
-        <v>70</v>
+        <v>134</v>
       </c>
       <c r="O46" s="52">
-        <v>-14.9</v>
+        <v>0.31779049296478201</v>
       </c>
       <c r="P46" s="1">
-        <f t="shared" si="9"/>
-        <v>-0.14899999999999999</v>
+        <f t="shared" ref="P46:P52" si="9">O46/100</f>
+        <v>3.1779049296478202E-3</v>
       </c>
       <c r="Q46" s="58"/>
     </row>
@@ -4537,26 +4587,27 @@
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="E47" s="86"/>
+      <c r="F47" s="72"/>
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
-      <c r="K47" s="1"/>
+      <c r="K47" s="89"/>
       <c r="L47" s="1"/>
       <c r="M47" s="60"/>
       <c r="N47" s="46" t="s">
-        <v>135</v>
+        <v>70</v>
       </c>
       <c r="O47" s="52">
-        <v>-5</v>
+        <v>-14.9</v>
       </c>
       <c r="P47" s="1">
         <f t="shared" si="9"/>
-        <v>-0.05</v>
+        <v>-0.14899999999999999</v>
       </c>
       <c r="Q47" s="58"/>
     </row>
-    <row r="48" spans="1:17" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -4566,24 +4617,20 @@
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
-      <c r="K48" s="1"/>
+      <c r="K48" s="89"/>
       <c r="L48" s="1"/>
-      <c r="M48" s="60" t="s">
-        <v>202</v>
-      </c>
-      <c r="N48" s="79" t="s">
-        <v>206</v>
-      </c>
-      <c r="O48" s="80">
-        <v>72.934574594694098</v>
+      <c r="M48" s="60"/>
+      <c r="N48" s="46" t="s">
+        <v>135</v>
+      </c>
+      <c r="O48" s="52">
+        <v>-5</v>
       </c>
       <c r="P48" s="1">
         <f t="shared" si="9"/>
-        <v>0.72934574594694102</v>
-      </c>
-      <c r="Q48" s="58" t="s">
-        <v>217</v>
-      </c>
+        <v>-0.05</v>
+      </c>
+      <c r="Q48" s="58"/>
     </row>
     <row r="49" spans="1:17" s="72" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
@@ -4595,20 +4642,20 @@
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
-      <c r="K49" s="1"/>
+      <c r="K49" s="89"/>
       <c r="L49" s="1"/>
       <c r="M49" s="60" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
       <c r="N49" s="79" t="s">
-        <v>207</v>
-      </c>
-      <c r="O49" s="72">
-        <v>3.5900360862934599</v>
+        <v>206</v>
+      </c>
+      <c r="O49" s="80">
+        <v>72.934574594694098</v>
       </c>
       <c r="P49" s="1">
-        <f>O49/100</f>
-        <v>3.5900360862934598E-2</v>
+        <f t="shared" si="9"/>
+        <v>0.72934574594694102</v>
       </c>
       <c r="Q49" s="58" t="s">
         <v>217</v>
@@ -4624,21 +4671,23 @@
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
       <c r="J50" s="1"/>
-      <c r="K50" s="1"/>
+      <c r="K50" s="89"/>
       <c r="L50" s="1"/>
-      <c r="M50" s="60"/>
+      <c r="M50" s="60" t="s">
+        <v>216</v>
+      </c>
       <c r="N50" s="79" t="s">
-        <v>204</v>
-      </c>
-      <c r="O50" s="52">
-        <v>42.467165475154701</v>
+        <v>207</v>
+      </c>
+      <c r="O50" s="72">
+        <v>3.5900360862934599</v>
       </c>
       <c r="P50" s="1">
-        <f t="shared" si="9"/>
-        <v>0.424671654751547</v>
+        <f>O50/100</f>
+        <v>3.5900360862934598E-2</v>
       </c>
       <c r="Q50" s="58" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="51" spans="1:17" s="72" customFormat="1" x14ac:dyDescent="0.25">
@@ -4651,18 +4700,18 @@
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
-      <c r="K51" s="1"/>
+      <c r="K51" s="89"/>
       <c r="L51" s="1"/>
       <c r="M51" s="60"/>
       <c r="N51" s="79" t="s">
-        <v>205</v>
-      </c>
-      <c r="O51" s="80">
-        <v>-2.12732489205733</v>
+        <v>204</v>
+      </c>
+      <c r="O51" s="52">
+        <v>42.467165475154701</v>
       </c>
       <c r="P51" s="1">
         <f t="shared" si="9"/>
-        <v>-2.12732489205733E-2</v>
+        <v>0.424671654751547</v>
       </c>
       <c r="Q51" s="58" t="s">
         <v>218</v>
@@ -4678,18 +4727,18 @@
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
       <c r="J52" s="1"/>
-      <c r="K52" s="1"/>
+      <c r="K52" s="89"/>
       <c r="L52" s="1"/>
       <c r="M52" s="60"/>
       <c r="N52" s="79" t="s">
-        <v>26</v>
+        <v>205</v>
       </c>
       <c r="O52" s="80">
-        <v>1.059999943</v>
+        <v>-2.12732489205733</v>
       </c>
       <c r="P52" s="1">
-        <f>O52</f>
-        <v>1.059999943</v>
+        <f t="shared" si="9"/>
+        <v>-2.12732489205733E-2</v>
       </c>
       <c r="Q52" s="58" t="s">
         <v>218</v>
@@ -4704,18 +4753,19 @@
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
-      <c r="K53" s="1"/>
+      <c r="J53" s="1"/>
+      <c r="K53" s="89"/>
       <c r="L53" s="1"/>
       <c r="M53" s="60"/>
-      <c r="N53" s="81" t="s">
-        <v>210</v>
+      <c r="N53" s="79" t="s">
+        <v>26</v>
       </c>
       <c r="O53" s="80">
-        <v>1.028092515</v>
+        <v>1.059999943</v>
       </c>
       <c r="P53" s="1">
         <f>O53</f>
-        <v>1.028092515</v>
+        <v>1.059999943</v>
       </c>
       <c r="Q53" s="58" t="s">
         <v>218</v>
@@ -4730,21 +4780,20 @@
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
-      <c r="K54" s="1"/>
       <c r="L54" s="1"/>
       <c r="M54" s="60"/>
       <c r="N54" s="81" t="s">
-        <v>94</v>
+        <v>210</v>
       </c>
       <c r="O54" s="80">
-        <v>1.009999997</v>
+        <v>1.028092515</v>
       </c>
       <c r="P54" s="1">
-        <f t="shared" ref="P54:P59" si="10">O54</f>
-        <v>1.009999997</v>
+        <f>O54</f>
+        <v>1.028092515</v>
       </c>
       <c r="Q54" s="58" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="55" spans="1:17" s="72" customFormat="1" x14ac:dyDescent="0.25">
@@ -4756,18 +4805,17 @@
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
-      <c r="K55" s="1"/>
       <c r="L55" s="1"/>
       <c r="M55" s="60"/>
       <c r="N55" s="81" t="s">
-        <v>211</v>
+        <v>94</v>
       </c>
       <c r="O55" s="80">
-        <v>1.085083507</v>
+        <v>1.009999997</v>
       </c>
       <c r="P55" s="1">
-        <f t="shared" si="10"/>
-        <v>1.085083507</v>
+        <f t="shared" ref="P55:P60" si="10">O55</f>
+        <v>1.009999997</v>
       </c>
       <c r="Q55" s="58" t="s">
         <v>217</v>
@@ -4782,21 +4830,20 @@
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
-      <c r="K56" s="1"/>
       <c r="L56" s="1"/>
       <c r="M56" s="60"/>
       <c r="N56" s="81" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="O56" s="80">
-        <v>1.0240525229999999</v>
+        <v>1.085083507</v>
       </c>
       <c r="P56" s="1">
         <f t="shared" si="10"/>
-        <v>1.0240525229999999</v>
+        <v>1.085083507</v>
       </c>
       <c r="Q56" s="58" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="57" spans="1:17" s="72" customFormat="1" x14ac:dyDescent="0.25">
@@ -4808,18 +4855,17 @@
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
-      <c r="K57" s="1"/>
       <c r="L57" s="1"/>
       <c r="M57" s="60"/>
       <c r="N57" s="81" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="O57" s="80">
-        <v>1.019923836</v>
+        <v>1.0240525229999999</v>
       </c>
       <c r="P57" s="1">
         <f t="shared" si="10"/>
-        <v>1.019923836</v>
+        <v>1.0240525229999999</v>
       </c>
       <c r="Q57" s="58" t="s">
         <v>219</v>
@@ -4834,21 +4880,20 @@
       <c r="G58" s="1"/>
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
-      <c r="K58" s="1"/>
       <c r="L58" s="1"/>
       <c r="M58" s="60"/>
       <c r="N58" s="81" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="O58" s="80">
-        <v>1.027986216</v>
+        <v>1.019923836</v>
       </c>
       <c r="P58" s="1">
         <f t="shared" si="10"/>
-        <v>1.027986216</v>
+        <v>1.019923836</v>
       </c>
       <c r="Q58" s="58" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="59" spans="1:17" s="72" customFormat="1" x14ac:dyDescent="0.25">
@@ -4860,24 +4905,23 @@
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
-      <c r="K59" s="1"/>
       <c r="L59" s="1"/>
       <c r="M59" s="60"/>
       <c r="N59" s="81" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="O59" s="80">
-        <v>1.0349152580000001</v>
+        <v>1.027986216</v>
       </c>
       <c r="P59" s="1">
         <f t="shared" si="10"/>
-        <v>1.0349152580000001</v>
+        <v>1.027986216</v>
       </c>
       <c r="Q59" s="58" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" s="72" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -4886,41 +4930,40 @@
       <c r="G60" s="1"/>
       <c r="H60" s="1"/>
       <c r="I60" s="1"/>
-      <c r="J60" s="1"/>
-      <c r="K60" s="1"/>
       <c r="L60" s="1"/>
-      <c r="N60" s="46"/>
-      <c r="O60" s="52"/>
-      <c r="P60" s="1"/>
-      <c r="Q60" s="58"/>
-    </row>
-    <row r="61" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M60" s="60"/>
+      <c r="N60" s="81" t="s">
+        <v>215</v>
+      </c>
+      <c r="O60" s="80">
+        <v>1.0349152580000001</v>
+      </c>
+      <c r="P60" s="1">
+        <f t="shared" si="10"/>
+        <v>1.0349152580000001</v>
+      </c>
+      <c r="Q60" s="58" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
       <c r="E61" s="86"/>
-      <c r="F61" s="1"/>
       <c r="G61" s="1"/>
       <c r="H61" s="1"/>
       <c r="I61" s="1"/>
       <c r="J61" s="1"/>
-      <c r="K61" s="1"/>
+      <c r="K61" s="89"/>
       <c r="L61" s="1"/>
-      <c r="N61" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="O61" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="P61" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="Q61" s="11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="62" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="N61" s="46"/>
+      <c r="O61" s="52"/>
+      <c r="P61" s="1"/>
+      <c r="Q61" s="58"/>
+    </row>
+    <row r="62" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -4931,52 +4974,49 @@
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
       <c r="J62" s="1"/>
-      <c r="K62" s="1"/>
+      <c r="K62" s="89"/>
       <c r="L62" s="1"/>
-      <c r="M62" t="s">
-        <v>138</v>
-      </c>
-      <c r="N62" s="42" t="s">
-        <v>41</v>
-      </c>
-      <c r="O62" s="50">
-        <v>0</v>
-      </c>
-      <c r="P62" s="54">
-        <f>O62</f>
-        <v>0</v>
-      </c>
-      <c r="Q62" s="58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N62" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="O62" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="P62" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q62" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
       <c r="E63" s="86"/>
       <c r="F63" s="1"/>
+      <c r="G63" s="1"/>
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
       <c r="J63" s="1"/>
-      <c r="K63" s="1"/>
+      <c r="K63" s="89"/>
       <c r="L63" s="1"/>
-      <c r="M63" s="55">
-        <v>4.8611111111111112E-2</v>
+      <c r="M63" t="s">
+        <v>138</v>
       </c>
       <c r="N63" s="42" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="O63" s="50">
-        <v>1.0599999427795399</v>
+        <v>0</v>
       </c>
       <c r="P63" s="54">
         <f>O63</f>
-        <v>1.0599999427795399</v>
+        <v>0</v>
       </c>
       <c r="Q63" s="58">
-        <v>-2.9953879373185301E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.25">
@@ -4984,1032 +5024,1055 @@
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
+      <c r="E64" s="86"/>
       <c r="F64" s="1"/>
-      <c r="G64" s="1"/>
       <c r="H64" s="1"/>
       <c r="I64" s="1"/>
       <c r="J64" s="1"/>
-      <c r="K64" s="1"/>
+      <c r="K64" s="89"/>
       <c r="L64" s="1"/>
+      <c r="M64" s="55">
+        <v>4.8611111111111112E-2</v>
+      </c>
       <c r="N64" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="O64" s="50">
+        <v>1.0599999427795399</v>
+      </c>
+      <c r="P64" s="54">
+        <f>O64</f>
+        <v>1.0599999427795399</v>
+      </c>
+      <c r="Q64" s="58">
+        <v>-2.9953879373185301E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A65" s="1"/>
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
+      <c r="F65" s="1"/>
+      <c r="G65" s="1"/>
+      <c r="H65" s="1"/>
+      <c r="I65" s="1"/>
+      <c r="J65" s="1"/>
+      <c r="K65" s="89"/>
+      <c r="L65" s="1"/>
+      <c r="N65" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="O64" s="50">
+      <c r="O65" s="50">
         <v>156.440731910842</v>
       </c>
-      <c r="P64" s="1">
-        <f>O64/100</f>
+      <c r="P65" s="1">
+        <f>O65/100</f>
         <v>1.56440731910842</v>
       </c>
-      <c r="Q64" s="58">
+      <c r="Q65" s="58">
         <v>-8.6738403137775998E-6</v>
       </c>
     </row>
-    <row r="65" spans="13:17" x14ac:dyDescent="0.25">
-      <c r="N65" s="42" t="s">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N66" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="O65" s="50">
+      <c r="O66" s="50">
         <v>-20.300935880694301</v>
       </c>
-      <c r="P65" s="1">
-        <f t="shared" ref="P65:P71" si="11">O65/100</f>
+      <c r="P66" s="1">
+        <f t="shared" ref="P66:P72" si="11">O66/100</f>
         <v>-0.20300935880694301</v>
       </c>
-      <c r="Q65" s="58">
+      <c r="Q66" s="58">
         <v>2.1648716178694401E-3</v>
       </c>
     </row>
-    <row r="66" spans="13:17" x14ac:dyDescent="0.25">
-      <c r="N66" s="42" t="s">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N67" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="O66" s="50">
+      <c r="O67" s="50">
         <v>75.916881283268793</v>
       </c>
-      <c r="P66" s="1">
+      <c r="P67" s="1">
         <f t="shared" si="11"/>
         <v>0.75916881283268789</v>
       </c>
-      <c r="Q66" s="58">
+      <c r="Q67" s="58">
         <v>6.4758759358596297E-4</v>
       </c>
     </row>
-    <row r="67" spans="13:17" x14ac:dyDescent="0.25">
-      <c r="N67" s="42" t="s">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N68" s="42" t="s">
         <v>117</v>
       </c>
-      <c r="O67" s="50">
+      <c r="O68" s="50">
         <v>-0.155506560051652</v>
       </c>
-      <c r="P67" s="1">
+      <c r="P68" s="1">
         <f t="shared" si="11"/>
         <v>-1.55506560051652E-3</v>
       </c>
-      <c r="Q67" s="58">
+      <c r="Q68" s="58">
         <v>-1.47979634931223E-3</v>
       </c>
     </row>
-    <row r="68" spans="13:17" x14ac:dyDescent="0.25">
-      <c r="N68" s="42" t="s">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N69" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="O68" s="50">
+      <c r="O69" s="50">
         <v>41.338725991097199</v>
       </c>
-      <c r="P68" s="1">
+      <c r="P69" s="1">
         <f t="shared" si="11"/>
         <v>0.41338725991097197</v>
       </c>
-      <c r="Q68" s="58">
+      <c r="Q69" s="58">
         <v>6.8870384835700903E-4</v>
       </c>
     </row>
-    <row r="69" spans="13:17" x14ac:dyDescent="0.25">
-      <c r="N69" s="42" t="s">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N70" s="42" t="s">
         <v>118</v>
       </c>
-      <c r="O69" s="50">
+      <c r="O70" s="50">
         <v>-3.8398609004379098</v>
       </c>
-      <c r="P69" s="1">
+      <c r="P70" s="1">
         <f t="shared" si="11"/>
         <v>-3.8398609004379101E-2</v>
       </c>
-      <c r="Q69" s="58">
+      <c r="Q70" s="58">
         <v>-1.3891657030102901E-3</v>
       </c>
     </row>
-    <row r="70" spans="13:17" x14ac:dyDescent="0.25">
-      <c r="N70" s="42" t="s">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N71" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="O70" s="50">
+      <c r="O71" s="50">
         <v>232.35762119293199</v>
       </c>
-      <c r="P70" s="1">
+      <c r="P71" s="1">
         <f t="shared" si="11"/>
         <v>2.32357621192932</v>
       </c>
-      <c r="Q70" s="58">
+      <c r="Q71" s="58">
         <v>6.3899375327158804E-4</v>
       </c>
     </row>
-    <row r="71" spans="13:17" x14ac:dyDescent="0.25">
-      <c r="N71" s="42" t="s">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N72" s="42" t="s">
         <v>83</v>
       </c>
-      <c r="O71" s="50">
+      <c r="O72" s="50">
         <v>-20.456442236900301</v>
       </c>
-      <c r="P71" s="1">
+      <c r="P72" s="1">
         <f t="shared" si="11"/>
         <v>-0.20456442236900302</v>
       </c>
-      <c r="Q71" s="58">
+      <c r="Q72" s="58">
         <v>6.8507826856001298E-4</v>
       </c>
     </row>
-    <row r="72" spans="13:17" x14ac:dyDescent="0.25">
-      <c r="M72" t="s">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M73" t="s">
         <v>139</v>
       </c>
-      <c r="N72" s="42" t="s">
+      <c r="N73" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="O72" s="50">
+      <c r="O73" s="50">
         <v>-0.22125272217770001</v>
-      </c>
-      <c r="P72" s="54">
-        <f>O72</f>
-        <v>-0.22125272217770001</v>
-      </c>
-      <c r="Q72" s="59">
-        <v>-0.2212527222</v>
-      </c>
-    </row>
-    <row r="73" spans="13:17" x14ac:dyDescent="0.25">
-      <c r="M73" s="55">
-        <v>0.47083333333333338</v>
-      </c>
-      <c r="N73" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="O73" s="50">
-        <v>1.0099999973080001</v>
       </c>
       <c r="P73" s="54">
         <f>O73</f>
+        <v>-0.22125272217770001</v>
+      </c>
+      <c r="Q73" s="59">
+        <v>-0.2212527222</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M74" s="55">
+        <v>0.47083333333333338</v>
+      </c>
+      <c r="N74" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="O74" s="50">
         <v>1.0099999973080001</v>
       </c>
-      <c r="Q73" s="59">
+      <c r="P74" s="54">
+        <f>O74</f>
+        <v>1.0099999973080001</v>
+      </c>
+      <c r="Q74" s="59">
         <v>2.17540256007367E-2</v>
       </c>
     </row>
-    <row r="74" spans="13:17" x14ac:dyDescent="0.25">
-      <c r="N74" s="42" t="s">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N75" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="O74" s="50">
+      <c r="O75" s="50">
         <v>-23.569740833506799</v>
       </c>
-      <c r="P74" s="1">
-        <f>O74/100</f>
+      <c r="P75" s="1">
+        <f>O75/100</f>
         <v>-0.235697408335068</v>
       </c>
-      <c r="Q74" s="58">
+      <c r="Q75" s="58">
         <v>-1.05523560178061E-3</v>
       </c>
     </row>
-    <row r="75" spans="13:17" x14ac:dyDescent="0.25">
-      <c r="N75" s="42" t="s">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N76" s="42" t="s">
         <v>119</v>
       </c>
-      <c r="O75" s="50">
+      <c r="O76" s="50">
         <v>0.96859150246414105</v>
       </c>
-      <c r="P75" s="1">
-        <f t="shared" ref="P75:P79" si="12">O75/100</f>
+      <c r="P76" s="1">
+        <f t="shared" ref="P76:P80" si="12">O76/100</f>
         <v>9.6859150246414102E-3</v>
       </c>
-      <c r="Q75" s="58">
+      <c r="Q76" s="58">
         <v>-2.2375145874756201E-3</v>
       </c>
     </row>
-    <row r="76" spans="13:17" x14ac:dyDescent="0.25">
-      <c r="N76" s="42" t="s">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N77" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="O76" s="50">
+      <c r="O77" s="50">
         <v>29.247688021076399</v>
       </c>
-      <c r="P76" s="1">
+      <c r="P77" s="1">
         <f t="shared" si="12"/>
         <v>0.29247688021076401</v>
       </c>
-      <c r="Q76" s="58">
+      <c r="Q77" s="58">
         <v>5.1585990707936401E-4</v>
       </c>
     </row>
-    <row r="77" spans="13:17" x14ac:dyDescent="0.25">
-      <c r="N77" s="42" t="s">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N78" s="42" t="s">
         <v>120</v>
       </c>
-      <c r="O77" s="50">
+      <c r="O78" s="50">
         <v>-10.134384235994199</v>
       </c>
-      <c r="P77" s="1">
+      <c r="P78" s="1">
         <f t="shared" si="12"/>
         <v>-0.101343842359942</v>
       </c>
-      <c r="Q77" s="58">
+      <c r="Q78" s="58">
         <v>-2.7105327863768802E-3</v>
       </c>
     </row>
-    <row r="78" spans="13:17" x14ac:dyDescent="0.25">
-      <c r="N78" s="42" t="s">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N79" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="O78" s="50">
+      <c r="O79" s="50">
         <v>4.9388912162000001E-5</v>
       </c>
-      <c r="P78" s="1">
+      <c r="P79" s="1">
         <f t="shared" si="12"/>
         <v>4.9388912162000003E-7</v>
       </c>
-      <c r="Q78" s="58">
+      <c r="Q79" s="58">
         <v>6.5059278082477401E-7</v>
       </c>
     </row>
-    <row r="79" spans="13:17" x14ac:dyDescent="0.25">
-      <c r="N79" s="42" t="s">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N80" s="42" t="s">
         <v>121</v>
       </c>
-      <c r="O79" s="50">
+      <c r="O80" s="50">
         <v>-23.1382548362844</v>
       </c>
-      <c r="P79" s="1">
+      <c r="P80" s="1">
         <f t="shared" si="12"/>
         <v>-0.231382548362844</v>
       </c>
-      <c r="Q79" s="58">
+      <c r="Q80" s="58">
         <v>1.7465773008429299E-7</v>
       </c>
     </row>
-    <row r="80" spans="13:17" x14ac:dyDescent="0.25">
-      <c r="M80" t="s">
+    <row r="81" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="M81" t="s">
         <v>140</v>
       </c>
-      <c r="N80" s="42" t="s">
+      <c r="N81" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="O80" s="50">
+      <c r="O81" s="50">
         <v>-0.25510563387813501</v>
-      </c>
-      <c r="P80" s="54">
-        <f>O80</f>
-        <v>-0.25510563387813501</v>
-      </c>
-      <c r="Q80" s="59">
-        <v>-0.25510563390000002</v>
-      </c>
-    </row>
-    <row r="81" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="M81" s="55">
-        <v>0.8125</v>
-      </c>
-      <c r="N81" s="42" t="s">
-        <v>114</v>
-      </c>
-      <c r="O81" s="50">
-        <v>1.0385379019832599</v>
       </c>
       <c r="P81" s="54">
         <f>O81</f>
+        <v>-0.25510563387813501</v>
+      </c>
+      <c r="Q81" s="59">
+        <v>-0.25510563390000002</v>
+      </c>
+    </row>
+    <row r="82" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="M82" s="55">
+        <v>0.8125</v>
+      </c>
+      <c r="N82" s="42" t="s">
+        <v>114</v>
+      </c>
+      <c r="O82" s="50">
         <v>1.0385379019832599</v>
       </c>
-      <c r="Q81" s="59">
+      <c r="P82" s="54">
+        <f>O82</f>
+        <v>1.0385379019832599</v>
+      </c>
+      <c r="Q82" s="59">
         <v>-5.12238863404413E-3</v>
-      </c>
-    </row>
-    <row r="82" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="N82" s="42" t="s">
-        <v>56</v>
-      </c>
-      <c r="O82" s="50">
-        <v>6.4193752642371704</v>
-      </c>
-      <c r="P82" s="1">
-        <f>O82/100</f>
-        <v>6.4193752642371704E-2</v>
-      </c>
-      <c r="Q82" s="58">
-        <v>1.2851248455257599E-4</v>
       </c>
     </row>
     <row r="83" spans="9:17" x14ac:dyDescent="0.25">
       <c r="N83" s="42" t="s">
-        <v>123</v>
+        <v>56</v>
       </c>
       <c r="O83" s="50">
-        <v>1.57798981550307</v>
+        <v>6.4193752642371704</v>
       </c>
       <c r="P83" s="1">
-        <f t="shared" ref="P83:P91" si="13">O83/100</f>
-        <v>1.5779898155030701E-2</v>
+        <f>O83/100</f>
+        <v>6.4193752642371704E-2</v>
       </c>
       <c r="Q83" s="58">
-        <v>1.0767413611616999E-3</v>
+        <v>1.2851248455257599E-4</v>
       </c>
     </row>
     <row r="84" spans="9:17" x14ac:dyDescent="0.25">
       <c r="N84" s="42" t="s">
+        <v>123</v>
+      </c>
+      <c r="O84" s="50">
+        <v>1.57798981550307</v>
+      </c>
+      <c r="P84" s="1">
+        <f t="shared" ref="P84:P92" si="13">O84/100</f>
+        <v>1.5779898155030701E-2</v>
+      </c>
+      <c r="Q84" s="58">
+        <v>1.0767413611616999E-3</v>
+      </c>
+    </row>
+    <row r="85" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="N85" s="42" t="s">
         <v>57</v>
       </c>
-      <c r="O84" s="50">
+      <c r="O85" s="50">
         <v>7.6111237412808599</v>
       </c>
-      <c r="P84" s="1">
+      <c r="P85" s="1">
         <f t="shared" si="13"/>
         <v>7.6111237412808605E-2</v>
       </c>
-      <c r="Q84" s="58">
+      <c r="Q85" s="58">
         <v>1.6297137374082799E-5</v>
       </c>
     </row>
-    <row r="85" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="N85" s="42" t="s">
+    <row r="86" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="N86" s="42" t="s">
         <v>122</v>
       </c>
-      <c r="O85" s="50">
+      <c r="O86" s="50">
         <v>2.2749299623984598</v>
       </c>
-      <c r="P85" s="1">
+      <c r="P86" s="1">
         <f t="shared" si="13"/>
         <v>2.2749299623984597E-2</v>
       </c>
-      <c r="Q85" s="58">
+      <c r="Q86" s="58">
         <v>9.80565804585901E-5</v>
       </c>
     </row>
-    <row r="86" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="N86" s="42" t="s">
+    <row r="87" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="N87" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="O86" s="50">
+      <c r="O87" s="50">
         <v>17.236621109828601</v>
       </c>
-      <c r="P86" s="1">
+      <c r="P87" s="1">
         <f t="shared" si="13"/>
         <v>0.17236621109828601</v>
       </c>
-      <c r="Q86" s="58">
+      <c r="Q87" s="58">
         <v>2.8072391037720099E-5</v>
       </c>
     </row>
-    <row r="87" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="N87" s="42" t="s">
+    <row r="88" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="N88" s="42" t="s">
         <v>124</v>
       </c>
-      <c r="O87" s="50">
+      <c r="O88" s="50">
         <v>6.2088690408799696</v>
       </c>
-      <c r="P87" s="1">
+      <c r="P88" s="1">
         <f t="shared" si="13"/>
         <v>6.2088690408799697E-2</v>
       </c>
-      <c r="Q87" s="58">
+      <c r="Q88" s="58">
         <v>3.8053003130694002E-4</v>
       </c>
     </row>
-    <row r="88" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="N88" s="42" t="s">
+    <row r="89" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="N89" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="O88" s="50">
+      <c r="O89" s="50">
         <v>1.4392071686730901</v>
       </c>
-      <c r="P88" s="1">
+      <c r="P89" s="1">
         <f t="shared" si="13"/>
         <v>1.4392071686730901E-2</v>
       </c>
-      <c r="Q88" s="58">
+      <c r="Q89" s="58">
         <v>3.3901950999533699E-5</v>
       </c>
     </row>
-    <row r="89" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="N89" s="42" t="s">
+    <row r="90" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="N90" s="42" t="s">
         <v>125</v>
       </c>
-      <c r="O89" s="50">
+      <c r="O90" s="50">
         <v>0.52526799870488805</v>
       </c>
-      <c r="P89" s="1">
+      <c r="P90" s="1">
         <f t="shared" si="13"/>
         <v>5.2526799870488807E-3</v>
       </c>
-      <c r="Q89" s="58">
+      <c r="Q90" s="58">
         <v>9.7871725652031802E-5</v>
       </c>
     </row>
-    <row r="90" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="N90" s="42" t="s">
+    <row r="91" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="N91" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="O90" s="50">
+      <c r="O91" s="50">
         <v>-6.1</v>
       </c>
-      <c r="P90" s="1">
+      <c r="P91" s="1">
         <f t="shared" si="13"/>
         <v>-6.0999999999999999E-2</v>
       </c>
-      <c r="Q90" s="58">
+      <c r="Q91" s="58">
         <v>-5.5804864002167998E-6</v>
       </c>
     </row>
-    <row r="91" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="N91" s="42" t="s">
+    <row r="92" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="N92" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="O91" s="50">
+      <c r="O92" s="50">
         <v>-1.6</v>
       </c>
-      <c r="P91" s="1">
+      <c r="P92" s="1">
         <f t="shared" si="13"/>
         <v>-1.6E-2</v>
       </c>
-      <c r="Q91" s="58">
+      <c r="Q92" s="58">
         <v>5.2797756594065403E-5</v>
       </c>
     </row>
-    <row r="92" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="M92" t="s">
+    <row r="93" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="M93" t="s">
         <v>141</v>
       </c>
-      <c r="N92" s="42" t="s">
+      <c r="N93" s="42" t="s">
         <v>60</v>
       </c>
-      <c r="O92" s="50">
+      <c r="O93" s="50">
         <v>-0.26806990591321</v>
-      </c>
-      <c r="P92" s="54">
-        <f>O92</f>
-        <v>-0.26806990591321</v>
-      </c>
-      <c r="Q92" s="59">
-        <v>-0.26806990590000002</v>
-      </c>
-    </row>
-    <row r="93" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="J93" s="72" t="s">
-        <v>208</v>
-      </c>
-      <c r="M93" s="56" t="s">
-        <v>146</v>
-      </c>
-      <c r="N93" s="42" t="s">
-        <v>115</v>
-      </c>
-      <c r="O93" s="50">
-        <v>1.0349152577221601</v>
       </c>
       <c r="P93" s="54">
         <f>O93</f>
-        <v>1.0349152577221601</v>
+        <v>-0.26806990591321</v>
       </c>
       <c r="Q93" s="59">
-        <v>-2.1765958813597698E-3</v>
+        <v>-0.26806990590000002</v>
       </c>
     </row>
     <row r="94" spans="9:17" x14ac:dyDescent="0.25">
       <c r="J94" s="72" t="s">
+        <v>208</v>
+      </c>
+      <c r="M94" s="56" t="s">
+        <v>146</v>
+      </c>
+      <c r="N94" s="42" t="s">
+        <v>115</v>
+      </c>
+      <c r="O94" s="50">
+        <v>1.0349152577221601</v>
+      </c>
+      <c r="P94" s="54">
+        <f>O94</f>
+        <v>1.0349152577221601</v>
+      </c>
+      <c r="Q94" s="59">
+        <v>-2.1765958813597698E-3</v>
+      </c>
+    </row>
+    <row r="95" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="J95" s="72" t="s">
         <v>209</v>
-      </c>
-      <c r="M94" s="47"/>
-      <c r="N94" s="42" t="s">
-        <v>61</v>
-      </c>
-      <c r="O94" s="50">
-        <v>6.1481308294477897</v>
-      </c>
-      <c r="P94" s="1">
-        <f>O94/100</f>
-        <v>6.1481308294477899E-2</v>
-      </c>
-      <c r="Q94" s="57">
-        <v>-1.88116567434796E-5</v>
-      </c>
-    </row>
-    <row r="95" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I95">
-        <v>1</v>
-      </c>
-      <c r="J95" s="72">
-        <v>1.0599999427795399</v>
       </c>
       <c r="M95" s="47"/>
       <c r="N95" s="42" t="s">
-        <v>126</v>
+        <v>61</v>
       </c>
       <c r="O95" s="50">
-        <v>6.1776975079165704</v>
+        <v>6.1481308294477897</v>
       </c>
       <c r="P95" s="1">
-        <f t="shared" ref="P95:P107" si="14">O95/100</f>
-        <v>6.1776975079165707E-2</v>
+        <f>O95/100</f>
+        <v>6.1481308294477899E-2</v>
       </c>
       <c r="Q95" s="57">
-        <v>-4.4567340559324698E-4</v>
+        <v>-1.88116567434796E-5</v>
       </c>
     </row>
     <row r="96" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I96">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J96" s="72">
-        <v>1.04499995797579</v>
+        <v>1.0599999427795399</v>
       </c>
       <c r="M96" s="47"/>
       <c r="N96" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="O96" s="50">
+        <v>6.1776975079165704</v>
+      </c>
+      <c r="P96" s="1">
+        <f t="shared" ref="P96:P108" si="14">O96/100</f>
+        <v>6.1776975079165707E-2</v>
+      </c>
+      <c r="Q96" s="57">
+        <v>-4.4567340559324698E-4</v>
+      </c>
+    </row>
+    <row r="97" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="I97">
+        <v>2</v>
+      </c>
+      <c r="J97" s="72">
+        <v>1.04499995797579</v>
+      </c>
+      <c r="M97" s="47"/>
+      <c r="N97" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="O96" s="50">
+      <c r="O97" s="50">
         <v>10.1258308263922</v>
       </c>
-      <c r="P96" s="1">
+      <c r="P97" s="1">
         <f t="shared" si="14"/>
         <v>0.101258308263922</v>
       </c>
-      <c r="Q96" s="58">
+      <c r="Q97" s="58">
         <v>-1.40656940313608E-4</v>
       </c>
     </row>
-    <row r="97" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I97">
+    <row r="98" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="I98">
         <v>3</v>
       </c>
-      <c r="J97" s="72">
+      <c r="J98" s="72">
         <v>1.0099999973080001</v>
       </c>
-      <c r="M97" s="47"/>
-      <c r="N97" s="42" t="s">
+      <c r="M98" s="47"/>
+      <c r="N98" s="42" t="s">
         <v>127</v>
       </c>
-      <c r="O97" s="50">
+      <c r="O98" s="50">
         <v>4.8779939913553596</v>
       </c>
-      <c r="P97" s="1">
+      <c r="P98" s="1">
         <f t="shared" si="14"/>
         <v>4.8779939913553595E-2</v>
       </c>
-      <c r="Q97" s="57">
+      <c r="Q98" s="57">
         <v>-6.3339605935184401E-4</v>
       </c>
     </row>
-    <row r="98" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I98">
+    <row r="99" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="I99">
         <v>4</v>
       </c>
-      <c r="J98" s="72">
+      <c r="J99" s="72">
         <v>1.02371286456331</v>
       </c>
-      <c r="M98" t="s">
+      <c r="M99" t="s">
         <v>142</v>
       </c>
-      <c r="N98" s="42" t="s">
+      <c r="N99" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="O98" s="50">
+      <c r="O99" s="50">
         <v>-7.6</v>
       </c>
-      <c r="P98" s="1">
+      <c r="P99" s="1">
         <f t="shared" si="14"/>
         <v>-7.5999999999999998E-2</v>
       </c>
-      <c r="Q98" s="58">
+      <c r="Q99" s="58">
         <v>-1.4483820858600399E-4</v>
       </c>
     </row>
-    <row r="99" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I99">
+    <row r="100" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="I100">
         <v>5</v>
       </c>
-      <c r="J99" s="72">
+      <c r="J100" s="72">
         <v>1.0280925147905799</v>
       </c>
-      <c r="M99" s="56" t="s">
+      <c r="M100" s="56" t="s">
         <v>147</v>
       </c>
-      <c r="N99" s="42" t="s">
+      <c r="N100" s="42" t="s">
         <v>128</v>
       </c>
-      <c r="O99" s="50">
+      <c r="O100" s="50">
         <v>-1.6</v>
       </c>
-      <c r="P99" s="1">
+      <c r="P100" s="1">
         <f t="shared" si="14"/>
         <v>-1.6E-2</v>
       </c>
-      <c r="Q99" s="58">
+      <c r="Q100" s="58">
         <v>-3.5573742834272E-3</v>
       </c>
     </row>
-    <row r="100" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I100">
+    <row r="101" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="I101">
         <v>6</v>
       </c>
-      <c r="J100" s="72">
+      <c r="J101" s="72">
         <v>1.0385379019832599</v>
       </c>
-      <c r="M100" t="s">
+      <c r="M101" t="s">
         <v>143</v>
       </c>
-      <c r="N100" s="42" t="s">
+      <c r="N101" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="O100" s="51">
+      <c r="O101" s="51">
         <v>-63.001699846354903</v>
       </c>
-      <c r="P100" s="1">
+      <c r="P101" s="1">
         <f t="shared" si="14"/>
         <v>-0.63001699846354908</v>
       </c>
-      <c r="Q100" s="58">
+      <c r="Q101" s="58">
         <v>-9.5060452610995505E-4</v>
       </c>
     </row>
-    <row r="101" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I101">
+    <row r="102" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="I102">
         <v>7</v>
       </c>
-      <c r="J101" s="72">
+      <c r="J102" s="72">
         <v>1.04612245201456</v>
       </c>
-      <c r="M101" s="56" t="s">
+      <c r="M102" s="56" t="s">
         <v>148</v>
       </c>
-      <c r="N101" s="42" t="s">
+      <c r="N102" s="42" t="s">
         <v>129</v>
       </c>
-      <c r="O101" s="50">
+      <c r="O102" s="50">
         <v>10.2039485868599</v>
       </c>
-      <c r="P101" s="1">
+      <c r="P102" s="1">
         <f t="shared" si="14"/>
         <v>0.102039485868599</v>
       </c>
-      <c r="Q101" s="58">
+      <c r="Q102" s="58">
         <v>-5.1145973996759402E-3</v>
       </c>
     </row>
-    <row r="102" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I102">
+    <row r="103" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="I103">
         <v>8</v>
       </c>
-      <c r="J102" s="72">
+      <c r="J103" s="72">
         <v>1.0850835071553799</v>
       </c>
-      <c r="N102" s="42" t="s">
+      <c r="N103" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="O102" s="50">
+      <c r="O103" s="50">
         <v>16.526211548050401</v>
       </c>
-      <c r="P102" s="1">
+      <c r="P103" s="1">
         <f t="shared" si="14"/>
         <v>0.16526211548050401</v>
       </c>
-      <c r="Q102" s="58">
+      <c r="Q103" s="58">
         <v>3.0418249791705498E-4</v>
       </c>
     </row>
-    <row r="103" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I103">
+    <row r="104" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="I104">
         <v>9</v>
       </c>
-      <c r="J103" s="72">
+      <c r="J104" s="72">
         <v>1.0349152577221601</v>
       </c>
-      <c r="N103" s="42" t="s">
+      <c r="N104" s="42" t="s">
         <v>130</v>
       </c>
-      <c r="O103" s="52">
+      <c r="O104" s="52">
         <v>-1.34369314780613</v>
       </c>
-      <c r="P103" s="1">
+      <c r="P104" s="1">
         <f t="shared" si="14"/>
         <v>-1.34369314780613E-2</v>
       </c>
-      <c r="Q103" s="58">
+      <c r="Q104" s="58">
         <v>-1.37670401876801E-3</v>
       </c>
     </row>
-    <row r="104" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I104">
+    <row r="105" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="I105">
         <v>10</v>
       </c>
-      <c r="J104" s="72">
+      <c r="J105" s="72">
         <v>1.02798621556374</v>
       </c>
-      <c r="N104" s="42" t="s">
+      <c r="N105" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="O104" s="52">
+      <c r="O105" s="52">
         <v>29.247637436823101</v>
       </c>
-      <c r="P104" s="1">
+      <c r="P105" s="1">
         <f t="shared" si="14"/>
         <v>0.29247637436823104</v>
       </c>
-      <c r="Q104" s="58">
+      <c r="Q105" s="58">
         <v>2.2761940039589499E-4</v>
       </c>
     </row>
-    <row r="105" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I105">
+    <row r="106" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="I106">
         <v>11</v>
       </c>
-      <c r="J105" s="72">
+      <c r="J106" s="72">
         <v>1.02970205350408</v>
       </c>
-      <c r="N105" s="42" t="s">
+      <c r="N106" s="42" t="s">
         <v>131</v>
       </c>
-      <c r="O105" s="52">
+      <c r="O106" s="52">
         <v>11.0919776937066</v>
       </c>
-      <c r="P105" s="1">
+      <c r="P106" s="1">
         <f t="shared" si="14"/>
         <v>0.11091977693706599</v>
       </c>
-      <c r="Q105" s="58">
+      <c r="Q106" s="58">
         <v>-1.3983824680780001E-3</v>
       </c>
     </row>
-    <row r="106" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I106">
+    <row r="107" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="I107">
         <v>12</v>
       </c>
-      <c r="J106" s="72">
+      <c r="J107" s="72">
         <v>1.0240525230119499</v>
       </c>
-      <c r="N106" s="42" t="s">
+      <c r="N107" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="O106" s="53">
+      <c r="O107" s="53">
         <v>-94.199996999999996</v>
       </c>
-      <c r="P106" s="1">
+      <c r="P107" s="1">
         <f t="shared" si="14"/>
         <v>-0.94199996999999991</v>
       </c>
-      <c r="Q106" s="58">
+      <c r="Q107" s="58">
         <v>-2.81965662445027E-3</v>
       </c>
     </row>
-    <row r="107" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I107">
+    <row r="108" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="I108">
         <v>13</v>
       </c>
-      <c r="J107" s="72">
+      <c r="J108" s="72">
         <v>1.01992383631813</v>
       </c>
-      <c r="N107" s="42" t="s">
+      <c r="N108" s="42" t="s">
         <v>132</v>
       </c>
-      <c r="O107">
+      <c r="O108">
         <f>21.4613437652587-19</f>
         <v>2.4613437652587002</v>
       </c>
-      <c r="P107" s="1">
+      <c r="P108" s="1">
         <f t="shared" si="14"/>
         <v>2.4613437652587004E-2</v>
       </c>
-      <c r="Q107" s="58">
+      <c r="Q108" s="58">
         <v>-6.8701998242329402E-3</v>
       </c>
     </row>
-    <row r="108" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I108">
+    <row r="109" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="I109">
         <v>14</v>
       </c>
-      <c r="J108" s="72">
+      <c r="J109" s="72">
         <v>1.00994172446495</v>
       </c>
-      <c r="N108" s="42" t="s">
+      <c r="N109" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="O108" s="52">
+      <c r="O109" s="52">
         <v>-0.22125272217770001</v>
-      </c>
-      <c r="P108" s="54">
-        <f>O108</f>
-        <v>-0.22125272217770001</v>
-      </c>
-      <c r="Q108" s="59">
-        <v>-0.2212527222</v>
-      </c>
-    </row>
-    <row r="109" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="N109" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="O109" s="52">
-        <v>1.0099999973080001</v>
       </c>
       <c r="P109" s="54">
         <f>O109</f>
+        <v>-0.22125272217770001</v>
+      </c>
+      <c r="Q109" s="59">
+        <v>-0.2212527222</v>
+      </c>
+    </row>
+    <row r="110" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="N110" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="O110" s="52">
         <v>1.0099999973080001</v>
       </c>
-      <c r="Q109" s="59">
+      <c r="P110" s="54">
+        <f>O110</f>
+        <v>1.0099999973080001</v>
+      </c>
+      <c r="Q110" s="59">
         <v>2.17540256007367E-2</v>
       </c>
     </row>
-    <row r="110" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="M110" t="s">
+    <row r="111" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="M111" t="s">
         <v>144</v>
       </c>
-      <c r="N110" s="42" t="s">
+      <c r="N111" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="O110" s="52">
+      <c r="O111" s="52">
         <v>4.9650161007164098</v>
       </c>
-      <c r="P110" s="1">
-        <f>O110/100</f>
+      <c r="P111" s="1">
+        <f>O111/100</f>
         <v>4.9650161007164101E-2</v>
       </c>
-      <c r="Q110" s="58">
+      <c r="Q111" s="58">
         <v>1.15284947015369E-4</v>
       </c>
     </row>
-    <row r="111" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="M111" s="56" t="s">
+    <row r="112" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="M112" s="56" t="s">
         <v>149</v>
       </c>
-      <c r="N111" s="42" t="s">
+      <c r="N112" s="42" t="s">
         <v>133</v>
       </c>
-      <c r="O111" s="52">
+      <c r="O112" s="52">
         <v>0.52427629116916796</v>
       </c>
-      <c r="P111" s="1">
-        <f t="shared" ref="P111:P113" si="15">O111/100</f>
+      <c r="P112" s="1">
+        <f t="shared" ref="P112:P114" si="15">O112/100</f>
         <v>5.2427629116916794E-3</v>
       </c>
-      <c r="Q111" s="58">
+      <c r="Q112" s="58">
         <v>6.2348925580496799E-4</v>
       </c>
     </row>
-    <row r="112" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="N112" s="42" t="s">
+    <row r="113" spans="13:17" x14ac:dyDescent="0.25">
+      <c r="N113" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="O112" s="52">
+      <c r="O113" s="52">
         <v>-13.5</v>
       </c>
-      <c r="P112" s="1">
+      <c r="P113" s="1">
         <f t="shared" si="15"/>
         <v>-0.13500000000000001</v>
       </c>
-      <c r="Q112" s="58">
+      <c r="Q113" s="58">
         <v>-1.30914832287277E-5</v>
       </c>
     </row>
-    <row r="113" spans="13:17" x14ac:dyDescent="0.25">
-      <c r="N113" s="42" t="s">
+    <row r="114" spans="13:17" x14ac:dyDescent="0.25">
+      <c r="N114" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="O113" s="52">
+      <c r="O114" s="52">
         <v>-5.8</v>
       </c>
-      <c r="P113" s="1">
+      <c r="P114" s="1">
         <f t="shared" si="15"/>
         <v>-5.7999999999999996E-2</v>
       </c>
-      <c r="Q113" s="58">
+      <c r="Q114" s="58">
         <v>1.15841086511394E-4</v>
-      </c>
-    </row>
-    <row r="114" spans="13:17" x14ac:dyDescent="0.25">
-      <c r="N114" s="42" t="s">
-        <v>55</v>
-      </c>
-      <c r="O114" s="52">
-        <v>-0.25510563387813501</v>
-      </c>
-      <c r="P114" s="54">
-        <f>O114</f>
-        <v>-0.25510563387813501</v>
-      </c>
-      <c r="Q114" s="59">
-        <v>-0.25510563390000002</v>
       </c>
     </row>
     <row r="115" spans="13:17" x14ac:dyDescent="0.25">
       <c r="N115" s="42" t="s">
-        <v>114</v>
+        <v>55</v>
       </c>
       <c r="O115" s="52">
-        <v>1.0385379019832599</v>
+        <v>-0.25510563387813501</v>
       </c>
       <c r="P115" s="54">
         <f>O115</f>
+        <v>-0.25510563387813501</v>
+      </c>
+      <c r="Q115" s="59">
+        <v>-0.25510563390000002</v>
+      </c>
+    </row>
+    <row r="116" spans="13:17" x14ac:dyDescent="0.25">
+      <c r="N116" s="42" t="s">
+        <v>114</v>
+      </c>
+      <c r="O116" s="52">
         <v>1.0385379019832599</v>
       </c>
-      <c r="Q115" s="59">
+      <c r="P116" s="54">
+        <f>O116</f>
+        <v>1.0385379019832599</v>
+      </c>
+      <c r="Q116" s="59">
         <v>-5.12238863404413E-3</v>
       </c>
     </row>
-    <row r="116" spans="13:17" x14ac:dyDescent="0.25">
-      <c r="M116" t="s">
+    <row r="117" spans="13:17" x14ac:dyDescent="0.25">
+      <c r="M117" t="s">
         <v>145</v>
       </c>
-      <c r="N116" s="42" t="s">
+      <c r="N117" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="O116" s="52">
+      <c r="O117" s="52">
         <v>-2.8744036925517298</v>
       </c>
-      <c r="P116" s="1">
-        <f>O116/100</f>
+      <c r="P117" s="1">
+        <f>O117/100</f>
         <v>-2.8744036925517299E-2</v>
       </c>
-      <c r="Q116" s="58">
+      <c r="Q117" s="58">
         <v>-9.7142222335186394E-5</v>
       </c>
     </row>
-    <row r="117" spans="13:17" x14ac:dyDescent="0.25">
-      <c r="M117" s="56" t="s">
+    <row r="118" spans="13:17" x14ac:dyDescent="0.25">
+      <c r="M118" s="56" t="s">
         <v>150</v>
       </c>
-      <c r="N117" s="42" t="s">
+      <c r="N118" s="42" t="s">
         <v>134</v>
       </c>
-      <c r="O117" s="52">
+      <c r="O118" s="52">
         <v>0.31779049296478201</v>
       </c>
-      <c r="P117" s="1">
-        <f t="shared" ref="P117:P119" si="16">O117/100</f>
+      <c r="P118" s="1">
+        <f t="shared" ref="P118:P120" si="16">O118/100</f>
         <v>3.1779049296478202E-3</v>
       </c>
-      <c r="Q117" s="58">
+      <c r="Q118" s="58">
         <v>-1.0332946463634299E-3</v>
       </c>
     </row>
-    <row r="118" spans="13:17" x14ac:dyDescent="0.25">
-      <c r="N118" s="42" t="s">
+    <row r="119" spans="13:17" x14ac:dyDescent="0.25">
+      <c r="N119" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="O118" s="52">
+      <c r="O119" s="52">
         <v>-14.9</v>
       </c>
-      <c r="P118" s="1">
+      <c r="P119" s="1">
         <f t="shared" si="16"/>
         <v>-0.14899999999999999</v>
       </c>
-      <c r="Q118" s="58">
+      <c r="Q119" s="58">
         <v>-4.6294745534552998E-5</v>
       </c>
     </row>
-    <row r="119" spans="13:17" x14ac:dyDescent="0.25">
-      <c r="N119" s="42" t="s">
+    <row r="120" spans="13:17" x14ac:dyDescent="0.25">
+      <c r="N120" s="42" t="s">
         <v>135</v>
       </c>
-      <c r="O119" s="52">
+      <c r="O120" s="52">
         <v>-5</v>
       </c>
-      <c r="P119" s="1">
+      <c r="P120" s="1">
         <f t="shared" si="16"/>
         <v>-0.05</v>
       </c>
-      <c r="Q119" s="58">
+      <c r="Q120" s="58">
         <v>-4.2582952991622499E-5</v>
-      </c>
-    </row>
-    <row r="120" spans="13:17" x14ac:dyDescent="0.25">
-      <c r="N120" s="42" t="s">
-        <v>60</v>
-      </c>
-      <c r="O120" s="52">
-        <v>-0.26806990591321</v>
-      </c>
-      <c r="P120" s="54">
-        <f>O120</f>
-        <v>-0.26806990591321</v>
-      </c>
-      <c r="Q120" s="59">
-        <v>-0.26806990590000002</v>
       </c>
     </row>
     <row r="121" spans="13:17" x14ac:dyDescent="0.25">
       <c r="N121" s="42" t="s">
-        <v>115</v>
+        <v>60</v>
       </c>
       <c r="O121" s="52">
-        <v>1.0349152577221601</v>
+        <v>-0.26806990591321</v>
       </c>
       <c r="P121" s="54">
         <f>O121</f>
+        <v>-0.26806990591321</v>
+      </c>
+      <c r="Q121" s="59">
+        <v>-0.26806990590000002</v>
+      </c>
+    </row>
+    <row r="122" spans="13:17" x14ac:dyDescent="0.25">
+      <c r="N122" s="42" t="s">
+        <v>115</v>
+      </c>
+      <c r="O122" s="52">
         <v>1.0349152577221601</v>
       </c>
-      <c r="Q121" s="59">
+      <c r="P122" s="54">
+        <f>O122</f>
+        <v>1.0349152577221601</v>
+      </c>
+      <c r="Q122" s="59">
         <v>-2.1765958813597698E-3</v>
       </c>
     </row>
-    <row r="122" spans="13:17" x14ac:dyDescent="0.25">
-      <c r="P122" s="1"/>
-      <c r="Q122" s="3"/>
-    </row>
     <row r="123" spans="13:17" x14ac:dyDescent="0.25">
-      <c r="N123" s="48"/>
-      <c r="O123" s="48"/>
       <c r="P123" s="1"/>
       <c r="Q123" s="3"/>
     </row>
     <row r="124" spans="13:17" x14ac:dyDescent="0.25">
       <c r="N124" s="48"/>
-      <c r="O124" s="47"/>
+      <c r="O124" s="48"/>
+      <c r="P124" s="1"/>
       <c r="Q124" s="3"/>
     </row>
     <row r="125" spans="13:17" x14ac:dyDescent="0.25">
@@ -6020,10 +6083,11 @@
     <row r="126" spans="13:17" x14ac:dyDescent="0.25">
       <c r="N126" s="48"/>
       <c r="O126" s="47"/>
+      <c r="Q126" s="3"/>
     </row>
     <row r="127" spans="13:17" x14ac:dyDescent="0.25">
-      <c r="N127" s="42"/>
-      <c r="O127" s="1"/>
+      <c r="N127" s="48"/>
+      <c r="O127" s="47"/>
     </row>
     <row r="128" spans="13:17" x14ac:dyDescent="0.25">
       <c r="N128" s="42"/>
@@ -6101,11 +6165,15 @@
       <c r="N146" s="42"/>
       <c r="O146" s="1"/>
     </row>
+    <row r="147" spans="14:15" x14ac:dyDescent="0.25">
+      <c r="N147" s="42"/>
+      <c r="O147" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A1:J1"/>
     <mergeCell ref="C2:G2"/>
-    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="H2:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="32" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -6116,9 +6184,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L50" sqref="L50"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6134,30 +6202,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="99" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="97"/>
-      <c r="D1" s="96" t="s">
+      <c r="B1" s="101"/>
+      <c r="D1" s="99" t="s">
         <v>293</v>
       </c>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98"/>
-      <c r="G1" s="98"/>
-      <c r="H1" s="98"/>
-      <c r="I1" s="98"/>
-      <c r="J1" s="97"/>
-      <c r="L1" s="96" t="s">
+      <c r="E1" s="100"/>
+      <c r="F1" s="100"/>
+      <c r="G1" s="100"/>
+      <c r="H1" s="100"/>
+      <c r="I1" s="100"/>
+      <c r="J1" s="101"/>
+      <c r="L1" s="99" t="s">
         <v>295</v>
       </c>
-      <c r="M1" s="98"/>
-      <c r="N1" s="98"/>
-      <c r="O1" s="98"/>
-      <c r="P1" s="98"/>
-      <c r="Q1" s="98"/>
-      <c r="R1" s="98"/>
-      <c r="S1" s="97"/>
-      <c r="T1" s="95"/>
+      <c r="M1" s="100"/>
+      <c r="N1" s="100"/>
+      <c r="O1" s="100"/>
+      <c r="P1" s="100"/>
+      <c r="Q1" s="100"/>
+      <c r="R1" s="100"/>
+      <c r="S1" s="101"/>
+      <c r="T1" s="90"/>
     </row>
     <row r="2" spans="1:20" s="72" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="80"/>
@@ -6706,6 +6774,9 @@
       </c>
       <c r="J19" s="72">
         <v>-0.22164303099970301</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
       </c>
       <c r="P19" s="72">
         <f t="shared" ref="P19:P25" si="1">O19*COS($O$34)+O5*SIN($O$34)</f>
@@ -7027,15 +7098,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="87" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="87"/>
-      <c r="G1" s="87"/>
+      <c r="A1" s="91" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
+      <c r="G1" s="91"/>
       <c r="I1" s="6" t="s">
         <v>1</v>
       </c>
@@ -7388,15 +7459,15 @@
       <c r="N11" s="1"/>
     </row>
     <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="88" t="s">
+      <c r="A12" s="92" t="s">
         <v>80</v>
       </c>
-      <c r="B12" s="88"/>
-      <c r="C12" s="88"/>
-      <c r="D12" s="88"/>
-      <c r="E12" s="88"/>
-      <c r="F12" s="88"/>
-      <c r="G12" s="88"/>
+      <c r="B12" s="92"/>
+      <c r="C12" s="92"/>
+      <c r="D12" s="92"/>
+      <c r="E12" s="92"/>
+      <c r="F12" s="92"/>
+      <c r="G12" s="92"/>
       <c r="I12" s="1"/>
       <c r="J12" s="6" t="s">
         <v>1</v>
@@ -7886,15 +7957,15 @@
       <c r="G31" s="1"/>
     </row>
     <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="88" t="s">
+      <c r="A32" s="92" t="s">
         <v>81</v>
       </c>
-      <c r="B32" s="88"/>
-      <c r="C32" s="88"/>
-      <c r="D32" s="88"/>
-      <c r="E32" s="88"/>
-      <c r="F32" s="88"/>
-      <c r="G32" s="88"/>
+      <c r="B32" s="92"/>
+      <c r="C32" s="92"/>
+      <c r="D32" s="92"/>
+      <c r="E32" s="92"/>
+      <c r="F32" s="92"/>
+      <c r="G32" s="92"/>
       <c r="I32" s="1"/>
       <c r="J32" s="6" t="s">
         <v>1</v>
@@ -8373,13 +8444,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="91" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
       <c r="G1" s="30" t="s">
         <v>100</v>
       </c>
@@ -8398,13 +8469,13 @@
       <c r="L1" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="P1" s="87" t="s">
+      <c r="P1" s="91" t="s">
         <v>106</v>
       </c>
-      <c r="Q1" s="87"/>
-      <c r="R1" s="87"/>
-      <c r="S1" s="87"/>
-      <c r="T1" s="87"/>
+      <c r="Q1" s="91"/>
+      <c r="R1" s="91"/>
+      <c r="S1" s="91"/>
+      <c r="T1" s="91"/>
       <c r="V1" s="30" t="s">
         <v>100</v>
       </c>
@@ -8939,12 +9010,12 @@
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="P10" s="87" t="s">
+      <c r="P10" s="91" t="s">
         <v>108</v>
       </c>
-      <c r="Q10" s="87"/>
-      <c r="R10" s="87"/>
-      <c r="S10" s="87"/>
+      <c r="Q10" s="91"/>
+      <c r="R10" s="91"/>
+      <c r="S10" s="91"/>
       <c r="T10" s="25"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
@@ -9960,12 +10031,12 @@
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A33" s="87" t="s">
+      <c r="A33" s="91" t="s">
         <v>102</v>
       </c>
-      <c r="B33" s="87"/>
-      <c r="C33" s="87"/>
-      <c r="D33" s="87"/>
+      <c r="B33" s="91"/>
+      <c r="C33" s="91"/>
+      <c r="D33" s="91"/>
       <c r="F33" s="30" t="s">
         <v>100</v>
       </c>
@@ -10343,12 +10414,12 @@
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A42" s="87" t="s">
+      <c r="A42" s="91" t="s">
         <v>104</v>
       </c>
-      <c r="B42" s="87"/>
-      <c r="C42" s="87"/>
-      <c r="D42" s="87"/>
+      <c r="B42" s="91"/>
+      <c r="C42" s="91"/>
+      <c r="D42" s="91"/>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
@@ -10847,15 +10918,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="92" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="88"/>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
-      <c r="F1" s="88"/>
-      <c r="G1" s="88"/>
+      <c r="B1" s="92"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="92"/>
+      <c r="G1" s="92"/>
       <c r="I1" s="1"/>
       <c r="J1" s="4"/>
       <c r="L1" s="4" t="s">
@@ -11917,18 +11988,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="89" t="s">
+      <c r="A1" s="93" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="89"/>
-      <c r="F1" s="89"/>
-      <c r="G1" s="89"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="89"/>
-      <c r="J1" s="89"/>
+      <c r="B1" s="93"/>
+      <c r="C1" s="93"/>
+      <c r="D1" s="93"/>
+      <c r="E1" s="93"/>
+      <c r="F1" s="93"/>
+      <c r="G1" s="93"/>
+      <c r="H1" s="93"/>
+      <c r="I1" s="93"/>
+      <c r="J1" s="93"/>
       <c r="L1" s="11" t="s">
         <v>1</v>
       </c>
@@ -11952,18 +12023,18 @@
       <c r="B2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="90" t="s">
+      <c r="C2" s="94" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90" t="s">
+      <c r="D2" s="94"/>
+      <c r="E2" s="94"/>
+      <c r="F2" s="94"/>
+      <c r="G2" s="94" t="s">
         <v>74</v>
       </c>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
+      <c r="H2" s="94"/>
+      <c r="I2" s="94"/>
+      <c r="J2" s="94"/>
       <c r="L2" s="8" t="s">
         <v>41</v>
       </c>
@@ -12756,18 +12827,18 @@
       <c r="O33" s="1"/>
     </row>
     <row r="35" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="89" t="s">
+      <c r="A35" s="93" t="s">
         <v>78</v>
       </c>
-      <c r="B35" s="89"/>
-      <c r="C35" s="89"/>
-      <c r="D35" s="89"/>
-      <c r="E35" s="89"/>
-      <c r="F35" s="89"/>
-      <c r="G35" s="89"/>
-      <c r="H35" s="89"/>
-      <c r="I35" s="89"/>
-      <c r="J35" s="89"/>
+      <c r="B35" s="93"/>
+      <c r="C35" s="93"/>
+      <c r="D35" s="93"/>
+      <c r="E35" s="93"/>
+      <c r="F35" s="93"/>
+      <c r="G35" s="93"/>
+      <c r="H35" s="93"/>
+      <c r="I35" s="93"/>
+      <c r="J35" s="93"/>
       <c r="L35" s="11" t="s">
         <v>1</v>
       </c>
@@ -20567,30 +20638,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="95" t="s">
         <v>222</v>
       </c>
-      <c r="B1" s="92"/>
-      <c r="C1" s="92"/>
-      <c r="D1" s="93"/>
-      <c r="F1" s="91" t="s">
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="97"/>
+      <c r="F1" s="95" t="s">
         <v>228</v>
       </c>
-      <c r="G1" s="92"/>
-      <c r="H1" s="92"/>
-      <c r="I1" s="93"/>
-      <c r="K1" s="91" t="s">
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
+      <c r="I1" s="97"/>
+      <c r="K1" s="95" t="s">
         <v>229</v>
       </c>
-      <c r="L1" s="92"/>
-      <c r="M1" s="92"/>
-      <c r="N1" s="93"/>
-      <c r="P1" s="91" t="s">
+      <c r="L1" s="96"/>
+      <c r="M1" s="96"/>
+      <c r="N1" s="97"/>
+      <c r="P1" s="95" t="s">
         <v>230</v>
       </c>
-      <c r="Q1" s="92"/>
-      <c r="R1" s="92"/>
-      <c r="S1" s="93"/>
+      <c r="Q1" s="96"/>
+      <c r="R1" s="96"/>
+      <c r="S1" s="97"/>
     </row>
     <row r="2" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="82" t="s">

</xml_diff>

<commit_message>
Trying to debug why the normres_r does not approach 0.
Why does the normres_r not approach 0? The normres_s seems to get very
very small relatively quickly. Perhaps try what happens when the the
areas only overlap by one bus, instead of overlapping by multiple buses.
Based on the x_k - c_k results, it seems like the overlapped buses have
the most error. Maybe that makes sense to some extent? Also, I still
don't quite like the way the indexing issue is addressed for x_k
(basically when you've added the slack bus, length(x_k) = 2*numbus_a,
but otherwise it's simply 2*numbus_a -1).
</commit_message>
<xml_diff>
--- a/DMASE - Test Results.xlsx
+++ b/DMASE - Test Results.xlsx
@@ -3059,7 +3059,7 @@
   <dimension ref="A1:S147"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3448,7 +3448,7 @@
       </c>
       <c r="I10" s="89"/>
       <c r="J10" s="89">
-        <f t="shared" ref="J8:J31" si="4">B10-F10</f>
+        <f t="shared" ref="J10:J31" si="4">B10-F10</f>
         <v>-1.1659750686900949E-3</v>
       </c>
       <c r="K10" s="89"/>

</xml_diff>

<commit_message>
14 bus ADMM works now
After correcting the function that pulls the measurements and autosaving
the Ybus, the 14 bus ADMM works. The sqrt(normres_r) ~= 3e-5, and
central - ADMM solution ~= 2e-5. Stops during the 5th iteration.
</commit_message>
<xml_diff>
--- a/DMASE - Test Results.xlsx
+++ b/DMASE - Test Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12240" windowHeight="9240" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12240" windowHeight="9240" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="3 Bus" sheetId="1" r:id="rId1"/>
@@ -1181,7 +1181,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1390,6 +1390,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1422,9 +1428,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1752,15 +1755,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="94" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94"/>
+      <c r="A1" s="96" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
       <c r="I1" s="6" t="s">
         <v>1</v>
       </c>
@@ -2113,15 +2116,15 @@
       <c r="N11" s="1"/>
     </row>
     <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="95" t="s">
+      <c r="A12" s="97" t="s">
         <v>80</v>
       </c>
-      <c r="B12" s="95"/>
-      <c r="C12" s="95"/>
-      <c r="D12" s="95"/>
-      <c r="E12" s="95"/>
-      <c r="F12" s="95"/>
-      <c r="G12" s="95"/>
+      <c r="B12" s="97"/>
+      <c r="C12" s="97"/>
+      <c r="D12" s="97"/>
+      <c r="E12" s="97"/>
+      <c r="F12" s="97"/>
+      <c r="G12" s="97"/>
       <c r="I12" s="1"/>
       <c r="J12" s="6" t="s">
         <v>1</v>
@@ -2611,15 +2614,15 @@
       <c r="G31" s="1"/>
     </row>
     <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="95" t="s">
+      <c r="A32" s="97" t="s">
         <v>81</v>
       </c>
-      <c r="B32" s="95"/>
-      <c r="C32" s="95"/>
-      <c r="D32" s="95"/>
-      <c r="E32" s="95"/>
-      <c r="F32" s="95"/>
-      <c r="G32" s="95"/>
+      <c r="B32" s="97"/>
+      <c r="C32" s="97"/>
+      <c r="D32" s="97"/>
+      <c r="E32" s="97"/>
+      <c r="F32" s="97"/>
+      <c r="G32" s="97"/>
       <c r="I32" s="1"/>
       <c r="J32" s="6" t="s">
         <v>1</v>
@@ -3104,29 +3107,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="104" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="104"/>
-      <c r="D1" s="102" t="s">
+      <c r="B1" s="106"/>
+      <c r="D1" s="104" t="s">
         <v>278</v>
       </c>
-      <c r="E1" s="103"/>
-      <c r="F1" s="103"/>
-      <c r="G1" s="103"/>
-      <c r="H1" s="103"/>
-      <c r="I1" s="103"/>
-      <c r="J1" s="104"/>
-      <c r="L1" s="102" t="s">
+      <c r="E1" s="105"/>
+      <c r="F1" s="105"/>
+      <c r="G1" s="105"/>
+      <c r="H1" s="105"/>
+      <c r="I1" s="105"/>
+      <c r="J1" s="106"/>
+      <c r="L1" s="104" t="s">
         <v>280</v>
       </c>
-      <c r="M1" s="103"/>
-      <c r="N1" s="103"/>
-      <c r="O1" s="103"/>
-      <c r="P1" s="103"/>
-      <c r="Q1" s="103"/>
-      <c r="R1" s="103"/>
-      <c r="S1" s="104"/>
+      <c r="M1" s="105"/>
+      <c r="N1" s="105"/>
+      <c r="O1" s="105"/>
+      <c r="P1" s="105"/>
+      <c r="Q1" s="105"/>
+      <c r="R1" s="105"/>
+      <c r="S1" s="106"/>
       <c r="T1" s="86"/>
     </row>
     <row r="2" spans="1:20" s="70" customFormat="1" x14ac:dyDescent="0.25">
@@ -4006,30 +4009,30 @@
       </c>
     </row>
     <row r="2" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="98" t="s">
+      <c r="A2" s="100" t="s">
         <v>207</v>
       </c>
-      <c r="B2" s="99"/>
-      <c r="C2" s="99"/>
-      <c r="D2" s="100"/>
-      <c r="F2" s="98" t="s">
+      <c r="B2" s="101"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="102"/>
+      <c r="F2" s="100" t="s">
         <v>213</v>
       </c>
-      <c r="G2" s="99"/>
-      <c r="H2" s="99"/>
-      <c r="I2" s="100"/>
-      <c r="K2" s="98" t="s">
+      <c r="G2" s="101"/>
+      <c r="H2" s="101"/>
+      <c r="I2" s="102"/>
+      <c r="K2" s="100" t="s">
         <v>214</v>
       </c>
-      <c r="L2" s="99"/>
-      <c r="M2" s="99"/>
-      <c r="N2" s="100"/>
-      <c r="P2" s="98" t="s">
+      <c r="L2" s="101"/>
+      <c r="M2" s="101"/>
+      <c r="N2" s="102"/>
+      <c r="P2" s="100" t="s">
         <v>215</v>
       </c>
-      <c r="Q2" s="99"/>
-      <c r="R2" s="99"/>
-      <c r="S2" s="100"/>
+      <c r="Q2" s="101"/>
+      <c r="R2" s="101"/>
+      <c r="S2" s="102"/>
     </row>
     <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="80" t="s">
@@ -4473,7 +4476,7 @@
         <v>-16.600000000000001</v>
       </c>
       <c r="R12" s="70">
-        <f t="shared" ref="R12:R24" si="7">Q12/100</f>
+        <f t="shared" ref="R12:R16" si="7">Q12/100</f>
         <v>-0.16600000000000001</v>
       </c>
     </row>
@@ -4866,7 +4869,7 @@
       <c r="F21" s="20" t="s">
         <v>223</v>
       </c>
-      <c r="G21" s="105">
+      <c r="G21" s="95">
         <v>23.999999463558101</v>
       </c>
       <c r="H21" s="20">
@@ -5204,13 +5207,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="96" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
       <c r="G1" s="30" t="s">
         <v>99</v>
       </c>
@@ -5229,13 +5232,13 @@
       <c r="L1" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="P1" s="94" t="s">
+      <c r="P1" s="96" t="s">
         <v>105</v>
       </c>
-      <c r="Q1" s="94"/>
-      <c r="R1" s="94"/>
-      <c r="S1" s="94"/>
-      <c r="T1" s="94"/>
+      <c r="Q1" s="96"/>
+      <c r="R1" s="96"/>
+      <c r="S1" s="96"/>
+      <c r="T1" s="96"/>
       <c r="V1" s="30" t="s">
         <v>99</v>
       </c>
@@ -5770,12 +5773,12 @@
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="P10" s="94" t="s">
+      <c r="P10" s="96" t="s">
         <v>107</v>
       </c>
-      <c r="Q10" s="94"/>
-      <c r="R10" s="94"/>
-      <c r="S10" s="94"/>
+      <c r="Q10" s="96"/>
+      <c r="R10" s="96"/>
+      <c r="S10" s="96"/>
       <c r="T10" s="25"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
@@ -6791,12 +6794,12 @@
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A33" s="94" t="s">
+      <c r="A33" s="96" t="s">
         <v>101</v>
       </c>
-      <c r="B33" s="94"/>
-      <c r="C33" s="94"/>
-      <c r="D33" s="94"/>
+      <c r="B33" s="96"/>
+      <c r="C33" s="96"/>
+      <c r="D33" s="96"/>
       <c r="F33" s="30" t="s">
         <v>99</v>
       </c>
@@ -7174,12 +7177,12 @@
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A42" s="94" t="s">
+      <c r="A42" s="96" t="s">
         <v>103</v>
       </c>
-      <c r="B42" s="94"/>
-      <c r="C42" s="94"/>
-      <c r="D42" s="94"/>
+      <c r="B42" s="96"/>
+      <c r="C42" s="96"/>
+      <c r="D42" s="96"/>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
@@ -7678,15 +7681,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="97" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
-      <c r="E1" s="95"/>
-      <c r="F1" s="95"/>
-      <c r="G1" s="95"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
       <c r="I1" s="1"/>
       <c r="J1" s="4"/>
       <c r="L1" s="4" t="s">
@@ -8748,18 +8751,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="98" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="98"/>
+      <c r="H1" s="98"/>
+      <c r="I1" s="98"/>
+      <c r="J1" s="98"/>
       <c r="L1" s="11" t="s">
         <v>1</v>
       </c>
@@ -8783,18 +8786,18 @@
       <c r="B2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="97" t="s">
+      <c r="C2" s="99" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97" t="s">
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99" t="s">
         <v>74</v>
       </c>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
       <c r="L2" s="8" t="s">
         <v>41</v>
       </c>
@@ -9587,18 +9590,18 @@
       <c r="O33" s="1"/>
     </row>
     <row r="35" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="96" t="s">
+      <c r="A35" s="98" t="s">
         <v>78</v>
       </c>
-      <c r="B35" s="96"/>
-      <c r="C35" s="96"/>
-      <c r="D35" s="96"/>
-      <c r="E35" s="96"/>
-      <c r="F35" s="96"/>
-      <c r="G35" s="96"/>
-      <c r="H35" s="96"/>
-      <c r="I35" s="96"/>
-      <c r="J35" s="96"/>
+      <c r="B35" s="98"/>
+      <c r="C35" s="98"/>
+      <c r="D35" s="98"/>
+      <c r="E35" s="98"/>
+      <c r="F35" s="98"/>
+      <c r="G35" s="98"/>
+      <c r="H35" s="98"/>
+      <c r="I35" s="98"/>
+      <c r="J35" s="98"/>
       <c r="L35" s="11" t="s">
         <v>1</v>
       </c>
@@ -12331,7 +12334,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R23" sqref="R23"/>
     </sheetView>
   </sheetViews>
@@ -12359,30 +12362,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="98" t="s">
+      <c r="A1" s="100" t="s">
         <v>207</v>
       </c>
-      <c r="B1" s="99"/>
-      <c r="C1" s="99"/>
-      <c r="D1" s="100"/>
-      <c r="F1" s="98" t="s">
+      <c r="B1" s="101"/>
+      <c r="C1" s="101"/>
+      <c r="D1" s="102"/>
+      <c r="F1" s="100" t="s">
         <v>213</v>
       </c>
-      <c r="G1" s="99"/>
-      <c r="H1" s="99"/>
-      <c r="I1" s="100"/>
-      <c r="K1" s="98" t="s">
+      <c r="G1" s="101"/>
+      <c r="H1" s="101"/>
+      <c r="I1" s="102"/>
+      <c r="K1" s="100" t="s">
         <v>214</v>
       </c>
-      <c r="L1" s="99"/>
-      <c r="M1" s="99"/>
-      <c r="N1" s="100"/>
-      <c r="P1" s="98" t="s">
+      <c r="L1" s="101"/>
+      <c r="M1" s="101"/>
+      <c r="N1" s="102"/>
+      <c r="P1" s="100" t="s">
         <v>215</v>
       </c>
-      <c r="Q1" s="99"/>
-      <c r="R1" s="99"/>
-      <c r="S1" s="100"/>
+      <c r="Q1" s="101"/>
+      <c r="R1" s="101"/>
+      <c r="S1" s="102"/>
     </row>
     <row r="2" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="80" t="s">
@@ -12464,7 +12467,7 @@
         <v>6.4193752642371704</v>
       </c>
       <c r="M3">
-        <f>L3/100</f>
+        <f t="shared" ref="M3:M10" si="0">L3/100</f>
         <v>6.4193752642371704E-2</v>
       </c>
       <c r="P3" t="s">
@@ -12486,7 +12489,7 @@
         <v>-20.300935880694301</v>
       </c>
       <c r="C4" s="72">
-        <f t="shared" ref="C4:C6" si="0">B4/100</f>
+        <f t="shared" ref="C4:C6" si="1">B4/100</f>
         <v>-0.20300935880694301</v>
       </c>
       <c r="D4" s="72"/>
@@ -12497,7 +12500,7 @@
         <v>0.96859150246414105</v>
       </c>
       <c r="H4" s="72">
-        <f t="shared" ref="H4:H8" si="1">G4/100</f>
+        <f t="shared" ref="H4:H8" si="2">G4/100</f>
         <v>9.6859150246414102E-3</v>
       </c>
       <c r="I4" s="72"/>
@@ -12508,7 +12511,7 @@
         <v>1.57798981550307</v>
       </c>
       <c r="M4" s="70">
-        <f>L4/100</f>
+        <f t="shared" si="0"/>
         <v>1.5779898155030701E-2</v>
       </c>
       <c r="P4" t="s">
@@ -12530,7 +12533,7 @@
         <v>75.916881283268793</v>
       </c>
       <c r="C5" s="72">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.75916881283268789</v>
       </c>
       <c r="D5" s="72"/>
@@ -12541,7 +12544,7 @@
         <v>29.247688021076399</v>
       </c>
       <c r="H5" s="72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.29247688021076401</v>
       </c>
       <c r="I5" s="72"/>
@@ -12552,7 +12555,7 @@
         <v>7.6111237412808599</v>
       </c>
       <c r="M5" s="70">
-        <f>L5/100</f>
+        <f t="shared" si="0"/>
         <v>7.6111237412808605E-2</v>
       </c>
       <c r="P5" t="s">
@@ -12574,7 +12577,7 @@
         <v>-0.155506560051652</v>
       </c>
       <c r="C6" s="72">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.55506560051652E-3</v>
       </c>
       <c r="D6" s="72"/>
@@ -12585,7 +12588,7 @@
         <v>-10.134384235994199</v>
       </c>
       <c r="H6" s="72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.101343842359942</v>
       </c>
       <c r="I6" s="72"/>
@@ -12596,7 +12599,7 @@
         <v>2.2749299623984598</v>
       </c>
       <c r="M6" s="70">
-        <f>L6/100</f>
+        <f t="shared" si="0"/>
         <v>2.2749299623984597E-2</v>
       </c>
       <c r="P6" t="s">
@@ -12629,7 +12632,7 @@
         <v>4.9388912162000001E-5</v>
       </c>
       <c r="H7" s="72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.9388912162000003E-7</v>
       </c>
       <c r="I7" s="72"/>
@@ -12640,7 +12643,7 @@
         <v>17.236621109828601</v>
       </c>
       <c r="M7" s="70">
-        <f>L7/100</f>
+        <f t="shared" si="0"/>
         <v>0.17236621109828601</v>
       </c>
       <c r="P7" s="70" t="s">
@@ -12673,7 +12676,7 @@
         <v>-23.1382548362844</v>
       </c>
       <c r="H8" s="72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.231382548362844</v>
       </c>
       <c r="I8" s="72"/>
@@ -12684,7 +12687,7 @@
         <v>6.2088690408799696</v>
       </c>
       <c r="M8" s="70">
-        <f>L8/100</f>
+        <f t="shared" si="0"/>
         <v>6.2088690408799697E-2</v>
       </c>
       <c r="P8" s="70" t="s">
@@ -12694,7 +12697,7 @@
         <v>1.02798621556374</v>
       </c>
       <c r="R8" s="70">
-        <f t="shared" ref="R8:R9" si="2">Q8</f>
+        <f t="shared" ref="R8:R9" si="3">Q8</f>
         <v>1.02798621556374</v>
       </c>
     </row>
@@ -12728,7 +12731,7 @@
         <v>1.4392071686730901</v>
       </c>
       <c r="M9" s="70">
-        <f>L9/100</f>
+        <f t="shared" si="0"/>
         <v>1.4392071686730901E-2</v>
       </c>
       <c r="P9" s="70" t="s">
@@ -12738,7 +12741,7 @@
         <v>1.00994172446495</v>
       </c>
       <c r="R9" s="70">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.00994172446495</v>
       </c>
     </row>
@@ -12750,7 +12753,7 @@
         <v>1.04499995797579</v>
       </c>
       <c r="C10" s="20">
-        <f t="shared" ref="C10:C11" si="3">B10</f>
+        <f t="shared" ref="C10:C11" si="4">B10</f>
         <v>1.04499995797579</v>
       </c>
       <c r="D10" s="72"/>
@@ -12761,7 +12764,7 @@
         <v>1.02371286456331</v>
       </c>
       <c r="H10" s="20">
-        <f t="shared" ref="H10:H12" si="4">G10</f>
+        <f t="shared" ref="H10:H12" si="5">G10</f>
         <v>1.02371286456331</v>
       </c>
       <c r="I10" s="72"/>
@@ -12772,7 +12775,7 @@
         <v>0.52526799870488805</v>
       </c>
       <c r="M10" s="70">
-        <f>L10/100</f>
+        <f t="shared" si="0"/>
         <v>5.2526799870488807E-3</v>
       </c>
       <c r="N10" s="70"/>
@@ -12795,7 +12798,7 @@
         <v>1.0280925147905799</v>
       </c>
       <c r="C11" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.0280925147905799</v>
       </c>
       <c r="D11" s="72"/>
@@ -12806,7 +12809,7 @@
         <v>1.04612245201456</v>
       </c>
       <c r="H11" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.04612245201456</v>
       </c>
       <c r="I11" s="72"/>
@@ -12828,7 +12831,7 @@
         <v>-16.599999</v>
       </c>
       <c r="R11" s="70">
-        <f t="shared" ref="R11:R15" si="5">Q11/100</f>
+        <f t="shared" ref="R11:R15" si="6">Q11/100</f>
         <v>-0.16599999000000001</v>
       </c>
     </row>
@@ -12851,7 +12854,7 @@
         <v>1.0850835071553799</v>
       </c>
       <c r="H12" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.0850835071553799</v>
       </c>
       <c r="I12" s="72"/>
@@ -12862,7 +12865,7 @@
         <v>1.02970205350408</v>
       </c>
       <c r="M12" s="70">
-        <f t="shared" ref="M12:M14" si="6">L12</f>
+        <f t="shared" ref="M12:M14" si="7">L12</f>
         <v>1.02970205350408</v>
       </c>
       <c r="P12" t="s">
@@ -12872,7 +12875,7 @@
         <v>-9</v>
       </c>
       <c r="R12" s="70">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-0.09</v>
       </c>
     </row>
@@ -12884,7 +12887,7 @@
         <v>-20.456442236900301</v>
       </c>
       <c r="C13" s="72">
-        <f t="shared" ref="C13:C23" si="7">B13/100</f>
+        <f t="shared" ref="C13:C23" si="8">B13/100</f>
         <v>-0.20456442236900302</v>
       </c>
       <c r="D13" s="72"/>
@@ -12906,7 +12909,7 @@
         <v>1.0240525230119499</v>
       </c>
       <c r="M13" s="70">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.0240525230119499</v>
       </c>
       <c r="P13" t="s">
@@ -12916,7 +12919,7 @@
         <v>-5.8</v>
       </c>
       <c r="R13" s="70">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-5.7999999999999996E-2</v>
       </c>
     </row>
@@ -12929,7 +12932,7 @@
         <v>18.3000015960464</v>
       </c>
       <c r="C14" s="72">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.183000015960464</v>
       </c>
       <c r="D14" s="72"/>
@@ -12941,7 +12944,7 @@
         <v>2.4613437652587002</v>
       </c>
       <c r="H14" s="20">
-        <f t="shared" ref="H14:H26" si="8">G14/100</f>
+        <f t="shared" ref="H14:H26" si="9">G14/100</f>
         <v>2.4613437652587004E-2</v>
       </c>
       <c r="I14" s="72"/>
@@ -12952,7 +12955,7 @@
         <v>1.01992383631813</v>
       </c>
       <c r="M14" s="70">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.01992383631813</v>
       </c>
       <c r="P14" t="s">
@@ -12962,7 +12965,7 @@
         <v>-14.9</v>
       </c>
       <c r="R14" s="70">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-0.14899999999999999</v>
       </c>
     </row>
@@ -12975,7 +12978,7 @@
         <v>22.194874691963104</v>
       </c>
       <c r="C15" s="72">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.22194874691963104</v>
       </c>
       <c r="D15" s="72"/>
@@ -12986,7 +12989,7 @@
         <v>-47.799999</v>
       </c>
       <c r="H15" s="20">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-0.47799998999999999</v>
       </c>
       <c r="I15" s="72"/>
@@ -13007,7 +13010,7 @@
         <v>-5</v>
       </c>
       <c r="R15" s="70">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-0.05</v>
       </c>
     </row>
@@ -13019,7 +13022,7 @@
         <v>-7.6</v>
       </c>
       <c r="C16" s="72">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-7.5999999999999998E-2</v>
       </c>
       <c r="D16" s="72"/>
@@ -13030,7 +13033,7 @@
         <v>3.9</v>
       </c>
       <c r="H16" s="20">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>3.9E-2</v>
       </c>
       <c r="I16" s="72"/>
@@ -13042,7 +13045,7 @@
         <v>16.499999463558101</v>
       </c>
       <c r="M16" s="70">
-        <f t="shared" ref="M16:M22" si="9">L16/100</f>
+        <f t="shared" ref="M16:M22" si="10">L16/100</f>
         <v>0.16499999463558102</v>
       </c>
       <c r="P16" s="70" t="s">
@@ -13052,7 +13055,7 @@
         <v>-16.079815706198001</v>
       </c>
       <c r="R16" s="70">
-        <f>Q16/100</f>
+        <f t="shared" ref="R16:R23" si="11">Q16/100</f>
         <v>-0.16079815706198</v>
       </c>
       <c r="S16" s="70"/>
@@ -13065,7 +13068,7 @@
         <v>-1.6</v>
       </c>
       <c r="C17" s="72">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-1.6E-2</v>
       </c>
       <c r="D17" s="72"/>
@@ -13076,7 +13079,7 @@
         <v>0</v>
       </c>
       <c r="H17" s="20">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="I17" s="72"/>
@@ -13087,7 +13090,7 @@
         <v>-3.5</v>
       </c>
       <c r="M17" s="70">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-3.5000000000000003E-2</v>
       </c>
       <c r="P17" s="70" t="s">
@@ -13097,7 +13100,7 @@
         <v>1.7323809918499999</v>
       </c>
       <c r="R17" s="70">
-        <f>Q17/100</f>
+        <f t="shared" si="11"/>
         <v>1.7323809918500001E-2</v>
       </c>
       <c r="S17" s="70"/>
@@ -13110,7 +13113,7 @@
         <v>72.934574594694098</v>
       </c>
       <c r="C18" s="72">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.72934574594694102</v>
       </c>
       <c r="D18" s="72" t="s">
@@ -13123,7 +13126,7 @@
         <v>0</v>
       </c>
       <c r="H18" s="20">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="I18" s="72"/>
@@ -13134,7 +13137,7 @@
         <v>-1.8</v>
       </c>
       <c r="M18" s="70">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-1.8000000000000002E-2</v>
       </c>
       <c r="P18" s="2" t="s">
@@ -13144,7 +13147,7 @@
         <v>-29.247637436823101</v>
       </c>
       <c r="R18" s="2">
-        <f>Q18/100</f>
+        <f t="shared" si="11"/>
         <v>-0.29247637436823104</v>
       </c>
       <c r="S18" s="83" t="s">
@@ -13159,7 +13162,7 @@
         <v>3.5900360862934599</v>
       </c>
       <c r="C19" s="72">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.5900360862934598E-2</v>
       </c>
       <c r="D19" s="72" t="s">
@@ -13172,7 +13175,7 @@
         <v>0</v>
       </c>
       <c r="H19" s="20">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="I19" s="72"/>
@@ -13183,7 +13186,7 @@
         <v>-6.1</v>
       </c>
       <c r="M19" s="70">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-6.0999999999999999E-2</v>
       </c>
       <c r="P19" s="2" t="s">
@@ -13193,7 +13196,7 @@
         <v>-11.0919776937066</v>
       </c>
       <c r="R19" s="2">
-        <f>Q19/100</f>
+        <f t="shared" si="11"/>
         <v>-0.11091977693706599</v>
       </c>
       <c r="S19" s="83" t="s">
@@ -13221,7 +13224,7 @@
         <v>23.999999463558101</v>
       </c>
       <c r="H20" s="20">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.239999994635581</v>
       </c>
       <c r="I20" s="72"/>
@@ -13232,7 +13235,7 @@
         <v>-1.6</v>
       </c>
       <c r="M20" s="70">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-1.6E-2</v>
       </c>
       <c r="P20" t="s">
@@ -13242,7 +13245,7 @@
         <v>-2.8744036925517298</v>
       </c>
       <c r="R20" s="70">
-        <f>Q20/100</f>
+        <f t="shared" si="11"/>
         <v>-2.8744036925517299E-2</v>
       </c>
       <c r="S20" s="72" t="s">
@@ -13283,7 +13286,7 @@
         <v>-13.5</v>
       </c>
       <c r="M21" s="70">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-0.13500000000000001</v>
       </c>
       <c r="P21" t="s">
@@ -13293,7 +13296,7 @@
         <v>0.31779049296478201</v>
       </c>
       <c r="R21" s="70">
-        <f>Q21/100</f>
+        <f t="shared" si="11"/>
         <v>3.1779049296478202E-3</v>
       </c>
       <c r="S21" s="72" t="s">
@@ -13308,7 +13311,7 @@
         <v>42.467165475154701</v>
       </c>
       <c r="C22" s="72">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.424671654751547</v>
       </c>
       <c r="D22" s="72" t="s">
@@ -13334,7 +13337,7 @@
         <v>-5.8</v>
       </c>
       <c r="M22" s="70">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-5.7999999999999996E-2</v>
       </c>
       <c r="P22" s="2" t="s">
@@ -13344,7 +13347,7 @@
         <v>-4.9650161007164098</v>
       </c>
       <c r="R22" s="2">
-        <f>Q22/100</f>
+        <f t="shared" si="11"/>
         <v>-4.9650161007164101E-2</v>
       </c>
       <c r="S22" s="83" t="s">
@@ -13359,7 +13362,7 @@
         <v>-2.12732489205733</v>
       </c>
       <c r="C23" s="72">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-2.12732489205733E-2</v>
       </c>
       <c r="D23" s="72" t="s">
@@ -13372,7 +13375,7 @@
         <v>-63.001699846354903</v>
       </c>
       <c r="H23" s="20">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-0.63001699846354908</v>
       </c>
       <c r="I23" s="72" t="s">
@@ -13385,7 +13388,7 @@
         <v>-42.467163764624999</v>
       </c>
       <c r="M23" s="2">
-        <f>L23/100</f>
+        <f t="shared" ref="M23:M28" si="12">L23/100</f>
         <v>-0.42467163764624999</v>
       </c>
       <c r="N23" s="83" t="s">
@@ -13398,7 +13401,7 @@
         <v>-0.52427629116916796</v>
       </c>
       <c r="R23" s="2">
-        <f>Q23/100</f>
+        <f t="shared" si="11"/>
         <v>-5.2427629116916794E-3</v>
       </c>
       <c r="S23" s="83" t="s">
@@ -13413,7 +13416,7 @@
         <v>10.2039485868599</v>
       </c>
       <c r="H24" s="20">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.102039485868599</v>
       </c>
       <c r="I24" s="72" t="s">
@@ -13426,7 +13429,7 @@
         <v>6.4382015347410002</v>
       </c>
       <c r="M24" s="2">
-        <f>L24/100</f>
+        <f t="shared" si="12"/>
         <v>6.4382015347410004E-2</v>
       </c>
       <c r="N24" s="83" t="s">
@@ -13441,7 +13444,7 @@
         <v>29.247637436823101</v>
       </c>
       <c r="H25" s="20">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.29247637436823104</v>
       </c>
       <c r="I25" s="72" t="s">
@@ -13454,7 +13457,7 @@
         <v>2.8808971477310599</v>
       </c>
       <c r="M25" s="2">
-        <f>L25/100</f>
+        <f t="shared" si="12"/>
         <v>2.88089714773106E-2</v>
       </c>
       <c r="N25" s="83" t="s">
@@ -13472,7 +13475,7 @@
         <v>11.0919776937066</v>
       </c>
       <c r="H26" s="20">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.11091977693706599</v>
       </c>
       <c r="I26" s="72" t="s">
@@ -13485,7 +13488,7 @@
         <v>-0.30259003060574602</v>
       </c>
       <c r="M26" s="2">
-        <f>L26/100</f>
+        <f t="shared" si="12"/>
         <v>-3.0259003060574604E-3</v>
       </c>
       <c r="N26" s="83" t="s">
@@ -13503,7 +13506,7 @@
         <v>4.9650161007164098</v>
       </c>
       <c r="M27" s="70">
-        <f>L27/100</f>
+        <f t="shared" si="12"/>
         <v>4.9650161007164101E-2</v>
       </c>
       <c r="N27" s="72" t="s">
@@ -13520,7 +13523,7 @@
         <v>0.52427629116916796</v>
       </c>
       <c r="M28" s="70">
-        <f>L28/100</f>
+        <f t="shared" si="12"/>
         <v>5.2427629116916794E-3</v>
       </c>
       <c r="N28" s="72" t="s">
@@ -13709,26 +13712,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" s="70" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="103" t="s">
         <v>261</v>
       </c>
-      <c r="B1" s="101"/>
-      <c r="C1" s="101"/>
-      <c r="D1" s="101"/>
-      <c r="E1" s="101"/>
-      <c r="F1" s="101"/>
-      <c r="J1" s="101" t="s">
+      <c r="B1" s="103"/>
+      <c r="C1" s="103"/>
+      <c r="D1" s="103"/>
+      <c r="E1" s="103"/>
+      <c r="F1" s="103"/>
+      <c r="J1" s="103" t="s">
         <v>261</v>
       </c>
-      <c r="K1" s="101"/>
-      <c r="L1" s="101"/>
-      <c r="M1" s="101"/>
-      <c r="N1" s="101"/>
-      <c r="O1" s="101"/>
-      <c r="P1" s="101"/>
-      <c r="Q1" s="101"/>
-      <c r="R1" s="101"/>
-      <c r="S1" s="101"/>
+      <c r="K1" s="103"/>
+      <c r="L1" s="103"/>
+      <c r="M1" s="103"/>
+      <c r="N1" s="103"/>
+      <c r="O1" s="103"/>
+      <c r="P1" s="103"/>
+      <c r="Q1" s="103"/>
+      <c r="R1" s="103"/>
+      <c r="S1" s="103"/>
       <c r="V1" s="70" t="s">
         <v>266</v>
       </c>
@@ -14746,8 +14749,8 @@
   </sheetPr>
   <dimension ref="A1:T146"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14768,20 +14771,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="98" t="s">
         <v>288</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
-      <c r="K1" s="96"/>
-      <c r="L1" s="96"/>
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="98"/>
+      <c r="H1" s="98"/>
+      <c r="I1" s="98"/>
+      <c r="J1" s="98"/>
+      <c r="K1" s="98"/>
+      <c r="L1" s="98"/>
       <c r="M1" s="87"/>
       <c r="N1" s="43"/>
       <c r="O1" s="11" t="s">
@@ -14805,22 +14808,22 @@
       <c r="B2" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="97" t="s">
+      <c r="C2" s="99" t="s">
         <v>285</v>
       </c>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97" t="s">
+      <c r="D2" s="99"/>
+      <c r="E2" s="99" t="s">
         <v>284</v>
       </c>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97" t="s">
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99" t="s">
         <v>74</v>
       </c>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
+      <c r="K2" s="99"/>
+      <c r="L2" s="99"/>
       <c r="M2" s="4"/>
       <c r="N2" s="60" t="s">
         <v>137</v>
@@ -14896,25 +14899,25 @@
       <c r="A4" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B4" s="1">
-        <v>1.05999768165375</v>
-      </c>
-      <c r="C4" s="89">
-        <v>1.0599997148008</v>
+      <c r="B4" s="94">
+        <v>1.05999477557869</v>
+      </c>
+      <c r="C4" s="94">
+        <v>1.0599997016213201</v>
       </c>
       <c r="D4" s="88">
         <f>B4-C4</f>
-        <v>-2.0331470500511983E-6</v>
+        <v>-4.9260426300268279E-6</v>
       </c>
       <c r="E4" s="78">
-        <v>1.0599997148008</v>
+        <v>1.0599997016213201</v>
       </c>
       <c r="F4" s="78"/>
       <c r="G4" s="78"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1">
         <f>B4-E4</f>
-        <v>-2.0331470500511983E-6</v>
+        <v>-4.9260426300268279E-6</v>
       </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -14937,31 +14940,31 @@
       <c r="A5" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B5" s="1">
-        <v>1.0410720611633699</v>
-      </c>
-      <c r="C5" s="89">
-        <v>1.0410736535334799</v>
-      </c>
-      <c r="D5" s="88">
+      <c r="B5" s="94">
+        <v>1.0410686897743699</v>
+      </c>
+      <c r="C5" s="94">
+        <v>1.04107363736397</v>
+      </c>
+      <c r="D5" s="94">
         <f t="shared" ref="D5:D31" si="1">B5-C5</f>
-        <v>-1.5923701099929133E-6</v>
+        <v>-4.9475896000128472E-6</v>
       </c>
       <c r="E5" s="78">
-        <v>1.0410737049553</v>
+        <v>1.0410736914149099</v>
       </c>
       <c r="F5" s="78">
-        <v>1.04107360211167</v>
+        <v>1.04107358331302</v>
       </c>
       <c r="G5" s="78"/>
       <c r="H5" s="1"/>
-      <c r="I5" s="85">
-        <f t="shared" ref="I5:I23" si="2">B5-E5</f>
-        <v>-1.6437919301282022E-6</v>
+      <c r="I5" s="94">
+        <f t="shared" ref="I5:I9" si="2">B5-E5</f>
+        <v>-5.0016405399588848E-6</v>
       </c>
       <c r="J5" s="1">
         <f>B5-F5</f>
-        <v>-1.5409483000716762E-6</v>
+        <v>-4.8935386500748024E-6</v>
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
@@ -14983,31 +14986,31 @@
       <c r="A6" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B6" s="1">
-        <v>0.98537777124357495</v>
-      </c>
-      <c r="C6" s="89">
-        <v>0.98538070092810903</v>
-      </c>
-      <c r="D6" s="88">
+      <c r="B6" s="94">
+        <v>0.98537560330584595</v>
+      </c>
+      <c r="C6" s="94">
+        <v>0.98538068323789896</v>
+      </c>
+      <c r="D6" s="94">
         <f t="shared" si="1"/>
-        <v>-2.9296845340809341E-6</v>
+        <v>-5.0799320530092729E-6</v>
       </c>
       <c r="E6" s="78">
-        <v>0.98538132252106703</v>
+        <v>0.98538130846403305</v>
       </c>
       <c r="F6" s="78">
-        <v>0.98538007933515104</v>
+        <v>0.98538005801176498</v>
       </c>
       <c r="G6" s="78"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="85">
+      <c r="I6" s="94">
         <f t="shared" si="2"/>
-        <v>-3.5512774920753998E-6</v>
-      </c>
-      <c r="J6" s="89">
+        <v>-5.705158187097048E-6</v>
+      </c>
+      <c r="J6" s="94">
         <f t="shared" ref="J6:J26" si="3">B6-F6</f>
-        <v>-2.3080915760864684E-6</v>
+        <v>-4.45470591903252E-6</v>
       </c>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -15029,38 +15032,38 @@
       <c r="A7" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B7" s="1">
-        <v>1.00695008061588</v>
-      </c>
-      <c r="C7" s="89">
-        <v>1.0079570192545</v>
-      </c>
-      <c r="D7" s="15">
+      <c r="B7" s="94">
+        <v>1.0069485784290699</v>
+      </c>
+      <c r="C7" s="94">
+        <v>1.00694708163546</v>
+      </c>
+      <c r="D7" s="94">
         <f t="shared" si="1"/>
-        <v>-1.006938638620003E-3</v>
+        <v>1.4967936099452572E-6</v>
       </c>
       <c r="E7" s="78">
-        <v>1.00695366520165</v>
+        <v>1.0069536496127001</v>
       </c>
       <c r="F7" s="78">
-        <v>1.0069525383039899</v>
+        <v>1.0069525153168799</v>
       </c>
       <c r="G7" s="78"/>
-      <c r="H7" s="89">
-        <v>1.0099648542578601</v>
-      </c>
-      <c r="I7" s="85">
+      <c r="H7" s="94">
+        <v>1.0069350799768</v>
+      </c>
+      <c r="I7" s="94">
         <f t="shared" si="2"/>
-        <v>-3.5845857699889905E-6</v>
-      </c>
-      <c r="J7" s="89">
+        <v>-5.0711836301342572E-6</v>
+      </c>
+      <c r="J7" s="94">
         <f t="shared" si="3"/>
-        <v>-2.4576881099136472E-6</v>
+        <v>-3.9368878099743654E-6</v>
       </c>
       <c r="K7" s="1"/>
       <c r="L7" s="1">
         <f>B7-H7</f>
-        <v>-3.0147736419801063E-3</v>
+        <v>1.3498452269944394E-5</v>
       </c>
       <c r="M7" s="88"/>
       <c r="N7" s="60"/>
@@ -15080,38 +15083,38 @@
       <c r="A8" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B8" s="1">
-        <v>1.01581292033021</v>
-      </c>
-      <c r="C8" s="89">
-        <v>1.01581184659879</v>
-      </c>
-      <c r="D8" s="88">
+      <c r="B8" s="94">
+        <v>1.0158116377075299</v>
+      </c>
+      <c r="C8" s="94">
+        <v>1.0158118296590799</v>
+      </c>
+      <c r="D8" s="94">
         <f t="shared" si="1"/>
-        <v>1.0737314199982251E-6</v>
+        <v>-1.9195154998818964E-7</v>
       </c>
       <c r="E8" s="78">
-        <v>1.01581624316023</v>
+        <v>1.01581622827343</v>
       </c>
       <c r="F8" s="78">
-        <v>1.0158153970250201</v>
+        <v>1.0158153744587</v>
       </c>
       <c r="G8" s="78">
-        <v>1.01580389961113</v>
-      </c>
-      <c r="I8" s="85">
+        <v>1.0158038862451</v>
+      </c>
+      <c r="I8" s="94">
         <f t="shared" si="2"/>
-        <v>-3.3228300200249805E-6</v>
-      </c>
-      <c r="J8" s="89">
+        <v>-4.5905659000755605E-6</v>
+      </c>
+      <c r="J8" s="94">
         <f t="shared" si="3"/>
-        <v>-2.4766948101273556E-6</v>
+        <v>-3.7367511700470146E-6</v>
       </c>
       <c r="K8" s="1">
         <f>B8-G8</f>
-        <v>9.0207190799329595E-6</v>
-      </c>
-      <c r="L8" s="89"/>
+        <v>7.7514624299279689E-6</v>
+      </c>
+      <c r="L8" s="94"/>
       <c r="M8" s="88"/>
       <c r="N8" s="60"/>
       <c r="O8" s="46" t="s">
@@ -15130,33 +15133,32 @@
       <c r="A9" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B9" s="1">
-        <v>1.0049243733889699</v>
-      </c>
-      <c r="C9" s="89">
-        <v>1.0049284290183</v>
-      </c>
-      <c r="D9" s="88">
+      <c r="B9" s="94">
+        <v>1.0049309967030799</v>
+      </c>
+      <c r="C9" s="94">
+        <v>1.00492841525779</v>
+      </c>
+      <c r="D9" s="94">
         <f t="shared" si="1"/>
-        <v>-4.0556293301463597E-6</v>
+        <v>2.5814452899730611E-6</v>
       </c>
       <c r="E9" s="78">
-        <v>1.0049288387483399</v>
-      </c>
-      <c r="F9" s="78"/>
+        <v>1.0049288225782</v>
+      </c>
       <c r="G9" s="78">
-        <v>1.0049280192882499</v>
-      </c>
-      <c r="I9" s="85">
+        <v>1.0049280079373799</v>
+      </c>
+      <c r="I9" s="94">
         <f t="shared" si="2"/>
-        <v>-4.4653593700427763E-6</v>
-      </c>
-      <c r="J9" s="89"/>
-      <c r="K9" s="89">
+        <v>2.1741248799056478E-6</v>
+      </c>
+      <c r="J9" s="94"/>
+      <c r="K9" s="94">
         <f t="shared" ref="K9:K31" si="4">B9-G9</f>
-        <v>-3.6458992800358914E-6</v>
-      </c>
-      <c r="L9" s="89"/>
+        <v>2.9887657000404744E-6</v>
+      </c>
+      <c r="L9" s="94"/>
       <c r="M9" s="88"/>
       <c r="N9" s="60"/>
       <c r="O9" s="46" t="s">
@@ -15175,33 +15177,31 @@
       <c r="A10" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B10" s="1">
-        <v>1.01654592268694</v>
-      </c>
-      <c r="C10" s="89">
-        <v>1.0171308048837</v>
-      </c>
-      <c r="D10" s="15">
+      <c r="B10" s="94">
+        <v>1.01654560910752</v>
+      </c>
+      <c r="C10" s="94">
+        <v>1.01654488667501</v>
+      </c>
+      <c r="D10" s="94">
         <f t="shared" si="1"/>
-        <v>-5.8488219676000597E-4</v>
-      </c>
-      <c r="E10" s="78"/>
+        <v>7.2243251003634157E-7</v>
+      </c>
       <c r="F10" s="78">
-        <v>1.0165489603217499</v>
-      </c>
-      <c r="G10" s="78"/>
+        <v>1.0165489370199501</v>
+      </c>
       <c r="H10" s="70">
-        <v>1.0177126494456501</v>
+        <v>1.0165408363300701</v>
       </c>
       <c r="I10" s="89"/>
-      <c r="J10" s="89">
+      <c r="J10" s="94">
         <f t="shared" si="3"/>
-        <v>-3.0376348099103723E-6</v>
-      </c>
-      <c r="K10" s="89"/>
-      <c r="L10" s="89">
-        <f t="shared" ref="L10:L31" si="5">B10-H10</f>
-        <v>-1.1667267587101016E-3</v>
+        <v>-3.3279124300733542E-6</v>
+      </c>
+      <c r="K10" s="94"/>
+      <c r="L10" s="94">
+        <f t="shared" ref="L8:L31" si="5">B10-H10</f>
+        <v>4.7727774499239928E-6</v>
       </c>
       <c r="M10" s="88"/>
       <c r="N10" s="60" t="s">
@@ -15223,28 +15223,26 @@
       <c r="A11" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B11" s="1">
-        <v>1.0544057013008099</v>
-      </c>
-      <c r="C11" s="89">
-        <v>1.0544084480406</v>
-      </c>
-      <c r="D11" s="88">
+      <c r="B11" s="94">
+        <v>1.0544046442934401</v>
+      </c>
+      <c r="C11" s="94">
+        <v>1.05440842639559</v>
+      </c>
+      <c r="D11" s="94">
         <f t="shared" si="1"/>
-        <v>-2.7467397900604595E-6</v>
-      </c>
-      <c r="E11" s="78"/>
+        <v>-3.7821021499073737E-6</v>
+      </c>
       <c r="F11" s="78">
-        <v>1.0544084480406</v>
-      </c>
-      <c r="G11" s="78"/>
+        <v>1.05440842639559</v>
+      </c>
       <c r="I11" s="89"/>
-      <c r="J11" s="89">
+      <c r="J11" s="94">
         <f t="shared" si="3"/>
-        <v>-2.7467397900604595E-6</v>
-      </c>
-      <c r="K11" s="89"/>
-      <c r="L11" s="89"/>
+        <v>-3.7821021499073737E-6</v>
+      </c>
+      <c r="K11" s="94"/>
+      <c r="L11" s="94"/>
       <c r="M11" s="88"/>
       <c r="N11" s="60" t="s">
         <v>173</v>
@@ -15265,33 +15263,31 @@
       <c r="A12" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B12" s="1">
-        <v>0.99794960680741096</v>
-      </c>
-      <c r="C12" s="89">
-        <v>0.99829818664175096</v>
-      </c>
-      <c r="D12" s="15">
+      <c r="B12" s="94">
+        <v>0.99795122261570202</v>
+      </c>
+      <c r="C12" s="94">
+        <v>0.99794996769674404</v>
+      </c>
+      <c r="D12" s="94">
         <f t="shared" si="1"/>
-        <v>-3.485798343400015E-4</v>
-      </c>
-      <c r="E12" s="78"/>
+        <v>1.2549189579713627E-6</v>
+      </c>
       <c r="F12" s="78">
-        <v>0.997952981014955</v>
-      </c>
-      <c r="G12" s="78"/>
+        <v>0.99795295635585701</v>
+      </c>
       <c r="H12" s="70">
-        <v>0.99864339226854604</v>
+        <v>0.99794697903762997</v>
       </c>
       <c r="I12" s="89"/>
-      <c r="J12" s="89">
+      <c r="J12" s="94">
         <f t="shared" si="3"/>
-        <v>-3.3742075440379438E-6</v>
-      </c>
-      <c r="K12" s="89"/>
-      <c r="L12" s="89">
+        <v>-1.7337401549966103E-6</v>
+      </c>
+      <c r="K12" s="94"/>
+      <c r="L12" s="94">
         <f t="shared" si="5"/>
-        <v>-6.9378546113507689E-4</v>
+        <v>4.2435780720495586E-6</v>
       </c>
       <c r="M12" s="88"/>
       <c r="N12" s="60"/>
@@ -15311,33 +15307,31 @@
       <c r="A13" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B13" s="1">
-        <v>0.990436803259924</v>
-      </c>
-      <c r="C13" s="89">
-        <v>0.99068493940870395</v>
-      </c>
-      <c r="D13" s="15">
+      <c r="B13" s="94">
+        <v>0.99043738711110496</v>
+      </c>
+      <c r="C13" s="94">
+        <v>0.99043329922193002</v>
+      </c>
+      <c r="D13" s="94">
         <f t="shared" si="1"/>
-        <v>-2.4813614877994272E-4</v>
-      </c>
-      <c r="E13" s="78"/>
-      <c r="F13" s="78"/>
+        <v>4.08788917494185E-6</v>
+      </c>
       <c r="G13" s="78">
-        <v>0.99043305219016098</v>
+        <v>0.99043303771721203</v>
       </c>
       <c r="H13" s="70">
-        <v>0.99093682662724702</v>
+        <v>0.99043356072664801</v>
       </c>
       <c r="I13" s="89"/>
-      <c r="J13" s="89"/>
-      <c r="K13" s="89">
+      <c r="J13" s="94"/>
+      <c r="K13" s="94">
         <f t="shared" si="4"/>
-        <v>3.7510697630249723E-6</v>
-      </c>
-      <c r="L13" s="89">
+        <v>4.3493938929328735E-6</v>
+      </c>
+      <c r="L13" s="94">
         <f t="shared" si="5"/>
-        <v>-5.0002336732302144E-4</v>
+        <v>3.8263844569508265E-6</v>
       </c>
       <c r="M13" s="88"/>
       <c r="N13" s="60"/>
@@ -15357,33 +15351,31 @@
       <c r="A14" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="B14" s="1">
-        <v>0.99358117274512303</v>
-      </c>
-      <c r="C14" s="89">
-        <v>0.99371778331877703</v>
-      </c>
-      <c r="D14" s="15">
+      <c r="B14" s="94">
+        <v>0.99358243743974495</v>
+      </c>
+      <c r="C14" s="94">
+        <v>0.99357879471724397</v>
+      </c>
+      <c r="D14" s="94">
         <f t="shared" si="1"/>
-        <v>-1.3661057365399465E-4</v>
-      </c>
-      <c r="E14" s="78"/>
-      <c r="F14" s="78"/>
+        <v>3.6427225009738606E-6</v>
+      </c>
       <c r="G14" s="78">
-        <v>0.99357991729689699</v>
+        <v>0.99357990430980803</v>
       </c>
       <c r="H14" s="70">
-        <v>0.99385564934065795</v>
+        <v>0.99357768512468103</v>
       </c>
       <c r="I14" s="89"/>
-      <c r="J14" s="89"/>
-      <c r="K14" s="89">
+      <c r="J14" s="94"/>
+      <c r="K14" s="94">
         <f t="shared" si="4"/>
-        <v>1.2554482260451749E-6</v>
-      </c>
-      <c r="L14" s="89">
+        <v>2.5331299369213411E-6</v>
+      </c>
+      <c r="L14" s="94">
         <f t="shared" si="5"/>
-        <v>-2.7447659553492265E-4</v>
+        <v>4.7523150639161571E-6</v>
       </c>
       <c r="M14" s="88"/>
       <c r="N14" s="60"/>
@@ -15403,28 +15395,26 @@
       <c r="A15" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B15" s="1">
-        <v>0.98674259047048396</v>
-      </c>
-      <c r="C15" s="89">
-        <v>0.98674139631796798</v>
-      </c>
-      <c r="D15" s="88">
+      <c r="B15" s="94">
+        <v>0.98674347394717699</v>
+      </c>
+      <c r="C15" s="94">
+        <v>0.986741385905198</v>
+      </c>
+      <c r="D15" s="94">
         <f t="shared" si="1"/>
-        <v>1.1941525159819832E-6</v>
-      </c>
-      <c r="E15" s="78"/>
-      <c r="F15" s="78"/>
+        <v>2.088041978987043E-6</v>
+      </c>
       <c r="G15" s="78">
-        <v>0.98674139631796798</v>
+        <v>0.986741385905198</v>
       </c>
       <c r="I15" s="89"/>
-      <c r="J15" s="89"/>
-      <c r="K15" s="89">
+      <c r="J15" s="94"/>
+      <c r="K15" s="94">
         <f t="shared" si="4"/>
-        <v>1.1941525159819832E-6</v>
-      </c>
-      <c r="L15" s="89"/>
+        <v>2.088041978987043E-6</v>
+      </c>
+      <c r="L15" s="94"/>
       <c r="M15" s="88"/>
       <c r="N15" s="60"/>
       <c r="O15" s="46" t="s">
@@ -15443,33 +15433,32 @@
       <c r="A16" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B16" s="1">
-        <v>0.98231334549872895</v>
-      </c>
-      <c r="C16" s="89">
-        <v>0.98239870844271104</v>
-      </c>
-      <c r="D16" s="88">
+      <c r="B16" s="94">
+        <v>0.98231520512326598</v>
+      </c>
+      <c r="C16" s="94">
+        <v>0.98230473663935702</v>
+      </c>
+      <c r="D16" s="94">
         <f t="shared" si="1"/>
-        <v>-8.5362943982092432E-5</v>
+        <v>1.0468483908954163E-5</v>
       </c>
       <c r="E16" s="78"/>
-      <c r="F16" s="78"/>
       <c r="G16" s="78">
-        <v>0.98231103136211795</v>
+        <v>0.98231101960685996</v>
       </c>
       <c r="H16" s="70">
-        <v>0.98248638552330303</v>
+        <v>0.98229845367185298</v>
       </c>
       <c r="I16" s="89"/>
-      <c r="J16" s="89"/>
-      <c r="K16" s="89">
+      <c r="J16" s="94"/>
+      <c r="K16" s="94">
         <f t="shared" si="4"/>
-        <v>2.3141366110035477E-6</v>
-      </c>
-      <c r="L16" s="89">
+        <v>4.1855164060189409E-6</v>
+      </c>
+      <c r="L16" s="94">
         <f t="shared" si="5"/>
-        <v>-1.7304002457407819E-4</v>
+        <v>1.6751451412999607E-5</v>
       </c>
       <c r="M16" s="88"/>
       <c r="N16" s="60" t="s">
@@ -15491,33 +15480,32 @@
       <c r="A17" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="B17" s="1">
-        <v>0.96825697606458705</v>
-      </c>
-      <c r="C17" s="89">
-        <v>0.96839530187483402</v>
-      </c>
-      <c r="D17" s="15">
+      <c r="B17" s="94">
+        <v>0.96825612557644003</v>
+      </c>
+      <c r="C17" s="94">
+        <v>0.96824324628943403</v>
+      </c>
+      <c r="D17" s="94">
         <f t="shared" si="1"/>
-        <v>-1.3832581024697532E-4</v>
+        <v>1.2879287005995721E-5</v>
       </c>
       <c r="E17" s="78"/>
-      <c r="F17" s="78"/>
       <c r="G17" s="78">
-        <v>0.96823584948891905</v>
+        <v>0.96823583653021394</v>
       </c>
       <c r="H17" s="70">
-        <v>0.96855475426074999</v>
+        <v>0.96825065604865401</v>
       </c>
       <c r="I17" s="89"/>
-      <c r="J17" s="89"/>
-      <c r="K17" s="89">
+      <c r="J17" s="94"/>
+      <c r="K17" s="94">
         <f t="shared" si="4"/>
-        <v>2.1126575667995695E-5</v>
-      </c>
-      <c r="L17" s="89">
+        <v>2.0289046226085183E-5</v>
+      </c>
+      <c r="L17" s="94">
         <f t="shared" si="5"/>
-        <v>-2.9777819616294554E-4</v>
+        <v>5.4695277860172808E-6</v>
       </c>
       <c r="M17" s="88"/>
       <c r="N17" s="60" t="s">
@@ -15539,28 +15527,26 @@
       <c r="A18" s="85" t="s">
         <v>86</v>
       </c>
-      <c r="B18" s="85">
-        <v>0</v>
-      </c>
-      <c r="C18" s="89">
-        <v>0</v>
-      </c>
-      <c r="D18" s="88">
+      <c r="B18" s="94">
+        <v>0</v>
+      </c>
+      <c r="C18" s="94">
+        <v>0</v>
+      </c>
+      <c r="D18" s="94">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E18" s="78">
         <v>0</v>
       </c>
-      <c r="F18" s="78"/>
-      <c r="G18" s="78"/>
-      <c r="I18" s="89">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J18" s="89"/>
-      <c r="K18" s="89"/>
-      <c r="L18" s="89"/>
+      <c r="I18" s="94">
+        <f>B18-E18</f>
+        <v>0</v>
+      </c>
+      <c r="J18" s="94"/>
+      <c r="K18" s="94"/>
+      <c r="L18" s="94"/>
       <c r="M18" s="88"/>
       <c r="N18" s="60"/>
       <c r="O18" s="46" t="s">
@@ -15580,33 +15566,32 @@
       <c r="A19" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B19" s="70">
-        <v>-9.0495834798616795E-2</v>
+      <c r="B19" s="94">
+        <v>-9.0497308536075197E-2</v>
       </c>
       <c r="C19" s="70">
-        <v>-9.0495006957268795E-2</v>
-      </c>
-      <c r="D19" s="88">
+        <v>-9.0495004080614297E-2</v>
+      </c>
+      <c r="D19" s="94">
         <f t="shared" si="1"/>
-        <v>-8.2784134800006903E-7</v>
+        <v>-2.3044554608997458E-6</v>
       </c>
       <c r="E19" s="78">
-        <v>-9.0496586093492606E-2</v>
+        <v>-9.0496586798202897E-2</v>
       </c>
       <c r="F19" s="78">
-        <v>-9.0493427821044997E-2</v>
-      </c>
-      <c r="G19" s="78"/>
-      <c r="I19" s="89">
-        <f t="shared" si="2"/>
-        <v>7.5129487581149235E-7</v>
-      </c>
-      <c r="J19" s="89">
+        <v>-9.0493421363025697E-2</v>
+      </c>
+      <c r="I19" s="94">
+        <f t="shared" ref="I19:I23" si="8">B19-E19</f>
+        <v>-7.217378723001211E-7</v>
+      </c>
+      <c r="J19" s="94">
         <f t="shared" si="3"/>
-        <v>-2.4069775717977526E-6</v>
-      </c>
-      <c r="K19" s="89"/>
-      <c r="L19" s="89"/>
+        <v>-3.8871730494993706E-6</v>
+      </c>
+      <c r="K19" s="94"/>
+      <c r="L19" s="94"/>
       <c r="M19" s="88"/>
       <c r="N19" s="60"/>
       <c r="O19" s="46" t="s">
@@ -15626,32 +15611,31 @@
         <v>88</v>
       </c>
       <c r="B20" s="70">
-        <v>-0.22164655627270699</v>
+        <v>-0.22164571889663801</v>
       </c>
       <c r="C20" s="70">
-        <v>-0.22164362773285601</v>
-      </c>
-      <c r="D20" s="88">
+        <v>-0.22164362857588699</v>
+      </c>
+      <c r="D20" s="94">
         <f t="shared" si="1"/>
-        <v>-2.9285398509826255E-6</v>
+        <v>-2.0903207510192257E-6</v>
       </c>
       <c r="E20" s="78">
-        <v>-0.22164304221862599</v>
+        <v>-0.22164304462450601</v>
       </c>
       <c r="F20" s="78">
-        <v>-0.221644213247086</v>
-      </c>
-      <c r="G20" s="78"/>
-      <c r="I20" s="89">
-        <f t="shared" si="2"/>
-        <v>-3.5140540809996956E-6</v>
-      </c>
-      <c r="J20" s="89">
+        <v>-0.22164421252726799</v>
+      </c>
+      <c r="I20" s="94">
+        <f t="shared" si="8"/>
+        <v>-2.6742721319916729E-6</v>
+      </c>
+      <c r="J20" s="94">
         <f t="shared" si="3"/>
-        <v>-2.3430256209933109E-6</v>
-      </c>
-      <c r="K20" s="89"/>
-      <c r="L20" s="89"/>
+        <v>-1.5063693700190228E-6</v>
+      </c>
+      <c r="K20" s="94"/>
+      <c r="L20" s="94"/>
       <c r="M20" s="88"/>
       <c r="N20" s="60"/>
       <c r="O20" s="46" t="s">
@@ -15671,37 +15655,36 @@
         <v>161</v>
       </c>
       <c r="B21" s="70">
-        <v>-0.18448701889772101</v>
+        <v>-0.18448669718473601</v>
       </c>
       <c r="C21" s="70">
-        <v>-0.184668139410924</v>
-      </c>
-      <c r="D21" s="15">
+        <v>-0.18448311517604801</v>
+      </c>
+      <c r="D21" s="94">
         <f t="shared" si="1"/>
-        <v>1.8112051320298694E-4</v>
+        <v>-3.5820086879967405E-6</v>
       </c>
       <c r="E21" s="78">
-        <v>-0.18448392181478299</v>
+        <v>-0.18448392409077399</v>
       </c>
       <c r="F21" s="78">
-        <v>-0.18448489483321101</v>
-      </c>
-      <c r="G21" s="78"/>
+        <v>-0.18448489948859101</v>
+      </c>
       <c r="H21" s="70">
-        <v>-0.185035601584779</v>
-      </c>
-      <c r="I21" s="89">
-        <f t="shared" si="2"/>
-        <v>-3.0970829380250198E-6</v>
-      </c>
-      <c r="J21" s="89">
+        <v>-0.18448052194877801</v>
+      </c>
+      <c r="I21" s="94">
+        <f t="shared" si="8"/>
+        <v>-2.7730939620163042E-6</v>
+      </c>
+      <c r="J21" s="94">
         <f t="shared" si="3"/>
-        <v>-2.1240645100006894E-6</v>
-      </c>
-      <c r="K21" s="89"/>
-      <c r="L21" s="89">
+        <v>-1.7976961450005824E-6</v>
+      </c>
+      <c r="K21" s="94"/>
+      <c r="L21" s="94">
         <f t="shared" si="5"/>
-        <v>5.4858268705798574E-4</v>
+        <v>-6.1752359580002913E-6</v>
       </c>
       <c r="M21" s="88"/>
       <c r="N21" s="60"/>
@@ -15722,37 +15705,37 @@
         <v>162</v>
       </c>
       <c r="B22" s="70">
-        <v>-0.158411156268046</v>
+        <v>-0.158410841039683</v>
       </c>
       <c r="C22" s="70">
-        <v>-0.15840751646811499</v>
-      </c>
-      <c r="D22" s="88">
+        <v>-0.158407517853214</v>
+      </c>
+      <c r="D22" s="94">
         <f t="shared" si="1"/>
-        <v>-3.639799931010046E-6</v>
+        <v>-3.3231864690064228E-6</v>
       </c>
       <c r="E22" s="78">
-        <v>-0.15840865307285701</v>
+        <v>-0.158408654175522</v>
       </c>
       <c r="F22" s="78">
-        <v>-0.15840900789638801</v>
+        <v>-0.158409012218196</v>
       </c>
       <c r="G22" s="78">
-        <v>-0.15840488843509901</v>
-      </c>
-      <c r="I22" s="89">
-        <f t="shared" si="2"/>
-        <v>-2.5031951889908921E-6</v>
-      </c>
-      <c r="J22" s="89">
+        <v>-0.15840488716592499</v>
+      </c>
+      <c r="I22" s="94">
+        <f t="shared" si="8"/>
+        <v>-2.1868641610078843E-6</v>
+      </c>
+      <c r="J22" s="94">
         <f t="shared" si="3"/>
-        <v>-2.148371657989534E-6</v>
-      </c>
-      <c r="K22" s="89">
+        <v>-1.8288214869988106E-6</v>
+      </c>
+      <c r="K22" s="94">
         <f t="shared" si="4"/>
-        <v>-6.2678329469934013E-6</v>
-      </c>
-      <c r="L22" s="89"/>
+        <v>-5.9538737580133727E-6</v>
+      </c>
+      <c r="L22" s="94"/>
       <c r="M22" s="88"/>
       <c r="N22" s="60"/>
       <c r="O22" s="46" t="s">
@@ -15772,32 +15755,31 @@
         <v>163</v>
       </c>
       <c r="B23" s="70">
-        <v>-0.26207372353015002</v>
+        <v>-0.26207421261853298</v>
       </c>
       <c r="C23" s="70">
-        <v>-0.26206993443009402</v>
-      </c>
-      <c r="D23" s="88">
+        <v>-0.26206994036895798</v>
+      </c>
+      <c r="D23" s="94">
         <f t="shared" si="1"/>
-        <v>-3.7891000559953092E-6</v>
+        <v>-4.2722495749991651E-6</v>
       </c>
       <c r="E23" s="78">
-        <v>-0.26206909243514398</v>
-      </c>
-      <c r="F23" s="78"/>
+        <v>-0.26206909640005899</v>
+      </c>
       <c r="G23" s="78">
-        <v>-0.26207077642504401</v>
-      </c>
-      <c r="I23" s="89">
-        <f t="shared" si="2"/>
-        <v>-4.631095006035757E-6</v>
-      </c>
-      <c r="J23" s="89"/>
-      <c r="K23" s="89">
+        <v>-0.26207078433785702</v>
+      </c>
+      <c r="I23" s="94">
+        <f t="shared" si="8"/>
+        <v>-5.1162184739883543E-6</v>
+      </c>
+      <c r="J23" s="94"/>
+      <c r="K23" s="94">
         <f t="shared" si="4"/>
-        <v>-2.9471051060103726E-6</v>
-      </c>
-      <c r="L23" s="89"/>
+        <v>-3.4282806759544648E-6</v>
+      </c>
+      <c r="L23" s="94"/>
       <c r="M23" s="88"/>
       <c r="N23" s="60"/>
       <c r="O23" s="46" t="s">
@@ -15817,32 +15799,31 @@
         <v>164</v>
       </c>
       <c r="B24" s="70">
-        <v>-0.246986077730002</v>
+        <v>-0.24698613878575901</v>
       </c>
       <c r="C24" s="70">
-        <v>-0.24595627779100401</v>
-      </c>
-      <c r="D24" s="15">
+        <v>-0.24698815398123899</v>
+      </c>
+      <c r="D24" s="94">
         <f t="shared" si="1"/>
-        <v>-1.0297999389979884E-3</v>
+        <v>2.0151954799874083E-6</v>
       </c>
       <c r="E24" s="78"/>
       <c r="F24" s="78">
-        <v>-0.246983697017881</v>
-      </c>
-      <c r="G24" s="78"/>
+        <v>-0.24698371524429699</v>
+      </c>
       <c r="H24" s="70">
-        <v>-0.24492885856412699</v>
+        <v>-0.246992592718181</v>
       </c>
       <c r="I24" s="1"/>
-      <c r="J24" s="89">
+      <c r="J24" s="94">
         <f t="shared" si="3"/>
-        <v>-2.3807121209973303E-6</v>
-      </c>
-      <c r="K24" s="89"/>
-      <c r="L24" s="89">
+        <v>-2.4235414620155105E-6</v>
+      </c>
+      <c r="K24" s="94"/>
+      <c r="L24" s="94">
         <f t="shared" si="5"/>
-        <v>-2.0572191658750072E-3</v>
+        <v>6.4539324219903271E-6</v>
       </c>
       <c r="M24" s="88"/>
       <c r="N24" s="60"/>
@@ -15863,27 +15844,26 @@
         <v>165</v>
       </c>
       <c r="B25" s="70">
-        <v>-0.25618480157818402</v>
+        <v>-0.25618355897582701</v>
       </c>
       <c r="C25" s="70">
-        <v>-0.25618214559653502</v>
-      </c>
-      <c r="D25" s="88">
+        <v>-0.256182166526431</v>
+      </c>
+      <c r="D25" s="94">
         <f t="shared" si="1"/>
-        <v>-2.6559816490023813E-6</v>
+        <v>-1.3924493960093542E-6</v>
       </c>
       <c r="E25" s="78"/>
       <c r="F25" s="78">
-        <v>-0.25618214559653502</v>
-      </c>
-      <c r="G25" s="78"/>
+        <v>-0.256182166526431</v>
+      </c>
       <c r="I25" s="1"/>
-      <c r="J25" s="89">
+      <c r="J25" s="94">
         <f t="shared" si="3"/>
-        <v>-2.6559816490023813E-6</v>
-      </c>
-      <c r="K25" s="89"/>
-      <c r="L25" s="89"/>
+        <v>-1.3924493960093542E-6</v>
+      </c>
+      <c r="K25" s="94"/>
+      <c r="L25" s="94"/>
       <c r="M25" s="88"/>
       <c r="N25" s="60"/>
       <c r="O25" s="46" t="s">
@@ -15903,32 +15883,31 @@
         <v>166</v>
       </c>
       <c r="B26" s="70">
-        <v>-0.27411931344698798</v>
+        <v>-0.27412190223542499</v>
       </c>
       <c r="C26" s="70">
-        <v>-0.27309010215351298</v>
-      </c>
-      <c r="D26" s="15">
+        <v>-0.27412310519893801</v>
+      </c>
+      <c r="D26" s="94">
         <f t="shared" si="1"/>
-        <v>-1.0292112934749964E-3</v>
+        <v>1.2029635130250682E-6</v>
       </c>
       <c r="E26" s="78"/>
       <c r="F26" s="78">
-        <v>-0.27411693909551499</v>
-      </c>
-      <c r="G26" s="78"/>
+        <v>-0.274116961011173</v>
+      </c>
       <c r="H26" s="70">
-        <v>-0.27206326521151197</v>
+        <v>-0.27412924938670302</v>
       </c>
       <c r="I26" s="1"/>
-      <c r="J26" s="89">
+      <c r="J26" s="94">
         <f t="shared" si="3"/>
-        <v>-2.3743514729890336E-6</v>
-      </c>
-      <c r="K26" s="89"/>
-      <c r="L26" s="89">
+        <v>-4.941224251986398E-6</v>
+      </c>
+      <c r="K26" s="94"/>
+      <c r="L26" s="94">
         <f t="shared" si="5"/>
-        <v>-2.0560482354760046E-3</v>
+        <v>7.3471512780365344E-6</v>
       </c>
       <c r="M26" s="88"/>
       <c r="N26" s="60" t="s">
@@ -15951,32 +15930,32 @@
         <v>167</v>
       </c>
       <c r="B27" s="70">
-        <v>-0.27529246082033898</v>
+        <v>-0.27529143375314102</v>
       </c>
       <c r="C27" s="70">
-        <v>-0.27416065913002602</v>
-      </c>
-      <c r="D27" s="15">
+        <v>-0.27529183747997399</v>
+      </c>
+      <c r="D27" s="94">
         <f t="shared" si="1"/>
-        <v>-1.1318016903129613E-3</v>
+        <v>4.037268329648569E-7</v>
       </c>
       <c r="E27" s="78"/>
       <c r="F27" s="78"/>
       <c r="G27" s="78">
-        <v>-0.27528366711101698</v>
-      </c>
-      <c r="H27" s="89">
-        <v>-0.273037651149036</v>
+        <v>-0.275283690855601</v>
+      </c>
+      <c r="H27" s="70">
+        <v>-0.27529998410434697</v>
       </c>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
-      <c r="K27" s="89">
+      <c r="K27" s="94">
         <f t="shared" si="4"/>
-        <v>-8.7937093219969675E-6</v>
-      </c>
-      <c r="L27" s="89">
+        <v>-7.7428975400195554E-6</v>
+      </c>
+      <c r="L27" s="94">
         <f t="shared" si="5"/>
-        <v>-2.2548096713029819E-3</v>
+        <v>8.5503512059492692E-6</v>
       </c>
       <c r="M27" s="88"/>
       <c r="N27" s="56" t="s">
@@ -15989,7 +15968,7 @@
         <v>6.1776975079165704</v>
       </c>
       <c r="Q27" s="1">
-        <f t="shared" ref="Q27:Q30" si="8">P27/100</f>
+        <f t="shared" ref="Q27:Q30" si="9">P27/100</f>
         <v>6.1776975079165707E-2</v>
       </c>
       <c r="R27" s="57"/>
@@ -15999,32 +15978,32 @@
         <v>168</v>
       </c>
       <c r="B28" s="70">
-        <v>-0.27032933293769501</v>
+        <v>-0.270326407772359</v>
       </c>
       <c r="C28" s="70">
-        <v>-0.26906488132364798</v>
-      </c>
-      <c r="D28" s="15">
+        <v>-0.27032809476306302</v>
+      </c>
+      <c r="D28" s="94">
         <f t="shared" si="1"/>
-        <v>-1.2644516140470352E-3</v>
+        <v>1.6869907040195642E-6</v>
       </c>
       <c r="E28" s="78"/>
       <c r="F28" s="78"/>
       <c r="G28" s="78">
-        <v>-0.27032226723179198</v>
+        <v>-0.27032228342655501</v>
       </c>
       <c r="H28" s="70">
-        <v>-0.26780749541550403</v>
+        <v>-0.27033390609957098</v>
       </c>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
-      <c r="K28" s="89">
+      <c r="K28" s="94">
         <f t="shared" si="4"/>
-        <v>-7.0657059030310165E-6</v>
-      </c>
-      <c r="L28" s="89">
+        <v>-4.1243458039907921E-6</v>
+      </c>
+      <c r="L28" s="94">
         <f t="shared" si="5"/>
-        <v>-2.5218375221909839E-3</v>
+        <v>7.4983272119744093E-6</v>
       </c>
       <c r="M28" s="88"/>
       <c r="N28" s="61"/>
@@ -16035,7 +16014,7 @@
         <v>10.1258308263922</v>
       </c>
       <c r="Q28" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.101258308263922</v>
       </c>
       <c r="R28" s="58"/>
@@ -16045,27 +16024,27 @@
         <v>169</v>
       </c>
       <c r="B29" s="70">
-        <v>-0.27392983143629202</v>
+        <v>-0.27392437565368799</v>
       </c>
       <c r="C29" s="70">
-        <v>-0.27392309975083301</v>
-      </c>
-      <c r="D29" s="88">
+        <v>-0.27392310756709498</v>
+      </c>
+      <c r="D29" s="94">
         <f t="shared" si="1"/>
-        <v>-6.7316854590049324E-6</v>
+        <v>-1.2680865930092544E-6</v>
       </c>
       <c r="E29" s="78"/>
       <c r="F29" s="78"/>
       <c r="G29" s="78">
-        <v>-0.27392309975083301</v>
+        <v>-0.27392310756709498</v>
       </c>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
-      <c r="K29" s="89">
+      <c r="K29" s="94">
         <f t="shared" si="4"/>
-        <v>-6.7316854590049324E-6</v>
-      </c>
-      <c r="L29" s="89"/>
+        <v>-1.2680865930092544E-6</v>
+      </c>
+      <c r="L29" s="94"/>
       <c r="M29" s="88"/>
       <c r="N29" s="61"/>
       <c r="O29" s="46" t="s">
@@ -16075,7 +16054,7 @@
         <v>4.8779939913553596</v>
       </c>
       <c r="Q29" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>4.8779939913553595E-2</v>
       </c>
       <c r="R29" s="57"/>
@@ -16085,32 +16064,32 @@
         <v>170</v>
       </c>
       <c r="B30" s="70">
-        <v>-0.27443829599560998</v>
+        <v>-0.274434092517713</v>
       </c>
       <c r="C30" s="70">
-        <v>-0.27284635464601098</v>
-      </c>
-      <c r="D30" s="15">
+        <v>-0.27442811683323298</v>
+      </c>
+      <c r="D30" s="94">
         <f t="shared" si="1"/>
-        <v>-1.591941349599002E-3</v>
+        <v>-5.9756844800196163E-6</v>
       </c>
       <c r="E30" s="78"/>
       <c r="F30" s="78"/>
       <c r="G30" s="78">
-        <v>-0.27442990721687799</v>
+        <v>-0.27442991980982201</v>
       </c>
       <c r="H30" s="70">
-        <v>-0.27126280207514403</v>
+        <v>-0.27442631385664301</v>
       </c>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
-      <c r="K30" s="89">
+      <c r="K30" s="94">
         <f t="shared" si="4"/>
-        <v>-8.388778731993618E-6</v>
-      </c>
-      <c r="L30" s="89">
+        <v>-4.1727078909925552E-6</v>
+      </c>
+      <c r="L30" s="94">
         <f t="shared" si="5"/>
-        <v>-3.1754939204659549E-3</v>
+        <v>-7.7786610699903669E-6</v>
       </c>
       <c r="M30" s="88"/>
       <c r="N30" s="56" t="s">
@@ -16123,7 +16102,7 @@
         <v>-7.6</v>
       </c>
       <c r="Q30" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-7.5999999999999998E-2</v>
       </c>
       <c r="R30" s="58"/>
@@ -16133,32 +16112,32 @@
         <v>171</v>
       </c>
       <c r="B31" s="70">
-        <v>-0.287190454321613</v>
+        <v>-0.28718451695640301</v>
       </c>
       <c r="C31" s="70">
-        <v>-0.28582841441131002</v>
-      </c>
-      <c r="D31" s="15">
+        <v>-0.28717834331726699</v>
+      </c>
+      <c r="D31" s="94">
         <f t="shared" si="1"/>
-        <v>-1.3620399103029812E-3</v>
+        <v>-6.1736391360200926E-6</v>
       </c>
       <c r="E31" s="78"/>
       <c r="F31" s="78"/>
       <c r="G31" s="78">
-        <v>-0.28716613340021302</v>
+        <v>-0.28716616958522601</v>
       </c>
       <c r="H31" s="70">
-        <v>-0.28449069542240601</v>
+        <v>-0.28719051704930898</v>
       </c>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
-      <c r="K31" s="89">
+      <c r="K31" s="94">
         <f t="shared" si="4"/>
-        <v>-2.4320921399978435E-5</v>
-      </c>
-      <c r="L31" s="89">
+        <v>-1.8347371177007687E-5</v>
+      </c>
+      <c r="L31" s="94">
         <f t="shared" si="5"/>
-        <v>-2.6997588992069832E-3</v>
+        <v>6.000092905966703E-6</v>
       </c>
       <c r="M31" s="88"/>
       <c r="N31" s="60" t="s">
@@ -16171,7 +16150,7 @@
         <v>-1.6</v>
       </c>
       <c r="Q31" s="1">
-        <f t="shared" ref="Q31:Q40" si="9">P31/100</f>
+        <f t="shared" ref="Q31:Q40" si="10">P31/100</f>
         <v>-1.6E-2</v>
       </c>
       <c r="R31" s="58"/>
@@ -16187,7 +16166,7 @@
         <v>-63.001699846354903</v>
       </c>
       <c r="Q32" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-0.63001699846354908</v>
       </c>
       <c r="R32" s="58"/>
@@ -16201,7 +16180,7 @@
         <v>10.2039485868599</v>
       </c>
       <c r="Q33" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.102039485868599</v>
       </c>
       <c r="R33" s="58"/>
@@ -16215,7 +16194,7 @@
         <v>16.526211548050401</v>
       </c>
       <c r="Q34" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.16526211548050401</v>
       </c>
       <c r="R34" s="58"/>
@@ -16231,7 +16210,7 @@
         <v>-1.34369314780613</v>
       </c>
       <c r="Q35" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-1.34369314780613E-2</v>
       </c>
       <c r="R35" s="58"/>
@@ -16258,7 +16237,7 @@
         <v>29.247637436823101</v>
       </c>
       <c r="Q36" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.29247637436823104</v>
       </c>
       <c r="R36" s="58"/>
@@ -16285,7 +16264,7 @@
         <v>11.0919776937066</v>
       </c>
       <c r="Q37" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.11091977693706599</v>
       </c>
       <c r="R37" s="58"/>
@@ -16312,7 +16291,7 @@
         <v>-94.199996999999996</v>
       </c>
       <c r="Q38" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-0.94199996999999991</v>
       </c>
       <c r="R38" s="58"/>
@@ -16342,7 +16321,7 @@
         <v>2.4613437652587002</v>
       </c>
       <c r="Q39" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2.4613437652587004E-2</v>
       </c>
       <c r="R39" s="58"/>
@@ -16369,7 +16348,7 @@
         <v>4.9650161007164098</v>
       </c>
       <c r="Q40" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>4.9650161007164101E-2</v>
       </c>
       <c r="R40" s="58"/>
@@ -16393,7 +16372,7 @@
         <v>0.52427629116916796</v>
       </c>
       <c r="Q41" s="1">
-        <f t="shared" ref="Q41:Q43" si="10">P41/100</f>
+        <f t="shared" ref="Q41:Q43" si="11">P41/100</f>
         <v>5.2427629116916794E-3</v>
       </c>
       <c r="R41" s="58"/>
@@ -16418,7 +16397,7 @@
         <v>-13.5</v>
       </c>
       <c r="Q42" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-0.13500000000000001</v>
       </c>
       <c r="R42" s="58"/>
@@ -16443,7 +16422,7 @@
         <v>-5.8</v>
       </c>
       <c r="Q43" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-5.7999999999999996E-2</v>
       </c>
       <c r="R43" s="58"/>
@@ -16499,7 +16478,7 @@
         <v>0.31779049296478201</v>
       </c>
       <c r="Q45" s="1">
-        <f t="shared" ref="Q45:Q51" si="11">P45/100</f>
+        <f t="shared" ref="Q45:Q51" si="12">P45/100</f>
         <v>3.1779049296478202E-3</v>
       </c>
       <c r="R45" s="58"/>
@@ -16526,7 +16505,7 @@
         <v>-14.9</v>
       </c>
       <c r="Q46" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-0.14899999999999999</v>
       </c>
       <c r="R46" s="58"/>
@@ -16555,7 +16534,7 @@
         <v>-5</v>
       </c>
       <c r="Q47" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-0.05</v>
       </c>
       <c r="R47" s="58"/>
@@ -16583,7 +16562,7 @@
         <v>72.934574594694098</v>
       </c>
       <c r="Q48" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.72934574594694102</v>
       </c>
       <c r="R48" s="58" t="s">
@@ -16639,7 +16618,7 @@
         <v>42.467165475154701</v>
       </c>
       <c r="Q50" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.424671654751547</v>
       </c>
       <c r="R50" s="58" t="s">
@@ -16667,7 +16646,7 @@
         <v>-2.12732489205733</v>
       </c>
       <c r="Q51" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-2.12732489205733E-2</v>
       </c>
       <c r="R51" s="58" t="s">
@@ -16749,7 +16728,7 @@
         <v>1.009999997</v>
       </c>
       <c r="Q54" s="1">
-        <f t="shared" ref="Q54:Q59" si="12">P54</f>
+        <f t="shared" ref="Q54:Q59" si="13">P54</f>
         <v>1.009999997</v>
       </c>
       <c r="R54" s="58" t="s">
@@ -16775,7 +16754,7 @@
         <v>1.085083507</v>
       </c>
       <c r="Q55" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.085083507</v>
       </c>
       <c r="R55" s="58" t="s">
@@ -16801,7 +16780,7 @@
         <v>1.0240525229999999</v>
       </c>
       <c r="Q56" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.0240525229999999</v>
       </c>
       <c r="R56" s="58" t="s">
@@ -16827,7 +16806,7 @@
         <v>1.019923836</v>
       </c>
       <c r="Q57" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.019923836</v>
       </c>
       <c r="R57" s="58" t="s">
@@ -16853,7 +16832,7 @@
         <v>1.027986216</v>
       </c>
       <c r="Q58" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.027986216</v>
       </c>
       <c r="R58" s="58" t="s">
@@ -16879,7 +16858,7 @@
         <v>1.0349152580000001</v>
       </c>
       <c r="Q59" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.0349152580000001</v>
       </c>
       <c r="R59" s="58" t="s">
@@ -17037,7 +17016,7 @@
         <v>-20.300935880694301</v>
       </c>
       <c r="Q65" s="1">
-        <f t="shared" ref="Q65:Q71" si="13">P65/100</f>
+        <f t="shared" ref="Q65:Q71" si="14">P65/100</f>
         <v>-0.20300935880694301</v>
       </c>
       <c r="R65" s="58">
@@ -17052,7 +17031,7 @@
         <v>75.916881283268793</v>
       </c>
       <c r="Q66" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.75916881283268789</v>
       </c>
       <c r="R66" s="58">
@@ -17067,7 +17046,7 @@
         <v>-0.155506560051652</v>
       </c>
       <c r="Q67" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>-1.55506560051652E-3</v>
       </c>
       <c r="R67" s="58">
@@ -17082,7 +17061,7 @@
         <v>41.338725991097199</v>
       </c>
       <c r="Q68" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.41338725991097197</v>
       </c>
       <c r="R68" s="58">
@@ -17097,7 +17076,7 @@
         <v>-3.8398609004379098</v>
       </c>
       <c r="Q69" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>-3.8398609004379101E-2</v>
       </c>
       <c r="R69" s="58">
@@ -17112,7 +17091,7 @@
         <v>232.35762119293199</v>
       </c>
       <c r="Q70" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2.32357621192932</v>
       </c>
       <c r="R70" s="58">
@@ -17130,7 +17109,7 @@
         <v>-20.456442236900301</v>
       </c>
       <c r="Q71" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>-0.20456442236900302</v>
       </c>
       <c r="R71" s="58">
@@ -17193,7 +17172,7 @@
         <v>0.96859150246414105</v>
       </c>
       <c r="Q75" s="1">
-        <f t="shared" ref="Q75:Q79" si="14">P75/100</f>
+        <f t="shared" ref="Q75:Q79" si="15">P75/100</f>
         <v>9.6859150246414102E-3</v>
       </c>
       <c r="R75" s="58">
@@ -17208,7 +17187,7 @@
         <v>29.247688021076399</v>
       </c>
       <c r="Q76" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.29247688021076401</v>
       </c>
       <c r="R76" s="58">
@@ -17223,7 +17202,7 @@
         <v>-10.134384235994199</v>
       </c>
       <c r="Q77" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-0.101343842359942</v>
       </c>
       <c r="R77" s="58">
@@ -17238,7 +17217,7 @@
         <v>4.9388912162000001E-5</v>
       </c>
       <c r="Q78" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>4.9388912162000003E-7</v>
       </c>
       <c r="R78" s="58">
@@ -17256,7 +17235,7 @@
         <v>-23.1382548362844</v>
       </c>
       <c r="Q79" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-0.231382548362844</v>
       </c>
       <c r="R79" s="58">
@@ -17319,7 +17298,7 @@
         <v>1.57798981550307</v>
       </c>
       <c r="Q83" s="1">
-        <f t="shared" ref="Q83:Q91" si="15">P83/100</f>
+        <f t="shared" ref="Q83:Q91" si="16">P83/100</f>
         <v>1.5779898155030701E-2</v>
       </c>
       <c r="R83" s="58">
@@ -17334,7 +17313,7 @@
         <v>7.6111237412808599</v>
       </c>
       <c r="Q84" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>7.6111237412808605E-2</v>
       </c>
       <c r="R84" s="58">
@@ -17349,7 +17328,7 @@
         <v>2.2749299623984598</v>
       </c>
       <c r="Q85" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>2.2749299623984597E-2</v>
       </c>
       <c r="R85" s="58">
@@ -17364,7 +17343,7 @@
         <v>17.236621109828601</v>
       </c>
       <c r="Q86" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.17236621109828601</v>
       </c>
       <c r="R86" s="58">
@@ -17379,7 +17358,7 @@
         <v>6.2088690408799696</v>
       </c>
       <c r="Q87" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>6.2088690408799697E-2</v>
       </c>
       <c r="R87" s="58">
@@ -17394,7 +17373,7 @@
         <v>1.4392071686730901</v>
       </c>
       <c r="Q88" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1.4392071686730901E-2</v>
       </c>
       <c r="R88" s="58">
@@ -17409,7 +17388,7 @@
         <v>0.52526799870488805</v>
       </c>
       <c r="Q89" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>5.2526799870488807E-3</v>
       </c>
       <c r="R89" s="58">
@@ -17424,7 +17403,7 @@
         <v>-6.1</v>
       </c>
       <c r="Q90" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-6.0999999999999999E-2</v>
       </c>
       <c r="R90" s="58">
@@ -17442,7 +17421,7 @@
         <v>-1.6</v>
       </c>
       <c r="Q91" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-1.6E-2</v>
       </c>
       <c r="R91" s="58">
@@ -17510,7 +17489,7 @@
         <v>6.1776975079165704</v>
       </c>
       <c r="Q95" s="1">
-        <f t="shared" ref="Q95:Q107" si="16">P95/100</f>
+        <f t="shared" ref="Q95:Q107" si="17">P95/100</f>
         <v>6.1776975079165707E-2</v>
       </c>
       <c r="R95" s="57">
@@ -17527,7 +17506,7 @@
         <v>10.1258308263922</v>
       </c>
       <c r="Q96" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.101258308263922</v>
       </c>
       <c r="R96" s="58">
@@ -17546,7 +17525,7 @@
         <v>4.8779939913553596</v>
       </c>
       <c r="Q97" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>4.8779939913553595E-2</v>
       </c>
       <c r="R97" s="57">
@@ -17565,7 +17544,7 @@
         <v>-7.6</v>
       </c>
       <c r="Q98" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>-7.5999999999999998E-2</v>
       </c>
       <c r="R98" s="58">
@@ -17584,7 +17563,7 @@
         <v>-1.6</v>
       </c>
       <c r="Q99" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>-1.6E-2</v>
       </c>
       <c r="R99" s="58">
@@ -17603,7 +17582,7 @@
         <v>-63.001699846354903</v>
       </c>
       <c r="Q100" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>-0.63001699846354908</v>
       </c>
       <c r="R100" s="58">
@@ -17619,7 +17598,7 @@
         <v>10.2039485868599</v>
       </c>
       <c r="Q101" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.102039485868599</v>
       </c>
       <c r="R101" s="58">
@@ -17635,7 +17614,7 @@
         <v>16.526211548050401</v>
       </c>
       <c r="Q102" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.16526211548050401</v>
       </c>
       <c r="R102" s="58">
@@ -17651,7 +17630,7 @@
         <v>-1.34369314780613</v>
       </c>
       <c r="Q103" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>-1.34369314780613E-2</v>
       </c>
       <c r="R103" s="58">
@@ -17667,7 +17646,7 @@
         <v>29.247637436823101</v>
       </c>
       <c r="Q104" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.29247637436823104</v>
       </c>
       <c r="R104" s="58">
@@ -17683,7 +17662,7 @@
         <v>11.0919776937066</v>
       </c>
       <c r="Q105" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.11091977693706599</v>
       </c>
       <c r="R105" s="58">
@@ -17699,7 +17678,7 @@
         <v>-94.199996999999996</v>
       </c>
       <c r="Q106" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>-0.94199996999999991</v>
       </c>
       <c r="R106" s="58">
@@ -17716,7 +17695,7 @@
         <v>2.4613437652587002</v>
       </c>
       <c r="Q107" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>2.4613437652587004E-2</v>
       </c>
       <c r="R107" s="58">
@@ -17784,7 +17763,7 @@
         <v>0.52427629116916796</v>
       </c>
       <c r="Q111" s="1">
-        <f t="shared" ref="Q111:Q113" si="17">P111/100</f>
+        <f t="shared" ref="Q111:Q113" si="18">P111/100</f>
         <v>5.2427629116916794E-3</v>
       </c>
       <c r="R111" s="58">
@@ -17799,7 +17778,7 @@
         <v>-13.5</v>
       </c>
       <c r="Q112" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>-0.13500000000000001</v>
       </c>
       <c r="R112" s="58">
@@ -17814,7 +17793,7 @@
         <v>-5.8</v>
       </c>
       <c r="Q113" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>-5.7999999999999996E-2</v>
       </c>
       <c r="R113" s="58">
@@ -17880,7 +17859,7 @@
         <v>0.31779049296478201</v>
       </c>
       <c r="Q117" s="1">
-        <f t="shared" ref="Q117:Q119" si="18">P117/100</f>
+        <f t="shared" ref="Q117:Q119" si="19">P117/100</f>
         <v>3.1779049296478202E-3</v>
       </c>
       <c r="R117" s="58">
@@ -17895,7 +17874,7 @@
         <v>-14.9</v>
       </c>
       <c r="Q118" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>-0.14899999999999999</v>
       </c>
       <c r="R118" s="58">
@@ -17910,7 +17889,7 @@
         <v>-5</v>
       </c>
       <c r="Q119" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>-0.05</v>
       </c>
       <c r="R119" s="58">
@@ -18092,20 +18071,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="98" t="s">
         <v>288</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
-      <c r="K1" s="96"/>
-      <c r="L1" s="96"/>
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="98"/>
+      <c r="H1" s="98"/>
+      <c r="I1" s="98"/>
+      <c r="J1" s="98"/>
+      <c r="K1" s="98"/>
+      <c r="L1" s="98"/>
       <c r="M1" s="91"/>
       <c r="N1" s="91"/>
       <c r="O1" s="11" t="s">
@@ -18129,22 +18108,22 @@
       <c r="B2" s="92" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="97" t="s">
+      <c r="C2" s="99" t="s">
         <v>285</v>
       </c>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97" t="s">
+      <c r="D2" s="99"/>
+      <c r="E2" s="99" t="s">
         <v>284</v>
       </c>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97" t="s">
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99" t="s">
         <v>74</v>
       </c>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
+      <c r="K2" s="99"/>
+      <c r="L2" s="99"/>
       <c r="M2" s="4"/>
       <c r="N2" s="60" t="s">
         <v>137</v>

</xml_diff>